<commit_message>
cost update Aug 18
</commit_message>
<xml_diff>
--- a/Cost.xlsx
+++ b/Cost.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chengkaiyan/cost/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB61572-8608-A341-B6A1-694166376203}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="225">
   <si>
     <t>日期</t>
   </si>
@@ -433,7 +428,7 @@
     <t>eckerolinjen till Åland</t>
   </si>
   <si>
-    <t xml:space="preserve">eckerolinjen </t>
+    <t>eckerolinjen </t>
   </si>
   <si>
     <t>hamburger</t>
@@ -686,45 +681,66 @@
   </si>
   <si>
     <t>parking</t>
+  </si>
+  <si>
+    <t>salad bowls; cabbage; flasksterk</t>
+  </si>
+  <si>
+    <t>citygrossen</t>
+  </si>
+  <si>
+    <t>Flaskkot ; face clean gel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy/m/d"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt formatCode="YYYY/M/D" numFmtId="165"/>
+    <numFmt formatCode="M/D/YYYY" numFmtId="166"/>
+    <numFmt formatCode="YYYY\-MM\-DD" numFmtId="167"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <family val="0"/>
       <sz val="10"/>
-      <name val="Arial"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <family val="0"/>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
     </font>
     <font>
-      <u/>
+      <name val="Arial"/>
+      <family val="0"/>
       <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF666666"/>
-      <name val="Lato"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <sz val="10"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF666666"/>
       <sz val="11"/>
-      <color rgb="FF666666"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="5">
@@ -737,24 +753,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE1DCDC"/>
-        <bgColor rgb="FFE1DCDC"/>
+        <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
@@ -762,364 +778,177 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+  <cellXfs count="11">
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="167" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
+        <patternFill>
           <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFE1DCDC"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666666"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Z175"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E165" sqref="E165"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E171" activeCellId="0" pane="topLeft" sqref="E171"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="37.83203125" customWidth="1"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="14.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1136,11 +965,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="13" hidden="1">
-      <c r="A2" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="2">
+      <c r="A2" s="2" t="n">
         <v>43121</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="1" t="n">
         <v>250</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1150,11 +979,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13" hidden="1">
-      <c r="A3" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="3">
+      <c r="A3" s="2" t="n">
         <v>43122</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="1" t="n">
         <v>305</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1164,11 +993,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="13" hidden="1">
-      <c r="A4" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="4">
+      <c r="A4" s="2" t="n">
         <v>43122</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1178,11 +1007,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="13" hidden="1">
-      <c r="A5" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="5">
+      <c r="A5" s="2" t="n">
         <v>43125</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="1" t="n">
         <v>98</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1192,11 +1021,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="13" hidden="1">
-      <c r="A6" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="6">
+      <c r="A6" s="2" t="n">
         <v>43126</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1206,11 +1035,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="13" hidden="1">
-      <c r="A7" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="7">
+      <c r="A7" s="2" t="n">
         <v>43127</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1220,11 +1049,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="13" hidden="1">
-      <c r="A8" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="8">
+      <c r="A8" s="2" t="n">
         <v>43128</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="1" t="n">
         <v>656</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1234,11 +1063,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="13" hidden="1">
-      <c r="A9" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="9">
+      <c r="A9" s="2" t="n">
         <v>43131</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="1" t="n">
         <v>486</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1248,11 +1077,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="13" hidden="1">
-      <c r="A10" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="10">
+      <c r="A10" s="2" t="n">
         <v>43132</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="1" t="n">
         <v>76</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1262,11 +1091,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="13" hidden="1">
-      <c r="A11" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="11">
+      <c r="A11" s="2" t="n">
         <v>43133</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="1" t="n">
         <v>399</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1276,11 +1105,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="13" hidden="1">
-      <c r="A12" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="12">
+      <c r="A12" s="2" t="n">
         <v>43135</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="1" t="n">
         <v>419</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1290,11 +1119,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="13" hidden="1">
-      <c r="A13" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="13">
+      <c r="A13" s="2" t="n">
         <v>43136</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="1" t="n">
         <v>521</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1304,11 +1133,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="13" hidden="1">
-      <c r="A14" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="14">
+      <c r="A14" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="1" t="n">
         <v>399</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1318,11 +1147,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="13" hidden="1">
-      <c r="A15" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="15">
+      <c r="A15" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="1" t="n">
         <v>138</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1332,11 +1161,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="13" hidden="1">
-      <c r="A16" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="16">
+      <c r="A16" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="1" t="n">
         <v>310</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1346,12 +1175,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="13" hidden="1">
-      <c r="A17" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="17">
+      <c r="A17" s="2" t="n">
         <v>43138</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="1">
+      <c r="C17" s="1" t="n">
         <v>700</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1361,12 +1190,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="13" hidden="1">
-      <c r="A18" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="18">
+      <c r="A18" s="2" t="n">
         <v>43141</v>
       </c>
-      <c r="C18" s="1">
-        <f>F18*G18</f>
+      <c r="C18" s="1" t="n">
+        <f aca="false">F18*G18</f>
         <v>1312</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -1375,18 +1204,18 @@
       <c r="E18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="1" t="n">
         <v>164</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="1" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="13" hidden="1">
-      <c r="A19" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="19">
+      <c r="A19" s="2" t="n">
         <v>43141</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="1" t="n">
         <v>1190</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1396,11 +1225,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="13" hidden="1">
-      <c r="A20" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="20">
+      <c r="A20" s="2" t="n">
         <v>43154</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="1" t="n">
         <v>438</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1410,11 +1239,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="13" hidden="1">
-      <c r="A21" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="21">
+      <c r="A21" s="2" t="n">
         <v>43154</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="1" t="n">
         <v>248</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -1424,22 +1253,22 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="13" hidden="1">
-      <c r="A22" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="22">
+      <c r="A22" s="2" t="n">
         <v>43166</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="1" t="n">
         <v>234</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="13" hidden="1">
-      <c r="A23" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="23">
+      <c r="A23" s="2" t="n">
         <v>43171</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="1" t="n">
         <v>118</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1449,22 +1278,22 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="13" hidden="1">
-      <c r="A24" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="24">
+      <c r="A24" s="2" t="n">
         <v>43173</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="1" t="n">
         <v>82</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="13" hidden="1">
-      <c r="A25" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="25">
+      <c r="A25" s="2" t="n">
         <v>43174</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1474,22 +1303,22 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="13" hidden="1">
-      <c r="A26" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="26">
+      <c r="A26" s="2" t="n">
         <v>43175</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="1" t="n">
         <v>370</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="13" hidden="1">
-      <c r="A27" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="27">
+      <c r="A27" s="2" t="n">
         <v>43175</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -1499,11 +1328,11 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="13" hidden="1">
-      <c r="A28" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="28">
+      <c r="A28" s="2" t="n">
         <v>43176</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="1" t="n">
         <v>624</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -1513,11 +1342,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="13" hidden="1">
-      <c r="A29" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="29">
+      <c r="A29" s="2" t="n">
         <v>43177</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="1" t="n">
         <v>170</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1527,22 +1356,22 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="13" hidden="1">
-      <c r="A30" s="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="30">
+      <c r="A30" s="4" t="n">
         <v>43179</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="13" hidden="1">
-      <c r="A31" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="31">
+      <c r="A31" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="1" t="n">
         <v>90</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -1552,11 +1381,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="13" hidden="1">
-      <c r="A32" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="32">
+      <c r="A32" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="1" t="n">
         <v>72</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -1566,11 +1395,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:26" ht="13" hidden="1">
-      <c r="A33" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="33">
+      <c r="A33" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="1" t="n">
         <v>908</v>
       </c>
       <c r="D33" s="6" t="s">
@@ -1580,11 +1409,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:26" ht="13" hidden="1">
-      <c r="A34" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="34">
+      <c r="A34" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -1594,11 +1423,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:26" ht="13" hidden="1">
-      <c r="A35" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="35">
+      <c r="A35" s="2" t="n">
         <v>43181</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -1608,11 +1437,11 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:26" ht="13" hidden="1">
-      <c r="A36" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="36">
+      <c r="A36" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="1" t="n">
         <v>135</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -1622,47 +1451,47 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:26" ht="13" hidden="1">
-      <c r="A37" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="37">
+      <c r="A37" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="B37" s="8">
+      <c r="B37" s="1" t="n">
         <v>110</v>
       </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="8" t="s">
+      <c r="C37" s="1"/>
+      <c r="D37" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="E37" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
-      <c r="J37" s="9"/>
-      <c r="K37" s="9"/>
-      <c r="L37" s="9"/>
-      <c r="M37" s="9"/>
-      <c r="N37" s="9"/>
-      <c r="O37" s="9"/>
-      <c r="P37" s="9"/>
-      <c r="Q37" s="9"/>
-      <c r="R37" s="9"/>
-      <c r="S37" s="9"/>
-      <c r="T37" s="9"/>
-      <c r="U37" s="9"/>
-      <c r="V37" s="9"/>
-      <c r="W37" s="9"/>
-      <c r="X37" s="9"/>
-      <c r="Y37" s="9"/>
-      <c r="Z37" s="9"/>
-    </row>
-    <row r="38" spans="1:26" ht="13" hidden="1">
-      <c r="A38" s="7">
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+      <c r="S37" s="1"/>
+      <c r="T37" s="1"/>
+      <c r="U37" s="1"/>
+      <c r="V37" s="1"/>
+      <c r="W37" s="1"/>
+      <c r="X37" s="1"/>
+      <c r="Y37" s="1"/>
+      <c r="Z37" s="1"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="38">
+      <c r="A38" s="2" t="n">
         <v>43185</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="1" t="n">
         <v>122</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -1672,22 +1501,22 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:26" ht="13" hidden="1">
-      <c r="A39" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="39">
+      <c r="A39" s="2" t="n">
         <v>43187</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="1" t="n">
         <v>750</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:26" ht="13" hidden="1">
-      <c r="A40" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="40">
+      <c r="A40" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="1" t="n">
         <v>379</v>
       </c>
       <c r="D40" s="6" t="s">
@@ -1697,22 +1526,22 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:26" ht="13" hidden="1">
-      <c r="A41" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="41">
+      <c r="A41" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="1" t="n">
         <v>240</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:26" ht="13" hidden="1">
-      <c r="A42" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="42">
+      <c r="A42" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="1" t="n">
         <v>540</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -1722,11 +1551,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:26" ht="13" hidden="1">
-      <c r="A43" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="43">
+      <c r="A43" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -1736,11 +1565,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:26" ht="13" hidden="1">
-      <c r="A44" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="44">
+      <c r="A44" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -1750,11 +1579,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:26" ht="13" hidden="1">
-      <c r="A45" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="45">
+      <c r="A45" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="1" t="n">
         <v>462</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -1764,11 +1593,11 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:26" ht="13" hidden="1">
-      <c r="A46" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="46">
+      <c r="A46" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46" s="1" t="n">
         <v>70</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -1778,11 +1607,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:26" ht="13" hidden="1">
-      <c r="A47" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="47">
+      <c r="A47" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -1792,11 +1621,11 @@
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="1:26" ht="13" hidden="1">
-      <c r="A48" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="48">
+      <c r="A48" s="2" t="n">
         <v>43190</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="1" t="n">
         <v>30</v>
       </c>
       <c r="C48" s="1"/>
@@ -1807,11 +1636,11 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="13" hidden="1">
-      <c r="A49" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="49">
+      <c r="A49" s="2" t="n">
         <v>43191</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="1" t="n">
         <v>40</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -1821,11 +1650,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="13" hidden="1">
-      <c r="A50" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="50">
+      <c r="A50" s="7" t="n">
         <v>43193</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50" s="1" t="n">
         <v>150</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -1835,11 +1664,11 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="13" hidden="1">
-      <c r="A51" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="51">
+      <c r="A51" s="2" t="n">
         <v>43194</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51" s="1" t="n">
         <v>1360</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -1849,11 +1678,11 @@
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="13" hidden="1">
-      <c r="A52" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="52">
+      <c r="A52" s="2" t="n">
         <v>43195</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" s="1" t="n">
         <v>94</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -1863,11 +1692,11 @@
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="13" hidden="1">
-      <c r="A53" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="53">
+      <c r="A53" s="2" t="n">
         <v>43196</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C53" s="1" t="n">
         <v>48</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -1877,11 +1706,11 @@
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="13" hidden="1">
-      <c r="A54" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="54">
+      <c r="A54" s="2" t="n">
         <v>43196</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C54" s="1" t="n">
         <v>205</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -1891,11 +1720,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="13" hidden="1">
-      <c r="A55" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="55">
+      <c r="A55" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -1905,11 +1734,11 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="13" hidden="1">
-      <c r="A56" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="56">
+      <c r="A56" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56" s="1" t="n">
         <v>421</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -1919,11 +1748,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="13" hidden="1">
-      <c r="A57" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="57">
+      <c r="A57" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="1" t="n">
         <v>191</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -1933,11 +1762,11 @@
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="13" hidden="1">
-      <c r="A58" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="58">
+      <c r="A58" s="2" t="n">
         <v>43198</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58" s="1" t="n">
         <v>226</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -1947,22 +1776,22 @@
         <v>96</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="13" hidden="1">
-      <c r="A59" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="59">
+      <c r="A59" s="2" t="n">
         <v>43200</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59" s="1" t="n">
         <v>250</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="13" hidden="1">
-      <c r="A60" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="60">
+      <c r="A60" s="2" t="n">
         <v>43200</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60" s="1" t="n">
         <v>1115</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -1972,11 +1801,11 @@
         <v>99</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="13" hidden="1">
-      <c r="A61" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="61">
+      <c r="A61" s="2" t="n">
         <v>43201</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -1986,11 +1815,11 @@
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="13" hidden="1">
-      <c r="A62" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="62">
+      <c r="A62" s="2" t="n">
         <v>43201</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62" s="1" t="n">
         <v>88</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -2000,11 +1829,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="13" hidden="1">
-      <c r="A63" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="63">
+      <c r="A63" s="2" t="n">
         <v>43203</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -2014,11 +1843,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="13" hidden="1">
-      <c r="A64" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="64">
+      <c r="A64" s="2" t="n">
         <v>43203</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C64" s="1" t="n">
         <v>364</v>
       </c>
       <c r="D64" s="1" t="s">
@@ -2028,11 +1857,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="13" hidden="1">
-      <c r="A65" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="65">
+      <c r="A65" s="2" t="n">
         <v>43204</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65" s="1" t="n">
         <v>65</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -2042,11 +1871,11 @@
         <v>105</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="13" hidden="1">
-      <c r="A66" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="66">
+      <c r="A66" s="2" t="n">
         <v>43208</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -2056,11 +1885,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="13" hidden="1">
-      <c r="A67" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="67">
+      <c r="A67" s="2" t="n">
         <v>43208</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C67" s="1" t="n">
         <v>470</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -2070,11 +1899,11 @@
         <v>107</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="13" hidden="1">
-      <c r="A68" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="68">
+      <c r="A68" s="2" t="n">
         <v>43209</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68" s="1" t="n">
         <v>180</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -2084,11 +1913,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="13" hidden="1">
-      <c r="A69" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="69">
+      <c r="A69" s="2" t="n">
         <v>43210</v>
       </c>
-      <c r="C69" s="1">
+      <c r="C69" s="1" t="n">
         <v>420</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -2098,11 +1927,11 @@
         <v>109</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="13" hidden="1">
-      <c r="A70" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="70">
+      <c r="A70" s="2" t="n">
         <v>43212</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70" s="1" t="n">
         <v>50</v>
       </c>
       <c r="D70" s="1" t="s">
@@ -2112,11 +1941,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="13" hidden="1">
-      <c r="A71" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="71">
+      <c r="A71" s="2" t="n">
         <v>43212</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71" s="1" t="n">
         <v>164</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -2126,11 +1955,11 @@
         <v>112</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="13" hidden="1">
-      <c r="A72" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="72">
+      <c r="A72" s="2" t="n">
         <v>43215</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B72" s="1" t="n">
         <v>300</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -2140,11 +1969,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="13" hidden="1">
-      <c r="A73" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="73">
+      <c r="A73" s="2" t="n">
         <v>43217</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73" s="1" t="n">
         <v>364</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -2154,11 +1983,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="13" hidden="1">
-      <c r="A74" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="74">
+      <c r="A74" s="2" t="n">
         <v>43218</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74" s="1" t="n">
         <v>185</v>
       </c>
       <c r="D74" s="1" t="s">
@@ -2168,11 +1997,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="13" hidden="1">
-      <c r="A75" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="75">
+      <c r="A75" s="2" t="n">
         <v>43218</v>
       </c>
-      <c r="C75" s="1">
+      <c r="C75" s="1" t="n">
         <v>404</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -2182,11 +2011,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="13" hidden="1">
-      <c r="A76" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="76">
+      <c r="A76" s="2" t="n">
         <v>43220</v>
       </c>
-      <c r="C76" s="1">
+      <c r="C76" s="1" t="n">
         <v>57</v>
       </c>
       <c r="D76" s="1" t="s">
@@ -2196,11 +2025,11 @@
         <v>114</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="13" hidden="1">
-      <c r="A77" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="77">
+      <c r="A77" s="2" t="n">
         <v>43221</v>
       </c>
-      <c r="C77" s="1">
+      <c r="C77" s="1" t="n">
         <v>282</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -2210,11 +2039,11 @@
         <v>116</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="13" hidden="1">
-      <c r="A78" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="78">
+      <c r="A78" s="2" t="n">
         <v>43220</v>
       </c>
-      <c r="C78" s="1">
+      <c r="C78" s="1" t="n">
         <v>87</v>
       </c>
       <c r="D78" s="1" t="s">
@@ -2224,11 +2053,11 @@
         <v>117</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="13" hidden="1">
-      <c r="A79" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="79">
+      <c r="A79" s="2" t="n">
         <v>43223</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B79" s="1" t="n">
         <v>1878</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -2238,11 +2067,11 @@
         <v>119</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="13" hidden="1">
-      <c r="A80" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="80">
+      <c r="A80" s="2" t="n">
         <v>43224</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B80" s="1" t="n">
         <v>98</v>
       </c>
       <c r="D80" s="1" t="s">
@@ -2252,11 +2081,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="13" hidden="1">
-      <c r="A81" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="81">
+      <c r="A81" s="2" t="n">
         <v>43225</v>
       </c>
-      <c r="C81" s="1">
+      <c r="C81" s="1" t="n">
         <v>198</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -2266,11 +2095,11 @@
         <v>122</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="13" hidden="1">
-      <c r="A82" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="82">
+      <c r="A82" s="2" t="n">
         <v>43225</v>
       </c>
-      <c r="C82" s="1">
+      <c r="C82" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -2280,11 +2109,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="13" hidden="1">
-      <c r="A83" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="83">
+      <c r="A83" s="2" t="n">
         <v>43228</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83" s="1" t="n">
         <v>168</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -2294,11 +2123,11 @@
         <v>124</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="13" hidden="1">
-      <c r="A84" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="84">
+      <c r="A84" s="2" t="n">
         <v>43229</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B84" s="1" t="n">
         <v>240</v>
       </c>
       <c r="D84" s="1" t="s">
@@ -2308,12 +2137,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="13" hidden="1">
-      <c r="A85" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="85">
+      <c r="A85" s="2" t="n">
         <v>43230</v>
       </c>
       <c r="B85" s="1"/>
-      <c r="C85" s="1">
+      <c r="C85" s="1" t="n">
         <v>420</v>
       </c>
       <c r="D85" s="1" t="s">
@@ -2323,11 +2152,11 @@
         <v>126</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="13" hidden="1">
-      <c r="A86" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="86">
+      <c r="A86" s="2" t="n">
         <v>43230</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B86" s="1" t="n">
         <v>200</v>
       </c>
       <c r="C86" s="1"/>
@@ -2338,11 +2167,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="13" hidden="1">
-      <c r="A87" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="87">
+      <c r="A87" s="2" t="n">
         <v>43230</v>
       </c>
-      <c r="C87" s="1">
+      <c r="C87" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D87" s="1" t="s">
@@ -2352,11 +2181,11 @@
         <v>128</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="13" hidden="1">
-      <c r="A88" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="88">
+      <c r="A88" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B88" s="1" t="n">
         <v>462</v>
       </c>
       <c r="D88" s="1" t="s">
@@ -2366,11 +2195,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="13" hidden="1">
-      <c r="A89" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="89">
+      <c r="A89" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B89" s="1" t="n">
         <v>499</v>
       </c>
       <c r="D89" s="1" t="s">
@@ -2380,11 +2209,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="13" hidden="1">
-      <c r="A90" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="90">
+      <c r="A90" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B90" s="1">
+      <c r="B90" s="1" t="n">
         <v>398</v>
       </c>
       <c r="D90" s="1" t="s">
@@ -2394,11 +2223,11 @@
         <v>133</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="13" hidden="1">
-      <c r="A91" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="91">
+      <c r="A91" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B91" s="1">
+      <c r="B91" s="1" t="n">
         <v>226</v>
       </c>
       <c r="D91" s="1" t="s">
@@ -2408,11 +2237,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="13" hidden="1">
-      <c r="A92" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="92">
+      <c r="A92" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B92" s="1">
+      <c r="B92" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D92" s="1" t="s">
@@ -2422,11 +2251,11 @@
         <v>137</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="13" hidden="1">
-      <c r="A93" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="93">
+      <c r="A93" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="B93" s="1">
+      <c r="B93" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D93" s="1" t="s">
@@ -2436,11 +2265,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="13" hidden="1">
-      <c r="A94" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="94">
+      <c r="A94" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="C94" s="1">
+      <c r="C94" s="1" t="n">
         <v>340</v>
       </c>
       <c r="D94" s="1" t="s">
@@ -2450,11 +2279,11 @@
         <v>139</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="13" hidden="1">
-      <c r="A95" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="95">
+      <c r="A95" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="B95" s="1">
+      <c r="B95" s="1" t="n">
         <v>510</v>
       </c>
       <c r="D95" s="1" t="s">
@@ -2464,11 +2293,11 @@
         <v>141</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="13" hidden="1">
-      <c r="A96" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="96">
+      <c r="A96" s="2" t="n">
         <v>43233</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B96" s="1" t="n">
         <v>170</v>
       </c>
       <c r="D96" s="1" t="s">
@@ -2478,11 +2307,11 @@
         <v>143</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="13" hidden="1">
-      <c r="A97" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="97">
+      <c r="A97" s="2" t="n">
         <v>43233</v>
       </c>
-      <c r="C97" s="1">
+      <c r="C97" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D97" s="1" t="s">
@@ -2492,11 +2321,11 @@
         <v>144</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="13" hidden="1">
-      <c r="A98" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="98">
+      <c r="A98" s="2" t="n">
         <v>43234</v>
       </c>
-      <c r="C98" s="1">
+      <c r="C98" s="1" t="n">
         <v>299</v>
       </c>
       <c r="D98" s="1" t="s">
@@ -2506,11 +2335,11 @@
         <v>145</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="13" hidden="1">
-      <c r="A99" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="99">
+      <c r="A99" s="2" t="n">
         <v>43236</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99" s="1" t="n">
         <v>3659</v>
       </c>
       <c r="D99" s="1" t="s">
@@ -2520,11 +2349,11 @@
         <v>146</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="13" hidden="1">
-      <c r="A100" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="100">
+      <c r="A100" s="2" t="n">
         <v>43237</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B100" s="1" t="n">
         <v>79</v>
       </c>
       <c r="D100" s="1" t="s">
@@ -2534,11 +2363,11 @@
         <v>147</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="13" hidden="1">
-      <c r="A101" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="101">
+      <c r="A101" s="2" t="n">
         <v>43236</v>
       </c>
-      <c r="C101" s="1">
+      <c r="C101" s="1" t="n">
         <v>173</v>
       </c>
       <c r="D101" s="1" t="s">
@@ -2548,11 +2377,11 @@
         <v>148</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="13" hidden="1">
-      <c r="A102" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="102">
+      <c r="A102" s="2" t="n">
         <v>43240</v>
       </c>
-      <c r="B102" s="1">
+      <c r="B102" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D102" s="1" t="s">
@@ -2562,22 +2391,22 @@
         <v>149</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="13" hidden="1">
-      <c r="A103" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="103">
+      <c r="A103" s="2" t="n">
         <v>43240</v>
       </c>
-      <c r="B103" s="1">
+      <c r="B103" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="13" hidden="1">
-      <c r="A104" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="104">
+      <c r="A104" s="2" t="n">
         <v>43241</v>
       </c>
-      <c r="B104" s="1">
+      <c r="B104" s="1" t="n">
         <v>4070</v>
       </c>
       <c r="D104" s="1" t="s">
@@ -2587,11 +2416,11 @@
         <v>150</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="13" hidden="1">
-      <c r="A105" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="105">
+      <c r="A105" s="2" t="n">
         <v>43241</v>
       </c>
-      <c r="C105" s="1">
+      <c r="C105" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D105" s="1" t="s">
@@ -2601,11 +2430,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="13" hidden="1">
-      <c r="A106" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="106">
+      <c r="A106" s="2" t="n">
         <v>43242</v>
       </c>
-      <c r="B106" s="1">
+      <c r="B106" s="1" t="n">
         <v>79</v>
       </c>
       <c r="D106" s="1" t="s">
@@ -2615,11 +2444,11 @@
         <v>152</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="13" hidden="1">
-      <c r="A107" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="107">
+      <c r="A107" s="2" t="n">
         <v>43246</v>
       </c>
-      <c r="B107" s="1">
+      <c r="B107" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D107" s="1" t="s">
@@ -2629,11 +2458,11 @@
         <v>154</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="13" hidden="1">
-      <c r="A108" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="108">
+      <c r="A108" s="2" t="n">
         <v>43247</v>
       </c>
-      <c r="B108" s="1">
+      <c r="B108" s="1" t="n">
         <v>70</v>
       </c>
       <c r="D108" s="1" t="s">
@@ -2643,44 +2472,44 @@
         <v>156</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="13" hidden="1">
-      <c r="A109" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="109">
+      <c r="A109" s="2" t="n">
         <v>43253</v>
       </c>
-      <c r="B109" s="1">
+      <c r="B109" s="1" t="n">
         <v>142</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="13" hidden="1">
-      <c r="A110" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="110">
+      <c r="A110" s="2" t="n">
         <v>43254</v>
       </c>
-      <c r="B110" s="1">
+      <c r="B110" s="1" t="n">
         <v>90</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="13" hidden="1">
-      <c r="A111" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="111">
+      <c r="A111" s="2" t="n">
         <v>43260</v>
       </c>
-      <c r="C111" s="1">
+      <c r="C111" s="1" t="n">
         <v>1400</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="13" hidden="1">
-      <c r="A112" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="112">
+      <c r="A112" s="2" t="n">
         <v>43260</v>
       </c>
-      <c r="C112" s="1">
+      <c r="C112" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D112" s="1" t="s">
@@ -2690,33 +2519,33 @@
         <v>91</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="13" hidden="1">
-      <c r="A113" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="113">
+      <c r="A113" s="2" t="n">
         <v>43264</v>
       </c>
-      <c r="B113" s="1">
+      <c r="B113" s="1" t="n">
         <v>546</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="13" hidden="1">
-      <c r="A114" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="114">
+      <c r="A114" s="2" t="n">
         <v>43264</v>
       </c>
-      <c r="B114" s="1">
+      <c r="B114" s="1" t="n">
         <v>95</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="13" hidden="1">
-      <c r="A115" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="115">
+      <c r="A115" s="2" t="n">
         <v>43266</v>
       </c>
-      <c r="B115" s="1">
+      <c r="B115" s="1" t="n">
         <v>394</v>
       </c>
       <c r="D115" s="1" t="s">
@@ -2726,11 +2555,11 @@
         <v>163</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="13" hidden="1">
-      <c r="A116" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="116">
+      <c r="A116" s="2" t="n">
         <v>43266</v>
       </c>
-      <c r="B116" s="1">
+      <c r="B116" s="1" t="n">
         <v>1055</v>
       </c>
       <c r="D116" s="1" t="s">
@@ -2740,11 +2569,11 @@
         <v>165</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="13" hidden="1">
-      <c r="A117" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="117">
+      <c r="A117" s="2" t="n">
         <v>43284</v>
       </c>
-      <c r="C117" s="1">
+      <c r="C117" s="1" t="n">
         <v>274</v>
       </c>
       <c r="D117" s="1" t="s">
@@ -2754,11 +2583,11 @@
         <v>167</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="13" hidden="1">
-      <c r="A118" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="118">
+      <c r="A118" s="2" t="n">
         <v>43283</v>
       </c>
-      <c r="C118" s="1">
+      <c r="C118" s="1" t="n">
         <v>105</v>
       </c>
       <c r="D118" s="1" t="s">
@@ -2768,11 +2597,11 @@
         <v>169</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="13" hidden="1">
-      <c r="A119" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="119">
+      <c r="A119" s="2" t="n">
         <v>43289</v>
       </c>
-      <c r="C119" s="1">
+      <c r="C119" s="1" t="n">
         <v>128</v>
       </c>
       <c r="D119" s="1" t="s">
@@ -2782,11 +2611,11 @@
         <v>171</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="13" hidden="1">
-      <c r="A120" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="120">
+      <c r="A120" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C120" s="1">
+      <c r="C120" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D120" s="1" t="s">
@@ -2796,11 +2625,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="13" hidden="1">
-      <c r="A121" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="121">
+      <c r="A121" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C121" s="1">
+      <c r="C121" s="1" t="n">
         <v>210</v>
       </c>
       <c r="D121" s="1" t="s">
@@ -2810,44 +2639,44 @@
         <v>173</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="13" hidden="1">
-      <c r="A122" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="122">
+      <c r="A122" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B122" s="1">
+      <c r="B122" s="1" t="n">
         <v>980</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="13" hidden="1">
-      <c r="A123" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="123">
+      <c r="A123" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B123" s="1">
+      <c r="B123" s="1" t="n">
         <v>1260</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="13" hidden="1">
-      <c r="A124" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="124">
+      <c r="A124" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B124" s="1">
+      <c r="B124" s="1" t="n">
         <v>3687</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="13" hidden="1">
-      <c r="A125" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="125">
+      <c r="A125" s="2" t="n">
         <v>43298</v>
       </c>
-      <c r="C125" s="1">
+      <c r="C125" s="1" t="n">
         <v>60</v>
       </c>
       <c r="D125" s="1" t="s">
@@ -2857,55 +2686,55 @@
         <v>178</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="13" hidden="1">
-      <c r="A126" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="126">
+      <c r="A126" s="2" t="n">
         <v>43291</v>
       </c>
-      <c r="C126" s="1">
+      <c r="C126" s="1" t="n">
         <v>404</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="13" hidden="1">
-      <c r="A127" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="127">
+      <c r="A127" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C127" s="1">
+      <c r="C127" s="1" t="n">
         <v>451</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="13" hidden="1">
-      <c r="A128" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="128">
+      <c r="A128" s="2" t="n">
         <v>43298</v>
       </c>
-      <c r="C128" s="1">
+      <c r="C128" s="1" t="n">
         <v>708</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="13" hidden="1">
-      <c r="A129" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="129">
+      <c r="A129" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C129" s="1">
+      <c r="C129" s="1" t="n">
         <v>160</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="13" hidden="1">
-      <c r="A130" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="130">
+      <c r="A130" s="2" t="n">
         <v>43288</v>
       </c>
-      <c r="C130" s="1">
+      <c r="C130" s="1" t="n">
         <v>72</v>
       </c>
       <c r="D130" s="1" t="s">
@@ -2915,11 +2744,11 @@
         <v>181</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="13" hidden="1">
-      <c r="A131" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="131">
+      <c r="A131" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C131" s="1">
+      <c r="C131" s="1" t="n">
         <v>300</v>
       </c>
       <c r="D131" s="1" t="s">
@@ -2929,11 +2758,11 @@
         <v>183</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="13" hidden="1">
-      <c r="A132" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="132">
+      <c r="A132" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C132" s="1">
+      <c r="C132" s="1" t="n">
         <v>230</v>
       </c>
       <c r="D132" s="1" t="s">
@@ -2943,22 +2772,22 @@
         <v>185</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="13" hidden="1">
-      <c r="A133" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="133">
+      <c r="A133" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C133" s="1">
+      <c r="C133" s="1" t="n">
         <v>454</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="13" hidden="1">
-      <c r="A134" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="134">
+      <c r="A134" s="2" t="n">
         <v>43299</v>
       </c>
-      <c r="C134" s="1">
+      <c r="C134" s="1" t="n">
         <v>686</v>
       </c>
       <c r="D134" s="1" t="s">
@@ -2968,11 +2797,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="13" hidden="1">
-      <c r="A135" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="135">
+      <c r="A135" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C135" s="1">
+      <c r="C135" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D135" s="1" t="s">
@@ -2982,11 +2811,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="13" hidden="1">
-      <c r="A136" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="136">
+      <c r="A136" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C136" s="1">
+      <c r="C136" s="1" t="n">
         <v>2067</v>
       </c>
       <c r="D136" s="1" t="s">
@@ -2996,11 +2825,11 @@
         <v>186</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="13" hidden="1">
-      <c r="A137" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="137">
+      <c r="A137" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B137" s="1">
+      <c r="B137" s="1" t="n">
         <v>109</v>
       </c>
       <c r="D137" s="1" t="s">
@@ -3010,11 +2839,11 @@
         <v>187</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="13" hidden="1">
-      <c r="A138" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="138">
+      <c r="A138" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B138" s="1">
+      <c r="B138" s="1" t="n">
         <v>97</v>
       </c>
       <c r="D138" s="1" t="s">
@@ -3024,11 +2853,11 @@
         <v>188</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="13" hidden="1">
-      <c r="A139" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="139">
+      <c r="A139" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B139" s="1">
+      <c r="B139" s="1" t="n">
         <v>1437</v>
       </c>
       <c r="D139" s="1" t="s">
@@ -3038,11 +2867,11 @@
         <v>189</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="13" hidden="1">
-      <c r="A140" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="140">
+      <c r="A140" s="2" t="n">
         <v>43306</v>
       </c>
-      <c r="C140" s="1">
+      <c r="C140" s="1" t="n">
         <v>650</v>
       </c>
       <c r="D140" s="1" t="s">
@@ -3052,11 +2881,11 @@
         <v>190</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="13" hidden="1">
-      <c r="A141" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="141">
+      <c r="A141" s="2" t="n">
         <v>43305</v>
       </c>
-      <c r="C141" s="1">
+      <c r="C141" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D141" s="1" t="s">
@@ -3066,11 +2895,11 @@
         <v>191</v>
       </c>
     </row>
-    <row r="142" spans="1:5" ht="13" hidden="1">
-      <c r="A142" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="142">
+      <c r="A142" s="2" t="n">
         <v>43309</v>
       </c>
-      <c r="C142" s="1">
+      <c r="C142" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D142" s="1" t="s">
@@ -3080,39 +2909,39 @@
         <v>192</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="14" hidden="1">
-      <c r="A143" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="0" r="143">
+      <c r="A143" s="2" t="n">
         <v>43306</v>
       </c>
-      <c r="B143" s="1">
+      <c r="B143" s="1" t="n">
         <v>167</v>
       </c>
       <c r="D143" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E143" s="11" t="s">
+      <c r="E143" s="8" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="14" hidden="1">
-      <c r="A144" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="0" r="144">
+      <c r="A144" s="2" t="n">
         <v>43304</v>
       </c>
-      <c r="C144" s="1">
+      <c r="C144" s="1" t="n">
         <v>93</v>
       </c>
       <c r="D144" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E144" s="12" t="s">
+      <c r="E144" s="9" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="13" hidden="1">
-      <c r="A145" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="145">
+      <c r="A145" s="2" t="n">
         <v>43305</v>
       </c>
-      <c r="C145" s="1">
+      <c r="C145" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D145" s="1" t="s">
@@ -3122,11 +2951,11 @@
         <v>195</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="13" hidden="1">
-      <c r="A146" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="146">
+      <c r="A146" s="2" t="n">
         <v>43303</v>
       </c>
-      <c r="C146" s="1">
+      <c r="C146" s="1" t="n">
         <v>244</v>
       </c>
       <c r="D146" s="1" t="s">
@@ -3136,11 +2965,11 @@
         <v>196</v>
       </c>
     </row>
-    <row r="147" spans="1:5" ht="13" hidden="1">
-      <c r="A147" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="147">
+      <c r="A147" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C147" s="1">
+      <c r="C147" s="1" t="n">
         <v>482</v>
       </c>
       <c r="D147" s="1" t="s">
@@ -3150,11 +2979,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="148" spans="1:5" ht="13" hidden="1">
-      <c r="A148" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="148">
+      <c r="A148" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C148" s="1">
+      <c r="C148" s="1" t="n">
         <v>172</v>
       </c>
       <c r="D148" s="1" t="s">
@@ -3164,44 +2993,44 @@
         <v>199</v>
       </c>
     </row>
-    <row r="149" spans="1:5" ht="13" hidden="1">
-      <c r="A149" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="149">
+      <c r="A149" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="B149" s="1">
+      <c r="B149" s="1" t="n">
         <v>89</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="150" spans="1:5" ht="13" hidden="1">
-      <c r="A150" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="150">
+      <c r="A150" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="C150" s="1">
+      <c r="C150" s="1" t="n">
         <v>107</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="151" spans="1:5" ht="13" hidden="1">
-      <c r="A151" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="151">
+      <c r="A151" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="C151" s="1">
+      <c r="C151" s="1" t="n">
         <v>124</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="152" spans="1:5" ht="13" hidden="1">
-      <c r="A152" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="152">
+      <c r="A152" s="7" t="n">
         <v>43316</v>
       </c>
-      <c r="C152" s="1">
+      <c r="C152" s="1" t="n">
         <v>4500</v>
       </c>
       <c r="D152" s="1" t="s">
@@ -3211,11 +3040,11 @@
         <v>202</v>
       </c>
     </row>
-    <row r="153" spans="1:5" ht="13" hidden="1">
-      <c r="A153" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="153">
+      <c r="A153" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C153" s="1">
+      <c r="C153" s="1" t="n">
         <v>247</v>
       </c>
       <c r="D153" s="1" t="s">
@@ -3225,11 +3054,11 @@
         <v>204</v>
       </c>
     </row>
-    <row r="154" spans="1:5" ht="13" hidden="1">
-      <c r="A154" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="154">
+      <c r="A154" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C154" s="1">
+      <c r="C154" s="1" t="n">
         <v>1150</v>
       </c>
       <c r="D154" s="1" t="s">
@@ -3239,11 +3068,11 @@
         <v>205</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="13" hidden="1">
-      <c r="A155" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="155">
+      <c r="A155" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C155" s="1">
+      <c r="C155" s="1" t="n">
         <v>313</v>
       </c>
       <c r="D155" s="1" t="s">
@@ -3253,11 +3082,11 @@
         <v>207</v>
       </c>
     </row>
-    <row r="156" spans="1:5" ht="13" hidden="1">
-      <c r="A156" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="156">
+      <c r="A156" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="B156" s="1">
+      <c r="B156" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D156" s="1" t="s">
@@ -3267,11 +3096,11 @@
         <v>209</v>
       </c>
     </row>
-    <row r="157" spans="1:5" ht="13" hidden="1">
-      <c r="A157" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="157">
+      <c r="A157" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="C157" s="1">
+      <c r="C157" s="1" t="n">
         <v>710</v>
       </c>
       <c r="D157" s="1" t="s">
@@ -3281,11 +3110,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="158" spans="1:5" ht="13">
-      <c r="A158" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="158">
+      <c r="A158" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="C158" s="1">
+      <c r="C158" s="1" t="n">
         <v>100</v>
       </c>
       <c r="D158" s="1" t="s">
@@ -3295,11 +3124,11 @@
         <v>212</v>
       </c>
     </row>
-    <row r="159" spans="1:5" ht="13">
-      <c r="A159" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="159">
+      <c r="A159" s="2" t="n">
         <v>43319</v>
       </c>
-      <c r="B159" s="1">
+      <c r="B159" s="1" t="n">
         <v>78</v>
       </c>
       <c r="D159" s="1" t="s">
@@ -3309,22 +3138,22 @@
         <v>213</v>
       </c>
     </row>
-    <row r="160" spans="1:5" ht="13">
-      <c r="A160" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="160">
+      <c r="A160" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="B160" s="1">
+      <c r="B160" s="1" t="n">
         <v>1840</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="161" spans="1:5" ht="13">
-      <c r="A161" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="161">
+      <c r="A161" s="2" t="n">
         <v>43322</v>
       </c>
-      <c r="B161" s="1">
+      <c r="B161" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D161" s="1" t="s">
@@ -3334,11 +3163,11 @@
         <v>216</v>
       </c>
     </row>
-    <row r="162" spans="1:5" ht="13">
-      <c r="A162" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="162">
+      <c r="A162" s="7" t="n">
         <v>43324</v>
       </c>
-      <c r="C162" s="1">
+      <c r="C162" s="1" t="n">
         <v>230</v>
       </c>
       <c r="D162" s="1" t="s">
@@ -3348,11 +3177,11 @@
         <v>217</v>
       </c>
     </row>
-    <row r="163" spans="1:5" ht="13">
-      <c r="A163" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="163">
+      <c r="A163" s="7" t="n">
         <v>43326</v>
       </c>
-      <c r="C163" s="1">
+      <c r="C163" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D163" s="1" t="s">
@@ -3362,11 +3191,11 @@
         <v>219</v>
       </c>
     </row>
-    <row r="164" spans="1:5" ht="13">
-      <c r="A164" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="164">
+      <c r="A164" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="B164" s="1">
+      <c r="B164" s="1" t="n">
         <v>45</v>
       </c>
       <c r="D164" s="1" t="s">
@@ -3376,37 +3205,71 @@
         <v>221</v>
       </c>
     </row>
-    <row r="165" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A165" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="165">
+      <c r="A165" s="7" t="n">
         <v>43326</v>
       </c>
-      <c r="C165">
+      <c r="C165" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="D165" s="9" t="s">
+      <c r="D165" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="175" spans="1:5" ht="13">
-      <c r="B175">
-        <f t="shared" ref="B175:C175" si="0">SUM(B2:B172)</f>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="166">
+      <c r="A166" s="10" t="n">
+        <v>43327</v>
+      </c>
+      <c r="C166" s="0" t="n">
+        <v>486</v>
+      </c>
+      <c r="D166" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="E166" s="0" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="167">
+      <c r="A167" s="10" t="n">
+        <v>43329</v>
+      </c>
+      <c r="C167" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="D167" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="E167" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="175">
+      <c r="B175" s="0" t="n">
+        <f aca="false">SUM(B2:B172)</f>
         <v>38181</v>
       </c>
-      <c r="C175">
-        <f t="shared" si="0"/>
-        <v>35406</v>
+      <c r="C175" s="0" t="n">
+        <f aca="false">SUM(C2:C172)</f>
+        <v>35984</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A30:Z32">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+    <cfRule aboveAverage="0" bottom="0" dxfId="0" operator="expression" percent="0" priority="2" rank="0" text="" type="expression">
       <formula>LEN(TRIM(A30))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D33" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D40" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink display="netonnet.se" ref="D33" r:id="rId1"/>
+    <hyperlink display="www.vidaxl.se" ref="D40" r:id="rId2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
cost update 0903 jenny
</commit_message>
<xml_diff>
--- a/Cost.xlsx
+++ b/Cost.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chengkaiyan/github/cost/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB534AB-9638-3840-B785-C78A41B4B8D2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="238">
   <si>
     <t>日期</t>
   </si>
@@ -725,41 +720,66 @@
   </si>
   <si>
     <t>安联保险</t>
+  </si>
+  <si>
+    <t>st1 coop taby</t>
+  </si>
+  <si>
+    <t>pork; milk powder etc</t>
+  </si>
+  <si>
+    <t>vegetables; hairspray; etc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="yyyy/m/d"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt formatCode="YYYY/M/D" numFmtId="165"/>
+    <numFmt formatCode="M/D/YYYY" numFmtId="166"/>
+    <numFmt formatCode="YYYY\-MM\-DD" numFmtId="167"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <family val="0"/>
       <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
       <name val="Arial"/>
       <family val="2"/>
+      <sz val="10"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF666666"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF666666"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="5">
@@ -789,7 +809,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
@@ -797,27 +817,88 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="167" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -828,7 +909,6 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -887,339 +967,31 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:Z207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D177" sqref="D177"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A163" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E185" activeCellId="0" pane="topLeft" sqref="E185"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="3" width="14.5"/>
-    <col min="4" max="4" width="26"/>
-    <col min="5" max="5" width="37.83203125"/>
-    <col min="6" max="1025" width="14.5"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="14.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1236,11 +1008,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="2">
+      <c r="A2" s="2" t="n">
         <v>43121</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="1" t="n">
         <v>250</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1250,11 +1022,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="3">
+      <c r="A3" s="2" t="n">
         <v>43122</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="1" t="n">
         <v>305</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1264,11 +1036,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="4">
+      <c r="A4" s="2" t="n">
         <v>43122</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1278,11 +1050,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="5">
+      <c r="A5" s="2" t="n">
         <v>43125</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="1" t="n">
         <v>98</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1292,11 +1064,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="6">
+      <c r="A6" s="2" t="n">
         <v>43126</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1306,11 +1078,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="7">
+      <c r="A7" s="2" t="n">
         <v>43127</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1320,11 +1092,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="8">
+      <c r="A8" s="2" t="n">
         <v>43128</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="1" t="n">
         <v>656</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1334,11 +1106,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="9">
+      <c r="A9" s="2" t="n">
         <v>43131</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="1" t="n">
         <v>486</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1348,11 +1120,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="10">
+      <c r="A10" s="2" t="n">
         <v>43132</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="1" t="n">
         <v>76</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1362,11 +1134,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="11">
+      <c r="A11" s="2" t="n">
         <v>43133</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="1" t="n">
         <v>399</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1376,11 +1148,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="12">
+      <c r="A12" s="2" t="n">
         <v>43135</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="1" t="n">
         <v>419</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1390,11 +1162,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="13">
+      <c r="A13" s="2" t="n">
         <v>43136</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="1" t="n">
         <v>521</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1404,11 +1176,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="14">
+      <c r="A14" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="1" t="n">
         <v>399</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1418,11 +1190,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="15">
+      <c r="A15" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="1" t="n">
         <v>138</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1432,11 +1204,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="16">
+      <c r="A16" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="1" t="n">
         <v>310</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1446,12 +1218,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="17">
+      <c r="A17" s="2" t="n">
         <v>43138</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="1">
+      <c r="C17" s="1" t="n">
         <v>700</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1461,12 +1233,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="18">
+      <c r="A18" s="2" t="n">
         <v>43141</v>
       </c>
-      <c r="C18" s="1">
-        <f>F18*G18</f>
+      <c r="C18" s="1" t="n">
+        <f aca="false">F18*G18</f>
         <v>1312</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -1475,18 +1247,18 @@
       <c r="E18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="1" t="n">
         <v>164</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="1" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="19">
+      <c r="A19" s="2" t="n">
         <v>43141</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="1" t="n">
         <v>1190</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1496,11 +1268,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="20">
+      <c r="A20" s="2" t="n">
         <v>43154</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="1" t="n">
         <v>438</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1510,11 +1282,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="21">
+      <c r="A21" s="2" t="n">
         <v>43154</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="1" t="n">
         <v>248</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -1524,22 +1296,22 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="22">
+      <c r="A22" s="2" t="n">
         <v>43166</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="1" t="n">
         <v>234</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="23">
+      <c r="A23" s="2" t="n">
         <v>43171</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="1" t="n">
         <v>118</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1549,22 +1321,22 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="24">
+      <c r="A24" s="2" t="n">
         <v>43173</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="1" t="n">
         <v>82</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="25">
+      <c r="A25" s="2" t="n">
         <v>43174</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1574,22 +1346,22 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="26">
+      <c r="A26" s="2" t="n">
         <v>43175</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="1" t="n">
         <v>370</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="27">
+      <c r="A27" s="2" t="n">
         <v>43175</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -1599,11 +1371,11 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="28">
+      <c r="A28" s="2" t="n">
         <v>43176</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="1" t="n">
         <v>624</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -1613,11 +1385,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="29">
+      <c r="A29" s="2" t="n">
         <v>43177</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="1" t="n">
         <v>170</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1627,22 +1399,22 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="30">
+      <c r="A30" s="4" t="n">
         <v>43179</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="31">
+      <c r="A31" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="1" t="n">
         <v>90</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -1652,11 +1424,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="32">
+      <c r="A32" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="1" t="n">
         <v>72</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -1666,11 +1438,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="33">
+      <c r="A33" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="1" t="n">
         <v>908</v>
       </c>
       <c r="D33" s="6" t="s">
@@ -1680,11 +1452,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="34">
+      <c r="A34" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -1694,11 +1466,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="35">
+      <c r="A35" s="2" t="n">
         <v>43181</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -1708,11 +1480,11 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="36">
+      <c r="A36" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="1" t="n">
         <v>135</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -1722,11 +1494,11 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="37">
+      <c r="A37" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="1" t="n">
         <v>110</v>
       </c>
       <c r="C37" s="1"/>
@@ -1758,11 +1530,11 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="38">
+      <c r="A38" s="2" t="n">
         <v>43185</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="1" t="n">
         <v>122</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -1772,22 +1544,22 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="39">
+      <c r="A39" s="2" t="n">
         <v>43187</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="1" t="n">
         <v>750</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="40">
+      <c r="A40" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="1" t="n">
         <v>379</v>
       </c>
       <c r="D40" s="6" t="s">
@@ -1797,22 +1569,22 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="41">
+      <c r="A41" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="1" t="n">
         <v>240</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="42">
+      <c r="A42" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="1" t="n">
         <v>540</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -1822,11 +1594,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="43">
+      <c r="A43" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -1836,11 +1608,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="44">
+      <c r="A44" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -1850,11 +1622,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="45">
+      <c r="A45" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="1" t="n">
         <v>462</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -1864,11 +1636,11 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="46">
+      <c r="A46" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46" s="1" t="n">
         <v>70</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -1878,11 +1650,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="47">
+      <c r="A47" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -1892,11 +1664,11 @@
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="48">
+      <c r="A48" s="2" t="n">
         <v>43190</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="1" t="n">
         <v>30</v>
       </c>
       <c r="C48" s="1"/>
@@ -1907,11 +1679,11 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="49">
+      <c r="A49" s="2" t="n">
         <v>43191</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="1" t="n">
         <v>40</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -1921,11 +1693,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="50">
+      <c r="A50" s="7" t="n">
         <v>43193</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50" s="1" t="n">
         <v>150</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -1935,11 +1707,11 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="51">
+      <c r="A51" s="2" t="n">
         <v>43194</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51" s="1" t="n">
         <v>1360</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -1949,11 +1721,11 @@
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="52">
+      <c r="A52" s="2" t="n">
         <v>43195</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" s="1" t="n">
         <v>94</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -1963,11 +1735,11 @@
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="53">
+      <c r="A53" s="2" t="n">
         <v>43196</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C53" s="1" t="n">
         <v>48</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -1977,11 +1749,11 @@
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="54">
+      <c r="A54" s="2" t="n">
         <v>43196</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C54" s="1" t="n">
         <v>205</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -1991,11 +1763,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="55">
+      <c r="A55" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -2005,11 +1777,11 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="56">
+      <c r="A56" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56" s="1" t="n">
         <v>421</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -2019,11 +1791,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="57">
+      <c r="A57" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="1" t="n">
         <v>191</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -2033,11 +1805,11 @@
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="58">
+      <c r="A58" s="2" t="n">
         <v>43198</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58" s="1" t="n">
         <v>226</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -2047,22 +1819,22 @@
         <v>96</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="59">
+      <c r="A59" s="2" t="n">
         <v>43200</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59" s="1" t="n">
         <v>250</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="60">
+      <c r="A60" s="2" t="n">
         <v>43200</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60" s="1" t="n">
         <v>1115</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -2072,11 +1844,11 @@
         <v>99</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="61">
+      <c r="A61" s="2" t="n">
         <v>43201</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -2086,11 +1858,11 @@
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="62">
+      <c r="A62" s="2" t="n">
         <v>43201</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62" s="1" t="n">
         <v>88</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -2100,11 +1872,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="63">
+      <c r="A63" s="2" t="n">
         <v>43203</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -2114,11 +1886,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="64">
+      <c r="A64" s="2" t="n">
         <v>43203</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C64" s="1" t="n">
         <v>364</v>
       </c>
       <c r="D64" s="1" t="s">
@@ -2128,11 +1900,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="65">
+      <c r="A65" s="2" t="n">
         <v>43204</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65" s="1" t="n">
         <v>65</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -2142,11 +1914,11 @@
         <v>105</v>
       </c>
     </row>
-    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="66">
+      <c r="A66" s="2" t="n">
         <v>43208</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -2156,11 +1928,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="67">
+      <c r="A67" s="2" t="n">
         <v>43208</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C67" s="1" t="n">
         <v>470</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -2170,11 +1942,11 @@
         <v>107</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="68">
+      <c r="A68" s="2" t="n">
         <v>43209</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68" s="1" t="n">
         <v>180</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -2184,11 +1956,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A69" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="69">
+      <c r="A69" s="2" t="n">
         <v>43210</v>
       </c>
-      <c r="C69" s="1">
+      <c r="C69" s="1" t="n">
         <v>420</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -2198,11 +1970,11 @@
         <v>109</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="70">
+      <c r="A70" s="2" t="n">
         <v>43212</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70" s="1" t="n">
         <v>50</v>
       </c>
       <c r="D70" s="1" t="s">
@@ -2212,11 +1984,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="71">
+      <c r="A71" s="2" t="n">
         <v>43212</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71" s="1" t="n">
         <v>164</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -2226,11 +1998,11 @@
         <v>112</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="72">
+      <c r="A72" s="2" t="n">
         <v>43215</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B72" s="1" t="n">
         <v>300</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -2240,11 +2012,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="73">
+      <c r="A73" s="2" t="n">
         <v>43217</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73" s="1" t="n">
         <v>364</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -2254,11 +2026,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A74" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="74">
+      <c r="A74" s="2" t="n">
         <v>43218</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74" s="1" t="n">
         <v>185</v>
       </c>
       <c r="D74" s="1" t="s">
@@ -2268,11 +2040,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A75" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="75">
+      <c r="A75" s="2" t="n">
         <v>43218</v>
       </c>
-      <c r="C75" s="1">
+      <c r="C75" s="1" t="n">
         <v>404</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -2282,11 +2054,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="76">
+      <c r="A76" s="2" t="n">
         <v>43220</v>
       </c>
-      <c r="C76" s="1">
+      <c r="C76" s="1" t="n">
         <v>57</v>
       </c>
       <c r="D76" s="1" t="s">
@@ -2296,11 +2068,11 @@
         <v>114</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="77">
+      <c r="A77" s="2" t="n">
         <v>43221</v>
       </c>
-      <c r="C77" s="1">
+      <c r="C77" s="1" t="n">
         <v>282</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -2310,11 +2082,11 @@
         <v>116</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="78">
+      <c r="A78" s="2" t="n">
         <v>43220</v>
       </c>
-      <c r="C78" s="1">
+      <c r="C78" s="1" t="n">
         <v>87</v>
       </c>
       <c r="D78" s="1" t="s">
@@ -2324,11 +2096,11 @@
         <v>117</v>
       </c>
     </row>
-    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A79" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="79">
+      <c r="A79" s="2" t="n">
         <v>43223</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B79" s="1" t="n">
         <v>1878</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -2338,11 +2110,11 @@
         <v>119</v>
       </c>
     </row>
-    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A80" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="80">
+      <c r="A80" s="2" t="n">
         <v>43224</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B80" s="1" t="n">
         <v>98</v>
       </c>
       <c r="D80" s="1" t="s">
@@ -2352,11 +2124,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A81" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="81">
+      <c r="A81" s="2" t="n">
         <v>43225</v>
       </c>
-      <c r="C81" s="1">
+      <c r="C81" s="1" t="n">
         <v>198</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -2366,11 +2138,11 @@
         <v>122</v>
       </c>
     </row>
-    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A82" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="82">
+      <c r="A82" s="2" t="n">
         <v>43225</v>
       </c>
-      <c r="C82" s="1">
+      <c r="C82" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -2380,11 +2152,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="83">
+      <c r="A83" s="2" t="n">
         <v>43228</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83" s="1" t="n">
         <v>168</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -2394,11 +2166,11 @@
         <v>124</v>
       </c>
     </row>
-    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A84" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="84">
+      <c r="A84" s="2" t="n">
         <v>43229</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B84" s="1" t="n">
         <v>240</v>
       </c>
       <c r="D84" s="1" t="s">
@@ -2408,12 +2180,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A85" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="85">
+      <c r="A85" s="2" t="n">
         <v>43230</v>
       </c>
       <c r="B85" s="1"/>
-      <c r="C85" s="1">
+      <c r="C85" s="1" t="n">
         <v>420</v>
       </c>
       <c r="D85" s="1" t="s">
@@ -2423,11 +2195,11 @@
         <v>126</v>
       </c>
     </row>
-    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A86" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="86">
+      <c r="A86" s="2" t="n">
         <v>43230</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B86" s="1" t="n">
         <v>200</v>
       </c>
       <c r="C86" s="1"/>
@@ -2438,11 +2210,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A87" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="87">
+      <c r="A87" s="2" t="n">
         <v>43230</v>
       </c>
-      <c r="C87" s="1">
+      <c r="C87" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D87" s="1" t="s">
@@ -2452,11 +2224,11 @@
         <v>128</v>
       </c>
     </row>
-    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A88" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="88">
+      <c r="A88" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B88" s="1" t="n">
         <v>462</v>
       </c>
       <c r="D88" s="1" t="s">
@@ -2466,11 +2238,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A89" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="89">
+      <c r="A89" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B89" s="1" t="n">
         <v>499</v>
       </c>
       <c r="D89" s="1" t="s">
@@ -2480,11 +2252,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A90" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="90">
+      <c r="A90" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B90" s="1">
+      <c r="B90" s="1" t="n">
         <v>398</v>
       </c>
       <c r="D90" s="1" t="s">
@@ -2494,11 +2266,11 @@
         <v>133</v>
       </c>
     </row>
-    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A91" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="91">
+      <c r="A91" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B91" s="1">
+      <c r="B91" s="1" t="n">
         <v>226</v>
       </c>
       <c r="D91" s="1" t="s">
@@ -2508,11 +2280,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A92" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="92">
+      <c r="A92" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B92" s="1">
+      <c r="B92" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D92" s="1" t="s">
@@ -2522,11 +2294,11 @@
         <v>137</v>
       </c>
     </row>
-    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A93" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="93">
+      <c r="A93" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="B93" s="1">
+      <c r="B93" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D93" s="1" t="s">
@@ -2536,11 +2308,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A94" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="94">
+      <c r="A94" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="C94" s="1">
+      <c r="C94" s="1" t="n">
         <v>340</v>
       </c>
       <c r="D94" s="1" t="s">
@@ -2550,11 +2322,11 @@
         <v>139</v>
       </c>
     </row>
-    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A95" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="95">
+      <c r="A95" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="B95" s="1">
+      <c r="B95" s="1" t="n">
         <v>510</v>
       </c>
       <c r="D95" s="1" t="s">
@@ -2564,11 +2336,11 @@
         <v>141</v>
       </c>
     </row>
-    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A96" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="96">
+      <c r="A96" s="2" t="n">
         <v>43233</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B96" s="1" t="n">
         <v>170</v>
       </c>
       <c r="D96" s="1" t="s">
@@ -2578,11 +2350,11 @@
         <v>143</v>
       </c>
     </row>
-    <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A97" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="97">
+      <c r="A97" s="2" t="n">
         <v>43233</v>
       </c>
-      <c r="C97" s="1">
+      <c r="C97" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D97" s="1" t="s">
@@ -2592,11 +2364,11 @@
         <v>144</v>
       </c>
     </row>
-    <row r="98" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A98" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="98">
+      <c r="A98" s="2" t="n">
         <v>43234</v>
       </c>
-      <c r="C98" s="1">
+      <c r="C98" s="1" t="n">
         <v>299</v>
       </c>
       <c r="D98" s="1" t="s">
@@ -2606,11 +2378,11 @@
         <v>145</v>
       </c>
     </row>
-    <row r="99" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A99" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="99">
+      <c r="A99" s="2" t="n">
         <v>43236</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99" s="1" t="n">
         <v>3659</v>
       </c>
       <c r="D99" s="1" t="s">
@@ -2620,11 +2392,11 @@
         <v>146</v>
       </c>
     </row>
-    <row r="100" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A100" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="100">
+      <c r="A100" s="2" t="n">
         <v>43237</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B100" s="1" t="n">
         <v>79</v>
       </c>
       <c r="D100" s="1" t="s">
@@ -2634,11 +2406,11 @@
         <v>147</v>
       </c>
     </row>
-    <row r="101" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A101" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="101">
+      <c r="A101" s="2" t="n">
         <v>43236</v>
       </c>
-      <c r="C101" s="1">
+      <c r="C101" s="1" t="n">
         <v>173</v>
       </c>
       <c r="D101" s="1" t="s">
@@ -2648,11 +2420,11 @@
         <v>148</v>
       </c>
     </row>
-    <row r="102" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A102" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="102">
+      <c r="A102" s="2" t="n">
         <v>43240</v>
       </c>
-      <c r="B102" s="1">
+      <c r="B102" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D102" s="1" t="s">
@@ -2662,22 +2434,22 @@
         <v>149</v>
       </c>
     </row>
-    <row r="103" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A103" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="103">
+      <c r="A103" s="2" t="n">
         <v>43240</v>
       </c>
-      <c r="B103" s="1">
+      <c r="B103" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="104" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A104" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="104">
+      <c r="A104" s="2" t="n">
         <v>43241</v>
       </c>
-      <c r="B104" s="1">
+      <c r="B104" s="1" t="n">
         <v>4070</v>
       </c>
       <c r="D104" s="1" t="s">
@@ -2687,11 +2459,11 @@
         <v>150</v>
       </c>
     </row>
-    <row r="105" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A105" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="105">
+      <c r="A105" s="2" t="n">
         <v>43241</v>
       </c>
-      <c r="C105" s="1">
+      <c r="C105" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D105" s="1" t="s">
@@ -2701,11 +2473,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="106" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A106" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="106">
+      <c r="A106" s="2" t="n">
         <v>43242</v>
       </c>
-      <c r="B106" s="1">
+      <c r="B106" s="1" t="n">
         <v>79</v>
       </c>
       <c r="D106" s="1" t="s">
@@ -2715,11 +2487,11 @@
         <v>152</v>
       </c>
     </row>
-    <row r="107" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A107" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="107">
+      <c r="A107" s="2" t="n">
         <v>43246</v>
       </c>
-      <c r="B107" s="1">
+      <c r="B107" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D107" s="1" t="s">
@@ -2729,11 +2501,11 @@
         <v>154</v>
       </c>
     </row>
-    <row r="108" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A108" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="108">
+      <c r="A108" s="2" t="n">
         <v>43247</v>
       </c>
-      <c r="B108" s="1">
+      <c r="B108" s="1" t="n">
         <v>70</v>
       </c>
       <c r="D108" s="1" t="s">
@@ -2743,44 +2515,44 @@
         <v>156</v>
       </c>
     </row>
-    <row r="109" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A109" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="109">
+      <c r="A109" s="2" t="n">
         <v>43253</v>
       </c>
-      <c r="B109" s="1">
+      <c r="B109" s="1" t="n">
         <v>142</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A110" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="110">
+      <c r="A110" s="2" t="n">
         <v>43254</v>
       </c>
-      <c r="B110" s="1">
+      <c r="B110" s="1" t="n">
         <v>90</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="111" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A111" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="111">
+      <c r="A111" s="2" t="n">
         <v>43260</v>
       </c>
-      <c r="C111" s="1">
+      <c r="C111" s="1" t="n">
         <v>1400</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="112" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A112" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="112">
+      <c r="A112" s="2" t="n">
         <v>43260</v>
       </c>
-      <c r="C112" s="1">
+      <c r="C112" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D112" s="1" t="s">
@@ -2790,33 +2562,33 @@
         <v>91</v>
       </c>
     </row>
-    <row r="113" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A113" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="113">
+      <c r="A113" s="2" t="n">
         <v>43264</v>
       </c>
-      <c r="B113" s="1">
+      <c r="B113" s="1" t="n">
         <v>546</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="114" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A114" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="114">
+      <c r="A114" s="2" t="n">
         <v>43264</v>
       </c>
-      <c r="B114" s="1">
+      <c r="B114" s="1" t="n">
         <v>95</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="115" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A115" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="115">
+      <c r="A115" s="2" t="n">
         <v>43266</v>
       </c>
-      <c r="B115" s="1">
+      <c r="B115" s="1" t="n">
         <v>394</v>
       </c>
       <c r="D115" s="1" t="s">
@@ -2826,11 +2598,11 @@
         <v>163</v>
       </c>
     </row>
-    <row r="116" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A116" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="116">
+      <c r="A116" s="2" t="n">
         <v>43266</v>
       </c>
-      <c r="B116" s="1">
+      <c r="B116" s="1" t="n">
         <v>1055</v>
       </c>
       <c r="D116" s="1" t="s">
@@ -2840,11 +2612,11 @@
         <v>165</v>
       </c>
     </row>
-    <row r="117" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A117" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="117">
+      <c r="A117" s="2" t="n">
         <v>43284</v>
       </c>
-      <c r="C117" s="1">
+      <c r="C117" s="1" t="n">
         <v>274</v>
       </c>
       <c r="D117" s="1" t="s">
@@ -2854,11 +2626,11 @@
         <v>167</v>
       </c>
     </row>
-    <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A118" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="118">
+      <c r="A118" s="2" t="n">
         <v>43283</v>
       </c>
-      <c r="C118" s="1">
+      <c r="C118" s="1" t="n">
         <v>105</v>
       </c>
       <c r="D118" s="1" t="s">
@@ -2868,11 +2640,11 @@
         <v>169</v>
       </c>
     </row>
-    <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A119" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="119">
+      <c r="A119" s="2" t="n">
         <v>43289</v>
       </c>
-      <c r="C119" s="1">
+      <c r="C119" s="1" t="n">
         <v>128</v>
       </c>
       <c r="D119" s="1" t="s">
@@ -2882,11 +2654,11 @@
         <v>171</v>
       </c>
     </row>
-    <row r="120" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A120" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="120">
+      <c r="A120" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C120" s="1">
+      <c r="C120" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D120" s="1" t="s">
@@ -2896,11 +2668,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A121" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="121">
+      <c r="A121" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C121" s="1">
+      <c r="C121" s="1" t="n">
         <v>210</v>
       </c>
       <c r="D121" s="1" t="s">
@@ -2910,44 +2682,44 @@
         <v>173</v>
       </c>
     </row>
-    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A122" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="122">
+      <c r="A122" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B122" s="1">
+      <c r="B122" s="1" t="n">
         <v>980</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="123" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A123" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="123">
+      <c r="A123" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B123" s="1">
+      <c r="B123" s="1" t="n">
         <v>1260</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A124" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="124">
+      <c r="A124" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B124" s="1">
+      <c r="B124" s="1" t="n">
         <v>3687</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A125" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="125">
+      <c r="A125" s="2" t="n">
         <v>43298</v>
       </c>
-      <c r="C125" s="1">
+      <c r="C125" s="1" t="n">
         <v>60</v>
       </c>
       <c r="D125" s="1" t="s">
@@ -2957,55 +2729,55 @@
         <v>178</v>
       </c>
     </row>
-    <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A126" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="126">
+      <c r="A126" s="2" t="n">
         <v>43291</v>
       </c>
-      <c r="C126" s="1">
+      <c r="C126" s="1" t="n">
         <v>404</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A127" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="127">
+      <c r="A127" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C127" s="1">
+      <c r="C127" s="1" t="n">
         <v>451</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="128" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A128" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="128">
+      <c r="A128" s="2" t="n">
         <v>43298</v>
       </c>
-      <c r="C128" s="1">
+      <c r="C128" s="1" t="n">
         <v>708</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A129" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="129">
+      <c r="A129" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C129" s="1">
+      <c r="C129" s="1" t="n">
         <v>160</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A130" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="130">
+      <c r="A130" s="2" t="n">
         <v>43288</v>
       </c>
-      <c r="C130" s="1">
+      <c r="C130" s="1" t="n">
         <v>72</v>
       </c>
       <c r="D130" s="1" t="s">
@@ -3015,11 +2787,11 @@
         <v>181</v>
       </c>
     </row>
-    <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A131" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="131">
+      <c r="A131" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C131" s="1">
+      <c r="C131" s="1" t="n">
         <v>300</v>
       </c>
       <c r="D131" s="1" t="s">
@@ -3029,11 +2801,11 @@
         <v>183</v>
       </c>
     </row>
-    <row r="132" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A132" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="132">
+      <c r="A132" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C132" s="1">
+      <c r="C132" s="1" t="n">
         <v>230</v>
       </c>
       <c r="D132" s="1" t="s">
@@ -3043,22 +2815,22 @@
         <v>185</v>
       </c>
     </row>
-    <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A133" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="133">
+      <c r="A133" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C133" s="1">
+      <c r="C133" s="1" t="n">
         <v>454</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="134" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A134" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="134">
+      <c r="A134" s="2" t="n">
         <v>43299</v>
       </c>
-      <c r="C134" s="1">
+      <c r="C134" s="1" t="n">
         <v>686</v>
       </c>
       <c r="D134" s="1" t="s">
@@ -3068,11 +2840,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A135" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="135">
+      <c r="A135" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C135" s="1">
+      <c r="C135" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D135" s="1" t="s">
@@ -3082,11 +2854,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A136" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="136">
+      <c r="A136" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C136" s="1">
+      <c r="C136" s="1" t="n">
         <v>2067</v>
       </c>
       <c r="D136" s="1" t="s">
@@ -3096,11 +2868,11 @@
         <v>186</v>
       </c>
     </row>
-    <row r="137" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A137" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="137">
+      <c r="A137" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B137" s="1">
+      <c r="B137" s="1" t="n">
         <v>109</v>
       </c>
       <c r="D137" s="1" t="s">
@@ -3110,11 +2882,11 @@
         <v>187</v>
       </c>
     </row>
-    <row r="138" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A138" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="138">
+      <c r="A138" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B138" s="1">
+      <c r="B138" s="1" t="n">
         <v>97</v>
       </c>
       <c r="D138" s="1" t="s">
@@ -3124,11 +2896,11 @@
         <v>188</v>
       </c>
     </row>
-    <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A139" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="139">
+      <c r="A139" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B139" s="1">
+      <c r="B139" s="1" t="n">
         <v>1437</v>
       </c>
       <c r="D139" s="1" t="s">
@@ -3138,11 +2910,11 @@
         <v>189</v>
       </c>
     </row>
-    <row r="140" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A140" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="140">
+      <c r="A140" s="2" t="n">
         <v>43306</v>
       </c>
-      <c r="C140" s="1">
+      <c r="C140" s="1" t="n">
         <v>650</v>
       </c>
       <c r="D140" s="1" t="s">
@@ -3152,11 +2924,11 @@
         <v>190</v>
       </c>
     </row>
-    <row r="141" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A141" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="141">
+      <c r="A141" s="2" t="n">
         <v>43305</v>
       </c>
-      <c r="C141" s="1">
+      <c r="C141" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D141" s="1" t="s">
@@ -3166,11 +2938,11 @@
         <v>191</v>
       </c>
     </row>
-    <row r="142" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A142" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="142">
+      <c r="A142" s="2" t="n">
         <v>43309</v>
       </c>
-      <c r="C142" s="1">
+      <c r="C142" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D142" s="1" t="s">
@@ -3180,11 +2952,11 @@
         <v>192</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A143" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="0" r="143">
+      <c r="A143" s="2" t="n">
         <v>43306</v>
       </c>
-      <c r="B143" s="1">
+      <c r="B143" s="1" t="n">
         <v>167</v>
       </c>
       <c r="D143" s="1" t="s">
@@ -3194,11 +2966,11 @@
         <v>193</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A144" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="0" r="144">
+      <c r="A144" s="2" t="n">
         <v>43304</v>
       </c>
-      <c r="C144" s="1">
+      <c r="C144" s="1" t="n">
         <v>93</v>
       </c>
       <c r="D144" s="1" t="s">
@@ -3208,11 +2980,11 @@
         <v>194</v>
       </c>
     </row>
-    <row r="145" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A145" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="145">
+      <c r="A145" s="2" t="n">
         <v>43305</v>
       </c>
-      <c r="C145" s="1">
+      <c r="C145" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D145" s="1" t="s">
@@ -3222,11 +2994,11 @@
         <v>195</v>
       </c>
     </row>
-    <row r="146" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A146" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="146">
+      <c r="A146" s="2" t="n">
         <v>43303</v>
       </c>
-      <c r="C146" s="1">
+      <c r="C146" s="1" t="n">
         <v>244</v>
       </c>
       <c r="D146" s="1" t="s">
@@ -3236,11 +3008,11 @@
         <v>196</v>
       </c>
     </row>
-    <row r="147" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A147" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="147">
+      <c r="A147" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C147" s="1">
+      <c r="C147" s="1" t="n">
         <v>482</v>
       </c>
       <c r="D147" s="1" t="s">
@@ -3250,11 +3022,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="148" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A148" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="148">
+      <c r="A148" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C148" s="1">
+      <c r="C148" s="1" t="n">
         <v>172</v>
       </c>
       <c r="D148" s="1" t="s">
@@ -3264,44 +3036,44 @@
         <v>199</v>
       </c>
     </row>
-    <row r="149" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A149" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="149">
+      <c r="A149" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="B149" s="1">
+      <c r="B149" s="1" t="n">
         <v>89</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="150" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A150" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="150">
+      <c r="A150" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="C150" s="1">
+      <c r="C150" s="1" t="n">
         <v>107</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="151" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A151" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="151">
+      <c r="A151" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="C151" s="1">
+      <c r="C151" s="1" t="n">
         <v>124</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="152" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A152" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="152">
+      <c r="A152" s="7" t="n">
         <v>43316</v>
       </c>
-      <c r="C152" s="1">
+      <c r="C152" s="1" t="n">
         <v>4500</v>
       </c>
       <c r="D152" s="1" t="s">
@@ -3311,11 +3083,11 @@
         <v>202</v>
       </c>
     </row>
-    <row r="153" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A153" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="153">
+      <c r="A153" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C153" s="1">
+      <c r="C153" s="1" t="n">
         <v>247</v>
       </c>
       <c r="D153" s="1" t="s">
@@ -3325,11 +3097,11 @@
         <v>204</v>
       </c>
     </row>
-    <row r="154" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A154" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="154">
+      <c r="A154" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C154" s="1">
+      <c r="C154" s="1" t="n">
         <v>1150</v>
       </c>
       <c r="D154" s="1" t="s">
@@ -3339,11 +3111,11 @@
         <v>205</v>
       </c>
     </row>
-    <row r="155" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A155" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="155">
+      <c r="A155" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C155" s="1">
+      <c r="C155" s="1" t="n">
         <v>313</v>
       </c>
       <c r="D155" s="1" t="s">
@@ -3353,11 +3125,11 @@
         <v>207</v>
       </c>
     </row>
-    <row r="156" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A156" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="156">
+      <c r="A156" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="B156" s="1">
+      <c r="B156" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D156" s="1" t="s">
@@ -3367,11 +3139,11 @@
         <v>209</v>
       </c>
     </row>
-    <row r="157" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A157" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="157">
+      <c r="A157" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="C157" s="1">
+      <c r="C157" s="1" t="n">
         <v>710</v>
       </c>
       <c r="D157" s="1" t="s">
@@ -3381,11 +3153,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A158" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="158">
+      <c r="A158" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="C158" s="1">
+      <c r="C158" s="1" t="n">
         <v>100</v>
       </c>
       <c r="D158" s="1" t="s">
@@ -3395,11 +3167,11 @@
         <v>212</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A159" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="159">
+      <c r="A159" s="2" t="n">
         <v>43319</v>
       </c>
-      <c r="B159" s="1">
+      <c r="B159" s="1" t="n">
         <v>78</v>
       </c>
       <c r="D159" s="1" t="s">
@@ -3409,22 +3181,22 @@
         <v>213</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A160" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="160">
+      <c r="A160" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="B160" s="1">
+      <c r="B160" s="1" t="n">
         <v>1840</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A161" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="161">
+      <c r="A161" s="2" t="n">
         <v>43322</v>
       </c>
-      <c r="B161" s="1">
+      <c r="B161" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D161" s="1" t="s">
@@ -3434,11 +3206,11 @@
         <v>216</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A162" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="162">
+      <c r="A162" s="7" t="n">
         <v>43324</v>
       </c>
-      <c r="C162" s="1">
+      <c r="C162" s="1" t="n">
         <v>230</v>
       </c>
       <c r="D162" s="1" t="s">
@@ -3448,11 +3220,11 @@
         <v>217</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A163" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="163">
+      <c r="A163" s="7" t="n">
         <v>43326</v>
       </c>
-      <c r="C163" s="1">
+      <c r="C163" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D163" s="1" t="s">
@@ -3462,11 +3234,11 @@
         <v>219</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A164" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="164">
+      <c r="A164" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="B164" s="1">
+      <c r="B164" s="1" t="n">
         <v>45</v>
       </c>
       <c r="D164" s="1" t="s">
@@ -3476,183 +3248,244 @@
         <v>221</v>
       </c>
     </row>
-    <row r="165" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A165" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="165">
+      <c r="A165" s="10" t="n">
         <v>43327</v>
       </c>
-      <c r="C165">
+      <c r="C165" s="0" t="n">
         <v>486</v>
       </c>
-      <c r="D165" t="s">
+      <c r="D165" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E165" t="s">
+      <c r="E165" s="0" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="166" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A166" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="166">
+      <c r="A166" s="10" t="n">
         <v>43329</v>
       </c>
-      <c r="C166">
+      <c r="C166" s="0" t="n">
         <v>92</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D166" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="E166" t="s">
+      <c r="E166" s="0" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A167" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="167">
+      <c r="A167" s="10" t="n">
         <v>43331</v>
       </c>
-      <c r="C167">
+      <c r="C167" s="0" t="n">
         <v>310</v>
       </c>
-      <c r="D167" t="s">
+      <c r="D167" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="E167" t="s">
+      <c r="E167" s="0" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A168" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="168">
+      <c r="A168" s="10" t="n">
         <v>43334</v>
       </c>
-      <c r="C168">
+      <c r="C168" s="0" t="n">
         <v>464</v>
       </c>
-      <c r="D168" t="s">
+      <c r="D168" s="0" t="s">
         <v>218</v>
       </c>
       <c r="E168" s="11" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A169" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="169">
+      <c r="A169" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="C169">
+      <c r="C169" s="0" t="n">
         <v>726</v>
       </c>
-      <c r="D169" t="s">
+      <c r="D169" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="E169" t="s">
+      <c r="E169" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A170" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="170">
+      <c r="A170" s="10" t="n">
         <v>43337</v>
       </c>
-      <c r="C170">
+      <c r="C170" s="0" t="n">
         <v>544</v>
       </c>
-      <c r="D170" t="s">
+      <c r="D170" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E170" t="s">
+      <c r="E170" s="0" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A171" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="171">
+      <c r="A171" s="10" t="n">
         <v>43337</v>
       </c>
-      <c r="B171">
+      <c r="B171" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D171" t="s">
+      <c r="D171" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="E171" t="s">
+      <c r="E171" s="0" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A172" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="172">
+      <c r="A172" s="10" t="n">
         <v>43341</v>
       </c>
-      <c r="C172">
+      <c r="C172" s="0" t="n">
         <v>830</v>
       </c>
-      <c r="D172" t="s">
+      <c r="D172" s="0" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A173" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="173">
+      <c r="A173" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="C173">
+      <c r="C173" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="D173" t="s">
+      <c r="D173" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="E173" t="s">
+      <c r="E173" s="0" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A174" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="174">
+      <c r="A174" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="B174">
+      <c r="B174" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D174" t="s">
+      <c r="D174" s="0" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A175" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="175">
+      <c r="A175" s="10" t="n">
         <v>43344</v>
       </c>
-      <c r="B175">
+      <c r="B175" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="D175" t="s">
+      <c r="D175" s="0" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A176" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="176">
+      <c r="A176" s="10" t="n">
         <v>43344</v>
       </c>
-      <c r="B176">
+      <c r="B176" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D176" t="s">
+      <c r="D176" s="0" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="207" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B207">
-        <f>SUM(B2:B206)</f>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="177">
+      <c r="A177" s="10" t="n">
+        <v>43345</v>
+      </c>
+      <c r="C177" s="0" t="n">
+        <v>607</v>
+      </c>
+      <c r="D177" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="E177" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="178">
+      <c r="A178" s="10" t="n">
+        <v>43345</v>
+      </c>
+      <c r="C178" s="0" t="n">
+        <v>444</v>
+      </c>
+      <c r="D178" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="E178" s="0" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="179">
+      <c r="A179" s="10" t="n">
+        <v>43345</v>
+      </c>
+      <c r="C179" s="0" t="n">
+        <v>312</v>
+      </c>
+      <c r="D179" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="E179" s="0" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="180">
+      <c r="A180" s="10" t="n">
+        <v>43345</v>
+      </c>
+      <c r="C180" s="0" t="n">
+        <v>501</v>
+      </c>
+      <c r="D180" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="E180" s="0" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="207">
+      <c r="B207" s="0" t="n">
+        <f aca="false">SUM(B2:B206)</f>
         <v>38931</v>
       </c>
-      <c r="C207">
-        <f>SUM(C2:C206)</f>
-        <v>38380</v>
+      <c r="C207" s="0" t="n">
+        <f aca="false">SUM(C2:C206)</f>
+        <v>40244</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A30:Z32">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule aboveAverage="0" bottom="0" dxfId="0" operator="expression" percent="0" priority="2" rank="0" text="" type="expression">
       <formula>LEN(TRIM(A30))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D33" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D40" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink display="netonnet.se" ref="D33" r:id="rId1"/>
+    <hyperlink display="www.vidaxl.se" ref="D40" r:id="rId2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
cost update 0907 jenny
</commit_message>
<xml_diff>
--- a/Cost.xlsx
+++ b/Cost.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="240">
   <si>
     <t>日期</t>
   </si>
@@ -729,6 +729,12 @@
   </si>
   <si>
     <t>vegetables; hairspray; etc</t>
+  </si>
+  <si>
+    <t>OKQ8 </t>
+  </si>
+  <si>
+    <t>Trip back to Taby from Linkoping</t>
   </si>
 </sst>
 </file>
@@ -979,8 +985,8 @@
   </sheetPr>
   <dimension ref="A1:Z207"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A163" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E185" activeCellId="0" pane="topLeft" sqref="E185"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D184" activeCellId="0" pane="topLeft" sqref="D184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
@@ -3460,6 +3466,20 @@
         <v>237</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="181">
+      <c r="A181" s="10" t="n">
+        <v>43349</v>
+      </c>
+      <c r="C181" s="0" t="n">
+        <v>711</v>
+      </c>
+      <c r="D181" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="E181" s="0" t="s">
+        <v>239</v>
+      </c>
+    </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="207">
       <c r="B207" s="0" t="n">
         <f aca="false">SUM(B2:B206)</f>
@@ -3467,7 +3487,7 @@
       </c>
       <c r="C207" s="0" t="n">
         <f aca="false">SUM(C2:C206)</f>
-        <v>40244</v>
+        <v>40955</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cost update 0911 JENNY
</commit_message>
<xml_diff>
--- a/Cost.xlsx
+++ b/Cost.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="243">
   <si>
     <t>日期</t>
   </si>
@@ -731,10 +731,19 @@
     <t>vegetables; hairspray; etc</t>
   </si>
   <si>
-    <t>OKQ8 </t>
+    <t>OKQ8</t>
   </si>
   <si>
     <t>Trip back to Taby from Linkoping</t>
+  </si>
+  <si>
+    <t>SUANCAI YU TIAOLIAO</t>
+  </si>
+  <si>
+    <t>ica maxi</t>
+  </si>
+  <si>
+    <t>milk yogurt vegetables etc</t>
   </si>
 </sst>
 </file>
@@ -986,7 +995,7 @@
   <dimension ref="A1:Z207"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D184" activeCellId="0" pane="topLeft" sqref="D184"/>
+      <selection activeCell="D183" activeCellId="0" pane="topLeft" sqref="D183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
@@ -3480,14 +3489,42 @@
         <v>239</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="182">
+      <c r="A182" s="10" t="n">
+        <v>43354</v>
+      </c>
+      <c r="B182" s="0" t="n">
+        <v>126</v>
+      </c>
+      <c r="D182" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="E182" s="0" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="183">
+      <c r="A183" s="10" t="n">
+        <v>43354</v>
+      </c>
+      <c r="C183" s="0" t="n">
+        <v>450</v>
+      </c>
+      <c r="D183" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="E183" s="0" t="s">
+        <v>242</v>
+      </c>
+    </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="207">
       <c r="B207" s="0" t="n">
         <f aca="false">SUM(B2:B206)</f>
-        <v>38931</v>
+        <v>39057</v>
       </c>
       <c r="C207" s="0" t="n">
         <f aca="false">SUM(C2:C206)</f>
-        <v>40955</v>
+        <v>41405</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cost update 0918 Jenny
</commit_message>
<xml_diff>
--- a/Cost.xlsx
+++ b/Cost.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="244">
   <si>
     <t>日期</t>
   </si>
@@ -744,6 +744,9 @@
   </si>
   <si>
     <t>milk yogurt vegetables etc</t>
+  </si>
+  <si>
+    <t>SHELL</t>
   </si>
 </sst>
 </file>
@@ -994,8 +997,8 @@
   </sheetPr>
   <dimension ref="A1:Z207"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D183" activeCellId="0" pane="topLeft" sqref="D183"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A182" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E190" activeCellId="0" pane="topLeft" sqref="E190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
@@ -3517,6 +3520,20 @@
         <v>242</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="184">
+      <c r="A184" s="10" t="n">
+        <v>43361</v>
+      </c>
+      <c r="C184" s="0" t="n">
+        <v>660</v>
+      </c>
+      <c r="D184" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="E184" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="207">
       <c r="B207" s="0" t="n">
         <f aca="false">SUM(B2:B206)</f>
@@ -3524,7 +3541,7 @@
       </c>
       <c r="C207" s="0" t="n">
         <f aca="false">SUM(C2:C206)</f>
-        <v>41405</v>
+        <v>42065</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cost update 0921 jenny
</commit_message>
<xml_diff>
--- a/Cost.xlsx
+++ b/Cost.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="245">
   <si>
     <t>日期</t>
   </si>
@@ -747,6 +747,9 @@
   </si>
   <si>
     <t>SHELL</t>
+  </si>
+  <si>
+    <t>libero series; milk; yogurt</t>
   </si>
 </sst>
 </file>
@@ -997,8 +1000,8 @@
   </sheetPr>
   <dimension ref="A1:Z207"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A182" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E190" activeCellId="0" pane="topLeft" sqref="E190"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A176" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D187" activeCellId="0" pane="topLeft" sqref="D187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
@@ -3534,6 +3537,20 @@
         <v>91</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="185">
+      <c r="A185" s="10" t="n">
+        <v>43363</v>
+      </c>
+      <c r="C185" s="0" t="n">
+        <v>230</v>
+      </c>
+      <c r="D185" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="E185" s="0" t="s">
+        <v>244</v>
+      </c>
+    </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="207">
       <c r="B207" s="0" t="n">
         <f aca="false">SUM(B2:B206)</f>
@@ -3541,7 +3558,7 @@
       </c>
       <c r="C207" s="0" t="n">
         <f aca="false">SUM(C2:C206)</f>
-        <v>42065</v>
+        <v>42295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cost update 1015 jenny
</commit_message>
<xml_diff>
--- a/Cost.xlsx
+++ b/Cost.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chengkaiyan/github/cost/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC743AE-3F74-7F4D-B3CA-4D3824764A53}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="256">
   <si>
     <t>日期</t>
   </si>
@@ -785,41 +780,60 @@
   </si>
   <si>
     <t>maxi barkby</t>
+  </si>
+  <si>
+    <t>The data is lost so I will just start from 46000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="yyyy/m/d"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt formatCode="YYYY/M/D" numFmtId="165"/>
+    <numFmt formatCode="M/D/YYYY" numFmtId="166"/>
+    <numFmt formatCode="YYYY\-MM\-DD" numFmtId="167"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <family val="0"/>
       <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
       <name val="Arial"/>
       <family val="2"/>
+      <sz val="10"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF666666"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF666666"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="5">
@@ -849,7 +863,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
@@ -857,27 +871,88 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="167" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -888,7 +963,6 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -947,339 +1021,31 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:Z207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A176" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D195" sqref="D195"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A188" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D202" activeCellId="0" pane="topLeft" sqref="D202"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="3" width="14.5"/>
-    <col min="4" max="4" width="26"/>
-    <col min="5" max="5" width="37.83203125"/>
-    <col min="6" max="1025" width="14.5"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="14.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1296,11 +1062,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="2">
+      <c r="A2" s="2" t="n">
         <v>43121</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="1" t="n">
         <v>250</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1310,11 +1076,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="3">
+      <c r="A3" s="2" t="n">
         <v>43122</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="1" t="n">
         <v>305</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1324,11 +1090,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="4">
+      <c r="A4" s="2" t="n">
         <v>43122</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1338,11 +1104,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="5">
+      <c r="A5" s="2" t="n">
         <v>43125</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="1" t="n">
         <v>98</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1352,11 +1118,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="6">
+      <c r="A6" s="2" t="n">
         <v>43126</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1366,11 +1132,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="7">
+      <c r="A7" s="2" t="n">
         <v>43127</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1380,11 +1146,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="8">
+      <c r="A8" s="2" t="n">
         <v>43128</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="1" t="n">
         <v>656</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1394,11 +1160,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="9">
+      <c r="A9" s="2" t="n">
         <v>43131</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="1" t="n">
         <v>486</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1408,11 +1174,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="10">
+      <c r="A10" s="2" t="n">
         <v>43132</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="1" t="n">
         <v>76</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1422,11 +1188,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="11">
+      <c r="A11" s="2" t="n">
         <v>43133</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="1" t="n">
         <v>399</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1436,11 +1202,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="12">
+      <c r="A12" s="2" t="n">
         <v>43135</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="1" t="n">
         <v>419</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1450,11 +1216,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="13">
+      <c r="A13" s="2" t="n">
         <v>43136</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="1" t="n">
         <v>521</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1464,11 +1230,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="14">
+      <c r="A14" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="1" t="n">
         <v>399</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1478,11 +1244,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="15">
+      <c r="A15" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="1" t="n">
         <v>138</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1492,11 +1258,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="16">
+      <c r="A16" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="1" t="n">
         <v>310</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1506,12 +1272,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="17">
+      <c r="A17" s="2" t="n">
         <v>43138</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="1">
+      <c r="C17" s="1" t="n">
         <v>700</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1521,12 +1287,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="18">
+      <c r="A18" s="2" t="n">
         <v>43141</v>
       </c>
-      <c r="C18" s="1">
-        <f>F18*G18</f>
+      <c r="C18" s="1" t="n">
+        <f aca="false">F18*G18</f>
         <v>1312</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -1535,18 +1301,18 @@
       <c r="E18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="1" t="n">
         <v>164</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="1" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="19">
+      <c r="A19" s="2" t="n">
         <v>43141</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="1" t="n">
         <v>1190</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1556,11 +1322,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="20">
+      <c r="A20" s="2" t="n">
         <v>43154</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="1" t="n">
         <v>438</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1570,11 +1336,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="21">
+      <c r="A21" s="2" t="n">
         <v>43154</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="1" t="n">
         <v>248</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -1584,22 +1350,22 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="22">
+      <c r="A22" s="2" t="n">
         <v>43166</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="1" t="n">
         <v>234</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="23">
+      <c r="A23" s="2" t="n">
         <v>43171</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="1" t="n">
         <v>118</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1609,22 +1375,22 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="24">
+      <c r="A24" s="2" t="n">
         <v>43173</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="1" t="n">
         <v>82</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="25">
+      <c r="A25" s="2" t="n">
         <v>43174</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1634,22 +1400,22 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="26">
+      <c r="A26" s="2" t="n">
         <v>43175</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="1" t="n">
         <v>370</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="27">
+      <c r="A27" s="2" t="n">
         <v>43175</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -1659,11 +1425,11 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="28">
+      <c r="A28" s="2" t="n">
         <v>43176</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="1" t="n">
         <v>624</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -1673,11 +1439,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="29">
+      <c r="A29" s="2" t="n">
         <v>43177</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="1" t="n">
         <v>170</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1687,22 +1453,22 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="30">
+      <c r="A30" s="4" t="n">
         <v>43179</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="31">
+      <c r="A31" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="1" t="n">
         <v>90</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -1712,11 +1478,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="32">
+      <c r="A32" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="1" t="n">
         <v>72</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -1726,11 +1492,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="33">
+      <c r="A33" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="1" t="n">
         <v>908</v>
       </c>
       <c r="D33" s="6" t="s">
@@ -1740,11 +1506,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="34">
+      <c r="A34" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -1754,11 +1520,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="35">
+      <c r="A35" s="2" t="n">
         <v>43181</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -1768,11 +1534,11 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="36">
+      <c r="A36" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="1" t="n">
         <v>135</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -1782,11 +1548,11 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="37">
+      <c r="A37" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="1" t="n">
         <v>110</v>
       </c>
       <c r="C37" s="1"/>
@@ -1818,11 +1584,11 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="38">
+      <c r="A38" s="2" t="n">
         <v>43185</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="1" t="n">
         <v>122</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -1832,22 +1598,22 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="39">
+      <c r="A39" s="2" t="n">
         <v>43187</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="1" t="n">
         <v>750</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="40">
+      <c r="A40" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="1" t="n">
         <v>379</v>
       </c>
       <c r="D40" s="6" t="s">
@@ -1857,22 +1623,22 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="41">
+      <c r="A41" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="1" t="n">
         <v>240</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="42">
+      <c r="A42" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="1" t="n">
         <v>540</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -1882,11 +1648,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="43">
+      <c r="A43" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -1896,11 +1662,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="44">
+      <c r="A44" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -1910,11 +1676,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="45">
+      <c r="A45" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="1" t="n">
         <v>462</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -1924,11 +1690,11 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="46">
+      <c r="A46" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46" s="1" t="n">
         <v>70</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -1938,11 +1704,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="47">
+      <c r="A47" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -1952,11 +1718,11 @@
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="48">
+      <c r="A48" s="2" t="n">
         <v>43190</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="1" t="n">
         <v>30</v>
       </c>
       <c r="C48" s="1"/>
@@ -1967,11 +1733,11 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="49">
+      <c r="A49" s="2" t="n">
         <v>43191</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="1" t="n">
         <v>40</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -1981,11 +1747,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="50">
+      <c r="A50" s="7" t="n">
         <v>43193</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50" s="1" t="n">
         <v>150</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -1995,11 +1761,11 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="51">
+      <c r="A51" s="2" t="n">
         <v>43194</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51" s="1" t="n">
         <v>1360</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -2009,11 +1775,11 @@
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="52">
+      <c r="A52" s="2" t="n">
         <v>43195</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" s="1" t="n">
         <v>94</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -2023,11 +1789,11 @@
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="53">
+      <c r="A53" s="2" t="n">
         <v>43196</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C53" s="1" t="n">
         <v>48</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -2037,11 +1803,11 @@
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="54">
+      <c r="A54" s="2" t="n">
         <v>43196</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C54" s="1" t="n">
         <v>205</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -2051,11 +1817,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="55">
+      <c r="A55" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -2065,11 +1831,11 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="56">
+      <c r="A56" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56" s="1" t="n">
         <v>421</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -2079,11 +1845,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="57">
+      <c r="A57" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="1" t="n">
         <v>191</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -2093,11 +1859,11 @@
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="58">
+      <c r="A58" s="2" t="n">
         <v>43198</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58" s="1" t="n">
         <v>226</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -2107,22 +1873,22 @@
         <v>96</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="59">
+      <c r="A59" s="2" t="n">
         <v>43200</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59" s="1" t="n">
         <v>250</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="60">
+      <c r="A60" s="2" t="n">
         <v>43200</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60" s="1" t="n">
         <v>1115</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -2132,11 +1898,11 @@
         <v>99</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="61">
+      <c r="A61" s="2" t="n">
         <v>43201</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -2146,11 +1912,11 @@
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="62">
+      <c r="A62" s="2" t="n">
         <v>43201</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62" s="1" t="n">
         <v>88</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -2160,11 +1926,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="63">
+      <c r="A63" s="2" t="n">
         <v>43203</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -2174,11 +1940,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="64">
+      <c r="A64" s="2" t="n">
         <v>43203</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C64" s="1" t="n">
         <v>364</v>
       </c>
       <c r="D64" s="1" t="s">
@@ -2188,11 +1954,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="65">
+      <c r="A65" s="2" t="n">
         <v>43204</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65" s="1" t="n">
         <v>65</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -2202,11 +1968,11 @@
         <v>105</v>
       </c>
     </row>
-    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="66">
+      <c r="A66" s="2" t="n">
         <v>43208</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -2216,11 +1982,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="67">
+      <c r="A67" s="2" t="n">
         <v>43208</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C67" s="1" t="n">
         <v>470</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -2230,11 +1996,11 @@
         <v>107</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="68">
+      <c r="A68" s="2" t="n">
         <v>43209</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68" s="1" t="n">
         <v>180</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -2244,11 +2010,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A69" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="69">
+      <c r="A69" s="2" t="n">
         <v>43210</v>
       </c>
-      <c r="C69" s="1">
+      <c r="C69" s="1" t="n">
         <v>420</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -2258,11 +2024,11 @@
         <v>109</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="70">
+      <c r="A70" s="2" t="n">
         <v>43212</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70" s="1" t="n">
         <v>50</v>
       </c>
       <c r="D70" s="1" t="s">
@@ -2272,11 +2038,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="71">
+      <c r="A71" s="2" t="n">
         <v>43212</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71" s="1" t="n">
         <v>164</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -2286,11 +2052,11 @@
         <v>112</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="72">
+      <c r="A72" s="2" t="n">
         <v>43215</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B72" s="1" t="n">
         <v>300</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -2300,11 +2066,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="73">
+      <c r="A73" s="2" t="n">
         <v>43217</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73" s="1" t="n">
         <v>364</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -2314,11 +2080,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A74" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="74">
+      <c r="A74" s="2" t="n">
         <v>43218</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74" s="1" t="n">
         <v>185</v>
       </c>
       <c r="D74" s="1" t="s">
@@ -2328,11 +2094,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A75" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="75">
+      <c r="A75" s="2" t="n">
         <v>43218</v>
       </c>
-      <c r="C75" s="1">
+      <c r="C75" s="1" t="n">
         <v>404</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -2342,11 +2108,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="76">
+      <c r="A76" s="2" t="n">
         <v>43220</v>
       </c>
-      <c r="C76" s="1">
+      <c r="C76" s="1" t="n">
         <v>57</v>
       </c>
       <c r="D76" s="1" t="s">
@@ -2356,11 +2122,11 @@
         <v>114</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="77">
+      <c r="A77" s="2" t="n">
         <v>43221</v>
       </c>
-      <c r="C77" s="1">
+      <c r="C77" s="1" t="n">
         <v>282</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -2370,11 +2136,11 @@
         <v>116</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="78">
+      <c r="A78" s="2" t="n">
         <v>43220</v>
       </c>
-      <c r="C78" s="1">
+      <c r="C78" s="1" t="n">
         <v>87</v>
       </c>
       <c r="D78" s="1" t="s">
@@ -2384,11 +2150,11 @@
         <v>117</v>
       </c>
     </row>
-    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A79" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="79">
+      <c r="A79" s="2" t="n">
         <v>43223</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B79" s="1" t="n">
         <v>1878</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -2398,11 +2164,11 @@
         <v>119</v>
       </c>
     </row>
-    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A80" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="80">
+      <c r="A80" s="2" t="n">
         <v>43224</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B80" s="1" t="n">
         <v>98</v>
       </c>
       <c r="D80" s="1" t="s">
@@ -2412,11 +2178,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A81" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="81">
+      <c r="A81" s="2" t="n">
         <v>43225</v>
       </c>
-      <c r="C81" s="1">
+      <c r="C81" s="1" t="n">
         <v>198</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -2426,11 +2192,11 @@
         <v>122</v>
       </c>
     </row>
-    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A82" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="82">
+      <c r="A82" s="2" t="n">
         <v>43225</v>
       </c>
-      <c r="C82" s="1">
+      <c r="C82" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -2440,11 +2206,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="83">
+      <c r="A83" s="2" t="n">
         <v>43228</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83" s="1" t="n">
         <v>168</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -2454,11 +2220,11 @@
         <v>124</v>
       </c>
     </row>
-    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A84" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="84">
+      <c r="A84" s="2" t="n">
         <v>43229</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B84" s="1" t="n">
         <v>240</v>
       </c>
       <c r="D84" s="1" t="s">
@@ -2468,12 +2234,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A85" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="85">
+      <c r="A85" s="2" t="n">
         <v>43230</v>
       </c>
       <c r="B85" s="1"/>
-      <c r="C85" s="1">
+      <c r="C85" s="1" t="n">
         <v>420</v>
       </c>
       <c r="D85" s="1" t="s">
@@ -2483,11 +2249,11 @@
         <v>126</v>
       </c>
     </row>
-    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A86" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="86">
+      <c r="A86" s="2" t="n">
         <v>43230</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B86" s="1" t="n">
         <v>200</v>
       </c>
       <c r="C86" s="1"/>
@@ -2498,11 +2264,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A87" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="87">
+      <c r="A87" s="2" t="n">
         <v>43230</v>
       </c>
-      <c r="C87" s="1">
+      <c r="C87" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D87" s="1" t="s">
@@ -2512,11 +2278,11 @@
         <v>128</v>
       </c>
     </row>
-    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A88" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="88">
+      <c r="A88" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B88" s="1" t="n">
         <v>462</v>
       </c>
       <c r="D88" s="1" t="s">
@@ -2526,11 +2292,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A89" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="89">
+      <c r="A89" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B89" s="1" t="n">
         <v>499</v>
       </c>
       <c r="D89" s="1" t="s">
@@ -2540,11 +2306,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A90" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="90">
+      <c r="A90" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B90" s="1">
+      <c r="B90" s="1" t="n">
         <v>398</v>
       </c>
       <c r="D90" s="1" t="s">
@@ -2554,11 +2320,11 @@
         <v>133</v>
       </c>
     </row>
-    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A91" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="91">
+      <c r="A91" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B91" s="1">
+      <c r="B91" s="1" t="n">
         <v>226</v>
       </c>
       <c r="D91" s="1" t="s">
@@ -2568,11 +2334,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A92" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="92">
+      <c r="A92" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B92" s="1">
+      <c r="B92" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D92" s="1" t="s">
@@ -2582,11 +2348,11 @@
         <v>137</v>
       </c>
     </row>
-    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A93" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="93">
+      <c r="A93" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="B93" s="1">
+      <c r="B93" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D93" s="1" t="s">
@@ -2596,11 +2362,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A94" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="94">
+      <c r="A94" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="C94" s="1">
+      <c r="C94" s="1" t="n">
         <v>340</v>
       </c>
       <c r="D94" s="1" t="s">
@@ -2610,11 +2376,11 @@
         <v>139</v>
       </c>
     </row>
-    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A95" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="95">
+      <c r="A95" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="B95" s="1">
+      <c r="B95" s="1" t="n">
         <v>510</v>
       </c>
       <c r="D95" s="1" t="s">
@@ -2624,11 +2390,11 @@
         <v>141</v>
       </c>
     </row>
-    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A96" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="96">
+      <c r="A96" s="2" t="n">
         <v>43233</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B96" s="1" t="n">
         <v>170</v>
       </c>
       <c r="D96" s="1" t="s">
@@ -2638,11 +2404,11 @@
         <v>143</v>
       </c>
     </row>
-    <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A97" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="97">
+      <c r="A97" s="2" t="n">
         <v>43233</v>
       </c>
-      <c r="C97" s="1">
+      <c r="C97" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D97" s="1" t="s">
@@ -2652,11 +2418,11 @@
         <v>144</v>
       </c>
     </row>
-    <row r="98" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A98" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="98">
+      <c r="A98" s="2" t="n">
         <v>43234</v>
       </c>
-      <c r="C98" s="1">
+      <c r="C98" s="1" t="n">
         <v>299</v>
       </c>
       <c r="D98" s="1" t="s">
@@ -2666,11 +2432,11 @@
         <v>145</v>
       </c>
     </row>
-    <row r="99" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A99" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="99">
+      <c r="A99" s="2" t="n">
         <v>43236</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99" s="1" t="n">
         <v>3659</v>
       </c>
       <c r="D99" s="1" t="s">
@@ -2680,11 +2446,11 @@
         <v>146</v>
       </c>
     </row>
-    <row r="100" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A100" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="100">
+      <c r="A100" s="2" t="n">
         <v>43237</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B100" s="1" t="n">
         <v>79</v>
       </c>
       <c r="D100" s="1" t="s">
@@ -2694,11 +2460,11 @@
         <v>147</v>
       </c>
     </row>
-    <row r="101" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A101" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="101">
+      <c r="A101" s="2" t="n">
         <v>43236</v>
       </c>
-      <c r="C101" s="1">
+      <c r="C101" s="1" t="n">
         <v>173</v>
       </c>
       <c r="D101" s="1" t="s">
@@ -2708,11 +2474,11 @@
         <v>148</v>
       </c>
     </row>
-    <row r="102" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A102" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="102">
+      <c r="A102" s="2" t="n">
         <v>43240</v>
       </c>
-      <c r="B102" s="1">
+      <c r="B102" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D102" s="1" t="s">
@@ -2722,22 +2488,22 @@
         <v>149</v>
       </c>
     </row>
-    <row r="103" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A103" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="103">
+      <c r="A103" s="2" t="n">
         <v>43240</v>
       </c>
-      <c r="B103" s="1">
+      <c r="B103" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="104" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A104" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="104">
+      <c r="A104" s="2" t="n">
         <v>43241</v>
       </c>
-      <c r="B104" s="1">
+      <c r="B104" s="1" t="n">
         <v>4070</v>
       </c>
       <c r="D104" s="1" t="s">
@@ -2747,11 +2513,11 @@
         <v>150</v>
       </c>
     </row>
-    <row r="105" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A105" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="105">
+      <c r="A105" s="2" t="n">
         <v>43241</v>
       </c>
-      <c r="C105" s="1">
+      <c r="C105" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D105" s="1" t="s">
@@ -2761,11 +2527,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="106" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A106" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="106">
+      <c r="A106" s="2" t="n">
         <v>43242</v>
       </c>
-      <c r="B106" s="1">
+      <c r="B106" s="1" t="n">
         <v>79</v>
       </c>
       <c r="D106" s="1" t="s">
@@ -2775,11 +2541,11 @@
         <v>152</v>
       </c>
     </row>
-    <row r="107" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A107" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="107">
+      <c r="A107" s="2" t="n">
         <v>43246</v>
       </c>
-      <c r="B107" s="1">
+      <c r="B107" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D107" s="1" t="s">
@@ -2789,11 +2555,11 @@
         <v>154</v>
       </c>
     </row>
-    <row r="108" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A108" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="108">
+      <c r="A108" s="2" t="n">
         <v>43247</v>
       </c>
-      <c r="B108" s="1">
+      <c r="B108" s="1" t="n">
         <v>70</v>
       </c>
       <c r="D108" s="1" t="s">
@@ -2803,44 +2569,44 @@
         <v>156</v>
       </c>
     </row>
-    <row r="109" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A109" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="109">
+      <c r="A109" s="2" t="n">
         <v>43253</v>
       </c>
-      <c r="B109" s="1">
+      <c r="B109" s="1" t="n">
         <v>142</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A110" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="110">
+      <c r="A110" s="2" t="n">
         <v>43254</v>
       </c>
-      <c r="B110" s="1">
+      <c r="B110" s="1" t="n">
         <v>90</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="111" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A111" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="111">
+      <c r="A111" s="2" t="n">
         <v>43260</v>
       </c>
-      <c r="C111" s="1">
+      <c r="C111" s="1" t="n">
         <v>1400</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="112" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A112" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="112">
+      <c r="A112" s="2" t="n">
         <v>43260</v>
       </c>
-      <c r="C112" s="1">
+      <c r="C112" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D112" s="1" t="s">
@@ -2850,33 +2616,33 @@
         <v>91</v>
       </c>
     </row>
-    <row r="113" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A113" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="113">
+      <c r="A113" s="2" t="n">
         <v>43264</v>
       </c>
-      <c r="B113" s="1">
+      <c r="B113" s="1" t="n">
         <v>546</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="114" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A114" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="114">
+      <c r="A114" s="2" t="n">
         <v>43264</v>
       </c>
-      <c r="B114" s="1">
+      <c r="B114" s="1" t="n">
         <v>95</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="115" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A115" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="115">
+      <c r="A115" s="2" t="n">
         <v>43266</v>
       </c>
-      <c r="B115" s="1">
+      <c r="B115" s="1" t="n">
         <v>394</v>
       </c>
       <c r="D115" s="1" t="s">
@@ -2886,11 +2652,11 @@
         <v>163</v>
       </c>
     </row>
-    <row r="116" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A116" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="116">
+      <c r="A116" s="2" t="n">
         <v>43266</v>
       </c>
-      <c r="B116" s="1">
+      <c r="B116" s="1" t="n">
         <v>1055</v>
       </c>
       <c r="D116" s="1" t="s">
@@ -2900,11 +2666,11 @@
         <v>165</v>
       </c>
     </row>
-    <row r="117" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A117" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="117">
+      <c r="A117" s="2" t="n">
         <v>43284</v>
       </c>
-      <c r="C117" s="1">
+      <c r="C117" s="1" t="n">
         <v>274</v>
       </c>
       <c r="D117" s="1" t="s">
@@ -2914,11 +2680,11 @@
         <v>167</v>
       </c>
     </row>
-    <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A118" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="118">
+      <c r="A118" s="2" t="n">
         <v>43283</v>
       </c>
-      <c r="C118" s="1">
+      <c r="C118" s="1" t="n">
         <v>105</v>
       </c>
       <c r="D118" s="1" t="s">
@@ -2928,11 +2694,11 @@
         <v>169</v>
       </c>
     </row>
-    <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A119" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="119">
+      <c r="A119" s="2" t="n">
         <v>43289</v>
       </c>
-      <c r="C119" s="1">
+      <c r="C119" s="1" t="n">
         <v>128</v>
       </c>
       <c r="D119" s="1" t="s">
@@ -2942,11 +2708,11 @@
         <v>171</v>
       </c>
     </row>
-    <row r="120" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A120" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="120">
+      <c r="A120" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C120" s="1">
+      <c r="C120" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D120" s="1" t="s">
@@ -2956,11 +2722,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A121" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="121">
+      <c r="A121" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C121" s="1">
+      <c r="C121" s="1" t="n">
         <v>210</v>
       </c>
       <c r="D121" s="1" t="s">
@@ -2970,44 +2736,44 @@
         <v>173</v>
       </c>
     </row>
-    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A122" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="122">
+      <c r="A122" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B122" s="1">
+      <c r="B122" s="1" t="n">
         <v>980</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="123" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A123" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="123">
+      <c r="A123" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B123" s="1">
+      <c r="B123" s="1" t="n">
         <v>1260</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A124" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="124">
+      <c r="A124" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B124" s="1">
+      <c r="B124" s="1" t="n">
         <v>3687</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A125" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="125">
+      <c r="A125" s="2" t="n">
         <v>43298</v>
       </c>
-      <c r="C125" s="1">
+      <c r="C125" s="1" t="n">
         <v>60</v>
       </c>
       <c r="D125" s="1" t="s">
@@ -3017,55 +2783,55 @@
         <v>178</v>
       </c>
     </row>
-    <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A126" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="126">
+      <c r="A126" s="2" t="n">
         <v>43291</v>
       </c>
-      <c r="C126" s="1">
+      <c r="C126" s="1" t="n">
         <v>404</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A127" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="127">
+      <c r="A127" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C127" s="1">
+      <c r="C127" s="1" t="n">
         <v>451</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="128" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A128" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="128">
+      <c r="A128" s="2" t="n">
         <v>43298</v>
       </c>
-      <c r="C128" s="1">
+      <c r="C128" s="1" t="n">
         <v>708</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A129" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="129">
+      <c r="A129" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C129" s="1">
+      <c r="C129" s="1" t="n">
         <v>160</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A130" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="130">
+      <c r="A130" s="2" t="n">
         <v>43288</v>
       </c>
-      <c r="C130" s="1">
+      <c r="C130" s="1" t="n">
         <v>72</v>
       </c>
       <c r="D130" s="1" t="s">
@@ -3075,11 +2841,11 @@
         <v>181</v>
       </c>
     </row>
-    <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A131" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="131">
+      <c r="A131" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C131" s="1">
+      <c r="C131" s="1" t="n">
         <v>300</v>
       </c>
       <c r="D131" s="1" t="s">
@@ -3089,11 +2855,11 @@
         <v>183</v>
       </c>
     </row>
-    <row r="132" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A132" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="132">
+      <c r="A132" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C132" s="1">
+      <c r="C132" s="1" t="n">
         <v>230</v>
       </c>
       <c r="D132" s="1" t="s">
@@ -3103,22 +2869,22 @@
         <v>185</v>
       </c>
     </row>
-    <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A133" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="133">
+      <c r="A133" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C133" s="1">
+      <c r="C133" s="1" t="n">
         <v>454</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="134" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A134" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="134">
+      <c r="A134" s="2" t="n">
         <v>43299</v>
       </c>
-      <c r="C134" s="1">
+      <c r="C134" s="1" t="n">
         <v>686</v>
       </c>
       <c r="D134" s="1" t="s">
@@ -3128,11 +2894,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A135" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="135">
+      <c r="A135" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C135" s="1">
+      <c r="C135" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D135" s="1" t="s">
@@ -3142,11 +2908,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A136" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="136">
+      <c r="A136" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C136" s="1">
+      <c r="C136" s="1" t="n">
         <v>2067</v>
       </c>
       <c r="D136" s="1" t="s">
@@ -3156,11 +2922,11 @@
         <v>186</v>
       </c>
     </row>
-    <row r="137" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A137" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="137">
+      <c r="A137" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B137" s="1">
+      <c r="B137" s="1" t="n">
         <v>109</v>
       </c>
       <c r="D137" s="1" t="s">
@@ -3170,11 +2936,11 @@
         <v>187</v>
       </c>
     </row>
-    <row r="138" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A138" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="138">
+      <c r="A138" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B138" s="1">
+      <c r="B138" s="1" t="n">
         <v>97</v>
       </c>
       <c r="D138" s="1" t="s">
@@ -3184,11 +2950,11 @@
         <v>188</v>
       </c>
     </row>
-    <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A139" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="139">
+      <c r="A139" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B139" s="1">
+      <c r="B139" s="1" t="n">
         <v>1437</v>
       </c>
       <c r="D139" s="1" t="s">
@@ -3198,11 +2964,11 @@
         <v>189</v>
       </c>
     </row>
-    <row r="140" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A140" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="140">
+      <c r="A140" s="2" t="n">
         <v>43306</v>
       </c>
-      <c r="C140" s="1">
+      <c r="C140" s="1" t="n">
         <v>650</v>
       </c>
       <c r="D140" s="1" t="s">
@@ -3212,11 +2978,11 @@
         <v>190</v>
       </c>
     </row>
-    <row r="141" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A141" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="141">
+      <c r="A141" s="2" t="n">
         <v>43305</v>
       </c>
-      <c r="C141" s="1">
+      <c r="C141" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D141" s="1" t="s">
@@ -3226,11 +2992,11 @@
         <v>191</v>
       </c>
     </row>
-    <row r="142" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A142" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="142">
+      <c r="A142" s="2" t="n">
         <v>43309</v>
       </c>
-      <c r="C142" s="1">
+      <c r="C142" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D142" s="1" t="s">
@@ -3240,11 +3006,11 @@
         <v>192</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A143" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="0" r="143">
+      <c r="A143" s="2" t="n">
         <v>43306</v>
       </c>
-      <c r="B143" s="1">
+      <c r="B143" s="1" t="n">
         <v>167</v>
       </c>
       <c r="D143" s="1" t="s">
@@ -3254,11 +3020,11 @@
         <v>193</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A144" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="0" r="144">
+      <c r="A144" s="2" t="n">
         <v>43304</v>
       </c>
-      <c r="C144" s="1">
+      <c r="C144" s="1" t="n">
         <v>93</v>
       </c>
       <c r="D144" s="1" t="s">
@@ -3268,11 +3034,11 @@
         <v>194</v>
       </c>
     </row>
-    <row r="145" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A145" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="145">
+      <c r="A145" s="2" t="n">
         <v>43305</v>
       </c>
-      <c r="C145" s="1">
+      <c r="C145" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D145" s="1" t="s">
@@ -3282,11 +3048,11 @@
         <v>195</v>
       </c>
     </row>
-    <row r="146" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A146" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="146">
+      <c r="A146" s="2" t="n">
         <v>43303</v>
       </c>
-      <c r="C146" s="1">
+      <c r="C146" s="1" t="n">
         <v>244</v>
       </c>
       <c r="D146" s="1" t="s">
@@ -3296,11 +3062,11 @@
         <v>196</v>
       </c>
     </row>
-    <row r="147" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A147" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="147">
+      <c r="A147" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C147" s="1">
+      <c r="C147" s="1" t="n">
         <v>482</v>
       </c>
       <c r="D147" s="1" t="s">
@@ -3310,11 +3076,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="148" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A148" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="148">
+      <c r="A148" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C148" s="1">
+      <c r="C148" s="1" t="n">
         <v>172</v>
       </c>
       <c r="D148" s="1" t="s">
@@ -3324,44 +3090,44 @@
         <v>199</v>
       </c>
     </row>
-    <row r="149" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A149" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="149">
+      <c r="A149" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="B149" s="1">
+      <c r="B149" s="1" t="n">
         <v>89</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="150" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A150" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="150">
+      <c r="A150" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="C150" s="1">
+      <c r="C150" s="1" t="n">
         <v>107</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="151" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A151" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="151">
+      <c r="A151" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="C151" s="1">
+      <c r="C151" s="1" t="n">
         <v>124</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="152" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A152" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="152">
+      <c r="A152" s="7" t="n">
         <v>43316</v>
       </c>
-      <c r="C152" s="1">
+      <c r="C152" s="1" t="n">
         <v>4500</v>
       </c>
       <c r="D152" s="1" t="s">
@@ -3371,11 +3137,11 @@
         <v>202</v>
       </c>
     </row>
-    <row r="153" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A153" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="153">
+      <c r="A153" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C153" s="1">
+      <c r="C153" s="1" t="n">
         <v>247</v>
       </c>
       <c r="D153" s="1" t="s">
@@ -3385,11 +3151,11 @@
         <v>204</v>
       </c>
     </row>
-    <row r="154" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A154" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="154">
+      <c r="A154" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C154" s="1">
+      <c r="C154" s="1" t="n">
         <v>1150</v>
       </c>
       <c r="D154" s="1" t="s">
@@ -3399,11 +3165,11 @@
         <v>205</v>
       </c>
     </row>
-    <row r="155" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A155" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="155">
+      <c r="A155" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C155" s="1">
+      <c r="C155" s="1" t="n">
         <v>313</v>
       </c>
       <c r="D155" s="1" t="s">
@@ -3413,11 +3179,11 @@
         <v>207</v>
       </c>
     </row>
-    <row r="156" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A156" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="156">
+      <c r="A156" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="B156" s="1">
+      <c r="B156" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D156" s="1" t="s">
@@ -3427,11 +3193,11 @@
         <v>209</v>
       </c>
     </row>
-    <row r="157" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A157" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="157">
+      <c r="A157" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="C157" s="1">
+      <c r="C157" s="1" t="n">
         <v>710</v>
       </c>
       <c r="D157" s="1" t="s">
@@ -3441,11 +3207,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A158" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="158">
+      <c r="A158" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="C158" s="1">
+      <c r="C158" s="1" t="n">
         <v>100</v>
       </c>
       <c r="D158" s="1" t="s">
@@ -3455,11 +3221,11 @@
         <v>212</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A159" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="159">
+      <c r="A159" s="2" t="n">
         <v>43319</v>
       </c>
-      <c r="B159" s="1">
+      <c r="B159" s="1" t="n">
         <v>78</v>
       </c>
       <c r="D159" s="1" t="s">
@@ -3469,22 +3235,22 @@
         <v>213</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A160" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="160">
+      <c r="A160" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="B160" s="1">
+      <c r="B160" s="1" t="n">
         <v>1840</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A161" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="161">
+      <c r="A161" s="2" t="n">
         <v>43322</v>
       </c>
-      <c r="B161" s="1">
+      <c r="B161" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D161" s="1" t="s">
@@ -3494,11 +3260,11 @@
         <v>216</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A162" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="162">
+      <c r="A162" s="7" t="n">
         <v>43324</v>
       </c>
-      <c r="C162" s="1">
+      <c r="C162" s="1" t="n">
         <v>230</v>
       </c>
       <c r="D162" s="1" t="s">
@@ -3508,11 +3274,11 @@
         <v>217</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A163" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="163">
+      <c r="A163" s="7" t="n">
         <v>43326</v>
       </c>
-      <c r="C163" s="1">
+      <c r="C163" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D163" s="1" t="s">
@@ -3522,11 +3288,11 @@
         <v>219</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A164" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="164">
+      <c r="A164" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="B164" s="1">
+      <c r="B164" s="1" t="n">
         <v>45</v>
       </c>
       <c r="D164" s="1" t="s">
@@ -3536,417 +3302,444 @@
         <v>221</v>
       </c>
     </row>
-    <row r="165" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A165" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="165">
+      <c r="A165" s="10" t="n">
         <v>43327</v>
       </c>
-      <c r="C165">
+      <c r="C165" s="0" t="n">
         <v>486</v>
       </c>
-      <c r="D165" t="s">
+      <c r="D165" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E165" t="s">
+      <c r="E165" s="0" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="166" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A166" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="166">
+      <c r="A166" s="10" t="n">
         <v>43329</v>
       </c>
-      <c r="C166">
+      <c r="C166" s="0" t="n">
         <v>92</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D166" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="E166" t="s">
+      <c r="E166" s="0" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A167" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="167">
+      <c r="A167" s="10" t="n">
         <v>43331</v>
       </c>
-      <c r="C167">
+      <c r="C167" s="0" t="n">
         <v>310</v>
       </c>
-      <c r="D167" t="s">
+      <c r="D167" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="E167" t="s">
+      <c r="E167" s="0" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A168" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="168">
+      <c r="A168" s="10" t="n">
         <v>43334</v>
       </c>
-      <c r="C168">
+      <c r="C168" s="0" t="n">
         <v>464</v>
       </c>
-      <c r="D168" t="s">
+      <c r="D168" s="0" t="s">
         <v>218</v>
       </c>
       <c r="E168" s="11" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A169" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="169">
+      <c r="A169" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="C169">
+      <c r="C169" s="0" t="n">
         <v>726</v>
       </c>
-      <c r="D169" t="s">
+      <c r="D169" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="E169" t="s">
+      <c r="E169" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A170" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="170">
+      <c r="A170" s="10" t="n">
         <v>43337</v>
       </c>
-      <c r="C170">
+      <c r="C170" s="0" t="n">
         <v>544</v>
       </c>
-      <c r="D170" t="s">
+      <c r="D170" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E170" t="s">
+      <c r="E170" s="0" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A171" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="171">
+      <c r="A171" s="10" t="n">
         <v>43337</v>
       </c>
-      <c r="B171">
+      <c r="B171" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D171" t="s">
+      <c r="D171" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="E171" t="s">
+      <c r="E171" s="0" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A172" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="172">
+      <c r="A172" s="10" t="n">
         <v>43341</v>
       </c>
-      <c r="C172">
+      <c r="C172" s="0" t="n">
         <v>830</v>
       </c>
-      <c r="D172" t="s">
+      <c r="D172" s="0" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A173" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="173">
+      <c r="A173" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="C173">
+      <c r="C173" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="D173" t="s">
+      <c r="D173" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="E173" t="s">
+      <c r="E173" s="0" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A174" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="174">
+      <c r="A174" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="B174">
+      <c r="B174" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D174" t="s">
+      <c r="D174" s="0" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A175" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="175">
+      <c r="A175" s="10" t="n">
         <v>43344</v>
       </c>
-      <c r="B175">
+      <c r="B175" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="D175" t="s">
+      <c r="D175" s="0" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A176" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="176">
+      <c r="A176" s="10" t="n">
         <v>43344</v>
       </c>
-      <c r="B176">
+      <c r="B176" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D176" t="s">
+      <c r="D176" s="0" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A177" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="177">
+      <c r="A177" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C177">
+      <c r="C177" s="0" t="n">
         <v>607</v>
       </c>
-      <c r="D177" t="s">
+      <c r="D177" s="0" t="s">
         <v>235</v>
       </c>
-      <c r="E177" t="s">
+      <c r="E177" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A178" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="178">
+      <c r="A178" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C178">
+      <c r="C178" s="0" t="n">
         <v>444</v>
       </c>
-      <c r="D178" t="s">
+      <c r="D178" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E178" t="s">
+      <c r="E178" s="0" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A179" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="179">
+      <c r="A179" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C179">
+      <c r="C179" s="0" t="n">
         <v>312</v>
       </c>
-      <c r="D179" t="s">
+      <c r="D179" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="E179" t="s">
+      <c r="E179" s="0" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A180" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="180">
+      <c r="A180" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C180">
+      <c r="C180" s="0" t="n">
         <v>501</v>
       </c>
-      <c r="D180" t="s">
+      <c r="D180" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E180" t="s">
+      <c r="E180" s="0" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A181" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="181">
+      <c r="A181" s="10" t="n">
         <v>43349</v>
       </c>
-      <c r="C181">
+      <c r="C181" s="0" t="n">
         <v>711</v>
       </c>
-      <c r="D181" t="s">
+      <c r="D181" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="E181" t="s">
+      <c r="E181" s="0" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A182" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="182">
+      <c r="A182" s="10" t="n">
         <v>43354</v>
       </c>
-      <c r="B182">
+      <c r="B182" s="0" t="n">
         <v>126</v>
       </c>
-      <c r="D182" t="s">
+      <c r="D182" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="E182" t="s">
+      <c r="E182" s="0" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A183" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="183">
+      <c r="A183" s="10" t="n">
         <v>43354</v>
       </c>
-      <c r="C183">
+      <c r="C183" s="0" t="n">
         <v>450</v>
       </c>
-      <c r="D183" t="s">
+      <c r="D183" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="E183" t="s">
+      <c r="E183" s="0" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A184" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="184">
+      <c r="A184" s="10" t="n">
         <v>43361</v>
       </c>
-      <c r="C184">
+      <c r="C184" s="0" t="n">
         <v>660</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D184" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="E184" t="s">
+      <c r="E184" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A185" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="185">
+      <c r="A185" s="10" t="n">
         <v>43363</v>
       </c>
-      <c r="C185">
+      <c r="C185" s="0" t="n">
         <v>230</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D185" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="E185" t="s">
+      <c r="E185" s="0" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A186" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="186">
+      <c r="A186" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B186">
+      <c r="B186" s="0" t="n">
         <v>4859</v>
       </c>
-      <c r="D186" t="s">
+      <c r="D186" s="0" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A187" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="187">
+      <c r="A187" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B187">
+      <c r="B187" s="0" t="n">
         <v>295</v>
       </c>
-      <c r="D187" t="s">
+      <c r="D187" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="E187" t="s">
+      <c r="E187" s="0" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A188" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="188">
+      <c r="A188" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B188">
+      <c r="B188" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D188" t="s">
+      <c r="D188" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="E188" t="s">
+      <c r="E188" s="0" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A189" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="189">
+      <c r="A189" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B189">
+      <c r="B189" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="D189" t="s">
+      <c r="D189" s="0" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A190" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="190">
+      <c r="A190" s="10" t="n">
         <v>43378</v>
       </c>
-      <c r="B190">
+      <c r="B190" s="0" t="n">
         <v>506</v>
       </c>
-      <c r="D190" t="s">
+      <c r="D190" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="E190" t="s">
+      <c r="E190" s="0" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A191" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="191">
+      <c r="A191" s="10" t="n">
         <v>43379</v>
       </c>
-      <c r="B191">
+      <c r="B191" s="0" t="n">
         <v>350</v>
       </c>
-      <c r="D191" t="s">
+      <c r="D191" s="0" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A192" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="192">
+      <c r="A192" s="10" t="n">
         <v>43383</v>
       </c>
-      <c r="B192">
+      <c r="B192" s="0" t="n">
         <v>189</v>
       </c>
-      <c r="D192" t="s">
+      <c r="D192" s="0" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A193" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="193">
+      <c r="A193" s="10" t="n">
         <v>43387</v>
       </c>
-      <c r="B193">
+      <c r="B193" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="D193" t="s">
+      <c r="D193" s="0" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A194" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="194">
+      <c r="A194" s="10" t="n">
         <v>43387</v>
       </c>
-      <c r="B194">
+      <c r="B194" s="0" t="n">
         <v>307</v>
       </c>
-      <c r="D194" t="s">
+      <c r="D194" s="0" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B207">
-        <f>SUM(B2:B206)</f>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="195">
+      <c r="C195" s="0" t="n">
+        <v>3705</v>
+      </c>
+      <c r="E195" s="0" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="196">
+      <c r="A196" s="10" t="n">
+        <v>43385</v>
+      </c>
+      <c r="C196" s="0" t="n">
+        <v>608</v>
+      </c>
+      <c r="D196" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="E196" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="207">
+      <c r="B207" s="0" t="n">
+        <f aca="false">SUM(B2:B206)</f>
         <v>46063</v>
       </c>
-      <c r="C207">
-        <f>SUM(C2:C206)</f>
-        <v>42295</v>
+      <c r="C207" s="0" t="n">
+        <f aca="false">SUM(C2:C206)</f>
+        <v>46608</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A30:Z32">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule aboveAverage="0" bottom="0" dxfId="0" operator="expression" percent="0" priority="2" rank="0" text="" type="expression">
       <formula>LEN(TRIM(A30))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D33" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D40" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink display="netonnet.se" ref="D33" r:id="rId1"/>
+    <hyperlink display="www.vidaxl.se" ref="D40" r:id="rId2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cost update jenny 1024
</commit_message>
<xml_diff>
--- a/Cost.xlsx
+++ b/Cost.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chengkaiyan/github/cost/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7CB356A-D429-A74C-881B-F4DACE4325EB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="261">
   <si>
     <t>日期</t>
   </si>
@@ -793,52 +788,81 @@
     <t>鸡蛋仔</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.vardia.se/ </t>
+    <t>https://www.vardia.se/ </t>
   </si>
   <si>
     <t>house insurance</t>
+  </si>
+  <si>
+    <t>kistagrossen</t>
+  </si>
+  <si>
+    <t>paprika; toothpaste;luobo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="yyyy/m/d"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt formatCode="YYYY/M/D" numFmtId="165"/>
+    <numFmt formatCode="M/D/YYYY" numFmtId="166"/>
+    <numFmt formatCode="YYYY\-MM\-DD" numFmtId="167"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <family val="0"/>
       <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
       <name val="Arial"/>
       <family val="2"/>
+      <sz val="10"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF666666"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF666666"/>
+      <sz val="11"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF0563C1"/>
+      <sz val="10"/>
+      <u val="single"/>
+    </font>
+    <font>
+      <name val="FreeSans"/>
+      <family val="2"/>
+      <color rgb="FF0563C1"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
   </fonts>
   <fills count="5">
@@ -868,7 +892,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
@@ -876,30 +900,96 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="167" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="20">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="7">
+    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle builtinId="8" customBuiltin="false" name="*unknown*" xfId="20"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -910,7 +1000,6 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -935,7 +1024,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FF0563C1"/>
       <rgbColor rgb="FFE1DCDC"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -969,339 +1058,31 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:Z207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A188" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E202" sqref="E202"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A188" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D205" activeCellId="0" pane="topLeft" sqref="D205"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="3" width="14.5"/>
-    <col min="4" max="4" width="26"/>
-    <col min="5" max="5" width="37.83203125"/>
-    <col min="6" max="1025" width="14.5"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="14.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1318,11 +1099,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="2">
+      <c r="A2" s="2" t="n">
         <v>43121</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="1" t="n">
         <v>250</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1332,11 +1113,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="3">
+      <c r="A3" s="2" t="n">
         <v>43122</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="1" t="n">
         <v>305</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1346,11 +1127,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="4">
+      <c r="A4" s="2" t="n">
         <v>43122</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1360,11 +1141,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="5">
+      <c r="A5" s="2" t="n">
         <v>43125</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="1" t="n">
         <v>98</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1374,11 +1155,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="6">
+      <c r="A6" s="2" t="n">
         <v>43126</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1388,11 +1169,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="7">
+      <c r="A7" s="2" t="n">
         <v>43127</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1402,11 +1183,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="8">
+      <c r="A8" s="2" t="n">
         <v>43128</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="1" t="n">
         <v>656</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1416,11 +1197,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="9">
+      <c r="A9" s="2" t="n">
         <v>43131</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="1" t="n">
         <v>486</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1430,11 +1211,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="10">
+      <c r="A10" s="2" t="n">
         <v>43132</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="1" t="n">
         <v>76</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1444,11 +1225,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="11">
+      <c r="A11" s="2" t="n">
         <v>43133</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="1" t="n">
         <v>399</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1458,11 +1239,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="12">
+      <c r="A12" s="2" t="n">
         <v>43135</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="1" t="n">
         <v>419</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1472,11 +1253,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="13">
+      <c r="A13" s="2" t="n">
         <v>43136</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="1" t="n">
         <v>521</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1486,11 +1267,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="14">
+      <c r="A14" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="1" t="n">
         <v>399</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1500,11 +1281,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="15">
+      <c r="A15" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="1" t="n">
         <v>138</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1514,11 +1295,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="16">
+      <c r="A16" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="1" t="n">
         <v>310</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1528,12 +1309,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="17">
+      <c r="A17" s="2" t="n">
         <v>43138</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="1">
+      <c r="C17" s="1" t="n">
         <v>700</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1543,12 +1324,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="18">
+      <c r="A18" s="2" t="n">
         <v>43141</v>
       </c>
-      <c r="C18" s="1">
-        <f>F18*G18</f>
+      <c r="C18" s="1" t="n">
+        <f aca="false">F18*G18</f>
         <v>1312</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -1557,18 +1338,18 @@
       <c r="E18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="1" t="n">
         <v>164</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="1" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="19">
+      <c r="A19" s="2" t="n">
         <v>43141</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="1" t="n">
         <v>1190</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1578,11 +1359,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="20">
+      <c r="A20" s="2" t="n">
         <v>43154</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="1" t="n">
         <v>438</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1592,11 +1373,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="21">
+      <c r="A21" s="2" t="n">
         <v>43154</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="1" t="n">
         <v>248</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -1606,22 +1387,22 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="22">
+      <c r="A22" s="2" t="n">
         <v>43166</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="1" t="n">
         <v>234</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="23">
+      <c r="A23" s="2" t="n">
         <v>43171</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="1" t="n">
         <v>118</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1631,22 +1412,22 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="24">
+      <c r="A24" s="2" t="n">
         <v>43173</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="1" t="n">
         <v>82</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="25">
+      <c r="A25" s="2" t="n">
         <v>43174</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1656,22 +1437,22 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="26">
+      <c r="A26" s="2" t="n">
         <v>43175</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="1" t="n">
         <v>370</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="27">
+      <c r="A27" s="2" t="n">
         <v>43175</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -1681,11 +1462,11 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="28">
+      <c r="A28" s="2" t="n">
         <v>43176</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="1" t="n">
         <v>624</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -1695,11 +1476,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="29">
+      <c r="A29" s="2" t="n">
         <v>43177</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="1" t="n">
         <v>170</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1709,22 +1490,22 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="30">
+      <c r="A30" s="4" t="n">
         <v>43179</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="31">
+      <c r="A31" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="1" t="n">
         <v>90</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -1734,11 +1515,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="32">
+      <c r="A32" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="1" t="n">
         <v>72</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -1748,11 +1529,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="33">
+      <c r="A33" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="1" t="n">
         <v>908</v>
       </c>
       <c r="D33" s="6" t="s">
@@ -1762,11 +1543,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="34">
+      <c r="A34" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -1776,11 +1557,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="35">
+      <c r="A35" s="2" t="n">
         <v>43181</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -1790,11 +1571,11 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="36">
+      <c r="A36" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="1" t="n">
         <v>135</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -1804,11 +1585,11 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="37">
+      <c r="A37" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="1" t="n">
         <v>110</v>
       </c>
       <c r="C37" s="1"/>
@@ -1840,11 +1621,11 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="38">
+      <c r="A38" s="2" t="n">
         <v>43185</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="1" t="n">
         <v>122</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -1854,22 +1635,22 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="39">
+      <c r="A39" s="2" t="n">
         <v>43187</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="1" t="n">
         <v>750</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="40">
+      <c r="A40" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="1" t="n">
         <v>379</v>
       </c>
       <c r="D40" s="6" t="s">
@@ -1879,22 +1660,22 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="41">
+      <c r="A41" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="1" t="n">
         <v>240</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="42">
+      <c r="A42" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="1" t="n">
         <v>540</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -1904,11 +1685,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="43">
+      <c r="A43" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -1918,11 +1699,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="44">
+      <c r="A44" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -1932,11 +1713,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="45">
+      <c r="A45" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="1" t="n">
         <v>462</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -1946,11 +1727,11 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="46">
+      <c r="A46" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46" s="1" t="n">
         <v>70</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -1960,11 +1741,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="47">
+      <c r="A47" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -1974,11 +1755,11 @@
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="1:26" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="48">
+      <c r="A48" s="2" t="n">
         <v>43190</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="1" t="n">
         <v>30</v>
       </c>
       <c r="C48" s="1"/>
@@ -1989,11 +1770,11 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="49">
+      <c r="A49" s="2" t="n">
         <v>43191</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="1" t="n">
         <v>40</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -2003,11 +1784,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="50">
+      <c r="A50" s="7" t="n">
         <v>43193</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50" s="1" t="n">
         <v>150</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -2017,11 +1798,11 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="51">
+      <c r="A51" s="2" t="n">
         <v>43194</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51" s="1" t="n">
         <v>1360</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -2031,11 +1812,11 @@
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="52">
+      <c r="A52" s="2" t="n">
         <v>43195</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" s="1" t="n">
         <v>94</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -2045,11 +1826,11 @@
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="53">
+      <c r="A53" s="2" t="n">
         <v>43196</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C53" s="1" t="n">
         <v>48</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -2059,11 +1840,11 @@
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="54">
+      <c r="A54" s="2" t="n">
         <v>43196</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C54" s="1" t="n">
         <v>205</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -2073,11 +1854,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="55">
+      <c r="A55" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -2087,11 +1868,11 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="56">
+      <c r="A56" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56" s="1" t="n">
         <v>421</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -2101,11 +1882,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="57">
+      <c r="A57" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="1" t="n">
         <v>191</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -2115,11 +1896,11 @@
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="58">
+      <c r="A58" s="2" t="n">
         <v>43198</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58" s="1" t="n">
         <v>226</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -2129,22 +1910,22 @@
         <v>96</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="59">
+      <c r="A59" s="2" t="n">
         <v>43200</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59" s="1" t="n">
         <v>250</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="60">
+      <c r="A60" s="2" t="n">
         <v>43200</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60" s="1" t="n">
         <v>1115</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -2154,11 +1935,11 @@
         <v>99</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="61">
+      <c r="A61" s="2" t="n">
         <v>43201</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -2168,11 +1949,11 @@
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="62">
+      <c r="A62" s="2" t="n">
         <v>43201</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62" s="1" t="n">
         <v>88</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -2182,11 +1963,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="63">
+      <c r="A63" s="2" t="n">
         <v>43203</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -2196,11 +1977,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="64">
+      <c r="A64" s="2" t="n">
         <v>43203</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C64" s="1" t="n">
         <v>364</v>
       </c>
       <c r="D64" s="1" t="s">
@@ -2210,11 +1991,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="65">
+      <c r="A65" s="2" t="n">
         <v>43204</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65" s="1" t="n">
         <v>65</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -2224,11 +2005,11 @@
         <v>105</v>
       </c>
     </row>
-    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="66">
+      <c r="A66" s="2" t="n">
         <v>43208</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -2238,11 +2019,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="67">
+      <c r="A67" s="2" t="n">
         <v>43208</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C67" s="1" t="n">
         <v>470</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -2252,11 +2033,11 @@
         <v>107</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="68">
+      <c r="A68" s="2" t="n">
         <v>43209</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68" s="1" t="n">
         <v>180</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -2266,11 +2047,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A69" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="69">
+      <c r="A69" s="2" t="n">
         <v>43210</v>
       </c>
-      <c r="C69" s="1">
+      <c r="C69" s="1" t="n">
         <v>420</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -2280,11 +2061,11 @@
         <v>109</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="70">
+      <c r="A70" s="2" t="n">
         <v>43212</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70" s="1" t="n">
         <v>50</v>
       </c>
       <c r="D70" s="1" t="s">
@@ -2294,11 +2075,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="71">
+      <c r="A71" s="2" t="n">
         <v>43212</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71" s="1" t="n">
         <v>164</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -2308,11 +2089,11 @@
         <v>112</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="72">
+      <c r="A72" s="2" t="n">
         <v>43215</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B72" s="1" t="n">
         <v>300</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -2322,11 +2103,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="73">
+      <c r="A73" s="2" t="n">
         <v>43217</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73" s="1" t="n">
         <v>364</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -2336,11 +2117,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A74" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="74">
+      <c r="A74" s="2" t="n">
         <v>43218</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74" s="1" t="n">
         <v>185</v>
       </c>
       <c r="D74" s="1" t="s">
@@ -2350,11 +2131,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A75" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="75">
+      <c r="A75" s="2" t="n">
         <v>43218</v>
       </c>
-      <c r="C75" s="1">
+      <c r="C75" s="1" t="n">
         <v>404</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -2364,11 +2145,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="76">
+      <c r="A76" s="2" t="n">
         <v>43220</v>
       </c>
-      <c r="C76" s="1">
+      <c r="C76" s="1" t="n">
         <v>57</v>
       </c>
       <c r="D76" s="1" t="s">
@@ -2378,11 +2159,11 @@
         <v>114</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="77">
+      <c r="A77" s="2" t="n">
         <v>43221</v>
       </c>
-      <c r="C77" s="1">
+      <c r="C77" s="1" t="n">
         <v>282</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -2392,11 +2173,11 @@
         <v>116</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="78">
+      <c r="A78" s="2" t="n">
         <v>43220</v>
       </c>
-      <c r="C78" s="1">
+      <c r="C78" s="1" t="n">
         <v>87</v>
       </c>
       <c r="D78" s="1" t="s">
@@ -2406,11 +2187,11 @@
         <v>117</v>
       </c>
     </row>
-    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A79" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="79">
+      <c r="A79" s="2" t="n">
         <v>43223</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B79" s="1" t="n">
         <v>1878</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -2420,11 +2201,11 @@
         <v>119</v>
       </c>
     </row>
-    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A80" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="80">
+      <c r="A80" s="2" t="n">
         <v>43224</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B80" s="1" t="n">
         <v>98</v>
       </c>
       <c r="D80" s="1" t="s">
@@ -2434,11 +2215,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A81" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="81">
+      <c r="A81" s="2" t="n">
         <v>43225</v>
       </c>
-      <c r="C81" s="1">
+      <c r="C81" s="1" t="n">
         <v>198</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -2448,11 +2229,11 @@
         <v>122</v>
       </c>
     </row>
-    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A82" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="82">
+      <c r="A82" s="2" t="n">
         <v>43225</v>
       </c>
-      <c r="C82" s="1">
+      <c r="C82" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -2462,11 +2243,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="83">
+      <c r="A83" s="2" t="n">
         <v>43228</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83" s="1" t="n">
         <v>168</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -2476,11 +2257,11 @@
         <v>124</v>
       </c>
     </row>
-    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A84" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="84">
+      <c r="A84" s="2" t="n">
         <v>43229</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B84" s="1" t="n">
         <v>240</v>
       </c>
       <c r="D84" s="1" t="s">
@@ -2490,12 +2271,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A85" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="85">
+      <c r="A85" s="2" t="n">
         <v>43230</v>
       </c>
       <c r="B85" s="1"/>
-      <c r="C85" s="1">
+      <c r="C85" s="1" t="n">
         <v>420</v>
       </c>
       <c r="D85" s="1" t="s">
@@ -2505,11 +2286,11 @@
         <v>126</v>
       </c>
     </row>
-    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A86" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="86">
+      <c r="A86" s="2" t="n">
         <v>43230</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B86" s="1" t="n">
         <v>200</v>
       </c>
       <c r="C86" s="1"/>
@@ -2520,11 +2301,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A87" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="87">
+      <c r="A87" s="2" t="n">
         <v>43230</v>
       </c>
-      <c r="C87" s="1">
+      <c r="C87" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D87" s="1" t="s">
@@ -2534,11 +2315,11 @@
         <v>128</v>
       </c>
     </row>
-    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A88" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="88">
+      <c r="A88" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B88" s="1" t="n">
         <v>462</v>
       </c>
       <c r="D88" s="1" t="s">
@@ -2548,11 +2329,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A89" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="89">
+      <c r="A89" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B89" s="1" t="n">
         <v>499</v>
       </c>
       <c r="D89" s="1" t="s">
@@ -2562,11 +2343,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A90" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="90">
+      <c r="A90" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B90" s="1">
+      <c r="B90" s="1" t="n">
         <v>398</v>
       </c>
       <c r="D90" s="1" t="s">
@@ -2576,11 +2357,11 @@
         <v>133</v>
       </c>
     </row>
-    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A91" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="91">
+      <c r="A91" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B91" s="1">
+      <c r="B91" s="1" t="n">
         <v>226</v>
       </c>
       <c r="D91" s="1" t="s">
@@ -2590,11 +2371,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A92" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="92">
+      <c r="A92" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B92" s="1">
+      <c r="B92" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D92" s="1" t="s">
@@ -2604,11 +2385,11 @@
         <v>137</v>
       </c>
     </row>
-    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A93" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="93">
+      <c r="A93" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="B93" s="1">
+      <c r="B93" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D93" s="1" t="s">
@@ -2618,11 +2399,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A94" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="94">
+      <c r="A94" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="C94" s="1">
+      <c r="C94" s="1" t="n">
         <v>340</v>
       </c>
       <c r="D94" s="1" t="s">
@@ -2632,11 +2413,11 @@
         <v>139</v>
       </c>
     </row>
-    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A95" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="95">
+      <c r="A95" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="B95" s="1">
+      <c r="B95" s="1" t="n">
         <v>510</v>
       </c>
       <c r="D95" s="1" t="s">
@@ -2646,11 +2427,11 @@
         <v>141</v>
       </c>
     </row>
-    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A96" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="96">
+      <c r="A96" s="2" t="n">
         <v>43233</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B96" s="1" t="n">
         <v>170</v>
       </c>
       <c r="D96" s="1" t="s">
@@ -2660,11 +2441,11 @@
         <v>143</v>
       </c>
     </row>
-    <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A97" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="97">
+      <c r="A97" s="2" t="n">
         <v>43233</v>
       </c>
-      <c r="C97" s="1">
+      <c r="C97" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D97" s="1" t="s">
@@ -2674,11 +2455,11 @@
         <v>144</v>
       </c>
     </row>
-    <row r="98" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A98" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="98">
+      <c r="A98" s="2" t="n">
         <v>43234</v>
       </c>
-      <c r="C98" s="1">
+      <c r="C98" s="1" t="n">
         <v>299</v>
       </c>
       <c r="D98" s="1" t="s">
@@ -2688,11 +2469,11 @@
         <v>145</v>
       </c>
     </row>
-    <row r="99" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A99" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="99">
+      <c r="A99" s="2" t="n">
         <v>43236</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99" s="1" t="n">
         <v>3659</v>
       </c>
       <c r="D99" s="1" t="s">
@@ -2702,11 +2483,11 @@
         <v>146</v>
       </c>
     </row>
-    <row r="100" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A100" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="100">
+      <c r="A100" s="2" t="n">
         <v>43237</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B100" s="1" t="n">
         <v>79</v>
       </c>
       <c r="D100" s="1" t="s">
@@ -2716,11 +2497,11 @@
         <v>147</v>
       </c>
     </row>
-    <row r="101" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A101" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="101">
+      <c r="A101" s="2" t="n">
         <v>43236</v>
       </c>
-      <c r="C101" s="1">
+      <c r="C101" s="1" t="n">
         <v>173</v>
       </c>
       <c r="D101" s="1" t="s">
@@ -2730,11 +2511,11 @@
         <v>148</v>
       </c>
     </row>
-    <row r="102" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A102" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="102">
+      <c r="A102" s="2" t="n">
         <v>43240</v>
       </c>
-      <c r="B102" s="1">
+      <c r="B102" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D102" s="1" t="s">
@@ -2744,22 +2525,22 @@
         <v>149</v>
       </c>
     </row>
-    <row r="103" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A103" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="103">
+      <c r="A103" s="2" t="n">
         <v>43240</v>
       </c>
-      <c r="B103" s="1">
+      <c r="B103" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="104" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A104" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="104">
+      <c r="A104" s="2" t="n">
         <v>43241</v>
       </c>
-      <c r="B104" s="1">
+      <c r="B104" s="1" t="n">
         <v>4070</v>
       </c>
       <c r="D104" s="1" t="s">
@@ -2769,11 +2550,11 @@
         <v>150</v>
       </c>
     </row>
-    <row r="105" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A105" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="105">
+      <c r="A105" s="2" t="n">
         <v>43241</v>
       </c>
-      <c r="C105" s="1">
+      <c r="C105" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D105" s="1" t="s">
@@ -2783,11 +2564,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="106" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A106" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="106">
+      <c r="A106" s="2" t="n">
         <v>43242</v>
       </c>
-      <c r="B106" s="1">
+      <c r="B106" s="1" t="n">
         <v>79</v>
       </c>
       <c r="D106" s="1" t="s">
@@ -2797,11 +2578,11 @@
         <v>152</v>
       </c>
     </row>
-    <row r="107" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A107" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="107">
+      <c r="A107" s="2" t="n">
         <v>43246</v>
       </c>
-      <c r="B107" s="1">
+      <c r="B107" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D107" s="1" t="s">
@@ -2811,11 +2592,11 @@
         <v>154</v>
       </c>
     </row>
-    <row r="108" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A108" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="108">
+      <c r="A108" s="2" t="n">
         <v>43247</v>
       </c>
-      <c r="B108" s="1">
+      <c r="B108" s="1" t="n">
         <v>70</v>
       </c>
       <c r="D108" s="1" t="s">
@@ -2825,44 +2606,44 @@
         <v>156</v>
       </c>
     </row>
-    <row r="109" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A109" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="109">
+      <c r="A109" s="2" t="n">
         <v>43253</v>
       </c>
-      <c r="B109" s="1">
+      <c r="B109" s="1" t="n">
         <v>142</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A110" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="110">
+      <c r="A110" s="2" t="n">
         <v>43254</v>
       </c>
-      <c r="B110" s="1">
+      <c r="B110" s="1" t="n">
         <v>90</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="111" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A111" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="111">
+      <c r="A111" s="2" t="n">
         <v>43260</v>
       </c>
-      <c r="C111" s="1">
+      <c r="C111" s="1" t="n">
         <v>1400</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="112" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A112" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="112">
+      <c r="A112" s="2" t="n">
         <v>43260</v>
       </c>
-      <c r="C112" s="1">
+      <c r="C112" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D112" s="1" t="s">
@@ -2872,33 +2653,33 @@
         <v>91</v>
       </c>
     </row>
-    <row r="113" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A113" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="113">
+      <c r="A113" s="2" t="n">
         <v>43264</v>
       </c>
-      <c r="B113" s="1">
+      <c r="B113" s="1" t="n">
         <v>546</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="114" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A114" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="114">
+      <c r="A114" s="2" t="n">
         <v>43264</v>
       </c>
-      <c r="B114" s="1">
+      <c r="B114" s="1" t="n">
         <v>95</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="115" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A115" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="115">
+      <c r="A115" s="2" t="n">
         <v>43266</v>
       </c>
-      <c r="B115" s="1">
+      <c r="B115" s="1" t="n">
         <v>394</v>
       </c>
       <c r="D115" s="1" t="s">
@@ -2908,11 +2689,11 @@
         <v>163</v>
       </c>
     </row>
-    <row r="116" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A116" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="116">
+      <c r="A116" s="2" t="n">
         <v>43266</v>
       </c>
-      <c r="B116" s="1">
+      <c r="B116" s="1" t="n">
         <v>1055</v>
       </c>
       <c r="D116" s="1" t="s">
@@ -2922,11 +2703,11 @@
         <v>165</v>
       </c>
     </row>
-    <row r="117" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A117" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="117">
+      <c r="A117" s="2" t="n">
         <v>43284</v>
       </c>
-      <c r="C117" s="1">
+      <c r="C117" s="1" t="n">
         <v>274</v>
       </c>
       <c r="D117" s="1" t="s">
@@ -2936,11 +2717,11 @@
         <v>167</v>
       </c>
     </row>
-    <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A118" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="118">
+      <c r="A118" s="2" t="n">
         <v>43283</v>
       </c>
-      <c r="C118" s="1">
+      <c r="C118" s="1" t="n">
         <v>105</v>
       </c>
       <c r="D118" s="1" t="s">
@@ -2950,11 +2731,11 @@
         <v>169</v>
       </c>
     </row>
-    <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A119" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="119">
+      <c r="A119" s="2" t="n">
         <v>43289</v>
       </c>
-      <c r="C119" s="1">
+      <c r="C119" s="1" t="n">
         <v>128</v>
       </c>
       <c r="D119" s="1" t="s">
@@ -2964,11 +2745,11 @@
         <v>171</v>
       </c>
     </row>
-    <row r="120" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A120" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="120">
+      <c r="A120" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C120" s="1">
+      <c r="C120" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D120" s="1" t="s">
@@ -2978,11 +2759,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A121" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="121">
+      <c r="A121" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C121" s="1">
+      <c r="C121" s="1" t="n">
         <v>210</v>
       </c>
       <c r="D121" s="1" t="s">
@@ -2992,44 +2773,44 @@
         <v>173</v>
       </c>
     </row>
-    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A122" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="122">
+      <c r="A122" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B122" s="1">
+      <c r="B122" s="1" t="n">
         <v>980</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="123" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A123" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="123">
+      <c r="A123" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B123" s="1">
+      <c r="B123" s="1" t="n">
         <v>1260</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A124" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="124">
+      <c r="A124" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B124" s="1">
+      <c r="B124" s="1" t="n">
         <v>3687</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A125" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="125">
+      <c r="A125" s="2" t="n">
         <v>43298</v>
       </c>
-      <c r="C125" s="1">
+      <c r="C125" s="1" t="n">
         <v>60</v>
       </c>
       <c r="D125" s="1" t="s">
@@ -3039,55 +2820,55 @@
         <v>178</v>
       </c>
     </row>
-    <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A126" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="126">
+      <c r="A126" s="2" t="n">
         <v>43291</v>
       </c>
-      <c r="C126" s="1">
+      <c r="C126" s="1" t="n">
         <v>404</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A127" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="127">
+      <c r="A127" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C127" s="1">
+      <c r="C127" s="1" t="n">
         <v>451</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="128" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A128" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="128">
+      <c r="A128" s="2" t="n">
         <v>43298</v>
       </c>
-      <c r="C128" s="1">
+      <c r="C128" s="1" t="n">
         <v>708</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A129" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="129">
+      <c r="A129" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C129" s="1">
+      <c r="C129" s="1" t="n">
         <v>160</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A130" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="130">
+      <c r="A130" s="2" t="n">
         <v>43288</v>
       </c>
-      <c r="C130" s="1">
+      <c r="C130" s="1" t="n">
         <v>72</v>
       </c>
       <c r="D130" s="1" t="s">
@@ -3097,11 +2878,11 @@
         <v>181</v>
       </c>
     </row>
-    <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A131" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="131">
+      <c r="A131" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C131" s="1">
+      <c r="C131" s="1" t="n">
         <v>300</v>
       </c>
       <c r="D131" s="1" t="s">
@@ -3111,11 +2892,11 @@
         <v>183</v>
       </c>
     </row>
-    <row r="132" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A132" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="132">
+      <c r="A132" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C132" s="1">
+      <c r="C132" s="1" t="n">
         <v>230</v>
       </c>
       <c r="D132" s="1" t="s">
@@ -3125,22 +2906,22 @@
         <v>185</v>
       </c>
     </row>
-    <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A133" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="133">
+      <c r="A133" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C133" s="1">
+      <c r="C133" s="1" t="n">
         <v>454</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="134" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A134" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="134">
+      <c r="A134" s="2" t="n">
         <v>43299</v>
       </c>
-      <c r="C134" s="1">
+      <c r="C134" s="1" t="n">
         <v>686</v>
       </c>
       <c r="D134" s="1" t="s">
@@ -3150,11 +2931,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A135" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="135">
+      <c r="A135" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C135" s="1">
+      <c r="C135" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D135" s="1" t="s">
@@ -3164,11 +2945,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A136" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="136">
+      <c r="A136" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C136" s="1">
+      <c r="C136" s="1" t="n">
         <v>2067</v>
       </c>
       <c r="D136" s="1" t="s">
@@ -3178,11 +2959,11 @@
         <v>186</v>
       </c>
     </row>
-    <row r="137" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A137" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="137">
+      <c r="A137" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B137" s="1">
+      <c r="B137" s="1" t="n">
         <v>109</v>
       </c>
       <c r="D137" s="1" t="s">
@@ -3192,11 +2973,11 @@
         <v>187</v>
       </c>
     </row>
-    <row r="138" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A138" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="138">
+      <c r="A138" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B138" s="1">
+      <c r="B138" s="1" t="n">
         <v>97</v>
       </c>
       <c r="D138" s="1" t="s">
@@ -3206,11 +2987,11 @@
         <v>188</v>
       </c>
     </row>
-    <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A139" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="139">
+      <c r="A139" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B139" s="1">
+      <c r="B139" s="1" t="n">
         <v>1437</v>
       </c>
       <c r="D139" s="1" t="s">
@@ -3220,11 +3001,11 @@
         <v>189</v>
       </c>
     </row>
-    <row r="140" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A140" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="140">
+      <c r="A140" s="2" t="n">
         <v>43306</v>
       </c>
-      <c r="C140" s="1">
+      <c r="C140" s="1" t="n">
         <v>650</v>
       </c>
       <c r="D140" s="1" t="s">
@@ -3234,11 +3015,11 @@
         <v>190</v>
       </c>
     </row>
-    <row r="141" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A141" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="141">
+      <c r="A141" s="2" t="n">
         <v>43305</v>
       </c>
-      <c r="C141" s="1">
+      <c r="C141" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D141" s="1" t="s">
@@ -3248,11 +3029,11 @@
         <v>191</v>
       </c>
     </row>
-    <row r="142" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A142" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="142">
+      <c r="A142" s="2" t="n">
         <v>43309</v>
       </c>
-      <c r="C142" s="1">
+      <c r="C142" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D142" s="1" t="s">
@@ -3262,11 +3043,11 @@
         <v>192</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A143" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="0" r="143">
+      <c r="A143" s="2" t="n">
         <v>43306</v>
       </c>
-      <c r="B143" s="1">
+      <c r="B143" s="1" t="n">
         <v>167</v>
       </c>
       <c r="D143" s="1" t="s">
@@ -3276,11 +3057,11 @@
         <v>193</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="14" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A144" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="0" r="144">
+      <c r="A144" s="2" t="n">
         <v>43304</v>
       </c>
-      <c r="C144" s="1">
+      <c r="C144" s="1" t="n">
         <v>93</v>
       </c>
       <c r="D144" s="1" t="s">
@@ -3290,11 +3071,11 @@
         <v>194</v>
       </c>
     </row>
-    <row r="145" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A145" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="145">
+      <c r="A145" s="2" t="n">
         <v>43305</v>
       </c>
-      <c r="C145" s="1">
+      <c r="C145" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D145" s="1" t="s">
@@ -3304,11 +3085,11 @@
         <v>195</v>
       </c>
     </row>
-    <row r="146" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A146" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="146">
+      <c r="A146" s="2" t="n">
         <v>43303</v>
       </c>
-      <c r="C146" s="1">
+      <c r="C146" s="1" t="n">
         <v>244</v>
       </c>
       <c r="D146" s="1" t="s">
@@ -3318,11 +3099,11 @@
         <v>196</v>
       </c>
     </row>
-    <row r="147" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A147" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="147">
+      <c r="A147" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C147" s="1">
+      <c r="C147" s="1" t="n">
         <v>482</v>
       </c>
       <c r="D147" s="1" t="s">
@@ -3332,11 +3113,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="148" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A148" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="148">
+      <c r="A148" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C148" s="1">
+      <c r="C148" s="1" t="n">
         <v>172</v>
       </c>
       <c r="D148" s="1" t="s">
@@ -3346,44 +3127,44 @@
         <v>199</v>
       </c>
     </row>
-    <row r="149" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A149" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="149">
+      <c r="A149" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="B149" s="1">
+      <c r="B149" s="1" t="n">
         <v>89</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="150" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A150" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="150">
+      <c r="A150" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="C150" s="1">
+      <c r="C150" s="1" t="n">
         <v>107</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="151" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A151" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="151">
+      <c r="A151" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="C151" s="1">
+      <c r="C151" s="1" t="n">
         <v>124</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="152" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A152" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="152">
+      <c r="A152" s="7" t="n">
         <v>43316</v>
       </c>
-      <c r="C152" s="1">
+      <c r="C152" s="1" t="n">
         <v>4500</v>
       </c>
       <c r="D152" s="1" t="s">
@@ -3393,11 +3174,11 @@
         <v>202</v>
       </c>
     </row>
-    <row r="153" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A153" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="153">
+      <c r="A153" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C153" s="1">
+      <c r="C153" s="1" t="n">
         <v>247</v>
       </c>
       <c r="D153" s="1" t="s">
@@ -3407,11 +3188,11 @@
         <v>204</v>
       </c>
     </row>
-    <row r="154" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A154" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="154">
+      <c r="A154" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C154" s="1">
+      <c r="C154" s="1" t="n">
         <v>1150</v>
       </c>
       <c r="D154" s="1" t="s">
@@ -3421,11 +3202,11 @@
         <v>205</v>
       </c>
     </row>
-    <row r="155" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A155" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="155">
+      <c r="A155" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C155" s="1">
+      <c r="C155" s="1" t="n">
         <v>313</v>
       </c>
       <c r="D155" s="1" t="s">
@@ -3435,11 +3216,11 @@
         <v>207</v>
       </c>
     </row>
-    <row r="156" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A156" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="156">
+      <c r="A156" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="B156" s="1">
+      <c r="B156" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D156" s="1" t="s">
@@ -3449,11 +3230,11 @@
         <v>209</v>
       </c>
     </row>
-    <row r="157" spans="1:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A157" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="157">
+      <c r="A157" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="C157" s="1">
+      <c r="C157" s="1" t="n">
         <v>710</v>
       </c>
       <c r="D157" s="1" t="s">
@@ -3463,11 +3244,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A158" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="158">
+      <c r="A158" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="C158" s="1">
+      <c r="C158" s="1" t="n">
         <v>100</v>
       </c>
       <c r="D158" s="1" t="s">
@@ -3477,11 +3258,11 @@
         <v>212</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A159" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="159">
+      <c r="A159" s="2" t="n">
         <v>43319</v>
       </c>
-      <c r="B159" s="1">
+      <c r="B159" s="1" t="n">
         <v>78</v>
       </c>
       <c r="D159" s="1" t="s">
@@ -3491,22 +3272,22 @@
         <v>213</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A160" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="160">
+      <c r="A160" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="B160" s="1">
+      <c r="B160" s="1" t="n">
         <v>1840</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A161" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="161">
+      <c r="A161" s="2" t="n">
         <v>43322</v>
       </c>
-      <c r="B161" s="1">
+      <c r="B161" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D161" s="1" t="s">
@@ -3516,11 +3297,11 @@
         <v>216</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A162" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="162">
+      <c r="A162" s="7" t="n">
         <v>43324</v>
       </c>
-      <c r="C162" s="1">
+      <c r="C162" s="1" t="n">
         <v>230</v>
       </c>
       <c r="D162" s="1" t="s">
@@ -3530,11 +3311,11 @@
         <v>217</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A163" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="163">
+      <c r="A163" s="7" t="n">
         <v>43326</v>
       </c>
-      <c r="C163" s="1">
+      <c r="C163" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D163" s="1" t="s">
@@ -3544,11 +3325,11 @@
         <v>219</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A164" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="164">
+      <c r="A164" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="B164" s="1">
+      <c r="B164" s="1" t="n">
         <v>45</v>
       </c>
       <c r="D164" s="1" t="s">
@@ -3558,501 +3339,531 @@
         <v>221</v>
       </c>
     </row>
-    <row r="165" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A165" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="165">
+      <c r="A165" s="10" t="n">
         <v>43327</v>
       </c>
-      <c r="C165">
+      <c r="C165" s="0" t="n">
         <v>486</v>
       </c>
-      <c r="D165" t="s">
+      <c r="D165" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E165" t="s">
+      <c r="E165" s="0" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="166" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A166" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="166">
+      <c r="A166" s="10" t="n">
         <v>43329</v>
       </c>
-      <c r="C166">
+      <c r="C166" s="0" t="n">
         <v>92</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D166" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="E166" t="s">
+      <c r="E166" s="0" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A167" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="167">
+      <c r="A167" s="10" t="n">
         <v>43331</v>
       </c>
-      <c r="C167">
+      <c r="C167" s="0" t="n">
         <v>310</v>
       </c>
-      <c r="D167" t="s">
+      <c r="D167" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="E167" t="s">
+      <c r="E167" s="0" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A168" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="168">
+      <c r="A168" s="10" t="n">
         <v>43334</v>
       </c>
-      <c r="C168">
+      <c r="C168" s="0" t="n">
         <v>464</v>
       </c>
-      <c r="D168" t="s">
+      <c r="D168" s="0" t="s">
         <v>218</v>
       </c>
       <c r="E168" s="11" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A169" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="169">
+      <c r="A169" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="C169">
+      <c r="C169" s="0" t="n">
         <v>726</v>
       </c>
-      <c r="D169" t="s">
+      <c r="D169" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="E169" t="s">
+      <c r="E169" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A170" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="170">
+      <c r="A170" s="10" t="n">
         <v>43337</v>
       </c>
-      <c r="C170">
+      <c r="C170" s="0" t="n">
         <v>544</v>
       </c>
-      <c r="D170" t="s">
+      <c r="D170" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E170" t="s">
+      <c r="E170" s="0" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A171" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="171">
+      <c r="A171" s="10" t="n">
         <v>43337</v>
       </c>
-      <c r="B171">
+      <c r="B171" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D171" t="s">
+      <c r="D171" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="E171" t="s">
+      <c r="E171" s="0" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A172" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="172">
+      <c r="A172" s="10" t="n">
         <v>43341</v>
       </c>
-      <c r="C172">
+      <c r="C172" s="0" t="n">
         <v>830</v>
       </c>
-      <c r="D172" t="s">
+      <c r="D172" s="0" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A173" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="173">
+      <c r="A173" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="C173">
+      <c r="C173" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="D173" t="s">
+      <c r="D173" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="E173" t="s">
+      <c r="E173" s="0" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A174" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="174">
+      <c r="A174" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="B174">
+      <c r="B174" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D174" t="s">
+      <c r="D174" s="0" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A175" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="175">
+      <c r="A175" s="10" t="n">
         <v>43344</v>
       </c>
-      <c r="B175">
+      <c r="B175" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="D175" t="s">
+      <c r="D175" s="0" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A176" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="176">
+      <c r="A176" s="10" t="n">
         <v>43344</v>
       </c>
-      <c r="B176">
+      <c r="B176" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D176" t="s">
+      <c r="D176" s="0" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A177" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="177">
+      <c r="A177" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C177">
+      <c r="C177" s="0" t="n">
         <v>607</v>
       </c>
-      <c r="D177" t="s">
+      <c r="D177" s="0" t="s">
         <v>235</v>
       </c>
-      <c r="E177" t="s">
+      <c r="E177" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A178" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="178">
+      <c r="A178" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C178">
+      <c r="C178" s="0" t="n">
         <v>444</v>
       </c>
-      <c r="D178" t="s">
+      <c r="D178" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E178" t="s">
+      <c r="E178" s="0" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A179" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="179">
+      <c r="A179" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C179">
+      <c r="C179" s="0" t="n">
         <v>312</v>
       </c>
-      <c r="D179" t="s">
+      <c r="D179" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="E179" t="s">
+      <c r="E179" s="0" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A180" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="180">
+      <c r="A180" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C180">
+      <c r="C180" s="0" t="n">
         <v>501</v>
       </c>
-      <c r="D180" t="s">
+      <c r="D180" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E180" t="s">
+      <c r="E180" s="0" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A181" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="181">
+      <c r="A181" s="10" t="n">
         <v>43349</v>
       </c>
-      <c r="C181">
+      <c r="C181" s="0" t="n">
         <v>711</v>
       </c>
-      <c r="D181" t="s">
+      <c r="D181" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="E181" t="s">
+      <c r="E181" s="0" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A182" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="182">
+      <c r="A182" s="10" t="n">
         <v>43354</v>
       </c>
-      <c r="B182">
+      <c r="B182" s="0" t="n">
         <v>126</v>
       </c>
-      <c r="D182" t="s">
+      <c r="D182" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="E182" t="s">
+      <c r="E182" s="0" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A183" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="183">
+      <c r="A183" s="10" t="n">
         <v>43354</v>
       </c>
-      <c r="C183">
+      <c r="C183" s="0" t="n">
         <v>450</v>
       </c>
-      <c r="D183" t="s">
+      <c r="D183" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="E183" t="s">
+      <c r="E183" s="0" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A184" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="184">
+      <c r="A184" s="10" t="n">
         <v>43361</v>
       </c>
-      <c r="C184">
+      <c r="C184" s="0" t="n">
         <v>660</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D184" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="E184" t="s">
+      <c r="E184" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A185" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="185">
+      <c r="A185" s="10" t="n">
         <v>43363</v>
       </c>
-      <c r="C185">
+      <c r="C185" s="0" t="n">
         <v>230</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D185" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="E185" t="s">
+      <c r="E185" s="0" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A186" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="186">
+      <c r="A186" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B186">
+      <c r="B186" s="0" t="n">
         <v>4859</v>
       </c>
-      <c r="D186" t="s">
+      <c r="D186" s="0" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A187" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="187">
+      <c r="A187" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B187">
+      <c r="B187" s="0" t="n">
         <v>295</v>
       </c>
-      <c r="D187" t="s">
+      <c r="D187" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="E187" t="s">
+      <c r="E187" s="0" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A188" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="188">
+      <c r="A188" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B188">
+      <c r="B188" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D188" t="s">
+      <c r="D188" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="E188" t="s">
+      <c r="E188" s="0" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A189" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="189">
+      <c r="A189" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B189">
+      <c r="B189" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="D189" t="s">
+      <c r="D189" s="0" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A190" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="190">
+      <c r="A190" s="10" t="n">
         <v>43378</v>
       </c>
-      <c r="B190">
+      <c r="B190" s="0" t="n">
         <v>506</v>
       </c>
-      <c r="D190" t="s">
+      <c r="D190" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="E190" t="s">
+      <c r="E190" s="0" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A191" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="191">
+      <c r="A191" s="10" t="n">
         <v>43379</v>
       </c>
-      <c r="B191">
+      <c r="B191" s="0" t="n">
         <v>350</v>
       </c>
-      <c r="D191" t="s">
+      <c r="D191" s="0" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A192" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="192">
+      <c r="A192" s="10" t="n">
         <v>43383</v>
       </c>
-      <c r="B192">
+      <c r="B192" s="0" t="n">
         <v>189</v>
       </c>
-      <c r="D192" t="s">
+      <c r="D192" s="0" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A193" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="193">
+      <c r="A193" s="10" t="n">
         <v>43387</v>
       </c>
-      <c r="B193">
+      <c r="B193" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="D193" t="s">
+      <c r="D193" s="0" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A194" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="194">
+      <c r="A194" s="10" t="n">
         <v>43387</v>
       </c>
-      <c r="B194">
+      <c r="B194" s="0" t="n">
         <v>307</v>
       </c>
-      <c r="D194" t="s">
+      <c r="D194" s="0" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="C195">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="195">
+      <c r="C195" s="0" t="n">
         <v>3705</v>
       </c>
-      <c r="E195" t="s">
+      <c r="E195" s="0" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A196" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="196">
+      <c r="A196" s="10" t="n">
         <v>43385</v>
       </c>
-      <c r="C196">
+      <c r="C196" s="0" t="n">
         <v>608</v>
       </c>
-      <c r="D196" t="s">
+      <c r="D196" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E196" t="s">
+      <c r="E196" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A197" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="197">
+      <c r="A197" s="10" t="n">
         <v>43391</v>
       </c>
-      <c r="B197">
+      <c r="B197" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="D197" t="s">
+      <c r="D197" s="0" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A198" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="198">
+      <c r="A198" s="10" t="n">
         <v>43392</v>
       </c>
-      <c r="B198">
+      <c r="B198" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="D198" t="s">
+      <c r="D198" s="0" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A199" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="199">
+      <c r="A199" s="10" t="n">
         <v>43393</v>
       </c>
-      <c r="B199">
+      <c r="B199" s="0" t="n">
         <v>177</v>
       </c>
-      <c r="D199" t="s">
+      <c r="D199" s="0" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A200" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="200">
+      <c r="A200" s="10" t="n">
         <v>43393</v>
       </c>
-      <c r="C200">
+      <c r="C200" s="0" t="n">
         <v>125</v>
       </c>
-      <c r="D200" t="s">
+      <c r="D200" s="0" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A201" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="201">
+      <c r="A201" s="10" t="n">
         <v>43395</v>
       </c>
-      <c r="B201">
+      <c r="B201" s="0" t="n">
         <v>2800</v>
       </c>
       <c r="D201" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="E201" t="s">
+      <c r="E201" s="0" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A202" s="10"/>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B207">
-        <f>SUM(B2:B206)</f>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="202">
+      <c r="A202" s="10" t="n">
+        <v>43395</v>
+      </c>
+      <c r="C202" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="D202" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="E202" s="0" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="203">
+      <c r="A203" s="10" t="n">
+        <v>43396</v>
+      </c>
+      <c r="C203" s="0" t="n">
+        <v>692</v>
+      </c>
+      <c r="D203" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="E203" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="207">
+      <c r="B207" s="0" t="n">
+        <f aca="false">SUM(B2:B206)</f>
         <v>49290</v>
       </c>
-      <c r="C207">
-        <f>SUM(C2:C206)</f>
-        <v>46733</v>
+      <c r="C207" s="0" t="n">
+        <f aca="false">SUM(C2:C206)</f>
+        <v>47496</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A30:Z32">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule aboveAverage="0" bottom="0" dxfId="0" operator="expression" percent="0" priority="2" rank="0" text="" type="expression">
       <formula>LEN(TRIM(A30))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D33" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D40" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D201" r:id="rId3" xr:uid="{757AE5B6-FCCC-3942-AD40-1B67446EFE1F}"/>
+    <hyperlink display="netonnet.se" ref="D33" r:id="rId1"/>
+    <hyperlink display="www.vidaxl.se" ref="D40" r:id="rId2"/>
+    <hyperlink display="https://www.vardia.se/ " ref="D201" r:id="rId3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cost update 1024 Jenny
</commit_message>
<xml_diff>
--- a/Cost.xlsx
+++ b/Cost.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="263">
   <si>
     <t>日期</t>
   </si>
@@ -788,7 +788,7 @@
     <t>鸡蛋仔</t>
   </si>
   <si>
-    <t>https://www.vardia.se/ </t>
+    <t>https://www.vardia.se/</t>
   </si>
   <si>
     <t>house insurance</t>
@@ -798,6 +798,12 @@
   </si>
   <si>
     <t>paprika; toothpaste;luobo</t>
+  </si>
+  <si>
+    <t>pay credit loan for Martin</t>
+  </si>
+  <si>
+    <t>3800 RMB/0.77=4935KR</t>
   </si>
 </sst>
 </file>
@@ -1068,10 +1074,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z207"/>
+  <dimension ref="A1:Z220"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A188" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D205" activeCellId="0" pane="topLeft" sqref="D205"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A191" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D218" activeCellId="0" pane="topLeft" sqref="D218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
@@ -3837,14 +3843,29 @@
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="207">
-      <c r="B207" s="0" t="n">
-        <f aca="false">SUM(B2:B206)</f>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="204">
+      <c r="A204" s="10" t="n">
+        <v>43397</v>
+      </c>
+      <c r="C204" s="0" t="n">
+        <v>4935</v>
+      </c>
+      <c r="D204" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="E204" s="0" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="207"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="220">
+      <c r="B220" s="0" t="n">
+        <f aca="false">SUM(B2:B219)</f>
         <v>49290</v>
       </c>
-      <c r="C207" s="0" t="n">
-        <f aca="false">SUM(C2:C206)</f>
-        <v>47496</v>
+      <c r="C220" s="0" t="n">
+        <f aca="false">SUM(C2:C219)</f>
+        <v>52431</v>
       </c>
     </row>
   </sheetData>
@@ -3856,7 +3877,7 @@
   <hyperlinks>
     <hyperlink display="netonnet.se" ref="D33" r:id="rId1"/>
     <hyperlink display="www.vidaxl.se" ref="D40" r:id="rId2"/>
-    <hyperlink display="https://www.vardia.se/ " ref="D201" r:id="rId3"/>
+    <hyperlink display="https://www.vardia.se/" ref="D201" r:id="rId3"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Cost update Jenny 1026
</commit_message>
<xml_diff>
--- a/Cost.xlsx
+++ b/Cost.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chengkaiyan/github/cost/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0533AB1F-1BC5-324A-93F0-BC0560547172}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="267">
   <si>
     <t>日期</t>
   </si>
@@ -815,55 +810,77 @@
   </si>
   <si>
     <t>car insurance</t>
+  </si>
+  <si>
+    <t>candies for Halloween</t>
+  </si>
+  <si>
+    <t>Kista hemmakvall</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="yyyy/m/d"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt formatCode="YYYY/M/D" numFmtId="165"/>
+    <numFmt formatCode="M/D/YYYY" numFmtId="166"/>
+    <numFmt formatCode="YYYY\-MM\-DD" numFmtId="167"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="9">
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <family val="0"/>
       <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
       <name val="Arial"/>
       <family val="2"/>
+      <sz val="10"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF666666"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF666666"/>
+      <sz val="11"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0563C1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF0563C1"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0563C1"/>
       <name val="FreeSans"/>
       <family val="2"/>
+      <color rgb="FF0563C1"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
   </fonts>
   <fills count="5">
@@ -893,7 +910,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
@@ -901,30 +918,96 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+  <cellStyleXfs count="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="167" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="20">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="7">
+    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle builtinId="8" customBuiltin="false" name="*unknown*" xfId="20"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -935,7 +1018,6 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -994,339 +1076,31 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:Z220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A191" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D208" sqref="D208"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A191" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D215" activeCellId="0" pane="topLeft" sqref="D215"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="3" width="14.5"/>
-    <col min="4" max="4" width="26"/>
-    <col min="5" max="5" width="37.83203125"/>
-    <col min="6" max="1025" width="14.5"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="14.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1343,11 +1117,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1">
-      <c r="A2" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="2">
+      <c r="A2" s="2" t="n">
         <v>43121</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="1" t="n">
         <v>250</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1357,11 +1131,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1">
-      <c r="A3" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="3">
+      <c r="A3" s="2" t="n">
         <v>43122</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="1" t="n">
         <v>305</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1371,11 +1145,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1">
-      <c r="A4" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="4">
+      <c r="A4" s="2" t="n">
         <v>43122</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1385,11 +1159,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1">
-      <c r="A5" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="5">
+      <c r="A5" s="2" t="n">
         <v>43125</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="1" t="n">
         <v>98</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1399,11 +1173,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1">
-      <c r="A6" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="6">
+      <c r="A6" s="2" t="n">
         <v>43126</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1413,11 +1187,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1">
-      <c r="A7" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="7">
+      <c r="A7" s="2" t="n">
         <v>43127</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1427,11 +1201,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1">
-      <c r="A8" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="8">
+      <c r="A8" s="2" t="n">
         <v>43128</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="1" t="n">
         <v>656</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1441,11 +1215,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1">
-      <c r="A9" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="9">
+      <c r="A9" s="2" t="n">
         <v>43131</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="1" t="n">
         <v>486</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1455,11 +1229,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1">
-      <c r="A10" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="10">
+      <c r="A10" s="2" t="n">
         <v>43132</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="1" t="n">
         <v>76</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1469,11 +1243,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1">
-      <c r="A11" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="11">
+      <c r="A11" s="2" t="n">
         <v>43133</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="1" t="n">
         <v>399</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1483,11 +1257,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1">
-      <c r="A12" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="12">
+      <c r="A12" s="2" t="n">
         <v>43135</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="1" t="n">
         <v>419</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1497,11 +1271,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1">
-      <c r="A13" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="13">
+      <c r="A13" s="2" t="n">
         <v>43136</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="1" t="n">
         <v>521</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1511,11 +1285,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1">
-      <c r="A14" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="14">
+      <c r="A14" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="1" t="n">
         <v>399</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1525,11 +1299,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1">
-      <c r="A15" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="15">
+      <c r="A15" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="1" t="n">
         <v>138</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1539,11 +1313,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1">
-      <c r="A16" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="16">
+      <c r="A16" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="1" t="n">
         <v>310</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1553,12 +1327,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1">
-      <c r="A17" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="17">
+      <c r="A17" s="2" t="n">
         <v>43138</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="1">
+      <c r="C17" s="1" t="n">
         <v>700</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1568,12 +1342,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1">
-      <c r="A18" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="18">
+      <c r="A18" s="2" t="n">
         <v>43141</v>
       </c>
-      <c r="C18" s="1">
-        <f>F18*G18</f>
+      <c r="C18" s="1" t="n">
+        <f aca="false">F18*G18</f>
         <v>1312</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -1582,18 +1356,18 @@
       <c r="E18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="1" t="n">
         <v>164</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="1" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1">
-      <c r="A19" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="19">
+      <c r="A19" s="2" t="n">
         <v>43141</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="1" t="n">
         <v>1190</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1603,11 +1377,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1">
-      <c r="A20" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="20">
+      <c r="A20" s="2" t="n">
         <v>43154</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="1" t="n">
         <v>438</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1617,11 +1391,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1">
-      <c r="A21" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="21">
+      <c r="A21" s="2" t="n">
         <v>43154</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="1" t="n">
         <v>248</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -1631,22 +1405,22 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1">
-      <c r="A22" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="22">
+      <c r="A22" s="2" t="n">
         <v>43166</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="1" t="n">
         <v>234</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1">
-      <c r="A23" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="23">
+      <c r="A23" s="2" t="n">
         <v>43171</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="1" t="n">
         <v>118</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1656,22 +1430,22 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1">
-      <c r="A24" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="24">
+      <c r="A24" s="2" t="n">
         <v>43173</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="1" t="n">
         <v>82</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1">
-      <c r="A25" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="25">
+      <c r="A25" s="2" t="n">
         <v>43174</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1681,22 +1455,22 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1">
-      <c r="A26" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="26">
+      <c r="A26" s="2" t="n">
         <v>43175</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="1" t="n">
         <v>370</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:7" hidden="1">
-      <c r="A27" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="27">
+      <c r="A27" s="2" t="n">
         <v>43175</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -1706,11 +1480,11 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1">
-      <c r="A28" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="28">
+      <c r="A28" s="2" t="n">
         <v>43176</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="1" t="n">
         <v>624</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -1720,11 +1494,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1">
-      <c r="A29" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="29">
+      <c r="A29" s="2" t="n">
         <v>43177</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="1" t="n">
         <v>170</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1734,22 +1508,22 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1">
-      <c r="A30" s="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="30">
+      <c r="A30" s="4" t="n">
         <v>43179</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1">
-      <c r="A31" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="31">
+      <c r="A31" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="1" t="n">
         <v>90</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -1759,11 +1533,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1">
-      <c r="A32" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="32">
+      <c r="A32" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="1" t="n">
         <v>72</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -1773,11 +1547,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:26" hidden="1">
-      <c r="A33" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="33">
+      <c r="A33" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="1" t="n">
         <v>908</v>
       </c>
       <c r="D33" s="6" t="s">
@@ -1787,11 +1561,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:26" hidden="1">
-      <c r="A34" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="34">
+      <c r="A34" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -1801,11 +1575,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:26" hidden="1">
-      <c r="A35" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="35">
+      <c r="A35" s="2" t="n">
         <v>43181</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -1815,11 +1589,11 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:26" hidden="1">
-      <c r="A36" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="36">
+      <c r="A36" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="1" t="n">
         <v>135</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -1829,11 +1603,11 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:26" hidden="1">
-      <c r="A37" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="37">
+      <c r="A37" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="1" t="n">
         <v>110</v>
       </c>
       <c r="C37" s="1"/>
@@ -1865,11 +1639,11 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38" spans="1:26" hidden="1">
-      <c r="A38" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="38">
+      <c r="A38" s="2" t="n">
         <v>43185</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="1" t="n">
         <v>122</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -1879,22 +1653,22 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:26" hidden="1">
-      <c r="A39" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="39">
+      <c r="A39" s="2" t="n">
         <v>43187</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="1" t="n">
         <v>750</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:26" hidden="1">
-      <c r="A40" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="40">
+      <c r="A40" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="1" t="n">
         <v>379</v>
       </c>
       <c r="D40" s="6" t="s">
@@ -1904,22 +1678,22 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:26" hidden="1">
-      <c r="A41" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="41">
+      <c r="A41" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="1" t="n">
         <v>240</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:26" hidden="1">
-      <c r="A42" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="42">
+      <c r="A42" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="1" t="n">
         <v>540</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -1929,11 +1703,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:26" hidden="1">
-      <c r="A43" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="43">
+      <c r="A43" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -1943,11 +1717,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:26" hidden="1">
-      <c r="A44" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="44">
+      <c r="A44" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -1957,11 +1731,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:26" hidden="1">
-      <c r="A45" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="45">
+      <c r="A45" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="1" t="n">
         <v>462</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -1971,11 +1745,11 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:26" hidden="1">
-      <c r="A46" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="46">
+      <c r="A46" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46" s="1" t="n">
         <v>70</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -1985,11 +1759,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:26" hidden="1">
-      <c r="A47" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="47">
+      <c r="A47" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -1999,11 +1773,11 @@
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="1:26" hidden="1">
-      <c r="A48" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="48">
+      <c r="A48" s="2" t="n">
         <v>43190</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="1" t="n">
         <v>30</v>
       </c>
       <c r="C48" s="1"/>
@@ -2014,11 +1788,11 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1">
-      <c r="A49" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="49">
+      <c r="A49" s="2" t="n">
         <v>43191</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="1" t="n">
         <v>40</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -2028,11 +1802,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1">
-      <c r="A50" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="50">
+      <c r="A50" s="7" t="n">
         <v>43193</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50" s="1" t="n">
         <v>150</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -2042,11 +1816,11 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1">
-      <c r="A51" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="51">
+      <c r="A51" s="2" t="n">
         <v>43194</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51" s="1" t="n">
         <v>1360</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -2056,11 +1830,11 @@
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1">
-      <c r="A52" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="52">
+      <c r="A52" s="2" t="n">
         <v>43195</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" s="1" t="n">
         <v>94</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -2070,11 +1844,11 @@
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1">
-      <c r="A53" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="53">
+      <c r="A53" s="2" t="n">
         <v>43196</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C53" s="1" t="n">
         <v>48</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -2084,11 +1858,11 @@
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1">
-      <c r="A54" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="54">
+      <c r="A54" s="2" t="n">
         <v>43196</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C54" s="1" t="n">
         <v>205</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -2098,11 +1872,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1">
-      <c r="A55" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="55">
+      <c r="A55" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -2112,11 +1886,11 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1">
-      <c r="A56" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="56">
+      <c r="A56" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56" s="1" t="n">
         <v>421</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -2126,11 +1900,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1">
-      <c r="A57" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="57">
+      <c r="A57" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="1" t="n">
         <v>191</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -2140,11 +1914,11 @@
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1">
-      <c r="A58" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="58">
+      <c r="A58" s="2" t="n">
         <v>43198</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58" s="1" t="n">
         <v>226</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -2154,22 +1928,22 @@
         <v>96</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1">
-      <c r="A59" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="59">
+      <c r="A59" s="2" t="n">
         <v>43200</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59" s="1" t="n">
         <v>250</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1">
-      <c r="A60" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="60">
+      <c r="A60" s="2" t="n">
         <v>43200</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60" s="1" t="n">
         <v>1115</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -2179,11 +1953,11 @@
         <v>99</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1">
-      <c r="A61" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="61">
+      <c r="A61" s="2" t="n">
         <v>43201</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -2193,11 +1967,11 @@
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1">
-      <c r="A62" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="62">
+      <c r="A62" s="2" t="n">
         <v>43201</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62" s="1" t="n">
         <v>88</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -2207,11 +1981,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1">
-      <c r="A63" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="63">
+      <c r="A63" s="2" t="n">
         <v>43203</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -2221,11 +1995,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1">
-      <c r="A64" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="64">
+      <c r="A64" s="2" t="n">
         <v>43203</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C64" s="1" t="n">
         <v>364</v>
       </c>
       <c r="D64" s="1" t="s">
@@ -2235,11 +2009,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1">
-      <c r="A65" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="65">
+      <c r="A65" s="2" t="n">
         <v>43204</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65" s="1" t="n">
         <v>65</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -2249,11 +2023,11 @@
         <v>105</v>
       </c>
     </row>
-    <row r="66" spans="1:5" hidden="1">
-      <c r="A66" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="66">
+      <c r="A66" s="2" t="n">
         <v>43208</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -2263,11 +2037,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1">
-      <c r="A67" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="67">
+      <c r="A67" s="2" t="n">
         <v>43208</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C67" s="1" t="n">
         <v>470</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -2277,11 +2051,11 @@
         <v>107</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1">
-      <c r="A68" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="68">
+      <c r="A68" s="2" t="n">
         <v>43209</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68" s="1" t="n">
         <v>180</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -2291,11 +2065,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1">
-      <c r="A69" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="69">
+      <c r="A69" s="2" t="n">
         <v>43210</v>
       </c>
-      <c r="C69" s="1">
+      <c r="C69" s="1" t="n">
         <v>420</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -2305,11 +2079,11 @@
         <v>109</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1">
-      <c r="A70" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="70">
+      <c r="A70" s="2" t="n">
         <v>43212</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70" s="1" t="n">
         <v>50</v>
       </c>
       <c r="D70" s="1" t="s">
@@ -2319,11 +2093,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1">
-      <c r="A71" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="71">
+      <c r="A71" s="2" t="n">
         <v>43212</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71" s="1" t="n">
         <v>164</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -2333,11 +2107,11 @@
         <v>112</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1">
-      <c r="A72" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="72">
+      <c r="A72" s="2" t="n">
         <v>43215</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B72" s="1" t="n">
         <v>300</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -2347,11 +2121,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1">
-      <c r="A73" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="73">
+      <c r="A73" s="2" t="n">
         <v>43217</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73" s="1" t="n">
         <v>364</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -2361,11 +2135,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1">
-      <c r="A74" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="74">
+      <c r="A74" s="2" t="n">
         <v>43218</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74" s="1" t="n">
         <v>185</v>
       </c>
       <c r="D74" s="1" t="s">
@@ -2375,11 +2149,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1">
-      <c r="A75" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="75">
+      <c r="A75" s="2" t="n">
         <v>43218</v>
       </c>
-      <c r="C75" s="1">
+      <c r="C75" s="1" t="n">
         <v>404</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -2389,11 +2163,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="76" spans="1:5" hidden="1">
-      <c r="A76" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="76">
+      <c r="A76" s="2" t="n">
         <v>43220</v>
       </c>
-      <c r="C76" s="1">
+      <c r="C76" s="1" t="n">
         <v>57</v>
       </c>
       <c r="D76" s="1" t="s">
@@ -2403,11 +2177,11 @@
         <v>114</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1">
-      <c r="A77" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="77">
+      <c r="A77" s="2" t="n">
         <v>43221</v>
       </c>
-      <c r="C77" s="1">
+      <c r="C77" s="1" t="n">
         <v>282</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -2417,11 +2191,11 @@
         <v>116</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1">
-      <c r="A78" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="78">
+      <c r="A78" s="2" t="n">
         <v>43220</v>
       </c>
-      <c r="C78" s="1">
+      <c r="C78" s="1" t="n">
         <v>87</v>
       </c>
       <c r="D78" s="1" t="s">
@@ -2431,11 +2205,11 @@
         <v>117</v>
       </c>
     </row>
-    <row r="79" spans="1:5" hidden="1">
-      <c r="A79" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="79">
+      <c r="A79" s="2" t="n">
         <v>43223</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B79" s="1" t="n">
         <v>1878</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -2445,11 +2219,11 @@
         <v>119</v>
       </c>
     </row>
-    <row r="80" spans="1:5" hidden="1">
-      <c r="A80" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="80">
+      <c r="A80" s="2" t="n">
         <v>43224</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B80" s="1" t="n">
         <v>98</v>
       </c>
       <c r="D80" s="1" t="s">
@@ -2459,11 +2233,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="81" spans="1:5" hidden="1">
-      <c r="A81" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="81">
+      <c r="A81" s="2" t="n">
         <v>43225</v>
       </c>
-      <c r="C81" s="1">
+      <c r="C81" s="1" t="n">
         <v>198</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -2473,11 +2247,11 @@
         <v>122</v>
       </c>
     </row>
-    <row r="82" spans="1:5" hidden="1">
-      <c r="A82" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="82">
+      <c r="A82" s="2" t="n">
         <v>43225</v>
       </c>
-      <c r="C82" s="1">
+      <c r="C82" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -2487,11 +2261,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="83" spans="1:5" hidden="1">
-      <c r="A83" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="83">
+      <c r="A83" s="2" t="n">
         <v>43228</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83" s="1" t="n">
         <v>168</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -2501,11 +2275,11 @@
         <v>124</v>
       </c>
     </row>
-    <row r="84" spans="1:5" hidden="1">
-      <c r="A84" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="84">
+      <c r="A84" s="2" t="n">
         <v>43229</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B84" s="1" t="n">
         <v>240</v>
       </c>
       <c r="D84" s="1" t="s">
@@ -2515,12 +2289,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:5" hidden="1">
-      <c r="A85" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="85">
+      <c r="A85" s="2" t="n">
         <v>43230</v>
       </c>
       <c r="B85" s="1"/>
-      <c r="C85" s="1">
+      <c r="C85" s="1" t="n">
         <v>420</v>
       </c>
       <c r="D85" s="1" t="s">
@@ -2530,11 +2304,11 @@
         <v>126</v>
       </c>
     </row>
-    <row r="86" spans="1:5" hidden="1">
-      <c r="A86" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="86">
+      <c r="A86" s="2" t="n">
         <v>43230</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B86" s="1" t="n">
         <v>200</v>
       </c>
       <c r="C86" s="1"/>
@@ -2545,11 +2319,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="87" spans="1:5" hidden="1">
-      <c r="A87" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="87">
+      <c r="A87" s="2" t="n">
         <v>43230</v>
       </c>
-      <c r="C87" s="1">
+      <c r="C87" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D87" s="1" t="s">
@@ -2559,11 +2333,11 @@
         <v>128</v>
       </c>
     </row>
-    <row r="88" spans="1:5" hidden="1">
-      <c r="A88" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="88">
+      <c r="A88" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B88" s="1" t="n">
         <v>462</v>
       </c>
       <c r="D88" s="1" t="s">
@@ -2573,11 +2347,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="89" spans="1:5" hidden="1">
-      <c r="A89" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="89">
+      <c r="A89" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B89" s="1" t="n">
         <v>499</v>
       </c>
       <c r="D89" s="1" t="s">
@@ -2587,11 +2361,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="90" spans="1:5" hidden="1">
-      <c r="A90" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="90">
+      <c r="A90" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B90" s="1">
+      <c r="B90" s="1" t="n">
         <v>398</v>
       </c>
       <c r="D90" s="1" t="s">
@@ -2601,11 +2375,11 @@
         <v>133</v>
       </c>
     </row>
-    <row r="91" spans="1:5" hidden="1">
-      <c r="A91" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="91">
+      <c r="A91" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B91" s="1">
+      <c r="B91" s="1" t="n">
         <v>226</v>
       </c>
       <c r="D91" s="1" t="s">
@@ -2615,11 +2389,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="92" spans="1:5" hidden="1">
-      <c r="A92" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="92">
+      <c r="A92" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B92" s="1">
+      <c r="B92" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D92" s="1" t="s">
@@ -2629,11 +2403,11 @@
         <v>137</v>
       </c>
     </row>
-    <row r="93" spans="1:5" hidden="1">
-      <c r="A93" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="93">
+      <c r="A93" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="B93" s="1">
+      <c r="B93" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D93" s="1" t="s">
@@ -2643,11 +2417,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="94" spans="1:5" hidden="1">
-      <c r="A94" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="94">
+      <c r="A94" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="C94" s="1">
+      <c r="C94" s="1" t="n">
         <v>340</v>
       </c>
       <c r="D94" s="1" t="s">
@@ -2657,11 +2431,11 @@
         <v>139</v>
       </c>
     </row>
-    <row r="95" spans="1:5" hidden="1">
-      <c r="A95" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="95">
+      <c r="A95" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="B95" s="1">
+      <c r="B95" s="1" t="n">
         <v>510</v>
       </c>
       <c r="D95" s="1" t="s">
@@ -2671,11 +2445,11 @@
         <v>141</v>
       </c>
     </row>
-    <row r="96" spans="1:5" hidden="1">
-      <c r="A96" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="96">
+      <c r="A96" s="2" t="n">
         <v>43233</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B96" s="1" t="n">
         <v>170</v>
       </c>
       <c r="D96" s="1" t="s">
@@ -2685,11 +2459,11 @@
         <v>143</v>
       </c>
     </row>
-    <row r="97" spans="1:5" hidden="1">
-      <c r="A97" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="97">
+      <c r="A97" s="2" t="n">
         <v>43233</v>
       </c>
-      <c r="C97" s="1">
+      <c r="C97" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D97" s="1" t="s">
@@ -2699,11 +2473,11 @@
         <v>144</v>
       </c>
     </row>
-    <row r="98" spans="1:5" hidden="1">
-      <c r="A98" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="98">
+      <c r="A98" s="2" t="n">
         <v>43234</v>
       </c>
-      <c r="C98" s="1">
+      <c r="C98" s="1" t="n">
         <v>299</v>
       </c>
       <c r="D98" s="1" t="s">
@@ -2713,11 +2487,11 @@
         <v>145</v>
       </c>
     </row>
-    <row r="99" spans="1:5" hidden="1">
-      <c r="A99" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="99">
+      <c r="A99" s="2" t="n">
         <v>43236</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99" s="1" t="n">
         <v>3659</v>
       </c>
       <c r="D99" s="1" t="s">
@@ -2727,11 +2501,11 @@
         <v>146</v>
       </c>
     </row>
-    <row r="100" spans="1:5" hidden="1">
-      <c r="A100" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="100">
+      <c r="A100" s="2" t="n">
         <v>43237</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B100" s="1" t="n">
         <v>79</v>
       </c>
       <c r="D100" s="1" t="s">
@@ -2741,11 +2515,11 @@
         <v>147</v>
       </c>
     </row>
-    <row r="101" spans="1:5" hidden="1">
-      <c r="A101" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="101">
+      <c r="A101" s="2" t="n">
         <v>43236</v>
       </c>
-      <c r="C101" s="1">
+      <c r="C101" s="1" t="n">
         <v>173</v>
       </c>
       <c r="D101" s="1" t="s">
@@ -2755,11 +2529,11 @@
         <v>148</v>
       </c>
     </row>
-    <row r="102" spans="1:5" hidden="1">
-      <c r="A102" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="102">
+      <c r="A102" s="2" t="n">
         <v>43240</v>
       </c>
-      <c r="B102" s="1">
+      <c r="B102" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D102" s="1" t="s">
@@ -2769,22 +2543,22 @@
         <v>149</v>
       </c>
     </row>
-    <row r="103" spans="1:5" hidden="1">
-      <c r="A103" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="103">
+      <c r="A103" s="2" t="n">
         <v>43240</v>
       </c>
-      <c r="B103" s="1">
+      <c r="B103" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="104" spans="1:5" hidden="1">
-      <c r="A104" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="104">
+      <c r="A104" s="2" t="n">
         <v>43241</v>
       </c>
-      <c r="B104" s="1">
+      <c r="B104" s="1" t="n">
         <v>4070</v>
       </c>
       <c r="D104" s="1" t="s">
@@ -2794,11 +2568,11 @@
         <v>150</v>
       </c>
     </row>
-    <row r="105" spans="1:5" hidden="1">
-      <c r="A105" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="105">
+      <c r="A105" s="2" t="n">
         <v>43241</v>
       </c>
-      <c r="C105" s="1">
+      <c r="C105" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D105" s="1" t="s">
@@ -2808,11 +2582,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="106" spans="1:5" hidden="1">
-      <c r="A106" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="106">
+      <c r="A106" s="2" t="n">
         <v>43242</v>
       </c>
-      <c r="B106" s="1">
+      <c r="B106" s="1" t="n">
         <v>79</v>
       </c>
       <c r="D106" s="1" t="s">
@@ -2822,11 +2596,11 @@
         <v>152</v>
       </c>
     </row>
-    <row r="107" spans="1:5" hidden="1">
-      <c r="A107" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="107">
+      <c r="A107" s="2" t="n">
         <v>43246</v>
       </c>
-      <c r="B107" s="1">
+      <c r="B107" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D107" s="1" t="s">
@@ -2836,11 +2610,11 @@
         <v>154</v>
       </c>
     </row>
-    <row r="108" spans="1:5" hidden="1">
-      <c r="A108" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="108">
+      <c r="A108" s="2" t="n">
         <v>43247</v>
       </c>
-      <c r="B108" s="1">
+      <c r="B108" s="1" t="n">
         <v>70</v>
       </c>
       <c r="D108" s="1" t="s">
@@ -2850,44 +2624,44 @@
         <v>156</v>
       </c>
     </row>
-    <row r="109" spans="1:5" hidden="1">
-      <c r="A109" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="109">
+      <c r="A109" s="2" t="n">
         <v>43253</v>
       </c>
-      <c r="B109" s="1">
+      <c r="B109" s="1" t="n">
         <v>142</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="110" spans="1:5" hidden="1">
-      <c r="A110" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="110">
+      <c r="A110" s="2" t="n">
         <v>43254</v>
       </c>
-      <c r="B110" s="1">
+      <c r="B110" s="1" t="n">
         <v>90</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="111" spans="1:5" hidden="1">
-      <c r="A111" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="111">
+      <c r="A111" s="2" t="n">
         <v>43260</v>
       </c>
-      <c r="C111" s="1">
+      <c r="C111" s="1" t="n">
         <v>1400</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="112" spans="1:5" hidden="1">
-      <c r="A112" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="112">
+      <c r="A112" s="2" t="n">
         <v>43260</v>
       </c>
-      <c r="C112" s="1">
+      <c r="C112" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D112" s="1" t="s">
@@ -2897,33 +2671,33 @@
         <v>91</v>
       </c>
     </row>
-    <row r="113" spans="1:5" hidden="1">
-      <c r="A113" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="113">
+      <c r="A113" s="2" t="n">
         <v>43264</v>
       </c>
-      <c r="B113" s="1">
+      <c r="B113" s="1" t="n">
         <v>546</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="114" spans="1:5" hidden="1">
-      <c r="A114" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="114">
+      <c r="A114" s="2" t="n">
         <v>43264</v>
       </c>
-      <c r="B114" s="1">
+      <c r="B114" s="1" t="n">
         <v>95</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="115" spans="1:5" hidden="1">
-      <c r="A115" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="115">
+      <c r="A115" s="2" t="n">
         <v>43266</v>
       </c>
-      <c r="B115" s="1">
+      <c r="B115" s="1" t="n">
         <v>394</v>
       </c>
       <c r="D115" s="1" t="s">
@@ -2933,11 +2707,11 @@
         <v>163</v>
       </c>
     </row>
-    <row r="116" spans="1:5" hidden="1">
-      <c r="A116" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="116">
+      <c r="A116" s="2" t="n">
         <v>43266</v>
       </c>
-      <c r="B116" s="1">
+      <c r="B116" s="1" t="n">
         <v>1055</v>
       </c>
       <c r="D116" s="1" t="s">
@@ -2947,11 +2721,11 @@
         <v>165</v>
       </c>
     </row>
-    <row r="117" spans="1:5" hidden="1">
-      <c r="A117" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="117">
+      <c r="A117" s="2" t="n">
         <v>43284</v>
       </c>
-      <c r="C117" s="1">
+      <c r="C117" s="1" t="n">
         <v>274</v>
       </c>
       <c r="D117" s="1" t="s">
@@ -2961,11 +2735,11 @@
         <v>167</v>
       </c>
     </row>
-    <row r="118" spans="1:5" hidden="1">
-      <c r="A118" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="118">
+      <c r="A118" s="2" t="n">
         <v>43283</v>
       </c>
-      <c r="C118" s="1">
+      <c r="C118" s="1" t="n">
         <v>105</v>
       </c>
       <c r="D118" s="1" t="s">
@@ -2975,11 +2749,11 @@
         <v>169</v>
       </c>
     </row>
-    <row r="119" spans="1:5" hidden="1">
-      <c r="A119" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="119">
+      <c r="A119" s="2" t="n">
         <v>43289</v>
       </c>
-      <c r="C119" s="1">
+      <c r="C119" s="1" t="n">
         <v>128</v>
       </c>
       <c r="D119" s="1" t="s">
@@ -2989,11 +2763,11 @@
         <v>171</v>
       </c>
     </row>
-    <row r="120" spans="1:5" hidden="1">
-      <c r="A120" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="120">
+      <c r="A120" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C120" s="1">
+      <c r="C120" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D120" s="1" t="s">
@@ -3003,11 +2777,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="121" spans="1:5" hidden="1">
-      <c r="A121" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="121">
+      <c r="A121" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C121" s="1">
+      <c r="C121" s="1" t="n">
         <v>210</v>
       </c>
       <c r="D121" s="1" t="s">
@@ -3017,44 +2791,44 @@
         <v>173</v>
       </c>
     </row>
-    <row r="122" spans="1:5" hidden="1">
-      <c r="A122" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="122">
+      <c r="A122" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B122" s="1">
+      <c r="B122" s="1" t="n">
         <v>980</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="123" spans="1:5" hidden="1">
-      <c r="A123" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="123">
+      <c r="A123" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B123" s="1">
+      <c r="B123" s="1" t="n">
         <v>1260</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="124" spans="1:5" hidden="1">
-      <c r="A124" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="124">
+      <c r="A124" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B124" s="1">
+      <c r="B124" s="1" t="n">
         <v>3687</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="125" spans="1:5" hidden="1">
-      <c r="A125" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="125">
+      <c r="A125" s="2" t="n">
         <v>43298</v>
       </c>
-      <c r="C125" s="1">
+      <c r="C125" s="1" t="n">
         <v>60</v>
       </c>
       <c r="D125" s="1" t="s">
@@ -3064,55 +2838,55 @@
         <v>178</v>
       </c>
     </row>
-    <row r="126" spans="1:5" hidden="1">
-      <c r="A126" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="126">
+      <c r="A126" s="2" t="n">
         <v>43291</v>
       </c>
-      <c r="C126" s="1">
+      <c r="C126" s="1" t="n">
         <v>404</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="127" spans="1:5" hidden="1">
-      <c r="A127" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="127">
+      <c r="A127" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C127" s="1">
+      <c r="C127" s="1" t="n">
         <v>451</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="128" spans="1:5" hidden="1">
-      <c r="A128" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="128">
+      <c r="A128" s="2" t="n">
         <v>43298</v>
       </c>
-      <c r="C128" s="1">
+      <c r="C128" s="1" t="n">
         <v>708</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="129" spans="1:5" hidden="1">
-      <c r="A129" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="129">
+      <c r="A129" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C129" s="1">
+      <c r="C129" s="1" t="n">
         <v>160</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="130" spans="1:5" hidden="1">
-      <c r="A130" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="130">
+      <c r="A130" s="2" t="n">
         <v>43288</v>
       </c>
-      <c r="C130" s="1">
+      <c r="C130" s="1" t="n">
         <v>72</v>
       </c>
       <c r="D130" s="1" t="s">
@@ -3122,11 +2896,11 @@
         <v>181</v>
       </c>
     </row>
-    <row r="131" spans="1:5" hidden="1">
-      <c r="A131" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="131">
+      <c r="A131" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C131" s="1">
+      <c r="C131" s="1" t="n">
         <v>300</v>
       </c>
       <c r="D131" s="1" t="s">
@@ -3136,11 +2910,11 @@
         <v>183</v>
       </c>
     </row>
-    <row r="132" spans="1:5" hidden="1">
-      <c r="A132" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="132">
+      <c r="A132" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C132" s="1">
+      <c r="C132" s="1" t="n">
         <v>230</v>
       </c>
       <c r="D132" s="1" t="s">
@@ -3150,22 +2924,22 @@
         <v>185</v>
       </c>
     </row>
-    <row r="133" spans="1:5" hidden="1">
-      <c r="A133" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="133">
+      <c r="A133" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C133" s="1">
+      <c r="C133" s="1" t="n">
         <v>454</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="134" spans="1:5" hidden="1">
-      <c r="A134" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="134">
+      <c r="A134" s="2" t="n">
         <v>43299</v>
       </c>
-      <c r="C134" s="1">
+      <c r="C134" s="1" t="n">
         <v>686</v>
       </c>
       <c r="D134" s="1" t="s">
@@ -3175,11 +2949,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="135" spans="1:5" hidden="1">
-      <c r="A135" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="135">
+      <c r="A135" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C135" s="1">
+      <c r="C135" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D135" s="1" t="s">
@@ -3189,11 +2963,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="136" spans="1:5" hidden="1">
-      <c r="A136" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="136">
+      <c r="A136" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C136" s="1">
+      <c r="C136" s="1" t="n">
         <v>2067</v>
       </c>
       <c r="D136" s="1" t="s">
@@ -3203,11 +2977,11 @@
         <v>186</v>
       </c>
     </row>
-    <row r="137" spans="1:5" hidden="1">
-      <c r="A137" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="137">
+      <c r="A137" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B137" s="1">
+      <c r="B137" s="1" t="n">
         <v>109</v>
       </c>
       <c r="D137" s="1" t="s">
@@ -3217,11 +2991,11 @@
         <v>187</v>
       </c>
     </row>
-    <row r="138" spans="1:5" hidden="1">
-      <c r="A138" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="138">
+      <c r="A138" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B138" s="1">
+      <c r="B138" s="1" t="n">
         <v>97</v>
       </c>
       <c r="D138" s="1" t="s">
@@ -3231,11 +3005,11 @@
         <v>188</v>
       </c>
     </row>
-    <row r="139" spans="1:5" hidden="1">
-      <c r="A139" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="139">
+      <c r="A139" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B139" s="1">
+      <c r="B139" s="1" t="n">
         <v>1437</v>
       </c>
       <c r="D139" s="1" t="s">
@@ -3245,11 +3019,11 @@
         <v>189</v>
       </c>
     </row>
-    <row r="140" spans="1:5" hidden="1">
-      <c r="A140" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="140">
+      <c r="A140" s="2" t="n">
         <v>43306</v>
       </c>
-      <c r="C140" s="1">
+      <c r="C140" s="1" t="n">
         <v>650</v>
       </c>
       <c r="D140" s="1" t="s">
@@ -3259,11 +3033,11 @@
         <v>190</v>
       </c>
     </row>
-    <row r="141" spans="1:5" hidden="1">
-      <c r="A141" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="141">
+      <c r="A141" s="2" t="n">
         <v>43305</v>
       </c>
-      <c r="C141" s="1">
+      <c r="C141" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D141" s="1" t="s">
@@ -3273,11 +3047,11 @@
         <v>191</v>
       </c>
     </row>
-    <row r="142" spans="1:5" hidden="1">
-      <c r="A142" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="142">
+      <c r="A142" s="2" t="n">
         <v>43309</v>
       </c>
-      <c r="C142" s="1">
+      <c r="C142" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D142" s="1" t="s">
@@ -3287,11 +3061,11 @@
         <v>192</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="14" hidden="1">
-      <c r="A143" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="0" r="143">
+      <c r="A143" s="2" t="n">
         <v>43306</v>
       </c>
-      <c r="B143" s="1">
+      <c r="B143" s="1" t="n">
         <v>167</v>
       </c>
       <c r="D143" s="1" t="s">
@@ -3301,11 +3075,11 @@
         <v>193</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="14" hidden="1">
-      <c r="A144" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="0" r="144">
+      <c r="A144" s="2" t="n">
         <v>43304</v>
       </c>
-      <c r="C144" s="1">
+      <c r="C144" s="1" t="n">
         <v>93</v>
       </c>
       <c r="D144" s="1" t="s">
@@ -3315,11 +3089,11 @@
         <v>194</v>
       </c>
     </row>
-    <row r="145" spans="1:5" hidden="1">
-      <c r="A145" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="145">
+      <c r="A145" s="2" t="n">
         <v>43305</v>
       </c>
-      <c r="C145" s="1">
+      <c r="C145" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D145" s="1" t="s">
@@ -3329,11 +3103,11 @@
         <v>195</v>
       </c>
     </row>
-    <row r="146" spans="1:5" hidden="1">
-      <c r="A146" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="146">
+      <c r="A146" s="2" t="n">
         <v>43303</v>
       </c>
-      <c r="C146" s="1">
+      <c r="C146" s="1" t="n">
         <v>244</v>
       </c>
       <c r="D146" s="1" t="s">
@@ -3343,11 +3117,11 @@
         <v>196</v>
       </c>
     </row>
-    <row r="147" spans="1:5" hidden="1">
-      <c r="A147" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="147">
+      <c r="A147" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C147" s="1">
+      <c r="C147" s="1" t="n">
         <v>482</v>
       </c>
       <c r="D147" s="1" t="s">
@@ -3357,11 +3131,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="148" spans="1:5" hidden="1">
-      <c r="A148" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="148">
+      <c r="A148" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C148" s="1">
+      <c r="C148" s="1" t="n">
         <v>172</v>
       </c>
       <c r="D148" s="1" t="s">
@@ -3371,44 +3145,44 @@
         <v>199</v>
       </c>
     </row>
-    <row r="149" spans="1:5" hidden="1">
-      <c r="A149" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="149">
+      <c r="A149" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="B149" s="1">
+      <c r="B149" s="1" t="n">
         <v>89</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="150" spans="1:5" hidden="1">
-      <c r="A150" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="150">
+      <c r="A150" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="C150" s="1">
+      <c r="C150" s="1" t="n">
         <v>107</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="151" spans="1:5" hidden="1">
-      <c r="A151" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="151">
+      <c r="A151" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="C151" s="1">
+      <c r="C151" s="1" t="n">
         <v>124</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="152" spans="1:5" hidden="1">
-      <c r="A152" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="152">
+      <c r="A152" s="7" t="n">
         <v>43316</v>
       </c>
-      <c r="C152" s="1">
+      <c r="C152" s="1" t="n">
         <v>4500</v>
       </c>
       <c r="D152" s="1" t="s">
@@ -3418,11 +3192,11 @@
         <v>202</v>
       </c>
     </row>
-    <row r="153" spans="1:5" hidden="1">
-      <c r="A153" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="153">
+      <c r="A153" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C153" s="1">
+      <c r="C153" s="1" t="n">
         <v>247</v>
       </c>
       <c r="D153" s="1" t="s">
@@ -3432,11 +3206,11 @@
         <v>204</v>
       </c>
     </row>
-    <row r="154" spans="1:5" hidden="1">
-      <c r="A154" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="154">
+      <c r="A154" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C154" s="1">
+      <c r="C154" s="1" t="n">
         <v>1150</v>
       </c>
       <c r="D154" s="1" t="s">
@@ -3446,11 +3220,11 @@
         <v>205</v>
       </c>
     </row>
-    <row r="155" spans="1:5" hidden="1">
-      <c r="A155" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="155">
+      <c r="A155" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C155" s="1">
+      <c r="C155" s="1" t="n">
         <v>313</v>
       </c>
       <c r="D155" s="1" t="s">
@@ -3460,11 +3234,11 @@
         <v>207</v>
       </c>
     </row>
-    <row r="156" spans="1:5" hidden="1">
-      <c r="A156" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="156">
+      <c r="A156" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="B156" s="1">
+      <c r="B156" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D156" s="1" t="s">
@@ -3474,11 +3248,11 @@
         <v>209</v>
       </c>
     </row>
-    <row r="157" spans="1:5" hidden="1">
-      <c r="A157" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="157">
+      <c r="A157" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="C157" s="1">
+      <c r="C157" s="1" t="n">
         <v>710</v>
       </c>
       <c r="D157" s="1" t="s">
@@ -3488,11 +3262,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="158" spans="1:5">
-      <c r="A158" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="158">
+      <c r="A158" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="C158" s="1">
+      <c r="C158" s="1" t="n">
         <v>100</v>
       </c>
       <c r="D158" s="1" t="s">
@@ -3502,11 +3276,11 @@
         <v>212</v>
       </c>
     </row>
-    <row r="159" spans="1:5">
-      <c r="A159" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="159">
+      <c r="A159" s="2" t="n">
         <v>43319</v>
       </c>
-      <c r="B159" s="1">
+      <c r="B159" s="1" t="n">
         <v>78</v>
       </c>
       <c r="D159" s="1" t="s">
@@ -3516,22 +3290,22 @@
         <v>213</v>
       </c>
     </row>
-    <row r="160" spans="1:5">
-      <c r="A160" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="160">
+      <c r="A160" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="B160" s="1">
+      <c r="B160" s="1" t="n">
         <v>1840</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="161" spans="1:5">
-      <c r="A161" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="161">
+      <c r="A161" s="2" t="n">
         <v>43322</v>
       </c>
-      <c r="B161" s="1">
+      <c r="B161" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D161" s="1" t="s">
@@ -3541,11 +3315,11 @@
         <v>216</v>
       </c>
     </row>
-    <row r="162" spans="1:5">
-      <c r="A162" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="162">
+      <c r="A162" s="7" t="n">
         <v>43324</v>
       </c>
-      <c r="C162" s="1">
+      <c r="C162" s="1" t="n">
         <v>230</v>
       </c>
       <c r="D162" s="1" t="s">
@@ -3555,11 +3329,11 @@
         <v>217</v>
       </c>
     </row>
-    <row r="163" spans="1:5">
-      <c r="A163" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="163">
+      <c r="A163" s="7" t="n">
         <v>43326</v>
       </c>
-      <c r="C163" s="1">
+      <c r="C163" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D163" s="1" t="s">
@@ -3569,11 +3343,11 @@
         <v>219</v>
       </c>
     </row>
-    <row r="164" spans="1:5">
-      <c r="A164" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="164">
+      <c r="A164" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="B164" s="1">
+      <c r="B164" s="1" t="n">
         <v>45</v>
       </c>
       <c r="D164" s="1" t="s">
@@ -3583,573 +3357,592 @@
         <v>221</v>
       </c>
     </row>
-    <row r="165" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A165" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="165">
+      <c r="A165" s="10" t="n">
         <v>43327</v>
       </c>
-      <c r="C165">
+      <c r="C165" s="0" t="n">
         <v>486</v>
       </c>
-      <c r="D165" t="s">
+      <c r="D165" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E165" t="s">
+      <c r="E165" s="0" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="166" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A166" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="166">
+      <c r="A166" s="10" t="n">
         <v>43329</v>
       </c>
-      <c r="C166">
+      <c r="C166" s="0" t="n">
         <v>92</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D166" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="E166" t="s">
+      <c r="E166" s="0" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="167" spans="1:5">
-      <c r="A167" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="167">
+      <c r="A167" s="10" t="n">
         <v>43331</v>
       </c>
-      <c r="C167">
+      <c r="C167" s="0" t="n">
         <v>310</v>
       </c>
-      <c r="D167" t="s">
+      <c r="D167" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="E167" t="s">
+      <c r="E167" s="0" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="168" spans="1:5">
-      <c r="A168" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="168">
+      <c r="A168" s="10" t="n">
         <v>43334</v>
       </c>
-      <c r="C168">
+      <c r="C168" s="0" t="n">
         <v>464</v>
       </c>
-      <c r="D168" t="s">
+      <c r="D168" s="0" t="s">
         <v>218</v>
       </c>
       <c r="E168" s="11" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="169" spans="1:5">
-      <c r="A169" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="169">
+      <c r="A169" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="C169">
+      <c r="C169" s="0" t="n">
         <v>726</v>
       </c>
-      <c r="D169" t="s">
+      <c r="D169" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="E169" t="s">
+      <c r="E169" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="170" spans="1:5">
-      <c r="A170" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="170">
+      <c r="A170" s="10" t="n">
         <v>43337</v>
       </c>
-      <c r="C170">
+      <c r="C170" s="0" t="n">
         <v>544</v>
       </c>
-      <c r="D170" t="s">
+      <c r="D170" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E170" t="s">
+      <c r="E170" s="0" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="171" spans="1:5">
-      <c r="A171" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="171">
+      <c r="A171" s="10" t="n">
         <v>43337</v>
       </c>
-      <c r="B171">
+      <c r="B171" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D171" t="s">
+      <c r="D171" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="E171" t="s">
+      <c r="E171" s="0" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="172" spans="1:5">
-      <c r="A172" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="172">
+      <c r="A172" s="10" t="n">
         <v>43341</v>
       </c>
-      <c r="C172">
+      <c r="C172" s="0" t="n">
         <v>830</v>
       </c>
-      <c r="D172" t="s">
+      <c r="D172" s="0" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="173" spans="1:5">
-      <c r="A173" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="173">
+      <c r="A173" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="C173">
+      <c r="C173" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="D173" t="s">
+      <c r="D173" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="E173" t="s">
+      <c r="E173" s="0" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="174" spans="1:5">
-      <c r="A174" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="174">
+      <c r="A174" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="B174">
+      <c r="B174" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D174" t="s">
+      <c r="D174" s="0" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="175" spans="1:5">
-      <c r="A175" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="175">
+      <c r="A175" s="10" t="n">
         <v>43344</v>
       </c>
-      <c r="B175">
+      <c r="B175" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="D175" t="s">
+      <c r="D175" s="0" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="176" spans="1:5">
-      <c r="A176" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="176">
+      <c r="A176" s="10" t="n">
         <v>43344</v>
       </c>
-      <c r="B176">
+      <c r="B176" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D176" t="s">
+      <c r="D176" s="0" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="177" spans="1:5">
-      <c r="A177" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="177">
+      <c r="A177" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C177">
+      <c r="C177" s="0" t="n">
         <v>607</v>
       </c>
-      <c r="D177" t="s">
+      <c r="D177" s="0" t="s">
         <v>235</v>
       </c>
-      <c r="E177" t="s">
+      <c r="E177" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="178" spans="1:5">
-      <c r="A178" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="178">
+      <c r="A178" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C178">
+      <c r="C178" s="0" t="n">
         <v>444</v>
       </c>
-      <c r="D178" t="s">
+      <c r="D178" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E178" t="s">
+      <c r="E178" s="0" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="179" spans="1:5">
-      <c r="A179" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="179">
+      <c r="A179" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C179">
+      <c r="C179" s="0" t="n">
         <v>312</v>
       </c>
-      <c r="D179" t="s">
+      <c r="D179" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="E179" t="s">
+      <c r="E179" s="0" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="180" spans="1:5">
-      <c r="A180" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="180">
+      <c r="A180" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C180">
+      <c r="C180" s="0" t="n">
         <v>501</v>
       </c>
-      <c r="D180" t="s">
+      <c r="D180" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E180" t="s">
+      <c r="E180" s="0" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="181" spans="1:5">
-      <c r="A181" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="181">
+      <c r="A181" s="10" t="n">
         <v>43349</v>
       </c>
-      <c r="C181">
+      <c r="C181" s="0" t="n">
         <v>711</v>
       </c>
-      <c r="D181" t="s">
+      <c r="D181" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="E181" t="s">
+      <c r="E181" s="0" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="182" spans="1:5">
-      <c r="A182" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="182">
+      <c r="A182" s="10" t="n">
         <v>43354</v>
       </c>
-      <c r="B182">
+      <c r="B182" s="0" t="n">
         <v>126</v>
       </c>
-      <c r="D182" t="s">
+      <c r="D182" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="E182" t="s">
+      <c r="E182" s="0" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="183" spans="1:5">
-      <c r="A183" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="183">
+      <c r="A183" s="10" t="n">
         <v>43354</v>
       </c>
-      <c r="C183">
+      <c r="C183" s="0" t="n">
         <v>450</v>
       </c>
-      <c r="D183" t="s">
+      <c r="D183" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="E183" t="s">
+      <c r="E183" s="0" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="184" spans="1:5">
-      <c r="A184" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="184">
+      <c r="A184" s="10" t="n">
         <v>43361</v>
       </c>
-      <c r="C184">
+      <c r="C184" s="0" t="n">
         <v>660</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D184" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="E184" t="s">
+      <c r="E184" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="185" spans="1:5">
-      <c r="A185" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="185">
+      <c r="A185" s="10" t="n">
         <v>43363</v>
       </c>
-      <c r="C185">
+      <c r="C185" s="0" t="n">
         <v>230</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D185" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="E185" t="s">
+      <c r="E185" s="0" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="186" spans="1:5">
-      <c r="A186" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="186">
+      <c r="A186" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B186">
+      <c r="B186" s="0" t="n">
         <v>4859</v>
       </c>
-      <c r="D186" t="s">
+      <c r="D186" s="0" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="187" spans="1:5">
-      <c r="A187" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="187">
+      <c r="A187" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B187">
+      <c r="B187" s="0" t="n">
         <v>295</v>
       </c>
-      <c r="D187" t="s">
+      <c r="D187" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="E187" t="s">
+      <c r="E187" s="0" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="188" spans="1:5">
-      <c r="A188" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="188">
+      <c r="A188" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B188">
+      <c r="B188" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D188" t="s">
+      <c r="D188" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="E188" t="s">
+      <c r="E188" s="0" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="189" spans="1:5">
-      <c r="A189" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="189">
+      <c r="A189" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B189">
+      <c r="B189" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="D189" t="s">
+      <c r="D189" s="0" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="190" spans="1:5">
-      <c r="A190" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="190">
+      <c r="A190" s="10" t="n">
         <v>43378</v>
       </c>
-      <c r="B190">
+      <c r="B190" s="0" t="n">
         <v>506</v>
       </c>
-      <c r="D190" t="s">
+      <c r="D190" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="E190" t="s">
+      <c r="E190" s="0" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="191" spans="1:5">
-      <c r="A191" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="191">
+      <c r="A191" s="10" t="n">
         <v>43379</v>
       </c>
-      <c r="B191">
+      <c r="B191" s="0" t="n">
         <v>350</v>
       </c>
-      <c r="D191" t="s">
+      <c r="D191" s="0" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="192" spans="1:5">
-      <c r="A192" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="192">
+      <c r="A192" s="10" t="n">
         <v>43383</v>
       </c>
-      <c r="B192">
+      <c r="B192" s="0" t="n">
         <v>189</v>
       </c>
-      <c r="D192" t="s">
+      <c r="D192" s="0" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="193" spans="1:5">
-      <c r="A193" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="193">
+      <c r="A193" s="10" t="n">
         <v>43387</v>
       </c>
-      <c r="B193">
+      <c r="B193" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="D193" t="s">
+      <c r="D193" s="0" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="194" spans="1:5">
-      <c r="A194" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="194">
+      <c r="A194" s="10" t="n">
         <v>43387</v>
       </c>
-      <c r="B194">
+      <c r="B194" s="0" t="n">
         <v>307</v>
       </c>
-      <c r="D194" t="s">
+      <c r="D194" s="0" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="195" spans="1:5">
-      <c r="C195">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="195">
+      <c r="C195" s="0" t="n">
         <v>3705</v>
       </c>
-      <c r="E195" t="s">
+      <c r="E195" s="0" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="196" spans="1:5">
-      <c r="A196" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="196">
+      <c r="A196" s="10" t="n">
         <v>43385</v>
       </c>
-      <c r="C196">
+      <c r="C196" s="0" t="n">
         <v>608</v>
       </c>
-      <c r="D196" t="s">
+      <c r="D196" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E196" t="s">
+      <c r="E196" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="197" spans="1:5">
-      <c r="A197" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="197">
+      <c r="A197" s="10" t="n">
         <v>43391</v>
       </c>
-      <c r="B197">
+      <c r="B197" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="D197" t="s">
+      <c r="D197" s="0" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="198" spans="1:5">
-      <c r="A198" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="198">
+      <c r="A198" s="10" t="n">
         <v>43392</v>
       </c>
-      <c r="B198">
+      <c r="B198" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="D198" t="s">
+      <c r="D198" s="0" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="199" spans="1:5">
-      <c r="A199" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="199">
+      <c r="A199" s="10" t="n">
         <v>43393</v>
       </c>
-      <c r="B199">
+      <c r="B199" s="0" t="n">
         <v>177</v>
       </c>
-      <c r="D199" t="s">
+      <c r="D199" s="0" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="200" spans="1:5">
-      <c r="A200" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="200">
+      <c r="A200" s="10" t="n">
         <v>43393</v>
       </c>
-      <c r="C200">
+      <c r="C200" s="0" t="n">
         <v>125</v>
       </c>
-      <c r="D200" t="s">
+      <c r="D200" s="0" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="201" spans="1:5">
-      <c r="A201" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="201">
+      <c r="A201" s="10" t="n">
         <v>43395</v>
       </c>
-      <c r="B201">
+      <c r="B201" s="0" t="n">
         <v>2800</v>
       </c>
       <c r="D201" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="E201" t="s">
+      <c r="E201" s="0" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="202" spans="1:5">
-      <c r="A202" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="202">
+      <c r="A202" s="10" t="n">
         <v>43395</v>
       </c>
-      <c r="C202">
+      <c r="C202" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="D202" t="s">
+      <c r="D202" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="E202" t="s">
+      <c r="E202" s="0" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="203" spans="1:5">
-      <c r="A203" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="203">
+      <c r="A203" s="10" t="n">
         <v>43396</v>
       </c>
-      <c r="C203">
+      <c r="C203" s="0" t="n">
         <v>692</v>
       </c>
-      <c r="D203" t="s">
+      <c r="D203" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E203" t="s">
+      <c r="E203" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="204" spans="1:5">
-      <c r="A204" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="204">
+      <c r="A204" s="10" t="n">
         <v>43397</v>
       </c>
-      <c r="C204">
+      <c r="C204" s="0" t="n">
         <v>4935</v>
       </c>
-      <c r="D204" t="s">
+      <c r="D204" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="E204" t="s">
+      <c r="E204" s="0" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="205" spans="1:5">
-      <c r="A205" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="205">
+      <c r="A205" s="10" t="n">
         <v>43398</v>
       </c>
-      <c r="B205">
+      <c r="B205" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="D205" t="s">
+      <c r="D205" s="0" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="206" spans="1:5">
-      <c r="A206" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="206">
+      <c r="A206" s="10" t="n">
         <v>43398</v>
       </c>
-      <c r="B206">
+      <c r="B206" s="0" t="n">
         <v>370</v>
       </c>
-      <c r="D206" t="s">
+      <c r="D206" s="0" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="207" spans="1:5">
-      <c r="A207" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="207">
+      <c r="A207" s="10" t="n">
         <v>43398</v>
       </c>
-      <c r="B207">
+      <c r="B207" s="0" t="n">
         <v>4966</v>
       </c>
-      <c r="D207" t="s">
+      <c r="D207" s="0" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="220" spans="2:3">
-      <c r="B220">
-        <f>SUM(B2:B219)</f>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="208">
+      <c r="A208" s="10" t="n">
+        <v>43397</v>
+      </c>
+      <c r="C208" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="D208" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="E208" s="0" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="220">
+      <c r="B220" s="0" t="n">
+        <f aca="false">SUM(B2:B219)</f>
         <v>54756</v>
       </c>
-      <c r="C220">
-        <f>SUM(C2:C219)</f>
-        <v>52431</v>
+      <c r="C220" s="0" t="n">
+        <f aca="false">SUM(C2:C219)</f>
+        <v>52501</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A30:Z32">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule aboveAverage="0" bottom="0" dxfId="0" operator="expression" percent="0" priority="2" rank="0" text="" type="expression">
       <formula>LEN(TRIM(A30))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D33" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D40" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D201" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink display="netonnet.se" ref="D33" r:id="rId1"/>
+    <hyperlink display="www.vidaxl.se" ref="D40" r:id="rId2"/>
+    <hyperlink display="https://www.vardia.se/" ref="D201" r:id="rId3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cost update 1030 Jenny
</commit_message>
<xml_diff>
--- a/Cost.xlsx
+++ b/Cost.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chengkaiyan/github/cost/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC49CF12-610D-0E43-99A0-A43629390945}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="270">
   <si>
     <t>日期</t>
   </si>
@@ -824,55 +819,77 @@
   </si>
   <si>
     <t>halloween things</t>
+  </si>
+  <si>
+    <t>ica banken</t>
+  </si>
+  <si>
+    <t>avgift</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="yyyy/m/d"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt formatCode="YYYY/M/D" numFmtId="165"/>
+    <numFmt formatCode="M/D/YYYY" numFmtId="166"/>
+    <numFmt formatCode="YYYY\-MM\-DD" numFmtId="167"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="9">
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <family val="0"/>
       <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
       <name val="Arial"/>
       <family val="2"/>
+      <sz val="10"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF666666"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF666666"/>
+      <sz val="11"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0563C1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF0563C1"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0563C1"/>
       <name val="FreeSans"/>
       <family val="2"/>
+      <color rgb="FF0563C1"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
   </fonts>
   <fills count="5">
@@ -902,7 +919,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
@@ -910,30 +927,96 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+  <cellStyleXfs count="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="167" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="20">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="7">
+    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle builtinId="8" customBuiltin="false" name="*unknown*" xfId="20"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -944,7 +1027,6 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1003,339 +1085,31 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:Z220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A191" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B211" sqref="B211"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A191" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E215" activeCellId="0" pane="topLeft" sqref="E215"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="3" width="14.5"/>
-    <col min="4" max="4" width="26"/>
-    <col min="5" max="5" width="37.83203125"/>
-    <col min="6" max="1025" width="14.5"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="14.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1352,11 +1126,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1">
-      <c r="A2" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="2">
+      <c r="A2" s="2" t="n">
         <v>43121</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="1" t="n">
         <v>250</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1366,11 +1140,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1">
-      <c r="A3" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="3">
+      <c r="A3" s="2" t="n">
         <v>43122</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="1" t="n">
         <v>305</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1380,11 +1154,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1">
-      <c r="A4" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="4">
+      <c r="A4" s="2" t="n">
         <v>43122</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1394,11 +1168,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1">
-      <c r="A5" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="5">
+      <c r="A5" s="2" t="n">
         <v>43125</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="1" t="n">
         <v>98</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1408,11 +1182,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1">
-      <c r="A6" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="6">
+      <c r="A6" s="2" t="n">
         <v>43126</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1422,11 +1196,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1">
-      <c r="A7" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="7">
+      <c r="A7" s="2" t="n">
         <v>43127</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1436,11 +1210,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1">
-      <c r="A8" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="8">
+      <c r="A8" s="2" t="n">
         <v>43128</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="1" t="n">
         <v>656</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1450,11 +1224,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1">
-      <c r="A9" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="9">
+      <c r="A9" s="2" t="n">
         <v>43131</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="1" t="n">
         <v>486</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1464,11 +1238,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1">
-      <c r="A10" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="10">
+      <c r="A10" s="2" t="n">
         <v>43132</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="1" t="n">
         <v>76</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1478,11 +1252,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1">
-      <c r="A11" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="11">
+      <c r="A11" s="2" t="n">
         <v>43133</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="1" t="n">
         <v>399</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1492,11 +1266,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1">
-      <c r="A12" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="12">
+      <c r="A12" s="2" t="n">
         <v>43135</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="1" t="n">
         <v>419</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1506,11 +1280,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1">
-      <c r="A13" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="13">
+      <c r="A13" s="2" t="n">
         <v>43136</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="1" t="n">
         <v>521</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1520,11 +1294,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1">
-      <c r="A14" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="14">
+      <c r="A14" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="1" t="n">
         <v>399</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1534,11 +1308,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1">
-      <c r="A15" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="15">
+      <c r="A15" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="1" t="n">
         <v>138</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1548,11 +1322,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1">
-      <c r="A16" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="16">
+      <c r="A16" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="1" t="n">
         <v>310</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1562,12 +1336,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1">
-      <c r="A17" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="17">
+      <c r="A17" s="2" t="n">
         <v>43138</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="1">
+      <c r="C17" s="1" t="n">
         <v>700</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1577,12 +1351,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1">
-      <c r="A18" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="18">
+      <c r="A18" s="2" t="n">
         <v>43141</v>
       </c>
-      <c r="C18" s="1">
-        <f>F18*G18</f>
+      <c r="C18" s="1" t="n">
+        <f aca="false">F18*G18</f>
         <v>1312</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -1591,18 +1365,18 @@
       <c r="E18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="1" t="n">
         <v>164</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="1" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1">
-      <c r="A19" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="19">
+      <c r="A19" s="2" t="n">
         <v>43141</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="1" t="n">
         <v>1190</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1612,11 +1386,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1">
-      <c r="A20" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="20">
+      <c r="A20" s="2" t="n">
         <v>43154</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="1" t="n">
         <v>438</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1626,11 +1400,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1">
-      <c r="A21" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="21">
+      <c r="A21" s="2" t="n">
         <v>43154</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="1" t="n">
         <v>248</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -1640,22 +1414,22 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1">
-      <c r="A22" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="22">
+      <c r="A22" s="2" t="n">
         <v>43166</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="1" t="n">
         <v>234</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1">
-      <c r="A23" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="23">
+      <c r="A23" s="2" t="n">
         <v>43171</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="1" t="n">
         <v>118</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1665,22 +1439,22 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1">
-      <c r="A24" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="24">
+      <c r="A24" s="2" t="n">
         <v>43173</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="1" t="n">
         <v>82</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1">
-      <c r="A25" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="25">
+      <c r="A25" s="2" t="n">
         <v>43174</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1690,22 +1464,22 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1">
-      <c r="A26" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="26">
+      <c r="A26" s="2" t="n">
         <v>43175</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="1" t="n">
         <v>370</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:7" hidden="1">
-      <c r="A27" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="27">
+      <c r="A27" s="2" t="n">
         <v>43175</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -1715,11 +1489,11 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1">
-      <c r="A28" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="28">
+      <c r="A28" s="2" t="n">
         <v>43176</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="1" t="n">
         <v>624</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -1729,11 +1503,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1">
-      <c r="A29" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="29">
+      <c r="A29" s="2" t="n">
         <v>43177</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="1" t="n">
         <v>170</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1743,22 +1517,22 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1">
-      <c r="A30" s="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="30">
+      <c r="A30" s="4" t="n">
         <v>43179</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1">
-      <c r="A31" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="31">
+      <c r="A31" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="1" t="n">
         <v>90</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -1768,11 +1542,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1">
-      <c r="A32" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="32">
+      <c r="A32" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="1" t="n">
         <v>72</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -1782,11 +1556,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:26" hidden="1">
-      <c r="A33" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="33">
+      <c r="A33" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="1" t="n">
         <v>908</v>
       </c>
       <c r="D33" s="6" t="s">
@@ -1796,11 +1570,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:26" hidden="1">
-      <c r="A34" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="34">
+      <c r="A34" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -1810,11 +1584,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:26" hidden="1">
-      <c r="A35" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="35">
+      <c r="A35" s="2" t="n">
         <v>43181</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -1824,11 +1598,11 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:26" hidden="1">
-      <c r="A36" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="36">
+      <c r="A36" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="1" t="n">
         <v>135</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -1838,11 +1612,11 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:26" hidden="1">
-      <c r="A37" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="37">
+      <c r="A37" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="1" t="n">
         <v>110</v>
       </c>
       <c r="C37" s="1"/>
@@ -1874,11 +1648,11 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38" spans="1:26" hidden="1">
-      <c r="A38" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="38">
+      <c r="A38" s="2" t="n">
         <v>43185</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="1" t="n">
         <v>122</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -1888,22 +1662,22 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:26" hidden="1">
-      <c r="A39" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="39">
+      <c r="A39" s="2" t="n">
         <v>43187</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="1" t="n">
         <v>750</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:26" hidden="1">
-      <c r="A40" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="40">
+      <c r="A40" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="1" t="n">
         <v>379</v>
       </c>
       <c r="D40" s="6" t="s">
@@ -1913,22 +1687,22 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:26" hidden="1">
-      <c r="A41" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="41">
+      <c r="A41" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="1" t="n">
         <v>240</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:26" hidden="1">
-      <c r="A42" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="42">
+      <c r="A42" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="1" t="n">
         <v>540</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -1938,11 +1712,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:26" hidden="1">
-      <c r="A43" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="43">
+      <c r="A43" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -1952,11 +1726,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:26" hidden="1">
-      <c r="A44" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="44">
+      <c r="A44" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -1966,11 +1740,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:26" hidden="1">
-      <c r="A45" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="45">
+      <c r="A45" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="1" t="n">
         <v>462</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -1980,11 +1754,11 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:26" hidden="1">
-      <c r="A46" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="46">
+      <c r="A46" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46" s="1" t="n">
         <v>70</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -1994,11 +1768,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:26" hidden="1">
-      <c r="A47" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="47">
+      <c r="A47" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -2008,11 +1782,11 @@
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="1:26" hidden="1">
-      <c r="A48" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="48">
+      <c r="A48" s="2" t="n">
         <v>43190</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="1" t="n">
         <v>30</v>
       </c>
       <c r="C48" s="1"/>
@@ -2023,11 +1797,11 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1">
-      <c r="A49" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="49">
+      <c r="A49" s="2" t="n">
         <v>43191</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="1" t="n">
         <v>40</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -2037,11 +1811,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1">
-      <c r="A50" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="50">
+      <c r="A50" s="7" t="n">
         <v>43193</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50" s="1" t="n">
         <v>150</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -2051,11 +1825,11 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1">
-      <c r="A51" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="51">
+      <c r="A51" s="2" t="n">
         <v>43194</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51" s="1" t="n">
         <v>1360</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -2065,11 +1839,11 @@
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1">
-      <c r="A52" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="52">
+      <c r="A52" s="2" t="n">
         <v>43195</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" s="1" t="n">
         <v>94</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -2079,11 +1853,11 @@
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1">
-      <c r="A53" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="53">
+      <c r="A53" s="2" t="n">
         <v>43196</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C53" s="1" t="n">
         <v>48</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -2093,11 +1867,11 @@
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1">
-      <c r="A54" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="54">
+      <c r="A54" s="2" t="n">
         <v>43196</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C54" s="1" t="n">
         <v>205</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -2107,11 +1881,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1">
-      <c r="A55" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="55">
+      <c r="A55" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -2121,11 +1895,11 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1">
-      <c r="A56" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="56">
+      <c r="A56" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56" s="1" t="n">
         <v>421</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -2135,11 +1909,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1">
-      <c r="A57" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="57">
+      <c r="A57" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="1" t="n">
         <v>191</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -2149,11 +1923,11 @@
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1">
-      <c r="A58" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="58">
+      <c r="A58" s="2" t="n">
         <v>43198</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58" s="1" t="n">
         <v>226</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -2163,22 +1937,22 @@
         <v>96</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1">
-      <c r="A59" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="59">
+      <c r="A59" s="2" t="n">
         <v>43200</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59" s="1" t="n">
         <v>250</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1">
-      <c r="A60" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="60">
+      <c r="A60" s="2" t="n">
         <v>43200</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60" s="1" t="n">
         <v>1115</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -2188,11 +1962,11 @@
         <v>99</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1">
-      <c r="A61" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="61">
+      <c r="A61" s="2" t="n">
         <v>43201</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -2202,11 +1976,11 @@
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1">
-      <c r="A62" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="62">
+      <c r="A62" s="2" t="n">
         <v>43201</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62" s="1" t="n">
         <v>88</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -2216,11 +1990,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1">
-      <c r="A63" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="63">
+      <c r="A63" s="2" t="n">
         <v>43203</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -2230,11 +2004,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1">
-      <c r="A64" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="64">
+      <c r="A64" s="2" t="n">
         <v>43203</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C64" s="1" t="n">
         <v>364</v>
       </c>
       <c r="D64" s="1" t="s">
@@ -2244,11 +2018,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1">
-      <c r="A65" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="65">
+      <c r="A65" s="2" t="n">
         <v>43204</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65" s="1" t="n">
         <v>65</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -2258,11 +2032,11 @@
         <v>105</v>
       </c>
     </row>
-    <row r="66" spans="1:5" hidden="1">
-      <c r="A66" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="66">
+      <c r="A66" s="2" t="n">
         <v>43208</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -2272,11 +2046,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1">
-      <c r="A67" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="67">
+      <c r="A67" s="2" t="n">
         <v>43208</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C67" s="1" t="n">
         <v>470</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -2286,11 +2060,11 @@
         <v>107</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1">
-      <c r="A68" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="68">
+      <c r="A68" s="2" t="n">
         <v>43209</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68" s="1" t="n">
         <v>180</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -2300,11 +2074,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1">
-      <c r="A69" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="69">
+      <c r="A69" s="2" t="n">
         <v>43210</v>
       </c>
-      <c r="C69" s="1">
+      <c r="C69" s="1" t="n">
         <v>420</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -2314,11 +2088,11 @@
         <v>109</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1">
-      <c r="A70" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="70">
+      <c r="A70" s="2" t="n">
         <v>43212</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70" s="1" t="n">
         <v>50</v>
       </c>
       <c r="D70" s="1" t="s">
@@ -2328,11 +2102,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1">
-      <c r="A71" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="71">
+      <c r="A71" s="2" t="n">
         <v>43212</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71" s="1" t="n">
         <v>164</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -2342,11 +2116,11 @@
         <v>112</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1">
-      <c r="A72" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="72">
+      <c r="A72" s="2" t="n">
         <v>43215</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B72" s="1" t="n">
         <v>300</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -2356,11 +2130,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1">
-      <c r="A73" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="73">
+      <c r="A73" s="2" t="n">
         <v>43217</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73" s="1" t="n">
         <v>364</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -2370,11 +2144,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1">
-      <c r="A74" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="74">
+      <c r="A74" s="2" t="n">
         <v>43218</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74" s="1" t="n">
         <v>185</v>
       </c>
       <c r="D74" s="1" t="s">
@@ -2384,11 +2158,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1">
-      <c r="A75" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="75">
+      <c r="A75" s="2" t="n">
         <v>43218</v>
       </c>
-      <c r="C75" s="1">
+      <c r="C75" s="1" t="n">
         <v>404</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -2398,11 +2172,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="76" spans="1:5" hidden="1">
-      <c r="A76" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="76">
+      <c r="A76" s="2" t="n">
         <v>43220</v>
       </c>
-      <c r="C76" s="1">
+      <c r="C76" s="1" t="n">
         <v>57</v>
       </c>
       <c r="D76" s="1" t="s">
@@ -2412,11 +2186,11 @@
         <v>114</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1">
-      <c r="A77" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="77">
+      <c r="A77" s="2" t="n">
         <v>43221</v>
       </c>
-      <c r="C77" s="1">
+      <c r="C77" s="1" t="n">
         <v>282</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -2426,11 +2200,11 @@
         <v>116</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1">
-      <c r="A78" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="78">
+      <c r="A78" s="2" t="n">
         <v>43220</v>
       </c>
-      <c r="C78" s="1">
+      <c r="C78" s="1" t="n">
         <v>87</v>
       </c>
       <c r="D78" s="1" t="s">
@@ -2440,11 +2214,11 @@
         <v>117</v>
       </c>
     </row>
-    <row r="79" spans="1:5" hidden="1">
-      <c r="A79" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="79">
+      <c r="A79" s="2" t="n">
         <v>43223</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B79" s="1" t="n">
         <v>1878</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -2454,11 +2228,11 @@
         <v>119</v>
       </c>
     </row>
-    <row r="80" spans="1:5" hidden="1">
-      <c r="A80" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="80">
+      <c r="A80" s="2" t="n">
         <v>43224</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B80" s="1" t="n">
         <v>98</v>
       </c>
       <c r="D80" s="1" t="s">
@@ -2468,11 +2242,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="81" spans="1:5" hidden="1">
-      <c r="A81" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="81">
+      <c r="A81" s="2" t="n">
         <v>43225</v>
       </c>
-      <c r="C81" s="1">
+      <c r="C81" s="1" t="n">
         <v>198</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -2482,11 +2256,11 @@
         <v>122</v>
       </c>
     </row>
-    <row r="82" spans="1:5" hidden="1">
-      <c r="A82" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="82">
+      <c r="A82" s="2" t="n">
         <v>43225</v>
       </c>
-      <c r="C82" s="1">
+      <c r="C82" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -2496,11 +2270,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="83" spans="1:5" hidden="1">
-      <c r="A83" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="83">
+      <c r="A83" s="2" t="n">
         <v>43228</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83" s="1" t="n">
         <v>168</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -2510,11 +2284,11 @@
         <v>124</v>
       </c>
     </row>
-    <row r="84" spans="1:5" hidden="1">
-      <c r="A84" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="84">
+      <c r="A84" s="2" t="n">
         <v>43229</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B84" s="1" t="n">
         <v>240</v>
       </c>
       <c r="D84" s="1" t="s">
@@ -2524,12 +2298,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:5" hidden="1">
-      <c r="A85" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="85">
+      <c r="A85" s="2" t="n">
         <v>43230</v>
       </c>
       <c r="B85" s="1"/>
-      <c r="C85" s="1">
+      <c r="C85" s="1" t="n">
         <v>420</v>
       </c>
       <c r="D85" s="1" t="s">
@@ -2539,11 +2313,11 @@
         <v>126</v>
       </c>
     </row>
-    <row r="86" spans="1:5" hidden="1">
-      <c r="A86" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="86">
+      <c r="A86" s="2" t="n">
         <v>43230</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B86" s="1" t="n">
         <v>200</v>
       </c>
       <c r="C86" s="1"/>
@@ -2554,11 +2328,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="87" spans="1:5" hidden="1">
-      <c r="A87" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="87">
+      <c r="A87" s="2" t="n">
         <v>43230</v>
       </c>
-      <c r="C87" s="1">
+      <c r="C87" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D87" s="1" t="s">
@@ -2568,11 +2342,11 @@
         <v>128</v>
       </c>
     </row>
-    <row r="88" spans="1:5" hidden="1">
-      <c r="A88" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="88">
+      <c r="A88" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B88" s="1" t="n">
         <v>462</v>
       </c>
       <c r="D88" s="1" t="s">
@@ -2582,11 +2356,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="89" spans="1:5" hidden="1">
-      <c r="A89" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="89">
+      <c r="A89" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B89" s="1" t="n">
         <v>499</v>
       </c>
       <c r="D89" s="1" t="s">
@@ -2596,11 +2370,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="90" spans="1:5" hidden="1">
-      <c r="A90" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="90">
+      <c r="A90" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B90" s="1">
+      <c r="B90" s="1" t="n">
         <v>398</v>
       </c>
       <c r="D90" s="1" t="s">
@@ -2610,11 +2384,11 @@
         <v>133</v>
       </c>
     </row>
-    <row r="91" spans="1:5" hidden="1">
-      <c r="A91" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="91">
+      <c r="A91" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B91" s="1">
+      <c r="B91" s="1" t="n">
         <v>226</v>
       </c>
       <c r="D91" s="1" t="s">
@@ -2624,11 +2398,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="92" spans="1:5" hidden="1">
-      <c r="A92" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="92">
+      <c r="A92" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B92" s="1">
+      <c r="B92" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D92" s="1" t="s">
@@ -2638,11 +2412,11 @@
         <v>137</v>
       </c>
     </row>
-    <row r="93" spans="1:5" hidden="1">
-      <c r="A93" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="93">
+      <c r="A93" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="B93" s="1">
+      <c r="B93" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D93" s="1" t="s">
@@ -2652,11 +2426,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="94" spans="1:5" hidden="1">
-      <c r="A94" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="94">
+      <c r="A94" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="C94" s="1">
+      <c r="C94" s="1" t="n">
         <v>340</v>
       </c>
       <c r="D94" s="1" t="s">
@@ -2666,11 +2440,11 @@
         <v>139</v>
       </c>
     </row>
-    <row r="95" spans="1:5" hidden="1">
-      <c r="A95" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="95">
+      <c r="A95" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="B95" s="1">
+      <c r="B95" s="1" t="n">
         <v>510</v>
       </c>
       <c r="D95" s="1" t="s">
@@ -2680,11 +2454,11 @@
         <v>141</v>
       </c>
     </row>
-    <row r="96" spans="1:5" hidden="1">
-      <c r="A96" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="96">
+      <c r="A96" s="2" t="n">
         <v>43233</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B96" s="1" t="n">
         <v>170</v>
       </c>
       <c r="D96" s="1" t="s">
@@ -2694,11 +2468,11 @@
         <v>143</v>
       </c>
     </row>
-    <row r="97" spans="1:5" hidden="1">
-      <c r="A97" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="97">
+      <c r="A97" s="2" t="n">
         <v>43233</v>
       </c>
-      <c r="C97" s="1">
+      <c r="C97" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D97" s="1" t="s">
@@ -2708,11 +2482,11 @@
         <v>144</v>
       </c>
     </row>
-    <row r="98" spans="1:5" hidden="1">
-      <c r="A98" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="98">
+      <c r="A98" s="2" t="n">
         <v>43234</v>
       </c>
-      <c r="C98" s="1">
+      <c r="C98" s="1" t="n">
         <v>299</v>
       </c>
       <c r="D98" s="1" t="s">
@@ -2722,11 +2496,11 @@
         <v>145</v>
       </c>
     </row>
-    <row r="99" spans="1:5" hidden="1">
-      <c r="A99" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="99">
+      <c r="A99" s="2" t="n">
         <v>43236</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99" s="1" t="n">
         <v>3659</v>
       </c>
       <c r="D99" s="1" t="s">
@@ -2736,11 +2510,11 @@
         <v>146</v>
       </c>
     </row>
-    <row r="100" spans="1:5" hidden="1">
-      <c r="A100" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="100">
+      <c r="A100" s="2" t="n">
         <v>43237</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B100" s="1" t="n">
         <v>79</v>
       </c>
       <c r="D100" s="1" t="s">
@@ -2750,11 +2524,11 @@
         <v>147</v>
       </c>
     </row>
-    <row r="101" spans="1:5" hidden="1">
-      <c r="A101" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="101">
+      <c r="A101" s="2" t="n">
         <v>43236</v>
       </c>
-      <c r="C101" s="1">
+      <c r="C101" s="1" t="n">
         <v>173</v>
       </c>
       <c r="D101" s="1" t="s">
@@ -2764,11 +2538,11 @@
         <v>148</v>
       </c>
     </row>
-    <row r="102" spans="1:5" hidden="1">
-      <c r="A102" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="102">
+      <c r="A102" s="2" t="n">
         <v>43240</v>
       </c>
-      <c r="B102" s="1">
+      <c r="B102" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D102" s="1" t="s">
@@ -2778,22 +2552,22 @@
         <v>149</v>
       </c>
     </row>
-    <row r="103" spans="1:5" hidden="1">
-      <c r="A103" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="103">
+      <c r="A103" s="2" t="n">
         <v>43240</v>
       </c>
-      <c r="B103" s="1">
+      <c r="B103" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="104" spans="1:5" hidden="1">
-      <c r="A104" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="104">
+      <c r="A104" s="2" t="n">
         <v>43241</v>
       </c>
-      <c r="B104" s="1">
+      <c r="B104" s="1" t="n">
         <v>4070</v>
       </c>
       <c r="D104" s="1" t="s">
@@ -2803,11 +2577,11 @@
         <v>150</v>
       </c>
     </row>
-    <row r="105" spans="1:5" hidden="1">
-      <c r="A105" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="105">
+      <c r="A105" s="2" t="n">
         <v>43241</v>
       </c>
-      <c r="C105" s="1">
+      <c r="C105" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D105" s="1" t="s">
@@ -2817,11 +2591,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="106" spans="1:5" hidden="1">
-      <c r="A106" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="106">
+      <c r="A106" s="2" t="n">
         <v>43242</v>
       </c>
-      <c r="B106" s="1">
+      <c r="B106" s="1" t="n">
         <v>79</v>
       </c>
       <c r="D106" s="1" t="s">
@@ -2831,11 +2605,11 @@
         <v>152</v>
       </c>
     </row>
-    <row r="107" spans="1:5" hidden="1">
-      <c r="A107" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="107">
+      <c r="A107" s="2" t="n">
         <v>43246</v>
       </c>
-      <c r="B107" s="1">
+      <c r="B107" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D107" s="1" t="s">
@@ -2845,11 +2619,11 @@
         <v>154</v>
       </c>
     </row>
-    <row r="108" spans="1:5" hidden="1">
-      <c r="A108" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="108">
+      <c r="A108" s="2" t="n">
         <v>43247</v>
       </c>
-      <c r="B108" s="1">
+      <c r="B108" s="1" t="n">
         <v>70</v>
       </c>
       <c r="D108" s="1" t="s">
@@ -2859,44 +2633,44 @@
         <v>156</v>
       </c>
     </row>
-    <row r="109" spans="1:5" hidden="1">
-      <c r="A109" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="109">
+      <c r="A109" s="2" t="n">
         <v>43253</v>
       </c>
-      <c r="B109" s="1">
+      <c r="B109" s="1" t="n">
         <v>142</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="110" spans="1:5" hidden="1">
-      <c r="A110" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="110">
+      <c r="A110" s="2" t="n">
         <v>43254</v>
       </c>
-      <c r="B110" s="1">
+      <c r="B110" s="1" t="n">
         <v>90</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="111" spans="1:5" hidden="1">
-      <c r="A111" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="111">
+      <c r="A111" s="2" t="n">
         <v>43260</v>
       </c>
-      <c r="C111" s="1">
+      <c r="C111" s="1" t="n">
         <v>1400</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="112" spans="1:5" hidden="1">
-      <c r="A112" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="112">
+      <c r="A112" s="2" t="n">
         <v>43260</v>
       </c>
-      <c r="C112" s="1">
+      <c r="C112" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D112" s="1" t="s">
@@ -2906,33 +2680,33 @@
         <v>91</v>
       </c>
     </row>
-    <row r="113" spans="1:5" hidden="1">
-      <c r="A113" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="113">
+      <c r="A113" s="2" t="n">
         <v>43264</v>
       </c>
-      <c r="B113" s="1">
+      <c r="B113" s="1" t="n">
         <v>546</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="114" spans="1:5" hidden="1">
-      <c r="A114" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="114">
+      <c r="A114" s="2" t="n">
         <v>43264</v>
       </c>
-      <c r="B114" s="1">
+      <c r="B114" s="1" t="n">
         <v>95</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="115" spans="1:5" hidden="1">
-      <c r="A115" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="115">
+      <c r="A115" s="2" t="n">
         <v>43266</v>
       </c>
-      <c r="B115" s="1">
+      <c r="B115" s="1" t="n">
         <v>394</v>
       </c>
       <c r="D115" s="1" t="s">
@@ -2942,11 +2716,11 @@
         <v>163</v>
       </c>
     </row>
-    <row r="116" spans="1:5" hidden="1">
-      <c r="A116" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="116">
+      <c r="A116" s="2" t="n">
         <v>43266</v>
       </c>
-      <c r="B116" s="1">
+      <c r="B116" s="1" t="n">
         <v>1055</v>
       </c>
       <c r="D116" s="1" t="s">
@@ -2956,11 +2730,11 @@
         <v>165</v>
       </c>
     </row>
-    <row r="117" spans="1:5" hidden="1">
-      <c r="A117" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="117">
+      <c r="A117" s="2" t="n">
         <v>43284</v>
       </c>
-      <c r="C117" s="1">
+      <c r="C117" s="1" t="n">
         <v>274</v>
       </c>
       <c r="D117" s="1" t="s">
@@ -2970,11 +2744,11 @@
         <v>167</v>
       </c>
     </row>
-    <row r="118" spans="1:5" hidden="1">
-      <c r="A118" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="118">
+      <c r="A118" s="2" t="n">
         <v>43283</v>
       </c>
-      <c r="C118" s="1">
+      <c r="C118" s="1" t="n">
         <v>105</v>
       </c>
       <c r="D118" s="1" t="s">
@@ -2984,11 +2758,11 @@
         <v>169</v>
       </c>
     </row>
-    <row r="119" spans="1:5" hidden="1">
-      <c r="A119" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="119">
+      <c r="A119" s="2" t="n">
         <v>43289</v>
       </c>
-      <c r="C119" s="1">
+      <c r="C119" s="1" t="n">
         <v>128</v>
       </c>
       <c r="D119" s="1" t="s">
@@ -2998,11 +2772,11 @@
         <v>171</v>
       </c>
     </row>
-    <row r="120" spans="1:5" hidden="1">
-      <c r="A120" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="120">
+      <c r="A120" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C120" s="1">
+      <c r="C120" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D120" s="1" t="s">
@@ -3012,11 +2786,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="121" spans="1:5" hidden="1">
-      <c r="A121" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="121">
+      <c r="A121" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C121" s="1">
+      <c r="C121" s="1" t="n">
         <v>210</v>
       </c>
       <c r="D121" s="1" t="s">
@@ -3026,44 +2800,44 @@
         <v>173</v>
       </c>
     </row>
-    <row r="122" spans="1:5" hidden="1">
-      <c r="A122" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="122">
+      <c r="A122" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B122" s="1">
+      <c r="B122" s="1" t="n">
         <v>980</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="123" spans="1:5" hidden="1">
-      <c r="A123" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="123">
+      <c r="A123" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B123" s="1">
+      <c r="B123" s="1" t="n">
         <v>1260</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="124" spans="1:5" hidden="1">
-      <c r="A124" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="124">
+      <c r="A124" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B124" s="1">
+      <c r="B124" s="1" t="n">
         <v>3687</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="125" spans="1:5" hidden="1">
-      <c r="A125" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="125">
+      <c r="A125" s="2" t="n">
         <v>43298</v>
       </c>
-      <c r="C125" s="1">
+      <c r="C125" s="1" t="n">
         <v>60</v>
       </c>
       <c r="D125" s="1" t="s">
@@ -3073,55 +2847,55 @@
         <v>178</v>
       </c>
     </row>
-    <row r="126" spans="1:5" hidden="1">
-      <c r="A126" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="126">
+      <c r="A126" s="2" t="n">
         <v>43291</v>
       </c>
-      <c r="C126" s="1">
+      <c r="C126" s="1" t="n">
         <v>404</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="127" spans="1:5" hidden="1">
-      <c r="A127" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="127">
+      <c r="A127" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C127" s="1">
+      <c r="C127" s="1" t="n">
         <v>451</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="128" spans="1:5" hidden="1">
-      <c r="A128" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="128">
+      <c r="A128" s="2" t="n">
         <v>43298</v>
       </c>
-      <c r="C128" s="1">
+      <c r="C128" s="1" t="n">
         <v>708</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="129" spans="1:5" hidden="1">
-      <c r="A129" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="129">
+      <c r="A129" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C129" s="1">
+      <c r="C129" s="1" t="n">
         <v>160</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="130" spans="1:5" hidden="1">
-      <c r="A130" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="130">
+      <c r="A130" s="2" t="n">
         <v>43288</v>
       </c>
-      <c r="C130" s="1">
+      <c r="C130" s="1" t="n">
         <v>72</v>
       </c>
       <c r="D130" s="1" t="s">
@@ -3131,11 +2905,11 @@
         <v>181</v>
       </c>
     </row>
-    <row r="131" spans="1:5" hidden="1">
-      <c r="A131" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="131">
+      <c r="A131" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C131" s="1">
+      <c r="C131" s="1" t="n">
         <v>300</v>
       </c>
       <c r="D131" s="1" t="s">
@@ -3145,11 +2919,11 @@
         <v>183</v>
       </c>
     </row>
-    <row r="132" spans="1:5" hidden="1">
-      <c r="A132" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="132">
+      <c r="A132" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C132" s="1">
+      <c r="C132" s="1" t="n">
         <v>230</v>
       </c>
       <c r="D132" s="1" t="s">
@@ -3159,22 +2933,22 @@
         <v>185</v>
       </c>
     </row>
-    <row r="133" spans="1:5" hidden="1">
-      <c r="A133" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="133">
+      <c r="A133" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C133" s="1">
+      <c r="C133" s="1" t="n">
         <v>454</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="134" spans="1:5" hidden="1">
-      <c r="A134" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="134">
+      <c r="A134" s="2" t="n">
         <v>43299</v>
       </c>
-      <c r="C134" s="1">
+      <c r="C134" s="1" t="n">
         <v>686</v>
       </c>
       <c r="D134" s="1" t="s">
@@ -3184,11 +2958,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="135" spans="1:5" hidden="1">
-      <c r="A135" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="135">
+      <c r="A135" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C135" s="1">
+      <c r="C135" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D135" s="1" t="s">
@@ -3198,11 +2972,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="136" spans="1:5" hidden="1">
-      <c r="A136" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="136">
+      <c r="A136" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C136" s="1">
+      <c r="C136" s="1" t="n">
         <v>2067</v>
       </c>
       <c r="D136" s="1" t="s">
@@ -3212,11 +2986,11 @@
         <v>186</v>
       </c>
     </row>
-    <row r="137" spans="1:5" hidden="1">
-      <c r="A137" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="137">
+      <c r="A137" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B137" s="1">
+      <c r="B137" s="1" t="n">
         <v>109</v>
       </c>
       <c r="D137" s="1" t="s">
@@ -3226,11 +3000,11 @@
         <v>187</v>
       </c>
     </row>
-    <row r="138" spans="1:5" hidden="1">
-      <c r="A138" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="138">
+      <c r="A138" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B138" s="1">
+      <c r="B138" s="1" t="n">
         <v>97</v>
       </c>
       <c r="D138" s="1" t="s">
@@ -3240,11 +3014,11 @@
         <v>188</v>
       </c>
     </row>
-    <row r="139" spans="1:5" hidden="1">
-      <c r="A139" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="139">
+      <c r="A139" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B139" s="1">
+      <c r="B139" s="1" t="n">
         <v>1437</v>
       </c>
       <c r="D139" s="1" t="s">
@@ -3254,11 +3028,11 @@
         <v>189</v>
       </c>
     </row>
-    <row r="140" spans="1:5" hidden="1">
-      <c r="A140" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="140">
+      <c r="A140" s="2" t="n">
         <v>43306</v>
       </c>
-      <c r="C140" s="1">
+      <c r="C140" s="1" t="n">
         <v>650</v>
       </c>
       <c r="D140" s="1" t="s">
@@ -3268,11 +3042,11 @@
         <v>190</v>
       </c>
     </row>
-    <row r="141" spans="1:5" hidden="1">
-      <c r="A141" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="141">
+      <c r="A141" s="2" t="n">
         <v>43305</v>
       </c>
-      <c r="C141" s="1">
+      <c r="C141" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D141" s="1" t="s">
@@ -3282,11 +3056,11 @@
         <v>191</v>
       </c>
     </row>
-    <row r="142" spans="1:5" hidden="1">
-      <c r="A142" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="142">
+      <c r="A142" s="2" t="n">
         <v>43309</v>
       </c>
-      <c r="C142" s="1">
+      <c r="C142" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D142" s="1" t="s">
@@ -3296,11 +3070,11 @@
         <v>192</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="14" hidden="1">
-      <c r="A143" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="0" r="143">
+      <c r="A143" s="2" t="n">
         <v>43306</v>
       </c>
-      <c r="B143" s="1">
+      <c r="B143" s="1" t="n">
         <v>167</v>
       </c>
       <c r="D143" s="1" t="s">
@@ -3310,11 +3084,11 @@
         <v>193</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="14" hidden="1">
-      <c r="A144" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="0" r="144">
+      <c r="A144" s="2" t="n">
         <v>43304</v>
       </c>
-      <c r="C144" s="1">
+      <c r="C144" s="1" t="n">
         <v>93</v>
       </c>
       <c r="D144" s="1" t="s">
@@ -3324,11 +3098,11 @@
         <v>194</v>
       </c>
     </row>
-    <row r="145" spans="1:5" hidden="1">
-      <c r="A145" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="145">
+      <c r="A145" s="2" t="n">
         <v>43305</v>
       </c>
-      <c r="C145" s="1">
+      <c r="C145" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D145" s="1" t="s">
@@ -3338,11 +3112,11 @@
         <v>195</v>
       </c>
     </row>
-    <row r="146" spans="1:5" hidden="1">
-      <c r="A146" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="146">
+      <c r="A146" s="2" t="n">
         <v>43303</v>
       </c>
-      <c r="C146" s="1">
+      <c r="C146" s="1" t="n">
         <v>244</v>
       </c>
       <c r="D146" s="1" t="s">
@@ -3352,11 +3126,11 @@
         <v>196</v>
       </c>
     </row>
-    <row r="147" spans="1:5" hidden="1">
-      <c r="A147" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="147">
+      <c r="A147" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C147" s="1">
+      <c r="C147" s="1" t="n">
         <v>482</v>
       </c>
       <c r="D147" s="1" t="s">
@@ -3366,11 +3140,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="148" spans="1:5" hidden="1">
-      <c r="A148" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="148">
+      <c r="A148" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C148" s="1">
+      <c r="C148" s="1" t="n">
         <v>172</v>
       </c>
       <c r="D148" s="1" t="s">
@@ -3380,44 +3154,44 @@
         <v>199</v>
       </c>
     </row>
-    <row r="149" spans="1:5" hidden="1">
-      <c r="A149" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="149">
+      <c r="A149" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="B149" s="1">
+      <c r="B149" s="1" t="n">
         <v>89</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="150" spans="1:5" hidden="1">
-      <c r="A150" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="150">
+      <c r="A150" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="C150" s="1">
+      <c r="C150" s="1" t="n">
         <v>107</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="151" spans="1:5" hidden="1">
-      <c r="A151" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="151">
+      <c r="A151" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="C151" s="1">
+      <c r="C151" s="1" t="n">
         <v>124</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="152" spans="1:5" hidden="1">
-      <c r="A152" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="152">
+      <c r="A152" s="7" t="n">
         <v>43316</v>
       </c>
-      <c r="C152" s="1">
+      <c r="C152" s="1" t="n">
         <v>4500</v>
       </c>
       <c r="D152" s="1" t="s">
@@ -3427,11 +3201,11 @@
         <v>202</v>
       </c>
     </row>
-    <row r="153" spans="1:5" hidden="1">
-      <c r="A153" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="153">
+      <c r="A153" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C153" s="1">
+      <c r="C153" s="1" t="n">
         <v>247</v>
       </c>
       <c r="D153" s="1" t="s">
@@ -3441,11 +3215,11 @@
         <v>204</v>
       </c>
     </row>
-    <row r="154" spans="1:5" hidden="1">
-      <c r="A154" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="154">
+      <c r="A154" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C154" s="1">
+      <c r="C154" s="1" t="n">
         <v>1150</v>
       </c>
       <c r="D154" s="1" t="s">
@@ -3455,11 +3229,11 @@
         <v>205</v>
       </c>
     </row>
-    <row r="155" spans="1:5" hidden="1">
-      <c r="A155" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="155">
+      <c r="A155" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C155" s="1">
+      <c r="C155" s="1" t="n">
         <v>313</v>
       </c>
       <c r="D155" s="1" t="s">
@@ -3469,11 +3243,11 @@
         <v>207</v>
       </c>
     </row>
-    <row r="156" spans="1:5" hidden="1">
-      <c r="A156" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="156">
+      <c r="A156" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="B156" s="1">
+      <c r="B156" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D156" s="1" t="s">
@@ -3483,11 +3257,11 @@
         <v>209</v>
       </c>
     </row>
-    <row r="157" spans="1:5" hidden="1">
-      <c r="A157" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="157">
+      <c r="A157" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="C157" s="1">
+      <c r="C157" s="1" t="n">
         <v>710</v>
       </c>
       <c r="D157" s="1" t="s">
@@ -3497,11 +3271,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="158" spans="1:5">
-      <c r="A158" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="158">
+      <c r="A158" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="C158" s="1">
+      <c r="C158" s="1" t="n">
         <v>100</v>
       </c>
       <c r="D158" s="1" t="s">
@@ -3511,11 +3285,11 @@
         <v>212</v>
       </c>
     </row>
-    <row r="159" spans="1:5">
-      <c r="A159" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="159">
+      <c r="A159" s="2" t="n">
         <v>43319</v>
       </c>
-      <c r="B159" s="1">
+      <c r="B159" s="1" t="n">
         <v>78</v>
       </c>
       <c r="D159" s="1" t="s">
@@ -3525,22 +3299,22 @@
         <v>213</v>
       </c>
     </row>
-    <row r="160" spans="1:5">
-      <c r="A160" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="160">
+      <c r="A160" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="B160" s="1">
+      <c r="B160" s="1" t="n">
         <v>1840</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="161" spans="1:5">
-      <c r="A161" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="161">
+      <c r="A161" s="2" t="n">
         <v>43322</v>
       </c>
-      <c r="B161" s="1">
+      <c r="B161" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D161" s="1" t="s">
@@ -3550,11 +3324,11 @@
         <v>216</v>
       </c>
     </row>
-    <row r="162" spans="1:5">
-      <c r="A162" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="162">
+      <c r="A162" s="7" t="n">
         <v>43324</v>
       </c>
-      <c r="C162" s="1">
+      <c r="C162" s="1" t="n">
         <v>230</v>
       </c>
       <c r="D162" s="1" t="s">
@@ -3564,11 +3338,11 @@
         <v>217</v>
       </c>
     </row>
-    <row r="163" spans="1:5">
-      <c r="A163" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="163">
+      <c r="A163" s="7" t="n">
         <v>43326</v>
       </c>
-      <c r="C163" s="1">
+      <c r="C163" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D163" s="1" t="s">
@@ -3578,11 +3352,11 @@
         <v>219</v>
       </c>
     </row>
-    <row r="164" spans="1:5">
-      <c r="A164" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="164">
+      <c r="A164" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="B164" s="1">
+      <c r="B164" s="1" t="n">
         <v>45</v>
       </c>
       <c r="D164" s="1" t="s">
@@ -3592,615 +3366,634 @@
         <v>221</v>
       </c>
     </row>
-    <row r="165" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A165" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="165">
+      <c r="A165" s="10" t="n">
         <v>43327</v>
       </c>
-      <c r="C165">
+      <c r="C165" s="0" t="n">
         <v>486</v>
       </c>
-      <c r="D165" t="s">
+      <c r="D165" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E165" t="s">
+      <c r="E165" s="0" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="166" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A166" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="166">
+      <c r="A166" s="10" t="n">
         <v>43329</v>
       </c>
-      <c r="C166">
+      <c r="C166" s="0" t="n">
         <v>92</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D166" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="E166" t="s">
+      <c r="E166" s="0" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="167" spans="1:5">
-      <c r="A167" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="167">
+      <c r="A167" s="10" t="n">
         <v>43331</v>
       </c>
-      <c r="C167">
+      <c r="C167" s="0" t="n">
         <v>310</v>
       </c>
-      <c r="D167" t="s">
+      <c r="D167" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="E167" t="s">
+      <c r="E167" s="0" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="168" spans="1:5">
-      <c r="A168" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="168">
+      <c r="A168" s="10" t="n">
         <v>43334</v>
       </c>
-      <c r="C168">
+      <c r="C168" s="0" t="n">
         <v>464</v>
       </c>
-      <c r="D168" t="s">
+      <c r="D168" s="0" t="s">
         <v>218</v>
       </c>
       <c r="E168" s="11" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="169" spans="1:5">
-      <c r="A169" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="169">
+      <c r="A169" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="C169">
+      <c r="C169" s="0" t="n">
         <v>726</v>
       </c>
-      <c r="D169" t="s">
+      <c r="D169" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="E169" t="s">
+      <c r="E169" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="170" spans="1:5">
-      <c r="A170" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="170">
+      <c r="A170" s="10" t="n">
         <v>43337</v>
       </c>
-      <c r="C170">
+      <c r="C170" s="0" t="n">
         <v>544</v>
       </c>
-      <c r="D170" t="s">
+      <c r="D170" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E170" t="s">
+      <c r="E170" s="0" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="171" spans="1:5">
-      <c r="A171" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="171">
+      <c r="A171" s="10" t="n">
         <v>43337</v>
       </c>
-      <c r="B171">
+      <c r="B171" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D171" t="s">
+      <c r="D171" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="E171" t="s">
+      <c r="E171" s="0" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="172" spans="1:5">
-      <c r="A172" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="172">
+      <c r="A172" s="10" t="n">
         <v>43341</v>
       </c>
-      <c r="C172">
+      <c r="C172" s="0" t="n">
         <v>830</v>
       </c>
-      <c r="D172" t="s">
+      <c r="D172" s="0" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="173" spans="1:5">
-      <c r="A173" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="173">
+      <c r="A173" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="C173">
+      <c r="C173" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="D173" t="s">
+      <c r="D173" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="E173" t="s">
+      <c r="E173" s="0" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="174" spans="1:5">
-      <c r="A174" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="174">
+      <c r="A174" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="B174">
+      <c r="B174" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D174" t="s">
+      <c r="D174" s="0" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="175" spans="1:5">
-      <c r="A175" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="175">
+      <c r="A175" s="10" t="n">
         <v>43344</v>
       </c>
-      <c r="B175">
+      <c r="B175" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="D175" t="s">
+      <c r="D175" s="0" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="176" spans="1:5">
-      <c r="A176" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="176">
+      <c r="A176" s="10" t="n">
         <v>43344</v>
       </c>
-      <c r="B176">
+      <c r="B176" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D176" t="s">
+      <c r="D176" s="0" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="177" spans="1:5">
-      <c r="A177" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="177">
+      <c r="A177" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C177">
+      <c r="C177" s="0" t="n">
         <v>607</v>
       </c>
-      <c r="D177" t="s">
+      <c r="D177" s="0" t="s">
         <v>235</v>
       </c>
-      <c r="E177" t="s">
+      <c r="E177" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="178" spans="1:5">
-      <c r="A178" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="178">
+      <c r="A178" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C178">
+      <c r="C178" s="0" t="n">
         <v>444</v>
       </c>
-      <c r="D178" t="s">
+      <c r="D178" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E178" t="s">
+      <c r="E178" s="0" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="179" spans="1:5">
-      <c r="A179" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="179">
+      <c r="A179" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C179">
+      <c r="C179" s="0" t="n">
         <v>312</v>
       </c>
-      <c r="D179" t="s">
+      <c r="D179" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="E179" t="s">
+      <c r="E179" s="0" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="180" spans="1:5">
-      <c r="A180" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="180">
+      <c r="A180" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C180">
+      <c r="C180" s="0" t="n">
         <v>501</v>
       </c>
-      <c r="D180" t="s">
+      <c r="D180" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E180" t="s">
+      <c r="E180" s="0" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="181" spans="1:5">
-      <c r="A181" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="181">
+      <c r="A181" s="10" t="n">
         <v>43349</v>
       </c>
-      <c r="C181">
+      <c r="C181" s="0" t="n">
         <v>711</v>
       </c>
-      <c r="D181" t="s">
+      <c r="D181" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="E181" t="s">
+      <c r="E181" s="0" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="182" spans="1:5">
-      <c r="A182" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="182">
+      <c r="A182" s="10" t="n">
         <v>43354</v>
       </c>
-      <c r="B182">
+      <c r="B182" s="0" t="n">
         <v>126</v>
       </c>
-      <c r="D182" t="s">
+      <c r="D182" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="E182" t="s">
+      <c r="E182" s="0" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="183" spans="1:5">
-      <c r="A183" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="183">
+      <c r="A183" s="10" t="n">
         <v>43354</v>
       </c>
-      <c r="C183">
+      <c r="C183" s="0" t="n">
         <v>450</v>
       </c>
-      <c r="D183" t="s">
+      <c r="D183" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="E183" t="s">
+      <c r="E183" s="0" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="184" spans="1:5">
-      <c r="A184" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="184">
+      <c r="A184" s="10" t="n">
         <v>43361</v>
       </c>
-      <c r="C184">
+      <c r="C184" s="0" t="n">
         <v>660</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D184" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="E184" t="s">
+      <c r="E184" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="185" spans="1:5">
-      <c r="A185" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="185">
+      <c r="A185" s="10" t="n">
         <v>43363</v>
       </c>
-      <c r="C185">
+      <c r="C185" s="0" t="n">
         <v>230</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D185" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="E185" t="s">
+      <c r="E185" s="0" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="186" spans="1:5">
-      <c r="A186" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="186">
+      <c r="A186" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B186">
+      <c r="B186" s="0" t="n">
         <v>4859</v>
       </c>
-      <c r="D186" t="s">
+      <c r="D186" s="0" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="187" spans="1:5">
-      <c r="A187" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="187">
+      <c r="A187" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B187">
+      <c r="B187" s="0" t="n">
         <v>295</v>
       </c>
-      <c r="D187" t="s">
+      <c r="D187" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="E187" t="s">
+      <c r="E187" s="0" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="188" spans="1:5">
-      <c r="A188" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="188">
+      <c r="A188" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B188">
+      <c r="B188" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D188" t="s">
+      <c r="D188" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="E188" t="s">
+      <c r="E188" s="0" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="189" spans="1:5">
-      <c r="A189" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="189">
+      <c r="A189" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B189">
+      <c r="B189" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="D189" t="s">
+      <c r="D189" s="0" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="190" spans="1:5">
-      <c r="A190" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="190">
+      <c r="A190" s="10" t="n">
         <v>43378</v>
       </c>
-      <c r="B190">
+      <c r="B190" s="0" t="n">
         <v>506</v>
       </c>
-      <c r="D190" t="s">
+      <c r="D190" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="E190" t="s">
+      <c r="E190" s="0" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="191" spans="1:5">
-      <c r="A191" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="191">
+      <c r="A191" s="10" t="n">
         <v>43379</v>
       </c>
-      <c r="B191">
+      <c r="B191" s="0" t="n">
         <v>350</v>
       </c>
-      <c r="D191" t="s">
+      <c r="D191" s="0" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="192" spans="1:5">
-      <c r="A192" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="192">
+      <c r="A192" s="10" t="n">
         <v>43383</v>
       </c>
-      <c r="B192">
+      <c r="B192" s="0" t="n">
         <v>189</v>
       </c>
-      <c r="D192" t="s">
+      <c r="D192" s="0" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="193" spans="1:5">
-      <c r="A193" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="193">
+      <c r="A193" s="10" t="n">
         <v>43387</v>
       </c>
-      <c r="B193">
+      <c r="B193" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="D193" t="s">
+      <c r="D193" s="0" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="194" spans="1:5">
-      <c r="A194" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="194">
+      <c r="A194" s="10" t="n">
         <v>43387</v>
       </c>
-      <c r="B194">
+      <c r="B194" s="0" t="n">
         <v>307</v>
       </c>
-      <c r="D194" t="s">
+      <c r="D194" s="0" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="195" spans="1:5">
-      <c r="C195">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="195">
+      <c r="C195" s="0" t="n">
         <v>3705</v>
       </c>
-      <c r="E195" t="s">
+      <c r="E195" s="0" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="196" spans="1:5">
-      <c r="A196" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="196">
+      <c r="A196" s="10" t="n">
         <v>43385</v>
       </c>
-      <c r="C196">
+      <c r="C196" s="0" t="n">
         <v>608</v>
       </c>
-      <c r="D196" t="s">
+      <c r="D196" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E196" t="s">
+      <c r="E196" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="197" spans="1:5">
-      <c r="A197" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="197">
+      <c r="A197" s="10" t="n">
         <v>43391</v>
       </c>
-      <c r="B197">
+      <c r="B197" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="D197" t="s">
+      <c r="D197" s="0" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="198" spans="1:5">
-      <c r="A198" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="198">
+      <c r="A198" s="10" t="n">
         <v>43392</v>
       </c>
-      <c r="B198">
+      <c r="B198" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="D198" t="s">
+      <c r="D198" s="0" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="199" spans="1:5">
-      <c r="A199" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="199">
+      <c r="A199" s="10" t="n">
         <v>43393</v>
       </c>
-      <c r="B199">
+      <c r="B199" s="0" t="n">
         <v>177</v>
       </c>
-      <c r="D199" t="s">
+      <c r="D199" s="0" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="200" spans="1:5">
-      <c r="A200" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="200">
+      <c r="A200" s="10" t="n">
         <v>43393</v>
       </c>
-      <c r="C200">
+      <c r="C200" s="0" t="n">
         <v>125</v>
       </c>
-      <c r="D200" t="s">
+      <c r="D200" s="0" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="201" spans="1:5">
-      <c r="A201" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="201">
+      <c r="A201" s="10" t="n">
         <v>43395</v>
       </c>
-      <c r="B201">
+      <c r="B201" s="0" t="n">
         <v>2800</v>
       </c>
       <c r="D201" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="E201" t="s">
+      <c r="E201" s="0" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="202" spans="1:5">
-      <c r="A202" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="202">
+      <c r="A202" s="10" t="n">
         <v>43395</v>
       </c>
-      <c r="C202">
+      <c r="C202" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="D202" t="s">
+      <c r="D202" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="E202" t="s">
+      <c r="E202" s="0" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="203" spans="1:5">
-      <c r="A203" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="203">
+      <c r="A203" s="10" t="n">
         <v>43396</v>
       </c>
-      <c r="C203">
+      <c r="C203" s="0" t="n">
         <v>692</v>
       </c>
-      <c r="D203" t="s">
+      <c r="D203" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E203" t="s">
+      <c r="E203" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="204" spans="1:5">
-      <c r="A204" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="204">
+      <c r="A204" s="10" t="n">
         <v>43397</v>
       </c>
-      <c r="C204">
+      <c r="C204" s="0" t="n">
         <v>4935</v>
       </c>
-      <c r="D204" t="s">
+      <c r="D204" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="E204" t="s">
+      <c r="E204" s="0" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="205" spans="1:5">
-      <c r="A205" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="205">
+      <c r="A205" s="10" t="n">
         <v>43398</v>
       </c>
-      <c r="B205">
+      <c r="B205" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="D205" t="s">
+      <c r="D205" s="0" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="206" spans="1:5">
-      <c r="A206" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="206">
+      <c r="A206" s="10" t="n">
         <v>43398</v>
       </c>
-      <c r="B206">
+      <c r="B206" s="0" t="n">
         <v>370</v>
       </c>
-      <c r="D206" t="s">
+      <c r="D206" s="0" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="207" spans="1:5">
-      <c r="A207" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="207">
+      <c r="A207" s="10" t="n">
         <v>43398</v>
       </c>
-      <c r="B207">
+      <c r="B207" s="0" t="n">
         <v>4966</v>
       </c>
-      <c r="D207" t="s">
+      <c r="D207" s="0" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="208" spans="1:5">
-      <c r="A208" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="208">
+      <c r="A208" s="10" t="n">
         <v>43397</v>
       </c>
-      <c r="C208">
+      <c r="C208" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="D208" t="s">
+      <c r="D208" s="0" t="s">
         <v>265</v>
       </c>
-      <c r="E208" t="s">
+      <c r="E208" s="0" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="209" spans="1:5">
-      <c r="A209" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="209">
+      <c r="A209" s="10" t="n">
         <v>43399</v>
       </c>
-      <c r="B209">
+      <c r="B209" s="0" t="n">
         <v>182</v>
       </c>
-      <c r="D209" t="s">
+      <c r="D209" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="E209" t="s">
+      <c r="E209" s="0" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="210" spans="1:5">
-      <c r="A210" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="210">
+      <c r="A210" s="10" t="n">
         <v>43401</v>
       </c>
-      <c r="B210">
+      <c r="B210" s="0" t="n">
         <v>700</v>
       </c>
-      <c r="D210" t="s">
+      <c r="D210" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="E210" t="s">
+      <c r="E210" s="0" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="220" spans="1:5">
-      <c r="B220">
-        <f>SUM(B2:B219)</f>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="211">
+      <c r="A211" s="10" t="n">
+        <v>43403</v>
+      </c>
+      <c r="C211" s="0" t="n">
+        <v>5561</v>
+      </c>
+      <c r="D211" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="E211" s="0" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="220">
+      <c r="B220" s="0" t="n">
+        <f aca="false">SUM(B2:B219)</f>
         <v>55638</v>
       </c>
-      <c r="C220">
-        <f>SUM(C2:C219)</f>
-        <v>52501</v>
+      <c r="C220" s="0" t="n">
+        <f aca="false">SUM(C2:C219)</f>
+        <v>58062</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A30:Z32">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule aboveAverage="0" bottom="0" dxfId="0" operator="expression" percent="0" priority="2" rank="0" text="" type="expression">
       <formula>LEN(TRIM(A30))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D33" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D40" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D201" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink display="netonnet.se" ref="D33" r:id="rId1"/>
+    <hyperlink display="www.vidaxl.se" ref="D40" r:id="rId2"/>
+    <hyperlink display="https://www.vardia.se/" ref="D201" r:id="rId3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cost update jenny 1106
</commit_message>
<xml_diff>
--- a/Cost.xlsx
+++ b/Cost.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chengkaiyan/github/cost/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD41423-9D62-7343-BE12-285B2902167C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="274">
   <si>
     <t>日期</t>
   </si>
@@ -836,61 +831,83 @@
   </si>
   <si>
     <t>avgift</t>
+  </si>
+  <si>
+    <t>ICA kista</t>
+  </si>
+  <si>
+    <t>ananas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="yyyy/m/d"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt formatCode="YYYY/M/D" numFmtId="165"/>
+    <numFmt formatCode="M/D/YYYY" numFmtId="166"/>
+    <numFmt formatCode="YYYY\-MM\-DD" numFmtId="167"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="10">
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <family val="0"/>
       <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
       <name val="Arial"/>
       <family val="2"/>
+      <sz val="10"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF666666"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF666666"/>
+      <sz val="11"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0563C1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF0563C1"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0563C1"/>
       <name val="FreeSans"/>
       <family val="2"/>
+      <color rgb="FF0563C1"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF444444"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF444444"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="5">
@@ -920,7 +937,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
@@ -928,31 +945,100 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+  <cellStyleXfs count="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="167" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="20">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="7">
+    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle builtinId="8" customBuiltin="false" name="*unknown*" xfId="20"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -963,7 +1049,6 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1021,340 +1106,32 @@
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="FF444444"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:Z220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A191" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C216" sqref="C216"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A194" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D221" activeCellId="0" pane="topLeft" sqref="D221"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="3" width="14.5"/>
-    <col min="4" max="4" width="26"/>
-    <col min="5" max="5" width="37.83203125"/>
-    <col min="6" max="1025" width="14.5"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="14.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1371,11 +1148,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1">
-      <c r="A2" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="2">
+      <c r="A2" s="2" t="n">
         <v>43121</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="1" t="n">
         <v>250</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1385,11 +1162,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1">
-      <c r="A3" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="3">
+      <c r="A3" s="2" t="n">
         <v>43122</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="1" t="n">
         <v>305</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1399,11 +1176,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1">
-      <c r="A4" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="4">
+      <c r="A4" s="2" t="n">
         <v>43122</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1413,11 +1190,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1">
-      <c r="A5" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="5">
+      <c r="A5" s="2" t="n">
         <v>43125</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="1" t="n">
         <v>98</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1427,11 +1204,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1">
-      <c r="A6" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="6">
+      <c r="A6" s="2" t="n">
         <v>43126</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1441,11 +1218,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1">
-      <c r="A7" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="7">
+      <c r="A7" s="2" t="n">
         <v>43127</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1455,11 +1232,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1">
-      <c r="A8" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="8">
+      <c r="A8" s="2" t="n">
         <v>43128</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="1" t="n">
         <v>656</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1469,11 +1246,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1">
-      <c r="A9" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="9">
+      <c r="A9" s="2" t="n">
         <v>43131</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="1" t="n">
         <v>486</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1483,11 +1260,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1">
-      <c r="A10" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="10">
+      <c r="A10" s="2" t="n">
         <v>43132</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="1" t="n">
         <v>76</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1497,11 +1274,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1">
-      <c r="A11" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="11">
+      <c r="A11" s="2" t="n">
         <v>43133</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="1" t="n">
         <v>399</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1511,11 +1288,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1">
-      <c r="A12" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="12">
+      <c r="A12" s="2" t="n">
         <v>43135</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="1" t="n">
         <v>419</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1525,11 +1302,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1">
-      <c r="A13" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="13">
+      <c r="A13" s="2" t="n">
         <v>43136</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="1" t="n">
         <v>521</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1539,11 +1316,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1">
-      <c r="A14" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="14">
+      <c r="A14" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="1" t="n">
         <v>399</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1553,11 +1330,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1">
-      <c r="A15" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="15">
+      <c r="A15" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="1" t="n">
         <v>138</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1567,11 +1344,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1">
-      <c r="A16" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="16">
+      <c r="A16" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="1" t="n">
         <v>310</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1581,12 +1358,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1">
-      <c r="A17" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="17">
+      <c r="A17" s="2" t="n">
         <v>43138</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="1">
+      <c r="C17" s="1" t="n">
         <v>700</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1596,12 +1373,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1">
-      <c r="A18" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="18">
+      <c r="A18" s="2" t="n">
         <v>43141</v>
       </c>
-      <c r="C18" s="1">
-        <f>F18*G18</f>
+      <c r="C18" s="1" t="n">
+        <f aca="false">F18*G18</f>
         <v>1312</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -1610,18 +1387,18 @@
       <c r="E18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="1" t="n">
         <v>164</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="1" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1">
-      <c r="A19" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="19">
+      <c r="A19" s="2" t="n">
         <v>43141</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="1" t="n">
         <v>1190</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1631,11 +1408,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1">
-      <c r="A20" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="20">
+      <c r="A20" s="2" t="n">
         <v>43154</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="1" t="n">
         <v>438</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1645,11 +1422,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1">
-      <c r="A21" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="21">
+      <c r="A21" s="2" t="n">
         <v>43154</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="1" t="n">
         <v>248</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -1659,22 +1436,22 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1">
-      <c r="A22" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="22">
+      <c r="A22" s="2" t="n">
         <v>43166</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="1" t="n">
         <v>234</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1">
-      <c r="A23" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="23">
+      <c r="A23" s="2" t="n">
         <v>43171</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="1" t="n">
         <v>118</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1684,22 +1461,22 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1">
-      <c r="A24" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="24">
+      <c r="A24" s="2" t="n">
         <v>43173</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="1" t="n">
         <v>82</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1">
-      <c r="A25" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="25">
+      <c r="A25" s="2" t="n">
         <v>43174</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1709,22 +1486,22 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1">
-      <c r="A26" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="26">
+      <c r="A26" s="2" t="n">
         <v>43175</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="1" t="n">
         <v>370</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:7" hidden="1">
-      <c r="A27" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="27">
+      <c r="A27" s="2" t="n">
         <v>43175</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -1734,11 +1511,11 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1">
-      <c r="A28" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="28">
+      <c r="A28" s="2" t="n">
         <v>43176</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="1" t="n">
         <v>624</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -1748,11 +1525,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1">
-      <c r="A29" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="29">
+      <c r="A29" s="2" t="n">
         <v>43177</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="1" t="n">
         <v>170</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1762,22 +1539,22 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1">
-      <c r="A30" s="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="30">
+      <c r="A30" s="4" t="n">
         <v>43179</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1">
-      <c r="A31" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="31">
+      <c r="A31" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="1" t="n">
         <v>90</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -1787,11 +1564,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1">
-      <c r="A32" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="32">
+      <c r="A32" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="1" t="n">
         <v>72</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -1801,11 +1578,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:26" hidden="1">
-      <c r="A33" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="33">
+      <c r="A33" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="1" t="n">
         <v>908</v>
       </c>
       <c r="D33" s="6" t="s">
@@ -1815,11 +1592,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:26" hidden="1">
-      <c r="A34" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="34">
+      <c r="A34" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -1829,11 +1606,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:26" hidden="1">
-      <c r="A35" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="35">
+      <c r="A35" s="2" t="n">
         <v>43181</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -1843,11 +1620,11 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:26" hidden="1">
-      <c r="A36" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="36">
+      <c r="A36" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="1" t="n">
         <v>135</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -1857,11 +1634,11 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:26" hidden="1">
-      <c r="A37" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="37">
+      <c r="A37" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="1" t="n">
         <v>110</v>
       </c>
       <c r="C37" s="1"/>
@@ -1893,11 +1670,11 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38" spans="1:26" hidden="1">
-      <c r="A38" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="38">
+      <c r="A38" s="2" t="n">
         <v>43185</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="1" t="n">
         <v>122</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -1907,22 +1684,22 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:26" hidden="1">
-      <c r="A39" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="39">
+      <c r="A39" s="2" t="n">
         <v>43187</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="1" t="n">
         <v>750</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:26" hidden="1">
-      <c r="A40" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="40">
+      <c r="A40" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="1" t="n">
         <v>379</v>
       </c>
       <c r="D40" s="6" t="s">
@@ -1932,22 +1709,22 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:26" hidden="1">
-      <c r="A41" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="41">
+      <c r="A41" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="1" t="n">
         <v>240</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:26" hidden="1">
-      <c r="A42" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="42">
+      <c r="A42" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="1" t="n">
         <v>540</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -1957,11 +1734,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:26" hidden="1">
-      <c r="A43" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="43">
+      <c r="A43" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -1971,11 +1748,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:26" hidden="1">
-      <c r="A44" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="44">
+      <c r="A44" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -1985,11 +1762,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:26" hidden="1">
-      <c r="A45" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="45">
+      <c r="A45" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="1" t="n">
         <v>462</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -1999,11 +1776,11 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:26" hidden="1">
-      <c r="A46" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="46">
+      <c r="A46" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46" s="1" t="n">
         <v>70</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -2013,11 +1790,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:26" hidden="1">
-      <c r="A47" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="47">
+      <c r="A47" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -2027,11 +1804,11 @@
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="1:26" hidden="1">
-      <c r="A48" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="48">
+      <c r="A48" s="2" t="n">
         <v>43190</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="1" t="n">
         <v>30</v>
       </c>
       <c r="C48" s="1"/>
@@ -2042,11 +1819,11 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1">
-      <c r="A49" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="49">
+      <c r="A49" s="2" t="n">
         <v>43191</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="1" t="n">
         <v>40</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -2056,11 +1833,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1">
-      <c r="A50" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="50">
+      <c r="A50" s="7" t="n">
         <v>43193</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50" s="1" t="n">
         <v>150</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -2070,11 +1847,11 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1">
-      <c r="A51" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="51">
+      <c r="A51" s="2" t="n">
         <v>43194</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51" s="1" t="n">
         <v>1360</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -2084,11 +1861,11 @@
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1">
-      <c r="A52" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="52">
+      <c r="A52" s="2" t="n">
         <v>43195</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" s="1" t="n">
         <v>94</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -2098,11 +1875,11 @@
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1">
-      <c r="A53" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="53">
+      <c r="A53" s="2" t="n">
         <v>43196</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C53" s="1" t="n">
         <v>48</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -2112,11 +1889,11 @@
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1">
-      <c r="A54" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="54">
+      <c r="A54" s="2" t="n">
         <v>43196</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C54" s="1" t="n">
         <v>205</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -2126,11 +1903,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1">
-      <c r="A55" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="55">
+      <c r="A55" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -2140,11 +1917,11 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1">
-      <c r="A56" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="56">
+      <c r="A56" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56" s="1" t="n">
         <v>421</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -2154,11 +1931,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1">
-      <c r="A57" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="57">
+      <c r="A57" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="1" t="n">
         <v>191</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -2168,11 +1945,11 @@
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1">
-      <c r="A58" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="58">
+      <c r="A58" s="2" t="n">
         <v>43198</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58" s="1" t="n">
         <v>226</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -2182,22 +1959,22 @@
         <v>96</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1">
-      <c r="A59" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="59">
+      <c r="A59" s="2" t="n">
         <v>43200</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59" s="1" t="n">
         <v>250</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1">
-      <c r="A60" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="60">
+      <c r="A60" s="2" t="n">
         <v>43200</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60" s="1" t="n">
         <v>1115</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -2207,11 +1984,11 @@
         <v>99</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1">
-      <c r="A61" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="61">
+      <c r="A61" s="2" t="n">
         <v>43201</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -2221,11 +1998,11 @@
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1">
-      <c r="A62" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="62">
+      <c r="A62" s="2" t="n">
         <v>43201</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62" s="1" t="n">
         <v>88</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -2235,11 +2012,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1">
-      <c r="A63" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="63">
+      <c r="A63" s="2" t="n">
         <v>43203</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -2249,11 +2026,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1">
-      <c r="A64" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="64">
+      <c r="A64" s="2" t="n">
         <v>43203</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C64" s="1" t="n">
         <v>364</v>
       </c>
       <c r="D64" s="1" t="s">
@@ -2263,11 +2040,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1">
-      <c r="A65" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="65">
+      <c r="A65" s="2" t="n">
         <v>43204</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65" s="1" t="n">
         <v>65</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -2277,11 +2054,11 @@
         <v>105</v>
       </c>
     </row>
-    <row r="66" spans="1:5" hidden="1">
-      <c r="A66" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="66">
+      <c r="A66" s="2" t="n">
         <v>43208</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -2291,11 +2068,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1">
-      <c r="A67" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="67">
+      <c r="A67" s="2" t="n">
         <v>43208</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C67" s="1" t="n">
         <v>470</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -2305,11 +2082,11 @@
         <v>107</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1">
-      <c r="A68" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="68">
+      <c r="A68" s="2" t="n">
         <v>43209</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68" s="1" t="n">
         <v>180</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -2319,11 +2096,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1">
-      <c r="A69" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="69">
+      <c r="A69" s="2" t="n">
         <v>43210</v>
       </c>
-      <c r="C69" s="1">
+      <c r="C69" s="1" t="n">
         <v>420</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -2333,11 +2110,11 @@
         <v>109</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1">
-      <c r="A70" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="70">
+      <c r="A70" s="2" t="n">
         <v>43212</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70" s="1" t="n">
         <v>50</v>
       </c>
       <c r="D70" s="1" t="s">
@@ -2347,11 +2124,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1">
-      <c r="A71" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="71">
+      <c r="A71" s="2" t="n">
         <v>43212</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71" s="1" t="n">
         <v>164</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -2361,11 +2138,11 @@
         <v>112</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1">
-      <c r="A72" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="72">
+      <c r="A72" s="2" t="n">
         <v>43215</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B72" s="1" t="n">
         <v>300</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -2375,11 +2152,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1">
-      <c r="A73" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="73">
+      <c r="A73" s="2" t="n">
         <v>43217</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73" s="1" t="n">
         <v>364</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -2389,11 +2166,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1">
-      <c r="A74" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="74">
+      <c r="A74" s="2" t="n">
         <v>43218</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74" s="1" t="n">
         <v>185</v>
       </c>
       <c r="D74" s="1" t="s">
@@ -2403,11 +2180,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1">
-      <c r="A75" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="75">
+      <c r="A75" s="2" t="n">
         <v>43218</v>
       </c>
-      <c r="C75" s="1">
+      <c r="C75" s="1" t="n">
         <v>404</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -2417,11 +2194,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="76" spans="1:5" hidden="1">
-      <c r="A76" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="76">
+      <c r="A76" s="2" t="n">
         <v>43220</v>
       </c>
-      <c r="C76" s="1">
+      <c r="C76" s="1" t="n">
         <v>57</v>
       </c>
       <c r="D76" s="1" t="s">
@@ -2431,11 +2208,11 @@
         <v>114</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1">
-      <c r="A77" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="77">
+      <c r="A77" s="2" t="n">
         <v>43221</v>
       </c>
-      <c r="C77" s="1">
+      <c r="C77" s="1" t="n">
         <v>282</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -2445,11 +2222,11 @@
         <v>116</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1">
-      <c r="A78" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="78">
+      <c r="A78" s="2" t="n">
         <v>43220</v>
       </c>
-      <c r="C78" s="1">
+      <c r="C78" s="1" t="n">
         <v>87</v>
       </c>
       <c r="D78" s="1" t="s">
@@ -2459,11 +2236,11 @@
         <v>117</v>
       </c>
     </row>
-    <row r="79" spans="1:5" hidden="1">
-      <c r="A79" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="79">
+      <c r="A79" s="2" t="n">
         <v>43223</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B79" s="1" t="n">
         <v>1878</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -2473,11 +2250,11 @@
         <v>119</v>
       </c>
     </row>
-    <row r="80" spans="1:5" hidden="1">
-      <c r="A80" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="80">
+      <c r="A80" s="2" t="n">
         <v>43224</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B80" s="1" t="n">
         <v>98</v>
       </c>
       <c r="D80" s="1" t="s">
@@ -2487,11 +2264,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="81" spans="1:5" hidden="1">
-      <c r="A81" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="81">
+      <c r="A81" s="2" t="n">
         <v>43225</v>
       </c>
-      <c r="C81" s="1">
+      <c r="C81" s="1" t="n">
         <v>198</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -2501,11 +2278,11 @@
         <v>122</v>
       </c>
     </row>
-    <row r="82" spans="1:5" hidden="1">
-      <c r="A82" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="82">
+      <c r="A82" s="2" t="n">
         <v>43225</v>
       </c>
-      <c r="C82" s="1">
+      <c r="C82" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -2515,11 +2292,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="83" spans="1:5" hidden="1">
-      <c r="A83" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="83">
+      <c r="A83" s="2" t="n">
         <v>43228</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83" s="1" t="n">
         <v>168</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -2529,11 +2306,11 @@
         <v>124</v>
       </c>
     </row>
-    <row r="84" spans="1:5" hidden="1">
-      <c r="A84" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="84">
+      <c r="A84" s="2" t="n">
         <v>43229</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B84" s="1" t="n">
         <v>240</v>
       </c>
       <c r="D84" s="1" t="s">
@@ -2543,12 +2320,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:5" hidden="1">
-      <c r="A85" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="85">
+      <c r="A85" s="2" t="n">
         <v>43230</v>
       </c>
       <c r="B85" s="1"/>
-      <c r="C85" s="1">
+      <c r="C85" s="1" t="n">
         <v>420</v>
       </c>
       <c r="D85" s="1" t="s">
@@ -2558,11 +2335,11 @@
         <v>126</v>
       </c>
     </row>
-    <row r="86" spans="1:5" hidden="1">
-      <c r="A86" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="86">
+      <c r="A86" s="2" t="n">
         <v>43230</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B86" s="1" t="n">
         <v>200</v>
       </c>
       <c r="C86" s="1"/>
@@ -2573,11 +2350,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="87" spans="1:5" hidden="1">
-      <c r="A87" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="87">
+      <c r="A87" s="2" t="n">
         <v>43230</v>
       </c>
-      <c r="C87" s="1">
+      <c r="C87" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D87" s="1" t="s">
@@ -2587,11 +2364,11 @@
         <v>128</v>
       </c>
     </row>
-    <row r="88" spans="1:5" hidden="1">
-      <c r="A88" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="88">
+      <c r="A88" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B88" s="1" t="n">
         <v>462</v>
       </c>
       <c r="D88" s="1" t="s">
@@ -2601,11 +2378,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="89" spans="1:5" hidden="1">
-      <c r="A89" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="89">
+      <c r="A89" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B89" s="1" t="n">
         <v>499</v>
       </c>
       <c r="D89" s="1" t="s">
@@ -2615,11 +2392,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="90" spans="1:5" hidden="1">
-      <c r="A90" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="90">
+      <c r="A90" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B90" s="1">
+      <c r="B90" s="1" t="n">
         <v>398</v>
       </c>
       <c r="D90" s="1" t="s">
@@ -2629,11 +2406,11 @@
         <v>133</v>
       </c>
     </row>
-    <row r="91" spans="1:5" hidden="1">
-      <c r="A91" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="91">
+      <c r="A91" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B91" s="1">
+      <c r="B91" s="1" t="n">
         <v>226</v>
       </c>
       <c r="D91" s="1" t="s">
@@ -2643,11 +2420,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="92" spans="1:5" hidden="1">
-      <c r="A92" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="92">
+      <c r="A92" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B92" s="1">
+      <c r="B92" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D92" s="1" t="s">
@@ -2657,11 +2434,11 @@
         <v>137</v>
       </c>
     </row>
-    <row r="93" spans="1:5" hidden="1">
-      <c r="A93" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="93">
+      <c r="A93" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="B93" s="1">
+      <c r="B93" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D93" s="1" t="s">
@@ -2671,11 +2448,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="94" spans="1:5" hidden="1">
-      <c r="A94" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="94">
+      <c r="A94" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="C94" s="1">
+      <c r="C94" s="1" t="n">
         <v>340</v>
       </c>
       <c r="D94" s="1" t="s">
@@ -2685,11 +2462,11 @@
         <v>139</v>
       </c>
     </row>
-    <row r="95" spans="1:5" hidden="1">
-      <c r="A95" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="95">
+      <c r="A95" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="B95" s="1">
+      <c r="B95" s="1" t="n">
         <v>510</v>
       </c>
       <c r="D95" s="1" t="s">
@@ -2699,11 +2476,11 @@
         <v>141</v>
       </c>
     </row>
-    <row r="96" spans="1:5" hidden="1">
-      <c r="A96" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="96">
+      <c r="A96" s="2" t="n">
         <v>43233</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B96" s="1" t="n">
         <v>170</v>
       </c>
       <c r="D96" s="1" t="s">
@@ -2713,11 +2490,11 @@
         <v>143</v>
       </c>
     </row>
-    <row r="97" spans="1:5" hidden="1">
-      <c r="A97" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="97">
+      <c r="A97" s="2" t="n">
         <v>43233</v>
       </c>
-      <c r="C97" s="1">
+      <c r="C97" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D97" s="1" t="s">
@@ -2727,11 +2504,11 @@
         <v>144</v>
       </c>
     </row>
-    <row r="98" spans="1:5" hidden="1">
-      <c r="A98" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="98">
+      <c r="A98" s="2" t="n">
         <v>43234</v>
       </c>
-      <c r="C98" s="1">
+      <c r="C98" s="1" t="n">
         <v>299</v>
       </c>
       <c r="D98" s="1" t="s">
@@ -2741,11 +2518,11 @@
         <v>145</v>
       </c>
     </row>
-    <row r="99" spans="1:5" hidden="1">
-      <c r="A99" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="99">
+      <c r="A99" s="2" t="n">
         <v>43236</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99" s="1" t="n">
         <v>3659</v>
       </c>
       <c r="D99" s="1" t="s">
@@ -2755,11 +2532,11 @@
         <v>146</v>
       </c>
     </row>
-    <row r="100" spans="1:5" hidden="1">
-      <c r="A100" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="100">
+      <c r="A100" s="2" t="n">
         <v>43237</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B100" s="1" t="n">
         <v>79</v>
       </c>
       <c r="D100" s="1" t="s">
@@ -2769,11 +2546,11 @@
         <v>147</v>
       </c>
     </row>
-    <row r="101" spans="1:5" hidden="1">
-      <c r="A101" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="101">
+      <c r="A101" s="2" t="n">
         <v>43236</v>
       </c>
-      <c r="C101" s="1">
+      <c r="C101" s="1" t="n">
         <v>173</v>
       </c>
       <c r="D101" s="1" t="s">
@@ -2783,11 +2560,11 @@
         <v>148</v>
       </c>
     </row>
-    <row r="102" spans="1:5" hidden="1">
-      <c r="A102" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="102">
+      <c r="A102" s="2" t="n">
         <v>43240</v>
       </c>
-      <c r="B102" s="1">
+      <c r="B102" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D102" s="1" t="s">
@@ -2797,22 +2574,22 @@
         <v>149</v>
       </c>
     </row>
-    <row r="103" spans="1:5" hidden="1">
-      <c r="A103" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="103">
+      <c r="A103" s="2" t="n">
         <v>43240</v>
       </c>
-      <c r="B103" s="1">
+      <c r="B103" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="104" spans="1:5" hidden="1">
-      <c r="A104" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="104">
+      <c r="A104" s="2" t="n">
         <v>43241</v>
       </c>
-      <c r="B104" s="1">
+      <c r="B104" s="1" t="n">
         <v>4070</v>
       </c>
       <c r="D104" s="1" t="s">
@@ -2822,11 +2599,11 @@
         <v>150</v>
       </c>
     </row>
-    <row r="105" spans="1:5" hidden="1">
-      <c r="A105" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="105">
+      <c r="A105" s="2" t="n">
         <v>43241</v>
       </c>
-      <c r="C105" s="1">
+      <c r="C105" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D105" s="1" t="s">
@@ -2836,11 +2613,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="106" spans="1:5" hidden="1">
-      <c r="A106" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="106">
+      <c r="A106" s="2" t="n">
         <v>43242</v>
       </c>
-      <c r="B106" s="1">
+      <c r="B106" s="1" t="n">
         <v>79</v>
       </c>
       <c r="D106" s="1" t="s">
@@ -2850,11 +2627,11 @@
         <v>152</v>
       </c>
     </row>
-    <row r="107" spans="1:5" hidden="1">
-      <c r="A107" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="107">
+      <c r="A107" s="2" t="n">
         <v>43246</v>
       </c>
-      <c r="B107" s="1">
+      <c r="B107" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D107" s="1" t="s">
@@ -2864,11 +2641,11 @@
         <v>154</v>
       </c>
     </row>
-    <row r="108" spans="1:5" hidden="1">
-      <c r="A108" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="108">
+      <c r="A108" s="2" t="n">
         <v>43247</v>
       </c>
-      <c r="B108" s="1">
+      <c r="B108" s="1" t="n">
         <v>70</v>
       </c>
       <c r="D108" s="1" t="s">
@@ -2878,44 +2655,44 @@
         <v>156</v>
       </c>
     </row>
-    <row r="109" spans="1:5" hidden="1">
-      <c r="A109" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="109">
+      <c r="A109" s="2" t="n">
         <v>43253</v>
       </c>
-      <c r="B109" s="1">
+      <c r="B109" s="1" t="n">
         <v>142</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="110" spans="1:5" hidden="1">
-      <c r="A110" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="110">
+      <c r="A110" s="2" t="n">
         <v>43254</v>
       </c>
-      <c r="B110" s="1">
+      <c r="B110" s="1" t="n">
         <v>90</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="111" spans="1:5" hidden="1">
-      <c r="A111" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="111">
+      <c r="A111" s="2" t="n">
         <v>43260</v>
       </c>
-      <c r="C111" s="1">
+      <c r="C111" s="1" t="n">
         <v>1400</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="112" spans="1:5" hidden="1">
-      <c r="A112" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="112">
+      <c r="A112" s="2" t="n">
         <v>43260</v>
       </c>
-      <c r="C112" s="1">
+      <c r="C112" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D112" s="1" t="s">
@@ -2925,33 +2702,33 @@
         <v>91</v>
       </c>
     </row>
-    <row r="113" spans="1:5" hidden="1">
-      <c r="A113" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="113">
+      <c r="A113" s="2" t="n">
         <v>43264</v>
       </c>
-      <c r="B113" s="1">
+      <c r="B113" s="1" t="n">
         <v>546</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="114" spans="1:5" hidden="1">
-      <c r="A114" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="114">
+      <c r="A114" s="2" t="n">
         <v>43264</v>
       </c>
-      <c r="B114" s="1">
+      <c r="B114" s="1" t="n">
         <v>95</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="115" spans="1:5" hidden="1">
-      <c r="A115" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="115">
+      <c r="A115" s="2" t="n">
         <v>43266</v>
       </c>
-      <c r="B115" s="1">
+      <c r="B115" s="1" t="n">
         <v>394</v>
       </c>
       <c r="D115" s="1" t="s">
@@ -2961,11 +2738,11 @@
         <v>163</v>
       </c>
     </row>
-    <row r="116" spans="1:5" hidden="1">
-      <c r="A116" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="116">
+      <c r="A116" s="2" t="n">
         <v>43266</v>
       </c>
-      <c r="B116" s="1">
+      <c r="B116" s="1" t="n">
         <v>1055</v>
       </c>
       <c r="D116" s="1" t="s">
@@ -2975,11 +2752,11 @@
         <v>165</v>
       </c>
     </row>
-    <row r="117" spans="1:5" hidden="1">
-      <c r="A117" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="117">
+      <c r="A117" s="2" t="n">
         <v>43284</v>
       </c>
-      <c r="C117" s="1">
+      <c r="C117" s="1" t="n">
         <v>274</v>
       </c>
       <c r="D117" s="1" t="s">
@@ -2989,11 +2766,11 @@
         <v>167</v>
       </c>
     </row>
-    <row r="118" spans="1:5" hidden="1">
-      <c r="A118" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="118">
+      <c r="A118" s="2" t="n">
         <v>43283</v>
       </c>
-      <c r="C118" s="1">
+      <c r="C118" s="1" t="n">
         <v>105</v>
       </c>
       <c r="D118" s="1" t="s">
@@ -3003,11 +2780,11 @@
         <v>169</v>
       </c>
     </row>
-    <row r="119" spans="1:5" hidden="1">
-      <c r="A119" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="119">
+      <c r="A119" s="2" t="n">
         <v>43289</v>
       </c>
-      <c r="C119" s="1">
+      <c r="C119" s="1" t="n">
         <v>128</v>
       </c>
       <c r="D119" s="1" t="s">
@@ -3017,11 +2794,11 @@
         <v>171</v>
       </c>
     </row>
-    <row r="120" spans="1:5" hidden="1">
-      <c r="A120" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="120">
+      <c r="A120" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C120" s="1">
+      <c r="C120" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D120" s="1" t="s">
@@ -3031,11 +2808,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="121" spans="1:5" hidden="1">
-      <c r="A121" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="121">
+      <c r="A121" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C121" s="1">
+      <c r="C121" s="1" t="n">
         <v>210</v>
       </c>
       <c r="D121" s="1" t="s">
@@ -3045,44 +2822,44 @@
         <v>173</v>
       </c>
     </row>
-    <row r="122" spans="1:5" hidden="1">
-      <c r="A122" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="122">
+      <c r="A122" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B122" s="1">
+      <c r="B122" s="1" t="n">
         <v>980</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="123" spans="1:5" hidden="1">
-      <c r="A123" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="123">
+      <c r="A123" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B123" s="1">
+      <c r="B123" s="1" t="n">
         <v>1260</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="124" spans="1:5" hidden="1">
-      <c r="A124" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="124">
+      <c r="A124" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B124" s="1">
+      <c r="B124" s="1" t="n">
         <v>3687</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="125" spans="1:5" hidden="1">
-      <c r="A125" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="125">
+      <c r="A125" s="2" t="n">
         <v>43298</v>
       </c>
-      <c r="C125" s="1">
+      <c r="C125" s="1" t="n">
         <v>60</v>
       </c>
       <c r="D125" s="1" t="s">
@@ -3092,55 +2869,55 @@
         <v>178</v>
       </c>
     </row>
-    <row r="126" spans="1:5" hidden="1">
-      <c r="A126" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="126">
+      <c r="A126" s="2" t="n">
         <v>43291</v>
       </c>
-      <c r="C126" s="1">
+      <c r="C126" s="1" t="n">
         <v>404</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="127" spans="1:5" hidden="1">
-      <c r="A127" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="127">
+      <c r="A127" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C127" s="1">
+      <c r="C127" s="1" t="n">
         <v>451</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="128" spans="1:5" hidden="1">
-      <c r="A128" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="128">
+      <c r="A128" s="2" t="n">
         <v>43298</v>
       </c>
-      <c r="C128" s="1">
+      <c r="C128" s="1" t="n">
         <v>708</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="129" spans="1:5" hidden="1">
-      <c r="A129" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="129">
+      <c r="A129" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C129" s="1">
+      <c r="C129" s="1" t="n">
         <v>160</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="130" spans="1:5" hidden="1">
-      <c r="A130" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="130">
+      <c r="A130" s="2" t="n">
         <v>43288</v>
       </c>
-      <c r="C130" s="1">
+      <c r="C130" s="1" t="n">
         <v>72</v>
       </c>
       <c r="D130" s="1" t="s">
@@ -3150,11 +2927,11 @@
         <v>181</v>
       </c>
     </row>
-    <row r="131" spans="1:5" hidden="1">
-      <c r="A131" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="131">
+      <c r="A131" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C131" s="1">
+      <c r="C131" s="1" t="n">
         <v>300</v>
       </c>
       <c r="D131" s="1" t="s">
@@ -3164,11 +2941,11 @@
         <v>183</v>
       </c>
     </row>
-    <row r="132" spans="1:5" hidden="1">
-      <c r="A132" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="132">
+      <c r="A132" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C132" s="1">
+      <c r="C132" s="1" t="n">
         <v>230</v>
       </c>
       <c r="D132" s="1" t="s">
@@ -3178,22 +2955,22 @@
         <v>185</v>
       </c>
     </row>
-    <row r="133" spans="1:5" hidden="1">
-      <c r="A133" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="133">
+      <c r="A133" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C133" s="1">
+      <c r="C133" s="1" t="n">
         <v>454</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="134" spans="1:5" hidden="1">
-      <c r="A134" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="134">
+      <c r="A134" s="2" t="n">
         <v>43299</v>
       </c>
-      <c r="C134" s="1">
+      <c r="C134" s="1" t="n">
         <v>686</v>
       </c>
       <c r="D134" s="1" t="s">
@@ -3203,11 +2980,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="135" spans="1:5" hidden="1">
-      <c r="A135" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="135">
+      <c r="A135" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C135" s="1">
+      <c r="C135" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D135" s="1" t="s">
@@ -3217,11 +2994,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="136" spans="1:5" hidden="1">
-      <c r="A136" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="136">
+      <c r="A136" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C136" s="1">
+      <c r="C136" s="1" t="n">
         <v>2067</v>
       </c>
       <c r="D136" s="1" t="s">
@@ -3231,11 +3008,11 @@
         <v>186</v>
       </c>
     </row>
-    <row r="137" spans="1:5" hidden="1">
-      <c r="A137" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="137">
+      <c r="A137" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B137" s="1">
+      <c r="B137" s="1" t="n">
         <v>109</v>
       </c>
       <c r="D137" s="1" t="s">
@@ -3245,11 +3022,11 @@
         <v>187</v>
       </c>
     </row>
-    <row r="138" spans="1:5" hidden="1">
-      <c r="A138" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="138">
+      <c r="A138" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B138" s="1">
+      <c r="B138" s="1" t="n">
         <v>97</v>
       </c>
       <c r="D138" s="1" t="s">
@@ -3259,11 +3036,11 @@
         <v>188</v>
       </c>
     </row>
-    <row r="139" spans="1:5" hidden="1">
-      <c r="A139" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="139">
+      <c r="A139" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B139" s="1">
+      <c r="B139" s="1" t="n">
         <v>1437</v>
       </c>
       <c r="D139" s="1" t="s">
@@ -3273,11 +3050,11 @@
         <v>189</v>
       </c>
     </row>
-    <row r="140" spans="1:5" hidden="1">
-      <c r="A140" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="140">
+      <c r="A140" s="2" t="n">
         <v>43306</v>
       </c>
-      <c r="C140" s="1">
+      <c r="C140" s="1" t="n">
         <v>650</v>
       </c>
       <c r="D140" s="1" t="s">
@@ -3287,11 +3064,11 @@
         <v>190</v>
       </c>
     </row>
-    <row r="141" spans="1:5" hidden="1">
-      <c r="A141" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="141">
+      <c r="A141" s="2" t="n">
         <v>43305</v>
       </c>
-      <c r="C141" s="1">
+      <c r="C141" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D141" s="1" t="s">
@@ -3301,11 +3078,11 @@
         <v>191</v>
       </c>
     </row>
-    <row r="142" spans="1:5" hidden="1">
-      <c r="A142" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="142">
+      <c r="A142" s="2" t="n">
         <v>43309</v>
       </c>
-      <c r="C142" s="1">
+      <c r="C142" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D142" s="1" t="s">
@@ -3315,11 +3092,11 @@
         <v>192</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="14" hidden="1">
-      <c r="A143" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="0" r="143">
+      <c r="A143" s="2" t="n">
         <v>43306</v>
       </c>
-      <c r="B143" s="1">
+      <c r="B143" s="1" t="n">
         <v>167</v>
       </c>
       <c r="D143" s="1" t="s">
@@ -3329,11 +3106,11 @@
         <v>193</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="14" hidden="1">
-      <c r="A144" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="0" r="144">
+      <c r="A144" s="2" t="n">
         <v>43304</v>
       </c>
-      <c r="C144" s="1">
+      <c r="C144" s="1" t="n">
         <v>93</v>
       </c>
       <c r="D144" s="1" t="s">
@@ -3343,11 +3120,11 @@
         <v>194</v>
       </c>
     </row>
-    <row r="145" spans="1:5" hidden="1">
-      <c r="A145" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="145">
+      <c r="A145" s="2" t="n">
         <v>43305</v>
       </c>
-      <c r="C145" s="1">
+      <c r="C145" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D145" s="1" t="s">
@@ -3357,11 +3134,11 @@
         <v>195</v>
       </c>
     </row>
-    <row r="146" spans="1:5" hidden="1">
-      <c r="A146" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="146">
+      <c r="A146" s="2" t="n">
         <v>43303</v>
       </c>
-      <c r="C146" s="1">
+      <c r="C146" s="1" t="n">
         <v>244</v>
       </c>
       <c r="D146" s="1" t="s">
@@ -3371,11 +3148,11 @@
         <v>196</v>
       </c>
     </row>
-    <row r="147" spans="1:5" hidden="1">
-      <c r="A147" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="147">
+      <c r="A147" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C147" s="1">
+      <c r="C147" s="1" t="n">
         <v>482</v>
       </c>
       <c r="D147" s="1" t="s">
@@ -3385,11 +3162,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="148" spans="1:5" hidden="1">
-      <c r="A148" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="148">
+      <c r="A148" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C148" s="1">
+      <c r="C148" s="1" t="n">
         <v>172</v>
       </c>
       <c r="D148" s="1" t="s">
@@ -3399,44 +3176,44 @@
         <v>199</v>
       </c>
     </row>
-    <row r="149" spans="1:5" hidden="1">
-      <c r="A149" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="149">
+      <c r="A149" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="B149" s="1">
+      <c r="B149" s="1" t="n">
         <v>89</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="150" spans="1:5" hidden="1">
-      <c r="A150" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="150">
+      <c r="A150" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="C150" s="1">
+      <c r="C150" s="1" t="n">
         <v>107</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="151" spans="1:5" hidden="1">
-      <c r="A151" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="151">
+      <c r="A151" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="C151" s="1">
+      <c r="C151" s="1" t="n">
         <v>124</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="152" spans="1:5" hidden="1">
-      <c r="A152" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="152">
+      <c r="A152" s="7" t="n">
         <v>43316</v>
       </c>
-      <c r="C152" s="1">
+      <c r="C152" s="1" t="n">
         <v>4500</v>
       </c>
       <c r="D152" s="1" t="s">
@@ -3446,11 +3223,11 @@
         <v>202</v>
       </c>
     </row>
-    <row r="153" spans="1:5" hidden="1">
-      <c r="A153" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="153">
+      <c r="A153" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C153" s="1">
+      <c r="C153" s="1" t="n">
         <v>247</v>
       </c>
       <c r="D153" s="1" t="s">
@@ -3460,11 +3237,11 @@
         <v>204</v>
       </c>
     </row>
-    <row r="154" spans="1:5" hidden="1">
-      <c r="A154" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="154">
+      <c r="A154" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C154" s="1">
+      <c r="C154" s="1" t="n">
         <v>1150</v>
       </c>
       <c r="D154" s="1" t="s">
@@ -3474,11 +3251,11 @@
         <v>205</v>
       </c>
     </row>
-    <row r="155" spans="1:5" hidden="1">
-      <c r="A155" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="155">
+      <c r="A155" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C155" s="1">
+      <c r="C155" s="1" t="n">
         <v>313</v>
       </c>
       <c r="D155" s="1" t="s">
@@ -3488,11 +3265,11 @@
         <v>207</v>
       </c>
     </row>
-    <row r="156" spans="1:5" hidden="1">
-      <c r="A156" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="156">
+      <c r="A156" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="B156" s="1">
+      <c r="B156" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D156" s="1" t="s">
@@ -3502,11 +3279,11 @@
         <v>209</v>
       </c>
     </row>
-    <row r="157" spans="1:5" hidden="1">
-      <c r="A157" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="157">
+      <c r="A157" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="C157" s="1">
+      <c r="C157" s="1" t="n">
         <v>710</v>
       </c>
       <c r="D157" s="1" t="s">
@@ -3516,11 +3293,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="158" spans="1:5">
-      <c r="A158" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="158">
+      <c r="A158" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="C158" s="1">
+      <c r="C158" s="1" t="n">
         <v>100</v>
       </c>
       <c r="D158" s="1" t="s">
@@ -3530,11 +3307,11 @@
         <v>212</v>
       </c>
     </row>
-    <row r="159" spans="1:5">
-      <c r="A159" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="159">
+      <c r="A159" s="2" t="n">
         <v>43319</v>
       </c>
-      <c r="B159" s="1">
+      <c r="B159" s="1" t="n">
         <v>78</v>
       </c>
       <c r="D159" s="1" t="s">
@@ -3544,22 +3321,22 @@
         <v>213</v>
       </c>
     </row>
-    <row r="160" spans="1:5">
-      <c r="A160" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="160">
+      <c r="A160" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="B160" s="1">
+      <c r="B160" s="1" t="n">
         <v>1840</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="161" spans="1:5">
-      <c r="A161" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="161">
+      <c r="A161" s="2" t="n">
         <v>43322</v>
       </c>
-      <c r="B161" s="1">
+      <c r="B161" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D161" s="1" t="s">
@@ -3569,11 +3346,11 @@
         <v>216</v>
       </c>
     </row>
-    <row r="162" spans="1:5">
-      <c r="A162" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="162">
+      <c r="A162" s="7" t="n">
         <v>43324</v>
       </c>
-      <c r="C162" s="1">
+      <c r="C162" s="1" t="n">
         <v>230</v>
       </c>
       <c r="D162" s="1" t="s">
@@ -3583,11 +3360,11 @@
         <v>217</v>
       </c>
     </row>
-    <row r="163" spans="1:5">
-      <c r="A163" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="163">
+      <c r="A163" s="7" t="n">
         <v>43326</v>
       </c>
-      <c r="C163" s="1">
+      <c r="C163" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D163" s="1" t="s">
@@ -3597,11 +3374,11 @@
         <v>219</v>
       </c>
     </row>
-    <row r="164" spans="1:5">
-      <c r="A164" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="164">
+      <c r="A164" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="B164" s="1">
+      <c r="B164" s="1" t="n">
         <v>45</v>
       </c>
       <c r="D164" s="1" t="s">
@@ -3611,685 +3388,718 @@
         <v>221</v>
       </c>
     </row>
-    <row r="165" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A165" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="165">
+      <c r="A165" s="10" t="n">
         <v>43327</v>
       </c>
-      <c r="C165">
+      <c r="C165" s="0" t="n">
         <v>486</v>
       </c>
-      <c r="D165" t="s">
+      <c r="D165" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E165" t="s">
+      <c r="E165" s="0" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="166" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A166" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="166">
+      <c r="A166" s="10" t="n">
         <v>43329</v>
       </c>
-      <c r="C166">
+      <c r="C166" s="0" t="n">
         <v>92</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D166" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="E166" t="s">
+      <c r="E166" s="0" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="167" spans="1:5">
-      <c r="A167" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="167">
+      <c r="A167" s="10" t="n">
         <v>43331</v>
       </c>
-      <c r="C167">
+      <c r="C167" s="0" t="n">
         <v>310</v>
       </c>
-      <c r="D167" t="s">
+      <c r="D167" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="E167" t="s">
+      <c r="E167" s="0" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="168" spans="1:5">
-      <c r="A168" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="168">
+      <c r="A168" s="10" t="n">
         <v>43334</v>
       </c>
-      <c r="C168">
+      <c r="C168" s="0" t="n">
         <v>464</v>
       </c>
-      <c r="D168" t="s">
+      <c r="D168" s="0" t="s">
         <v>218</v>
       </c>
       <c r="E168" s="11" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="169" spans="1:5">
-      <c r="A169" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="169">
+      <c r="A169" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="C169">
+      <c r="C169" s="0" t="n">
         <v>726</v>
       </c>
-      <c r="D169" t="s">
+      <c r="D169" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="E169" t="s">
+      <c r="E169" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="170" spans="1:5">
-      <c r="A170" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="170">
+      <c r="A170" s="10" t="n">
         <v>43337</v>
       </c>
-      <c r="C170">
+      <c r="C170" s="0" t="n">
         <v>544</v>
       </c>
-      <c r="D170" t="s">
+      <c r="D170" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E170" t="s">
+      <c r="E170" s="0" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="171" spans="1:5">
-      <c r="A171" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="171">
+      <c r="A171" s="10" t="n">
         <v>43337</v>
       </c>
-      <c r="B171">
+      <c r="B171" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D171" t="s">
+      <c r="D171" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="E171" t="s">
+      <c r="E171" s="0" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="172" spans="1:5">
-      <c r="A172" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="172">
+      <c r="A172" s="10" t="n">
         <v>43341</v>
       </c>
-      <c r="C172">
+      <c r="C172" s="0" t="n">
         <v>830</v>
       </c>
-      <c r="D172" t="s">
+      <c r="D172" s="0" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="173" spans="1:5">
-      <c r="A173" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="173">
+      <c r="A173" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="C173">
+      <c r="C173" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="D173" t="s">
+      <c r="D173" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="E173" t="s">
+      <c r="E173" s="0" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="174" spans="1:5">
-      <c r="A174" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="174">
+      <c r="A174" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="B174">
+      <c r="B174" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D174" t="s">
+      <c r="D174" s="0" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="175" spans="1:5">
-      <c r="A175" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="175">
+      <c r="A175" s="10" t="n">
         <v>43344</v>
       </c>
-      <c r="B175">
+      <c r="B175" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="D175" t="s">
+      <c r="D175" s="0" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="176" spans="1:5">
-      <c r="A176" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="176">
+      <c r="A176" s="10" t="n">
         <v>43344</v>
       </c>
-      <c r="B176">
+      <c r="B176" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D176" t="s">
+      <c r="D176" s="0" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="177" spans="1:5">
-      <c r="A177" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="177">
+      <c r="A177" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C177">
+      <c r="C177" s="0" t="n">
         <v>607</v>
       </c>
-      <c r="D177" t="s">
+      <c r="D177" s="0" t="s">
         <v>235</v>
       </c>
-      <c r="E177" t="s">
+      <c r="E177" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="178" spans="1:5">
-      <c r="A178" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="178">
+      <c r="A178" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C178">
+      <c r="C178" s="0" t="n">
         <v>444</v>
       </c>
-      <c r="D178" t="s">
+      <c r="D178" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E178" t="s">
+      <c r="E178" s="0" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="179" spans="1:5">
-      <c r="A179" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="179">
+      <c r="A179" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C179">
+      <c r="C179" s="0" t="n">
         <v>312</v>
       </c>
-      <c r="D179" t="s">
+      <c r="D179" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="E179" t="s">
+      <c r="E179" s="0" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="180" spans="1:5">
-      <c r="A180" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="180">
+      <c r="A180" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C180">
+      <c r="C180" s="0" t="n">
         <v>501</v>
       </c>
-      <c r="D180" t="s">
+      <c r="D180" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E180" t="s">
+      <c r="E180" s="0" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="181" spans="1:5">
-      <c r="A181" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="181">
+      <c r="A181" s="10" t="n">
         <v>43349</v>
       </c>
-      <c r="C181">
+      <c r="C181" s="0" t="n">
         <v>711</v>
       </c>
-      <c r="D181" t="s">
+      <c r="D181" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="E181" t="s">
+      <c r="E181" s="0" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="182" spans="1:5">
-      <c r="A182" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="182">
+      <c r="A182" s="10" t="n">
         <v>43354</v>
       </c>
-      <c r="B182">
+      <c r="B182" s="0" t="n">
         <v>126</v>
       </c>
-      <c r="D182" t="s">
+      <c r="D182" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="E182" t="s">
+      <c r="E182" s="0" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="183" spans="1:5">
-      <c r="A183" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="183">
+      <c r="A183" s="10" t="n">
         <v>43354</v>
       </c>
-      <c r="C183">
+      <c r="C183" s="0" t="n">
         <v>450</v>
       </c>
-      <c r="D183" t="s">
+      <c r="D183" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="E183" t="s">
+      <c r="E183" s="0" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="184" spans="1:5">
-      <c r="A184" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="184">
+      <c r="A184" s="10" t="n">
         <v>43361</v>
       </c>
-      <c r="C184">
+      <c r="C184" s="0" t="n">
         <v>660</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D184" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="E184" t="s">
+      <c r="E184" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="185" spans="1:5">
-      <c r="A185" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="185">
+      <c r="A185" s="10" t="n">
         <v>43363</v>
       </c>
-      <c r="C185">
+      <c r="C185" s="0" t="n">
         <v>230</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D185" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="E185" t="s">
+      <c r="E185" s="0" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="186" spans="1:5">
-      <c r="A186" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="186">
+      <c r="A186" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B186">
+      <c r="B186" s="0" t="n">
         <v>4859</v>
       </c>
-      <c r="D186" t="s">
+      <c r="D186" s="0" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="187" spans="1:5">
-      <c r="A187" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="187">
+      <c r="A187" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B187">
+      <c r="B187" s="0" t="n">
         <v>295</v>
       </c>
-      <c r="D187" t="s">
+      <c r="D187" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="E187" t="s">
+      <c r="E187" s="0" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="188" spans="1:5">
-      <c r="A188" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="188">
+      <c r="A188" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B188">
+      <c r="B188" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D188" t="s">
+      <c r="D188" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="E188" t="s">
+      <c r="E188" s="0" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="189" spans="1:5">
-      <c r="A189" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="189">
+      <c r="A189" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B189">
+      <c r="B189" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="D189" t="s">
+      <c r="D189" s="0" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="190" spans="1:5">
-      <c r="A190" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="190">
+      <c r="A190" s="10" t="n">
         <v>43378</v>
       </c>
-      <c r="B190">
+      <c r="B190" s="0" t="n">
         <v>506</v>
       </c>
-      <c r="D190" t="s">
+      <c r="D190" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="E190" t="s">
+      <c r="E190" s="0" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="191" spans="1:5">
-      <c r="A191" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="191">
+      <c r="A191" s="10" t="n">
         <v>43379</v>
       </c>
-      <c r="B191">
+      <c r="B191" s="0" t="n">
         <v>350</v>
       </c>
-      <c r="D191" t="s">
+      <c r="D191" s="0" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="192" spans="1:5">
-      <c r="A192" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="192">
+      <c r="A192" s="10" t="n">
         <v>43383</v>
       </c>
-      <c r="B192">
+      <c r="B192" s="0" t="n">
         <v>189</v>
       </c>
-      <c r="D192" t="s">
+      <c r="D192" s="0" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="193" spans="1:5">
-      <c r="A193" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="193">
+      <c r="A193" s="10" t="n">
         <v>43387</v>
       </c>
-      <c r="B193">
+      <c r="B193" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="D193" t="s">
+      <c r="D193" s="0" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="194" spans="1:5">
-      <c r="A194" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="194">
+      <c r="A194" s="10" t="n">
         <v>43387</v>
       </c>
-      <c r="B194">
+      <c r="B194" s="0" t="n">
         <v>307</v>
       </c>
-      <c r="D194" t="s">
+      <c r="D194" s="0" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="195" spans="1:5">
-      <c r="C195">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="195">
+      <c r="C195" s="0" t="n">
         <v>3705</v>
       </c>
-      <c r="E195" t="s">
+      <c r="E195" s="0" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="196" spans="1:5">
-      <c r="A196" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="196">
+      <c r="A196" s="10" t="n">
         <v>43385</v>
       </c>
-      <c r="C196">
+      <c r="C196" s="0" t="n">
         <v>608</v>
       </c>
-      <c r="D196" t="s">
+      <c r="D196" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E196" t="s">
+      <c r="E196" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="197" spans="1:5">
-      <c r="A197" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="197">
+      <c r="A197" s="10" t="n">
         <v>43391</v>
       </c>
-      <c r="B197">
+      <c r="B197" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="D197" t="s">
+      <c r="D197" s="0" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="198" spans="1:5">
-      <c r="A198" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="198">
+      <c r="A198" s="10" t="n">
         <v>43392</v>
       </c>
-      <c r="B198">
+      <c r="B198" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="D198" t="s">
+      <c r="D198" s="0" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="199" spans="1:5">
-      <c r="A199" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="199">
+      <c r="A199" s="10" t="n">
         <v>43393</v>
       </c>
-      <c r="B199">
+      <c r="B199" s="0" t="n">
         <v>177</v>
       </c>
-      <c r="D199" t="s">
+      <c r="D199" s="0" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="200" spans="1:5">
-      <c r="A200" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="200">
+      <c r="A200" s="10" t="n">
         <v>43393</v>
       </c>
-      <c r="C200">
+      <c r="C200" s="0" t="n">
         <v>125</v>
       </c>
-      <c r="D200" t="s">
+      <c r="D200" s="0" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="201" spans="1:5">
-      <c r="A201" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="201">
+      <c r="A201" s="10" t="n">
         <v>43395</v>
       </c>
-      <c r="B201">
+      <c r="B201" s="0" t="n">
         <v>2800</v>
       </c>
       <c r="D201" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="E201" t="s">
+      <c r="E201" s="0" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="202" spans="1:5">
-      <c r="A202" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="202">
+      <c r="A202" s="10" t="n">
         <v>43395</v>
       </c>
-      <c r="C202">
+      <c r="C202" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="D202" t="s">
+      <c r="D202" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="E202" t="s">
+      <c r="E202" s="0" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="203" spans="1:5">
-      <c r="A203" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="203">
+      <c r="A203" s="10" t="n">
         <v>43396</v>
       </c>
-      <c r="C203">
+      <c r="C203" s="0" t="n">
         <v>692</v>
       </c>
-      <c r="D203" t="s">
+      <c r="D203" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E203" t="s">
+      <c r="E203" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="204" spans="1:5">
-      <c r="A204" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="204">
+      <c r="A204" s="10" t="n">
         <v>43397</v>
       </c>
-      <c r="C204">
+      <c r="C204" s="0" t="n">
         <v>4935</v>
       </c>
-      <c r="D204" t="s">
+      <c r="D204" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="E204" t="s">
+      <c r="E204" s="0" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="205" spans="1:5">
-      <c r="A205" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="205">
+      <c r="A205" s="10" t="n">
         <v>43398</v>
       </c>
-      <c r="B205">
+      <c r="B205" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="D205" t="s">
+      <c r="D205" s="0" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="206" spans="1:5">
-      <c r="A206" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="206">
+      <c r="A206" s="10" t="n">
         <v>43398</v>
       </c>
-      <c r="B206">
+      <c r="B206" s="0" t="n">
         <v>370</v>
       </c>
-      <c r="D206" t="s">
+      <c r="D206" s="0" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="207" spans="1:5">
-      <c r="A207" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="207">
+      <c r="A207" s="10" t="n">
         <v>43398</v>
       </c>
-      <c r="B207">
+      <c r="B207" s="0" t="n">
         <v>4966</v>
       </c>
-      <c r="D207" t="s">
+      <c r="D207" s="0" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="208" spans="1:5">
-      <c r="A208" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="208">
+      <c r="A208" s="10" t="n">
         <v>43397</v>
       </c>
-      <c r="C208">
+      <c r="C208" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="D208" t="s">
+      <c r="D208" s="0" t="s">
         <v>265</v>
       </c>
-      <c r="E208" t="s">
+      <c r="E208" s="0" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="209" spans="1:5">
-      <c r="A209" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="209">
+      <c r="A209" s="10" t="n">
         <v>43399</v>
       </c>
-      <c r="B209">
+      <c r="B209" s="0" t="n">
         <v>182</v>
       </c>
-      <c r="D209" t="s">
+      <c r="D209" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="E209" t="s">
+      <c r="E209" s="0" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="210" spans="1:5">
-      <c r="A210" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="210">
+      <c r="A210" s="10" t="n">
         <v>43401</v>
       </c>
-      <c r="B210">
+      <c r="B210" s="0" t="n">
         <v>700</v>
       </c>
-      <c r="D210" t="s">
+      <c r="D210" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="E210" t="s">
+      <c r="E210" s="0" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="211" spans="1:5">
-      <c r="A211" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="211">
+      <c r="A211" s="10" t="n">
         <v>43405</v>
       </c>
-      <c r="B211">
+      <c r="B211" s="0" t="n">
         <v>274</v>
       </c>
-      <c r="D211" t="s">
+      <c r="D211" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="E211" t="s">
+      <c r="E211" s="0" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="212" spans="1:5">
-      <c r="A212" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="212">
+      <c r="A212" s="10" t="n">
         <v>43405</v>
       </c>
-      <c r="C212">
+      <c r="C212" s="0" t="n">
         <v>590</v>
       </c>
-      <c r="D212" t="s">
+      <c r="D212" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="E212" t="s">
+      <c r="E212" s="0" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="213" spans="1:5" ht="14">
-      <c r="A213" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="213">
+      <c r="A213" s="10" t="n">
         <v>43407</v>
       </c>
-      <c r="C213">
+      <c r="C213" s="0" t="n">
         <v>1275</v>
       </c>
       <c r="D213" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="E213" t="s">
+      <c r="E213" s="0" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="214" spans="1:5" ht="14">
-      <c r="A214" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="214">
+      <c r="A214" s="10" t="n">
         <v>43407</v>
       </c>
-      <c r="C214">
+      <c r="C214" s="0" t="n">
         <v>4781</v>
       </c>
       <c r="D214" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="E214" t="s">
+      <c r="E214" s="0" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="215" spans="1:5" ht="14">
-      <c r="A215" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="215">
+      <c r="A215" s="10" t="n">
         <v>43407</v>
       </c>
-      <c r="C215">
+      <c r="C215" s="0" t="n">
         <v>4781</v>
       </c>
       <c r="D215" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="E215" t="s">
+      <c r="E215" s="0" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="220" spans="1:5">
-      <c r="B220">
-        <f>SUM(B2:B219)</f>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="216">
+      <c r="A216" s="10" t="n">
+        <v>43406</v>
+      </c>
+      <c r="C216" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D216" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="E216" s="0" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="217">
+      <c r="A217" s="10" t="n">
+        <v>43409</v>
+      </c>
+      <c r="C217" s="0" t="n">
+        <v>677</v>
+      </c>
+      <c r="D217" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="E217" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="220">
+      <c r="B220" s="0" t="n">
+        <f aca="false">SUM(B2:B219)</f>
         <v>55912</v>
       </c>
-      <c r="C220">
-        <f>SUM(C2:C219)</f>
-        <v>63928</v>
+      <c r="C220" s="0" t="n">
+        <f aca="false">SUM(C2:C219)</f>
+        <v>64655</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A30:Z32">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule aboveAverage="0" bottom="0" dxfId="0" operator="expression" percent="0" priority="2" rank="0" text="" type="expression">
       <formula>LEN(TRIM(A30))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D33" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D40" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D201" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink display="netonnet.se" ref="D33" r:id="rId1"/>
+    <hyperlink display="www.vidaxl.se" ref="D40" r:id="rId2"/>
+    <hyperlink display="https://www.vardia.se/" ref="D201" r:id="rId3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cost update 1109 Jenny
</commit_message>
<xml_diff>
--- a/Cost.xlsx
+++ b/Cost.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chengkaiyan/github/cost/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C8F268-222F-4B48-A5C9-FCDE337A1EDE}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21020" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="280">
   <si>
     <t>日期</t>
   </si>
@@ -857,61 +852,80 @@
   </si>
   <si>
     <t>Danderyd Sjukhus curs</t>
+  </si>
+  <si>
+    <t>milk;fruits;donuts,etc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="yyyy/m/d"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt formatCode="YYYY/M/D" numFmtId="165"/>
+    <numFmt formatCode="M/D/YYYY" numFmtId="166"/>
+    <numFmt formatCode="YYYY\-MM\-DD" numFmtId="167"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="10">
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <family val="0"/>
       <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
       <name val="Arial"/>
       <family val="2"/>
+      <sz val="10"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF666666"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF666666"/>
+      <sz val="11"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0563C1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF0563C1"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0563C1"/>
       <name val="FreeSans"/>
       <family val="2"/>
+      <color rgb="FF0563C1"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF444444"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF444444"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="5">
@@ -941,7 +955,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
@@ -949,31 +963,100 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+  <cellStyleXfs count="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="167" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="20">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="7">
+    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle builtinId="8" customBuiltin="false" name="*unknown*" xfId="20"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -984,7 +1067,6 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1043,339 +1125,31 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF444444"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:Z241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A197" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D221" sqref="D221"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A212" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E222" activeCellId="0" pane="topLeft" sqref="E222"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="3" width="14.5"/>
-    <col min="4" max="4" width="26"/>
-    <col min="5" max="5" width="37.83203125"/>
-    <col min="6" max="1025" width="14.5"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="14.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1392,11 +1166,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1">
-      <c r="A2" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="2">
+      <c r="A2" s="2" t="n">
         <v>43121</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="1" t="n">
         <v>250</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1406,11 +1180,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1">
-      <c r="A3" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="3">
+      <c r="A3" s="2" t="n">
         <v>43122</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="1" t="n">
         <v>305</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1420,11 +1194,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1">
-      <c r="A4" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="4">
+      <c r="A4" s="2" t="n">
         <v>43122</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1434,11 +1208,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1">
-      <c r="A5" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="5">
+      <c r="A5" s="2" t="n">
         <v>43125</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="1" t="n">
         <v>98</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1448,11 +1222,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1">
-      <c r="A6" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="6">
+      <c r="A6" s="2" t="n">
         <v>43126</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1462,11 +1236,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1">
-      <c r="A7" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="7">
+      <c r="A7" s="2" t="n">
         <v>43127</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1476,11 +1250,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1">
-      <c r="A8" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="8">
+      <c r="A8" s="2" t="n">
         <v>43128</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="1" t="n">
         <v>656</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1490,11 +1264,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1">
-      <c r="A9" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="9">
+      <c r="A9" s="2" t="n">
         <v>43131</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="1" t="n">
         <v>486</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1504,11 +1278,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1">
-      <c r="A10" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="10">
+      <c r="A10" s="2" t="n">
         <v>43132</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="1" t="n">
         <v>76</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1518,11 +1292,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1">
-      <c r="A11" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="11">
+      <c r="A11" s="2" t="n">
         <v>43133</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="1" t="n">
         <v>399</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1532,11 +1306,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1">
-      <c r="A12" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="12">
+      <c r="A12" s="2" t="n">
         <v>43135</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="1" t="n">
         <v>419</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1546,11 +1320,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1">
-      <c r="A13" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="13">
+      <c r="A13" s="2" t="n">
         <v>43136</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="1" t="n">
         <v>521</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1560,11 +1334,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1">
-      <c r="A14" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="14">
+      <c r="A14" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="1" t="n">
         <v>399</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1574,11 +1348,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1">
-      <c r="A15" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="15">
+      <c r="A15" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="1" t="n">
         <v>138</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1588,11 +1362,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1">
-      <c r="A16" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="16">
+      <c r="A16" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="1" t="n">
         <v>310</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1602,12 +1376,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1">
-      <c r="A17" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="17">
+      <c r="A17" s="2" t="n">
         <v>43138</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="1">
+      <c r="C17" s="1" t="n">
         <v>700</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1617,12 +1391,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1">
-      <c r="A18" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="18">
+      <c r="A18" s="2" t="n">
         <v>43141</v>
       </c>
-      <c r="C18" s="1">
-        <f>F18*G18</f>
+      <c r="C18" s="1" t="n">
+        <f aca="false">F18*G18</f>
         <v>1312</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -1631,18 +1405,18 @@
       <c r="E18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="1" t="n">
         <v>164</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="1" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1">
-      <c r="A19" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="19">
+      <c r="A19" s="2" t="n">
         <v>43141</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="1" t="n">
         <v>1190</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1652,11 +1426,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1">
-      <c r="A20" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="20">
+      <c r="A20" s="2" t="n">
         <v>43154</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="1" t="n">
         <v>438</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1666,11 +1440,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1">
-      <c r="A21" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="21">
+      <c r="A21" s="2" t="n">
         <v>43154</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="1" t="n">
         <v>248</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -1680,22 +1454,22 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1">
-      <c r="A22" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="22">
+      <c r="A22" s="2" t="n">
         <v>43166</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="1" t="n">
         <v>234</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1">
-      <c r="A23" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="23">
+      <c r="A23" s="2" t="n">
         <v>43171</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="1" t="n">
         <v>118</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1705,22 +1479,22 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1">
-      <c r="A24" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="24">
+      <c r="A24" s="2" t="n">
         <v>43173</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="1" t="n">
         <v>82</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1">
-      <c r="A25" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="25">
+      <c r="A25" s="2" t="n">
         <v>43174</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1730,22 +1504,22 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1">
-      <c r="A26" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="26">
+      <c r="A26" s="2" t="n">
         <v>43175</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="1" t="n">
         <v>370</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:7" hidden="1">
-      <c r="A27" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="27">
+      <c r="A27" s="2" t="n">
         <v>43175</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -1755,11 +1529,11 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1">
-      <c r="A28" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="28">
+      <c r="A28" s="2" t="n">
         <v>43176</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="1" t="n">
         <v>624</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -1769,11 +1543,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1">
-      <c r="A29" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="29">
+      <c r="A29" s="2" t="n">
         <v>43177</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="1" t="n">
         <v>170</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1783,22 +1557,22 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1">
-      <c r="A30" s="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="30">
+      <c r="A30" s="4" t="n">
         <v>43179</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1">
-      <c r="A31" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="31">
+      <c r="A31" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="1" t="n">
         <v>90</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -1808,11 +1582,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1">
-      <c r="A32" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="32">
+      <c r="A32" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="1" t="n">
         <v>72</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -1822,11 +1596,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:26" hidden="1">
-      <c r="A33" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="33">
+      <c r="A33" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="1" t="n">
         <v>908</v>
       </c>
       <c r="D33" s="6" t="s">
@@ -1836,11 +1610,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:26" hidden="1">
-      <c r="A34" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="34">
+      <c r="A34" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -1850,11 +1624,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:26" hidden="1">
-      <c r="A35" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="35">
+      <c r="A35" s="2" t="n">
         <v>43181</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -1864,11 +1638,11 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:26" hidden="1">
-      <c r="A36" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="36">
+      <c r="A36" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="1" t="n">
         <v>135</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -1878,11 +1652,11 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:26" hidden="1">
-      <c r="A37" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="37">
+      <c r="A37" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="1" t="n">
         <v>110</v>
       </c>
       <c r="C37" s="1"/>
@@ -1914,11 +1688,11 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38" spans="1:26" hidden="1">
-      <c r="A38" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="38">
+      <c r="A38" s="2" t="n">
         <v>43185</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="1" t="n">
         <v>122</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -1928,22 +1702,22 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:26" hidden="1">
-      <c r="A39" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="39">
+      <c r="A39" s="2" t="n">
         <v>43187</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="1" t="n">
         <v>750</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:26" hidden="1">
-      <c r="A40" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="40">
+      <c r="A40" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="1" t="n">
         <v>379</v>
       </c>
       <c r="D40" s="6" t="s">
@@ -1953,22 +1727,22 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:26" hidden="1">
-      <c r="A41" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="41">
+      <c r="A41" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="1" t="n">
         <v>240</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:26" hidden="1">
-      <c r="A42" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="42">
+      <c r="A42" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="1" t="n">
         <v>540</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -1978,11 +1752,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:26" hidden="1">
-      <c r="A43" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="43">
+      <c r="A43" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -1992,11 +1766,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:26" hidden="1">
-      <c r="A44" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="44">
+      <c r="A44" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -2006,11 +1780,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:26" hidden="1">
-      <c r="A45" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="45">
+      <c r="A45" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="1" t="n">
         <v>462</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -2020,11 +1794,11 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:26" hidden="1">
-      <c r="A46" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="46">
+      <c r="A46" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46" s="1" t="n">
         <v>70</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -2034,11 +1808,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:26" hidden="1">
-      <c r="A47" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="47">
+      <c r="A47" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -2048,11 +1822,11 @@
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="1:26" hidden="1">
-      <c r="A48" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="48">
+      <c r="A48" s="2" t="n">
         <v>43190</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="1" t="n">
         <v>30</v>
       </c>
       <c r="C48" s="1"/>
@@ -2063,11 +1837,11 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1">
-      <c r="A49" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="49">
+      <c r="A49" s="2" t="n">
         <v>43191</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="1" t="n">
         <v>40</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -2077,11 +1851,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1">
-      <c r="A50" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="50">
+      <c r="A50" s="7" t="n">
         <v>43193</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50" s="1" t="n">
         <v>150</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -2091,11 +1865,11 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1">
-      <c r="A51" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="51">
+      <c r="A51" s="2" t="n">
         <v>43194</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51" s="1" t="n">
         <v>1360</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -2105,11 +1879,11 @@
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1">
-      <c r="A52" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="52">
+      <c r="A52" s="2" t="n">
         <v>43195</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" s="1" t="n">
         <v>94</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -2119,11 +1893,11 @@
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1">
-      <c r="A53" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="53">
+      <c r="A53" s="2" t="n">
         <v>43196</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C53" s="1" t="n">
         <v>48</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -2133,11 +1907,11 @@
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1">
-      <c r="A54" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="54">
+      <c r="A54" s="2" t="n">
         <v>43196</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C54" s="1" t="n">
         <v>205</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -2147,11 +1921,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1">
-      <c r="A55" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="55">
+      <c r="A55" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -2161,11 +1935,11 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1">
-      <c r="A56" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="56">
+      <c r="A56" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56" s="1" t="n">
         <v>421</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -2175,11 +1949,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1">
-      <c r="A57" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="57">
+      <c r="A57" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="1" t="n">
         <v>191</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -2189,11 +1963,11 @@
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1">
-      <c r="A58" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="58">
+      <c r="A58" s="2" t="n">
         <v>43198</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58" s="1" t="n">
         <v>226</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -2203,22 +1977,22 @@
         <v>96</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1">
-      <c r="A59" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="59">
+      <c r="A59" s="2" t="n">
         <v>43200</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59" s="1" t="n">
         <v>250</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1">
-      <c r="A60" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="60">
+      <c r="A60" s="2" t="n">
         <v>43200</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60" s="1" t="n">
         <v>1115</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -2228,11 +2002,11 @@
         <v>99</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1">
-      <c r="A61" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="61">
+      <c r="A61" s="2" t="n">
         <v>43201</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -2242,11 +2016,11 @@
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1">
-      <c r="A62" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="62">
+      <c r="A62" s="2" t="n">
         <v>43201</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62" s="1" t="n">
         <v>88</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -2256,11 +2030,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1">
-      <c r="A63" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="63">
+      <c r="A63" s="2" t="n">
         <v>43203</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -2270,11 +2044,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1">
-      <c r="A64" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="64">
+      <c r="A64" s="2" t="n">
         <v>43203</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C64" s="1" t="n">
         <v>364</v>
       </c>
       <c r="D64" s="1" t="s">
@@ -2284,11 +2058,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1">
-      <c r="A65" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="65">
+      <c r="A65" s="2" t="n">
         <v>43204</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65" s="1" t="n">
         <v>65</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -2298,11 +2072,11 @@
         <v>105</v>
       </c>
     </row>
-    <row r="66" spans="1:5" hidden="1">
-      <c r="A66" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="66">
+      <c r="A66" s="2" t="n">
         <v>43208</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -2312,11 +2086,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1">
-      <c r="A67" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="67">
+      <c r="A67" s="2" t="n">
         <v>43208</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C67" s="1" t="n">
         <v>470</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -2326,11 +2100,11 @@
         <v>107</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1">
-      <c r="A68" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="68">
+      <c r="A68" s="2" t="n">
         <v>43209</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68" s="1" t="n">
         <v>180</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -2340,11 +2114,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1">
-      <c r="A69" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="69">
+      <c r="A69" s="2" t="n">
         <v>43210</v>
       </c>
-      <c r="C69" s="1">
+      <c r="C69" s="1" t="n">
         <v>420</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -2354,11 +2128,11 @@
         <v>109</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1">
-      <c r="A70" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="70">
+      <c r="A70" s="2" t="n">
         <v>43212</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70" s="1" t="n">
         <v>50</v>
       </c>
       <c r="D70" s="1" t="s">
@@ -2368,11 +2142,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1">
-      <c r="A71" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="71">
+      <c r="A71" s="2" t="n">
         <v>43212</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71" s="1" t="n">
         <v>164</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -2382,11 +2156,11 @@
         <v>112</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1">
-      <c r="A72" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="72">
+      <c r="A72" s="2" t="n">
         <v>43215</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B72" s="1" t="n">
         <v>300</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -2396,11 +2170,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1">
-      <c r="A73" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="73">
+      <c r="A73" s="2" t="n">
         <v>43217</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73" s="1" t="n">
         <v>364</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -2410,11 +2184,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1">
-      <c r="A74" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="74">
+      <c r="A74" s="2" t="n">
         <v>43218</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74" s="1" t="n">
         <v>185</v>
       </c>
       <c r="D74" s="1" t="s">
@@ -2424,11 +2198,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1">
-      <c r="A75" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="75">
+      <c r="A75" s="2" t="n">
         <v>43218</v>
       </c>
-      <c r="C75" s="1">
+      <c r="C75" s="1" t="n">
         <v>404</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -2438,11 +2212,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="76" spans="1:5" hidden="1">
-      <c r="A76" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="76">
+      <c r="A76" s="2" t="n">
         <v>43220</v>
       </c>
-      <c r="C76" s="1">
+      <c r="C76" s="1" t="n">
         <v>57</v>
       </c>
       <c r="D76" s="1" t="s">
@@ -2452,11 +2226,11 @@
         <v>114</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1">
-      <c r="A77" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="77">
+      <c r="A77" s="2" t="n">
         <v>43221</v>
       </c>
-      <c r="C77" s="1">
+      <c r="C77" s="1" t="n">
         <v>282</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -2466,11 +2240,11 @@
         <v>116</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1">
-      <c r="A78" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="78">
+      <c r="A78" s="2" t="n">
         <v>43220</v>
       </c>
-      <c r="C78" s="1">
+      <c r="C78" s="1" t="n">
         <v>87</v>
       </c>
       <c r="D78" s="1" t="s">
@@ -2480,11 +2254,11 @@
         <v>117</v>
       </c>
     </row>
-    <row r="79" spans="1:5" hidden="1">
-      <c r="A79" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="79">
+      <c r="A79" s="2" t="n">
         <v>43223</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B79" s="1" t="n">
         <v>1878</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -2494,11 +2268,11 @@
         <v>119</v>
       </c>
     </row>
-    <row r="80" spans="1:5" hidden="1">
-      <c r="A80" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="80">
+      <c r="A80" s="2" t="n">
         <v>43224</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B80" s="1" t="n">
         <v>98</v>
       </c>
       <c r="D80" s="1" t="s">
@@ -2508,11 +2282,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="81" spans="1:5" hidden="1">
-      <c r="A81" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="81">
+      <c r="A81" s="2" t="n">
         <v>43225</v>
       </c>
-      <c r="C81" s="1">
+      <c r="C81" s="1" t="n">
         <v>198</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -2522,11 +2296,11 @@
         <v>122</v>
       </c>
     </row>
-    <row r="82" spans="1:5" hidden="1">
-      <c r="A82" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="82">
+      <c r="A82" s="2" t="n">
         <v>43225</v>
       </c>
-      <c r="C82" s="1">
+      <c r="C82" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -2536,11 +2310,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="83" spans="1:5" hidden="1">
-      <c r="A83" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="83">
+      <c r="A83" s="2" t="n">
         <v>43228</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83" s="1" t="n">
         <v>168</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -2550,11 +2324,11 @@
         <v>124</v>
       </c>
     </row>
-    <row r="84" spans="1:5" hidden="1">
-      <c r="A84" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="84">
+      <c r="A84" s="2" t="n">
         <v>43229</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B84" s="1" t="n">
         <v>240</v>
       </c>
       <c r="D84" s="1" t="s">
@@ -2564,12 +2338,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:5" hidden="1">
-      <c r="A85" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="85">
+      <c r="A85" s="2" t="n">
         <v>43230</v>
       </c>
       <c r="B85" s="1"/>
-      <c r="C85" s="1">
+      <c r="C85" s="1" t="n">
         <v>420</v>
       </c>
       <c r="D85" s="1" t="s">
@@ -2579,11 +2353,11 @@
         <v>126</v>
       </c>
     </row>
-    <row r="86" spans="1:5" hidden="1">
-      <c r="A86" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="86">
+      <c r="A86" s="2" t="n">
         <v>43230</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B86" s="1" t="n">
         <v>200</v>
       </c>
       <c r="C86" s="1"/>
@@ -2594,11 +2368,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="87" spans="1:5" hidden="1">
-      <c r="A87" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="87">
+      <c r="A87" s="2" t="n">
         <v>43230</v>
       </c>
-      <c r="C87" s="1">
+      <c r="C87" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D87" s="1" t="s">
@@ -2608,11 +2382,11 @@
         <v>128</v>
       </c>
     </row>
-    <row r="88" spans="1:5" hidden="1">
-      <c r="A88" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="88">
+      <c r="A88" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B88" s="1" t="n">
         <v>462</v>
       </c>
       <c r="D88" s="1" t="s">
@@ -2622,11 +2396,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="89" spans="1:5" hidden="1">
-      <c r="A89" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="89">
+      <c r="A89" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B89" s="1" t="n">
         <v>499</v>
       </c>
       <c r="D89" s="1" t="s">
@@ -2636,11 +2410,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="90" spans="1:5" hidden="1">
-      <c r="A90" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="90">
+      <c r="A90" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B90" s="1">
+      <c r="B90" s="1" t="n">
         <v>398</v>
       </c>
       <c r="D90" s="1" t="s">
@@ -2650,11 +2424,11 @@
         <v>133</v>
       </c>
     </row>
-    <row r="91" spans="1:5" hidden="1">
-      <c r="A91" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="91">
+      <c r="A91" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B91" s="1">
+      <c r="B91" s="1" t="n">
         <v>226</v>
       </c>
       <c r="D91" s="1" t="s">
@@ -2664,11 +2438,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="92" spans="1:5" hidden="1">
-      <c r="A92" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="92">
+      <c r="A92" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B92" s="1">
+      <c r="B92" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D92" s="1" t="s">
@@ -2678,11 +2452,11 @@
         <v>137</v>
       </c>
     </row>
-    <row r="93" spans="1:5" hidden="1">
-      <c r="A93" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="93">
+      <c r="A93" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="B93" s="1">
+      <c r="B93" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D93" s="1" t="s">
@@ -2692,11 +2466,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="94" spans="1:5" hidden="1">
-      <c r="A94" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="94">
+      <c r="A94" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="C94" s="1">
+      <c r="C94" s="1" t="n">
         <v>340</v>
       </c>
       <c r="D94" s="1" t="s">
@@ -2706,11 +2480,11 @@
         <v>139</v>
       </c>
     </row>
-    <row r="95" spans="1:5" hidden="1">
-      <c r="A95" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="95">
+      <c r="A95" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="B95" s="1">
+      <c r="B95" s="1" t="n">
         <v>510</v>
       </c>
       <c r="D95" s="1" t="s">
@@ -2720,11 +2494,11 @@
         <v>141</v>
       </c>
     </row>
-    <row r="96" spans="1:5" hidden="1">
-      <c r="A96" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="96">
+      <c r="A96" s="2" t="n">
         <v>43233</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B96" s="1" t="n">
         <v>170</v>
       </c>
       <c r="D96" s="1" t="s">
@@ -2734,11 +2508,11 @@
         <v>143</v>
       </c>
     </row>
-    <row r="97" spans="1:5" hidden="1">
-      <c r="A97" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="97">
+      <c r="A97" s="2" t="n">
         <v>43233</v>
       </c>
-      <c r="C97" s="1">
+      <c r="C97" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D97" s="1" t="s">
@@ -2748,11 +2522,11 @@
         <v>144</v>
       </c>
     </row>
-    <row r="98" spans="1:5" hidden="1">
-      <c r="A98" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="98">
+      <c r="A98" s="2" t="n">
         <v>43234</v>
       </c>
-      <c r="C98" s="1">
+      <c r="C98" s="1" t="n">
         <v>299</v>
       </c>
       <c r="D98" s="1" t="s">
@@ -2762,11 +2536,11 @@
         <v>145</v>
       </c>
     </row>
-    <row r="99" spans="1:5" hidden="1">
-      <c r="A99" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="99">
+      <c r="A99" s="2" t="n">
         <v>43236</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99" s="1" t="n">
         <v>3659</v>
       </c>
       <c r="D99" s="1" t="s">
@@ -2776,11 +2550,11 @@
         <v>146</v>
       </c>
     </row>
-    <row r="100" spans="1:5" hidden="1">
-      <c r="A100" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="100">
+      <c r="A100" s="2" t="n">
         <v>43237</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B100" s="1" t="n">
         <v>79</v>
       </c>
       <c r="D100" s="1" t="s">
@@ -2790,11 +2564,11 @@
         <v>147</v>
       </c>
     </row>
-    <row r="101" spans="1:5" hidden="1">
-      <c r="A101" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="101">
+      <c r="A101" s="2" t="n">
         <v>43236</v>
       </c>
-      <c r="C101" s="1">
+      <c r="C101" s="1" t="n">
         <v>173</v>
       </c>
       <c r="D101" s="1" t="s">
@@ -2804,11 +2578,11 @@
         <v>148</v>
       </c>
     </row>
-    <row r="102" spans="1:5" hidden="1">
-      <c r="A102" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="102">
+      <c r="A102" s="2" t="n">
         <v>43240</v>
       </c>
-      <c r="B102" s="1">
+      <c r="B102" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D102" s="1" t="s">
@@ -2818,22 +2592,22 @@
         <v>149</v>
       </c>
     </row>
-    <row r="103" spans="1:5" hidden="1">
-      <c r="A103" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="103">
+      <c r="A103" s="2" t="n">
         <v>43240</v>
       </c>
-      <c r="B103" s="1">
+      <c r="B103" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="104" spans="1:5" hidden="1">
-      <c r="A104" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="104">
+      <c r="A104" s="2" t="n">
         <v>43241</v>
       </c>
-      <c r="B104" s="1">
+      <c r="B104" s="1" t="n">
         <v>4070</v>
       </c>
       <c r="D104" s="1" t="s">
@@ -2843,11 +2617,11 @@
         <v>150</v>
       </c>
     </row>
-    <row r="105" spans="1:5" hidden="1">
-      <c r="A105" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="105">
+      <c r="A105" s="2" t="n">
         <v>43241</v>
       </c>
-      <c r="C105" s="1">
+      <c r="C105" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D105" s="1" t="s">
@@ -2857,11 +2631,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="106" spans="1:5" hidden="1">
-      <c r="A106" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="106">
+      <c r="A106" s="2" t="n">
         <v>43242</v>
       </c>
-      <c r="B106" s="1">
+      <c r="B106" s="1" t="n">
         <v>79</v>
       </c>
       <c r="D106" s="1" t="s">
@@ -2871,11 +2645,11 @@
         <v>152</v>
       </c>
     </row>
-    <row r="107" spans="1:5" hidden="1">
-      <c r="A107" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="107">
+      <c r="A107" s="2" t="n">
         <v>43246</v>
       </c>
-      <c r="B107" s="1">
+      <c r="B107" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D107" s="1" t="s">
@@ -2885,11 +2659,11 @@
         <v>154</v>
       </c>
     </row>
-    <row r="108" spans="1:5" hidden="1">
-      <c r="A108" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="108">
+      <c r="A108" s="2" t="n">
         <v>43247</v>
       </c>
-      <c r="B108" s="1">
+      <c r="B108" s="1" t="n">
         <v>70</v>
       </c>
       <c r="D108" s="1" t="s">
@@ -2899,44 +2673,44 @@
         <v>156</v>
       </c>
     </row>
-    <row r="109" spans="1:5" hidden="1">
-      <c r="A109" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="109">
+      <c r="A109" s="2" t="n">
         <v>43253</v>
       </c>
-      <c r="B109" s="1">
+      <c r="B109" s="1" t="n">
         <v>142</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="110" spans="1:5" hidden="1">
-      <c r="A110" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="110">
+      <c r="A110" s="2" t="n">
         <v>43254</v>
       </c>
-      <c r="B110" s="1">
+      <c r="B110" s="1" t="n">
         <v>90</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="111" spans="1:5" hidden="1">
-      <c r="A111" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="111">
+      <c r="A111" s="2" t="n">
         <v>43260</v>
       </c>
-      <c r="C111" s="1">
+      <c r="C111" s="1" t="n">
         <v>1400</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="112" spans="1:5" hidden="1">
-      <c r="A112" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="112">
+      <c r="A112" s="2" t="n">
         <v>43260</v>
       </c>
-      <c r="C112" s="1">
+      <c r="C112" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D112" s="1" t="s">
@@ -2946,33 +2720,33 @@
         <v>91</v>
       </c>
     </row>
-    <row r="113" spans="1:5" hidden="1">
-      <c r="A113" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="113">
+      <c r="A113" s="2" t="n">
         <v>43264</v>
       </c>
-      <c r="B113" s="1">
+      <c r="B113" s="1" t="n">
         <v>546</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="114" spans="1:5" hidden="1">
-      <c r="A114" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="114">
+      <c r="A114" s="2" t="n">
         <v>43264</v>
       </c>
-      <c r="B114" s="1">
+      <c r="B114" s="1" t="n">
         <v>95</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="115" spans="1:5" hidden="1">
-      <c r="A115" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="115">
+      <c r="A115" s="2" t="n">
         <v>43266</v>
       </c>
-      <c r="B115" s="1">
+      <c r="B115" s="1" t="n">
         <v>394</v>
       </c>
       <c r="D115" s="1" t="s">
@@ -2982,11 +2756,11 @@
         <v>163</v>
       </c>
     </row>
-    <row r="116" spans="1:5" hidden="1">
-      <c r="A116" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="116">
+      <c r="A116" s="2" t="n">
         <v>43266</v>
       </c>
-      <c r="B116" s="1">
+      <c r="B116" s="1" t="n">
         <v>1055</v>
       </c>
       <c r="D116" s="1" t="s">
@@ -2996,11 +2770,11 @@
         <v>165</v>
       </c>
     </row>
-    <row r="117" spans="1:5" hidden="1">
-      <c r="A117" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="117">
+      <c r="A117" s="2" t="n">
         <v>43284</v>
       </c>
-      <c r="C117" s="1">
+      <c r="C117" s="1" t="n">
         <v>274</v>
       </c>
       <c r="D117" s="1" t="s">
@@ -3010,11 +2784,11 @@
         <v>167</v>
       </c>
     </row>
-    <row r="118" spans="1:5" hidden="1">
-      <c r="A118" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="118">
+      <c r="A118" s="2" t="n">
         <v>43283</v>
       </c>
-      <c r="C118" s="1">
+      <c r="C118" s="1" t="n">
         <v>105</v>
       </c>
       <c r="D118" s="1" t="s">
@@ -3024,11 +2798,11 @@
         <v>169</v>
       </c>
     </row>
-    <row r="119" spans="1:5" hidden="1">
-      <c r="A119" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="119">
+      <c r="A119" s="2" t="n">
         <v>43289</v>
       </c>
-      <c r="C119" s="1">
+      <c r="C119" s="1" t="n">
         <v>128</v>
       </c>
       <c r="D119" s="1" t="s">
@@ -3038,11 +2812,11 @@
         <v>171</v>
       </c>
     </row>
-    <row r="120" spans="1:5" hidden="1">
-      <c r="A120" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="120">
+      <c r="A120" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C120" s="1">
+      <c r="C120" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D120" s="1" t="s">
@@ -3052,11 +2826,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="121" spans="1:5" hidden="1">
-      <c r="A121" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="121">
+      <c r="A121" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C121" s="1">
+      <c r="C121" s="1" t="n">
         <v>210</v>
       </c>
       <c r="D121" s="1" t="s">
@@ -3066,44 +2840,44 @@
         <v>173</v>
       </c>
     </row>
-    <row r="122" spans="1:5" hidden="1">
-      <c r="A122" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="122">
+      <c r="A122" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B122" s="1">
+      <c r="B122" s="1" t="n">
         <v>980</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="123" spans="1:5" hidden="1">
-      <c r="A123" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="123">
+      <c r="A123" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B123" s="1">
+      <c r="B123" s="1" t="n">
         <v>1260</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="124" spans="1:5" hidden="1">
-      <c r="A124" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="124">
+      <c r="A124" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B124" s="1">
+      <c r="B124" s="1" t="n">
         <v>3687</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="125" spans="1:5" hidden="1">
-      <c r="A125" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="125">
+      <c r="A125" s="2" t="n">
         <v>43298</v>
       </c>
-      <c r="C125" s="1">
+      <c r="C125" s="1" t="n">
         <v>60</v>
       </c>
       <c r="D125" s="1" t="s">
@@ -3113,55 +2887,55 @@
         <v>178</v>
       </c>
     </row>
-    <row r="126" spans="1:5" hidden="1">
-      <c r="A126" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="126">
+      <c r="A126" s="2" t="n">
         <v>43291</v>
       </c>
-      <c r="C126" s="1">
+      <c r="C126" s="1" t="n">
         <v>404</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="127" spans="1:5" hidden="1">
-      <c r="A127" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="127">
+      <c r="A127" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C127" s="1">
+      <c r="C127" s="1" t="n">
         <v>451</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="128" spans="1:5" hidden="1">
-      <c r="A128" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="128">
+      <c r="A128" s="2" t="n">
         <v>43298</v>
       </c>
-      <c r="C128" s="1">
+      <c r="C128" s="1" t="n">
         <v>708</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="129" spans="1:5" hidden="1">
-      <c r="A129" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="129">
+      <c r="A129" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C129" s="1">
+      <c r="C129" s="1" t="n">
         <v>160</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="130" spans="1:5" hidden="1">
-      <c r="A130" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="130">
+      <c r="A130" s="2" t="n">
         <v>43288</v>
       </c>
-      <c r="C130" s="1">
+      <c r="C130" s="1" t="n">
         <v>72</v>
       </c>
       <c r="D130" s="1" t="s">
@@ -3171,11 +2945,11 @@
         <v>181</v>
       </c>
     </row>
-    <row r="131" spans="1:5" hidden="1">
-      <c r="A131" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="131">
+      <c r="A131" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C131" s="1">
+      <c r="C131" s="1" t="n">
         <v>300</v>
       </c>
       <c r="D131" s="1" t="s">
@@ -3185,11 +2959,11 @@
         <v>183</v>
       </c>
     </row>
-    <row r="132" spans="1:5" hidden="1">
-      <c r="A132" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="132">
+      <c r="A132" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C132" s="1">
+      <c r="C132" s="1" t="n">
         <v>230</v>
       </c>
       <c r="D132" s="1" t="s">
@@ -3199,22 +2973,22 @@
         <v>185</v>
       </c>
     </row>
-    <row r="133" spans="1:5" hidden="1">
-      <c r="A133" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="133">
+      <c r="A133" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C133" s="1">
+      <c r="C133" s="1" t="n">
         <v>454</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="134" spans="1:5" hidden="1">
-      <c r="A134" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="134">
+      <c r="A134" s="2" t="n">
         <v>43299</v>
       </c>
-      <c r="C134" s="1">
+      <c r="C134" s="1" t="n">
         <v>686</v>
       </c>
       <c r="D134" s="1" t="s">
@@ -3224,11 +2998,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="135" spans="1:5" hidden="1">
-      <c r="A135" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="135">
+      <c r="A135" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C135" s="1">
+      <c r="C135" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D135" s="1" t="s">
@@ -3238,11 +3012,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="136" spans="1:5" hidden="1">
-      <c r="A136" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="136">
+      <c r="A136" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C136" s="1">
+      <c r="C136" s="1" t="n">
         <v>2067</v>
       </c>
       <c r="D136" s="1" t="s">
@@ -3252,11 +3026,11 @@
         <v>186</v>
       </c>
     </row>
-    <row r="137" spans="1:5" hidden="1">
-      <c r="A137" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="137">
+      <c r="A137" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B137" s="1">
+      <c r="B137" s="1" t="n">
         <v>109</v>
       </c>
       <c r="D137" s="1" t="s">
@@ -3266,11 +3040,11 @@
         <v>187</v>
       </c>
     </row>
-    <row r="138" spans="1:5" hidden="1">
-      <c r="A138" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="138">
+      <c r="A138" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B138" s="1">
+      <c r="B138" s="1" t="n">
         <v>97</v>
       </c>
       <c r="D138" s="1" t="s">
@@ -3280,11 +3054,11 @@
         <v>188</v>
       </c>
     </row>
-    <row r="139" spans="1:5" hidden="1">
-      <c r="A139" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="139">
+      <c r="A139" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B139" s="1">
+      <c r="B139" s="1" t="n">
         <v>1437</v>
       </c>
       <c r="D139" s="1" t="s">
@@ -3294,11 +3068,11 @@
         <v>189</v>
       </c>
     </row>
-    <row r="140" spans="1:5" hidden="1">
-      <c r="A140" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="140">
+      <c r="A140" s="2" t="n">
         <v>43306</v>
       </c>
-      <c r="C140" s="1">
+      <c r="C140" s="1" t="n">
         <v>650</v>
       </c>
       <c r="D140" s="1" t="s">
@@ -3308,11 +3082,11 @@
         <v>190</v>
       </c>
     </row>
-    <row r="141" spans="1:5" hidden="1">
-      <c r="A141" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="141">
+      <c r="A141" s="2" t="n">
         <v>43305</v>
       </c>
-      <c r="C141" s="1">
+      <c r="C141" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D141" s="1" t="s">
@@ -3322,11 +3096,11 @@
         <v>191</v>
       </c>
     </row>
-    <row r="142" spans="1:5" hidden="1">
-      <c r="A142" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="142">
+      <c r="A142" s="2" t="n">
         <v>43309</v>
       </c>
-      <c r="C142" s="1">
+      <c r="C142" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D142" s="1" t="s">
@@ -3336,11 +3110,11 @@
         <v>192</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="14" hidden="1">
-      <c r="A143" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="0" r="143">
+      <c r="A143" s="2" t="n">
         <v>43306</v>
       </c>
-      <c r="B143" s="1">
+      <c r="B143" s="1" t="n">
         <v>167</v>
       </c>
       <c r="D143" s="1" t="s">
@@ -3350,11 +3124,11 @@
         <v>193</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="14" hidden="1">
-      <c r="A144" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="0" r="144">
+      <c r="A144" s="2" t="n">
         <v>43304</v>
       </c>
-      <c r="C144" s="1">
+      <c r="C144" s="1" t="n">
         <v>93</v>
       </c>
       <c r="D144" s="1" t="s">
@@ -3364,11 +3138,11 @@
         <v>194</v>
       </c>
     </row>
-    <row r="145" spans="1:5" hidden="1">
-      <c r="A145" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="145">
+      <c r="A145" s="2" t="n">
         <v>43305</v>
       </c>
-      <c r="C145" s="1">
+      <c r="C145" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D145" s="1" t="s">
@@ -3378,11 +3152,11 @@
         <v>195</v>
       </c>
     </row>
-    <row r="146" spans="1:5" hidden="1">
-      <c r="A146" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="146">
+      <c r="A146" s="2" t="n">
         <v>43303</v>
       </c>
-      <c r="C146" s="1">
+      <c r="C146" s="1" t="n">
         <v>244</v>
       </c>
       <c r="D146" s="1" t="s">
@@ -3392,11 +3166,11 @@
         <v>196</v>
       </c>
     </row>
-    <row r="147" spans="1:5" hidden="1">
-      <c r="A147" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="147">
+      <c r="A147" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C147" s="1">
+      <c r="C147" s="1" t="n">
         <v>482</v>
       </c>
       <c r="D147" s="1" t="s">
@@ -3406,11 +3180,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="148" spans="1:5" hidden="1">
-      <c r="A148" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="148">
+      <c r="A148" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C148" s="1">
+      <c r="C148" s="1" t="n">
         <v>172</v>
       </c>
       <c r="D148" s="1" t="s">
@@ -3420,44 +3194,44 @@
         <v>199</v>
       </c>
     </row>
-    <row r="149" spans="1:5" hidden="1">
-      <c r="A149" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="149">
+      <c r="A149" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="B149" s="1">
+      <c r="B149" s="1" t="n">
         <v>89</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="150" spans="1:5" hidden="1">
-      <c r="A150" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="150">
+      <c r="A150" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="C150" s="1">
+      <c r="C150" s="1" t="n">
         <v>107</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="151" spans="1:5" hidden="1">
-      <c r="A151" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="151">
+      <c r="A151" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="C151" s="1">
+      <c r="C151" s="1" t="n">
         <v>124</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="152" spans="1:5" hidden="1">
-      <c r="A152" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="152">
+      <c r="A152" s="7" t="n">
         <v>43316</v>
       </c>
-      <c r="C152" s="1">
+      <c r="C152" s="1" t="n">
         <v>4500</v>
       </c>
       <c r="D152" s="1" t="s">
@@ -3467,11 +3241,11 @@
         <v>202</v>
       </c>
     </row>
-    <row r="153" spans="1:5" hidden="1">
-      <c r="A153" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="153">
+      <c r="A153" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C153" s="1">
+      <c r="C153" s="1" t="n">
         <v>247</v>
       </c>
       <c r="D153" s="1" t="s">
@@ -3481,11 +3255,11 @@
         <v>204</v>
       </c>
     </row>
-    <row r="154" spans="1:5" hidden="1">
-      <c r="A154" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="154">
+      <c r="A154" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C154" s="1">
+      <c r="C154" s="1" t="n">
         <v>1150</v>
       </c>
       <c r="D154" s="1" t="s">
@@ -3495,11 +3269,11 @@
         <v>205</v>
       </c>
     </row>
-    <row r="155" spans="1:5" hidden="1">
-      <c r="A155" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="155">
+      <c r="A155" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C155" s="1">
+      <c r="C155" s="1" t="n">
         <v>313</v>
       </c>
       <c r="D155" s="1" t="s">
@@ -3509,11 +3283,11 @@
         <v>207</v>
       </c>
     </row>
-    <row r="156" spans="1:5" hidden="1">
-      <c r="A156" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="156">
+      <c r="A156" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="B156" s="1">
+      <c r="B156" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D156" s="1" t="s">
@@ -3523,11 +3297,11 @@
         <v>209</v>
       </c>
     </row>
-    <row r="157" spans="1:5" hidden="1">
-      <c r="A157" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="157">
+      <c r="A157" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="C157" s="1">
+      <c r="C157" s="1" t="n">
         <v>710</v>
       </c>
       <c r="D157" s="1" t="s">
@@ -3537,11 +3311,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="158" spans="1:5">
-      <c r="A158" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="158">
+      <c r="A158" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="C158" s="1">
+      <c r="C158" s="1" t="n">
         <v>100</v>
       </c>
       <c r="D158" s="1" t="s">
@@ -3551,11 +3325,11 @@
         <v>212</v>
       </c>
     </row>
-    <row r="159" spans="1:5">
-      <c r="A159" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="159">
+      <c r="A159" s="2" t="n">
         <v>43319</v>
       </c>
-      <c r="B159" s="1">
+      <c r="B159" s="1" t="n">
         <v>78</v>
       </c>
       <c r="D159" s="1" t="s">
@@ -3565,22 +3339,22 @@
         <v>213</v>
       </c>
     </row>
-    <row r="160" spans="1:5">
-      <c r="A160" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="160">
+      <c r="A160" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="B160" s="1">
+      <c r="B160" s="1" t="n">
         <v>1840</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="161" spans="1:5">
-      <c r="A161" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="161">
+      <c r="A161" s="2" t="n">
         <v>43322</v>
       </c>
-      <c r="B161" s="1">
+      <c r="B161" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D161" s="1" t="s">
@@ -3590,11 +3364,11 @@
         <v>216</v>
       </c>
     </row>
-    <row r="162" spans="1:5">
-      <c r="A162" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="162">
+      <c r="A162" s="7" t="n">
         <v>43324</v>
       </c>
-      <c r="C162" s="1">
+      <c r="C162" s="1" t="n">
         <v>230</v>
       </c>
       <c r="D162" s="1" t="s">
@@ -3604,11 +3378,11 @@
         <v>217</v>
       </c>
     </row>
-    <row r="163" spans="1:5">
-      <c r="A163" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="163">
+      <c r="A163" s="7" t="n">
         <v>43326</v>
       </c>
-      <c r="C163" s="1">
+      <c r="C163" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D163" s="1" t="s">
@@ -3618,11 +3392,11 @@
         <v>219</v>
       </c>
     </row>
-    <row r="164" spans="1:5">
-      <c r="A164" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="164">
+      <c r="A164" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="B164" s="1">
+      <c r="B164" s="1" t="n">
         <v>45</v>
       </c>
       <c r="D164" s="1" t="s">
@@ -3632,760 +3406,779 @@
         <v>221</v>
       </c>
     </row>
-    <row r="165" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A165" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="165">
+      <c r="A165" s="10" t="n">
         <v>43327</v>
       </c>
-      <c r="C165">
+      <c r="C165" s="0" t="n">
         <v>486</v>
       </c>
-      <c r="D165" t="s">
+      <c r="D165" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E165" t="s">
+      <c r="E165" s="0" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="166" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A166" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="166">
+      <c r="A166" s="10" t="n">
         <v>43329</v>
       </c>
-      <c r="C166">
+      <c r="C166" s="0" t="n">
         <v>92</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D166" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="E166" t="s">
+      <c r="E166" s="0" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="167" spans="1:5">
-      <c r="A167" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="167">
+      <c r="A167" s="10" t="n">
         <v>43331</v>
       </c>
-      <c r="C167">
+      <c r="C167" s="0" t="n">
         <v>310</v>
       </c>
-      <c r="D167" t="s">
+      <c r="D167" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="E167" t="s">
+      <c r="E167" s="0" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="168" spans="1:5">
-      <c r="A168" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="168">
+      <c r="A168" s="10" t="n">
         <v>43334</v>
       </c>
-      <c r="C168">
+      <c r="C168" s="0" t="n">
         <v>464</v>
       </c>
-      <c r="D168" t="s">
+      <c r="D168" s="0" t="s">
         <v>218</v>
       </c>
       <c r="E168" s="11" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="169" spans="1:5">
-      <c r="A169" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="169">
+      <c r="A169" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="C169">
+      <c r="C169" s="0" t="n">
         <v>726</v>
       </c>
-      <c r="D169" t="s">
+      <c r="D169" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="E169" t="s">
+      <c r="E169" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="170" spans="1:5">
-      <c r="A170" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="170">
+      <c r="A170" s="10" t="n">
         <v>43337</v>
       </c>
-      <c r="C170">
+      <c r="C170" s="0" t="n">
         <v>544</v>
       </c>
-      <c r="D170" t="s">
+      <c r="D170" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E170" t="s">
+      <c r="E170" s="0" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="171" spans="1:5">
-      <c r="A171" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="171">
+      <c r="A171" s="10" t="n">
         <v>43337</v>
       </c>
-      <c r="B171">
+      <c r="B171" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D171" t="s">
+      <c r="D171" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="E171" t="s">
+      <c r="E171" s="0" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="172" spans="1:5">
-      <c r="A172" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="172">
+      <c r="A172" s="10" t="n">
         <v>43341</v>
       </c>
-      <c r="C172">
+      <c r="C172" s="0" t="n">
         <v>830</v>
       </c>
-      <c r="D172" t="s">
+      <c r="D172" s="0" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="173" spans="1:5">
-      <c r="A173" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="173">
+      <c r="A173" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="C173">
+      <c r="C173" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="D173" t="s">
+      <c r="D173" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="E173" t="s">
+      <c r="E173" s="0" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="174" spans="1:5">
-      <c r="A174" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="174">
+      <c r="A174" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="B174">
+      <c r="B174" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D174" t="s">
+      <c r="D174" s="0" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="175" spans="1:5">
-      <c r="A175" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="175">
+      <c r="A175" s="10" t="n">
         <v>43344</v>
       </c>
-      <c r="B175">
+      <c r="B175" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="D175" t="s">
+      <c r="D175" s="0" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="176" spans="1:5">
-      <c r="A176" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="176">
+      <c r="A176" s="10" t="n">
         <v>43344</v>
       </c>
-      <c r="B176">
+      <c r="B176" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D176" t="s">
+      <c r="D176" s="0" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="177" spans="1:5">
-      <c r="A177" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="177">
+      <c r="A177" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C177">
+      <c r="C177" s="0" t="n">
         <v>607</v>
       </c>
-      <c r="D177" t="s">
+      <c r="D177" s="0" t="s">
         <v>235</v>
       </c>
-      <c r="E177" t="s">
+      <c r="E177" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="178" spans="1:5">
-      <c r="A178" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="178">
+      <c r="A178" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C178">
+      <c r="C178" s="0" t="n">
         <v>444</v>
       </c>
-      <c r="D178" t="s">
+      <c r="D178" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E178" t="s">
+      <c r="E178" s="0" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="179" spans="1:5">
-      <c r="A179" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="179">
+      <c r="A179" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C179">
+      <c r="C179" s="0" t="n">
         <v>312</v>
       </c>
-      <c r="D179" t="s">
+      <c r="D179" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="E179" t="s">
+      <c r="E179" s="0" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="180" spans="1:5">
-      <c r="A180" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="180">
+      <c r="A180" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C180">
+      <c r="C180" s="0" t="n">
         <v>501</v>
       </c>
-      <c r="D180" t="s">
+      <c r="D180" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E180" t="s">
+      <c r="E180" s="0" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="181" spans="1:5">
-      <c r="A181" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="181">
+      <c r="A181" s="10" t="n">
         <v>43349</v>
       </c>
-      <c r="C181">
+      <c r="C181" s="0" t="n">
         <v>711</v>
       </c>
-      <c r="D181" t="s">
+      <c r="D181" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="E181" t="s">
+      <c r="E181" s="0" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="182" spans="1:5">
-      <c r="A182" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="182">
+      <c r="A182" s="10" t="n">
         <v>43354</v>
       </c>
-      <c r="B182">
+      <c r="B182" s="0" t="n">
         <v>126</v>
       </c>
-      <c r="D182" t="s">
+      <c r="D182" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="E182" t="s">
+      <c r="E182" s="0" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="183" spans="1:5">
-      <c r="A183" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="183">
+      <c r="A183" s="10" t="n">
         <v>43354</v>
       </c>
-      <c r="C183">
+      <c r="C183" s="0" t="n">
         <v>450</v>
       </c>
-      <c r="D183" t="s">
+      <c r="D183" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="E183" t="s">
+      <c r="E183" s="0" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="184" spans="1:5">
-      <c r="A184" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="184">
+      <c r="A184" s="10" t="n">
         <v>43361</v>
       </c>
-      <c r="C184">
+      <c r="C184" s="0" t="n">
         <v>660</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D184" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="E184" t="s">
+      <c r="E184" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="185" spans="1:5">
-      <c r="A185" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="185">
+      <c r="A185" s="10" t="n">
         <v>43363</v>
       </c>
-      <c r="C185">
+      <c r="C185" s="0" t="n">
         <v>230</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D185" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="E185" t="s">
+      <c r="E185" s="0" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="186" spans="1:5">
-      <c r="A186" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="186">
+      <c r="A186" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B186">
+      <c r="B186" s="0" t="n">
         <v>4859</v>
       </c>
-      <c r="D186" t="s">
+      <c r="D186" s="0" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="187" spans="1:5">
-      <c r="A187" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="187">
+      <c r="A187" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B187">
+      <c r="B187" s="0" t="n">
         <v>295</v>
       </c>
-      <c r="D187" t="s">
+      <c r="D187" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="E187" t="s">
+      <c r="E187" s="0" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="188" spans="1:5">
-      <c r="A188" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="188">
+      <c r="A188" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B188">
+      <c r="B188" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D188" t="s">
+      <c r="D188" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="E188" t="s">
+      <c r="E188" s="0" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="189" spans="1:5">
-      <c r="A189" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="189">
+      <c r="A189" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B189">
+      <c r="B189" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="D189" t="s">
+      <c r="D189" s="0" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="190" spans="1:5">
-      <c r="A190" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="190">
+      <c r="A190" s="10" t="n">
         <v>43378</v>
       </c>
-      <c r="B190">
+      <c r="B190" s="0" t="n">
         <v>506</v>
       </c>
-      <c r="D190" t="s">
+      <c r="D190" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="E190" t="s">
+      <c r="E190" s="0" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="191" spans="1:5">
-      <c r="A191" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="191">
+      <c r="A191" s="10" t="n">
         <v>43379</v>
       </c>
-      <c r="B191">
+      <c r="B191" s="0" t="n">
         <v>350</v>
       </c>
-      <c r="D191" t="s">
+      <c r="D191" s="0" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="192" spans="1:5" ht="20" customHeight="1">
-      <c r="A192" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="20" outlineLevel="0" r="192">
+      <c r="A192" s="10" t="n">
         <v>43383</v>
       </c>
-      <c r="B192">
+      <c r="B192" s="0" t="n">
         <v>189</v>
       </c>
-      <c r="D192" t="s">
+      <c r="D192" s="0" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="193" spans="1:5" ht="1">
-      <c r="A193" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="1" outlineLevel="0" r="193">
+      <c r="A193" s="10" t="n">
         <v>43387</v>
       </c>
-      <c r="B193">
+      <c r="B193" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="D193" t="s">
+      <c r="D193" s="0" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="194" spans="1:5">
-      <c r="A194" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="194">
+      <c r="A194" s="10" t="n">
         <v>43387</v>
       </c>
-      <c r="B194">
+      <c r="B194" s="0" t="n">
         <v>307</v>
       </c>
-      <c r="D194" t="s">
+      <c r="D194" s="0" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="195" spans="1:5">
-      <c r="C195">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="195">
+      <c r="C195" s="0" t="n">
         <v>3705</v>
       </c>
-      <c r="E195" t="s">
+      <c r="E195" s="0" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="196" spans="1:5">
-      <c r="A196" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="196">
+      <c r="A196" s="10" t="n">
         <v>43385</v>
       </c>
-      <c r="C196">
+      <c r="C196" s="0" t="n">
         <v>608</v>
       </c>
-      <c r="D196" t="s">
+      <c r="D196" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E196" t="s">
+      <c r="E196" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="197" spans="1:5">
-      <c r="A197" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="197">
+      <c r="A197" s="10" t="n">
         <v>43391</v>
       </c>
-      <c r="B197">
+      <c r="B197" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="D197" t="s">
+      <c r="D197" s="0" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="198" spans="1:5">
-      <c r="A198" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="198">
+      <c r="A198" s="10" t="n">
         <v>43392</v>
       </c>
-      <c r="B198">
+      <c r="B198" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="D198" t="s">
+      <c r="D198" s="0" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="199" spans="1:5">
-      <c r="A199" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="199">
+      <c r="A199" s="10" t="n">
         <v>43393</v>
       </c>
-      <c r="B199">
+      <c r="B199" s="0" t="n">
         <v>177</v>
       </c>
-      <c r="D199" t="s">
+      <c r="D199" s="0" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="200" spans="1:5">
-      <c r="A200" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="200">
+      <c r="A200" s="10" t="n">
         <v>43393</v>
       </c>
-      <c r="C200">
+      <c r="C200" s="0" t="n">
         <v>125</v>
       </c>
-      <c r="D200" t="s">
+      <c r="D200" s="0" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="201" spans="1:5">
-      <c r="A201" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="201">
+      <c r="A201" s="10" t="n">
         <v>43395</v>
       </c>
-      <c r="B201">
+      <c r="B201" s="0" t="n">
         <v>2800</v>
       </c>
       <c r="D201" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="E201" t="s">
+      <c r="E201" s="0" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="202" spans="1:5">
-      <c r="A202" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="202">
+      <c r="A202" s="10" t="n">
         <v>43395</v>
       </c>
-      <c r="C202">
+      <c r="C202" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="D202" t="s">
+      <c r="D202" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="E202" t="s">
+      <c r="E202" s="0" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="203" spans="1:5">
-      <c r="A203" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="203">
+      <c r="A203" s="10" t="n">
         <v>43396</v>
       </c>
-      <c r="C203">
+      <c r="C203" s="0" t="n">
         <v>692</v>
       </c>
-      <c r="D203" t="s">
+      <c r="D203" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E203" t="s">
+      <c r="E203" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="204" spans="1:5">
-      <c r="A204" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="204">
+      <c r="A204" s="10" t="n">
         <v>43397</v>
       </c>
-      <c r="C204">
+      <c r="C204" s="0" t="n">
         <v>4935</v>
       </c>
-      <c r="D204" t="s">
+      <c r="D204" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="E204" t="s">
+      <c r="E204" s="0" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="205" spans="1:5" ht="10" customHeight="1">
-      <c r="A205" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10" outlineLevel="0" r="205">
+      <c r="A205" s="10" t="n">
         <v>43398</v>
       </c>
-      <c r="B205">
+      <c r="B205" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="D205" t="s">
+      <c r="D205" s="0" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="206" spans="1:5">
-      <c r="A206" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="206">
+      <c r="A206" s="10" t="n">
         <v>43398</v>
       </c>
-      <c r="B206">
+      <c r="B206" s="0" t="n">
         <v>370</v>
       </c>
-      <c r="D206" t="s">
+      <c r="D206" s="0" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="207" spans="1:5">
-      <c r="A207" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="207">
+      <c r="A207" s="10" t="n">
         <v>43398</v>
       </c>
-      <c r="B207">
+      <c r="B207" s="0" t="n">
         <v>4966</v>
       </c>
-      <c r="D207" t="s">
+      <c r="D207" s="0" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="208" spans="1:5">
-      <c r="A208" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="208">
+      <c r="A208" s="10" t="n">
         <v>43397</v>
       </c>
-      <c r="C208">
+      <c r="C208" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="D208" t="s">
+      <c r="D208" s="0" t="s">
         <v>265</v>
       </c>
-      <c r="E208" t="s">
+      <c r="E208" s="0" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="209" spans="1:5">
-      <c r="A209" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="209">
+      <c r="A209" s="10" t="n">
         <v>43399</v>
       </c>
-      <c r="B209">
+      <c r="B209" s="0" t="n">
         <v>182</v>
       </c>
-      <c r="D209" t="s">
+      <c r="D209" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="E209" t="s">
+      <c r="E209" s="0" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="210" spans="1:5">
-      <c r="A210" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="210">
+      <c r="A210" s="10" t="n">
         <v>43401</v>
       </c>
-      <c r="B210">
+      <c r="B210" s="0" t="n">
         <v>700</v>
       </c>
-      <c r="D210" t="s">
+      <c r="D210" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="E210" t="s">
+      <c r="E210" s="0" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="211" spans="1:5">
-      <c r="A211" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="211">
+      <c r="A211" s="10" t="n">
         <v>43405</v>
       </c>
-      <c r="B211">
+      <c r="B211" s="0" t="n">
         <v>274</v>
       </c>
-      <c r="D211" t="s">
+      <c r="D211" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="E211" t="s">
+      <c r="E211" s="0" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="212" spans="1:5">
-      <c r="A212" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="212">
+      <c r="A212" s="10" t="n">
         <v>43405</v>
       </c>
-      <c r="C212">
+      <c r="C212" s="0" t="n">
         <v>590</v>
       </c>
-      <c r="D212" t="s">
+      <c r="D212" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="E212" t="s">
+      <c r="E212" s="0" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="213" spans="1:5" ht="14">
-      <c r="A213" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="213">
+      <c r="A213" s="10" t="n">
         <v>43407</v>
       </c>
-      <c r="C213">
+      <c r="C213" s="0" t="n">
         <v>1275</v>
       </c>
       <c r="D213" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="E213" t="s">
+      <c r="E213" s="0" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="214" spans="1:5" ht="14">
-      <c r="A214" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="214">
+      <c r="A214" s="10" t="n">
         <v>43407</v>
       </c>
-      <c r="C214">
+      <c r="C214" s="0" t="n">
         <v>4781</v>
       </c>
       <c r="D214" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="E214" t="s">
+      <c r="E214" s="0" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="215" spans="1:5" ht="14">
-      <c r="A215" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="215">
+      <c r="A215" s="10" t="n">
         <v>43407</v>
       </c>
-      <c r="C215">
+      <c r="C215" s="0" t="n">
         <v>4781</v>
       </c>
       <c r="D215" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="E215" t="s">
+      <c r="E215" s="0" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="216" spans="1:5">
-      <c r="A216" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="216">
+      <c r="A216" s="10" t="n">
         <v>43406</v>
       </c>
-      <c r="C216">
+      <c r="C216" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D216" t="s">
+      <c r="D216" s="0" t="s">
         <v>272</v>
       </c>
-      <c r="E216" t="s">
+      <c r="E216" s="0" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="217" spans="1:5">
-      <c r="A217" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="217">
+      <c r="A217" s="10" t="n">
         <v>43409</v>
       </c>
-      <c r="C217">
+      <c r="C217" s="0" t="n">
         <v>677</v>
       </c>
-      <c r="D217" t="s">
+      <c r="D217" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E217" t="s">
+      <c r="E217" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="218" spans="1:5" ht="14">
-      <c r="A218" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="218">
+      <c r="A218" s="10" t="n">
         <v>43410</v>
       </c>
-      <c r="B218">
+      <c r="B218" s="0" t="n">
         <v>285</v>
       </c>
       <c r="D218" s="13" t="s">
         <v>274</v>
       </c>
-      <c r="E218" t="s">
+      <c r="E218" s="0" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="219" spans="1:5" ht="14">
-      <c r="A219" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="219">
+      <c r="A219" s="10" t="n">
         <v>43410</v>
       </c>
-      <c r="B219">
+      <c r="B219" s="0" t="n">
         <v>125</v>
       </c>
       <c r="D219" s="13" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="220" spans="1:5" ht="14">
-      <c r="A220" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="220">
+      <c r="A220" s="10" t="n">
         <v>43409</v>
       </c>
-      <c r="B220">
+      <c r="B220" s="0" t="n">
         <v>85</v>
       </c>
       <c r="D220" s="13" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="221" spans="1:5" ht="14">
-      <c r="A221" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="221">
+      <c r="A221" s="10" t="n">
         <v>43410</v>
       </c>
-      <c r="B221">
+      <c r="B221" s="0" t="n">
         <v>44</v>
       </c>
       <c r="D221" s="13" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="241" spans="2:3">
-      <c r="B241">
-        <f>SUM(B2:B240)</f>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="222">
+      <c r="A222" s="10" t="n">
+        <v>43412</v>
+      </c>
+      <c r="C222" s="0" t="n">
+        <v>190</v>
+      </c>
+      <c r="D222" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="E222" s="0" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="241">
+      <c r="B241" s="0" t="n">
+        <f aca="false">SUM(B2:B240)</f>
         <v>56451</v>
       </c>
-      <c r="C241">
-        <f>SUM(C2:C240)</f>
-        <v>64655</v>
+      <c r="C241" s="0" t="n">
+        <f aca="false">SUM(C2:C240)</f>
+        <v>64845</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A30:Z32">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule aboveAverage="0" bottom="0" dxfId="0" operator="expression" percent="0" priority="2" rank="0" text="" type="expression">
       <formula>LEN(TRIM(A30))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D33" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D40" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D201" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink display="netonnet.se" ref="D33" r:id="rId1"/>
+    <hyperlink display="www.vidaxl.se" ref="D40" r:id="rId2"/>
+    <hyperlink display="https://www.vardia.se/" ref="D201" r:id="rId3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cost update Jenny 1116
</commit_message>
<xml_diff>
--- a/Cost.xlsx
+++ b/Cost.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chengkaiyan/github/cost/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163A60C6-D9B2-8B42-8BCD-208879F09E44}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19820" windowHeight="12320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="288">
   <si>
     <t>日期</t>
   </si>
@@ -872,61 +867,89 @@
   </si>
   <si>
     <t>滤网</t>
+  </si>
+  <si>
+    <t>Restarang 88</t>
+  </si>
+  <si>
+    <t>paron;beef;vegetables,etc</t>
+  </si>
+  <si>
+    <t>ICA taby centrum</t>
+  </si>
+  <si>
+    <t>brioche;stekflask,juice;etc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="yyyy/m/d"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt formatCode="YYYY/M/D" numFmtId="165"/>
+    <numFmt formatCode="M/D/YYYY" numFmtId="166"/>
+    <numFmt formatCode="YYYY\-MM\-DD" numFmtId="167"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="10">
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <family val="0"/>
       <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
       <name val="Arial"/>
       <family val="2"/>
+      <sz val="10"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF666666"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF666666"/>
+      <sz val="11"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0563C1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF0563C1"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0563C1"/>
       <name val="FreeSans"/>
       <family val="2"/>
+      <color rgb="FF0563C1"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF444444"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF444444"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="5">
@@ -956,7 +979,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
@@ -964,31 +987,100 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+  <cellStyleXfs count="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="167" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="20">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="7">
+    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle builtinId="8" customBuiltin="false" name="*unknown*" xfId="20"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -999,7 +1091,6 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1058,339 +1149,31 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF444444"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:Z241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A212" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E226" sqref="E226"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A212" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E230" activeCellId="0" pane="topLeft" sqref="E230"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="3" width="14.5"/>
-    <col min="4" max="4" width="26"/>
-    <col min="5" max="5" width="37.83203125"/>
-    <col min="6" max="1025" width="14.5"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="14.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1407,11 +1190,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1">
-      <c r="A2" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="2">
+      <c r="A2" s="2" t="n">
         <v>43121</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="1" t="n">
         <v>250</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1421,11 +1204,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1">
-      <c r="A3" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="3">
+      <c r="A3" s="2" t="n">
         <v>43122</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="1" t="n">
         <v>305</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1435,11 +1218,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1">
-      <c r="A4" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="4">
+      <c r="A4" s="2" t="n">
         <v>43122</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1449,11 +1232,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1">
-      <c r="A5" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="5">
+      <c r="A5" s="2" t="n">
         <v>43125</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="1" t="n">
         <v>98</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1463,11 +1246,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1">
-      <c r="A6" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="6">
+      <c r="A6" s="2" t="n">
         <v>43126</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1477,11 +1260,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1">
-      <c r="A7" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="7">
+      <c r="A7" s="2" t="n">
         <v>43127</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1491,11 +1274,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1">
-      <c r="A8" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="8">
+      <c r="A8" s="2" t="n">
         <v>43128</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="1" t="n">
         <v>656</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1505,11 +1288,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1">
-      <c r="A9" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="9">
+      <c r="A9" s="2" t="n">
         <v>43131</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="1" t="n">
         <v>486</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1519,11 +1302,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1">
-      <c r="A10" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="10">
+      <c r="A10" s="2" t="n">
         <v>43132</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="1" t="n">
         <v>76</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1533,11 +1316,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1">
-      <c r="A11" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="11">
+      <c r="A11" s="2" t="n">
         <v>43133</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="1" t="n">
         <v>399</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1547,11 +1330,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1">
-      <c r="A12" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="12">
+      <c r="A12" s="2" t="n">
         <v>43135</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="1" t="n">
         <v>419</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1561,11 +1344,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1">
-      <c r="A13" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="13">
+      <c r="A13" s="2" t="n">
         <v>43136</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="1" t="n">
         <v>521</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1575,11 +1358,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1">
-      <c r="A14" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="14">
+      <c r="A14" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="1" t="n">
         <v>399</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1589,11 +1372,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1">
-      <c r="A15" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="15">
+      <c r="A15" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="1" t="n">
         <v>138</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1603,11 +1386,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1">
-      <c r="A16" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="16">
+      <c r="A16" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="1" t="n">
         <v>310</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1617,12 +1400,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1">
-      <c r="A17" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="17">
+      <c r="A17" s="2" t="n">
         <v>43138</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="1">
+      <c r="C17" s="1" t="n">
         <v>700</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1632,12 +1415,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1">
-      <c r="A18" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="18">
+      <c r="A18" s="2" t="n">
         <v>43141</v>
       </c>
-      <c r="C18" s="1">
-        <f>F18*G18</f>
+      <c r="C18" s="1" t="n">
+        <f aca="false">F18*G18</f>
         <v>1312</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -1646,18 +1429,18 @@
       <c r="E18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="1" t="n">
         <v>164</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="1" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1">
-      <c r="A19" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="19">
+      <c r="A19" s="2" t="n">
         <v>43141</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="1" t="n">
         <v>1190</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1667,11 +1450,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1">
-      <c r="A20" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="20">
+      <c r="A20" s="2" t="n">
         <v>43154</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="1" t="n">
         <v>438</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1681,11 +1464,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1">
-      <c r="A21" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="21">
+      <c r="A21" s="2" t="n">
         <v>43154</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="1" t="n">
         <v>248</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -1695,22 +1478,22 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1">
-      <c r="A22" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="22">
+      <c r="A22" s="2" t="n">
         <v>43166</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="1" t="n">
         <v>234</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1">
-      <c r="A23" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="23">
+      <c r="A23" s="2" t="n">
         <v>43171</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="1" t="n">
         <v>118</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1720,22 +1503,22 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1">
-      <c r="A24" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="24">
+      <c r="A24" s="2" t="n">
         <v>43173</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="1" t="n">
         <v>82</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1">
-      <c r="A25" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="25">
+      <c r="A25" s="2" t="n">
         <v>43174</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1745,22 +1528,22 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1">
-      <c r="A26" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="26">
+      <c r="A26" s="2" t="n">
         <v>43175</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="1" t="n">
         <v>370</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:7" hidden="1">
-      <c r="A27" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="27">
+      <c r="A27" s="2" t="n">
         <v>43175</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -1770,11 +1553,11 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1">
-      <c r="A28" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="28">
+      <c r="A28" s="2" t="n">
         <v>43176</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="1" t="n">
         <v>624</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -1784,11 +1567,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1">
-      <c r="A29" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="29">
+      <c r="A29" s="2" t="n">
         <v>43177</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="1" t="n">
         <v>170</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1798,22 +1581,22 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1">
-      <c r="A30" s="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="30">
+      <c r="A30" s="4" t="n">
         <v>43179</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1">
-      <c r="A31" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="31">
+      <c r="A31" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="1" t="n">
         <v>90</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -1823,11 +1606,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1">
-      <c r="A32" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="32">
+      <c r="A32" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="1" t="n">
         <v>72</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -1837,11 +1620,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:26" hidden="1">
-      <c r="A33" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="33">
+      <c r="A33" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="1" t="n">
         <v>908</v>
       </c>
       <c r="D33" s="6" t="s">
@@ -1851,11 +1634,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:26" hidden="1">
-      <c r="A34" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="34">
+      <c r="A34" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -1865,11 +1648,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:26" hidden="1">
-      <c r="A35" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="35">
+      <c r="A35" s="2" t="n">
         <v>43181</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -1879,11 +1662,11 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:26" hidden="1">
-      <c r="A36" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="36">
+      <c r="A36" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="1" t="n">
         <v>135</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -1893,11 +1676,11 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:26" hidden="1">
-      <c r="A37" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="37">
+      <c r="A37" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="1" t="n">
         <v>110</v>
       </c>
       <c r="C37" s="1"/>
@@ -1929,11 +1712,11 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38" spans="1:26" hidden="1">
-      <c r="A38" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="38">
+      <c r="A38" s="2" t="n">
         <v>43185</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="1" t="n">
         <v>122</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -1943,22 +1726,22 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:26" hidden="1">
-      <c r="A39" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="39">
+      <c r="A39" s="2" t="n">
         <v>43187</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="1" t="n">
         <v>750</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:26" hidden="1">
-      <c r="A40" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="40">
+      <c r="A40" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="1" t="n">
         <v>379</v>
       </c>
       <c r="D40" s="6" t="s">
@@ -1968,22 +1751,22 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:26" hidden="1">
-      <c r="A41" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="41">
+      <c r="A41" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="1" t="n">
         <v>240</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:26" hidden="1">
-      <c r="A42" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="42">
+      <c r="A42" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="1" t="n">
         <v>540</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -1993,11 +1776,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:26" hidden="1">
-      <c r="A43" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="43">
+      <c r="A43" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -2007,11 +1790,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:26" hidden="1">
-      <c r="A44" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="44">
+      <c r="A44" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -2021,11 +1804,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:26" hidden="1">
-      <c r="A45" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="45">
+      <c r="A45" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="1" t="n">
         <v>462</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -2035,11 +1818,11 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:26" hidden="1">
-      <c r="A46" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="46">
+      <c r="A46" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46" s="1" t="n">
         <v>70</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -2049,11 +1832,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:26" hidden="1">
-      <c r="A47" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="47">
+      <c r="A47" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -2063,11 +1846,11 @@
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="1:26" hidden="1">
-      <c r="A48" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="48">
+      <c r="A48" s="2" t="n">
         <v>43190</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="1" t="n">
         <v>30</v>
       </c>
       <c r="C48" s="1"/>
@@ -2078,11 +1861,11 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1">
-      <c r="A49" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="49">
+      <c r="A49" s="2" t="n">
         <v>43191</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="1" t="n">
         <v>40</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -2092,11 +1875,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1">
-      <c r="A50" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="50">
+      <c r="A50" s="7" t="n">
         <v>43193</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50" s="1" t="n">
         <v>150</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -2106,11 +1889,11 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1">
-      <c r="A51" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="51">
+      <c r="A51" s="2" t="n">
         <v>43194</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51" s="1" t="n">
         <v>1360</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -2120,11 +1903,11 @@
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1">
-      <c r="A52" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="52">
+      <c r="A52" s="2" t="n">
         <v>43195</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" s="1" t="n">
         <v>94</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -2134,11 +1917,11 @@
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1">
-      <c r="A53" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="53">
+      <c r="A53" s="2" t="n">
         <v>43196</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C53" s="1" t="n">
         <v>48</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -2148,11 +1931,11 @@
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1">
-      <c r="A54" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="54">
+      <c r="A54" s="2" t="n">
         <v>43196</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C54" s="1" t="n">
         <v>205</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -2162,11 +1945,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1">
-      <c r="A55" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="55">
+      <c r="A55" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -2176,11 +1959,11 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1">
-      <c r="A56" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="56">
+      <c r="A56" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56" s="1" t="n">
         <v>421</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -2190,11 +1973,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1">
-      <c r="A57" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="57">
+      <c r="A57" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="1" t="n">
         <v>191</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -2204,11 +1987,11 @@
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1">
-      <c r="A58" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="58">
+      <c r="A58" s="2" t="n">
         <v>43198</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58" s="1" t="n">
         <v>226</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -2218,22 +2001,22 @@
         <v>96</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1">
-      <c r="A59" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="59">
+      <c r="A59" s="2" t="n">
         <v>43200</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59" s="1" t="n">
         <v>250</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1">
-      <c r="A60" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="60">
+      <c r="A60" s="2" t="n">
         <v>43200</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60" s="1" t="n">
         <v>1115</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -2243,11 +2026,11 @@
         <v>99</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1">
-      <c r="A61" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="61">
+      <c r="A61" s="2" t="n">
         <v>43201</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -2257,11 +2040,11 @@
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1">
-      <c r="A62" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="62">
+      <c r="A62" s="2" t="n">
         <v>43201</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62" s="1" t="n">
         <v>88</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -2271,11 +2054,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1">
-      <c r="A63" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="63">
+      <c r="A63" s="2" t="n">
         <v>43203</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -2285,11 +2068,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1">
-      <c r="A64" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="64">
+      <c r="A64" s="2" t="n">
         <v>43203</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C64" s="1" t="n">
         <v>364</v>
       </c>
       <c r="D64" s="1" t="s">
@@ -2299,11 +2082,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1">
-      <c r="A65" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="65">
+      <c r="A65" s="2" t="n">
         <v>43204</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65" s="1" t="n">
         <v>65</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -2313,11 +2096,11 @@
         <v>105</v>
       </c>
     </row>
-    <row r="66" spans="1:5" hidden="1">
-      <c r="A66" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="66">
+      <c r="A66" s="2" t="n">
         <v>43208</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -2327,11 +2110,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1">
-      <c r="A67" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="67">
+      <c r="A67" s="2" t="n">
         <v>43208</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C67" s="1" t="n">
         <v>470</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -2341,11 +2124,11 @@
         <v>107</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1">
-      <c r="A68" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="68">
+      <c r="A68" s="2" t="n">
         <v>43209</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68" s="1" t="n">
         <v>180</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -2355,11 +2138,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1">
-      <c r="A69" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="69">
+      <c r="A69" s="2" t="n">
         <v>43210</v>
       </c>
-      <c r="C69" s="1">
+      <c r="C69" s="1" t="n">
         <v>420</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -2369,11 +2152,11 @@
         <v>109</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1">
-      <c r="A70" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="70">
+      <c r="A70" s="2" t="n">
         <v>43212</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70" s="1" t="n">
         <v>50</v>
       </c>
       <c r="D70" s="1" t="s">
@@ -2383,11 +2166,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1">
-      <c r="A71" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="71">
+      <c r="A71" s="2" t="n">
         <v>43212</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71" s="1" t="n">
         <v>164</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -2397,11 +2180,11 @@
         <v>112</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1">
-      <c r="A72" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="72">
+      <c r="A72" s="2" t="n">
         <v>43215</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B72" s="1" t="n">
         <v>300</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -2411,11 +2194,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1">
-      <c r="A73" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="73">
+      <c r="A73" s="2" t="n">
         <v>43217</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73" s="1" t="n">
         <v>364</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -2425,11 +2208,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1">
-      <c r="A74" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="74">
+      <c r="A74" s="2" t="n">
         <v>43218</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74" s="1" t="n">
         <v>185</v>
       </c>
       <c r="D74" s="1" t="s">
@@ -2439,11 +2222,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1">
-      <c r="A75" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="75">
+      <c r="A75" s="2" t="n">
         <v>43218</v>
       </c>
-      <c r="C75" s="1">
+      <c r="C75" s="1" t="n">
         <v>404</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -2453,11 +2236,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="76" spans="1:5" hidden="1">
-      <c r="A76" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="76">
+      <c r="A76" s="2" t="n">
         <v>43220</v>
       </c>
-      <c r="C76" s="1">
+      <c r="C76" s="1" t="n">
         <v>57</v>
       </c>
       <c r="D76" s="1" t="s">
@@ -2467,11 +2250,11 @@
         <v>114</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1">
-      <c r="A77" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="77">
+      <c r="A77" s="2" t="n">
         <v>43221</v>
       </c>
-      <c r="C77" s="1">
+      <c r="C77" s="1" t="n">
         <v>282</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -2481,11 +2264,11 @@
         <v>116</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1">
-      <c r="A78" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="78">
+      <c r="A78" s="2" t="n">
         <v>43220</v>
       </c>
-      <c r="C78" s="1">
+      <c r="C78" s="1" t="n">
         <v>87</v>
       </c>
       <c r="D78" s="1" t="s">
@@ -2495,11 +2278,11 @@
         <v>117</v>
       </c>
     </row>
-    <row r="79" spans="1:5" hidden="1">
-      <c r="A79" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="79">
+      <c r="A79" s="2" t="n">
         <v>43223</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B79" s="1" t="n">
         <v>1878</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -2509,11 +2292,11 @@
         <v>119</v>
       </c>
     </row>
-    <row r="80" spans="1:5" hidden="1">
-      <c r="A80" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="80">
+      <c r="A80" s="2" t="n">
         <v>43224</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B80" s="1" t="n">
         <v>98</v>
       </c>
       <c r="D80" s="1" t="s">
@@ -2523,11 +2306,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="81" spans="1:5" hidden="1">
-      <c r="A81" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="81">
+      <c r="A81" s="2" t="n">
         <v>43225</v>
       </c>
-      <c r="C81" s="1">
+      <c r="C81" s="1" t="n">
         <v>198</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -2537,11 +2320,11 @@
         <v>122</v>
       </c>
     </row>
-    <row r="82" spans="1:5" hidden="1">
-      <c r="A82" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="82">
+      <c r="A82" s="2" t="n">
         <v>43225</v>
       </c>
-      <c r="C82" s="1">
+      <c r="C82" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -2551,11 +2334,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="83" spans="1:5" hidden="1">
-      <c r="A83" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="83">
+      <c r="A83" s="2" t="n">
         <v>43228</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83" s="1" t="n">
         <v>168</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -2565,11 +2348,11 @@
         <v>124</v>
       </c>
     </row>
-    <row r="84" spans="1:5" hidden="1">
-      <c r="A84" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="84">
+      <c r="A84" s="2" t="n">
         <v>43229</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B84" s="1" t="n">
         <v>240</v>
       </c>
       <c r="D84" s="1" t="s">
@@ -2579,12 +2362,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:5" hidden="1">
-      <c r="A85" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="85">
+      <c r="A85" s="2" t="n">
         <v>43230</v>
       </c>
       <c r="B85" s="1"/>
-      <c r="C85" s="1">
+      <c r="C85" s="1" t="n">
         <v>420</v>
       </c>
       <c r="D85" s="1" t="s">
@@ -2594,11 +2377,11 @@
         <v>126</v>
       </c>
     </row>
-    <row r="86" spans="1:5" hidden="1">
-      <c r="A86" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="86">
+      <c r="A86" s="2" t="n">
         <v>43230</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B86" s="1" t="n">
         <v>200</v>
       </c>
       <c r="C86" s="1"/>
@@ -2609,11 +2392,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="87" spans="1:5" hidden="1">
-      <c r="A87" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="87">
+      <c r="A87" s="2" t="n">
         <v>43230</v>
       </c>
-      <c r="C87" s="1">
+      <c r="C87" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D87" s="1" t="s">
@@ -2623,11 +2406,11 @@
         <v>128</v>
       </c>
     </row>
-    <row r="88" spans="1:5" hidden="1">
-      <c r="A88" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="88">
+      <c r="A88" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B88" s="1" t="n">
         <v>462</v>
       </c>
       <c r="D88" s="1" t="s">
@@ -2637,11 +2420,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="89" spans="1:5" hidden="1">
-      <c r="A89" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="89">
+      <c r="A89" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B89" s="1" t="n">
         <v>499</v>
       </c>
       <c r="D89" s="1" t="s">
@@ -2651,11 +2434,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="90" spans="1:5" hidden="1">
-      <c r="A90" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="90">
+      <c r="A90" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B90" s="1">
+      <c r="B90" s="1" t="n">
         <v>398</v>
       </c>
       <c r="D90" s="1" t="s">
@@ -2665,11 +2448,11 @@
         <v>133</v>
       </c>
     </row>
-    <row r="91" spans="1:5" hidden="1">
-      <c r="A91" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="91">
+      <c r="A91" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B91" s="1">
+      <c r="B91" s="1" t="n">
         <v>226</v>
       </c>
       <c r="D91" s="1" t="s">
@@ -2679,11 +2462,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="92" spans="1:5" hidden="1">
-      <c r="A92" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="92">
+      <c r="A92" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B92" s="1">
+      <c r="B92" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D92" s="1" t="s">
@@ -2693,11 +2476,11 @@
         <v>137</v>
       </c>
     </row>
-    <row r="93" spans="1:5" hidden="1">
-      <c r="A93" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="93">
+      <c r="A93" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="B93" s="1">
+      <c r="B93" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D93" s="1" t="s">
@@ -2707,11 +2490,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="94" spans="1:5" hidden="1">
-      <c r="A94" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="94">
+      <c r="A94" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="C94" s="1">
+      <c r="C94" s="1" t="n">
         <v>340</v>
       </c>
       <c r="D94" s="1" t="s">
@@ -2721,11 +2504,11 @@
         <v>139</v>
       </c>
     </row>
-    <row r="95" spans="1:5" hidden="1">
-      <c r="A95" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="95">
+      <c r="A95" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="B95" s="1">
+      <c r="B95" s="1" t="n">
         <v>510</v>
       </c>
       <c r="D95" s="1" t="s">
@@ -2735,11 +2518,11 @@
         <v>141</v>
       </c>
     </row>
-    <row r="96" spans="1:5" hidden="1">
-      <c r="A96" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="96">
+      <c r="A96" s="2" t="n">
         <v>43233</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B96" s="1" t="n">
         <v>170</v>
       </c>
       <c r="D96" s="1" t="s">
@@ -2749,11 +2532,11 @@
         <v>143</v>
       </c>
     </row>
-    <row r="97" spans="1:5" hidden="1">
-      <c r="A97" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="97">
+      <c r="A97" s="2" t="n">
         <v>43233</v>
       </c>
-      <c r="C97" s="1">
+      <c r="C97" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D97" s="1" t="s">
@@ -2763,11 +2546,11 @@
         <v>144</v>
       </c>
     </row>
-    <row r="98" spans="1:5" hidden="1">
-      <c r="A98" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="98">
+      <c r="A98" s="2" t="n">
         <v>43234</v>
       </c>
-      <c r="C98" s="1">
+      <c r="C98" s="1" t="n">
         <v>299</v>
       </c>
       <c r="D98" s="1" t="s">
@@ -2777,11 +2560,11 @@
         <v>145</v>
       </c>
     </row>
-    <row r="99" spans="1:5" hidden="1">
-      <c r="A99" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="99">
+      <c r="A99" s="2" t="n">
         <v>43236</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99" s="1" t="n">
         <v>3659</v>
       </c>
       <c r="D99" s="1" t="s">
@@ -2791,11 +2574,11 @@
         <v>146</v>
       </c>
     </row>
-    <row r="100" spans="1:5" hidden="1">
-      <c r="A100" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="100">
+      <c r="A100" s="2" t="n">
         <v>43237</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B100" s="1" t="n">
         <v>79</v>
       </c>
       <c r="D100" s="1" t="s">
@@ -2805,11 +2588,11 @@
         <v>147</v>
       </c>
     </row>
-    <row r="101" spans="1:5" hidden="1">
-      <c r="A101" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="101">
+      <c r="A101" s="2" t="n">
         <v>43236</v>
       </c>
-      <c r="C101" s="1">
+      <c r="C101" s="1" t="n">
         <v>173</v>
       </c>
       <c r="D101" s="1" t="s">
@@ -2819,11 +2602,11 @@
         <v>148</v>
       </c>
     </row>
-    <row r="102" spans="1:5" hidden="1">
-      <c r="A102" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="102">
+      <c r="A102" s="2" t="n">
         <v>43240</v>
       </c>
-      <c r="B102" s="1">
+      <c r="B102" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D102" s="1" t="s">
@@ -2833,22 +2616,22 @@
         <v>149</v>
       </c>
     </row>
-    <row r="103" spans="1:5" hidden="1">
-      <c r="A103" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="103">
+      <c r="A103" s="2" t="n">
         <v>43240</v>
       </c>
-      <c r="B103" s="1">
+      <c r="B103" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="104" spans="1:5" hidden="1">
-      <c r="A104" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="104">
+      <c r="A104" s="2" t="n">
         <v>43241</v>
       </c>
-      <c r="B104" s="1">
+      <c r="B104" s="1" t="n">
         <v>4070</v>
       </c>
       <c r="D104" s="1" t="s">
@@ -2858,11 +2641,11 @@
         <v>150</v>
       </c>
     </row>
-    <row r="105" spans="1:5" hidden="1">
-      <c r="A105" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="105">
+      <c r="A105" s="2" t="n">
         <v>43241</v>
       </c>
-      <c r="C105" s="1">
+      <c r="C105" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D105" s="1" t="s">
@@ -2872,11 +2655,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="106" spans="1:5" hidden="1">
-      <c r="A106" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="106">
+      <c r="A106" s="2" t="n">
         <v>43242</v>
       </c>
-      <c r="B106" s="1">
+      <c r="B106" s="1" t="n">
         <v>79</v>
       </c>
       <c r="D106" s="1" t="s">
@@ -2886,11 +2669,11 @@
         <v>152</v>
       </c>
     </row>
-    <row r="107" spans="1:5" hidden="1">
-      <c r="A107" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="107">
+      <c r="A107" s="2" t="n">
         <v>43246</v>
       </c>
-      <c r="B107" s="1">
+      <c r="B107" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D107" s="1" t="s">
@@ -2900,11 +2683,11 @@
         <v>154</v>
       </c>
     </row>
-    <row r="108" spans="1:5" hidden="1">
-      <c r="A108" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="108">
+      <c r="A108" s="2" t="n">
         <v>43247</v>
       </c>
-      <c r="B108" s="1">
+      <c r="B108" s="1" t="n">
         <v>70</v>
       </c>
       <c r="D108" s="1" t="s">
@@ -2914,44 +2697,44 @@
         <v>156</v>
       </c>
     </row>
-    <row r="109" spans="1:5" hidden="1">
-      <c r="A109" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="109">
+      <c r="A109" s="2" t="n">
         <v>43253</v>
       </c>
-      <c r="B109" s="1">
+      <c r="B109" s="1" t="n">
         <v>142</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="110" spans="1:5" hidden="1">
-      <c r="A110" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="110">
+      <c r="A110" s="2" t="n">
         <v>43254</v>
       </c>
-      <c r="B110" s="1">
+      <c r="B110" s="1" t="n">
         <v>90</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="111" spans="1:5" hidden="1">
-      <c r="A111" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="111">
+      <c r="A111" s="2" t="n">
         <v>43260</v>
       </c>
-      <c r="C111" s="1">
+      <c r="C111" s="1" t="n">
         <v>1400</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="112" spans="1:5" hidden="1">
-      <c r="A112" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="112">
+      <c r="A112" s="2" t="n">
         <v>43260</v>
       </c>
-      <c r="C112" s="1">
+      <c r="C112" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D112" s="1" t="s">
@@ -2961,33 +2744,33 @@
         <v>91</v>
       </c>
     </row>
-    <row r="113" spans="1:5" hidden="1">
-      <c r="A113" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="113">
+      <c r="A113" s="2" t="n">
         <v>43264</v>
       </c>
-      <c r="B113" s="1">
+      <c r="B113" s="1" t="n">
         <v>546</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="114" spans="1:5" hidden="1">
-      <c r="A114" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="114">
+      <c r="A114" s="2" t="n">
         <v>43264</v>
       </c>
-      <c r="B114" s="1">
+      <c r="B114" s="1" t="n">
         <v>95</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="115" spans="1:5" hidden="1">
-      <c r="A115" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="115">
+      <c r="A115" s="2" t="n">
         <v>43266</v>
       </c>
-      <c r="B115" s="1">
+      <c r="B115" s="1" t="n">
         <v>394</v>
       </c>
       <c r="D115" s="1" t="s">
@@ -2997,11 +2780,11 @@
         <v>163</v>
       </c>
     </row>
-    <row r="116" spans="1:5" hidden="1">
-      <c r="A116" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="116">
+      <c r="A116" s="2" t="n">
         <v>43266</v>
       </c>
-      <c r="B116" s="1">
+      <c r="B116" s="1" t="n">
         <v>1055</v>
       </c>
       <c r="D116" s="1" t="s">
@@ -3011,11 +2794,11 @@
         <v>165</v>
       </c>
     </row>
-    <row r="117" spans="1:5" hidden="1">
-      <c r="A117" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="117">
+      <c r="A117" s="2" t="n">
         <v>43284</v>
       </c>
-      <c r="C117" s="1">
+      <c r="C117" s="1" t="n">
         <v>274</v>
       </c>
       <c r="D117" s="1" t="s">
@@ -3025,11 +2808,11 @@
         <v>167</v>
       </c>
     </row>
-    <row r="118" spans="1:5" hidden="1">
-      <c r="A118" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="118">
+      <c r="A118" s="2" t="n">
         <v>43283</v>
       </c>
-      <c r="C118" s="1">
+      <c r="C118" s="1" t="n">
         <v>105</v>
       </c>
       <c r="D118" s="1" t="s">
@@ -3039,11 +2822,11 @@
         <v>169</v>
       </c>
     </row>
-    <row r="119" spans="1:5" hidden="1">
-      <c r="A119" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="119">
+      <c r="A119" s="2" t="n">
         <v>43289</v>
       </c>
-      <c r="C119" s="1">
+      <c r="C119" s="1" t="n">
         <v>128</v>
       </c>
       <c r="D119" s="1" t="s">
@@ -3053,11 +2836,11 @@
         <v>171</v>
       </c>
     </row>
-    <row r="120" spans="1:5" hidden="1">
-      <c r="A120" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="120">
+      <c r="A120" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C120" s="1">
+      <c r="C120" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D120" s="1" t="s">
@@ -3067,11 +2850,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="121" spans="1:5" hidden="1">
-      <c r="A121" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="121">
+      <c r="A121" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C121" s="1">
+      <c r="C121" s="1" t="n">
         <v>210</v>
       </c>
       <c r="D121" s="1" t="s">
@@ -3081,44 +2864,44 @@
         <v>173</v>
       </c>
     </row>
-    <row r="122" spans="1:5" hidden="1">
-      <c r="A122" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="122">
+      <c r="A122" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B122" s="1">
+      <c r="B122" s="1" t="n">
         <v>980</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="123" spans="1:5" hidden="1">
-      <c r="A123" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="123">
+      <c r="A123" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B123" s="1">
+      <c r="B123" s="1" t="n">
         <v>1260</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="124" spans="1:5" hidden="1">
-      <c r="A124" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="124">
+      <c r="A124" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B124" s="1">
+      <c r="B124" s="1" t="n">
         <v>3687</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="125" spans="1:5" hidden="1">
-      <c r="A125" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="125">
+      <c r="A125" s="2" t="n">
         <v>43298</v>
       </c>
-      <c r="C125" s="1">
+      <c r="C125" s="1" t="n">
         <v>60</v>
       </c>
       <c r="D125" s="1" t="s">
@@ -3128,55 +2911,55 @@
         <v>178</v>
       </c>
     </row>
-    <row r="126" spans="1:5" hidden="1">
-      <c r="A126" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="126">
+      <c r="A126" s="2" t="n">
         <v>43291</v>
       </c>
-      <c r="C126" s="1">
+      <c r="C126" s="1" t="n">
         <v>404</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="127" spans="1:5" hidden="1">
-      <c r="A127" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="127">
+      <c r="A127" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C127" s="1">
+      <c r="C127" s="1" t="n">
         <v>451</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="128" spans="1:5" hidden="1">
-      <c r="A128" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="128">
+      <c r="A128" s="2" t="n">
         <v>43298</v>
       </c>
-      <c r="C128" s="1">
+      <c r="C128" s="1" t="n">
         <v>708</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="129" spans="1:5" hidden="1">
-      <c r="A129" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="129">
+      <c r="A129" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C129" s="1">
+      <c r="C129" s="1" t="n">
         <v>160</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="130" spans="1:5" hidden="1">
-      <c r="A130" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="130">
+      <c r="A130" s="2" t="n">
         <v>43288</v>
       </c>
-      <c r="C130" s="1">
+      <c r="C130" s="1" t="n">
         <v>72</v>
       </c>
       <c r="D130" s="1" t="s">
@@ -3186,11 +2969,11 @@
         <v>181</v>
       </c>
     </row>
-    <row r="131" spans="1:5" hidden="1">
-      <c r="A131" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="131">
+      <c r="A131" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C131" s="1">
+      <c r="C131" s="1" t="n">
         <v>300</v>
       </c>
       <c r="D131" s="1" t="s">
@@ -3200,11 +2983,11 @@
         <v>183</v>
       </c>
     </row>
-    <row r="132" spans="1:5" hidden="1">
-      <c r="A132" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="132">
+      <c r="A132" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C132" s="1">
+      <c r="C132" s="1" t="n">
         <v>230</v>
       </c>
       <c r="D132" s="1" t="s">
@@ -3214,22 +2997,22 @@
         <v>185</v>
       </c>
     </row>
-    <row r="133" spans="1:5" hidden="1">
-      <c r="A133" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="133">
+      <c r="A133" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C133" s="1">
+      <c r="C133" s="1" t="n">
         <v>454</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="134" spans="1:5" hidden="1">
-      <c r="A134" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="134">
+      <c r="A134" s="2" t="n">
         <v>43299</v>
       </c>
-      <c r="C134" s="1">
+      <c r="C134" s="1" t="n">
         <v>686</v>
       </c>
       <c r="D134" s="1" t="s">
@@ -3239,11 +3022,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="135" spans="1:5" hidden="1">
-      <c r="A135" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="135">
+      <c r="A135" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C135" s="1">
+      <c r="C135" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D135" s="1" t="s">
@@ -3253,11 +3036,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="136" spans="1:5" hidden="1">
-      <c r="A136" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="136">
+      <c r="A136" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C136" s="1">
+      <c r="C136" s="1" t="n">
         <v>2067</v>
       </c>
       <c r="D136" s="1" t="s">
@@ -3267,11 +3050,11 @@
         <v>186</v>
       </c>
     </row>
-    <row r="137" spans="1:5" hidden="1">
-      <c r="A137" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="137">
+      <c r="A137" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B137" s="1">
+      <c r="B137" s="1" t="n">
         <v>109</v>
       </c>
       <c r="D137" s="1" t="s">
@@ -3281,11 +3064,11 @@
         <v>187</v>
       </c>
     </row>
-    <row r="138" spans="1:5" hidden="1">
-      <c r="A138" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="138">
+      <c r="A138" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B138" s="1">
+      <c r="B138" s="1" t="n">
         <v>97</v>
       </c>
       <c r="D138" s="1" t="s">
@@ -3295,11 +3078,11 @@
         <v>188</v>
       </c>
     </row>
-    <row r="139" spans="1:5" hidden="1">
-      <c r="A139" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="139">
+      <c r="A139" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B139" s="1">
+      <c r="B139" s="1" t="n">
         <v>1437</v>
       </c>
       <c r="D139" s="1" t="s">
@@ -3309,11 +3092,11 @@
         <v>189</v>
       </c>
     </row>
-    <row r="140" spans="1:5" hidden="1">
-      <c r="A140" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="140">
+      <c r="A140" s="2" t="n">
         <v>43306</v>
       </c>
-      <c r="C140" s="1">
+      <c r="C140" s="1" t="n">
         <v>650</v>
       </c>
       <c r="D140" s="1" t="s">
@@ -3323,11 +3106,11 @@
         <v>190</v>
       </c>
     </row>
-    <row r="141" spans="1:5" hidden="1">
-      <c r="A141" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="141">
+      <c r="A141" s="2" t="n">
         <v>43305</v>
       </c>
-      <c r="C141" s="1">
+      <c r="C141" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D141" s="1" t="s">
@@ -3337,11 +3120,11 @@
         <v>191</v>
       </c>
     </row>
-    <row r="142" spans="1:5" hidden="1">
-      <c r="A142" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="142">
+      <c r="A142" s="2" t="n">
         <v>43309</v>
       </c>
-      <c r="C142" s="1">
+      <c r="C142" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D142" s="1" t="s">
@@ -3351,11 +3134,11 @@
         <v>192</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="14" hidden="1">
-      <c r="A143" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="0" r="143">
+      <c r="A143" s="2" t="n">
         <v>43306</v>
       </c>
-      <c r="B143" s="1">
+      <c r="B143" s="1" t="n">
         <v>167</v>
       </c>
       <c r="D143" s="1" t="s">
@@ -3365,11 +3148,11 @@
         <v>193</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="14" hidden="1">
-      <c r="A144" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="0" r="144">
+      <c r="A144" s="2" t="n">
         <v>43304</v>
       </c>
-      <c r="C144" s="1">
+      <c r="C144" s="1" t="n">
         <v>93</v>
       </c>
       <c r="D144" s="1" t="s">
@@ -3379,11 +3162,11 @@
         <v>194</v>
       </c>
     </row>
-    <row r="145" spans="1:5" hidden="1">
-      <c r="A145" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="145">
+      <c r="A145" s="2" t="n">
         <v>43305</v>
       </c>
-      <c r="C145" s="1">
+      <c r="C145" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D145" s="1" t="s">
@@ -3393,11 +3176,11 @@
         <v>195</v>
       </c>
     </row>
-    <row r="146" spans="1:5" hidden="1">
-      <c r="A146" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="146">
+      <c r="A146" s="2" t="n">
         <v>43303</v>
       </c>
-      <c r="C146" s="1">
+      <c r="C146" s="1" t="n">
         <v>244</v>
       </c>
       <c r="D146" s="1" t="s">
@@ -3407,11 +3190,11 @@
         <v>196</v>
       </c>
     </row>
-    <row r="147" spans="1:5" hidden="1">
-      <c r="A147" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="147">
+      <c r="A147" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C147" s="1">
+      <c r="C147" s="1" t="n">
         <v>482</v>
       </c>
       <c r="D147" s="1" t="s">
@@ -3421,11 +3204,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="148" spans="1:5" hidden="1">
-      <c r="A148" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="148">
+      <c r="A148" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C148" s="1">
+      <c r="C148" s="1" t="n">
         <v>172</v>
       </c>
       <c r="D148" s="1" t="s">
@@ -3435,44 +3218,44 @@
         <v>199</v>
       </c>
     </row>
-    <row r="149" spans="1:5" hidden="1">
-      <c r="A149" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="149">
+      <c r="A149" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="B149" s="1">
+      <c r="B149" s="1" t="n">
         <v>89</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="150" spans="1:5" hidden="1">
-      <c r="A150" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="150">
+      <c r="A150" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="C150" s="1">
+      <c r="C150" s="1" t="n">
         <v>107</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="151" spans="1:5" hidden="1">
-      <c r="A151" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="151">
+      <c r="A151" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="C151" s="1">
+      <c r="C151" s="1" t="n">
         <v>124</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="152" spans="1:5" hidden="1">
-      <c r="A152" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="152">
+      <c r="A152" s="7" t="n">
         <v>43316</v>
       </c>
-      <c r="C152" s="1">
+      <c r="C152" s="1" t="n">
         <v>4500</v>
       </c>
       <c r="D152" s="1" t="s">
@@ -3482,11 +3265,11 @@
         <v>202</v>
       </c>
     </row>
-    <row r="153" spans="1:5" hidden="1">
-      <c r="A153" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="153">
+      <c r="A153" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C153" s="1">
+      <c r="C153" s="1" t="n">
         <v>247</v>
       </c>
       <c r="D153" s="1" t="s">
@@ -3496,11 +3279,11 @@
         <v>204</v>
       </c>
     </row>
-    <row r="154" spans="1:5" hidden="1">
-      <c r="A154" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="154">
+      <c r="A154" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C154" s="1">
+      <c r="C154" s="1" t="n">
         <v>1150</v>
       </c>
       <c r="D154" s="1" t="s">
@@ -3510,11 +3293,11 @@
         <v>205</v>
       </c>
     </row>
-    <row r="155" spans="1:5" hidden="1">
-      <c r="A155" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="155">
+      <c r="A155" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C155" s="1">
+      <c r="C155" s="1" t="n">
         <v>313</v>
       </c>
       <c r="D155" s="1" t="s">
@@ -3524,11 +3307,11 @@
         <v>207</v>
       </c>
     </row>
-    <row r="156" spans="1:5" hidden="1">
-      <c r="A156" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="156">
+      <c r="A156" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="B156" s="1">
+      <c r="B156" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D156" s="1" t="s">
@@ -3538,11 +3321,11 @@
         <v>209</v>
       </c>
     </row>
-    <row r="157" spans="1:5" hidden="1">
-      <c r="A157" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="157">
+      <c r="A157" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="C157" s="1">
+      <c r="C157" s="1" t="n">
         <v>710</v>
       </c>
       <c r="D157" s="1" t="s">
@@ -3552,11 +3335,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="158" spans="1:5">
-      <c r="A158" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="158">
+      <c r="A158" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="C158" s="1">
+      <c r="C158" s="1" t="n">
         <v>100</v>
       </c>
       <c r="D158" s="1" t="s">
@@ -3566,11 +3349,11 @@
         <v>212</v>
       </c>
     </row>
-    <row r="159" spans="1:5">
-      <c r="A159" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="159">
+      <c r="A159" s="2" t="n">
         <v>43319</v>
       </c>
-      <c r="B159" s="1">
+      <c r="B159" s="1" t="n">
         <v>78</v>
       </c>
       <c r="D159" s="1" t="s">
@@ -3580,22 +3363,22 @@
         <v>213</v>
       </c>
     </row>
-    <row r="160" spans="1:5">
-      <c r="A160" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="160">
+      <c r="A160" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="B160" s="1">
+      <c r="B160" s="1" t="n">
         <v>1840</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="161" spans="1:5">
-      <c r="A161" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="161">
+      <c r="A161" s="2" t="n">
         <v>43322</v>
       </c>
-      <c r="B161" s="1">
+      <c r="B161" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D161" s="1" t="s">
@@ -3605,11 +3388,11 @@
         <v>216</v>
       </c>
     </row>
-    <row r="162" spans="1:5">
-      <c r="A162" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="162">
+      <c r="A162" s="7" t="n">
         <v>43324</v>
       </c>
-      <c r="C162" s="1">
+      <c r="C162" s="1" t="n">
         <v>230</v>
       </c>
       <c r="D162" s="1" t="s">
@@ -3619,11 +3402,11 @@
         <v>217</v>
       </c>
     </row>
-    <row r="163" spans="1:5">
-      <c r="A163" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="163">
+      <c r="A163" s="7" t="n">
         <v>43326</v>
       </c>
-      <c r="C163" s="1">
+      <c r="C163" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D163" s="1" t="s">
@@ -3633,11 +3416,11 @@
         <v>219</v>
       </c>
     </row>
-    <row r="164" spans="1:5">
-      <c r="A164" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="164">
+      <c r="A164" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="B164" s="1">
+      <c r="B164" s="1" t="n">
         <v>45</v>
       </c>
       <c r="D164" s="1" t="s">
@@ -3647,813 +3430,860 @@
         <v>221</v>
       </c>
     </row>
-    <row r="165" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A165" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="165">
+      <c r="A165" s="10" t="n">
         <v>43327</v>
       </c>
-      <c r="C165">
+      <c r="C165" s="0" t="n">
         <v>486</v>
       </c>
-      <c r="D165" t="s">
+      <c r="D165" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E165" t="s">
+      <c r="E165" s="0" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="166" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A166" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="166">
+      <c r="A166" s="10" t="n">
         <v>43329</v>
       </c>
-      <c r="C166">
+      <c r="C166" s="0" t="n">
         <v>92</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D166" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="E166" t="s">
+      <c r="E166" s="0" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="167" spans="1:5">
-      <c r="A167" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="167">
+      <c r="A167" s="10" t="n">
         <v>43331</v>
       </c>
-      <c r="C167">
+      <c r="C167" s="0" t="n">
         <v>310</v>
       </c>
-      <c r="D167" t="s">
+      <c r="D167" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="E167" t="s">
+      <c r="E167" s="0" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="168" spans="1:5">
-      <c r="A168" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="168">
+      <c r="A168" s="10" t="n">
         <v>43334</v>
       </c>
-      <c r="C168">
+      <c r="C168" s="0" t="n">
         <v>464</v>
       </c>
-      <c r="D168" t="s">
+      <c r="D168" s="0" t="s">
         <v>218</v>
       </c>
       <c r="E168" s="11" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="169" spans="1:5">
-      <c r="A169" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="169">
+      <c r="A169" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="C169">
+      <c r="C169" s="0" t="n">
         <v>726</v>
       </c>
-      <c r="D169" t="s">
+      <c r="D169" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="E169" t="s">
+      <c r="E169" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="170" spans="1:5">
-      <c r="A170" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="170">
+      <c r="A170" s="10" t="n">
         <v>43337</v>
       </c>
-      <c r="C170">
+      <c r="C170" s="0" t="n">
         <v>544</v>
       </c>
-      <c r="D170" t="s">
+      <c r="D170" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E170" t="s">
+      <c r="E170" s="0" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="171" spans="1:5">
-      <c r="A171" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="171">
+      <c r="A171" s="10" t="n">
         <v>43337</v>
       </c>
-      <c r="B171">
+      <c r="B171" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D171" t="s">
+      <c r="D171" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="E171" t="s">
+      <c r="E171" s="0" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="172" spans="1:5">
-      <c r="A172" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="172">
+      <c r="A172" s="10" t="n">
         <v>43341</v>
       </c>
-      <c r="C172">
+      <c r="C172" s="0" t="n">
         <v>830</v>
       </c>
-      <c r="D172" t="s">
+      <c r="D172" s="0" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="173" spans="1:5">
-      <c r="A173" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="173">
+      <c r="A173" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="C173">
+      <c r="C173" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="D173" t="s">
+      <c r="D173" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="E173" t="s">
+      <c r="E173" s="0" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="174" spans="1:5">
-      <c r="A174" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="174">
+      <c r="A174" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="B174">
+      <c r="B174" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D174" t="s">
+      <c r="D174" s="0" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="175" spans="1:5">
-      <c r="A175" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="175">
+      <c r="A175" s="10" t="n">
         <v>43344</v>
       </c>
-      <c r="B175">
+      <c r="B175" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="D175" t="s">
+      <c r="D175" s="0" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="176" spans="1:5">
-      <c r="A176" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="176">
+      <c r="A176" s="10" t="n">
         <v>43344</v>
       </c>
-      <c r="B176">
+      <c r="B176" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D176" t="s">
+      <c r="D176" s="0" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="177" spans="1:5">
-      <c r="A177" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="177">
+      <c r="A177" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C177">
+      <c r="C177" s="0" t="n">
         <v>607</v>
       </c>
-      <c r="D177" t="s">
+      <c r="D177" s="0" t="s">
         <v>235</v>
       </c>
-      <c r="E177" t="s">
+      <c r="E177" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="178" spans="1:5">
-      <c r="A178" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="178">
+      <c r="A178" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C178">
+      <c r="C178" s="0" t="n">
         <v>444</v>
       </c>
-      <c r="D178" t="s">
+      <c r="D178" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E178" t="s">
+      <c r="E178" s="0" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="179" spans="1:5">
-      <c r="A179" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="179">
+      <c r="A179" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C179">
+      <c r="C179" s="0" t="n">
         <v>312</v>
       </c>
-      <c r="D179" t="s">
+      <c r="D179" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="E179" t="s">
+      <c r="E179" s="0" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="180" spans="1:5">
-      <c r="A180" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="180">
+      <c r="A180" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C180">
+      <c r="C180" s="0" t="n">
         <v>501</v>
       </c>
-      <c r="D180" t="s">
+      <c r="D180" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E180" t="s">
+      <c r="E180" s="0" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="181" spans="1:5">
-      <c r="A181" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="181">
+      <c r="A181" s="10" t="n">
         <v>43349</v>
       </c>
-      <c r="C181">
+      <c r="C181" s="0" t="n">
         <v>711</v>
       </c>
-      <c r="D181" t="s">
+      <c r="D181" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="E181" t="s">
+      <c r="E181" s="0" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="182" spans="1:5">
-      <c r="A182" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="182">
+      <c r="A182" s="10" t="n">
         <v>43354</v>
       </c>
-      <c r="B182">
+      <c r="B182" s="0" t="n">
         <v>126</v>
       </c>
-      <c r="D182" t="s">
+      <c r="D182" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="E182" t="s">
+      <c r="E182" s="0" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="183" spans="1:5">
-      <c r="A183" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="183">
+      <c r="A183" s="10" t="n">
         <v>43354</v>
       </c>
-      <c r="C183">
+      <c r="C183" s="0" t="n">
         <v>450</v>
       </c>
-      <c r="D183" t="s">
+      <c r="D183" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="E183" t="s">
+      <c r="E183" s="0" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="184" spans="1:5">
-      <c r="A184" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="184">
+      <c r="A184" s="10" t="n">
         <v>43361</v>
       </c>
-      <c r="C184">
+      <c r="C184" s="0" t="n">
         <v>660</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D184" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="E184" t="s">
+      <c r="E184" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="185" spans="1:5">
-      <c r="A185" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="185">
+      <c r="A185" s="10" t="n">
         <v>43363</v>
       </c>
-      <c r="C185">
+      <c r="C185" s="0" t="n">
         <v>230</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D185" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="E185" t="s">
+      <c r="E185" s="0" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="186" spans="1:5">
-      <c r="A186" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="186">
+      <c r="A186" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B186">
+      <c r="B186" s="0" t="n">
         <v>4859</v>
       </c>
-      <c r="D186" t="s">
+      <c r="D186" s="0" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="187" spans="1:5">
-      <c r="A187" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="187">
+      <c r="A187" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B187">
+      <c r="B187" s="0" t="n">
         <v>295</v>
       </c>
-      <c r="D187" t="s">
+      <c r="D187" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="E187" t="s">
+      <c r="E187" s="0" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="188" spans="1:5">
-      <c r="A188" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="188">
+      <c r="A188" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B188">
+      <c r="B188" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D188" t="s">
+      <c r="D188" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="E188" t="s">
+      <c r="E188" s="0" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="189" spans="1:5">
-      <c r="A189" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="189">
+      <c r="A189" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B189">
+      <c r="B189" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="D189" t="s">
+      <c r="D189" s="0" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="190" spans="1:5">
-      <c r="A190" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="190">
+      <c r="A190" s="10" t="n">
         <v>43378</v>
       </c>
-      <c r="B190">
+      <c r="B190" s="0" t="n">
         <v>506</v>
       </c>
-      <c r="D190" t="s">
+      <c r="D190" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="E190" t="s">
+      <c r="E190" s="0" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="191" spans="1:5">
-      <c r="A191" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="191">
+      <c r="A191" s="10" t="n">
         <v>43379</v>
       </c>
-      <c r="B191">
+      <c r="B191" s="0" t="n">
         <v>350</v>
       </c>
-      <c r="D191" t="s">
+      <c r="D191" s="0" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="192" spans="1:5" ht="20" customHeight="1">
-      <c r="A192" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="20" outlineLevel="0" r="192">
+      <c r="A192" s="10" t="n">
         <v>43383</v>
       </c>
-      <c r="B192">
+      <c r="B192" s="0" t="n">
         <v>189</v>
       </c>
-      <c r="D192" t="s">
+      <c r="D192" s="0" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="193" spans="1:5">
-      <c r="A193" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="193">
+      <c r="A193" s="10" t="n">
         <v>43387</v>
       </c>
-      <c r="B193">
+      <c r="B193" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="D193" t="s">
+      <c r="D193" s="0" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="194" spans="1:5">
-      <c r="A194" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="194">
+      <c r="A194" s="10" t="n">
         <v>43387</v>
       </c>
-      <c r="B194">
+      <c r="B194" s="0" t="n">
         <v>307</v>
       </c>
-      <c r="D194" t="s">
+      <c r="D194" s="0" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="195" spans="1:5">
-      <c r="C195">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="195">
+      <c r="C195" s="0" t="n">
         <v>3705</v>
       </c>
-      <c r="E195" t="s">
+      <c r="E195" s="0" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="196" spans="1:5">
-      <c r="A196" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="196">
+      <c r="A196" s="10" t="n">
         <v>43385</v>
       </c>
-      <c r="C196">
+      <c r="C196" s="0" t="n">
         <v>608</v>
       </c>
-      <c r="D196" t="s">
+      <c r="D196" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E196" t="s">
+      <c r="E196" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="197" spans="1:5">
-      <c r="A197" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="197">
+      <c r="A197" s="10" t="n">
         <v>43391</v>
       </c>
-      <c r="B197">
+      <c r="B197" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="D197" t="s">
+      <c r="D197" s="0" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="198" spans="1:5">
-      <c r="A198" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="198">
+      <c r="A198" s="10" t="n">
         <v>43392</v>
       </c>
-      <c r="B198">
+      <c r="B198" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="D198" t="s">
+      <c r="D198" s="0" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="199" spans="1:5">
-      <c r="A199" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="199">
+      <c r="A199" s="10" t="n">
         <v>43393</v>
       </c>
-      <c r="B199">
+      <c r="B199" s="0" t="n">
         <v>177</v>
       </c>
-      <c r="D199" t="s">
+      <c r="D199" s="0" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="200" spans="1:5">
-      <c r="A200" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="200">
+      <c r="A200" s="10" t="n">
         <v>43393</v>
       </c>
-      <c r="C200">
+      <c r="C200" s="0" t="n">
         <v>125</v>
       </c>
-      <c r="D200" t="s">
+      <c r="D200" s="0" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="201" spans="1:5">
-      <c r="A201" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="201">
+      <c r="A201" s="10" t="n">
         <v>43395</v>
       </c>
-      <c r="B201">
+      <c r="B201" s="0" t="n">
         <v>2800</v>
       </c>
       <c r="D201" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="E201" t="s">
+      <c r="E201" s="0" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="202" spans="1:5">
-      <c r="A202" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="202">
+      <c r="A202" s="10" t="n">
         <v>43395</v>
       </c>
-      <c r="C202">
+      <c r="C202" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="D202" t="s">
+      <c r="D202" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="E202" t="s">
+      <c r="E202" s="0" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="203" spans="1:5">
-      <c r="A203" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="203">
+      <c r="A203" s="10" t="n">
         <v>43396</v>
       </c>
-      <c r="C203">
+      <c r="C203" s="0" t="n">
         <v>692</v>
       </c>
-      <c r="D203" t="s">
+      <c r="D203" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E203" t="s">
+      <c r="E203" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="204" spans="1:5">
-      <c r="A204" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="204">
+      <c r="A204" s="10" t="n">
         <v>43397</v>
       </c>
-      <c r="C204">
+      <c r="C204" s="0" t="n">
         <v>4935</v>
       </c>
-      <c r="D204" t="s">
+      <c r="D204" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="E204" t="s">
+      <c r="E204" s="0" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="205" spans="1:5" ht="10" customHeight="1">
-      <c r="A205" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10" outlineLevel="0" r="205">
+      <c r="A205" s="10" t="n">
         <v>43398</v>
       </c>
-      <c r="B205">
+      <c r="B205" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="D205" t="s">
+      <c r="D205" s="0" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="206" spans="1:5">
-      <c r="A206" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="206">
+      <c r="A206" s="10" t="n">
         <v>43398</v>
       </c>
-      <c r="B206">
+      <c r="B206" s="0" t="n">
         <v>370</v>
       </c>
-      <c r="D206" t="s">
+      <c r="D206" s="0" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="207" spans="1:5">
-      <c r="A207" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="207">
+      <c r="A207" s="10" t="n">
         <v>43398</v>
       </c>
-      <c r="B207">
+      <c r="B207" s="0" t="n">
         <v>4966</v>
       </c>
-      <c r="D207" t="s">
+      <c r="D207" s="0" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="208" spans="1:5">
-      <c r="A208" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="208">
+      <c r="A208" s="10" t="n">
         <v>43397</v>
       </c>
-      <c r="C208">
+      <c r="C208" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="D208" t="s">
+      <c r="D208" s="0" t="s">
         <v>265</v>
       </c>
-      <c r="E208" t="s">
+      <c r="E208" s="0" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="209" spans="1:5">
-      <c r="A209" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="209">
+      <c r="A209" s="10" t="n">
         <v>43399</v>
       </c>
-      <c r="B209">
+      <c r="B209" s="0" t="n">
         <v>182</v>
       </c>
-      <c r="D209" t="s">
+      <c r="D209" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="E209" t="s">
+      <c r="E209" s="0" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="210" spans="1:5">
-      <c r="A210" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="210">
+      <c r="A210" s="10" t="n">
         <v>43401</v>
       </c>
-      <c r="B210">
+      <c r="B210" s="0" t="n">
         <v>700</v>
       </c>
-      <c r="D210" t="s">
+      <c r="D210" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="E210" t="s">
+      <c r="E210" s="0" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="211" spans="1:5">
-      <c r="A211" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="211">
+      <c r="A211" s="10" t="n">
         <v>43405</v>
       </c>
-      <c r="B211">
+      <c r="B211" s="0" t="n">
         <v>274</v>
       </c>
-      <c r="D211" t="s">
+      <c r="D211" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="E211" t="s">
+      <c r="E211" s="0" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="212" spans="1:5">
-      <c r="A212" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="212">
+      <c r="A212" s="10" t="n">
         <v>43405</v>
       </c>
-      <c r="C212">
+      <c r="C212" s="0" t="n">
         <v>590</v>
       </c>
-      <c r="D212" t="s">
+      <c r="D212" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="E212" t="s">
+      <c r="E212" s="0" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="213" spans="1:5" ht="14">
-      <c r="A213" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="213">
+      <c r="A213" s="10" t="n">
         <v>43407</v>
       </c>
-      <c r="C213">
+      <c r="C213" s="0" t="n">
         <v>1275</v>
       </c>
       <c r="D213" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="E213" t="s">
+      <c r="E213" s="0" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="214" spans="1:5" ht="14">
-      <c r="A214" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="214">
+      <c r="A214" s="10" t="n">
         <v>43407</v>
       </c>
-      <c r="C214">
+      <c r="C214" s="0" t="n">
         <v>4781</v>
       </c>
       <c r="D214" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="E214" t="s">
+      <c r="E214" s="0" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="215" spans="1:5" ht="14">
-      <c r="A215" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="215">
+      <c r="A215" s="10" t="n">
         <v>43407</v>
       </c>
-      <c r="C215">
+      <c r="C215" s="0" t="n">
         <v>4781</v>
       </c>
       <c r="D215" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="E215" t="s">
+      <c r="E215" s="0" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="216" spans="1:5">
-      <c r="A216" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="216">
+      <c r="A216" s="10" t="n">
         <v>43406</v>
       </c>
-      <c r="C216">
+      <c r="C216" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D216" t="s">
+      <c r="D216" s="0" t="s">
         <v>272</v>
       </c>
-      <c r="E216" t="s">
+      <c r="E216" s="0" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="217" spans="1:5">
-      <c r="A217" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="217">
+      <c r="A217" s="10" t="n">
         <v>43409</v>
       </c>
-      <c r="C217">
+      <c r="C217" s="0" t="n">
         <v>677</v>
       </c>
-      <c r="D217" t="s">
+      <c r="D217" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E217" t="s">
+      <c r="E217" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="218" spans="1:5" ht="14">
-      <c r="A218" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="218">
+      <c r="A218" s="10" t="n">
         <v>43410</v>
       </c>
-      <c r="B218">
+      <c r="B218" s="0" t="n">
         <v>285</v>
       </c>
       <c r="D218" s="13" t="s">
         <v>274</v>
       </c>
-      <c r="E218" t="s">
+      <c r="E218" s="0" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="219" spans="1:5" ht="14">
-      <c r="A219" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="219">
+      <c r="A219" s="10" t="n">
         <v>43410</v>
       </c>
-      <c r="B219">
+      <c r="B219" s="0" t="n">
         <v>125</v>
       </c>
       <c r="D219" s="13" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="220" spans="1:5" ht="14">
-      <c r="A220" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="220">
+      <c r="A220" s="10" t="n">
         <v>43409</v>
       </c>
-      <c r="B220">
+      <c r="B220" s="0" t="n">
         <v>85</v>
       </c>
       <c r="D220" s="13" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="221" spans="1:5" ht="14">
-      <c r="A221" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="221">
+      <c r="A221" s="10" t="n">
         <v>43410</v>
       </c>
-      <c r="B221">
+      <c r="B221" s="0" t="n">
         <v>44</v>
       </c>
       <c r="D221" s="13" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="222" spans="1:5">
-      <c r="A222" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="222">
+      <c r="A222" s="10" t="n">
         <v>43412</v>
       </c>
-      <c r="C222">
+      <c r="C222" s="0" t="n">
         <v>190</v>
       </c>
-      <c r="D222" t="s">
+      <c r="D222" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="E222" t="s">
+      <c r="E222" s="0" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="223" spans="1:5" ht="14">
-      <c r="A223" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="223">
+      <c r="A223" s="10" t="n">
         <v>43415</v>
       </c>
-      <c r="B223">
+      <c r="B223" s="0" t="n">
         <v>189</v>
       </c>
       <c r="D223" s="13" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="224" spans="1:5" ht="14">
-      <c r="A224" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="224">
+      <c r="A224" s="10" t="n">
         <v>43415</v>
       </c>
-      <c r="B224">
+      <c r="B224" s="0" t="n">
         <v>336</v>
       </c>
       <c r="D224" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="E224" t="s">
+      <c r="E224" s="0" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="225" spans="1:5" ht="14">
-      <c r="A225" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="225">
+      <c r="A225" s="10" t="n">
         <v>43419</v>
       </c>
-      <c r="B225">
+      <c r="B225" s="0" t="n">
         <v>158</v>
       </c>
       <c r="D225" s="13" t="s">
         <v>282</v>
       </c>
-      <c r="E225" t="s">
+      <c r="E225" s="0" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="241" spans="2:3">
-      <c r="B241">
-        <f>SUM(B2:B240)</f>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="226">
+      <c r="A226" s="10" t="n">
+        <v>43418</v>
+      </c>
+      <c r="C226" s="0" t="n">
+        <v>642</v>
+      </c>
+      <c r="D226" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="E226" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="227">
+      <c r="A227" s="10" t="n">
+        <v>43419</v>
+      </c>
+      <c r="C227" s="0" t="n">
+        <v>370</v>
+      </c>
+      <c r="D227" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="E227" s="0" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="228">
+      <c r="A228" s="10" t="n">
+        <v>43419</v>
+      </c>
+      <c r="C228" s="0" t="n">
+        <v>222</v>
+      </c>
+      <c r="D228" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="E228" s="0" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="241">
+      <c r="B241" s="0" t="n">
+        <f aca="false">SUM(B2:B240)</f>
         <v>57134</v>
       </c>
-      <c r="C241">
-        <f>SUM(C2:C240)</f>
-        <v>64845</v>
+      <c r="C241" s="0" t="n">
+        <f aca="false">SUM(C2:C240)</f>
+        <v>66079</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A30:Z32">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule aboveAverage="0" bottom="0" dxfId="0" operator="expression" percent="0" priority="2" rank="0" text="" type="expression">
       <formula>LEN(TRIM(A30))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D33" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D40" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D201" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink display="netonnet.se" ref="D33" r:id="rId1"/>
+    <hyperlink display="www.vidaxl.se" ref="D40" r:id="rId2"/>
+    <hyperlink display="https://www.vardia.se/" ref="D201" r:id="rId3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cost update 1119 Jenny
</commit_message>
<xml_diff>
--- a/Cost.xlsx
+++ b/Cost.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chengkaiyan/github/cost/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D3CC59-31DB-7D44-B8D7-8A560CF81669}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19980" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="290">
   <si>
     <t>日期</t>
   </si>
@@ -887,61 +882,80 @@
   </si>
   <si>
     <t>change tire</t>
+  </si>
+  <si>
+    <t>blommer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="yyyy/m/d"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt formatCode="YYYY/M/D" numFmtId="165"/>
+    <numFmt formatCode="M/D/YYYY" numFmtId="166"/>
+    <numFmt formatCode="YYYY\-MM\-DD" numFmtId="167"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="10">
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <family val="0"/>
       <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
       <name val="Arial"/>
       <family val="2"/>
+      <sz val="10"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF666666"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF666666"/>
+      <sz val="11"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0563C1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF0563C1"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0563C1"/>
       <name val="FreeSans"/>
       <family val="2"/>
+      <color rgb="FF0563C1"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF444444"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF444444"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="5">
@@ -971,7 +985,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
@@ -979,31 +993,100 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+  <cellStyleXfs count="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="167" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="20">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="7">
+    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle builtinId="8" customBuiltin="false" name="*unknown*" xfId="20"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1014,7 +1097,6 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1073,339 +1155,31 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF444444"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:Z241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A212" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E231" sqref="E231"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A212" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D239" activeCellId="0" pane="topLeft" sqref="D239"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="3" width="14.5"/>
-    <col min="4" max="4" width="26"/>
-    <col min="5" max="5" width="37.83203125"/>
-    <col min="6" max="1025" width="14.5"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="14.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1422,11 +1196,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1">
-      <c r="A2" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="2">
+      <c r="A2" s="2" t="n">
         <v>43121</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="1" t="n">
         <v>250</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1436,11 +1210,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1">
-      <c r="A3" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="3">
+      <c r="A3" s="2" t="n">
         <v>43122</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="1" t="n">
         <v>305</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1450,11 +1224,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1">
-      <c r="A4" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="4">
+      <c r="A4" s="2" t="n">
         <v>43122</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1464,11 +1238,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1">
-      <c r="A5" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="5">
+      <c r="A5" s="2" t="n">
         <v>43125</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="1" t="n">
         <v>98</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1478,11 +1252,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1">
-      <c r="A6" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="6">
+      <c r="A6" s="2" t="n">
         <v>43126</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1492,11 +1266,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1">
-      <c r="A7" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="7">
+      <c r="A7" s="2" t="n">
         <v>43127</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1506,11 +1280,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1">
-      <c r="A8" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="8">
+      <c r="A8" s="2" t="n">
         <v>43128</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="1" t="n">
         <v>656</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1520,11 +1294,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1">
-      <c r="A9" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="9">
+      <c r="A9" s="2" t="n">
         <v>43131</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="1" t="n">
         <v>486</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1534,11 +1308,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1">
-      <c r="A10" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="10">
+      <c r="A10" s="2" t="n">
         <v>43132</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="1" t="n">
         <v>76</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1548,11 +1322,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1">
-      <c r="A11" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="11">
+      <c r="A11" s="2" t="n">
         <v>43133</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="1" t="n">
         <v>399</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1562,11 +1336,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1">
-      <c r="A12" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="12">
+      <c r="A12" s="2" t="n">
         <v>43135</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="1" t="n">
         <v>419</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1576,11 +1350,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1">
-      <c r="A13" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="13">
+      <c r="A13" s="2" t="n">
         <v>43136</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="1" t="n">
         <v>521</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1590,11 +1364,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1">
-      <c r="A14" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="14">
+      <c r="A14" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="1" t="n">
         <v>399</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1604,11 +1378,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1">
-      <c r="A15" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="15">
+      <c r="A15" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="1" t="n">
         <v>138</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1618,11 +1392,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1">
-      <c r="A16" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="16">
+      <c r="A16" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="1" t="n">
         <v>310</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1632,12 +1406,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1">
-      <c r="A17" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="17">
+      <c r="A17" s="2" t="n">
         <v>43138</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="1">
+      <c r="C17" s="1" t="n">
         <v>700</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1647,12 +1421,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1">
-      <c r="A18" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="18">
+      <c r="A18" s="2" t="n">
         <v>43141</v>
       </c>
-      <c r="C18" s="1">
-        <f>F18*G18</f>
+      <c r="C18" s="1" t="n">
+        <f aca="false">F18*G18</f>
         <v>1312</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -1661,18 +1435,18 @@
       <c r="E18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="1" t="n">
         <v>164</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="1" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1">
-      <c r="A19" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="19">
+      <c r="A19" s="2" t="n">
         <v>43141</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="1" t="n">
         <v>1190</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1682,11 +1456,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1">
-      <c r="A20" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="20">
+      <c r="A20" s="2" t="n">
         <v>43154</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="1" t="n">
         <v>438</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1696,11 +1470,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1">
-      <c r="A21" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="21">
+      <c r="A21" s="2" t="n">
         <v>43154</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="1" t="n">
         <v>248</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -1710,22 +1484,22 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1">
-      <c r="A22" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="22">
+      <c r="A22" s="2" t="n">
         <v>43166</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="1" t="n">
         <v>234</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1">
-      <c r="A23" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="23">
+      <c r="A23" s="2" t="n">
         <v>43171</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="1" t="n">
         <v>118</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1735,22 +1509,22 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1">
-      <c r="A24" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="24">
+      <c r="A24" s="2" t="n">
         <v>43173</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="1" t="n">
         <v>82</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1">
-      <c r="A25" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="25">
+      <c r="A25" s="2" t="n">
         <v>43174</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1760,22 +1534,22 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1">
-      <c r="A26" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="26">
+      <c r="A26" s="2" t="n">
         <v>43175</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="1" t="n">
         <v>370</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:7" hidden="1">
-      <c r="A27" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="27">
+      <c r="A27" s="2" t="n">
         <v>43175</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -1785,11 +1559,11 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1">
-      <c r="A28" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="28">
+      <c r="A28" s="2" t="n">
         <v>43176</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="1" t="n">
         <v>624</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -1799,11 +1573,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1">
-      <c r="A29" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="29">
+      <c r="A29" s="2" t="n">
         <v>43177</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="1" t="n">
         <v>170</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1813,22 +1587,22 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1">
-      <c r="A30" s="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="30">
+      <c r="A30" s="4" t="n">
         <v>43179</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1">
-      <c r="A31" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="31">
+      <c r="A31" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="1" t="n">
         <v>90</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -1838,11 +1612,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1">
-      <c r="A32" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="32">
+      <c r="A32" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="1" t="n">
         <v>72</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -1852,11 +1626,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:26" hidden="1">
-      <c r="A33" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="33">
+      <c r="A33" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="1" t="n">
         <v>908</v>
       </c>
       <c r="D33" s="6" t="s">
@@ -1866,11 +1640,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:26" hidden="1">
-      <c r="A34" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="34">
+      <c r="A34" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -1880,11 +1654,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:26" hidden="1">
-      <c r="A35" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="35">
+      <c r="A35" s="2" t="n">
         <v>43181</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -1894,11 +1668,11 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:26" hidden="1">
-      <c r="A36" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="36">
+      <c r="A36" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="1" t="n">
         <v>135</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -1908,11 +1682,11 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:26" hidden="1">
-      <c r="A37" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="37">
+      <c r="A37" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="1" t="n">
         <v>110</v>
       </c>
       <c r="C37" s="1"/>
@@ -1944,11 +1718,11 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38" spans="1:26" hidden="1">
-      <c r="A38" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="38">
+      <c r="A38" s="2" t="n">
         <v>43185</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="1" t="n">
         <v>122</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -1958,22 +1732,22 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:26" hidden="1">
-      <c r="A39" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="39">
+      <c r="A39" s="2" t="n">
         <v>43187</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="1" t="n">
         <v>750</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:26" hidden="1">
-      <c r="A40" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="40">
+      <c r="A40" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="1" t="n">
         <v>379</v>
       </c>
       <c r="D40" s="6" t="s">
@@ -1983,22 +1757,22 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:26" hidden="1">
-      <c r="A41" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="41">
+      <c r="A41" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="1" t="n">
         <v>240</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:26" hidden="1">
-      <c r="A42" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="42">
+      <c r="A42" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="1" t="n">
         <v>540</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -2008,11 +1782,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:26" hidden="1">
-      <c r="A43" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="43">
+      <c r="A43" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -2022,11 +1796,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:26" hidden="1">
-      <c r="A44" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="44">
+      <c r="A44" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -2036,11 +1810,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:26" hidden="1">
-      <c r="A45" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="45">
+      <c r="A45" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="1" t="n">
         <v>462</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -2050,11 +1824,11 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:26" hidden="1">
-      <c r="A46" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="46">
+      <c r="A46" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46" s="1" t="n">
         <v>70</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -2064,11 +1838,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:26" hidden="1">
-      <c r="A47" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="47">
+      <c r="A47" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -2078,11 +1852,11 @@
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="1:26" hidden="1">
-      <c r="A48" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="48">
+      <c r="A48" s="2" t="n">
         <v>43190</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="1" t="n">
         <v>30</v>
       </c>
       <c r="C48" s="1"/>
@@ -2093,11 +1867,11 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1">
-      <c r="A49" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="49">
+      <c r="A49" s="2" t="n">
         <v>43191</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="1" t="n">
         <v>40</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -2107,11 +1881,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1">
-      <c r="A50" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="50">
+      <c r="A50" s="7" t="n">
         <v>43193</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50" s="1" t="n">
         <v>150</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -2121,11 +1895,11 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1">
-      <c r="A51" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="51">
+      <c r="A51" s="2" t="n">
         <v>43194</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51" s="1" t="n">
         <v>1360</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -2135,11 +1909,11 @@
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1">
-      <c r="A52" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="52">
+      <c r="A52" s="2" t="n">
         <v>43195</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" s="1" t="n">
         <v>94</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -2149,11 +1923,11 @@
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1">
-      <c r="A53" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="53">
+      <c r="A53" s="2" t="n">
         <v>43196</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C53" s="1" t="n">
         <v>48</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -2163,11 +1937,11 @@
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1">
-      <c r="A54" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="54">
+      <c r="A54" s="2" t="n">
         <v>43196</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C54" s="1" t="n">
         <v>205</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -2177,11 +1951,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1">
-      <c r="A55" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="55">
+      <c r="A55" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -2191,11 +1965,11 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1">
-      <c r="A56" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="56">
+      <c r="A56" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56" s="1" t="n">
         <v>421</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -2205,11 +1979,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1">
-      <c r="A57" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="57">
+      <c r="A57" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="1" t="n">
         <v>191</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -2219,11 +1993,11 @@
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1">
-      <c r="A58" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="58">
+      <c r="A58" s="2" t="n">
         <v>43198</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58" s="1" t="n">
         <v>226</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -2233,22 +2007,22 @@
         <v>96</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1">
-      <c r="A59" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="59">
+      <c r="A59" s="2" t="n">
         <v>43200</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59" s="1" t="n">
         <v>250</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1">
-      <c r="A60" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="60">
+      <c r="A60" s="2" t="n">
         <v>43200</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60" s="1" t="n">
         <v>1115</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -2258,11 +2032,11 @@
         <v>99</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1">
-      <c r="A61" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="61">
+      <c r="A61" s="2" t="n">
         <v>43201</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -2272,11 +2046,11 @@
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1">
-      <c r="A62" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="62">
+      <c r="A62" s="2" t="n">
         <v>43201</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62" s="1" t="n">
         <v>88</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -2286,11 +2060,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1">
-      <c r="A63" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="63">
+      <c r="A63" s="2" t="n">
         <v>43203</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -2300,11 +2074,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1">
-      <c r="A64" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="64">
+      <c r="A64" s="2" t="n">
         <v>43203</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C64" s="1" t="n">
         <v>364</v>
       </c>
       <c r="D64" s="1" t="s">
@@ -2314,11 +2088,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1">
-      <c r="A65" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="65">
+      <c r="A65" s="2" t="n">
         <v>43204</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65" s="1" t="n">
         <v>65</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -2328,11 +2102,11 @@
         <v>105</v>
       </c>
     </row>
-    <row r="66" spans="1:5" hidden="1">
-      <c r="A66" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="66">
+      <c r="A66" s="2" t="n">
         <v>43208</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -2342,11 +2116,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1">
-      <c r="A67" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="67">
+      <c r="A67" s="2" t="n">
         <v>43208</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C67" s="1" t="n">
         <v>470</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -2356,11 +2130,11 @@
         <v>107</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1">
-      <c r="A68" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="68">
+      <c r="A68" s="2" t="n">
         <v>43209</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68" s="1" t="n">
         <v>180</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -2370,11 +2144,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1">
-      <c r="A69" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="69">
+      <c r="A69" s="2" t="n">
         <v>43210</v>
       </c>
-      <c r="C69" s="1">
+      <c r="C69" s="1" t="n">
         <v>420</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -2384,11 +2158,11 @@
         <v>109</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1">
-      <c r="A70" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="70">
+      <c r="A70" s="2" t="n">
         <v>43212</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70" s="1" t="n">
         <v>50</v>
       </c>
       <c r="D70" s="1" t="s">
@@ -2398,11 +2172,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1">
-      <c r="A71" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="71">
+      <c r="A71" s="2" t="n">
         <v>43212</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71" s="1" t="n">
         <v>164</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -2412,11 +2186,11 @@
         <v>112</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1">
-      <c r="A72" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="72">
+      <c r="A72" s="2" t="n">
         <v>43215</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B72" s="1" t="n">
         <v>300</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -2426,11 +2200,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1">
-      <c r="A73" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="73">
+      <c r="A73" s="2" t="n">
         <v>43217</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73" s="1" t="n">
         <v>364</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -2440,11 +2214,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1">
-      <c r="A74" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="74">
+      <c r="A74" s="2" t="n">
         <v>43218</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74" s="1" t="n">
         <v>185</v>
       </c>
       <c r="D74" s="1" t="s">
@@ -2454,11 +2228,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1">
-      <c r="A75" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="75">
+      <c r="A75" s="2" t="n">
         <v>43218</v>
       </c>
-      <c r="C75" s="1">
+      <c r="C75" s="1" t="n">
         <v>404</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -2468,11 +2242,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="76" spans="1:5" hidden="1">
-      <c r="A76" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="76">
+      <c r="A76" s="2" t="n">
         <v>43220</v>
       </c>
-      <c r="C76" s="1">
+      <c r="C76" s="1" t="n">
         <v>57</v>
       </c>
       <c r="D76" s="1" t="s">
@@ -2482,11 +2256,11 @@
         <v>114</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1">
-      <c r="A77" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="77">
+      <c r="A77" s="2" t="n">
         <v>43221</v>
       </c>
-      <c r="C77" s="1">
+      <c r="C77" s="1" t="n">
         <v>282</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -2496,11 +2270,11 @@
         <v>116</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1">
-      <c r="A78" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="78">
+      <c r="A78" s="2" t="n">
         <v>43220</v>
       </c>
-      <c r="C78" s="1">
+      <c r="C78" s="1" t="n">
         <v>87</v>
       </c>
       <c r="D78" s="1" t="s">
@@ -2510,11 +2284,11 @@
         <v>117</v>
       </c>
     </row>
-    <row r="79" spans="1:5" hidden="1">
-      <c r="A79" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="79">
+      <c r="A79" s="2" t="n">
         <v>43223</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B79" s="1" t="n">
         <v>1878</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -2524,11 +2298,11 @@
         <v>119</v>
       </c>
     </row>
-    <row r="80" spans="1:5" hidden="1">
-      <c r="A80" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="80">
+      <c r="A80" s="2" t="n">
         <v>43224</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B80" s="1" t="n">
         <v>98</v>
       </c>
       <c r="D80" s="1" t="s">
@@ -2538,11 +2312,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="81" spans="1:5" hidden="1">
-      <c r="A81" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="81">
+      <c r="A81" s="2" t="n">
         <v>43225</v>
       </c>
-      <c r="C81" s="1">
+      <c r="C81" s="1" t="n">
         <v>198</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -2552,11 +2326,11 @@
         <v>122</v>
       </c>
     </row>
-    <row r="82" spans="1:5" hidden="1">
-      <c r="A82" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="82">
+      <c r="A82" s="2" t="n">
         <v>43225</v>
       </c>
-      <c r="C82" s="1">
+      <c r="C82" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -2566,11 +2340,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="83" spans="1:5" hidden="1">
-      <c r="A83" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="83">
+      <c r="A83" s="2" t="n">
         <v>43228</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83" s="1" t="n">
         <v>168</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -2580,11 +2354,11 @@
         <v>124</v>
       </c>
     </row>
-    <row r="84" spans="1:5" hidden="1">
-      <c r="A84" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="84">
+      <c r="A84" s="2" t="n">
         <v>43229</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B84" s="1" t="n">
         <v>240</v>
       </c>
       <c r="D84" s="1" t="s">
@@ -2594,12 +2368,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:5" hidden="1">
-      <c r="A85" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="85">
+      <c r="A85" s="2" t="n">
         <v>43230</v>
       </c>
       <c r="B85" s="1"/>
-      <c r="C85" s="1">
+      <c r="C85" s="1" t="n">
         <v>420</v>
       </c>
       <c r="D85" s="1" t="s">
@@ -2609,11 +2383,11 @@
         <v>126</v>
       </c>
     </row>
-    <row r="86" spans="1:5" hidden="1">
-      <c r="A86" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="86">
+      <c r="A86" s="2" t="n">
         <v>43230</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B86" s="1" t="n">
         <v>200</v>
       </c>
       <c r="C86" s="1"/>
@@ -2624,11 +2398,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="87" spans="1:5" hidden="1">
-      <c r="A87" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="87">
+      <c r="A87" s="2" t="n">
         <v>43230</v>
       </c>
-      <c r="C87" s="1">
+      <c r="C87" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D87" s="1" t="s">
@@ -2638,11 +2412,11 @@
         <v>128</v>
       </c>
     </row>
-    <row r="88" spans="1:5" hidden="1">
-      <c r="A88" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="88">
+      <c r="A88" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B88" s="1" t="n">
         <v>462</v>
       </c>
       <c r="D88" s="1" t="s">
@@ -2652,11 +2426,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="89" spans="1:5" hidden="1">
-      <c r="A89" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="89">
+      <c r="A89" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B89" s="1" t="n">
         <v>499</v>
       </c>
       <c r="D89" s="1" t="s">
@@ -2666,11 +2440,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="90" spans="1:5" hidden="1">
-      <c r="A90" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="90">
+      <c r="A90" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B90" s="1">
+      <c r="B90" s="1" t="n">
         <v>398</v>
       </c>
       <c r="D90" s="1" t="s">
@@ -2680,11 +2454,11 @@
         <v>133</v>
       </c>
     </row>
-    <row r="91" spans="1:5" hidden="1">
-      <c r="A91" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="91">
+      <c r="A91" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B91" s="1">
+      <c r="B91" s="1" t="n">
         <v>226</v>
       </c>
       <c r="D91" s="1" t="s">
@@ -2694,11 +2468,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="92" spans="1:5" hidden="1">
-      <c r="A92" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="92">
+      <c r="A92" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B92" s="1">
+      <c r="B92" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D92" s="1" t="s">
@@ -2708,11 +2482,11 @@
         <v>137</v>
       </c>
     </row>
-    <row r="93" spans="1:5" hidden="1">
-      <c r="A93" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="93">
+      <c r="A93" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="B93" s="1">
+      <c r="B93" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D93" s="1" t="s">
@@ -2722,11 +2496,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="94" spans="1:5" hidden="1">
-      <c r="A94" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="94">
+      <c r="A94" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="C94" s="1">
+      <c r="C94" s="1" t="n">
         <v>340</v>
       </c>
       <c r="D94" s="1" t="s">
@@ -2736,11 +2510,11 @@
         <v>139</v>
       </c>
     </row>
-    <row r="95" spans="1:5" hidden="1">
-      <c r="A95" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="95">
+      <c r="A95" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="B95" s="1">
+      <c r="B95" s="1" t="n">
         <v>510</v>
       </c>
       <c r="D95" s="1" t="s">
@@ -2750,11 +2524,11 @@
         <v>141</v>
       </c>
     </row>
-    <row r="96" spans="1:5" hidden="1">
-      <c r="A96" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="96">
+      <c r="A96" s="2" t="n">
         <v>43233</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B96" s="1" t="n">
         <v>170</v>
       </c>
       <c r="D96" s="1" t="s">
@@ -2764,11 +2538,11 @@
         <v>143</v>
       </c>
     </row>
-    <row r="97" spans="1:5" hidden="1">
-      <c r="A97" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="97">
+      <c r="A97" s="2" t="n">
         <v>43233</v>
       </c>
-      <c r="C97" s="1">
+      <c r="C97" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D97" s="1" t="s">
@@ -2778,11 +2552,11 @@
         <v>144</v>
       </c>
     </row>
-    <row r="98" spans="1:5" hidden="1">
-      <c r="A98" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="98">
+      <c r="A98" s="2" t="n">
         <v>43234</v>
       </c>
-      <c r="C98" s="1">
+      <c r="C98" s="1" t="n">
         <v>299</v>
       </c>
       <c r="D98" s="1" t="s">
@@ -2792,11 +2566,11 @@
         <v>145</v>
       </c>
     </row>
-    <row r="99" spans="1:5" hidden="1">
-      <c r="A99" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="99">
+      <c r="A99" s="2" t="n">
         <v>43236</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99" s="1" t="n">
         <v>3659</v>
       </c>
       <c r="D99" s="1" t="s">
@@ -2806,11 +2580,11 @@
         <v>146</v>
       </c>
     </row>
-    <row r="100" spans="1:5" hidden="1">
-      <c r="A100" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="100">
+      <c r="A100" s="2" t="n">
         <v>43237</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B100" s="1" t="n">
         <v>79</v>
       </c>
       <c r="D100" s="1" t="s">
@@ -2820,11 +2594,11 @@
         <v>147</v>
       </c>
     </row>
-    <row r="101" spans="1:5" hidden="1">
-      <c r="A101" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="101">
+      <c r="A101" s="2" t="n">
         <v>43236</v>
       </c>
-      <c r="C101" s="1">
+      <c r="C101" s="1" t="n">
         <v>173</v>
       </c>
       <c r="D101" s="1" t="s">
@@ -2834,11 +2608,11 @@
         <v>148</v>
       </c>
     </row>
-    <row r="102" spans="1:5" hidden="1">
-      <c r="A102" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="102">
+      <c r="A102" s="2" t="n">
         <v>43240</v>
       </c>
-      <c r="B102" s="1">
+      <c r="B102" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D102" s="1" t="s">
@@ -2848,22 +2622,22 @@
         <v>149</v>
       </c>
     </row>
-    <row r="103" spans="1:5" hidden="1">
-      <c r="A103" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="103">
+      <c r="A103" s="2" t="n">
         <v>43240</v>
       </c>
-      <c r="B103" s="1">
+      <c r="B103" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="104" spans="1:5" hidden="1">
-      <c r="A104" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="104">
+      <c r="A104" s="2" t="n">
         <v>43241</v>
       </c>
-      <c r="B104" s="1">
+      <c r="B104" s="1" t="n">
         <v>4070</v>
       </c>
       <c r="D104" s="1" t="s">
@@ -2873,11 +2647,11 @@
         <v>150</v>
       </c>
     </row>
-    <row r="105" spans="1:5" hidden="1">
-      <c r="A105" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="105">
+      <c r="A105" s="2" t="n">
         <v>43241</v>
       </c>
-      <c r="C105" s="1">
+      <c r="C105" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D105" s="1" t="s">
@@ -2887,11 +2661,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="106" spans="1:5" hidden="1">
-      <c r="A106" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="106">
+      <c r="A106" s="2" t="n">
         <v>43242</v>
       </c>
-      <c r="B106" s="1">
+      <c r="B106" s="1" t="n">
         <v>79</v>
       </c>
       <c r="D106" s="1" t="s">
@@ -2901,11 +2675,11 @@
         <v>152</v>
       </c>
     </row>
-    <row r="107" spans="1:5" hidden="1">
-      <c r="A107" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="107">
+      <c r="A107" s="2" t="n">
         <v>43246</v>
       </c>
-      <c r="B107" s="1">
+      <c r="B107" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D107" s="1" t="s">
@@ -2915,11 +2689,11 @@
         <v>154</v>
       </c>
     </row>
-    <row r="108" spans="1:5" hidden="1">
-      <c r="A108" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="108">
+      <c r="A108" s="2" t="n">
         <v>43247</v>
       </c>
-      <c r="B108" s="1">
+      <c r="B108" s="1" t="n">
         <v>70</v>
       </c>
       <c r="D108" s="1" t="s">
@@ -2929,44 +2703,44 @@
         <v>156</v>
       </c>
     </row>
-    <row r="109" spans="1:5" hidden="1">
-      <c r="A109" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="109">
+      <c r="A109" s="2" t="n">
         <v>43253</v>
       </c>
-      <c r="B109" s="1">
+      <c r="B109" s="1" t="n">
         <v>142</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="110" spans="1:5" hidden="1">
-      <c r="A110" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="110">
+      <c r="A110" s="2" t="n">
         <v>43254</v>
       </c>
-      <c r="B110" s="1">
+      <c r="B110" s="1" t="n">
         <v>90</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="111" spans="1:5" hidden="1">
-      <c r="A111" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="111">
+      <c r="A111" s="2" t="n">
         <v>43260</v>
       </c>
-      <c r="C111" s="1">
+      <c r="C111" s="1" t="n">
         <v>1400</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="112" spans="1:5" hidden="1">
-      <c r="A112" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="112">
+      <c r="A112" s="2" t="n">
         <v>43260</v>
       </c>
-      <c r="C112" s="1">
+      <c r="C112" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D112" s="1" t="s">
@@ -2976,33 +2750,33 @@
         <v>91</v>
       </c>
     </row>
-    <row r="113" spans="1:5" hidden="1">
-      <c r="A113" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="113">
+      <c r="A113" s="2" t="n">
         <v>43264</v>
       </c>
-      <c r="B113" s="1">
+      <c r="B113" s="1" t="n">
         <v>546</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="114" spans="1:5" hidden="1">
-      <c r="A114" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="114">
+      <c r="A114" s="2" t="n">
         <v>43264</v>
       </c>
-      <c r="B114" s="1">
+      <c r="B114" s="1" t="n">
         <v>95</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="115" spans="1:5" hidden="1">
-      <c r="A115" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="115">
+      <c r="A115" s="2" t="n">
         <v>43266</v>
       </c>
-      <c r="B115" s="1">
+      <c r="B115" s="1" t="n">
         <v>394</v>
       </c>
       <c r="D115" s="1" t="s">
@@ -3012,11 +2786,11 @@
         <v>163</v>
       </c>
     </row>
-    <row r="116" spans="1:5" hidden="1">
-      <c r="A116" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="116">
+      <c r="A116" s="2" t="n">
         <v>43266</v>
       </c>
-      <c r="B116" s="1">
+      <c r="B116" s="1" t="n">
         <v>1055</v>
       </c>
       <c r="D116" s="1" t="s">
@@ -3026,11 +2800,11 @@
         <v>165</v>
       </c>
     </row>
-    <row r="117" spans="1:5" hidden="1">
-      <c r="A117" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="117">
+      <c r="A117" s="2" t="n">
         <v>43284</v>
       </c>
-      <c r="C117" s="1">
+      <c r="C117" s="1" t="n">
         <v>274</v>
       </c>
       <c r="D117" s="1" t="s">
@@ -3040,11 +2814,11 @@
         <v>167</v>
       </c>
     </row>
-    <row r="118" spans="1:5" hidden="1">
-      <c r="A118" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="118">
+      <c r="A118" s="2" t="n">
         <v>43283</v>
       </c>
-      <c r="C118" s="1">
+      <c r="C118" s="1" t="n">
         <v>105</v>
       </c>
       <c r="D118" s="1" t="s">
@@ -3054,11 +2828,11 @@
         <v>169</v>
       </c>
     </row>
-    <row r="119" spans="1:5" hidden="1">
-      <c r="A119" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="119">
+      <c r="A119" s="2" t="n">
         <v>43289</v>
       </c>
-      <c r="C119" s="1">
+      <c r="C119" s="1" t="n">
         <v>128</v>
       </c>
       <c r="D119" s="1" t="s">
@@ -3068,11 +2842,11 @@
         <v>171</v>
       </c>
     </row>
-    <row r="120" spans="1:5" hidden="1">
-      <c r="A120" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="120">
+      <c r="A120" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C120" s="1">
+      <c r="C120" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D120" s="1" t="s">
@@ -3082,11 +2856,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="121" spans="1:5" hidden="1">
-      <c r="A121" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="121">
+      <c r="A121" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C121" s="1">
+      <c r="C121" s="1" t="n">
         <v>210</v>
       </c>
       <c r="D121" s="1" t="s">
@@ -3096,44 +2870,44 @@
         <v>173</v>
       </c>
     </row>
-    <row r="122" spans="1:5" hidden="1">
-      <c r="A122" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="122">
+      <c r="A122" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B122" s="1">
+      <c r="B122" s="1" t="n">
         <v>980</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="123" spans="1:5" hidden="1">
-      <c r="A123" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="123">
+      <c r="A123" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B123" s="1">
+      <c r="B123" s="1" t="n">
         <v>1260</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="124" spans="1:5" hidden="1">
-      <c r="A124" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="124">
+      <c r="A124" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B124" s="1">
+      <c r="B124" s="1" t="n">
         <v>3687</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="125" spans="1:5" hidden="1">
-      <c r="A125" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="125">
+      <c r="A125" s="2" t="n">
         <v>43298</v>
       </c>
-      <c r="C125" s="1">
+      <c r="C125" s="1" t="n">
         <v>60</v>
       </c>
       <c r="D125" s="1" t="s">
@@ -3143,55 +2917,55 @@
         <v>178</v>
       </c>
     </row>
-    <row r="126" spans="1:5" hidden="1">
-      <c r="A126" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="126">
+      <c r="A126" s="2" t="n">
         <v>43291</v>
       </c>
-      <c r="C126" s="1">
+      <c r="C126" s="1" t="n">
         <v>404</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="127" spans="1:5" hidden="1">
-      <c r="A127" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="127">
+      <c r="A127" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C127" s="1">
+      <c r="C127" s="1" t="n">
         <v>451</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="128" spans="1:5" hidden="1">
-      <c r="A128" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="128">
+      <c r="A128" s="2" t="n">
         <v>43298</v>
       </c>
-      <c r="C128" s="1">
+      <c r="C128" s="1" t="n">
         <v>708</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="129" spans="1:5" hidden="1">
-      <c r="A129" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="129">
+      <c r="A129" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C129" s="1">
+      <c r="C129" s="1" t="n">
         <v>160</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="130" spans="1:5" hidden="1">
-      <c r="A130" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="130">
+      <c r="A130" s="2" t="n">
         <v>43288</v>
       </c>
-      <c r="C130" s="1">
+      <c r="C130" s="1" t="n">
         <v>72</v>
       </c>
       <c r="D130" s="1" t="s">
@@ -3201,11 +2975,11 @@
         <v>181</v>
       </c>
     </row>
-    <row r="131" spans="1:5" hidden="1">
-      <c r="A131" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="131">
+      <c r="A131" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C131" s="1">
+      <c r="C131" s="1" t="n">
         <v>300</v>
       </c>
       <c r="D131" s="1" t="s">
@@ -3215,11 +2989,11 @@
         <v>183</v>
       </c>
     </row>
-    <row r="132" spans="1:5" hidden="1">
-      <c r="A132" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="132">
+      <c r="A132" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C132" s="1">
+      <c r="C132" s="1" t="n">
         <v>230</v>
       </c>
       <c r="D132" s="1" t="s">
@@ -3229,22 +3003,22 @@
         <v>185</v>
       </c>
     </row>
-    <row r="133" spans="1:5" hidden="1">
-      <c r="A133" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="133">
+      <c r="A133" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C133" s="1">
+      <c r="C133" s="1" t="n">
         <v>454</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="134" spans="1:5" hidden="1">
-      <c r="A134" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="134">
+      <c r="A134" s="2" t="n">
         <v>43299</v>
       </c>
-      <c r="C134" s="1">
+      <c r="C134" s="1" t="n">
         <v>686</v>
       </c>
       <c r="D134" s="1" t="s">
@@ -3254,11 +3028,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="135" spans="1:5" hidden="1">
-      <c r="A135" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="135">
+      <c r="A135" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C135" s="1">
+      <c r="C135" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D135" s="1" t="s">
@@ -3268,11 +3042,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="136" spans="1:5" hidden="1">
-      <c r="A136" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="136">
+      <c r="A136" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C136" s="1">
+      <c r="C136" s="1" t="n">
         <v>2067</v>
       </c>
       <c r="D136" s="1" t="s">
@@ -3282,11 +3056,11 @@
         <v>186</v>
       </c>
     </row>
-    <row r="137" spans="1:5" hidden="1">
-      <c r="A137" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="137">
+      <c r="A137" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B137" s="1">
+      <c r="B137" s="1" t="n">
         <v>109</v>
       </c>
       <c r="D137" s="1" t="s">
@@ -3296,11 +3070,11 @@
         <v>187</v>
       </c>
     </row>
-    <row r="138" spans="1:5" hidden="1">
-      <c r="A138" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="138">
+      <c r="A138" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B138" s="1">
+      <c r="B138" s="1" t="n">
         <v>97</v>
       </c>
       <c r="D138" s="1" t="s">
@@ -3310,11 +3084,11 @@
         <v>188</v>
       </c>
     </row>
-    <row r="139" spans="1:5" hidden="1">
-      <c r="A139" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="139">
+      <c r="A139" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B139" s="1">
+      <c r="B139" s="1" t="n">
         <v>1437</v>
       </c>
       <c r="D139" s="1" t="s">
@@ -3324,11 +3098,11 @@
         <v>189</v>
       </c>
     </row>
-    <row r="140" spans="1:5" hidden="1">
-      <c r="A140" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="140">
+      <c r="A140" s="2" t="n">
         <v>43306</v>
       </c>
-      <c r="C140" s="1">
+      <c r="C140" s="1" t="n">
         <v>650</v>
       </c>
       <c r="D140" s="1" t="s">
@@ -3338,11 +3112,11 @@
         <v>190</v>
       </c>
     </row>
-    <row r="141" spans="1:5" hidden="1">
-      <c r="A141" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="141">
+      <c r="A141" s="2" t="n">
         <v>43305</v>
       </c>
-      <c r="C141" s="1">
+      <c r="C141" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D141" s="1" t="s">
@@ -3352,11 +3126,11 @@
         <v>191</v>
       </c>
     </row>
-    <row r="142" spans="1:5" hidden="1">
-      <c r="A142" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="142">
+      <c r="A142" s="2" t="n">
         <v>43309</v>
       </c>
-      <c r="C142" s="1">
+      <c r="C142" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D142" s="1" t="s">
@@ -3366,11 +3140,11 @@
         <v>192</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="14" hidden="1">
-      <c r="A143" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="0" r="143">
+      <c r="A143" s="2" t="n">
         <v>43306</v>
       </c>
-      <c r="B143" s="1">
+      <c r="B143" s="1" t="n">
         <v>167</v>
       </c>
       <c r="D143" s="1" t="s">
@@ -3380,11 +3154,11 @@
         <v>193</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="14" hidden="1">
-      <c r="A144" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="0" r="144">
+      <c r="A144" s="2" t="n">
         <v>43304</v>
       </c>
-      <c r="C144" s="1">
+      <c r="C144" s="1" t="n">
         <v>93</v>
       </c>
       <c r="D144" s="1" t="s">
@@ -3394,11 +3168,11 @@
         <v>194</v>
       </c>
     </row>
-    <row r="145" spans="1:5" hidden="1">
-      <c r="A145" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="145">
+      <c r="A145" s="2" t="n">
         <v>43305</v>
       </c>
-      <c r="C145" s="1">
+      <c r="C145" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D145" s="1" t="s">
@@ -3408,11 +3182,11 @@
         <v>195</v>
       </c>
     </row>
-    <row r="146" spans="1:5" hidden="1">
-      <c r="A146" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="146">
+      <c r="A146" s="2" t="n">
         <v>43303</v>
       </c>
-      <c r="C146" s="1">
+      <c r="C146" s="1" t="n">
         <v>244</v>
       </c>
       <c r="D146" s="1" t="s">
@@ -3422,11 +3196,11 @@
         <v>196</v>
       </c>
     </row>
-    <row r="147" spans="1:5" hidden="1">
-      <c r="A147" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="147">
+      <c r="A147" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C147" s="1">
+      <c r="C147" s="1" t="n">
         <v>482</v>
       </c>
       <c r="D147" s="1" t="s">
@@ -3436,11 +3210,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="148" spans="1:5" hidden="1">
-      <c r="A148" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="148">
+      <c r="A148" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C148" s="1">
+      <c r="C148" s="1" t="n">
         <v>172</v>
       </c>
       <c r="D148" s="1" t="s">
@@ -3450,44 +3224,44 @@
         <v>199</v>
       </c>
     </row>
-    <row r="149" spans="1:5" hidden="1">
-      <c r="A149" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="149">
+      <c r="A149" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="B149" s="1">
+      <c r="B149" s="1" t="n">
         <v>89</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="150" spans="1:5" hidden="1">
-      <c r="A150" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="150">
+      <c r="A150" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="C150" s="1">
+      <c r="C150" s="1" t="n">
         <v>107</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="151" spans="1:5" hidden="1">
-      <c r="A151" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="151">
+      <c r="A151" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="C151" s="1">
+      <c r="C151" s="1" t="n">
         <v>124</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="152" spans="1:5" hidden="1">
-      <c r="A152" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="152">
+      <c r="A152" s="7" t="n">
         <v>43316</v>
       </c>
-      <c r="C152" s="1">
+      <c r="C152" s="1" t="n">
         <v>4500</v>
       </c>
       <c r="D152" s="1" t="s">
@@ -3497,11 +3271,11 @@
         <v>202</v>
       </c>
     </row>
-    <row r="153" spans="1:5" hidden="1">
-      <c r="A153" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="153">
+      <c r="A153" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C153" s="1">
+      <c r="C153" s="1" t="n">
         <v>247</v>
       </c>
       <c r="D153" s="1" t="s">
@@ -3511,11 +3285,11 @@
         <v>204</v>
       </c>
     </row>
-    <row r="154" spans="1:5" hidden="1">
-      <c r="A154" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="154">
+      <c r="A154" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C154" s="1">
+      <c r="C154" s="1" t="n">
         <v>1150</v>
       </c>
       <c r="D154" s="1" t="s">
@@ -3525,11 +3299,11 @@
         <v>205</v>
       </c>
     </row>
-    <row r="155" spans="1:5" hidden="1">
-      <c r="A155" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="155">
+      <c r="A155" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C155" s="1">
+      <c r="C155" s="1" t="n">
         <v>313</v>
       </c>
       <c r="D155" s="1" t="s">
@@ -3539,11 +3313,11 @@
         <v>207</v>
       </c>
     </row>
-    <row r="156" spans="1:5" hidden="1">
-      <c r="A156" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="156">
+      <c r="A156" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="B156" s="1">
+      <c r="B156" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D156" s="1" t="s">
@@ -3553,11 +3327,11 @@
         <v>209</v>
       </c>
     </row>
-    <row r="157" spans="1:5" hidden="1">
-      <c r="A157" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="157">
+      <c r="A157" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="C157" s="1">
+      <c r="C157" s="1" t="n">
         <v>710</v>
       </c>
       <c r="D157" s="1" t="s">
@@ -3567,11 +3341,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="158" spans="1:5">
-      <c r="A158" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="158">
+      <c r="A158" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="C158" s="1">
+      <c r="C158" s="1" t="n">
         <v>100</v>
       </c>
       <c r="D158" s="1" t="s">
@@ -3581,11 +3355,11 @@
         <v>212</v>
       </c>
     </row>
-    <row r="159" spans="1:5">
-      <c r="A159" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="159">
+      <c r="A159" s="2" t="n">
         <v>43319</v>
       </c>
-      <c r="B159" s="1">
+      <c r="B159" s="1" t="n">
         <v>78</v>
       </c>
       <c r="D159" s="1" t="s">
@@ -3595,22 +3369,22 @@
         <v>213</v>
       </c>
     </row>
-    <row r="160" spans="1:5">
-      <c r="A160" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="160">
+      <c r="A160" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="B160" s="1">
+      <c r="B160" s="1" t="n">
         <v>1840</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="161" spans="1:5">
-      <c r="A161" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="161">
+      <c r="A161" s="2" t="n">
         <v>43322</v>
       </c>
-      <c r="B161" s="1">
+      <c r="B161" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D161" s="1" t="s">
@@ -3620,11 +3394,11 @@
         <v>216</v>
       </c>
     </row>
-    <row r="162" spans="1:5">
-      <c r="A162" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="162">
+      <c r="A162" s="7" t="n">
         <v>43324</v>
       </c>
-      <c r="C162" s="1">
+      <c r="C162" s="1" t="n">
         <v>230</v>
       </c>
       <c r="D162" s="1" t="s">
@@ -3634,11 +3408,11 @@
         <v>217</v>
       </c>
     </row>
-    <row r="163" spans="1:5">
-      <c r="A163" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="163">
+      <c r="A163" s="7" t="n">
         <v>43326</v>
       </c>
-      <c r="C163" s="1">
+      <c r="C163" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D163" s="1" t="s">
@@ -3648,11 +3422,11 @@
         <v>219</v>
       </c>
     </row>
-    <row r="164" spans="1:5">
-      <c r="A164" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="164">
+      <c r="A164" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="B164" s="1">
+      <c r="B164" s="1" t="n">
         <v>45</v>
       </c>
       <c r="D164" s="1" t="s">
@@ -3662,894 +3436,913 @@
         <v>221</v>
       </c>
     </row>
-    <row r="165" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A165" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="165">
+      <c r="A165" s="10" t="n">
         <v>43327</v>
       </c>
-      <c r="C165">
+      <c r="C165" s="0" t="n">
         <v>486</v>
       </c>
-      <c r="D165" t="s">
+      <c r="D165" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E165" t="s">
+      <c r="E165" s="0" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="166" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A166" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="166">
+      <c r="A166" s="10" t="n">
         <v>43329</v>
       </c>
-      <c r="C166">
+      <c r="C166" s="0" t="n">
         <v>92</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D166" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="E166" t="s">
+      <c r="E166" s="0" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="167" spans="1:5">
-      <c r="A167" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="167">
+      <c r="A167" s="10" t="n">
         <v>43331</v>
       </c>
-      <c r="C167">
+      <c r="C167" s="0" t="n">
         <v>310</v>
       </c>
-      <c r="D167" t="s">
+      <c r="D167" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="E167" t="s">
+      <c r="E167" s="0" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="168" spans="1:5">
-      <c r="A168" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="168">
+      <c r="A168" s="10" t="n">
         <v>43334</v>
       </c>
-      <c r="C168">
+      <c r="C168" s="0" t="n">
         <v>464</v>
       </c>
-      <c r="D168" t="s">
+      <c r="D168" s="0" t="s">
         <v>218</v>
       </c>
       <c r="E168" s="11" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="169" spans="1:5">
-      <c r="A169" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="169">
+      <c r="A169" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="C169">
+      <c r="C169" s="0" t="n">
         <v>726</v>
       </c>
-      <c r="D169" t="s">
+      <c r="D169" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="E169" t="s">
+      <c r="E169" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="170" spans="1:5">
-      <c r="A170" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="170">
+      <c r="A170" s="10" t="n">
         <v>43337</v>
       </c>
-      <c r="C170">
+      <c r="C170" s="0" t="n">
         <v>544</v>
       </c>
-      <c r="D170" t="s">
+      <c r="D170" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E170" t="s">
+      <c r="E170" s="0" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="171" spans="1:5">
-      <c r="A171" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="171">
+      <c r="A171" s="10" t="n">
         <v>43337</v>
       </c>
-      <c r="B171">
+      <c r="B171" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D171" t="s">
+      <c r="D171" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="E171" t="s">
+      <c r="E171" s="0" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="172" spans="1:5">
-      <c r="A172" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="172">
+      <c r="A172" s="10" t="n">
         <v>43341</v>
       </c>
-      <c r="C172">
+      <c r="C172" s="0" t="n">
         <v>830</v>
       </c>
-      <c r="D172" t="s">
+      <c r="D172" s="0" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="173" spans="1:5">
-      <c r="A173" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="173">
+      <c r="A173" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="C173">
+      <c r="C173" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="D173" t="s">
+      <c r="D173" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="E173" t="s">
+      <c r="E173" s="0" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="174" spans="1:5">
-      <c r="A174" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="174">
+      <c r="A174" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="B174">
+      <c r="B174" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D174" t="s">
+      <c r="D174" s="0" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="175" spans="1:5">
-      <c r="A175" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="175">
+      <c r="A175" s="10" t="n">
         <v>43344</v>
       </c>
-      <c r="B175">
+      <c r="B175" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="D175" t="s">
+      <c r="D175" s="0" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="176" spans="1:5">
-      <c r="A176" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="176">
+      <c r="A176" s="10" t="n">
         <v>43344</v>
       </c>
-      <c r="B176">
+      <c r="B176" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D176" t="s">
+      <c r="D176" s="0" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="177" spans="1:5">
-      <c r="A177" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="177">
+      <c r="A177" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C177">
+      <c r="C177" s="0" t="n">
         <v>607</v>
       </c>
-      <c r="D177" t="s">
+      <c r="D177" s="0" t="s">
         <v>235</v>
       </c>
-      <c r="E177" t="s">
+      <c r="E177" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="178" spans="1:5">
-      <c r="A178" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="178">
+      <c r="A178" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C178">
+      <c r="C178" s="0" t="n">
         <v>444</v>
       </c>
-      <c r="D178" t="s">
+      <c r="D178" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E178" t="s">
+      <c r="E178" s="0" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="179" spans="1:5">
-      <c r="A179" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="179">
+      <c r="A179" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C179">
+      <c r="C179" s="0" t="n">
         <v>312</v>
       </c>
-      <c r="D179" t="s">
+      <c r="D179" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="E179" t="s">
+      <c r="E179" s="0" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="180" spans="1:5">
-      <c r="A180" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="180">
+      <c r="A180" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C180">
+      <c r="C180" s="0" t="n">
         <v>501</v>
       </c>
-      <c r="D180" t="s">
+      <c r="D180" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E180" t="s">
+      <c r="E180" s="0" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="181" spans="1:5">
-      <c r="A181" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="181">
+      <c r="A181" s="10" t="n">
         <v>43349</v>
       </c>
-      <c r="C181">
+      <c r="C181" s="0" t="n">
         <v>711</v>
       </c>
-      <c r="D181" t="s">
+      <c r="D181" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="E181" t="s">
+      <c r="E181" s="0" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="182" spans="1:5">
-      <c r="A182" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="182">
+      <c r="A182" s="10" t="n">
         <v>43354</v>
       </c>
-      <c r="B182">
+      <c r="B182" s="0" t="n">
         <v>126</v>
       </c>
-      <c r="D182" t="s">
+      <c r="D182" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="E182" t="s">
+      <c r="E182" s="0" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="183" spans="1:5">
-      <c r="A183" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="183">
+      <c r="A183" s="10" t="n">
         <v>43354</v>
       </c>
-      <c r="C183">
+      <c r="C183" s="0" t="n">
         <v>450</v>
       </c>
-      <c r="D183" t="s">
+      <c r="D183" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="E183" t="s">
+      <c r="E183" s="0" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="184" spans="1:5">
-      <c r="A184" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="184">
+      <c r="A184" s="10" t="n">
         <v>43361</v>
       </c>
-      <c r="C184">
+      <c r="C184" s="0" t="n">
         <v>660</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D184" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="E184" t="s">
+      <c r="E184" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="185" spans="1:5">
-      <c r="A185" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="185">
+      <c r="A185" s="10" t="n">
         <v>43363</v>
       </c>
-      <c r="C185">
+      <c r="C185" s="0" t="n">
         <v>230</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D185" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="E185" t="s">
+      <c r="E185" s="0" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="186" spans="1:5">
-      <c r="A186" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="186">
+      <c r="A186" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B186">
+      <c r="B186" s="0" t="n">
         <v>4859</v>
       </c>
-      <c r="D186" t="s">
+      <c r="D186" s="0" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="187" spans="1:5">
-      <c r="A187" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="187">
+      <c r="A187" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B187">
+      <c r="B187" s="0" t="n">
         <v>295</v>
       </c>
-      <c r="D187" t="s">
+      <c r="D187" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="E187" t="s">
+      <c r="E187" s="0" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="188" spans="1:5">
-      <c r="A188" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="188">
+      <c r="A188" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B188">
+      <c r="B188" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D188" t="s">
+      <c r="D188" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="E188" t="s">
+      <c r="E188" s="0" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="189" spans="1:5">
-      <c r="A189" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="189">
+      <c r="A189" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B189">
+      <c r="B189" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="D189" t="s">
+      <c r="D189" s="0" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="190" spans="1:5">
-      <c r="A190" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="190">
+      <c r="A190" s="10" t="n">
         <v>43378</v>
       </c>
-      <c r="B190">
+      <c r="B190" s="0" t="n">
         <v>506</v>
       </c>
-      <c r="D190" t="s">
+      <c r="D190" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="E190" t="s">
+      <c r="E190" s="0" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="191" spans="1:5">
-      <c r="A191" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="191">
+      <c r="A191" s="10" t="n">
         <v>43379</v>
       </c>
-      <c r="B191">
+      <c r="B191" s="0" t="n">
         <v>350</v>
       </c>
-      <c r="D191" t="s">
+      <c r="D191" s="0" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="192" spans="1:5" ht="20" customHeight="1">
-      <c r="A192" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="20" outlineLevel="0" r="192">
+      <c r="A192" s="10" t="n">
         <v>43383</v>
       </c>
-      <c r="B192">
+      <c r="B192" s="0" t="n">
         <v>189</v>
       </c>
-      <c r="D192" t="s">
+      <c r="D192" s="0" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="193" spans="1:5">
-      <c r="A193" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="193">
+      <c r="A193" s="10" t="n">
         <v>43387</v>
       </c>
-      <c r="B193">
+      <c r="B193" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="D193" t="s">
+      <c r="D193" s="0" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="194" spans="1:5">
-      <c r="A194" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="194">
+      <c r="A194" s="10" t="n">
         <v>43387</v>
       </c>
-      <c r="B194">
+      <c r="B194" s="0" t="n">
         <v>307</v>
       </c>
-      <c r="D194" t="s">
+      <c r="D194" s="0" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="195" spans="1:5">
-      <c r="C195">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="195">
+      <c r="C195" s="0" t="n">
         <v>3705</v>
       </c>
-      <c r="E195" t="s">
+      <c r="E195" s="0" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="196" spans="1:5">
-      <c r="A196" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="196">
+      <c r="A196" s="10" t="n">
         <v>43385</v>
       </c>
-      <c r="C196">
+      <c r="C196" s="0" t="n">
         <v>608</v>
       </c>
-      <c r="D196" t="s">
+      <c r="D196" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E196" t="s">
+      <c r="E196" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="197" spans="1:5">
-      <c r="A197" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="197">
+      <c r="A197" s="10" t="n">
         <v>43391</v>
       </c>
-      <c r="B197">
+      <c r="B197" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="D197" t="s">
+      <c r="D197" s="0" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="198" spans="1:5">
-      <c r="A198" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="198">
+      <c r="A198" s="10" t="n">
         <v>43392</v>
       </c>
-      <c r="B198">
+      <c r="B198" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="D198" t="s">
+      <c r="D198" s="0" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="199" spans="1:5">
-      <c r="A199" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="199">
+      <c r="A199" s="10" t="n">
         <v>43393</v>
       </c>
-      <c r="B199">
+      <c r="B199" s="0" t="n">
         <v>177</v>
       </c>
-      <c r="D199" t="s">
+      <c r="D199" s="0" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="200" spans="1:5">
-      <c r="A200" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="200">
+      <c r="A200" s="10" t="n">
         <v>43393</v>
       </c>
-      <c r="C200">
+      <c r="C200" s="0" t="n">
         <v>125</v>
       </c>
-      <c r="D200" t="s">
+      <c r="D200" s="0" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="201" spans="1:5">
-      <c r="A201" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="201">
+      <c r="A201" s="10" t="n">
         <v>43395</v>
       </c>
-      <c r="B201">
+      <c r="B201" s="0" t="n">
         <v>2800</v>
       </c>
       <c r="D201" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="E201" t="s">
+      <c r="E201" s="0" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="202" spans="1:5">
-      <c r="A202" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="202">
+      <c r="A202" s="10" t="n">
         <v>43395</v>
       </c>
-      <c r="C202">
+      <c r="C202" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="D202" t="s">
+      <c r="D202" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="E202" t="s">
+      <c r="E202" s="0" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="203" spans="1:5">
-      <c r="A203" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="203">
+      <c r="A203" s="10" t="n">
         <v>43396</v>
       </c>
-      <c r="C203">
+      <c r="C203" s="0" t="n">
         <v>692</v>
       </c>
-      <c r="D203" t="s">
+      <c r="D203" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E203" t="s">
+      <c r="E203" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="204" spans="1:5">
-      <c r="A204" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="204">
+      <c r="A204" s="10" t="n">
         <v>43397</v>
       </c>
-      <c r="C204">
+      <c r="C204" s="0" t="n">
         <v>4935</v>
       </c>
-      <c r="D204" t="s">
+      <c r="D204" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="E204" t="s">
+      <c r="E204" s="0" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="205" spans="1:5" ht="10" customHeight="1">
-      <c r="A205" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10" outlineLevel="0" r="205">
+      <c r="A205" s="10" t="n">
         <v>43398</v>
       </c>
-      <c r="B205">
+      <c r="B205" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="D205" t="s">
+      <c r="D205" s="0" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="206" spans="1:5">
-      <c r="A206" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="206">
+      <c r="A206" s="10" t="n">
         <v>43398</v>
       </c>
-      <c r="B206">
+      <c r="B206" s="0" t="n">
         <v>370</v>
       </c>
-      <c r="D206" t="s">
+      <c r="D206" s="0" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="207" spans="1:5">
-      <c r="A207" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="207">
+      <c r="A207" s="10" t="n">
         <v>43398</v>
       </c>
-      <c r="B207">
+      <c r="B207" s="0" t="n">
         <v>4966</v>
       </c>
-      <c r="D207" t="s">
+      <c r="D207" s="0" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="208" spans="1:5">
-      <c r="A208" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="208">
+      <c r="A208" s="10" t="n">
         <v>43397</v>
       </c>
-      <c r="C208">
+      <c r="C208" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="D208" t="s">
+      <c r="D208" s="0" t="s">
         <v>265</v>
       </c>
-      <c r="E208" t="s">
+      <c r="E208" s="0" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="209" spans="1:5">
-      <c r="A209" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="209">
+      <c r="A209" s="10" t="n">
         <v>43399</v>
       </c>
-      <c r="B209">
+      <c r="B209" s="0" t="n">
         <v>182</v>
       </c>
-      <c r="D209" t="s">
+      <c r="D209" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="E209" t="s">
+      <c r="E209" s="0" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="210" spans="1:5">
-      <c r="A210" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="210">
+      <c r="A210" s="10" t="n">
         <v>43401</v>
       </c>
-      <c r="B210">
+      <c r="B210" s="0" t="n">
         <v>700</v>
       </c>
-      <c r="D210" t="s">
+      <c r="D210" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="E210" t="s">
+      <c r="E210" s="0" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="211" spans="1:5">
-      <c r="A211" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="211">
+      <c r="A211" s="10" t="n">
         <v>43405</v>
       </c>
-      <c r="B211">
+      <c r="B211" s="0" t="n">
         <v>274</v>
       </c>
-      <c r="D211" t="s">
+      <c r="D211" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="E211" t="s">
+      <c r="E211" s="0" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="212" spans="1:5">
-      <c r="A212" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="212">
+      <c r="A212" s="10" t="n">
         <v>43405</v>
       </c>
-      <c r="C212">
+      <c r="C212" s="0" t="n">
         <v>590</v>
       </c>
-      <c r="D212" t="s">
+      <c r="D212" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="E212" t="s">
+      <c r="E212" s="0" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="213" spans="1:5" ht="14">
-      <c r="A213" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="213">
+      <c r="A213" s="10" t="n">
         <v>43407</v>
       </c>
-      <c r="C213">
+      <c r="C213" s="0" t="n">
         <v>1275</v>
       </c>
       <c r="D213" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="E213" t="s">
+      <c r="E213" s="0" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="214" spans="1:5" ht="14">
-      <c r="A214" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="214">
+      <c r="A214" s="10" t="n">
         <v>43407</v>
       </c>
-      <c r="C214">
+      <c r="C214" s="0" t="n">
         <v>4781</v>
       </c>
       <c r="D214" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="E214" t="s">
+      <c r="E214" s="0" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="215" spans="1:5" ht="14">
-      <c r="A215" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="215">
+      <c r="A215" s="10" t="n">
         <v>43407</v>
       </c>
-      <c r="C215">
+      <c r="C215" s="0" t="n">
         <v>4781</v>
       </c>
       <c r="D215" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="E215" t="s">
+      <c r="E215" s="0" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="216" spans="1:5">
-      <c r="A216" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="216">
+      <c r="A216" s="10" t="n">
         <v>43406</v>
       </c>
-      <c r="C216">
+      <c r="C216" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D216" t="s">
+      <c r="D216" s="0" t="s">
         <v>272</v>
       </c>
-      <c r="E216" t="s">
+      <c r="E216" s="0" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="217" spans="1:5">
-      <c r="A217" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="217">
+      <c r="A217" s="10" t="n">
         <v>43409</v>
       </c>
-      <c r="C217">
+      <c r="C217" s="0" t="n">
         <v>677</v>
       </c>
-      <c r="D217" t="s">
+      <c r="D217" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E217" t="s">
+      <c r="E217" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="218" spans="1:5" ht="14">
-      <c r="A218" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="218">
+      <c r="A218" s="10" t="n">
         <v>43410</v>
       </c>
-      <c r="B218">
+      <c r="B218" s="0" t="n">
         <v>285</v>
       </c>
       <c r="D218" s="13" t="s">
         <v>274</v>
       </c>
-      <c r="E218" t="s">
+      <c r="E218" s="0" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="219" spans="1:5" ht="14">
-      <c r="A219" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="219">
+      <c r="A219" s="10" t="n">
         <v>43410</v>
       </c>
-      <c r="B219">
+      <c r="B219" s="0" t="n">
         <v>125</v>
       </c>
       <c r="D219" s="13" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="220" spans="1:5" ht="14">
-      <c r="A220" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="220">
+      <c r="A220" s="10" t="n">
         <v>43409</v>
       </c>
-      <c r="B220">
+      <c r="B220" s="0" t="n">
         <v>85</v>
       </c>
       <c r="D220" s="13" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="221" spans="1:5" ht="14">
-      <c r="A221" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="221">
+      <c r="A221" s="10" t="n">
         <v>43410</v>
       </c>
-      <c r="B221">
+      <c r="B221" s="0" t="n">
         <v>44</v>
       </c>
       <c r="D221" s="13" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="222" spans="1:5">
-      <c r="A222" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="222">
+      <c r="A222" s="10" t="n">
         <v>43412</v>
       </c>
-      <c r="C222">
+      <c r="C222" s="0" t="n">
         <v>190</v>
       </c>
-      <c r="D222" t="s">
+      <c r="D222" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="E222" t="s">
+      <c r="E222" s="0" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="223" spans="1:5" ht="14">
-      <c r="A223" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="223">
+      <c r="A223" s="10" t="n">
         <v>43415</v>
       </c>
-      <c r="B223">
+      <c r="B223" s="0" t="n">
         <v>189</v>
       </c>
       <c r="D223" s="13" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="224" spans="1:5" ht="14">
-      <c r="A224" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="224">
+      <c r="A224" s="10" t="n">
         <v>43415</v>
       </c>
-      <c r="B224">
+      <c r="B224" s="0" t="n">
         <v>336</v>
       </c>
       <c r="D224" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="E224" t="s">
+      <c r="E224" s="0" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="225" spans="1:5" ht="14">
-      <c r="A225" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="225">
+      <c r="A225" s="10" t="n">
         <v>43419</v>
       </c>
-      <c r="B225">
+      <c r="B225" s="0" t="n">
         <v>158</v>
       </c>
       <c r="D225" s="13" t="s">
         <v>282</v>
       </c>
-      <c r="E225" t="s">
+      <c r="E225" s="0" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="226" spans="1:5">
-      <c r="A226" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="226">
+      <c r="A226" s="10" t="n">
         <v>43418</v>
       </c>
-      <c r="C226">
+      <c r="C226" s="0" t="n">
         <v>642</v>
       </c>
-      <c r="D226" t="s">
+      <c r="D226" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E226" t="s">
+      <c r="E226" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="227" spans="1:5">
-      <c r="A227" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="227">
+      <c r="A227" s="10" t="n">
         <v>43419</v>
       </c>
-      <c r="C227">
+      <c r="C227" s="0" t="n">
         <v>370</v>
       </c>
-      <c r="D227" t="s">
+      <c r="D227" s="0" t="s">
         <v>284</v>
       </c>
-      <c r="E227" t="s">
+      <c r="E227" s="0" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="228" spans="1:5">
-      <c r="A228" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="228">
+      <c r="A228" s="10" t="n">
         <v>43419</v>
       </c>
-      <c r="C228">
+      <c r="C228" s="0" t="n">
         <v>222</v>
       </c>
-      <c r="D228" t="s">
+      <c r="D228" s="0" t="s">
         <v>286</v>
       </c>
-      <c r="E228" t="s">
+      <c r="E228" s="0" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="229" spans="1:5">
-      <c r="A229" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="229">
+      <c r="A229" s="10" t="n">
         <v>43421</v>
       </c>
-      <c r="B229">
+      <c r="B229" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="D229" t="s">
+      <c r="D229" s="0" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="230" spans="1:5">
-      <c r="A230" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="230">
+      <c r="A230" s="10" t="n">
         <v>43422</v>
       </c>
-      <c r="B230">
+      <c r="B230" s="0" t="n">
         <v>158</v>
       </c>
-      <c r="D230" t="s">
+      <c r="D230" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="E230" t="s">
+      <c r="E230" s="0" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="231" spans="1:5">
-      <c r="A231" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="231">
+      <c r="A231" s="10" t="n">
         <v>43422</v>
       </c>
-      <c r="B231">
+      <c r="B231" s="0" t="n">
         <v>159</v>
       </c>
-      <c r="D231" t="s">
+      <c r="D231" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="E231" t="s">
+      <c r="E231" s="0" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="241" spans="2:3">
-      <c r="B241">
-        <f>SUM(B2:B240)</f>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="232">
+      <c r="A232" s="10" t="n">
+        <v>43421</v>
+      </c>
+      <c r="C232" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="D232" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="E232" s="0" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="241">
+      <c r="B241" s="0" t="n">
+        <f aca="false">SUM(B2:B240)</f>
         <v>57751</v>
       </c>
-      <c r="C241">
-        <f>SUM(C2:C240)</f>
-        <v>66079</v>
+      <c r="C241" s="0" t="n">
+        <f aca="false">SUM(C2:C240)</f>
+        <v>66159</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A30:Z32">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule aboveAverage="0" bottom="0" dxfId="0" operator="expression" percent="0" priority="2" rank="0" text="" type="expression">
       <formula>LEN(TRIM(A30))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D33" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D40" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D201" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink display="netonnet.se" ref="D33" r:id="rId1"/>
+    <hyperlink display="www.vidaxl.se" ref="D40" r:id="rId2"/>
+    <hyperlink display="https://www.vardia.se/" ref="D201" r:id="rId3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cost update Jenny 1122
</commit_message>
<xml_diff>
--- a/Cost.xlsx
+++ b/Cost.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chengkaiyan/github/cost/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A36A1A-35B7-4A4D-8E9E-E33678C6BBEB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20260" windowHeight="13360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="293">
   <si>
     <t>日期</t>
   </si>
@@ -896,61 +891,80 @@
   </si>
   <si>
     <t>lön</t>
+  </si>
+  <si>
+    <t>diaper,kyckling,etc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="yyyy/m/d"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt formatCode="YYYY/M/D" numFmtId="165"/>
+    <numFmt formatCode="M/D/YYYY" numFmtId="166"/>
+    <numFmt formatCode="YYYY\-MM\-DD" numFmtId="167"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="10">
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <family val="0"/>
       <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
       <name val="Arial"/>
       <family val="2"/>
+      <sz val="10"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF666666"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF666666"/>
+      <sz val="11"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0563C1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF0563C1"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0563C1"/>
       <name val="FreeSans"/>
       <family val="2"/>
+      <color rgb="FF0563C1"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF444444"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF444444"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="5">
@@ -980,7 +994,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
@@ -988,31 +1002,100 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+  <cellStyleXfs count="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="167" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="20">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="7">
+    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle builtinId="8" customBuiltin="false" name="*unknown*" xfId="20"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1023,7 +1106,6 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1082,339 +1164,31 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF444444"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:Z241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A212" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E233" sqref="E233"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A215" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E234" activeCellId="0" pane="topLeft" sqref="E234"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="3" width="14.5"/>
-    <col min="4" max="4" width="26"/>
-    <col min="5" max="5" width="37.83203125"/>
-    <col min="6" max="1025" width="14.5"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="14.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1431,11 +1205,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1">
-      <c r="A2" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="2">
+      <c r="A2" s="2" t="n">
         <v>43121</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="1" t="n">
         <v>250</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1445,11 +1219,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1">
-      <c r="A3" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="3">
+      <c r="A3" s="2" t="n">
         <v>43122</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="1" t="n">
         <v>305</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1459,11 +1233,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1">
-      <c r="A4" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="4">
+      <c r="A4" s="2" t="n">
         <v>43122</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1473,11 +1247,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1">
-      <c r="A5" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="5">
+      <c r="A5" s="2" t="n">
         <v>43125</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="1" t="n">
         <v>98</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1487,11 +1261,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1">
-      <c r="A6" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="6">
+      <c r="A6" s="2" t="n">
         <v>43126</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1501,11 +1275,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1">
-      <c r="A7" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="7">
+      <c r="A7" s="2" t="n">
         <v>43127</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1515,11 +1289,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1">
-      <c r="A8" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="8">
+      <c r="A8" s="2" t="n">
         <v>43128</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="1" t="n">
         <v>656</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1529,11 +1303,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1">
-      <c r="A9" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="9">
+      <c r="A9" s="2" t="n">
         <v>43131</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="1" t="n">
         <v>486</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1543,11 +1317,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1">
-      <c r="A10" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="10">
+      <c r="A10" s="2" t="n">
         <v>43132</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="1" t="n">
         <v>76</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1557,11 +1331,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1">
-      <c r="A11" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="11">
+      <c r="A11" s="2" t="n">
         <v>43133</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="1" t="n">
         <v>399</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1571,11 +1345,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1">
-      <c r="A12" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="12">
+      <c r="A12" s="2" t="n">
         <v>43135</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="1" t="n">
         <v>419</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1585,11 +1359,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1">
-      <c r="A13" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="13">
+      <c r="A13" s="2" t="n">
         <v>43136</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="1" t="n">
         <v>521</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1599,11 +1373,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1">
-      <c r="A14" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="14">
+      <c r="A14" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="1" t="n">
         <v>399</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1613,11 +1387,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1">
-      <c r="A15" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="15">
+      <c r="A15" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="1" t="n">
         <v>138</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1627,11 +1401,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1">
-      <c r="A16" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="16">
+      <c r="A16" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="1" t="n">
         <v>310</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1641,12 +1415,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1">
-      <c r="A17" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="17">
+      <c r="A17" s="2" t="n">
         <v>43138</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="1">
+      <c r="C17" s="1" t="n">
         <v>700</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1656,12 +1430,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1">
-      <c r="A18" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="18">
+      <c r="A18" s="2" t="n">
         <v>43141</v>
       </c>
-      <c r="C18" s="1">
-        <f>F18*G18</f>
+      <c r="C18" s="1" t="n">
+        <f aca="false">F18*G18</f>
         <v>1312</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -1670,18 +1444,18 @@
       <c r="E18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="1" t="n">
         <v>164</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="1" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1">
-      <c r="A19" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="19">
+      <c r="A19" s="2" t="n">
         <v>43141</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="1" t="n">
         <v>1190</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1691,11 +1465,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1">
-      <c r="A20" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="20">
+      <c r="A20" s="2" t="n">
         <v>43154</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="1" t="n">
         <v>438</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1705,11 +1479,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1">
-      <c r="A21" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="21">
+      <c r="A21" s="2" t="n">
         <v>43154</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="1" t="n">
         <v>248</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -1719,22 +1493,22 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1">
-      <c r="A22" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="22">
+      <c r="A22" s="2" t="n">
         <v>43166</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="1" t="n">
         <v>234</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1">
-      <c r="A23" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="23">
+      <c r="A23" s="2" t="n">
         <v>43171</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="1" t="n">
         <v>118</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1744,22 +1518,22 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1">
-      <c r="A24" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="24">
+      <c r="A24" s="2" t="n">
         <v>43173</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="1" t="n">
         <v>82</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1">
-      <c r="A25" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="25">
+      <c r="A25" s="2" t="n">
         <v>43174</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1769,22 +1543,22 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1">
-      <c r="A26" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="26">
+      <c r="A26" s="2" t="n">
         <v>43175</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="1" t="n">
         <v>370</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:7" hidden="1">
-      <c r="A27" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="27">
+      <c r="A27" s="2" t="n">
         <v>43175</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -1794,11 +1568,11 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1">
-      <c r="A28" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="28">
+      <c r="A28" s="2" t="n">
         <v>43176</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="1" t="n">
         <v>624</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -1808,11 +1582,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1">
-      <c r="A29" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="29">
+      <c r="A29" s="2" t="n">
         <v>43177</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="1" t="n">
         <v>170</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1822,22 +1596,22 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1">
-      <c r="A30" s="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="30">
+      <c r="A30" s="4" t="n">
         <v>43179</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1">
-      <c r="A31" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="31">
+      <c r="A31" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="1" t="n">
         <v>90</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -1847,11 +1621,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1">
-      <c r="A32" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="32">
+      <c r="A32" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="1" t="n">
         <v>72</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -1861,11 +1635,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:26" hidden="1">
-      <c r="A33" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="33">
+      <c r="A33" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="1" t="n">
         <v>908</v>
       </c>
       <c r="D33" s="6" t="s">
@@ -1875,11 +1649,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:26" hidden="1">
-      <c r="A34" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="34">
+      <c r="A34" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -1889,11 +1663,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:26" hidden="1">
-      <c r="A35" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="35">
+      <c r="A35" s="2" t="n">
         <v>43181</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -1903,11 +1677,11 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:26" hidden="1">
-      <c r="A36" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="36">
+      <c r="A36" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="1" t="n">
         <v>135</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -1917,11 +1691,11 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:26" hidden="1">
-      <c r="A37" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="37">
+      <c r="A37" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="1" t="n">
         <v>110</v>
       </c>
       <c r="C37" s="1"/>
@@ -1953,11 +1727,11 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38" spans="1:26" hidden="1">
-      <c r="A38" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="38">
+      <c r="A38" s="2" t="n">
         <v>43185</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="1" t="n">
         <v>122</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -1967,22 +1741,22 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:26" hidden="1">
-      <c r="A39" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="39">
+      <c r="A39" s="2" t="n">
         <v>43187</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="1" t="n">
         <v>750</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:26" hidden="1">
-      <c r="A40" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="40">
+      <c r="A40" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="1" t="n">
         <v>379</v>
       </c>
       <c r="D40" s="6" t="s">
@@ -1992,22 +1766,22 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:26" hidden="1">
-      <c r="A41" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="41">
+      <c r="A41" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="1" t="n">
         <v>240</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:26" hidden="1">
-      <c r="A42" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="42">
+      <c r="A42" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="1" t="n">
         <v>540</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -2017,11 +1791,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:26" hidden="1">
-      <c r="A43" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="43">
+      <c r="A43" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -2031,11 +1805,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:26" hidden="1">
-      <c r="A44" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="44">
+      <c r="A44" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -2045,11 +1819,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:26" hidden="1">
-      <c r="A45" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="45">
+      <c r="A45" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="1" t="n">
         <v>462</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -2059,11 +1833,11 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:26" hidden="1">
-      <c r="A46" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="46">
+      <c r="A46" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46" s="1" t="n">
         <v>70</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -2073,11 +1847,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:26" hidden="1">
-      <c r="A47" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="47">
+      <c r="A47" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -2087,11 +1861,11 @@
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="1:26" hidden="1">
-      <c r="A48" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="48">
+      <c r="A48" s="2" t="n">
         <v>43190</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="1" t="n">
         <v>30</v>
       </c>
       <c r="C48" s="1"/>
@@ -2102,11 +1876,11 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1">
-      <c r="A49" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="49">
+      <c r="A49" s="2" t="n">
         <v>43191</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="1" t="n">
         <v>40</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -2116,11 +1890,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1">
-      <c r="A50" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="50">
+      <c r="A50" s="7" t="n">
         <v>43193</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50" s="1" t="n">
         <v>150</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -2130,11 +1904,11 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1">
-      <c r="A51" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="51">
+      <c r="A51" s="2" t="n">
         <v>43194</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51" s="1" t="n">
         <v>1360</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -2144,11 +1918,11 @@
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1">
-      <c r="A52" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="52">
+      <c r="A52" s="2" t="n">
         <v>43195</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" s="1" t="n">
         <v>94</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -2158,11 +1932,11 @@
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1">
-      <c r="A53" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="53">
+      <c r="A53" s="2" t="n">
         <v>43196</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C53" s="1" t="n">
         <v>48</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -2172,11 +1946,11 @@
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1">
-      <c r="A54" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="54">
+      <c r="A54" s="2" t="n">
         <v>43196</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C54" s="1" t="n">
         <v>205</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -2186,11 +1960,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1">
-      <c r="A55" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="55">
+      <c r="A55" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -2200,11 +1974,11 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1">
-      <c r="A56" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="56">
+      <c r="A56" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56" s="1" t="n">
         <v>421</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -2214,11 +1988,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1">
-      <c r="A57" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="57">
+      <c r="A57" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="1" t="n">
         <v>191</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -2228,11 +2002,11 @@
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1">
-      <c r="A58" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="58">
+      <c r="A58" s="2" t="n">
         <v>43198</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58" s="1" t="n">
         <v>226</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -2242,22 +2016,22 @@
         <v>96</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1">
-      <c r="A59" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="59">
+      <c r="A59" s="2" t="n">
         <v>43200</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59" s="1" t="n">
         <v>250</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1">
-      <c r="A60" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="60">
+      <c r="A60" s="2" t="n">
         <v>43200</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60" s="1" t="n">
         <v>1115</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -2267,11 +2041,11 @@
         <v>99</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1">
-      <c r="A61" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="61">
+      <c r="A61" s="2" t="n">
         <v>43201</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -2281,11 +2055,11 @@
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1">
-      <c r="A62" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="62">
+      <c r="A62" s="2" t="n">
         <v>43201</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62" s="1" t="n">
         <v>88</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -2295,11 +2069,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1">
-      <c r="A63" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="63">
+      <c r="A63" s="2" t="n">
         <v>43203</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -2309,11 +2083,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1">
-      <c r="A64" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="64">
+      <c r="A64" s="2" t="n">
         <v>43203</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C64" s="1" t="n">
         <v>364</v>
       </c>
       <c r="D64" s="1" t="s">
@@ -2323,11 +2097,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1">
-      <c r="A65" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="65">
+      <c r="A65" s="2" t="n">
         <v>43204</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65" s="1" t="n">
         <v>65</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -2337,11 +2111,11 @@
         <v>105</v>
       </c>
     </row>
-    <row r="66" spans="1:5" hidden="1">
-      <c r="A66" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="66">
+      <c r="A66" s="2" t="n">
         <v>43208</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -2351,11 +2125,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1">
-      <c r="A67" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="67">
+      <c r="A67" s="2" t="n">
         <v>43208</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C67" s="1" t="n">
         <v>470</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -2365,11 +2139,11 @@
         <v>107</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1">
-      <c r="A68" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="68">
+      <c r="A68" s="2" t="n">
         <v>43209</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68" s="1" t="n">
         <v>180</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -2379,11 +2153,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1">
-      <c r="A69" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="69">
+      <c r="A69" s="2" t="n">
         <v>43210</v>
       </c>
-      <c r="C69" s="1">
+      <c r="C69" s="1" t="n">
         <v>420</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -2393,11 +2167,11 @@
         <v>109</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1">
-      <c r="A70" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="70">
+      <c r="A70" s="2" t="n">
         <v>43212</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70" s="1" t="n">
         <v>50</v>
       </c>
       <c r="D70" s="1" t="s">
@@ -2407,11 +2181,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1">
-      <c r="A71" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="71">
+      <c r="A71" s="2" t="n">
         <v>43212</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71" s="1" t="n">
         <v>164</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -2421,11 +2195,11 @@
         <v>112</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1">
-      <c r="A72" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="72">
+      <c r="A72" s="2" t="n">
         <v>43215</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B72" s="1" t="n">
         <v>300</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -2435,11 +2209,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1">
-      <c r="A73" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="73">
+      <c r="A73" s="2" t="n">
         <v>43217</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73" s="1" t="n">
         <v>364</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -2449,11 +2223,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1">
-      <c r="A74" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="74">
+      <c r="A74" s="2" t="n">
         <v>43218</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74" s="1" t="n">
         <v>185</v>
       </c>
       <c r="D74" s="1" t="s">
@@ -2463,11 +2237,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1">
-      <c r="A75" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="75">
+      <c r="A75" s="2" t="n">
         <v>43218</v>
       </c>
-      <c r="C75" s="1">
+      <c r="C75" s="1" t="n">
         <v>404</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -2477,11 +2251,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="76" spans="1:5" hidden="1">
-      <c r="A76" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="76">
+      <c r="A76" s="2" t="n">
         <v>43220</v>
       </c>
-      <c r="C76" s="1">
+      <c r="C76" s="1" t="n">
         <v>57</v>
       </c>
       <c r="D76" s="1" t="s">
@@ -2491,11 +2265,11 @@
         <v>114</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1">
-      <c r="A77" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="77">
+      <c r="A77" s="2" t="n">
         <v>43221</v>
       </c>
-      <c r="C77" s="1">
+      <c r="C77" s="1" t="n">
         <v>282</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -2505,11 +2279,11 @@
         <v>116</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1">
-      <c r="A78" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="78">
+      <c r="A78" s="2" t="n">
         <v>43220</v>
       </c>
-      <c r="C78" s="1">
+      <c r="C78" s="1" t="n">
         <v>87</v>
       </c>
       <c r="D78" s="1" t="s">
@@ -2519,11 +2293,11 @@
         <v>117</v>
       </c>
     </row>
-    <row r="79" spans="1:5" hidden="1">
-      <c r="A79" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="79">
+      <c r="A79" s="2" t="n">
         <v>43223</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B79" s="1" t="n">
         <v>1878</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -2533,11 +2307,11 @@
         <v>119</v>
       </c>
     </row>
-    <row r="80" spans="1:5" hidden="1">
-      <c r="A80" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="80">
+      <c r="A80" s="2" t="n">
         <v>43224</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B80" s="1" t="n">
         <v>98</v>
       </c>
       <c r="D80" s="1" t="s">
@@ -2547,11 +2321,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="81" spans="1:5" hidden="1">
-      <c r="A81" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="81">
+      <c r="A81" s="2" t="n">
         <v>43225</v>
       </c>
-      <c r="C81" s="1">
+      <c r="C81" s="1" t="n">
         <v>198</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -2561,11 +2335,11 @@
         <v>122</v>
       </c>
     </row>
-    <row r="82" spans="1:5" hidden="1">
-      <c r="A82" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="82">
+      <c r="A82" s="2" t="n">
         <v>43225</v>
       </c>
-      <c r="C82" s="1">
+      <c r="C82" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -2575,11 +2349,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="83" spans="1:5" hidden="1">
-      <c r="A83" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="83">
+      <c r="A83" s="2" t="n">
         <v>43228</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83" s="1" t="n">
         <v>168</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -2589,11 +2363,11 @@
         <v>124</v>
       </c>
     </row>
-    <row r="84" spans="1:5" hidden="1">
-      <c r="A84" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="84">
+      <c r="A84" s="2" t="n">
         <v>43229</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B84" s="1" t="n">
         <v>240</v>
       </c>
       <c r="D84" s="1" t="s">
@@ -2603,12 +2377,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:5" hidden="1">
-      <c r="A85" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="85">
+      <c r="A85" s="2" t="n">
         <v>43230</v>
       </c>
       <c r="B85" s="1"/>
-      <c r="C85" s="1">
+      <c r="C85" s="1" t="n">
         <v>420</v>
       </c>
       <c r="D85" s="1" t="s">
@@ -2618,11 +2392,11 @@
         <v>126</v>
       </c>
     </row>
-    <row r="86" spans="1:5" hidden="1">
-      <c r="A86" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="86">
+      <c r="A86" s="2" t="n">
         <v>43230</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B86" s="1" t="n">
         <v>200</v>
       </c>
       <c r="C86" s="1"/>
@@ -2633,11 +2407,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="87" spans="1:5" hidden="1">
-      <c r="A87" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="87">
+      <c r="A87" s="2" t="n">
         <v>43230</v>
       </c>
-      <c r="C87" s="1">
+      <c r="C87" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D87" s="1" t="s">
@@ -2647,11 +2421,11 @@
         <v>128</v>
       </c>
     </row>
-    <row r="88" spans="1:5" hidden="1">
-      <c r="A88" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="88">
+      <c r="A88" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B88" s="1" t="n">
         <v>462</v>
       </c>
       <c r="D88" s="1" t="s">
@@ -2661,11 +2435,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="89" spans="1:5" hidden="1">
-      <c r="A89" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="89">
+      <c r="A89" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B89" s="1" t="n">
         <v>499</v>
       </c>
       <c r="D89" s="1" t="s">
@@ -2675,11 +2449,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="90" spans="1:5" hidden="1">
-      <c r="A90" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="90">
+      <c r="A90" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B90" s="1">
+      <c r="B90" s="1" t="n">
         <v>398</v>
       </c>
       <c r="D90" s="1" t="s">
@@ -2689,11 +2463,11 @@
         <v>133</v>
       </c>
     </row>
-    <row r="91" spans="1:5" hidden="1">
-      <c r="A91" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="91">
+      <c r="A91" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B91" s="1">
+      <c r="B91" s="1" t="n">
         <v>226</v>
       </c>
       <c r="D91" s="1" t="s">
@@ -2703,11 +2477,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="92" spans="1:5" hidden="1">
-      <c r="A92" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="92">
+      <c r="A92" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B92" s="1">
+      <c r="B92" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D92" s="1" t="s">
@@ -2717,11 +2491,11 @@
         <v>137</v>
       </c>
     </row>
-    <row r="93" spans="1:5" hidden="1">
-      <c r="A93" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="93">
+      <c r="A93" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="B93" s="1">
+      <c r="B93" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D93" s="1" t="s">
@@ -2731,11 +2505,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="94" spans="1:5" hidden="1">
-      <c r="A94" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="94">
+      <c r="A94" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="C94" s="1">
+      <c r="C94" s="1" t="n">
         <v>340</v>
       </c>
       <c r="D94" s="1" t="s">
@@ -2745,11 +2519,11 @@
         <v>139</v>
       </c>
     </row>
-    <row r="95" spans="1:5" hidden="1">
-      <c r="A95" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="95">
+      <c r="A95" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="B95" s="1">
+      <c r="B95" s="1" t="n">
         <v>510</v>
       </c>
       <c r="D95" s="1" t="s">
@@ -2759,11 +2533,11 @@
         <v>141</v>
       </c>
     </row>
-    <row r="96" spans="1:5" hidden="1">
-      <c r="A96" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="96">
+      <c r="A96" s="2" t="n">
         <v>43233</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B96" s="1" t="n">
         <v>170</v>
       </c>
       <c r="D96" s="1" t="s">
@@ -2773,11 +2547,11 @@
         <v>143</v>
       </c>
     </row>
-    <row r="97" spans="1:5" hidden="1">
-      <c r="A97" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="97">
+      <c r="A97" s="2" t="n">
         <v>43233</v>
       </c>
-      <c r="C97" s="1">
+      <c r="C97" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D97" s="1" t="s">
@@ -2787,11 +2561,11 @@
         <v>144</v>
       </c>
     </row>
-    <row r="98" spans="1:5" hidden="1">
-      <c r="A98" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="98">
+      <c r="A98" s="2" t="n">
         <v>43234</v>
       </c>
-      <c r="C98" s="1">
+      <c r="C98" s="1" t="n">
         <v>299</v>
       </c>
       <c r="D98" s="1" t="s">
@@ -2801,11 +2575,11 @@
         <v>145</v>
       </c>
     </row>
-    <row r="99" spans="1:5" hidden="1">
-      <c r="A99" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="99">
+      <c r="A99" s="2" t="n">
         <v>43236</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99" s="1" t="n">
         <v>3659</v>
       </c>
       <c r="D99" s="1" t="s">
@@ -2815,11 +2589,11 @@
         <v>146</v>
       </c>
     </row>
-    <row r="100" spans="1:5" hidden="1">
-      <c r="A100" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="100">
+      <c r="A100" s="2" t="n">
         <v>43237</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B100" s="1" t="n">
         <v>79</v>
       </c>
       <c r="D100" s="1" t="s">
@@ -2829,11 +2603,11 @@
         <v>147</v>
       </c>
     </row>
-    <row r="101" spans="1:5" hidden="1">
-      <c r="A101" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="101">
+      <c r="A101" s="2" t="n">
         <v>43236</v>
       </c>
-      <c r="C101" s="1">
+      <c r="C101" s="1" t="n">
         <v>173</v>
       </c>
       <c r="D101" s="1" t="s">
@@ -2843,11 +2617,11 @@
         <v>148</v>
       </c>
     </row>
-    <row r="102" spans="1:5" hidden="1">
-      <c r="A102" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="102">
+      <c r="A102" s="2" t="n">
         <v>43240</v>
       </c>
-      <c r="B102" s="1">
+      <c r="B102" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D102" s="1" t="s">
@@ -2857,22 +2631,22 @@
         <v>149</v>
       </c>
     </row>
-    <row r="103" spans="1:5" hidden="1">
-      <c r="A103" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="103">
+      <c r="A103" s="2" t="n">
         <v>43240</v>
       </c>
-      <c r="B103" s="1">
+      <c r="B103" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="104" spans="1:5" hidden="1">
-      <c r="A104" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="104">
+      <c r="A104" s="2" t="n">
         <v>43241</v>
       </c>
-      <c r="B104" s="1">
+      <c r="B104" s="1" t="n">
         <v>4070</v>
       </c>
       <c r="D104" s="1" t="s">
@@ -2882,11 +2656,11 @@
         <v>150</v>
       </c>
     </row>
-    <row r="105" spans="1:5" hidden="1">
-      <c r="A105" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="105">
+      <c r="A105" s="2" t="n">
         <v>43241</v>
       </c>
-      <c r="C105" s="1">
+      <c r="C105" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D105" s="1" t="s">
@@ -2896,11 +2670,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="106" spans="1:5" hidden="1">
-      <c r="A106" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="106">
+      <c r="A106" s="2" t="n">
         <v>43242</v>
       </c>
-      <c r="B106" s="1">
+      <c r="B106" s="1" t="n">
         <v>79</v>
       </c>
       <c r="D106" s="1" t="s">
@@ -2910,11 +2684,11 @@
         <v>152</v>
       </c>
     </row>
-    <row r="107" spans="1:5" hidden="1">
-      <c r="A107" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="107">
+      <c r="A107" s="2" t="n">
         <v>43246</v>
       </c>
-      <c r="B107" s="1">
+      <c r="B107" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D107" s="1" t="s">
@@ -2924,11 +2698,11 @@
         <v>154</v>
       </c>
     </row>
-    <row r="108" spans="1:5" hidden="1">
-      <c r="A108" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="108">
+      <c r="A108" s="2" t="n">
         <v>43247</v>
       </c>
-      <c r="B108" s="1">
+      <c r="B108" s="1" t="n">
         <v>70</v>
       </c>
       <c r="D108" s="1" t="s">
@@ -2938,44 +2712,44 @@
         <v>156</v>
       </c>
     </row>
-    <row r="109" spans="1:5" hidden="1">
-      <c r="A109" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="109">
+      <c r="A109" s="2" t="n">
         <v>43253</v>
       </c>
-      <c r="B109" s="1">
+      <c r="B109" s="1" t="n">
         <v>142</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="110" spans="1:5" hidden="1">
-      <c r="A110" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="110">
+      <c r="A110" s="2" t="n">
         <v>43254</v>
       </c>
-      <c r="B110" s="1">
+      <c r="B110" s="1" t="n">
         <v>90</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="111" spans="1:5" hidden="1">
-      <c r="A111" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="111">
+      <c r="A111" s="2" t="n">
         <v>43260</v>
       </c>
-      <c r="C111" s="1">
+      <c r="C111" s="1" t="n">
         <v>1400</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="112" spans="1:5" hidden="1">
-      <c r="A112" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="112">
+      <c r="A112" s="2" t="n">
         <v>43260</v>
       </c>
-      <c r="C112" s="1">
+      <c r="C112" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D112" s="1" t="s">
@@ -2985,33 +2759,33 @@
         <v>91</v>
       </c>
     </row>
-    <row r="113" spans="1:5" hidden="1">
-      <c r="A113" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="113">
+      <c r="A113" s="2" t="n">
         <v>43264</v>
       </c>
-      <c r="B113" s="1">
+      <c r="B113" s="1" t="n">
         <v>546</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="114" spans="1:5" hidden="1">
-      <c r="A114" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="114">
+      <c r="A114" s="2" t="n">
         <v>43264</v>
       </c>
-      <c r="B114" s="1">
+      <c r="B114" s="1" t="n">
         <v>95</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="115" spans="1:5" hidden="1">
-      <c r="A115" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="115">
+      <c r="A115" s="2" t="n">
         <v>43266</v>
       </c>
-      <c r="B115" s="1">
+      <c r="B115" s="1" t="n">
         <v>394</v>
       </c>
       <c r="D115" s="1" t="s">
@@ -3021,11 +2795,11 @@
         <v>163</v>
       </c>
     </row>
-    <row r="116" spans="1:5" hidden="1">
-      <c r="A116" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="116">
+      <c r="A116" s="2" t="n">
         <v>43266</v>
       </c>
-      <c r="B116" s="1">
+      <c r="B116" s="1" t="n">
         <v>1055</v>
       </c>
       <c r="D116" s="1" t="s">
@@ -3035,11 +2809,11 @@
         <v>165</v>
       </c>
     </row>
-    <row r="117" spans="1:5" hidden="1">
-      <c r="A117" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="117">
+      <c r="A117" s="2" t="n">
         <v>43284</v>
       </c>
-      <c r="C117" s="1">
+      <c r="C117" s="1" t="n">
         <v>274</v>
       </c>
       <c r="D117" s="1" t="s">
@@ -3049,11 +2823,11 @@
         <v>167</v>
       </c>
     </row>
-    <row r="118" spans="1:5" hidden="1">
-      <c r="A118" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="118">
+      <c r="A118" s="2" t="n">
         <v>43283</v>
       </c>
-      <c r="C118" s="1">
+      <c r="C118" s="1" t="n">
         <v>105</v>
       </c>
       <c r="D118" s="1" t="s">
@@ -3063,11 +2837,11 @@
         <v>169</v>
       </c>
     </row>
-    <row r="119" spans="1:5" hidden="1">
-      <c r="A119" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="119">
+      <c r="A119" s="2" t="n">
         <v>43289</v>
       </c>
-      <c r="C119" s="1">
+      <c r="C119" s="1" t="n">
         <v>128</v>
       </c>
       <c r="D119" s="1" t="s">
@@ -3077,11 +2851,11 @@
         <v>171</v>
       </c>
     </row>
-    <row r="120" spans="1:5" hidden="1">
-      <c r="A120" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="120">
+      <c r="A120" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C120" s="1">
+      <c r="C120" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D120" s="1" t="s">
@@ -3091,11 +2865,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="121" spans="1:5" hidden="1">
-      <c r="A121" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="121">
+      <c r="A121" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C121" s="1">
+      <c r="C121" s="1" t="n">
         <v>210</v>
       </c>
       <c r="D121" s="1" t="s">
@@ -3105,44 +2879,44 @@
         <v>173</v>
       </c>
     </row>
-    <row r="122" spans="1:5" hidden="1">
-      <c r="A122" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="122">
+      <c r="A122" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B122" s="1">
+      <c r="B122" s="1" t="n">
         <v>980</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="123" spans="1:5" hidden="1">
-      <c r="A123" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="123">
+      <c r="A123" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B123" s="1">
+      <c r="B123" s="1" t="n">
         <v>1260</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="124" spans="1:5" hidden="1">
-      <c r="A124" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="124">
+      <c r="A124" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B124" s="1">
+      <c r="B124" s="1" t="n">
         <v>3687</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="125" spans="1:5" hidden="1">
-      <c r="A125" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="125">
+      <c r="A125" s="2" t="n">
         <v>43298</v>
       </c>
-      <c r="C125" s="1">
+      <c r="C125" s="1" t="n">
         <v>60</v>
       </c>
       <c r="D125" s="1" t="s">
@@ -3152,55 +2926,55 @@
         <v>178</v>
       </c>
     </row>
-    <row r="126" spans="1:5" hidden="1">
-      <c r="A126" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="126">
+      <c r="A126" s="2" t="n">
         <v>43291</v>
       </c>
-      <c r="C126" s="1">
+      <c r="C126" s="1" t="n">
         <v>404</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="127" spans="1:5" hidden="1">
-      <c r="A127" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="127">
+      <c r="A127" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C127" s="1">
+      <c r="C127" s="1" t="n">
         <v>451</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="128" spans="1:5" hidden="1">
-      <c r="A128" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="128">
+      <c r="A128" s="2" t="n">
         <v>43298</v>
       </c>
-      <c r="C128" s="1">
+      <c r="C128" s="1" t="n">
         <v>708</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="129" spans="1:5" hidden="1">
-      <c r="A129" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="129">
+      <c r="A129" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C129" s="1">
+      <c r="C129" s="1" t="n">
         <v>160</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="130" spans="1:5" hidden="1">
-      <c r="A130" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="130">
+      <c r="A130" s="2" t="n">
         <v>43288</v>
       </c>
-      <c r="C130" s="1">
+      <c r="C130" s="1" t="n">
         <v>72</v>
       </c>
       <c r="D130" s="1" t="s">
@@ -3210,11 +2984,11 @@
         <v>181</v>
       </c>
     </row>
-    <row r="131" spans="1:5" hidden="1">
-      <c r="A131" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="131">
+      <c r="A131" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C131" s="1">
+      <c r="C131" s="1" t="n">
         <v>300</v>
       </c>
       <c r="D131" s="1" t="s">
@@ -3224,11 +2998,11 @@
         <v>183</v>
       </c>
     </row>
-    <row r="132" spans="1:5" hidden="1">
-      <c r="A132" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="132">
+      <c r="A132" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C132" s="1">
+      <c r="C132" s="1" t="n">
         <v>230</v>
       </c>
       <c r="D132" s="1" t="s">
@@ -3238,22 +3012,22 @@
         <v>185</v>
       </c>
     </row>
-    <row r="133" spans="1:5" hidden="1">
-      <c r="A133" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="133">
+      <c r="A133" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C133" s="1">
+      <c r="C133" s="1" t="n">
         <v>454</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="134" spans="1:5" hidden="1">
-      <c r="A134" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="134">
+      <c r="A134" s="2" t="n">
         <v>43299</v>
       </c>
-      <c r="C134" s="1">
+      <c r="C134" s="1" t="n">
         <v>686</v>
       </c>
       <c r="D134" s="1" t="s">
@@ -3263,11 +3037,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="135" spans="1:5" hidden="1">
-      <c r="A135" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="135">
+      <c r="A135" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C135" s="1">
+      <c r="C135" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D135" s="1" t="s">
@@ -3277,11 +3051,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="136" spans="1:5" hidden="1">
-      <c r="A136" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="136">
+      <c r="A136" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C136" s="1">
+      <c r="C136" s="1" t="n">
         <v>2067</v>
       </c>
       <c r="D136" s="1" t="s">
@@ -3291,11 +3065,11 @@
         <v>186</v>
       </c>
     </row>
-    <row r="137" spans="1:5" hidden="1">
-      <c r="A137" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="137">
+      <c r="A137" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B137" s="1">
+      <c r="B137" s="1" t="n">
         <v>109</v>
       </c>
       <c r="D137" s="1" t="s">
@@ -3305,11 +3079,11 @@
         <v>187</v>
       </c>
     </row>
-    <row r="138" spans="1:5" hidden="1">
-      <c r="A138" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="138">
+      <c r="A138" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B138" s="1">
+      <c r="B138" s="1" t="n">
         <v>97</v>
       </c>
       <c r="D138" s="1" t="s">
@@ -3319,11 +3093,11 @@
         <v>188</v>
       </c>
     </row>
-    <row r="139" spans="1:5" hidden="1">
-      <c r="A139" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="139">
+      <c r="A139" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B139" s="1">
+      <c r="B139" s="1" t="n">
         <v>1437</v>
       </c>
       <c r="D139" s="1" t="s">
@@ -3333,11 +3107,11 @@
         <v>189</v>
       </c>
     </row>
-    <row r="140" spans="1:5" hidden="1">
-      <c r="A140" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="140">
+      <c r="A140" s="2" t="n">
         <v>43306</v>
       </c>
-      <c r="C140" s="1">
+      <c r="C140" s="1" t="n">
         <v>650</v>
       </c>
       <c r="D140" s="1" t="s">
@@ -3347,11 +3121,11 @@
         <v>190</v>
       </c>
     </row>
-    <row r="141" spans="1:5" hidden="1">
-      <c r="A141" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="141">
+      <c r="A141" s="2" t="n">
         <v>43305</v>
       </c>
-      <c r="C141" s="1">
+      <c r="C141" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D141" s="1" t="s">
@@ -3361,11 +3135,11 @@
         <v>191</v>
       </c>
     </row>
-    <row r="142" spans="1:5" hidden="1">
-      <c r="A142" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="142">
+      <c r="A142" s="2" t="n">
         <v>43309</v>
       </c>
-      <c r="C142" s="1">
+      <c r="C142" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D142" s="1" t="s">
@@ -3375,11 +3149,11 @@
         <v>192</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="14" hidden="1">
-      <c r="A143" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="0" r="143">
+      <c r="A143" s="2" t="n">
         <v>43306</v>
       </c>
-      <c r="B143" s="1">
+      <c r="B143" s="1" t="n">
         <v>167</v>
       </c>
       <c r="D143" s="1" t="s">
@@ -3389,11 +3163,11 @@
         <v>193</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="14" hidden="1">
-      <c r="A144" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="0" r="144">
+      <c r="A144" s="2" t="n">
         <v>43304</v>
       </c>
-      <c r="C144" s="1">
+      <c r="C144" s="1" t="n">
         <v>93</v>
       </c>
       <c r="D144" s="1" t="s">
@@ -3403,11 +3177,11 @@
         <v>194</v>
       </c>
     </row>
-    <row r="145" spans="1:5" hidden="1">
-      <c r="A145" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="145">
+      <c r="A145" s="2" t="n">
         <v>43305</v>
       </c>
-      <c r="C145" s="1">
+      <c r="C145" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D145" s="1" t="s">
@@ -3417,11 +3191,11 @@
         <v>195</v>
       </c>
     </row>
-    <row r="146" spans="1:5" hidden="1">
-      <c r="A146" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="146">
+      <c r="A146" s="2" t="n">
         <v>43303</v>
       </c>
-      <c r="C146" s="1">
+      <c r="C146" s="1" t="n">
         <v>244</v>
       </c>
       <c r="D146" s="1" t="s">
@@ -3431,11 +3205,11 @@
         <v>196</v>
       </c>
     </row>
-    <row r="147" spans="1:5" hidden="1">
-      <c r="A147" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="147">
+      <c r="A147" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C147" s="1">
+      <c r="C147" s="1" t="n">
         <v>482</v>
       </c>
       <c r="D147" s="1" t="s">
@@ -3445,11 +3219,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="148" spans="1:5" hidden="1">
-      <c r="A148" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="148">
+      <c r="A148" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C148" s="1">
+      <c r="C148" s="1" t="n">
         <v>172</v>
       </c>
       <c r="D148" s="1" t="s">
@@ -3459,44 +3233,44 @@
         <v>199</v>
       </c>
     </row>
-    <row r="149" spans="1:5" hidden="1">
-      <c r="A149" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="149">
+      <c r="A149" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="B149" s="1">
+      <c r="B149" s="1" t="n">
         <v>89</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="150" spans="1:5" hidden="1">
-      <c r="A150" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="150">
+      <c r="A150" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="C150" s="1">
+      <c r="C150" s="1" t="n">
         <v>107</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="151" spans="1:5" hidden="1">
-      <c r="A151" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="151">
+      <c r="A151" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="C151" s="1">
+      <c r="C151" s="1" t="n">
         <v>124</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="152" spans="1:5" hidden="1">
-      <c r="A152" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="152">
+      <c r="A152" s="7" t="n">
         <v>43316</v>
       </c>
-      <c r="C152" s="1">
+      <c r="C152" s="1" t="n">
         <v>4500</v>
       </c>
       <c r="D152" s="1" t="s">
@@ -3506,11 +3280,11 @@
         <v>202</v>
       </c>
     </row>
-    <row r="153" spans="1:5" hidden="1">
-      <c r="A153" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="153">
+      <c r="A153" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C153" s="1">
+      <c r="C153" s="1" t="n">
         <v>247</v>
       </c>
       <c r="D153" s="1" t="s">
@@ -3520,11 +3294,11 @@
         <v>204</v>
       </c>
     </row>
-    <row r="154" spans="1:5" hidden="1">
-      <c r="A154" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="154">
+      <c r="A154" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C154" s="1">
+      <c r="C154" s="1" t="n">
         <v>1150</v>
       </c>
       <c r="D154" s="1" t="s">
@@ -3534,11 +3308,11 @@
         <v>205</v>
       </c>
     </row>
-    <row r="155" spans="1:5" hidden="1">
-      <c r="A155" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="155">
+      <c r="A155" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C155" s="1">
+      <c r="C155" s="1" t="n">
         <v>313</v>
       </c>
       <c r="D155" s="1" t="s">
@@ -3548,11 +3322,11 @@
         <v>207</v>
       </c>
     </row>
-    <row r="156" spans="1:5" hidden="1">
-      <c r="A156" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="156">
+      <c r="A156" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="B156" s="1">
+      <c r="B156" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D156" s="1" t="s">
@@ -3562,11 +3336,11 @@
         <v>209</v>
       </c>
     </row>
-    <row r="157" spans="1:5" hidden="1">
-      <c r="A157" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="157">
+      <c r="A157" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="C157" s="1">
+      <c r="C157" s="1" t="n">
         <v>710</v>
       </c>
       <c r="D157" s="1" t="s">
@@ -3576,11 +3350,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="158" spans="1:5">
-      <c r="A158" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="158">
+      <c r="A158" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="C158" s="1">
+      <c r="C158" s="1" t="n">
         <v>100</v>
       </c>
       <c r="D158" s="1" t="s">
@@ -3590,11 +3364,11 @@
         <v>212</v>
       </c>
     </row>
-    <row r="159" spans="1:5">
-      <c r="A159" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="159">
+      <c r="A159" s="2" t="n">
         <v>43319</v>
       </c>
-      <c r="B159" s="1">
+      <c r="B159" s="1" t="n">
         <v>78</v>
       </c>
       <c r="D159" s="1" t="s">
@@ -3604,22 +3378,22 @@
         <v>213</v>
       </c>
     </row>
-    <row r="160" spans="1:5">
-      <c r="A160" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="160">
+      <c r="A160" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="B160" s="1">
+      <c r="B160" s="1" t="n">
         <v>1840</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="161" spans="1:5">
-      <c r="A161" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="161">
+      <c r="A161" s="2" t="n">
         <v>43322</v>
       </c>
-      <c r="B161" s="1">
+      <c r="B161" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D161" s="1" t="s">
@@ -3629,11 +3403,11 @@
         <v>216</v>
       </c>
     </row>
-    <row r="162" spans="1:5">
-      <c r="A162" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="162">
+      <c r="A162" s="7" t="n">
         <v>43324</v>
       </c>
-      <c r="C162" s="1">
+      <c r="C162" s="1" t="n">
         <v>230</v>
       </c>
       <c r="D162" s="1" t="s">
@@ -3643,11 +3417,11 @@
         <v>217</v>
       </c>
     </row>
-    <row r="163" spans="1:5">
-      <c r="A163" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="163">
+      <c r="A163" s="7" t="n">
         <v>43326</v>
       </c>
-      <c r="C163" s="1">
+      <c r="C163" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D163" s="1" t="s">
@@ -3657,11 +3431,11 @@
         <v>219</v>
       </c>
     </row>
-    <row r="164" spans="1:5">
-      <c r="A164" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="164">
+      <c r="A164" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="B164" s="1">
+      <c r="B164" s="1" t="n">
         <v>45</v>
       </c>
       <c r="D164" s="1" t="s">
@@ -3671,922 +3445,941 @@
         <v>221</v>
       </c>
     </row>
-    <row r="165" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A165" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="165">
+      <c r="A165" s="10" t="n">
         <v>43327</v>
       </c>
-      <c r="C165">
+      <c r="C165" s="0" t="n">
         <v>486</v>
       </c>
-      <c r="D165" t="s">
+      <c r="D165" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E165" t="s">
+      <c r="E165" s="0" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="166" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A166" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="166">
+      <c r="A166" s="10" t="n">
         <v>43329</v>
       </c>
-      <c r="C166">
+      <c r="C166" s="0" t="n">
         <v>92</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D166" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="E166" t="s">
+      <c r="E166" s="0" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="167" spans="1:5">
-      <c r="A167" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="167">
+      <c r="A167" s="10" t="n">
         <v>43331</v>
       </c>
-      <c r="C167">
+      <c r="C167" s="0" t="n">
         <v>310</v>
       </c>
-      <c r="D167" t="s">
+      <c r="D167" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="E167" t="s">
+      <c r="E167" s="0" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="168" spans="1:5">
-      <c r="A168" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="168">
+      <c r="A168" s="10" t="n">
         <v>43334</v>
       </c>
-      <c r="C168">
+      <c r="C168" s="0" t="n">
         <v>464</v>
       </c>
-      <c r="D168" t="s">
+      <c r="D168" s="0" t="s">
         <v>218</v>
       </c>
       <c r="E168" s="11" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="169" spans="1:5">
-      <c r="A169" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="169">
+      <c r="A169" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="C169">
+      <c r="C169" s="0" t="n">
         <v>726</v>
       </c>
-      <c r="D169" t="s">
+      <c r="D169" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="E169" t="s">
+      <c r="E169" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="170" spans="1:5">
-      <c r="A170" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="170">
+      <c r="A170" s="10" t="n">
         <v>43337</v>
       </c>
-      <c r="C170">
+      <c r="C170" s="0" t="n">
         <v>544</v>
       </c>
-      <c r="D170" t="s">
+      <c r="D170" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E170" t="s">
+      <c r="E170" s="0" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="171" spans="1:5">
-      <c r="A171" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="171">
+      <c r="A171" s="10" t="n">
         <v>43337</v>
       </c>
-      <c r="B171">
+      <c r="B171" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D171" t="s">
+      <c r="D171" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="E171" t="s">
+      <c r="E171" s="0" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="172" spans="1:5">
-      <c r="A172" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="172">
+      <c r="A172" s="10" t="n">
         <v>43341</v>
       </c>
-      <c r="C172">
+      <c r="C172" s="0" t="n">
         <v>830</v>
       </c>
-      <c r="D172" t="s">
+      <c r="D172" s="0" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="173" spans="1:5">
-      <c r="A173" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="173">
+      <c r="A173" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="C173">
+      <c r="C173" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="D173" t="s">
+      <c r="D173" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="E173" t="s">
+      <c r="E173" s="0" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="174" spans="1:5">
-      <c r="A174" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="174">
+      <c r="A174" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="B174">
+      <c r="B174" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D174" t="s">
+      <c r="D174" s="0" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="175" spans="1:5">
-      <c r="A175" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="175">
+      <c r="A175" s="10" t="n">
         <v>43344</v>
       </c>
-      <c r="B175">
+      <c r="B175" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="D175" t="s">
+      <c r="D175" s="0" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="176" spans="1:5">
-      <c r="A176" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="176">
+      <c r="A176" s="10" t="n">
         <v>43344</v>
       </c>
-      <c r="B176">
+      <c r="B176" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D176" t="s">
+      <c r="D176" s="0" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="177" spans="1:5">
-      <c r="A177" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="177">
+      <c r="A177" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C177">
+      <c r="C177" s="0" t="n">
         <v>607</v>
       </c>
-      <c r="D177" t="s">
+      <c r="D177" s="0" t="s">
         <v>235</v>
       </c>
-      <c r="E177" t="s">
+      <c r="E177" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="178" spans="1:5">
-      <c r="A178" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="178">
+      <c r="A178" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C178">
+      <c r="C178" s="0" t="n">
         <v>444</v>
       </c>
-      <c r="D178" t="s">
+      <c r="D178" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E178" t="s">
+      <c r="E178" s="0" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="179" spans="1:5">
-      <c r="A179" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="179">
+      <c r="A179" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C179">
+      <c r="C179" s="0" t="n">
         <v>312</v>
       </c>
-      <c r="D179" t="s">
+      <c r="D179" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="E179" t="s">
+      <c r="E179" s="0" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="180" spans="1:5">
-      <c r="A180" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="180">
+      <c r="A180" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C180">
+      <c r="C180" s="0" t="n">
         <v>501</v>
       </c>
-      <c r="D180" t="s">
+      <c r="D180" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E180" t="s">
+      <c r="E180" s="0" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="181" spans="1:5">
-      <c r="A181" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="181">
+      <c r="A181" s="10" t="n">
         <v>43349</v>
       </c>
-      <c r="C181">
+      <c r="C181" s="0" t="n">
         <v>711</v>
       </c>
-      <c r="D181" t="s">
+      <c r="D181" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="E181" t="s">
+      <c r="E181" s="0" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="182" spans="1:5">
-      <c r="A182" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="182">
+      <c r="A182" s="10" t="n">
         <v>43354</v>
       </c>
-      <c r="B182">
+      <c r="B182" s="0" t="n">
         <v>126</v>
       </c>
-      <c r="D182" t="s">
+      <c r="D182" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="E182" t="s">
+      <c r="E182" s="0" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="183" spans="1:5">
-      <c r="A183" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="183">
+      <c r="A183" s="10" t="n">
         <v>43354</v>
       </c>
-      <c r="C183">
+      <c r="C183" s="0" t="n">
         <v>450</v>
       </c>
-      <c r="D183" t="s">
+      <c r="D183" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="E183" t="s">
+      <c r="E183" s="0" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="184" spans="1:5">
-      <c r="A184" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="184">
+      <c r="A184" s="10" t="n">
         <v>43361</v>
       </c>
-      <c r="C184">
+      <c r="C184" s="0" t="n">
         <v>660</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D184" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="E184" t="s">
+      <c r="E184" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="185" spans="1:5">
-      <c r="A185" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="185">
+      <c r="A185" s="10" t="n">
         <v>43363</v>
       </c>
-      <c r="C185">
+      <c r="C185" s="0" t="n">
         <v>230</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D185" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="E185" t="s">
+      <c r="E185" s="0" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="186" spans="1:5">
-      <c r="A186" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="186">
+      <c r="A186" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B186">
+      <c r="B186" s="0" t="n">
         <v>4859</v>
       </c>
-      <c r="D186" t="s">
+      <c r="D186" s="0" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="187" spans="1:5">
-      <c r="A187" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="187">
+      <c r="A187" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B187">
+      <c r="B187" s="0" t="n">
         <v>295</v>
       </c>
-      <c r="D187" t="s">
+      <c r="D187" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="E187" t="s">
+      <c r="E187" s="0" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="188" spans="1:5">
-      <c r="A188" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="188">
+      <c r="A188" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B188">
+      <c r="B188" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D188" t="s">
+      <c r="D188" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="E188" t="s">
+      <c r="E188" s="0" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="189" spans="1:5">
-      <c r="A189" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="189">
+      <c r="A189" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B189">
+      <c r="B189" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="D189" t="s">
+      <c r="D189" s="0" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="190" spans="1:5">
-      <c r="A190" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="190">
+      <c r="A190" s="10" t="n">
         <v>43378</v>
       </c>
-      <c r="B190">
+      <c r="B190" s="0" t="n">
         <v>506</v>
       </c>
-      <c r="D190" t="s">
+      <c r="D190" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="E190" t="s">
+      <c r="E190" s="0" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="191" spans="1:5">
-      <c r="A191" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="191">
+      <c r="A191" s="10" t="n">
         <v>43379</v>
       </c>
-      <c r="B191">
+      <c r="B191" s="0" t="n">
         <v>350</v>
       </c>
-      <c r="D191" t="s">
+      <c r="D191" s="0" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="192" spans="1:5" ht="20" customHeight="1">
-      <c r="A192" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="20" outlineLevel="0" r="192">
+      <c r="A192" s="10" t="n">
         <v>43383</v>
       </c>
-      <c r="B192">
+      <c r="B192" s="0" t="n">
         <v>189</v>
       </c>
-      <c r="D192" t="s">
+      <c r="D192" s="0" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="193" spans="1:5">
-      <c r="A193" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="193">
+      <c r="A193" s="10" t="n">
         <v>43387</v>
       </c>
-      <c r="B193">
+      <c r="B193" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="D193" t="s">
+      <c r="D193" s="0" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="194" spans="1:5">
-      <c r="A194" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="194">
+      <c r="A194" s="10" t="n">
         <v>43387</v>
       </c>
-      <c r="B194">
+      <c r="B194" s="0" t="n">
         <v>307</v>
       </c>
-      <c r="D194" t="s">
+      <c r="D194" s="0" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="195" spans="1:5">
-      <c r="C195">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="195">
+      <c r="C195" s="0" t="n">
         <v>3705</v>
       </c>
-      <c r="E195" t="s">
+      <c r="E195" s="0" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="196" spans="1:5">
-      <c r="A196" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="196">
+      <c r="A196" s="10" t="n">
         <v>43385</v>
       </c>
-      <c r="C196">
+      <c r="C196" s="0" t="n">
         <v>608</v>
       </c>
-      <c r="D196" t="s">
+      <c r="D196" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E196" t="s">
+      <c r="E196" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="197" spans="1:5">
-      <c r="A197" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="197">
+      <c r="A197" s="10" t="n">
         <v>43391</v>
       </c>
-      <c r="B197">
+      <c r="B197" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="D197" t="s">
+      <c r="D197" s="0" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="198" spans="1:5">
-      <c r="A198" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="198">
+      <c r="A198" s="10" t="n">
         <v>43392</v>
       </c>
-      <c r="B198">
+      <c r="B198" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="D198" t="s">
+      <c r="D198" s="0" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="199" spans="1:5">
-      <c r="A199" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="199">
+      <c r="A199" s="10" t="n">
         <v>43393</v>
       </c>
-      <c r="B199">
+      <c r="B199" s="0" t="n">
         <v>177</v>
       </c>
-      <c r="D199" t="s">
+      <c r="D199" s="0" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="200" spans="1:5">
-      <c r="A200" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="200">
+      <c r="A200" s="10" t="n">
         <v>43393</v>
       </c>
-      <c r="C200">
+      <c r="C200" s="0" t="n">
         <v>125</v>
       </c>
-      <c r="D200" t="s">
+      <c r="D200" s="0" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="201" spans="1:5">
-      <c r="A201" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="201">
+      <c r="A201" s="10" t="n">
         <v>43395</v>
       </c>
-      <c r="B201">
+      <c r="B201" s="0" t="n">
         <v>2800</v>
       </c>
       <c r="D201" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="E201" t="s">
+      <c r="E201" s="0" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="202" spans="1:5">
-      <c r="A202" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="202">
+      <c r="A202" s="10" t="n">
         <v>43395</v>
       </c>
-      <c r="C202">
+      <c r="C202" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="D202" t="s">
+      <c r="D202" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="E202" t="s">
+      <c r="E202" s="0" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="203" spans="1:5">
-      <c r="A203" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="203">
+      <c r="A203" s="10" t="n">
         <v>43396</v>
       </c>
-      <c r="C203">
+      <c r="C203" s="0" t="n">
         <v>692</v>
       </c>
-      <c r="D203" t="s">
+      <c r="D203" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E203" t="s">
+      <c r="E203" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="204" spans="1:5">
-      <c r="A204" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="204">
+      <c r="A204" s="10" t="n">
         <v>43397</v>
       </c>
-      <c r="C204">
+      <c r="C204" s="0" t="n">
         <v>4935</v>
       </c>
-      <c r="D204" t="s">
+      <c r="D204" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="E204" t="s">
+      <c r="E204" s="0" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="205" spans="1:5" ht="10" customHeight="1">
-      <c r="A205" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10" outlineLevel="0" r="205">
+      <c r="A205" s="10" t="n">
         <v>43398</v>
       </c>
-      <c r="B205">
+      <c r="B205" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="D205" t="s">
+      <c r="D205" s="0" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="206" spans="1:5">
-      <c r="A206" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="206">
+      <c r="A206" s="10" t="n">
         <v>43398</v>
       </c>
-      <c r="B206">
+      <c r="B206" s="0" t="n">
         <v>370</v>
       </c>
-      <c r="D206" t="s">
+      <c r="D206" s="0" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="207" spans="1:5">
-      <c r="A207" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="207">
+      <c r="A207" s="10" t="n">
         <v>43398</v>
       </c>
-      <c r="B207">
+      <c r="B207" s="0" t="n">
         <v>4966</v>
       </c>
-      <c r="D207" t="s">
+      <c r="D207" s="0" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="208" spans="1:5">
-      <c r="A208" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="208">
+      <c r="A208" s="10" t="n">
         <v>43397</v>
       </c>
-      <c r="C208">
+      <c r="C208" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="D208" t="s">
+      <c r="D208" s="0" t="s">
         <v>265</v>
       </c>
-      <c r="E208" t="s">
+      <c r="E208" s="0" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="209" spans="1:5">
-      <c r="A209" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="209">
+      <c r="A209" s="10" t="n">
         <v>43399</v>
       </c>
-      <c r="B209">
+      <c r="B209" s="0" t="n">
         <v>182</v>
       </c>
-      <c r="D209" t="s">
+      <c r="D209" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="E209" t="s">
+      <c r="E209" s="0" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="210" spans="1:5">
-      <c r="A210" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="210">
+      <c r="A210" s="10" t="n">
         <v>43401</v>
       </c>
-      <c r="B210">
+      <c r="B210" s="0" t="n">
         <v>700</v>
       </c>
-      <c r="D210" t="s">
+      <c r="D210" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="E210" t="s">
+      <c r="E210" s="0" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="211" spans="1:5">
-      <c r="A211" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="211">
+      <c r="A211" s="10" t="n">
         <v>43405</v>
       </c>
-      <c r="B211">
+      <c r="B211" s="0" t="n">
         <v>274</v>
       </c>
-      <c r="D211" t="s">
+      <c r="D211" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="E211" t="s">
+      <c r="E211" s="0" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="212" spans="1:5">
-      <c r="A212" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="212">
+      <c r="A212" s="10" t="n">
         <v>43405</v>
       </c>
-      <c r="C212">
+      <c r="C212" s="0" t="n">
         <v>590</v>
       </c>
-      <c r="D212" t="s">
+      <c r="D212" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="E212" t="s">
+      <c r="E212" s="0" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="213" spans="1:5" ht="14">
-      <c r="A213" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="213">
+      <c r="A213" s="10" t="n">
         <v>43407</v>
       </c>
-      <c r="C213">
+      <c r="C213" s="0" t="n">
         <v>1275</v>
       </c>
       <c r="D213" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="E213" t="s">
+      <c r="E213" s="0" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="214" spans="1:5" ht="14">
-      <c r="A214" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="214">
+      <c r="A214" s="10" t="n">
         <v>43407</v>
       </c>
-      <c r="C214">
+      <c r="C214" s="0" t="n">
         <v>4781</v>
       </c>
       <c r="D214" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="E214" t="s">
+      <c r="E214" s="0" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="215" spans="1:5" ht="14">
-      <c r="A215" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="215">
+      <c r="A215" s="10" t="n">
         <v>43407</v>
       </c>
-      <c r="C215">
+      <c r="C215" s="0" t="n">
         <v>4781</v>
       </c>
       <c r="D215" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="E215" t="s">
+      <c r="E215" s="0" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="216" spans="1:5">
-      <c r="A216" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="216">
+      <c r="A216" s="10" t="n">
         <v>43406</v>
       </c>
-      <c r="C216">
+      <c r="C216" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D216" t="s">
+      <c r="D216" s="0" t="s">
         <v>272</v>
       </c>
-      <c r="E216" t="s">
+      <c r="E216" s="0" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="217" spans="1:5">
-      <c r="A217" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="217">
+      <c r="A217" s="10" t="n">
         <v>43409</v>
       </c>
-      <c r="C217">
+      <c r="C217" s="0" t="n">
         <v>677</v>
       </c>
-      <c r="D217" t="s">
+      <c r="D217" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E217" t="s">
+      <c r="E217" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="218" spans="1:5" ht="14">
-      <c r="A218" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="218">
+      <c r="A218" s="10" t="n">
         <v>43410</v>
       </c>
-      <c r="B218">
+      <c r="B218" s="0" t="n">
         <v>285</v>
       </c>
       <c r="D218" s="13" t="s">
         <v>274</v>
       </c>
-      <c r="E218" t="s">
+      <c r="E218" s="0" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="219" spans="1:5" ht="14">
-      <c r="A219" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="219">
+      <c r="A219" s="10" t="n">
         <v>43410</v>
       </c>
-      <c r="B219">
+      <c r="B219" s="0" t="n">
         <v>125</v>
       </c>
       <c r="D219" s="13" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="220" spans="1:5" ht="14">
-      <c r="A220" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="220">
+      <c r="A220" s="10" t="n">
         <v>43409</v>
       </c>
-      <c r="B220">
+      <c r="B220" s="0" t="n">
         <v>85</v>
       </c>
       <c r="D220" s="13" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="221" spans="1:5" ht="14">
-      <c r="A221" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="221">
+      <c r="A221" s="10" t="n">
         <v>43410</v>
       </c>
-      <c r="B221">
+      <c r="B221" s="0" t="n">
         <v>44</v>
       </c>
       <c r="D221" s="13" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="222" spans="1:5">
-      <c r="A222" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="222">
+      <c r="A222" s="10" t="n">
         <v>43412</v>
       </c>
-      <c r="C222">
+      <c r="C222" s="0" t="n">
         <v>190</v>
       </c>
-      <c r="D222" t="s">
+      <c r="D222" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="E222" t="s">
+      <c r="E222" s="0" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="223" spans="1:5" ht="14">
-      <c r="A223" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="223">
+      <c r="A223" s="10" t="n">
         <v>43415</v>
       </c>
-      <c r="B223">
+      <c r="B223" s="0" t="n">
         <v>189</v>
       </c>
       <c r="D223" s="13" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="224" spans="1:5" ht="14">
-      <c r="A224" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="224">
+      <c r="A224" s="10" t="n">
         <v>43415</v>
       </c>
-      <c r="B224">
+      <c r="B224" s="0" t="n">
         <v>336</v>
       </c>
       <c r="D224" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="E224" t="s">
+      <c r="E224" s="0" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="225" spans="1:5" ht="14">
-      <c r="A225" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="225">
+      <c r="A225" s="10" t="n">
         <v>43419</v>
       </c>
-      <c r="B225">
+      <c r="B225" s="0" t="n">
         <v>158</v>
       </c>
       <c r="D225" s="13" t="s">
         <v>282</v>
       </c>
-      <c r="E225" t="s">
+      <c r="E225" s="0" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="226" spans="1:5">
-      <c r="A226" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="226">
+      <c r="A226" s="10" t="n">
         <v>43418</v>
       </c>
-      <c r="C226">
+      <c r="C226" s="0" t="n">
         <v>642</v>
       </c>
-      <c r="D226" t="s">
+      <c r="D226" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E226" t="s">
+      <c r="E226" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="227" spans="1:5">
-      <c r="A227" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="227">
+      <c r="A227" s="10" t="n">
         <v>43419</v>
       </c>
-      <c r="C227">
+      <c r="C227" s="0" t="n">
         <v>370</v>
       </c>
-      <c r="D227" t="s">
+      <c r="D227" s="0" t="s">
         <v>284</v>
       </c>
-      <c r="E227" t="s">
+      <c r="E227" s="0" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="228" spans="1:5">
-      <c r="A228" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="228">
+      <c r="A228" s="10" t="n">
         <v>43419</v>
       </c>
-      <c r="C228">
+      <c r="C228" s="0" t="n">
         <v>222</v>
       </c>
-      <c r="D228" t="s">
+      <c r="D228" s="0" t="s">
         <v>286</v>
       </c>
-      <c r="E228" t="s">
+      <c r="E228" s="0" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="229" spans="1:5">
-      <c r="A229" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="229">
+      <c r="A229" s="10" t="n">
         <v>43421</v>
       </c>
-      <c r="B229">
+      <c r="B229" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="D229" t="s">
+      <c r="D229" s="0" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="230" spans="1:5">
-      <c r="A230" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="230">
+      <c r="A230" s="10" t="n">
         <v>43422</v>
       </c>
-      <c r="B230">
+      <c r="B230" s="0" t="n">
         <v>158</v>
       </c>
-      <c r="D230" t="s">
+      <c r="D230" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="E230" t="s">
+      <c r="E230" s="0" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="231" spans="1:5">
-      <c r="A231" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="231">
+      <c r="A231" s="10" t="n">
         <v>43422</v>
       </c>
-      <c r="B231">
+      <c r="B231" s="0" t="n">
         <v>159</v>
       </c>
-      <c r="D231" t="s">
+      <c r="D231" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="E231" t="s">
+      <c r="E231" s="0" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="232" spans="1:5">
-      <c r="A232" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="232">
+      <c r="A232" s="10" t="n">
         <v>43421</v>
       </c>
-      <c r="C232">
+      <c r="C232" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="D232" t="s">
+      <c r="D232" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="E232" t="s">
+      <c r="E232" s="0" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="233" spans="1:5">
-      <c r="A233" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="233">
+      <c r="A233" s="10" t="n">
         <v>43422</v>
       </c>
-      <c r="B233">
+      <c r="B233" s="0" t="n">
         <v>11649</v>
       </c>
-      <c r="D233" t="s">
+      <c r="D233" s="0" t="s">
         <v>290</v>
       </c>
-      <c r="E233" t="s">
+      <c r="E233" s="0" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="241" spans="2:3">
-      <c r="B241">
-        <f>SUM(B2:B240)</f>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="234">
+      <c r="A234" s="10" t="n">
+        <v>43426</v>
+      </c>
+      <c r="C234" s="0" t="n">
+        <v>308</v>
+      </c>
+      <c r="D234" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="E234" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="241">
+      <c r="B241" s="0" t="n">
+        <f aca="false">SUM(B2:B240)</f>
         <v>69400</v>
       </c>
-      <c r="C241">
-        <f>SUM(C2:C240)</f>
-        <v>66159</v>
+      <c r="C241" s="0" t="n">
+        <f aca="false">SUM(C2:C240)</f>
+        <v>66467</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A30:Z32">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule aboveAverage="0" bottom="0" dxfId="0" operator="expression" percent="0" priority="2" rank="0" text="" type="expression">
       <formula>LEN(TRIM(A30))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D33" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D40" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D201" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink display="netonnet.se" ref="D33" r:id="rId1"/>
+    <hyperlink display="www.vidaxl.se" ref="D40" r:id="rId2"/>
+    <hyperlink display="https://www.vardia.se/" ref="D201" r:id="rId3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cost update Jenny Nov 27
</commit_message>
<xml_diff>
--- a/Cost.xlsx
+++ b/Cost.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chengkaiyan/github/cost/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE21A6D-122B-9C47-B93C-A87C791B66D1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="299">
   <si>
     <t>日期</t>
   </si>
@@ -902,61 +897,92 @@
   </si>
   <si>
     <t>菠萝 饮料</t>
+  </si>
+  <si>
+    <t>Kokosolja, tomat plommon, etc</t>
+  </si>
+  <si>
+    <t>willys aninge</t>
+  </si>
+  <si>
+    <t>majkyckling, kottbullar, libero series, etc</t>
+  </si>
+  <si>
+    <t>ica nära näsbydal</t>
+  </si>
+  <si>
+    <t>blossa,grape rod,pangasiusfile, tebaguette fransk, etc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="yyyy/m/d"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt formatCode="YYYY/M/D" numFmtId="165"/>
+    <numFmt formatCode="M/D/YYYY" numFmtId="166"/>
+    <numFmt formatCode="YYYY\-MM\-DD" numFmtId="167"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="10">
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <family val="0"/>
       <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
       <name val="Arial"/>
       <family val="2"/>
+      <sz val="10"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF666666"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF666666"/>
+      <sz val="11"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0563C1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF0563C1"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0563C1"/>
       <name val="FreeSans"/>
       <family val="2"/>
+      <color rgb="FF0563C1"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF444444"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF444444"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="5">
@@ -986,7 +1012,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
@@ -994,31 +1020,100 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+  <cellStyleXfs count="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="167" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="20">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="7">
+    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle builtinId="8" customBuiltin="false" name="*unknown*" xfId="20"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1029,7 +1124,6 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1088,339 +1182,31 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF444444"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z241"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:Z260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A223" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E236" sqref="E236"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A244" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E242" activeCellId="0" pane="topLeft" sqref="E242"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="3" width="14.5"/>
-    <col min="4" max="4" width="26"/>
-    <col min="5" max="5" width="37.83203125"/>
-    <col min="6" max="1025" width="14.5"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="14.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1437,11 +1223,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1">
-      <c r="A2" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="2">
+      <c r="A2" s="2" t="n">
         <v>43121</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="1" t="n">
         <v>250</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1451,11 +1237,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1">
-      <c r="A3" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="3">
+      <c r="A3" s="2" t="n">
         <v>43122</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="1" t="n">
         <v>305</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1465,11 +1251,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1">
-      <c r="A4" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="4">
+      <c r="A4" s="2" t="n">
         <v>43122</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1479,11 +1265,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1">
-      <c r="A5" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="5">
+      <c r="A5" s="2" t="n">
         <v>43125</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="1" t="n">
         <v>98</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1493,11 +1279,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1">
-      <c r="A6" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="6">
+      <c r="A6" s="2" t="n">
         <v>43126</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1507,11 +1293,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1">
-      <c r="A7" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="7">
+      <c r="A7" s="2" t="n">
         <v>43127</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1521,11 +1307,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1">
-      <c r="A8" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="8">
+      <c r="A8" s="2" t="n">
         <v>43128</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="1" t="n">
         <v>656</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1535,11 +1321,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1">
-      <c r="A9" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="9">
+      <c r="A9" s="2" t="n">
         <v>43131</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="1" t="n">
         <v>486</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1549,11 +1335,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1">
-      <c r="A10" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="10">
+      <c r="A10" s="2" t="n">
         <v>43132</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="1" t="n">
         <v>76</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1563,11 +1349,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1">
-      <c r="A11" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="11">
+      <c r="A11" s="2" t="n">
         <v>43133</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="1" t="n">
         <v>399</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1577,11 +1363,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1">
-      <c r="A12" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="12">
+      <c r="A12" s="2" t="n">
         <v>43135</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="1" t="n">
         <v>419</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1591,11 +1377,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1">
-      <c r="A13" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="13">
+      <c r="A13" s="2" t="n">
         <v>43136</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="1" t="n">
         <v>521</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1605,11 +1391,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1">
-      <c r="A14" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="14">
+      <c r="A14" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="1" t="n">
         <v>399</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1619,11 +1405,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1">
-      <c r="A15" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="15">
+      <c r="A15" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="1" t="n">
         <v>138</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1633,11 +1419,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1">
-      <c r="A16" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="16">
+      <c r="A16" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="1" t="n">
         <v>310</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1647,12 +1433,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1">
-      <c r="A17" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="17">
+      <c r="A17" s="2" t="n">
         <v>43138</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="1">
+      <c r="C17" s="1" t="n">
         <v>700</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1662,12 +1448,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1">
-      <c r="A18" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="18">
+      <c r="A18" s="2" t="n">
         <v>43141</v>
       </c>
-      <c r="C18" s="1">
-        <f>F18*G18</f>
+      <c r="C18" s="1" t="n">
+        <f aca="false">F18*G18</f>
         <v>1312</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -1676,18 +1462,18 @@
       <c r="E18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="1" t="n">
         <v>164</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="1" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1">
-      <c r="A19" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="19">
+      <c r="A19" s="2" t="n">
         <v>43141</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="1" t="n">
         <v>1190</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1697,11 +1483,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1">
-      <c r="A20" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="20">
+      <c r="A20" s="2" t="n">
         <v>43154</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="1" t="n">
         <v>438</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1711,11 +1497,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1">
-      <c r="A21" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="21">
+      <c r="A21" s="2" t="n">
         <v>43154</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="1" t="n">
         <v>248</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -1725,22 +1511,22 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1">
-      <c r="A22" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="22">
+      <c r="A22" s="2" t="n">
         <v>43166</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="1" t="n">
         <v>234</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1">
-      <c r="A23" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="23">
+      <c r="A23" s="2" t="n">
         <v>43171</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="1" t="n">
         <v>118</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1750,22 +1536,22 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1">
-      <c r="A24" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="24">
+      <c r="A24" s="2" t="n">
         <v>43173</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="1" t="n">
         <v>82</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1">
-      <c r="A25" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="25">
+      <c r="A25" s="2" t="n">
         <v>43174</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1775,22 +1561,22 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1">
-      <c r="A26" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="26">
+      <c r="A26" s="2" t="n">
         <v>43175</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="1" t="n">
         <v>370</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:7" hidden="1">
-      <c r="A27" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="27">
+      <c r="A27" s="2" t="n">
         <v>43175</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -1800,11 +1586,11 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1">
-      <c r="A28" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="28">
+      <c r="A28" s="2" t="n">
         <v>43176</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="1" t="n">
         <v>624</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -1814,11 +1600,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1">
-      <c r="A29" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="29">
+      <c r="A29" s="2" t="n">
         <v>43177</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="1" t="n">
         <v>170</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1828,22 +1614,22 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1">
-      <c r="A30" s="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="30">
+      <c r="A30" s="4" t="n">
         <v>43179</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1">
-      <c r="A31" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="31">
+      <c r="A31" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="1" t="n">
         <v>90</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -1853,11 +1639,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1">
-      <c r="A32" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="32">
+      <c r="A32" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="1" t="n">
         <v>72</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -1867,11 +1653,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:26" hidden="1">
-      <c r="A33" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="33">
+      <c r="A33" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="1" t="n">
         <v>908</v>
       </c>
       <c r="D33" s="6" t="s">
@@ -1881,11 +1667,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:26" hidden="1">
-      <c r="A34" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="34">
+      <c r="A34" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -1895,11 +1681,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:26" hidden="1">
-      <c r="A35" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="35">
+      <c r="A35" s="2" t="n">
         <v>43181</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -1909,11 +1695,11 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:26" hidden="1">
-      <c r="A36" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="36">
+      <c r="A36" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="1" t="n">
         <v>135</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -1923,11 +1709,11 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:26" hidden="1">
-      <c r="A37" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="37">
+      <c r="A37" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="1" t="n">
         <v>110</v>
       </c>
       <c r="C37" s="1"/>
@@ -1959,11 +1745,11 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38" spans="1:26" hidden="1">
-      <c r="A38" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="38">
+      <c r="A38" s="2" t="n">
         <v>43185</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="1" t="n">
         <v>122</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -1973,22 +1759,22 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:26" hidden="1">
-      <c r="A39" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="39">
+      <c r="A39" s="2" t="n">
         <v>43187</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="1" t="n">
         <v>750</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:26" hidden="1">
-      <c r="A40" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="40">
+      <c r="A40" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="1" t="n">
         <v>379</v>
       </c>
       <c r="D40" s="6" t="s">
@@ -1998,22 +1784,22 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:26" hidden="1">
-      <c r="A41" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="41">
+      <c r="A41" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="1" t="n">
         <v>240</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:26" hidden="1">
-      <c r="A42" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="42">
+      <c r="A42" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="1" t="n">
         <v>540</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -2023,11 +1809,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:26" hidden="1">
-      <c r="A43" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="43">
+      <c r="A43" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -2037,11 +1823,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:26" hidden="1">
-      <c r="A44" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="44">
+      <c r="A44" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -2051,11 +1837,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:26" hidden="1">
-      <c r="A45" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="45">
+      <c r="A45" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="1" t="n">
         <v>462</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -2065,11 +1851,11 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:26" hidden="1">
-      <c r="A46" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="46">
+      <c r="A46" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46" s="1" t="n">
         <v>70</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -2079,11 +1865,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:26" hidden="1">
-      <c r="A47" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="47">
+      <c r="A47" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -2093,11 +1879,11 @@
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="1:26" hidden="1">
-      <c r="A48" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="48">
+      <c r="A48" s="2" t="n">
         <v>43190</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="1" t="n">
         <v>30</v>
       </c>
       <c r="C48" s="1"/>
@@ -2108,11 +1894,11 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1">
-      <c r="A49" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="49">
+      <c r="A49" s="2" t="n">
         <v>43191</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="1" t="n">
         <v>40</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -2122,11 +1908,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1">
-      <c r="A50" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="50">
+      <c r="A50" s="7" t="n">
         <v>43193</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50" s="1" t="n">
         <v>150</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -2136,11 +1922,11 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1">
-      <c r="A51" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="51">
+      <c r="A51" s="2" t="n">
         <v>43194</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51" s="1" t="n">
         <v>1360</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -2150,11 +1936,11 @@
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1">
-      <c r="A52" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="52">
+      <c r="A52" s="2" t="n">
         <v>43195</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" s="1" t="n">
         <v>94</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -2164,11 +1950,11 @@
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1">
-      <c r="A53" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="53">
+      <c r="A53" s="2" t="n">
         <v>43196</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C53" s="1" t="n">
         <v>48</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -2178,11 +1964,11 @@
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1">
-      <c r="A54" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="54">
+      <c r="A54" s="2" t="n">
         <v>43196</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C54" s="1" t="n">
         <v>205</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -2192,11 +1978,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1">
-      <c r="A55" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="55">
+      <c r="A55" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -2206,11 +1992,11 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1">
-      <c r="A56" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="56">
+      <c r="A56" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56" s="1" t="n">
         <v>421</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -2220,11 +2006,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1">
-      <c r="A57" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="57">
+      <c r="A57" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="1" t="n">
         <v>191</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -2234,11 +2020,11 @@
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1">
-      <c r="A58" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="58">
+      <c r="A58" s="2" t="n">
         <v>43198</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58" s="1" t="n">
         <v>226</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -2248,22 +2034,22 @@
         <v>96</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1">
-      <c r="A59" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="59">
+      <c r="A59" s="2" t="n">
         <v>43200</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59" s="1" t="n">
         <v>250</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1">
-      <c r="A60" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="60">
+      <c r="A60" s="2" t="n">
         <v>43200</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60" s="1" t="n">
         <v>1115</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -2273,11 +2059,11 @@
         <v>99</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1">
-      <c r="A61" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="61">
+      <c r="A61" s="2" t="n">
         <v>43201</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -2287,11 +2073,11 @@
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1">
-      <c r="A62" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="62">
+      <c r="A62" s="2" t="n">
         <v>43201</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62" s="1" t="n">
         <v>88</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -2301,11 +2087,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1">
-      <c r="A63" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="63">
+      <c r="A63" s="2" t="n">
         <v>43203</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -2315,11 +2101,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1">
-      <c r="A64" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="64">
+      <c r="A64" s="2" t="n">
         <v>43203</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C64" s="1" t="n">
         <v>364</v>
       </c>
       <c r="D64" s="1" t="s">
@@ -2329,11 +2115,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1">
-      <c r="A65" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="65">
+      <c r="A65" s="2" t="n">
         <v>43204</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65" s="1" t="n">
         <v>65</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -2343,11 +2129,11 @@
         <v>105</v>
       </c>
     </row>
-    <row r="66" spans="1:5" hidden="1">
-      <c r="A66" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="66">
+      <c r="A66" s="2" t="n">
         <v>43208</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -2357,11 +2143,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1">
-      <c r="A67" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="67">
+      <c r="A67" s="2" t="n">
         <v>43208</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C67" s="1" t="n">
         <v>470</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -2371,11 +2157,11 @@
         <v>107</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1">
-      <c r="A68" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="68">
+      <c r="A68" s="2" t="n">
         <v>43209</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68" s="1" t="n">
         <v>180</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -2385,11 +2171,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1">
-      <c r="A69" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="69">
+      <c r="A69" s="2" t="n">
         <v>43210</v>
       </c>
-      <c r="C69" s="1">
+      <c r="C69" s="1" t="n">
         <v>420</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -2399,11 +2185,11 @@
         <v>109</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1">
-      <c r="A70" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="70">
+      <c r="A70" s="2" t="n">
         <v>43212</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70" s="1" t="n">
         <v>50</v>
       </c>
       <c r="D70" s="1" t="s">
@@ -2413,11 +2199,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1">
-      <c r="A71" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="71">
+      <c r="A71" s="2" t="n">
         <v>43212</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71" s="1" t="n">
         <v>164</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -2427,11 +2213,11 @@
         <v>112</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1">
-      <c r="A72" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="72">
+      <c r="A72" s="2" t="n">
         <v>43215</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B72" s="1" t="n">
         <v>300</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -2441,11 +2227,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1">
-      <c r="A73" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="73">
+      <c r="A73" s="2" t="n">
         <v>43217</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73" s="1" t="n">
         <v>364</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -2455,11 +2241,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1">
-      <c r="A74" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="74">
+      <c r="A74" s="2" t="n">
         <v>43218</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74" s="1" t="n">
         <v>185</v>
       </c>
       <c r="D74" s="1" t="s">
@@ -2469,11 +2255,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1">
-      <c r="A75" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="75">
+      <c r="A75" s="2" t="n">
         <v>43218</v>
       </c>
-      <c r="C75" s="1">
+      <c r="C75" s="1" t="n">
         <v>404</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -2483,11 +2269,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="76" spans="1:5" hidden="1">
-      <c r="A76" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="76">
+      <c r="A76" s="2" t="n">
         <v>43220</v>
       </c>
-      <c r="C76" s="1">
+      <c r="C76" s="1" t="n">
         <v>57</v>
       </c>
       <c r="D76" s="1" t="s">
@@ -2497,11 +2283,11 @@
         <v>114</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1">
-      <c r="A77" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="77">
+      <c r="A77" s="2" t="n">
         <v>43221</v>
       </c>
-      <c r="C77" s="1">
+      <c r="C77" s="1" t="n">
         <v>282</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -2511,11 +2297,11 @@
         <v>116</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1">
-      <c r="A78" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="78">
+      <c r="A78" s="2" t="n">
         <v>43220</v>
       </c>
-      <c r="C78" s="1">
+      <c r="C78" s="1" t="n">
         <v>87</v>
       </c>
       <c r="D78" s="1" t="s">
@@ -2525,11 +2311,11 @@
         <v>117</v>
       </c>
     </row>
-    <row r="79" spans="1:5" hidden="1">
-      <c r="A79" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="79">
+      <c r="A79" s="2" t="n">
         <v>43223</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B79" s="1" t="n">
         <v>1878</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -2539,11 +2325,11 @@
         <v>119</v>
       </c>
     </row>
-    <row r="80" spans="1:5" hidden="1">
-      <c r="A80" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="80">
+      <c r="A80" s="2" t="n">
         <v>43224</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B80" s="1" t="n">
         <v>98</v>
       </c>
       <c r="D80" s="1" t="s">
@@ -2553,11 +2339,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="81" spans="1:5" hidden="1">
-      <c r="A81" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="81">
+      <c r="A81" s="2" t="n">
         <v>43225</v>
       </c>
-      <c r="C81" s="1">
+      <c r="C81" s="1" t="n">
         <v>198</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -2567,11 +2353,11 @@
         <v>122</v>
       </c>
     </row>
-    <row r="82" spans="1:5" hidden="1">
-      <c r="A82" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="82">
+      <c r="A82" s="2" t="n">
         <v>43225</v>
       </c>
-      <c r="C82" s="1">
+      <c r="C82" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -2581,11 +2367,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="83" spans="1:5" hidden="1">
-      <c r="A83" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="83">
+      <c r="A83" s="2" t="n">
         <v>43228</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83" s="1" t="n">
         <v>168</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -2595,11 +2381,11 @@
         <v>124</v>
       </c>
     </row>
-    <row r="84" spans="1:5" hidden="1">
-      <c r="A84" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="84">
+      <c r="A84" s="2" t="n">
         <v>43229</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B84" s="1" t="n">
         <v>240</v>
       </c>
       <c r="D84" s="1" t="s">
@@ -2609,12 +2395,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:5" hidden="1">
-      <c r="A85" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="85">
+      <c r="A85" s="2" t="n">
         <v>43230</v>
       </c>
       <c r="B85" s="1"/>
-      <c r="C85" s="1">
+      <c r="C85" s="1" t="n">
         <v>420</v>
       </c>
       <c r="D85" s="1" t="s">
@@ -2624,11 +2410,11 @@
         <v>126</v>
       </c>
     </row>
-    <row r="86" spans="1:5" hidden="1">
-      <c r="A86" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="86">
+      <c r="A86" s="2" t="n">
         <v>43230</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B86" s="1" t="n">
         <v>200</v>
       </c>
       <c r="C86" s="1"/>
@@ -2639,11 +2425,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="87" spans="1:5" hidden="1">
-      <c r="A87" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="87">
+      <c r="A87" s="2" t="n">
         <v>43230</v>
       </c>
-      <c r="C87" s="1">
+      <c r="C87" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D87" s="1" t="s">
@@ -2653,11 +2439,11 @@
         <v>128</v>
       </c>
     </row>
-    <row r="88" spans="1:5" hidden="1">
-      <c r="A88" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="88">
+      <c r="A88" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B88" s="1" t="n">
         <v>462</v>
       </c>
       <c r="D88" s="1" t="s">
@@ -2667,11 +2453,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="89" spans="1:5" hidden="1">
-      <c r="A89" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="89">
+      <c r="A89" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B89" s="1" t="n">
         <v>499</v>
       </c>
       <c r="D89" s="1" t="s">
@@ -2681,11 +2467,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="90" spans="1:5" hidden="1">
-      <c r="A90" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="90">
+      <c r="A90" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B90" s="1">
+      <c r="B90" s="1" t="n">
         <v>398</v>
       </c>
       <c r="D90" s="1" t="s">
@@ -2695,11 +2481,11 @@
         <v>133</v>
       </c>
     </row>
-    <row r="91" spans="1:5" hidden="1">
-      <c r="A91" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="91">
+      <c r="A91" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B91" s="1">
+      <c r="B91" s="1" t="n">
         <v>226</v>
       </c>
       <c r="D91" s="1" t="s">
@@ -2709,11 +2495,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="92" spans="1:5" hidden="1">
-      <c r="A92" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="92">
+      <c r="A92" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B92" s="1">
+      <c r="B92" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D92" s="1" t="s">
@@ -2723,11 +2509,11 @@
         <v>137</v>
       </c>
     </row>
-    <row r="93" spans="1:5" hidden="1">
-      <c r="A93" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="93">
+      <c r="A93" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="B93" s="1">
+      <c r="B93" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D93" s="1" t="s">
@@ -2737,11 +2523,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="94" spans="1:5" hidden="1">
-      <c r="A94" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="94">
+      <c r="A94" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="C94" s="1">
+      <c r="C94" s="1" t="n">
         <v>340</v>
       </c>
       <c r="D94" s="1" t="s">
@@ -2751,11 +2537,11 @@
         <v>139</v>
       </c>
     </row>
-    <row r="95" spans="1:5" hidden="1">
-      <c r="A95" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="95">
+      <c r="A95" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="B95" s="1">
+      <c r="B95" s="1" t="n">
         <v>510</v>
       </c>
       <c r="D95" s="1" t="s">
@@ -2765,11 +2551,11 @@
         <v>141</v>
       </c>
     </row>
-    <row r="96" spans="1:5" hidden="1">
-      <c r="A96" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="96">
+      <c r="A96" s="2" t="n">
         <v>43233</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B96" s="1" t="n">
         <v>170</v>
       </c>
       <c r="D96" s="1" t="s">
@@ -2779,11 +2565,11 @@
         <v>143</v>
       </c>
     </row>
-    <row r="97" spans="1:5" hidden="1">
-      <c r="A97" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="97">
+      <c r="A97" s="2" t="n">
         <v>43233</v>
       </c>
-      <c r="C97" s="1">
+      <c r="C97" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D97" s="1" t="s">
@@ -2793,11 +2579,11 @@
         <v>144</v>
       </c>
     </row>
-    <row r="98" spans="1:5" hidden="1">
-      <c r="A98" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="98">
+      <c r="A98" s="2" t="n">
         <v>43234</v>
       </c>
-      <c r="C98" s="1">
+      <c r="C98" s="1" t="n">
         <v>299</v>
       </c>
       <c r="D98" s="1" t="s">
@@ -2807,11 +2593,11 @@
         <v>145</v>
       </c>
     </row>
-    <row r="99" spans="1:5" hidden="1">
-      <c r="A99" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="99">
+      <c r="A99" s="2" t="n">
         <v>43236</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99" s="1" t="n">
         <v>3659</v>
       </c>
       <c r="D99" s="1" t="s">
@@ -2821,11 +2607,11 @@
         <v>146</v>
       </c>
     </row>
-    <row r="100" spans="1:5" hidden="1">
-      <c r="A100" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="100">
+      <c r="A100" s="2" t="n">
         <v>43237</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B100" s="1" t="n">
         <v>79</v>
       </c>
       <c r="D100" s="1" t="s">
@@ -2835,11 +2621,11 @@
         <v>147</v>
       </c>
     </row>
-    <row r="101" spans="1:5" hidden="1">
-      <c r="A101" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="101">
+      <c r="A101" s="2" t="n">
         <v>43236</v>
       </c>
-      <c r="C101" s="1">
+      <c r="C101" s="1" t="n">
         <v>173</v>
       </c>
       <c r="D101" s="1" t="s">
@@ -2849,11 +2635,11 @@
         <v>148</v>
       </c>
     </row>
-    <row r="102" spans="1:5" hidden="1">
-      <c r="A102" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="102">
+      <c r="A102" s="2" t="n">
         <v>43240</v>
       </c>
-      <c r="B102" s="1">
+      <c r="B102" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D102" s="1" t="s">
@@ -2863,22 +2649,22 @@
         <v>149</v>
       </c>
     </row>
-    <row r="103" spans="1:5" hidden="1">
-      <c r="A103" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="103">
+      <c r="A103" s="2" t="n">
         <v>43240</v>
       </c>
-      <c r="B103" s="1">
+      <c r="B103" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="104" spans="1:5" hidden="1">
-      <c r="A104" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="104">
+      <c r="A104" s="2" t="n">
         <v>43241</v>
       </c>
-      <c r="B104" s="1">
+      <c r="B104" s="1" t="n">
         <v>4070</v>
       </c>
       <c r="D104" s="1" t="s">
@@ -2888,11 +2674,11 @@
         <v>150</v>
       </c>
     </row>
-    <row r="105" spans="1:5" hidden="1">
-      <c r="A105" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="105">
+      <c r="A105" s="2" t="n">
         <v>43241</v>
       </c>
-      <c r="C105" s="1">
+      <c r="C105" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D105" s="1" t="s">
@@ -2902,11 +2688,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="106" spans="1:5" hidden="1">
-      <c r="A106" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="106">
+      <c r="A106" s="2" t="n">
         <v>43242</v>
       </c>
-      <c r="B106" s="1">
+      <c r="B106" s="1" t="n">
         <v>79</v>
       </c>
       <c r="D106" s="1" t="s">
@@ -2916,11 +2702,11 @@
         <v>152</v>
       </c>
     </row>
-    <row r="107" spans="1:5" hidden="1">
-      <c r="A107" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="107">
+      <c r="A107" s="2" t="n">
         <v>43246</v>
       </c>
-      <c r="B107" s="1">
+      <c r="B107" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D107" s="1" t="s">
@@ -2930,11 +2716,11 @@
         <v>154</v>
       </c>
     </row>
-    <row r="108" spans="1:5" hidden="1">
-      <c r="A108" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="108">
+      <c r="A108" s="2" t="n">
         <v>43247</v>
       </c>
-      <c r="B108" s="1">
+      <c r="B108" s="1" t="n">
         <v>70</v>
       </c>
       <c r="D108" s="1" t="s">
@@ -2944,44 +2730,44 @@
         <v>156</v>
       </c>
     </row>
-    <row r="109" spans="1:5" hidden="1">
-      <c r="A109" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="109">
+      <c r="A109" s="2" t="n">
         <v>43253</v>
       </c>
-      <c r="B109" s="1">
+      <c r="B109" s="1" t="n">
         <v>142</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="110" spans="1:5" hidden="1">
-      <c r="A110" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="110">
+      <c r="A110" s="2" t="n">
         <v>43254</v>
       </c>
-      <c r="B110" s="1">
+      <c r="B110" s="1" t="n">
         <v>90</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="111" spans="1:5" hidden="1">
-      <c r="A111" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="111">
+      <c r="A111" s="2" t="n">
         <v>43260</v>
       </c>
-      <c r="C111" s="1">
+      <c r="C111" s="1" t="n">
         <v>1400</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="112" spans="1:5" hidden="1">
-      <c r="A112" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="112">
+      <c r="A112" s="2" t="n">
         <v>43260</v>
       </c>
-      <c r="C112" s="1">
+      <c r="C112" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D112" s="1" t="s">
@@ -2991,33 +2777,33 @@
         <v>91</v>
       </c>
     </row>
-    <row r="113" spans="1:5" hidden="1">
-      <c r="A113" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="113">
+      <c r="A113" s="2" t="n">
         <v>43264</v>
       </c>
-      <c r="B113" s="1">
+      <c r="B113" s="1" t="n">
         <v>546</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="114" spans="1:5" hidden="1">
-      <c r="A114" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="114">
+      <c r="A114" s="2" t="n">
         <v>43264</v>
       </c>
-      <c r="B114" s="1">
+      <c r="B114" s="1" t="n">
         <v>95</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="115" spans="1:5" hidden="1">
-      <c r="A115" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="115">
+      <c r="A115" s="2" t="n">
         <v>43266</v>
       </c>
-      <c r="B115" s="1">
+      <c r="B115" s="1" t="n">
         <v>394</v>
       </c>
       <c r="D115" s="1" t="s">
@@ -3027,11 +2813,11 @@
         <v>163</v>
       </c>
     </row>
-    <row r="116" spans="1:5" hidden="1">
-      <c r="A116" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="116">
+      <c r="A116" s="2" t="n">
         <v>43266</v>
       </c>
-      <c r="B116" s="1">
+      <c r="B116" s="1" t="n">
         <v>1055</v>
       </c>
       <c r="D116" s="1" t="s">
@@ -3041,11 +2827,11 @@
         <v>165</v>
       </c>
     </row>
-    <row r="117" spans="1:5" hidden="1">
-      <c r="A117" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="117">
+      <c r="A117" s="2" t="n">
         <v>43284</v>
       </c>
-      <c r="C117" s="1">
+      <c r="C117" s="1" t="n">
         <v>274</v>
       </c>
       <c r="D117" s="1" t="s">
@@ -3055,11 +2841,11 @@
         <v>167</v>
       </c>
     </row>
-    <row r="118" spans="1:5" hidden="1">
-      <c r="A118" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="118">
+      <c r="A118" s="2" t="n">
         <v>43283</v>
       </c>
-      <c r="C118" s="1">
+      <c r="C118" s="1" t="n">
         <v>105</v>
       </c>
       <c r="D118" s="1" t="s">
@@ -3069,11 +2855,11 @@
         <v>169</v>
       </c>
     </row>
-    <row r="119" spans="1:5" hidden="1">
-      <c r="A119" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="119">
+      <c r="A119" s="2" t="n">
         <v>43289</v>
       </c>
-      <c r="C119" s="1">
+      <c r="C119" s="1" t="n">
         <v>128</v>
       </c>
       <c r="D119" s="1" t="s">
@@ -3083,11 +2869,11 @@
         <v>171</v>
       </c>
     </row>
-    <row r="120" spans="1:5" hidden="1">
-      <c r="A120" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="120">
+      <c r="A120" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C120" s="1">
+      <c r="C120" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D120" s="1" t="s">
@@ -3097,11 +2883,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="121" spans="1:5" hidden="1">
-      <c r="A121" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="121">
+      <c r="A121" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C121" s="1">
+      <c r="C121" s="1" t="n">
         <v>210</v>
       </c>
       <c r="D121" s="1" t="s">
@@ -3111,44 +2897,44 @@
         <v>173</v>
       </c>
     </row>
-    <row r="122" spans="1:5" hidden="1">
-      <c r="A122" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="122">
+      <c r="A122" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B122" s="1">
+      <c r="B122" s="1" t="n">
         <v>980</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="123" spans="1:5" hidden="1">
-      <c r="A123" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="123">
+      <c r="A123" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B123" s="1">
+      <c r="B123" s="1" t="n">
         <v>1260</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="124" spans="1:5" hidden="1">
-      <c r="A124" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="124">
+      <c r="A124" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B124" s="1">
+      <c r="B124" s="1" t="n">
         <v>3687</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="125" spans="1:5" hidden="1">
-      <c r="A125" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="125">
+      <c r="A125" s="2" t="n">
         <v>43298</v>
       </c>
-      <c r="C125" s="1">
+      <c r="C125" s="1" t="n">
         <v>60</v>
       </c>
       <c r="D125" s="1" t="s">
@@ -3158,55 +2944,55 @@
         <v>178</v>
       </c>
     </row>
-    <row r="126" spans="1:5" hidden="1">
-      <c r="A126" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="126">
+      <c r="A126" s="2" t="n">
         <v>43291</v>
       </c>
-      <c r="C126" s="1">
+      <c r="C126" s="1" t="n">
         <v>404</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="127" spans="1:5" hidden="1">
-      <c r="A127" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="127">
+      <c r="A127" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C127" s="1">
+      <c r="C127" s="1" t="n">
         <v>451</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="128" spans="1:5" hidden="1">
-      <c r="A128" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="128">
+      <c r="A128" s="2" t="n">
         <v>43298</v>
       </c>
-      <c r="C128" s="1">
+      <c r="C128" s="1" t="n">
         <v>708</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="129" spans="1:5" hidden="1">
-      <c r="A129" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="129">
+      <c r="A129" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C129" s="1">
+      <c r="C129" s="1" t="n">
         <v>160</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="130" spans="1:5" hidden="1">
-      <c r="A130" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="130">
+      <c r="A130" s="2" t="n">
         <v>43288</v>
       </c>
-      <c r="C130" s="1">
+      <c r="C130" s="1" t="n">
         <v>72</v>
       </c>
       <c r="D130" s="1" t="s">
@@ -3216,11 +3002,11 @@
         <v>181</v>
       </c>
     </row>
-    <row r="131" spans="1:5" hidden="1">
-      <c r="A131" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="131">
+      <c r="A131" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C131" s="1">
+      <c r="C131" s="1" t="n">
         <v>300</v>
       </c>
       <c r="D131" s="1" t="s">
@@ -3230,11 +3016,11 @@
         <v>183</v>
       </c>
     </row>
-    <row r="132" spans="1:5" hidden="1">
-      <c r="A132" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="132">
+      <c r="A132" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C132" s="1">
+      <c r="C132" s="1" t="n">
         <v>230</v>
       </c>
       <c r="D132" s="1" t="s">
@@ -3244,22 +3030,22 @@
         <v>185</v>
       </c>
     </row>
-    <row r="133" spans="1:5" hidden="1">
-      <c r="A133" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="133">
+      <c r="A133" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C133" s="1">
+      <c r="C133" s="1" t="n">
         <v>454</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="134" spans="1:5" hidden="1">
-      <c r="A134" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="134">
+      <c r="A134" s="2" t="n">
         <v>43299</v>
       </c>
-      <c r="C134" s="1">
+      <c r="C134" s="1" t="n">
         <v>686</v>
       </c>
       <c r="D134" s="1" t="s">
@@ -3269,11 +3055,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="135" spans="1:5" hidden="1">
-      <c r="A135" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="135">
+      <c r="A135" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C135" s="1">
+      <c r="C135" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D135" s="1" t="s">
@@ -3283,11 +3069,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="136" spans="1:5" hidden="1">
-      <c r="A136" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="136">
+      <c r="A136" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C136" s="1">
+      <c r="C136" s="1" t="n">
         <v>2067</v>
       </c>
       <c r="D136" s="1" t="s">
@@ -3297,11 +3083,11 @@
         <v>186</v>
       </c>
     </row>
-    <row r="137" spans="1:5" hidden="1">
-      <c r="A137" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="137">
+      <c r="A137" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B137" s="1">
+      <c r="B137" s="1" t="n">
         <v>109</v>
       </c>
       <c r="D137" s="1" t="s">
@@ -3311,11 +3097,11 @@
         <v>187</v>
       </c>
     </row>
-    <row r="138" spans="1:5" hidden="1">
-      <c r="A138" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="138">
+      <c r="A138" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B138" s="1">
+      <c r="B138" s="1" t="n">
         <v>97</v>
       </c>
       <c r="D138" s="1" t="s">
@@ -3325,11 +3111,11 @@
         <v>188</v>
       </c>
     </row>
-    <row r="139" spans="1:5" hidden="1">
-      <c r="A139" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="139">
+      <c r="A139" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B139" s="1">
+      <c r="B139" s="1" t="n">
         <v>1437</v>
       </c>
       <c r="D139" s="1" t="s">
@@ -3339,11 +3125,11 @@
         <v>189</v>
       </c>
     </row>
-    <row r="140" spans="1:5" hidden="1">
-      <c r="A140" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="140">
+      <c r="A140" s="2" t="n">
         <v>43306</v>
       </c>
-      <c r="C140" s="1">
+      <c r="C140" s="1" t="n">
         <v>650</v>
       </c>
       <c r="D140" s="1" t="s">
@@ -3353,11 +3139,11 @@
         <v>190</v>
       </c>
     </row>
-    <row r="141" spans="1:5" hidden="1">
-      <c r="A141" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="141">
+      <c r="A141" s="2" t="n">
         <v>43305</v>
       </c>
-      <c r="C141" s="1">
+      <c r="C141" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D141" s="1" t="s">
@@ -3367,11 +3153,11 @@
         <v>191</v>
       </c>
     </row>
-    <row r="142" spans="1:5" hidden="1">
-      <c r="A142" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="142">
+      <c r="A142" s="2" t="n">
         <v>43309</v>
       </c>
-      <c r="C142" s="1">
+      <c r="C142" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D142" s="1" t="s">
@@ -3381,11 +3167,11 @@
         <v>192</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="14" hidden="1">
-      <c r="A143" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="0" r="143">
+      <c r="A143" s="2" t="n">
         <v>43306</v>
       </c>
-      <c r="B143" s="1">
+      <c r="B143" s="1" t="n">
         <v>167</v>
       </c>
       <c r="D143" s="1" t="s">
@@ -3395,11 +3181,11 @@
         <v>193</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="14" hidden="1">
-      <c r="A144" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="0" r="144">
+      <c r="A144" s="2" t="n">
         <v>43304</v>
       </c>
-      <c r="C144" s="1">
+      <c r="C144" s="1" t="n">
         <v>93</v>
       </c>
       <c r="D144" s="1" t="s">
@@ -3409,11 +3195,11 @@
         <v>194</v>
       </c>
     </row>
-    <row r="145" spans="1:5" hidden="1">
-      <c r="A145" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="145">
+      <c r="A145" s="2" t="n">
         <v>43305</v>
       </c>
-      <c r="C145" s="1">
+      <c r="C145" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D145" s="1" t="s">
@@ -3423,11 +3209,11 @@
         <v>195</v>
       </c>
     </row>
-    <row r="146" spans="1:5" hidden="1">
-      <c r="A146" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="146">
+      <c r="A146" s="2" t="n">
         <v>43303</v>
       </c>
-      <c r="C146" s="1">
+      <c r="C146" s="1" t="n">
         <v>244</v>
       </c>
       <c r="D146" s="1" t="s">
@@ -3437,11 +3223,11 @@
         <v>196</v>
       </c>
     </row>
-    <row r="147" spans="1:5" hidden="1">
-      <c r="A147" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="147">
+      <c r="A147" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C147" s="1">
+      <c r="C147" s="1" t="n">
         <v>482</v>
       </c>
       <c r="D147" s="1" t="s">
@@ -3451,11 +3237,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="148" spans="1:5" hidden="1">
-      <c r="A148" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="148">
+      <c r="A148" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C148" s="1">
+      <c r="C148" s="1" t="n">
         <v>172</v>
       </c>
       <c r="D148" s="1" t="s">
@@ -3465,44 +3251,44 @@
         <v>199</v>
       </c>
     </row>
-    <row r="149" spans="1:5" hidden="1">
-      <c r="A149" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="149">
+      <c r="A149" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="B149" s="1">
+      <c r="B149" s="1" t="n">
         <v>89</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="150" spans="1:5" hidden="1">
-      <c r="A150" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="150">
+      <c r="A150" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="C150" s="1">
+      <c r="C150" s="1" t="n">
         <v>107</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="151" spans="1:5" hidden="1">
-      <c r="A151" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="151">
+      <c r="A151" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="C151" s="1">
+      <c r="C151" s="1" t="n">
         <v>124</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="152" spans="1:5" hidden="1">
-      <c r="A152" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="152">
+      <c r="A152" s="7" t="n">
         <v>43316</v>
       </c>
-      <c r="C152" s="1">
+      <c r="C152" s="1" t="n">
         <v>4500</v>
       </c>
       <c r="D152" s="1" t="s">
@@ -3512,11 +3298,11 @@
         <v>202</v>
       </c>
     </row>
-    <row r="153" spans="1:5" hidden="1">
-      <c r="A153" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="153">
+      <c r="A153" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C153" s="1">
+      <c r="C153" s="1" t="n">
         <v>247</v>
       </c>
       <c r="D153" s="1" t="s">
@@ -3526,11 +3312,11 @@
         <v>204</v>
       </c>
     </row>
-    <row r="154" spans="1:5" hidden="1">
-      <c r="A154" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="154">
+      <c r="A154" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C154" s="1">
+      <c r="C154" s="1" t="n">
         <v>1150</v>
       </c>
       <c r="D154" s="1" t="s">
@@ -3540,11 +3326,11 @@
         <v>205</v>
       </c>
     </row>
-    <row r="155" spans="1:5" hidden="1">
-      <c r="A155" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="155">
+      <c r="A155" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C155" s="1">
+      <c r="C155" s="1" t="n">
         <v>313</v>
       </c>
       <c r="D155" s="1" t="s">
@@ -3554,11 +3340,11 @@
         <v>207</v>
       </c>
     </row>
-    <row r="156" spans="1:5" hidden="1">
-      <c r="A156" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="156">
+      <c r="A156" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="B156" s="1">
+      <c r="B156" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D156" s="1" t="s">
@@ -3568,11 +3354,11 @@
         <v>209</v>
       </c>
     </row>
-    <row r="157" spans="1:5" hidden="1">
-      <c r="A157" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="157">
+      <c r="A157" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="C157" s="1">
+      <c r="C157" s="1" t="n">
         <v>710</v>
       </c>
       <c r="D157" s="1" t="s">
@@ -3582,11 +3368,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="158" spans="1:5">
-      <c r="A158" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="158">
+      <c r="A158" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="C158" s="1">
+      <c r="C158" s="1" t="n">
         <v>100</v>
       </c>
       <c r="D158" s="1" t="s">
@@ -3596,11 +3382,11 @@
         <v>212</v>
       </c>
     </row>
-    <row r="159" spans="1:5">
-      <c r="A159" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="159">
+      <c r="A159" s="2" t="n">
         <v>43319</v>
       </c>
-      <c r="B159" s="1">
+      <c r="B159" s="1" t="n">
         <v>78</v>
       </c>
       <c r="D159" s="1" t="s">
@@ -3610,22 +3396,22 @@
         <v>213</v>
       </c>
     </row>
-    <row r="160" spans="1:5">
-      <c r="A160" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="160">
+      <c r="A160" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="B160" s="1">
+      <c r="B160" s="1" t="n">
         <v>1840</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="161" spans="1:5">
-      <c r="A161" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="161">
+      <c r="A161" s="2" t="n">
         <v>43322</v>
       </c>
-      <c r="B161" s="1">
+      <c r="B161" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D161" s="1" t="s">
@@ -3635,11 +3421,11 @@
         <v>216</v>
       </c>
     </row>
-    <row r="162" spans="1:5">
-      <c r="A162" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="162">
+      <c r="A162" s="7" t="n">
         <v>43324</v>
       </c>
-      <c r="C162" s="1">
+      <c r="C162" s="1" t="n">
         <v>230</v>
       </c>
       <c r="D162" s="1" t="s">
@@ -3649,11 +3435,11 @@
         <v>217</v>
       </c>
     </row>
-    <row r="163" spans="1:5">
-      <c r="A163" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="163">
+      <c r="A163" s="7" t="n">
         <v>43326</v>
       </c>
-      <c r="C163" s="1">
+      <c r="C163" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D163" s="1" t="s">
@@ -3663,11 +3449,11 @@
         <v>219</v>
       </c>
     </row>
-    <row r="164" spans="1:5">
-      <c r="A164" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="164">
+      <c r="A164" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="B164" s="1">
+      <c r="B164" s="1" t="n">
         <v>45</v>
       </c>
       <c r="D164" s="1" t="s">
@@ -3677,964 +3463,1026 @@
         <v>221</v>
       </c>
     </row>
-    <row r="165" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A165" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="165">
+      <c r="A165" s="10" t="n">
         <v>43327</v>
       </c>
-      <c r="C165">
+      <c r="C165" s="0" t="n">
         <v>486</v>
       </c>
-      <c r="D165" t="s">
+      <c r="D165" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E165" t="s">
+      <c r="E165" s="0" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="166" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A166" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="166">
+      <c r="A166" s="10" t="n">
         <v>43329</v>
       </c>
-      <c r="C166">
+      <c r="C166" s="0" t="n">
         <v>92</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D166" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="E166" t="s">
+      <c r="E166" s="0" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="167" spans="1:5">
-      <c r="A167" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="167">
+      <c r="A167" s="10" t="n">
         <v>43331</v>
       </c>
-      <c r="C167">
+      <c r="C167" s="0" t="n">
         <v>310</v>
       </c>
-      <c r="D167" t="s">
+      <c r="D167" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="E167" t="s">
+      <c r="E167" s="0" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="168" spans="1:5">
-      <c r="A168" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="168">
+      <c r="A168" s="10" t="n">
         <v>43334</v>
       </c>
-      <c r="C168">
+      <c r="C168" s="0" t="n">
         <v>464</v>
       </c>
-      <c r="D168" t="s">
+      <c r="D168" s="0" t="s">
         <v>218</v>
       </c>
       <c r="E168" s="11" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="169" spans="1:5">
-      <c r="A169" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="169">
+      <c r="A169" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="C169">
+      <c r="C169" s="0" t="n">
         <v>726</v>
       </c>
-      <c r="D169" t="s">
+      <c r="D169" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="E169" t="s">
+      <c r="E169" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="170" spans="1:5">
-      <c r="A170" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="170">
+      <c r="A170" s="10" t="n">
         <v>43337</v>
       </c>
-      <c r="C170">
+      <c r="C170" s="0" t="n">
         <v>544</v>
       </c>
-      <c r="D170" t="s">
+      <c r="D170" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E170" t="s">
+      <c r="E170" s="0" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="171" spans="1:5">
-      <c r="A171" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="171">
+      <c r="A171" s="10" t="n">
         <v>43337</v>
       </c>
-      <c r="B171">
+      <c r="B171" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D171" t="s">
+      <c r="D171" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="E171" t="s">
+      <c r="E171" s="0" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="172" spans="1:5">
-      <c r="A172" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="172">
+      <c r="A172" s="10" t="n">
         <v>43341</v>
       </c>
-      <c r="C172">
+      <c r="C172" s="0" t="n">
         <v>830</v>
       </c>
-      <c r="D172" t="s">
+      <c r="D172" s="0" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="173" spans="1:5">
-      <c r="A173" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="173">
+      <c r="A173" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="C173">
+      <c r="C173" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="D173" t="s">
+      <c r="D173" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="E173" t="s">
+      <c r="E173" s="0" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="174" spans="1:5">
-      <c r="A174" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="174">
+      <c r="A174" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="B174">
+      <c r="B174" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D174" t="s">
+      <c r="D174" s="0" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="175" spans="1:5">
-      <c r="A175" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="175">
+      <c r="A175" s="10" t="n">
         <v>43344</v>
       </c>
-      <c r="B175">
+      <c r="B175" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="D175" t="s">
+      <c r="D175" s="0" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="176" spans="1:5">
-      <c r="A176" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="176">
+      <c r="A176" s="10" t="n">
         <v>43344</v>
       </c>
-      <c r="B176">
+      <c r="B176" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D176" t="s">
+      <c r="D176" s="0" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="177" spans="1:5">
-      <c r="A177" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="177">
+      <c r="A177" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C177">
+      <c r="C177" s="0" t="n">
         <v>607</v>
       </c>
-      <c r="D177" t="s">
+      <c r="D177" s="0" t="s">
         <v>235</v>
       </c>
-      <c r="E177" t="s">
+      <c r="E177" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="178" spans="1:5">
-      <c r="A178" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="178">
+      <c r="A178" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C178">
+      <c r="C178" s="0" t="n">
         <v>444</v>
       </c>
-      <c r="D178" t="s">
+      <c r="D178" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E178" t="s">
+      <c r="E178" s="0" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="179" spans="1:5">
-      <c r="A179" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="179">
+      <c r="A179" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C179">
+      <c r="C179" s="0" t="n">
         <v>312</v>
       </c>
-      <c r="D179" t="s">
+      <c r="D179" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="E179" t="s">
+      <c r="E179" s="0" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="180" spans="1:5">
-      <c r="A180" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="180">
+      <c r="A180" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C180">
+      <c r="C180" s="0" t="n">
         <v>501</v>
       </c>
-      <c r="D180" t="s">
+      <c r="D180" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E180" t="s">
+      <c r="E180" s="0" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="181" spans="1:5">
-      <c r="A181" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="181">
+      <c r="A181" s="10" t="n">
         <v>43349</v>
       </c>
-      <c r="C181">
+      <c r="C181" s="0" t="n">
         <v>711</v>
       </c>
-      <c r="D181" t="s">
+      <c r="D181" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="E181" t="s">
+      <c r="E181" s="0" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="182" spans="1:5">
-      <c r="A182" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="182">
+      <c r="A182" s="10" t="n">
         <v>43354</v>
       </c>
-      <c r="B182">
+      <c r="B182" s="0" t="n">
         <v>126</v>
       </c>
-      <c r="D182" t="s">
+      <c r="D182" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="E182" t="s">
+      <c r="E182" s="0" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="183" spans="1:5">
-      <c r="A183" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="183">
+      <c r="A183" s="10" t="n">
         <v>43354</v>
       </c>
-      <c r="C183">
+      <c r="C183" s="0" t="n">
         <v>450</v>
       </c>
-      <c r="D183" t="s">
+      <c r="D183" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="E183" t="s">
+      <c r="E183" s="0" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="184" spans="1:5">
-      <c r="A184" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="184">
+      <c r="A184" s="10" t="n">
         <v>43361</v>
       </c>
-      <c r="C184">
+      <c r="C184" s="0" t="n">
         <v>660</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D184" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="E184" t="s">
+      <c r="E184" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="185" spans="1:5">
-      <c r="A185" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="185">
+      <c r="A185" s="10" t="n">
         <v>43363</v>
       </c>
-      <c r="C185">
+      <c r="C185" s="0" t="n">
         <v>230</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D185" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="E185" t="s">
+      <c r="E185" s="0" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="186" spans="1:5">
-      <c r="A186" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="186">
+      <c r="A186" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B186">
+      <c r="B186" s="0" t="n">
         <v>4859</v>
       </c>
-      <c r="D186" t="s">
+      <c r="D186" s="0" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="187" spans="1:5">
-      <c r="A187" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="187">
+      <c r="A187" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B187">
+      <c r="B187" s="0" t="n">
         <v>295</v>
       </c>
-      <c r="D187" t="s">
+      <c r="D187" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="E187" t="s">
+      <c r="E187" s="0" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="188" spans="1:5">
-      <c r="A188" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="188">
+      <c r="A188" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B188">
+      <c r="B188" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D188" t="s">
+      <c r="D188" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="E188" t="s">
+      <c r="E188" s="0" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="189" spans="1:5">
-      <c r="A189" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="189">
+      <c r="A189" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B189">
+      <c r="B189" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="D189" t="s">
+      <c r="D189" s="0" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="190" spans="1:5">
-      <c r="A190" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="190">
+      <c r="A190" s="10" t="n">
         <v>43378</v>
       </c>
-      <c r="B190">
+      <c r="B190" s="0" t="n">
         <v>506</v>
       </c>
-      <c r="D190" t="s">
+      <c r="D190" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="E190" t="s">
+      <c r="E190" s="0" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="191" spans="1:5">
-      <c r="A191" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="191">
+      <c r="A191" s="10" t="n">
         <v>43379</v>
       </c>
-      <c r="B191">
+      <c r="B191" s="0" t="n">
         <v>350</v>
       </c>
-      <c r="D191" t="s">
+      <c r="D191" s="0" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="192" spans="1:5" ht="20" customHeight="1">
-      <c r="A192" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="20" outlineLevel="0" r="192">
+      <c r="A192" s="10" t="n">
         <v>43383</v>
       </c>
-      <c r="B192">
+      <c r="B192" s="0" t="n">
         <v>189</v>
       </c>
-      <c r="D192" t="s">
+      <c r="D192" s="0" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="193" spans="1:5">
-      <c r="A193" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="193">
+      <c r="A193" s="10" t="n">
         <v>43387</v>
       </c>
-      <c r="B193">
+      <c r="B193" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="D193" t="s">
+      <c r="D193" s="0" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="194" spans="1:5">
-      <c r="A194" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="194">
+      <c r="A194" s="10" t="n">
         <v>43387</v>
       </c>
-      <c r="B194">
+      <c r="B194" s="0" t="n">
         <v>307</v>
       </c>
-      <c r="D194" t="s">
+      <c r="D194" s="0" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="195" spans="1:5">
-      <c r="C195">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="195">
+      <c r="C195" s="0" t="n">
         <v>3705</v>
       </c>
-      <c r="E195" t="s">
+      <c r="E195" s="0" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="196" spans="1:5">
-      <c r="A196" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="196">
+      <c r="A196" s="10" t="n">
         <v>43385</v>
       </c>
-      <c r="C196">
+      <c r="C196" s="0" t="n">
         <v>608</v>
       </c>
-      <c r="D196" t="s">
+      <c r="D196" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E196" t="s">
+      <c r="E196" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="197" spans="1:5">
-      <c r="A197" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="197">
+      <c r="A197" s="10" t="n">
         <v>43391</v>
       </c>
-      <c r="B197">
+      <c r="B197" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="D197" t="s">
+      <c r="D197" s="0" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="198" spans="1:5">
-      <c r="A198" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="198">
+      <c r="A198" s="10" t="n">
         <v>43392</v>
       </c>
-      <c r="B198">
+      <c r="B198" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="D198" t="s">
+      <c r="D198" s="0" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="199" spans="1:5">
-      <c r="A199" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="199">
+      <c r="A199" s="10" t="n">
         <v>43393</v>
       </c>
-      <c r="B199">
+      <c r="B199" s="0" t="n">
         <v>177</v>
       </c>
-      <c r="D199" t="s">
+      <c r="D199" s="0" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="200" spans="1:5">
-      <c r="A200" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="200">
+      <c r="A200" s="10" t="n">
         <v>43393</v>
       </c>
-      <c r="C200">
+      <c r="C200" s="0" t="n">
         <v>125</v>
       </c>
-      <c r="D200" t="s">
+      <c r="D200" s="0" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="201" spans="1:5">
-      <c r="A201" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="201">
+      <c r="A201" s="10" t="n">
         <v>43395</v>
       </c>
-      <c r="B201">
+      <c r="B201" s="0" t="n">
         <v>2800</v>
       </c>
       <c r="D201" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="E201" t="s">
+      <c r="E201" s="0" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="202" spans="1:5">
-      <c r="A202" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="202">
+      <c r="A202" s="10" t="n">
         <v>43395</v>
       </c>
-      <c r="C202">
+      <c r="C202" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="D202" t="s">
+      <c r="D202" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="E202" t="s">
+      <c r="E202" s="0" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="203" spans="1:5">
-      <c r="A203" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="203">
+      <c r="A203" s="10" t="n">
         <v>43396</v>
       </c>
-      <c r="C203">
+      <c r="C203" s="0" t="n">
         <v>692</v>
       </c>
-      <c r="D203" t="s">
+      <c r="D203" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E203" t="s">
+      <c r="E203" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="204" spans="1:5">
-      <c r="A204" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="204">
+      <c r="A204" s="10" t="n">
         <v>43397</v>
       </c>
-      <c r="C204">
+      <c r="C204" s="0" t="n">
         <v>4935</v>
       </c>
-      <c r="D204" t="s">
+      <c r="D204" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="E204" t="s">
+      <c r="E204" s="0" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="205" spans="1:5" ht="10" customHeight="1">
-      <c r="A205" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10" outlineLevel="0" r="205">
+      <c r="A205" s="10" t="n">
         <v>43398</v>
       </c>
-      <c r="B205">
+      <c r="B205" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="D205" t="s">
+      <c r="D205" s="0" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="206" spans="1:5">
-      <c r="A206" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="206">
+      <c r="A206" s="10" t="n">
         <v>43398</v>
       </c>
-      <c r="B206">
+      <c r="B206" s="0" t="n">
         <v>370</v>
       </c>
-      <c r="D206" t="s">
+      <c r="D206" s="0" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="207" spans="1:5">
-      <c r="A207" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="207">
+      <c r="A207" s="10" t="n">
         <v>43398</v>
       </c>
-      <c r="B207">
+      <c r="B207" s="0" t="n">
         <v>4966</v>
       </c>
-      <c r="D207" t="s">
+      <c r="D207" s="0" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="208" spans="1:5">
-      <c r="A208" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="208">
+      <c r="A208" s="10" t="n">
         <v>43397</v>
       </c>
-      <c r="C208">
+      <c r="C208" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="D208" t="s">
+      <c r="D208" s="0" t="s">
         <v>265</v>
       </c>
-      <c r="E208" t="s">
+      <c r="E208" s="0" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="209" spans="1:5">
-      <c r="A209" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="209">
+      <c r="A209" s="10" t="n">
         <v>43399</v>
       </c>
-      <c r="B209">
+      <c r="B209" s="0" t="n">
         <v>182</v>
       </c>
-      <c r="D209" t="s">
+      <c r="D209" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="E209" t="s">
+      <c r="E209" s="0" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="210" spans="1:5">
-      <c r="A210" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="210">
+      <c r="A210" s="10" t="n">
         <v>43401</v>
       </c>
-      <c r="B210">
+      <c r="B210" s="0" t="n">
         <v>700</v>
       </c>
-      <c r="D210" t="s">
+      <c r="D210" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="E210" t="s">
+      <c r="E210" s="0" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="211" spans="1:5">
-      <c r="A211" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="211">
+      <c r="A211" s="10" t="n">
         <v>43405</v>
       </c>
-      <c r="B211">
+      <c r="B211" s="0" t="n">
         <v>274</v>
       </c>
-      <c r="D211" t="s">
+      <c r="D211" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="E211" t="s">
+      <c r="E211" s="0" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="212" spans="1:5">
-      <c r="A212" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="212">
+      <c r="A212" s="10" t="n">
         <v>43405</v>
       </c>
-      <c r="C212">
+      <c r="C212" s="0" t="n">
         <v>590</v>
       </c>
-      <c r="D212" t="s">
+      <c r="D212" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="E212" t="s">
+      <c r="E212" s="0" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="213" spans="1:5" ht="14">
-      <c r="A213" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="213">
+      <c r="A213" s="10" t="n">
         <v>43407</v>
       </c>
-      <c r="C213">
+      <c r="C213" s="0" t="n">
         <v>1275</v>
       </c>
       <c r="D213" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="E213" t="s">
+      <c r="E213" s="0" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="214" spans="1:5" ht="14">
-      <c r="A214" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="214">
+      <c r="A214" s="10" t="n">
         <v>43407</v>
       </c>
-      <c r="C214">
+      <c r="C214" s="0" t="n">
         <v>4781</v>
       </c>
       <c r="D214" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="E214" t="s">
+      <c r="E214" s="0" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="215" spans="1:5" ht="14">
-      <c r="A215" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="215">
+      <c r="A215" s="10" t="n">
         <v>43407</v>
       </c>
-      <c r="C215">
+      <c r="C215" s="0" t="n">
         <v>4781</v>
       </c>
       <c r="D215" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="E215" t="s">
+      <c r="E215" s="0" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="216" spans="1:5">
-      <c r="A216" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="216">
+      <c r="A216" s="10" t="n">
         <v>43406</v>
       </c>
-      <c r="C216">
+      <c r="C216" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D216" t="s">
+      <c r="D216" s="0" t="s">
         <v>272</v>
       </c>
-      <c r="E216" t="s">
+      <c r="E216" s="0" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="217" spans="1:5">
-      <c r="A217" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="217">
+      <c r="A217" s="10" t="n">
         <v>43409</v>
       </c>
-      <c r="C217">
+      <c r="C217" s="0" t="n">
         <v>677</v>
       </c>
-      <c r="D217" t="s">
+      <c r="D217" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E217" t="s">
+      <c r="E217" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="218" spans="1:5" ht="14">
-      <c r="A218" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="218">
+      <c r="A218" s="10" t="n">
         <v>43410</v>
       </c>
-      <c r="B218">
+      <c r="B218" s="0" t="n">
         <v>285</v>
       </c>
       <c r="D218" s="13" t="s">
         <v>274</v>
       </c>
-      <c r="E218" t="s">
+      <c r="E218" s="0" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="219" spans="1:5" ht="14">
-      <c r="A219" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="219">
+      <c r="A219" s="10" t="n">
         <v>43410</v>
       </c>
-      <c r="B219">
+      <c r="B219" s="0" t="n">
         <v>125</v>
       </c>
       <c r="D219" s="13" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="220" spans="1:5" ht="14">
-      <c r="A220" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="220">
+      <c r="A220" s="10" t="n">
         <v>43409</v>
       </c>
-      <c r="B220">
+      <c r="B220" s="0" t="n">
         <v>85</v>
       </c>
       <c r="D220" s="13" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="221" spans="1:5" ht="14">
-      <c r="A221" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="221">
+      <c r="A221" s="10" t="n">
         <v>43410</v>
       </c>
-      <c r="B221">
+      <c r="B221" s="0" t="n">
         <v>44</v>
       </c>
       <c r="D221" s="13" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="222" spans="1:5">
-      <c r="A222" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="222">
+      <c r="A222" s="10" t="n">
         <v>43412</v>
       </c>
-      <c r="C222">
+      <c r="C222" s="0" t="n">
         <v>190</v>
       </c>
-      <c r="D222" t="s">
+      <c r="D222" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="E222" t="s">
+      <c r="E222" s="0" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="223" spans="1:5" ht="14">
-      <c r="A223" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="223">
+      <c r="A223" s="10" t="n">
         <v>43415</v>
       </c>
-      <c r="B223">
+      <c r="B223" s="0" t="n">
         <v>189</v>
       </c>
       <c r="D223" s="13" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="224" spans="1:5" ht="14">
-      <c r="A224" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="224">
+      <c r="A224" s="10" t="n">
         <v>43415</v>
       </c>
-      <c r="B224">
+      <c r="B224" s="0" t="n">
         <v>336</v>
       </c>
       <c r="D224" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="E224" t="s">
+      <c r="E224" s="0" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="225" spans="1:5" ht="14">
-      <c r="A225" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="225">
+      <c r="A225" s="10" t="n">
         <v>43419</v>
       </c>
-      <c r="B225">
+      <c r="B225" s="0" t="n">
         <v>158</v>
       </c>
       <c r="D225" s="13" t="s">
         <v>282</v>
       </c>
-      <c r="E225" t="s">
+      <c r="E225" s="0" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="226" spans="1:5">
-      <c r="A226" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="226">
+      <c r="A226" s="10" t="n">
         <v>43418</v>
       </c>
-      <c r="C226">
+      <c r="C226" s="0" t="n">
         <v>642</v>
       </c>
-      <c r="D226" t="s">
+      <c r="D226" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E226" t="s">
+      <c r="E226" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="227" spans="1:5">
-      <c r="A227" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="227">
+      <c r="A227" s="10" t="n">
         <v>43419</v>
       </c>
-      <c r="C227">
+      <c r="C227" s="0" t="n">
         <v>370</v>
       </c>
-      <c r="D227" t="s">
+      <c r="D227" s="0" t="s">
         <v>284</v>
       </c>
-      <c r="E227" t="s">
+      <c r="E227" s="0" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="228" spans="1:5">
-      <c r="A228" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="228">
+      <c r="A228" s="10" t="n">
         <v>43419</v>
       </c>
-      <c r="C228">
+      <c r="C228" s="0" t="n">
         <v>222</v>
       </c>
-      <c r="D228" t="s">
+      <c r="D228" s="0" t="s">
         <v>286</v>
       </c>
-      <c r="E228" t="s">
+      <c r="E228" s="0" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="229" spans="1:5">
-      <c r="A229" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="229">
+      <c r="A229" s="10" t="n">
         <v>43421</v>
       </c>
-      <c r="B229">
+      <c r="B229" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="D229" t="s">
+      <c r="D229" s="0" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="230" spans="1:5">
-      <c r="A230" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="230">
+      <c r="A230" s="10" t="n">
         <v>43422</v>
       </c>
-      <c r="B230">
+      <c r="B230" s="0" t="n">
         <v>158</v>
       </c>
-      <c r="D230" t="s">
+      <c r="D230" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="E230" t="s">
+      <c r="E230" s="0" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="231" spans="1:5">
-      <c r="A231" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="231">
+      <c r="A231" s="10" t="n">
         <v>43422</v>
       </c>
-      <c r="B231">
+      <c r="B231" s="0" t="n">
         <v>159</v>
       </c>
-      <c r="D231" t="s">
+      <c r="D231" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="E231" t="s">
+      <c r="E231" s="0" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="232" spans="1:5">
-      <c r="A232" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="232">
+      <c r="A232" s="10" t="n">
         <v>43421</v>
       </c>
-      <c r="C232">
+      <c r="C232" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="D232" t="s">
+      <c r="D232" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="E232" t="s">
+      <c r="E232" s="0" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="233" spans="1:5">
-      <c r="A233" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="233">
+      <c r="A233" s="10" t="n">
         <v>43422</v>
       </c>
-      <c r="B233">
+      <c r="B233" s="0" t="n">
         <v>11649</v>
       </c>
-      <c r="D233" t="s">
+      <c r="D233" s="0" t="s">
         <v>290</v>
       </c>
-      <c r="E233" t="s">
+      <c r="E233" s="0" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="234" spans="1:5">
-      <c r="A234" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="234">
+      <c r="A234" s="10" t="n">
         <v>43426</v>
       </c>
-      <c r="C234">
+      <c r="C234" s="0" t="n">
         <v>308</v>
       </c>
-      <c r="D234" t="s">
+      <c r="D234" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="E234" t="s">
+      <c r="E234" s="0" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="235" spans="1:5">
-      <c r="A235" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="235">
+      <c r="A235" s="10" t="n">
         <v>43428</v>
       </c>
-      <c r="B235">
+      <c r="B235" s="0" t="n">
         <v>112</v>
       </c>
-      <c r="D235" t="s">
+      <c r="D235" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="E235" t="s">
+      <c r="E235" s="0" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="236" spans="1:5">
-      <c r="A236" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="236">
+      <c r="A236" s="10" t="n">
         <v>43428</v>
       </c>
-      <c r="B236">
+      <c r="B236" s="0" t="n">
         <v>79</v>
       </c>
-      <c r="D236" t="s">
+      <c r="D236" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="E236" t="s">
+      <c r="E236" s="0" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="241" spans="2:3">
-      <c r="B241">
-        <f>SUM(B2:B240)</f>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="237">
+      <c r="A237" s="10" t="n">
+        <v>43425</v>
+      </c>
+      <c r="C237" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="D237" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="E237" s="0" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="238">
+      <c r="A238" s="10" t="n">
+        <v>43426</v>
+      </c>
+      <c r="C238" s="0" t="n">
+        <v>308</v>
+      </c>
+      <c r="D238" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="E238" s="0" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="239">
+      <c r="A239" s="10" t="n">
+        <v>43430</v>
+      </c>
+      <c r="C239" s="0" t="n">
+        <v>616</v>
+      </c>
+      <c r="D239" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="E239" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="240">
+      <c r="A240" s="10" t="n">
+        <v>43430</v>
+      </c>
+      <c r="C240" s="0" t="n">
+        <v>243</v>
+      </c>
+      <c r="D240" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="E240" s="0" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="241"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="260">
+      <c r="B260" s="0" t="n">
+        <f aca="false">SUM(B2:B259)</f>
         <v>69591</v>
       </c>
-      <c r="C241">
-        <f>SUM(C2:C240)</f>
-        <v>66467</v>
+      <c r="C260" s="0" t="n">
+        <f aca="false">SUM(C2:C259)</f>
+        <v>67727</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A30:Z32">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule aboveAverage="0" bottom="0" dxfId="0" operator="expression" percent="0" priority="2" rank="0" text="" type="expression">
       <formula>LEN(TRIM(A30))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D33" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D40" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D201" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink display="netonnet.se" ref="D33" r:id="rId1"/>
+    <hyperlink display="www.vidaxl.se" ref="D40" r:id="rId2"/>
+    <hyperlink display="https://www.vardia.se/" ref="D201" r:id="rId3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cost update nov 28 jenny
</commit_message>
<xml_diff>
--- a/Cost.xlsx
+++ b/Cost.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="301">
   <si>
     <t>日期</t>
   </si>
@@ -912,6 +912,12 @@
   </si>
   <si>
     <t>blossa,grape rod,pangasiusfile, tebaguette fransk, etc</t>
+  </si>
+  <si>
+    <t>Parkeringsanmarkning</t>
+  </si>
+  <si>
+    <t>vallingby</t>
   </si>
 </sst>
 </file>
@@ -1194,8 +1200,8 @@
   </sheetPr>
   <dimension ref="A1:Z260"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A244" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E242" activeCellId="0" pane="topLeft" sqref="E242"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A229" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E241" activeCellId="0" pane="topLeft" sqref="E241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
@@ -4455,7 +4461,20 @@
         <v>298</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="241"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="241">
+      <c r="A241" s="10" t="n">
+        <v>43432</v>
+      </c>
+      <c r="C241" s="0" t="n">
+        <v>850</v>
+      </c>
+      <c r="D241" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="E241" s="0" t="s">
+        <v>300</v>
+      </c>
+    </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="260">
       <c r="B260" s="0" t="n">
         <f aca="false">SUM(B2:B259)</f>
@@ -4463,7 +4482,7 @@
       </c>
       <c r="C260" s="0" t="n">
         <f aca="false">SUM(C2:C259)</f>
-        <v>67727</v>
+        <v>68577</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cost update nov 29 jenny&martin
</commit_message>
<xml_diff>
--- a/Cost.xlsx
+++ b/Cost.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vhub.rnd.ki.sw.ericsson.se\home\eyanizh\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{86F691CA-7312-45D9-8D43-65E73A5A9670}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8194" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="179017" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="305">
   <si>
     <t>日期</t>
   </si>
@@ -918,77 +923,73 @@
   </si>
   <si>
     <t>vallingby</t>
+  </si>
+  <si>
+    <t>biltvätta</t>
+  </si>
+  <si>
+    <t>沙琪玛；tofu，etc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICA taby </t>
+  </si>
+  <si>
+    <t>mjork；chips；etc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="YYYY/M/D" numFmtId="165"/>
-    <numFmt formatCode="M/D/YYYY" numFmtId="166"/>
-    <numFmt formatCode="YYYY\-MM\-DD" numFmtId="167"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="yyyy/m/d"/>
+    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="7">
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <family val="2"/>
     </font>
     <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF666666"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <family val="2"/>
     </font>
     <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0563C1"/>
       <name val="Arial"/>
       <family val="2"/>
-      <sz val="10"/>
     </font>
     <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0563C1"/>
+      <name val="FreeSans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
       <name val="Arial"/>
       <family val="2"/>
-      <color rgb="FF0000FF"/>
-      <sz val="10"/>
-      <u val="single"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
-      <color rgb="FF666666"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
-      <color rgb="FF0563C1"/>
-      <sz val="10"/>
-      <u val="single"/>
-    </font>
-    <font>
-      <name val="FreeSans"/>
-      <family val="2"/>
-      <color rgb="FF0563C1"/>
-      <sz val="10"/>
-      <u val="single"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
-      <color rgb="FF444444"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1018,7 +1019,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1026,100 +1027,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="4" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="167" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="20">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="8" customBuiltin="false" name="*unknown*" xfId="20"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1130,6 +1062,7 @@
       </fill>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1188,31 +1121,339 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF444444"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z260"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A229" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E241" activeCellId="0" pane="topLeft" sqref="E241"/>
+    <sheetView tabSelected="1" topLeftCell="A229" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D246" sqref="D246"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="12.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="14.5"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.8316326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="14.5"/>
+    <col min="1" max="3" width="14.4609375"/>
+    <col min="4" max="4" width="26"/>
+    <col min="5" max="5" width="37.84375"/>
+    <col min="6" max="1025" width="14.4609375"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="1">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1229,11 +1470,11 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="2">
-      <c r="A2" s="2" t="n">
+    <row r="2" spans="1:5" hidden="1">
+      <c r="A2" s="2">
         <v>43121</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="1">
         <v>250</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1243,11 +1484,11 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="3">
-      <c r="A3" s="2" t="n">
+    <row r="3" spans="1:5" hidden="1">
+      <c r="A3" s="2">
         <v>43122</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="1">
         <v>305</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1257,11 +1498,11 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="4">
-      <c r="A4" s="2" t="n">
+    <row r="4" spans="1:5" hidden="1">
+      <c r="A4" s="2">
         <v>43122</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="1">
         <v>120</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1271,11 +1512,11 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="5">
-      <c r="A5" s="2" t="n">
+    <row r="5" spans="1:5" hidden="1">
+      <c r="A5" s="2">
         <v>43125</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="1">
         <v>98</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1285,11 +1526,11 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="6">
-      <c r="A6" s="2" t="n">
+    <row r="6" spans="1:5" hidden="1">
+      <c r="A6" s="2">
         <v>43126</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="1">
         <v>190</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1299,11 +1540,11 @@
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="7">
-      <c r="A7" s="2" t="n">
+    <row r="7" spans="1:5" hidden="1">
+      <c r="A7" s="2">
         <v>43127</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="C7" s="1">
         <v>406</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1313,11 +1554,11 @@
         <v>16</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="8">
-      <c r="A8" s="2" t="n">
+    <row r="8" spans="1:5" hidden="1">
+      <c r="A8" s="2">
         <v>43128</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8" s="1">
         <v>656</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1327,11 +1568,11 @@
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="9">
-      <c r="A9" s="2" t="n">
+    <row r="9" spans="1:5" hidden="1">
+      <c r="A9" s="2">
         <v>43131</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" s="1">
         <v>486</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1341,11 +1582,11 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="10">
-      <c r="A10" s="2" t="n">
+    <row r="10" spans="1:5" hidden="1">
+      <c r="A10" s="2">
         <v>43132</v>
       </c>
-      <c r="B10" s="1" t="n">
+      <c r="B10" s="1">
         <v>76</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1355,11 +1596,11 @@
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="11">
-      <c r="A11" s="2" t="n">
+    <row r="11" spans="1:5" hidden="1">
+      <c r="A11" s="2">
         <v>43133</v>
       </c>
-      <c r="C11" s="1" t="n">
+      <c r="C11" s="1">
         <v>399</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1369,11 +1610,11 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="12">
-      <c r="A12" s="2" t="n">
+    <row r="12" spans="1:5" hidden="1">
+      <c r="A12" s="2">
         <v>43135</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="B12" s="1">
         <v>419</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1383,11 +1624,11 @@
         <v>23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="13">
-      <c r="A13" s="2" t="n">
+    <row r="13" spans="1:5" hidden="1">
+      <c r="A13" s="2">
         <v>43136</v>
       </c>
-      <c r="B13" s="1" t="n">
+      <c r="B13" s="1">
         <v>521</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1397,11 +1638,11 @@
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="14">
-      <c r="A14" s="2" t="n">
+    <row r="14" spans="1:5" hidden="1">
+      <c r="A14" s="2">
         <v>43137</v>
       </c>
-      <c r="B14" s="1" t="n">
+      <c r="B14" s="1">
         <v>399</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1411,11 +1652,11 @@
         <v>27</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="15">
-      <c r="A15" s="2" t="n">
+    <row r="15" spans="1:5" hidden="1">
+      <c r="A15" s="2">
         <v>43137</v>
       </c>
-      <c r="B15" s="1" t="n">
+      <c r="B15" s="1">
         <v>138</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1425,11 +1666,11 @@
         <v>29</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="16">
-      <c r="A16" s="2" t="n">
+    <row r="16" spans="1:5" hidden="1">
+      <c r="A16" s="2">
         <v>43137</v>
       </c>
-      <c r="B16" s="1" t="n">
+      <c r="B16" s="1">
         <v>310</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1439,12 +1680,12 @@
         <v>31</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="17">
-      <c r="A17" s="2" t="n">
+    <row r="17" spans="1:7" hidden="1">
+      <c r="A17" s="2">
         <v>43138</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="1" t="n">
+      <c r="C17" s="1">
         <v>700</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1454,12 +1695,12 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="18">
-      <c r="A18" s="2" t="n">
+    <row r="18" spans="1:7" hidden="1">
+      <c r="A18" s="2">
         <v>43141</v>
       </c>
-      <c r="C18" s="1" t="n">
-        <f aca="false">F18*G18</f>
+      <c r="C18" s="1">
+        <f>F18*G18</f>
         <v>1312</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -1468,18 +1709,18 @@
       <c r="E18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="1" t="n">
+      <c r="F18" s="1">
         <v>164</v>
       </c>
-      <c r="G18" s="1" t="n">
+      <c r="G18" s="1">
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="19">
-      <c r="A19" s="2" t="n">
+    <row r="19" spans="1:7" hidden="1">
+      <c r="A19" s="2">
         <v>43141</v>
       </c>
-      <c r="B19" s="1" t="n">
+      <c r="B19" s="1">
         <v>1190</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1489,11 +1730,11 @@
         <v>37</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="20">
-      <c r="A20" s="2" t="n">
+    <row r="20" spans="1:7" hidden="1">
+      <c r="A20" s="2">
         <v>43154</v>
       </c>
-      <c r="B20" s="1" t="n">
+      <c r="B20" s="1">
         <v>438</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1503,11 +1744,11 @@
         <v>39</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="21">
-      <c r="A21" s="2" t="n">
+    <row r="21" spans="1:7" hidden="1">
+      <c r="A21" s="2">
         <v>43154</v>
       </c>
-      <c r="B21" s="1" t="n">
+      <c r="B21" s="1">
         <v>248</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -1517,22 +1758,22 @@
         <v>40</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="22">
-      <c r="A22" s="2" t="n">
+    <row r="22" spans="1:7" hidden="1">
+      <c r="A22" s="2">
         <v>43166</v>
       </c>
-      <c r="B22" s="1" t="n">
+      <c r="B22" s="1">
         <v>234</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="23">
-      <c r="A23" s="2" t="n">
+    <row r="23" spans="1:7" hidden="1">
+      <c r="A23" s="2">
         <v>43171</v>
       </c>
-      <c r="B23" s="1" t="n">
+      <c r="B23" s="1">
         <v>118</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1542,22 +1783,22 @@
         <v>43</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="24">
-      <c r="A24" s="2" t="n">
+    <row r="24" spans="1:7" hidden="1">
+      <c r="A24" s="2">
         <v>43173</v>
       </c>
-      <c r="C24" s="1" t="n">
+      <c r="C24" s="1">
         <v>82</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="25">
-      <c r="A25" s="2" t="n">
+    <row r="25" spans="1:7" hidden="1">
+      <c r="A25" s="2">
         <v>43174</v>
       </c>
-      <c r="B25" s="1" t="n">
+      <c r="B25" s="1">
         <v>280</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1567,22 +1808,22 @@
         <v>46</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="26">
-      <c r="A26" s="2" t="n">
+    <row r="26" spans="1:7" hidden="1">
+      <c r="A26" s="2">
         <v>43175</v>
       </c>
-      <c r="C26" s="1" t="n">
+      <c r="C26" s="1">
         <v>370</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="27">
-      <c r="A27" s="2" t="n">
+    <row r="27" spans="1:7" hidden="1">
+      <c r="A27" s="2">
         <v>43175</v>
       </c>
-      <c r="C27" s="1" t="n">
+      <c r="C27" s="1">
         <v>400</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -1592,11 +1833,11 @@
         <v>48</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="28">
-      <c r="A28" s="2" t="n">
+    <row r="28" spans="1:7" hidden="1">
+      <c r="A28" s="2">
         <v>43176</v>
       </c>
-      <c r="B28" s="1" t="n">
+      <c r="B28" s="1">
         <v>624</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -1606,11 +1847,11 @@
         <v>50</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="29">
-      <c r="A29" s="2" t="n">
+    <row r="29" spans="1:7" hidden="1">
+      <c r="A29" s="2">
         <v>43177</v>
       </c>
-      <c r="B29" s="1" t="n">
+      <c r="B29" s="1">
         <v>170</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1620,22 +1861,22 @@
         <v>52</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="30">
-      <c r="A30" s="4" t="n">
+    <row r="30" spans="1:7" hidden="1">
+      <c r="A30" s="4">
         <v>43179</v>
       </c>
-      <c r="C30" s="1" t="n">
+      <c r="C30" s="1">
         <v>190</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="31">
-      <c r="A31" s="2" t="n">
+    <row r="31" spans="1:7" hidden="1">
+      <c r="A31" s="2">
         <v>43179</v>
       </c>
-      <c r="C31" s="1" t="n">
+      <c r="C31" s="1">
         <v>90</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -1645,11 +1886,11 @@
         <v>55</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="32">
-      <c r="A32" s="2" t="n">
+    <row r="32" spans="1:7" hidden="1">
+      <c r="A32" s="2">
         <v>43179</v>
       </c>
-      <c r="B32" s="1" t="n">
+      <c r="B32" s="1">
         <v>72</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -1659,11 +1900,11 @@
         <v>57</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="33">
-      <c r="A33" s="2" t="n">
+    <row r="33" spans="1:26" hidden="1">
+      <c r="A33" s="2">
         <v>43179</v>
       </c>
-      <c r="C33" s="1" t="n">
+      <c r="C33" s="1">
         <v>908</v>
       </c>
       <c r="D33" s="6" t="s">
@@ -1673,11 +1914,11 @@
         <v>59</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="34">
-      <c r="A34" s="2" t="n">
+    <row r="34" spans="1:26" hidden="1">
+      <c r="A34" s="2">
         <v>43184</v>
       </c>
-      <c r="B34" s="1" t="n">
+      <c r="B34" s="1">
         <v>400</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -1687,11 +1928,11 @@
         <v>60</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="35">
-      <c r="A35" s="2" t="n">
+    <row r="35" spans="1:26" hidden="1">
+      <c r="A35" s="2">
         <v>43181</v>
       </c>
-      <c r="C35" s="1" t="n">
+      <c r="C35" s="1">
         <v>80</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -1701,11 +1942,11 @@
         <v>62</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="36">
-      <c r="A36" s="2" t="n">
+    <row r="36" spans="1:26" hidden="1">
+      <c r="A36" s="2">
         <v>43184</v>
       </c>
-      <c r="C36" s="1" t="n">
+      <c r="C36" s="1">
         <v>135</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -1715,11 +1956,11 @@
         <v>64</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="37">
-      <c r="A37" s="2" t="n">
+    <row r="37" spans="1:26" hidden="1">
+      <c r="A37" s="2">
         <v>43184</v>
       </c>
-      <c r="B37" s="1" t="n">
+      <c r="B37" s="1">
         <v>110</v>
       </c>
       <c r="C37" s="1"/>
@@ -1751,11 +1992,11 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="38">
-      <c r="A38" s="2" t="n">
+    <row r="38" spans="1:26" hidden="1">
+      <c r="A38" s="2">
         <v>43185</v>
       </c>
-      <c r="B38" s="1" t="n">
+      <c r="B38" s="1">
         <v>122</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -1765,22 +2006,22 @@
         <v>64</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="39">
-      <c r="A39" s="2" t="n">
+    <row r="39" spans="1:26" hidden="1">
+      <c r="A39" s="2">
         <v>43187</v>
       </c>
-      <c r="B39" s="1" t="n">
+      <c r="B39" s="1">
         <v>750</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="40">
-      <c r="A40" s="2" t="n">
+    <row r="40" spans="1:26" hidden="1">
+      <c r="A40" s="2">
         <v>43188</v>
       </c>
-      <c r="B40" s="1" t="n">
+      <c r="B40" s="1">
         <v>379</v>
       </c>
       <c r="D40" s="6" t="s">
@@ -1790,22 +2031,22 @@
         <v>68</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="41">
-      <c r="A41" s="2" t="n">
+    <row r="41" spans="1:26" hidden="1">
+      <c r="A41" s="2">
         <v>43188</v>
       </c>
-      <c r="B41" s="1" t="n">
+      <c r="B41" s="1">
         <v>240</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="42">
-      <c r="A42" s="2" t="n">
+    <row r="42" spans="1:26" hidden="1">
+      <c r="A42" s="2">
         <v>43188</v>
       </c>
-      <c r="C42" s="1" t="n">
+      <c r="C42" s="1">
         <v>540</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -1815,11 +2056,11 @@
         <v>70</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="43">
-      <c r="A43" s="2" t="n">
+    <row r="43" spans="1:26" hidden="1">
+      <c r="A43" s="2">
         <v>43188</v>
       </c>
-      <c r="C43" s="1" t="n">
+      <c r="C43" s="1">
         <v>220</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -1829,11 +2070,11 @@
         <v>72</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="44">
-      <c r="A44" s="2" t="n">
+    <row r="44" spans="1:26" hidden="1">
+      <c r="A44" s="2">
         <v>43189</v>
       </c>
-      <c r="C44" s="1" t="n">
+      <c r="C44" s="1">
         <v>400</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -1843,11 +2084,11 @@
         <v>60</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="45">
-      <c r="A45" s="2" t="n">
+    <row r="45" spans="1:26" hidden="1">
+      <c r="A45" s="2">
         <v>43189</v>
       </c>
-      <c r="C45" s="1" t="n">
+      <c r="C45" s="1">
         <v>462</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -1857,11 +2098,11 @@
         <v>75</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="46">
-      <c r="A46" s="2" t="n">
+    <row r="46" spans="1:26" hidden="1">
+      <c r="A46" s="2">
         <v>43189</v>
       </c>
-      <c r="C46" s="1" t="n">
+      <c r="C46" s="1">
         <v>70</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -1871,11 +2112,11 @@
         <v>77</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="47">
-      <c r="A47" s="2" t="n">
+    <row r="47" spans="1:26" hidden="1">
+      <c r="A47" s="2">
         <v>43189</v>
       </c>
-      <c r="C47" s="1" t="n">
+      <c r="C47" s="1">
         <v>80</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -1885,11 +2126,11 @@
         <v>79</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="48">
-      <c r="A48" s="2" t="n">
+    <row r="48" spans="1:26" hidden="1">
+      <c r="A48" s="2">
         <v>43190</v>
       </c>
-      <c r="B48" s="1" t="n">
+      <c r="B48" s="1">
         <v>30</v>
       </c>
       <c r="C48" s="1"/>
@@ -1900,11 +2141,11 @@
         <v>81</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="49">
-      <c r="A49" s="2" t="n">
+    <row r="49" spans="1:5" hidden="1">
+      <c r="A49" s="2">
         <v>43191</v>
       </c>
-      <c r="B49" s="1" t="n">
+      <c r="B49" s="1">
         <v>40</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -1914,11 +2155,11 @@
         <v>83</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="50">
-      <c r="A50" s="7" t="n">
+    <row r="50" spans="1:5" hidden="1">
+      <c r="A50" s="7">
         <v>43193</v>
       </c>
-      <c r="C50" s="1" t="n">
+      <c r="C50" s="1">
         <v>150</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -1928,11 +2169,11 @@
         <v>85</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="51">
-      <c r="A51" s="2" t="n">
+    <row r="51" spans="1:5" hidden="1">
+      <c r="A51" s="2">
         <v>43194</v>
       </c>
-      <c r="C51" s="1" t="n">
+      <c r="C51" s="1">
         <v>1360</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -1942,11 +2183,11 @@
         <v>87</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="52">
-      <c r="A52" s="2" t="n">
+    <row r="52" spans="1:5" hidden="1">
+      <c r="A52" s="2">
         <v>43195</v>
       </c>
-      <c r="C52" s="1" t="n">
+      <c r="C52" s="1">
         <v>94</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -1956,11 +2197,11 @@
         <v>88</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="53">
-      <c r="A53" s="2" t="n">
+    <row r="53" spans="1:5" hidden="1">
+      <c r="A53" s="2">
         <v>43196</v>
       </c>
-      <c r="C53" s="1" t="n">
+      <c r="C53" s="1">
         <v>48</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -1970,11 +2211,11 @@
         <v>90</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="54">
-      <c r="A54" s="2" t="n">
+    <row r="54" spans="1:5" hidden="1">
+      <c r="A54" s="2">
         <v>43196</v>
       </c>
-      <c r="C54" s="1" t="n">
+      <c r="C54" s="1">
         <v>205</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -1984,11 +2225,11 @@
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="55">
-      <c r="A55" s="2" t="n">
+    <row r="55" spans="1:5" hidden="1">
+      <c r="A55" s="2">
         <v>43197</v>
       </c>
-      <c r="C55" s="1" t="n">
+      <c r="C55" s="1">
         <v>130</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -1998,11 +2239,11 @@
         <v>93</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="56">
-      <c r="A56" s="2" t="n">
+    <row r="56" spans="1:5" hidden="1">
+      <c r="A56" s="2">
         <v>43197</v>
       </c>
-      <c r="C56" s="1" t="n">
+      <c r="C56" s="1">
         <v>421</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -2012,11 +2253,11 @@
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="57">
-      <c r="A57" s="2" t="n">
+    <row r="57" spans="1:5" hidden="1">
+      <c r="A57" s="2">
         <v>43197</v>
       </c>
-      <c r="B57" s="1" t="n">
+      <c r="B57" s="1">
         <v>191</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -2026,11 +2267,11 @@
         <v>95</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="58">
-      <c r="A58" s="2" t="n">
+    <row r="58" spans="1:5" hidden="1">
+      <c r="A58" s="2">
         <v>43198</v>
       </c>
-      <c r="B58" s="1" t="n">
+      <c r="B58" s="1">
         <v>226</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -2040,22 +2281,22 @@
         <v>96</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="59">
-      <c r="A59" s="2" t="n">
+    <row r="59" spans="1:5" hidden="1">
+      <c r="A59" s="2">
         <v>43200</v>
       </c>
-      <c r="B59" s="1" t="n">
+      <c r="B59" s="1">
         <v>250</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="60">
-      <c r="A60" s="2" t="n">
+    <row r="60" spans="1:5" hidden="1">
+      <c r="A60" s="2">
         <v>43200</v>
       </c>
-      <c r="B60" s="1" t="n">
+      <c r="B60" s="1">
         <v>1115</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -2065,11 +2306,11 @@
         <v>99</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="61">
-      <c r="A61" s="2" t="n">
+    <row r="61" spans="1:5" hidden="1">
+      <c r="A61" s="2">
         <v>43201</v>
       </c>
-      <c r="C61" s="1" t="n">
+      <c r="C61" s="1">
         <v>220</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -2079,11 +2320,11 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="62">
-      <c r="A62" s="2" t="n">
+    <row r="62" spans="1:5" hidden="1">
+      <c r="A62" s="2">
         <v>43201</v>
       </c>
-      <c r="C62" s="1" t="n">
+      <c r="C62" s="1">
         <v>88</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -2093,11 +2334,11 @@
         <v>102</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="63">
-      <c r="A63" s="2" t="n">
+    <row r="63" spans="1:5" hidden="1">
+      <c r="A63" s="2">
         <v>43203</v>
       </c>
-      <c r="B63" s="1" t="n">
+      <c r="B63" s="1">
         <v>400</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -2107,11 +2348,11 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="64">
-      <c r="A64" s="2" t="n">
+    <row r="64" spans="1:5" hidden="1">
+      <c r="A64" s="2">
         <v>43203</v>
       </c>
-      <c r="C64" s="1" t="n">
+      <c r="C64" s="1">
         <v>364</v>
       </c>
       <c r="D64" s="1" t="s">
@@ -2121,11 +2362,11 @@
         <v>103</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="65">
-      <c r="A65" s="2" t="n">
+    <row r="65" spans="1:5" hidden="1">
+      <c r="A65" s="2">
         <v>43204</v>
       </c>
-      <c r="C65" s="1" t="n">
+      <c r="C65" s="1">
         <v>65</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -2135,11 +2376,11 @@
         <v>105</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="66">
-      <c r="A66" s="2" t="n">
+    <row r="66" spans="1:5" hidden="1">
+      <c r="A66" s="2">
         <v>43208</v>
       </c>
-      <c r="C66" s="1" t="n">
+      <c r="C66" s="1">
         <v>406</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -2149,11 +2390,11 @@
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="67">
-      <c r="A67" s="2" t="n">
+    <row r="67" spans="1:5" hidden="1">
+      <c r="A67" s="2">
         <v>43208</v>
       </c>
-      <c r="C67" s="1" t="n">
+      <c r="C67" s="1">
         <v>470</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -2163,11 +2404,11 @@
         <v>107</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="68">
-      <c r="A68" s="2" t="n">
+    <row r="68" spans="1:5" hidden="1">
+      <c r="A68" s="2">
         <v>43209</v>
       </c>
-      <c r="B68" s="1" t="n">
+      <c r="B68" s="1">
         <v>180</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -2177,11 +2418,11 @@
         <v>103</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="69">
-      <c r="A69" s="2" t="n">
+    <row r="69" spans="1:5" hidden="1">
+      <c r="A69" s="2">
         <v>43210</v>
       </c>
-      <c r="C69" s="1" t="n">
+      <c r="C69" s="1">
         <v>420</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -2191,11 +2432,11 @@
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="70">
-      <c r="A70" s="2" t="n">
+    <row r="70" spans="1:5" hidden="1">
+      <c r="A70" s="2">
         <v>43212</v>
       </c>
-      <c r="B70" s="1" t="n">
+      <c r="B70" s="1">
         <v>50</v>
       </c>
       <c r="D70" s="1" t="s">
@@ -2205,11 +2446,11 @@
         <v>83</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="71">
-      <c r="A71" s="2" t="n">
+    <row r="71" spans="1:5" hidden="1">
+      <c r="A71" s="2">
         <v>43212</v>
       </c>
-      <c r="B71" s="1" t="n">
+      <c r="B71" s="1">
         <v>164</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -2219,11 +2460,11 @@
         <v>112</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="72">
-      <c r="A72" s="2" t="n">
+    <row r="72" spans="1:5" hidden="1">
+      <c r="A72" s="2">
         <v>43215</v>
       </c>
-      <c r="B72" s="1" t="n">
+      <c r="B72" s="1">
         <v>300</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -2233,11 +2474,11 @@
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="73">
-      <c r="A73" s="2" t="n">
+    <row r="73" spans="1:5" hidden="1">
+      <c r="A73" s="2">
         <v>43217</v>
       </c>
-      <c r="B73" s="1" t="n">
+      <c r="B73" s="1">
         <v>364</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -2247,11 +2488,11 @@
         <v>103</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="74">
-      <c r="A74" s="2" t="n">
+    <row r="74" spans="1:5" hidden="1">
+      <c r="A74" s="2">
         <v>43218</v>
       </c>
-      <c r="B74" s="1" t="n">
+      <c r="B74" s="1">
         <v>185</v>
       </c>
       <c r="D74" s="1" t="s">
@@ -2261,11 +2502,11 @@
         <v>103</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="75">
-      <c r="A75" s="2" t="n">
+    <row r="75" spans="1:5" hidden="1">
+      <c r="A75" s="2">
         <v>43218</v>
       </c>
-      <c r="C75" s="1" t="n">
+      <c r="C75" s="1">
         <v>404</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -2275,11 +2516,11 @@
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="76">
-      <c r="A76" s="2" t="n">
+    <row r="76" spans="1:5" hidden="1">
+      <c r="A76" s="2">
         <v>43220</v>
       </c>
-      <c r="C76" s="1" t="n">
+      <c r="C76" s="1">
         <v>57</v>
       </c>
       <c r="D76" s="1" t="s">
@@ -2289,11 +2530,11 @@
         <v>114</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="77">
-      <c r="A77" s="2" t="n">
+    <row r="77" spans="1:5" hidden="1">
+      <c r="A77" s="2">
         <v>43221</v>
       </c>
-      <c r="C77" s="1" t="n">
+      <c r="C77" s="1">
         <v>282</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -2303,11 +2544,11 @@
         <v>116</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="78">
-      <c r="A78" s="2" t="n">
+    <row r="78" spans="1:5" hidden="1">
+      <c r="A78" s="2">
         <v>43220</v>
       </c>
-      <c r="C78" s="1" t="n">
+      <c r="C78" s="1">
         <v>87</v>
       </c>
       <c r="D78" s="1" t="s">
@@ -2317,11 +2558,11 @@
         <v>117</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="79">
-      <c r="A79" s="2" t="n">
+    <row r="79" spans="1:5" hidden="1">
+      <c r="A79" s="2">
         <v>43223</v>
       </c>
-      <c r="B79" s="1" t="n">
+      <c r="B79" s="1">
         <v>1878</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -2331,11 +2572,11 @@
         <v>119</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="80">
-      <c r="A80" s="2" t="n">
+    <row r="80" spans="1:5" hidden="1">
+      <c r="A80" s="2">
         <v>43224</v>
       </c>
-      <c r="B80" s="1" t="n">
+      <c r="B80" s="1">
         <v>98</v>
       </c>
       <c r="D80" s="1" t="s">
@@ -2345,11 +2586,11 @@
         <v>120</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="81">
-      <c r="A81" s="2" t="n">
+    <row r="81" spans="1:5" hidden="1">
+      <c r="A81" s="2">
         <v>43225</v>
       </c>
-      <c r="C81" s="1" t="n">
+      <c r="C81" s="1">
         <v>198</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -2359,11 +2600,11 @@
         <v>122</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="82">
-      <c r="A82" s="2" t="n">
+    <row r="82" spans="1:5" hidden="1">
+      <c r="A82" s="2">
         <v>43225</v>
       </c>
-      <c r="C82" s="1" t="n">
+      <c r="C82" s="1">
         <v>406</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -2373,11 +2614,11 @@
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="83">
-      <c r="A83" s="2" t="n">
+    <row r="83" spans="1:5" hidden="1">
+      <c r="A83" s="2">
         <v>43228</v>
       </c>
-      <c r="B83" s="1" t="n">
+      <c r="B83" s="1">
         <v>168</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -2387,11 +2628,11 @@
         <v>124</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="84">
-      <c r="A84" s="2" t="n">
+    <row r="84" spans="1:5" hidden="1">
+      <c r="A84" s="2">
         <v>43229</v>
       </c>
-      <c r="B84" s="1" t="n">
+      <c r="B84" s="1">
         <v>240</v>
       </c>
       <c r="D84" s="1" t="s">
@@ -2401,12 +2642,12 @@
         <v>69</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="85">
-      <c r="A85" s="2" t="n">
+    <row r="85" spans="1:5" hidden="1">
+      <c r="A85" s="2">
         <v>43230</v>
       </c>
       <c r="B85" s="1"/>
-      <c r="C85" s="1" t="n">
+      <c r="C85" s="1">
         <v>420</v>
       </c>
       <c r="D85" s="1" t="s">
@@ -2416,11 +2657,11 @@
         <v>126</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="86">
-      <c r="A86" s="2" t="n">
+    <row r="86" spans="1:5" hidden="1">
+      <c r="A86" s="2">
         <v>43230</v>
       </c>
-      <c r="B86" s="1" t="n">
+      <c r="B86" s="1">
         <v>200</v>
       </c>
       <c r="C86" s="1"/>
@@ -2431,11 +2672,11 @@
         <v>127</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="87">
-      <c r="A87" s="2" t="n">
+    <row r="87" spans="1:5" hidden="1">
+      <c r="A87" s="2">
         <v>43230</v>
       </c>
-      <c r="C87" s="1" t="n">
+      <c r="C87" s="1">
         <v>280</v>
       </c>
       <c r="D87" s="1" t="s">
@@ -2445,11 +2686,11 @@
         <v>128</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="88">
-      <c r="A88" s="2" t="n">
+    <row r="88" spans="1:5" hidden="1">
+      <c r="A88" s="2">
         <v>43231</v>
       </c>
-      <c r="B88" s="1" t="n">
+      <c r="B88" s="1">
         <v>462</v>
       </c>
       <c r="D88" s="1" t="s">
@@ -2459,11 +2700,11 @@
         <v>130</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="89">
-      <c r="A89" s="2" t="n">
+    <row r="89" spans="1:5" hidden="1">
+      <c r="A89" s="2">
         <v>43231</v>
       </c>
-      <c r="B89" s="1" t="n">
+      <c r="B89" s="1">
         <v>499</v>
       </c>
       <c r="D89" s="1" t="s">
@@ -2473,11 +2714,11 @@
         <v>130</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="90">
-      <c r="A90" s="2" t="n">
+    <row r="90" spans="1:5" hidden="1">
+      <c r="A90" s="2">
         <v>43231</v>
       </c>
-      <c r="B90" s="1" t="n">
+      <c r="B90" s="1">
         <v>398</v>
       </c>
       <c r="D90" s="1" t="s">
@@ -2487,11 +2728,11 @@
         <v>133</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="91">
-      <c r="A91" s="2" t="n">
+    <row r="91" spans="1:5" hidden="1">
+      <c r="A91" s="2">
         <v>43231</v>
       </c>
-      <c r="B91" s="1" t="n">
+      <c r="B91" s="1">
         <v>226</v>
       </c>
       <c r="D91" s="1" t="s">
@@ -2501,11 +2742,11 @@
         <v>135</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="92">
-      <c r="A92" s="2" t="n">
+    <row r="92" spans="1:5" hidden="1">
+      <c r="A92" s="2">
         <v>43231</v>
       </c>
-      <c r="B92" s="1" t="n">
+      <c r="B92" s="1">
         <v>120</v>
       </c>
       <c r="D92" s="1" t="s">
@@ -2515,11 +2756,11 @@
         <v>137</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="93">
-      <c r="A93" s="2" t="n">
+    <row r="93" spans="1:5" hidden="1">
+      <c r="A93" s="2">
         <v>43232</v>
       </c>
-      <c r="B93" s="1" t="n">
+      <c r="B93" s="1">
         <v>80</v>
       </c>
       <c r="D93" s="1" t="s">
@@ -2529,11 +2770,11 @@
         <v>138</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="94">
-      <c r="A94" s="2" t="n">
+    <row r="94" spans="1:5" hidden="1">
+      <c r="A94" s="2">
         <v>43232</v>
       </c>
-      <c r="C94" s="1" t="n">
+      <c r="C94" s="1">
         <v>340</v>
       </c>
       <c r="D94" s="1" t="s">
@@ -2543,11 +2784,11 @@
         <v>139</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="95">
-      <c r="A95" s="2" t="n">
+    <row r="95" spans="1:5" hidden="1">
+      <c r="A95" s="2">
         <v>43232</v>
       </c>
-      <c r="B95" s="1" t="n">
+      <c r="B95" s="1">
         <v>510</v>
       </c>
       <c r="D95" s="1" t="s">
@@ -2557,11 +2798,11 @@
         <v>141</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="96">
-      <c r="A96" s="2" t="n">
+    <row r="96" spans="1:5" hidden="1">
+      <c r="A96" s="2">
         <v>43233</v>
       </c>
-      <c r="B96" s="1" t="n">
+      <c r="B96" s="1">
         <v>170</v>
       </c>
       <c r="D96" s="1" t="s">
@@ -2571,11 +2812,11 @@
         <v>143</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="97">
-      <c r="A97" s="2" t="n">
+    <row r="97" spans="1:5" hidden="1">
+      <c r="A97" s="2">
         <v>43233</v>
       </c>
-      <c r="C97" s="1" t="n">
+      <c r="C97" s="1">
         <v>130</v>
       </c>
       <c r="D97" s="1" t="s">
@@ -2585,11 +2826,11 @@
         <v>144</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="98">
-      <c r="A98" s="2" t="n">
+    <row r="98" spans="1:5" hidden="1">
+      <c r="A98" s="2">
         <v>43234</v>
       </c>
-      <c r="C98" s="1" t="n">
+      <c r="C98" s="1">
         <v>299</v>
       </c>
       <c r="D98" s="1" t="s">
@@ -2599,11 +2840,11 @@
         <v>145</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="99">
-      <c r="A99" s="2" t="n">
+    <row r="99" spans="1:5" hidden="1">
+      <c r="A99" s="2">
         <v>43236</v>
       </c>
-      <c r="B99" s="1" t="n">
+      <c r="B99" s="1">
         <v>3659</v>
       </c>
       <c r="D99" s="1" t="s">
@@ -2613,11 +2854,11 @@
         <v>146</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="100">
-      <c r="A100" s="2" t="n">
+    <row r="100" spans="1:5" hidden="1">
+      <c r="A100" s="2">
         <v>43237</v>
       </c>
-      <c r="B100" s="1" t="n">
+      <c r="B100" s="1">
         <v>79</v>
       </c>
       <c r="D100" s="1" t="s">
@@ -2627,11 +2868,11 @@
         <v>147</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="101">
-      <c r="A101" s="2" t="n">
+    <row r="101" spans="1:5" hidden="1">
+      <c r="A101" s="2">
         <v>43236</v>
       </c>
-      <c r="C101" s="1" t="n">
+      <c r="C101" s="1">
         <v>173</v>
       </c>
       <c r="D101" s="1" t="s">
@@ -2641,11 +2882,11 @@
         <v>148</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="102">
-      <c r="A102" s="2" t="n">
+    <row r="102" spans="1:5" hidden="1">
+      <c r="A102" s="2">
         <v>43240</v>
       </c>
-      <c r="B102" s="1" t="n">
+      <c r="B102" s="1">
         <v>130</v>
       </c>
       <c r="D102" s="1" t="s">
@@ -2655,22 +2896,22 @@
         <v>149</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="103">
-      <c r="A103" s="2" t="n">
+    <row r="103" spans="1:5" hidden="1">
+      <c r="A103" s="2">
         <v>43240</v>
       </c>
-      <c r="B103" s="1" t="n">
+      <c r="B103" s="1">
         <v>190</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="104">
-      <c r="A104" s="2" t="n">
+    <row r="104" spans="1:5" hidden="1">
+      <c r="A104" s="2">
         <v>43241</v>
       </c>
-      <c r="B104" s="1" t="n">
+      <c r="B104" s="1">
         <v>4070</v>
       </c>
       <c r="D104" s="1" t="s">
@@ -2680,11 +2921,11 @@
         <v>150</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="105">
-      <c r="A105" s="2" t="n">
+    <row r="105" spans="1:5" hidden="1">
+      <c r="A105" s="2">
         <v>43241</v>
       </c>
-      <c r="C105" s="1" t="n">
+      <c r="C105" s="1">
         <v>450</v>
       </c>
       <c r="D105" s="1" t="s">
@@ -2694,11 +2935,11 @@
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="106">
-      <c r="A106" s="2" t="n">
+    <row r="106" spans="1:5" hidden="1">
+      <c r="A106" s="2">
         <v>43242</v>
       </c>
-      <c r="B106" s="1" t="n">
+      <c r="B106" s="1">
         <v>79</v>
       </c>
       <c r="D106" s="1" t="s">
@@ -2708,11 +2949,11 @@
         <v>152</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="107">
-      <c r="A107" s="2" t="n">
+    <row r="107" spans="1:5" hidden="1">
+      <c r="A107" s="2">
         <v>43246</v>
       </c>
-      <c r="B107" s="1" t="n">
+      <c r="B107" s="1">
         <v>220</v>
       </c>
       <c r="D107" s="1" t="s">
@@ -2722,11 +2963,11 @@
         <v>154</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="108">
-      <c r="A108" s="2" t="n">
+    <row r="108" spans="1:5" hidden="1">
+      <c r="A108" s="2">
         <v>43247</v>
       </c>
-      <c r="B108" s="1" t="n">
+      <c r="B108" s="1">
         <v>70</v>
       </c>
       <c r="D108" s="1" t="s">
@@ -2736,44 +2977,44 @@
         <v>156</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="109">
-      <c r="A109" s="2" t="n">
+    <row r="109" spans="1:5" hidden="1">
+      <c r="A109" s="2">
         <v>43253</v>
       </c>
-      <c r="B109" s="1" t="n">
+      <c r="B109" s="1">
         <v>142</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="110">
-      <c r="A110" s="2" t="n">
+    <row r="110" spans="1:5" hidden="1">
+      <c r="A110" s="2">
         <v>43254</v>
       </c>
-      <c r="B110" s="1" t="n">
+      <c r="B110" s="1">
         <v>90</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="111">
-      <c r="A111" s="2" t="n">
+    <row r="111" spans="1:5" hidden="1">
+      <c r="A111" s="2">
         <v>43260</v>
       </c>
-      <c r="C111" s="1" t="n">
+      <c r="C111" s="1">
         <v>1400</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="112">
-      <c r="A112" s="2" t="n">
+    <row r="112" spans="1:5" hidden="1">
+      <c r="A112" s="2">
         <v>43260</v>
       </c>
-      <c r="C112" s="1" t="n">
+      <c r="C112" s="1">
         <v>400</v>
       </c>
       <c r="D112" s="1" t="s">
@@ -2783,33 +3024,33 @@
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="113">
-      <c r="A113" s="2" t="n">
+    <row r="113" spans="1:5" hidden="1">
+      <c r="A113" s="2">
         <v>43264</v>
       </c>
-      <c r="B113" s="1" t="n">
+      <c r="B113" s="1">
         <v>546</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="114">
-      <c r="A114" s="2" t="n">
+    <row r="114" spans="1:5" hidden="1">
+      <c r="A114" s="2">
         <v>43264</v>
       </c>
-      <c r="B114" s="1" t="n">
+      <c r="B114" s="1">
         <v>95</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="115">
-      <c r="A115" s="2" t="n">
+    <row r="115" spans="1:5" hidden="1">
+      <c r="A115" s="2">
         <v>43266</v>
       </c>
-      <c r="B115" s="1" t="n">
+      <c r="B115" s="1">
         <v>394</v>
       </c>
       <c r="D115" s="1" t="s">
@@ -2819,11 +3060,11 @@
         <v>163</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="116">
-      <c r="A116" s="2" t="n">
+    <row r="116" spans="1:5" hidden="1">
+      <c r="A116" s="2">
         <v>43266</v>
       </c>
-      <c r="B116" s="1" t="n">
+      <c r="B116" s="1">
         <v>1055</v>
       </c>
       <c r="D116" s="1" t="s">
@@ -2833,11 +3074,11 @@
         <v>165</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="117">
-      <c r="A117" s="2" t="n">
+    <row r="117" spans="1:5" hidden="1">
+      <c r="A117" s="2">
         <v>43284</v>
       </c>
-      <c r="C117" s="1" t="n">
+      <c r="C117" s="1">
         <v>274</v>
       </c>
       <c r="D117" s="1" t="s">
@@ -2847,11 +3088,11 @@
         <v>167</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="118">
-      <c r="A118" s="2" t="n">
+    <row r="118" spans="1:5" hidden="1">
+      <c r="A118" s="2">
         <v>43283</v>
       </c>
-      <c r="C118" s="1" t="n">
+      <c r="C118" s="1">
         <v>105</v>
       </c>
       <c r="D118" s="1" t="s">
@@ -2861,11 +3102,11 @@
         <v>169</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="119">
-      <c r="A119" s="2" t="n">
+    <row r="119" spans="1:5" hidden="1">
+      <c r="A119" s="2">
         <v>43289</v>
       </c>
-      <c r="C119" s="1" t="n">
+      <c r="C119" s="1">
         <v>128</v>
       </c>
       <c r="D119" s="1" t="s">
@@ -2875,11 +3116,11 @@
         <v>171</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="120">
-      <c r="A120" s="2" t="n">
+    <row r="120" spans="1:5" hidden="1">
+      <c r="A120" s="2">
         <v>43290</v>
       </c>
-      <c r="C120" s="1" t="n">
+      <c r="C120" s="1">
         <v>450</v>
       </c>
       <c r="D120" s="1" t="s">
@@ -2889,11 +3130,11 @@
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="121">
-      <c r="A121" s="2" t="n">
+    <row r="121" spans="1:5" hidden="1">
+      <c r="A121" s="2">
         <v>43290</v>
       </c>
-      <c r="C121" s="1" t="n">
+      <c r="C121" s="1">
         <v>210</v>
       </c>
       <c r="D121" s="1" t="s">
@@ -2903,44 +3144,44 @@
         <v>173</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="122">
-      <c r="A122" s="2" t="n">
+    <row r="122" spans="1:5" hidden="1">
+      <c r="A122" s="2">
         <v>43297</v>
       </c>
-      <c r="B122" s="1" t="n">
+      <c r="B122" s="1">
         <v>980</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="123">
-      <c r="A123" s="2" t="n">
+    <row r="123" spans="1:5" hidden="1">
+      <c r="A123" s="2">
         <v>43297</v>
       </c>
-      <c r="B123" s="1" t="n">
+      <c r="B123" s="1">
         <v>1260</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="124">
-      <c r="A124" s="2" t="n">
+    <row r="124" spans="1:5" hidden="1">
+      <c r="A124" s="2">
         <v>43297</v>
       </c>
-      <c r="B124" s="1" t="n">
+      <c r="B124" s="1">
         <v>3687</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="125">
-      <c r="A125" s="2" t="n">
+    <row r="125" spans="1:5" hidden="1">
+      <c r="A125" s="2">
         <v>43298</v>
       </c>
-      <c r="C125" s="1" t="n">
+      <c r="C125" s="1">
         <v>60</v>
       </c>
       <c r="D125" s="1" t="s">
@@ -2950,55 +3191,55 @@
         <v>178</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="126">
-      <c r="A126" s="2" t="n">
+    <row r="126" spans="1:5" hidden="1">
+      <c r="A126" s="2">
         <v>43291</v>
       </c>
-      <c r="C126" s="1" t="n">
+      <c r="C126" s="1">
         <v>404</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="127">
-      <c r="A127" s="2" t="n">
+    <row r="127" spans="1:5" hidden="1">
+      <c r="A127" s="2">
         <v>43290</v>
       </c>
-      <c r="C127" s="1" t="n">
+      <c r="C127" s="1">
         <v>451</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="128">
-      <c r="A128" s="2" t="n">
+    <row r="128" spans="1:5" hidden="1">
+      <c r="A128" s="2">
         <v>43298</v>
       </c>
-      <c r="C128" s="1" t="n">
+      <c r="C128" s="1">
         <v>708</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="129">
-      <c r="A129" s="2" t="n">
+    <row r="129" spans="1:5" hidden="1">
+      <c r="A129" s="2">
         <v>43293</v>
       </c>
-      <c r="C129" s="1" t="n">
+      <c r="C129" s="1">
         <v>160</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="130">
-      <c r="A130" s="2" t="n">
+    <row r="130" spans="1:5" hidden="1">
+      <c r="A130" s="2">
         <v>43288</v>
       </c>
-      <c r="C130" s="1" t="n">
+      <c r="C130" s="1">
         <v>72</v>
       </c>
       <c r="D130" s="1" t="s">
@@ -3008,11 +3249,11 @@
         <v>181</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="131">
-      <c r="A131" s="2" t="n">
+    <row r="131" spans="1:5" hidden="1">
+      <c r="A131" s="2">
         <v>43293</v>
       </c>
-      <c r="C131" s="1" t="n">
+      <c r="C131" s="1">
         <v>300</v>
       </c>
       <c r="D131" s="1" t="s">
@@ -3022,11 +3263,11 @@
         <v>183</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="132">
-      <c r="A132" s="2" t="n">
+    <row r="132" spans="1:5" hidden="1">
+      <c r="A132" s="2">
         <v>43293</v>
       </c>
-      <c r="C132" s="1" t="n">
+      <c r="C132" s="1">
         <v>230</v>
       </c>
       <c r="D132" s="1" t="s">
@@ -3036,22 +3277,22 @@
         <v>185</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="133">
-      <c r="A133" s="2" t="n">
+    <row r="133" spans="1:5" hidden="1">
+      <c r="A133" s="2">
         <v>43293</v>
       </c>
-      <c r="C133" s="1" t="n">
+      <c r="C133" s="1">
         <v>454</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="134">
-      <c r="A134" s="2" t="n">
+    <row r="134" spans="1:5" hidden="1">
+      <c r="A134" s="2">
         <v>43299</v>
       </c>
-      <c r="C134" s="1" t="n">
+      <c r="C134" s="1">
         <v>686</v>
       </c>
       <c r="D134" s="1" t="s">
@@ -3061,11 +3302,11 @@
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="135">
-      <c r="A135" s="2" t="n">
+    <row r="135" spans="1:5" hidden="1">
+      <c r="A135" s="2">
         <v>43310</v>
       </c>
-      <c r="C135" s="1" t="n">
+      <c r="C135" s="1">
         <v>400</v>
       </c>
       <c r="D135" s="1" t="s">
@@ -3075,11 +3316,11 @@
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="136">
-      <c r="A136" s="2" t="n">
+    <row r="136" spans="1:5" hidden="1">
+      <c r="A136" s="2">
         <v>43310</v>
       </c>
-      <c r="C136" s="1" t="n">
+      <c r="C136" s="1">
         <v>2067</v>
       </c>
       <c r="D136" s="1" t="s">
@@ -3089,11 +3330,11 @@
         <v>186</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="137">
-      <c r="A137" s="2" t="n">
+    <row r="137" spans="1:5" hidden="1">
+      <c r="A137" s="2">
         <v>43310</v>
       </c>
-      <c r="B137" s="1" t="n">
+      <c r="B137" s="1">
         <v>109</v>
       </c>
       <c r="D137" s="1" t="s">
@@ -3103,11 +3344,11 @@
         <v>187</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="138">
-      <c r="A138" s="2" t="n">
+    <row r="138" spans="1:5" hidden="1">
+      <c r="A138" s="2">
         <v>43310</v>
       </c>
-      <c r="B138" s="1" t="n">
+      <c r="B138" s="1">
         <v>97</v>
       </c>
       <c r="D138" s="1" t="s">
@@ -3117,11 +3358,11 @@
         <v>188</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="139">
-      <c r="A139" s="2" t="n">
+    <row r="139" spans="1:5" hidden="1">
+      <c r="A139" s="2">
         <v>43310</v>
       </c>
-      <c r="B139" s="1" t="n">
+      <c r="B139" s="1">
         <v>1437</v>
       </c>
       <c r="D139" s="1" t="s">
@@ -3131,11 +3372,11 @@
         <v>189</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="140">
-      <c r="A140" s="2" t="n">
+    <row r="140" spans="1:5" hidden="1">
+      <c r="A140" s="2">
         <v>43306</v>
       </c>
-      <c r="C140" s="1" t="n">
+      <c r="C140" s="1">
         <v>650</v>
       </c>
       <c r="D140" s="1" t="s">
@@ -3145,11 +3386,11 @@
         <v>190</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="141">
-      <c r="A141" s="2" t="n">
+    <row r="141" spans="1:5" hidden="1">
+      <c r="A141" s="2">
         <v>43305</v>
       </c>
-      <c r="C141" s="1" t="n">
+      <c r="C141" s="1">
         <v>120</v>
       </c>
       <c r="D141" s="1" t="s">
@@ -3159,11 +3400,11 @@
         <v>191</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="142">
-      <c r="A142" s="2" t="n">
+    <row r="142" spans="1:5" hidden="1">
+      <c r="A142" s="2">
         <v>43309</v>
       </c>
-      <c r="C142" s="1" t="n">
+      <c r="C142" s="1">
         <v>120</v>
       </c>
       <c r="D142" s="1" t="s">
@@ -3173,11 +3414,11 @@
         <v>192</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="0" r="143">
-      <c r="A143" s="2" t="n">
+    <row r="143" spans="1:5" ht="14.15" hidden="1">
+      <c r="A143" s="2">
         <v>43306</v>
       </c>
-      <c r="B143" s="1" t="n">
+      <c r="B143" s="1">
         <v>167</v>
       </c>
       <c r="D143" s="1" t="s">
@@ -3187,11 +3428,11 @@
         <v>193</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="0" r="144">
-      <c r="A144" s="2" t="n">
+    <row r="144" spans="1:5" ht="14.15" hidden="1">
+      <c r="A144" s="2">
         <v>43304</v>
       </c>
-      <c r="C144" s="1" t="n">
+      <c r="C144" s="1">
         <v>93</v>
       </c>
       <c r="D144" s="1" t="s">
@@ -3201,11 +3442,11 @@
         <v>194</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="145">
-      <c r="A145" s="2" t="n">
+    <row r="145" spans="1:5" hidden="1">
+      <c r="A145" s="2">
         <v>43305</v>
       </c>
-      <c r="C145" s="1" t="n">
+      <c r="C145" s="1">
         <v>450</v>
       </c>
       <c r="D145" s="1" t="s">
@@ -3215,11 +3456,11 @@
         <v>195</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="146">
-      <c r="A146" s="2" t="n">
+    <row r="146" spans="1:5" hidden="1">
+      <c r="A146" s="2">
         <v>43303</v>
       </c>
-      <c r="C146" s="1" t="n">
+      <c r="C146" s="1">
         <v>244</v>
       </c>
       <c r="D146" s="1" t="s">
@@ -3229,11 +3470,11 @@
         <v>196</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="147">
-      <c r="A147" s="2" t="n">
+    <row r="147" spans="1:5" hidden="1">
+      <c r="A147" s="2">
         <v>43310</v>
       </c>
-      <c r="C147" s="1" t="n">
+      <c r="C147" s="1">
         <v>482</v>
       </c>
       <c r="D147" s="1" t="s">
@@ -3243,11 +3484,11 @@
         <v>197</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="148">
-      <c r="A148" s="2" t="n">
+    <row r="148" spans="1:5" hidden="1">
+      <c r="A148" s="2">
         <v>43310</v>
       </c>
-      <c r="C148" s="1" t="n">
+      <c r="C148" s="1">
         <v>172</v>
       </c>
       <c r="D148" s="1" t="s">
@@ -3257,44 +3498,44 @@
         <v>199</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="149">
-      <c r="A149" s="7" t="n">
+    <row r="149" spans="1:5" hidden="1">
+      <c r="A149" s="7">
         <v>43314</v>
       </c>
-      <c r="B149" s="1" t="n">
+      <c r="B149" s="1">
         <v>89</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="150">
-      <c r="A150" s="7" t="n">
+    <row r="150" spans="1:5" hidden="1">
+      <c r="A150" s="7">
         <v>43314</v>
       </c>
-      <c r="C150" s="1" t="n">
+      <c r="C150" s="1">
         <v>107</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="151">
-      <c r="A151" s="7" t="n">
+    <row r="151" spans="1:5" hidden="1">
+      <c r="A151" s="7">
         <v>43314</v>
       </c>
-      <c r="C151" s="1" t="n">
+      <c r="C151" s="1">
         <v>124</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="152">
-      <c r="A152" s="7" t="n">
+    <row r="152" spans="1:5" hidden="1">
+      <c r="A152" s="7">
         <v>43316</v>
       </c>
-      <c r="C152" s="1" t="n">
+      <c r="C152" s="1">
         <v>4500</v>
       </c>
       <c r="D152" s="1" t="s">
@@ -3304,11 +3545,11 @@
         <v>202</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="153">
-      <c r="A153" s="2" t="n">
+    <row r="153" spans="1:5" hidden="1">
+      <c r="A153" s="2">
         <v>43317</v>
       </c>
-      <c r="C153" s="1" t="n">
+      <c r="C153" s="1">
         <v>247</v>
       </c>
       <c r="D153" s="1" t="s">
@@ -3318,11 +3559,11 @@
         <v>204</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="154">
-      <c r="A154" s="2" t="n">
+    <row r="154" spans="1:5" hidden="1">
+      <c r="A154" s="2">
         <v>43317</v>
       </c>
-      <c r="C154" s="1" t="n">
+      <c r="C154" s="1">
         <v>1150</v>
       </c>
       <c r="D154" s="1" t="s">
@@ -3332,11 +3573,11 @@
         <v>205</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="155">
-      <c r="A155" s="2" t="n">
+    <row r="155" spans="1:5" hidden="1">
+      <c r="A155" s="2">
         <v>43317</v>
       </c>
-      <c r="C155" s="1" t="n">
+      <c r="C155" s="1">
         <v>313</v>
       </c>
       <c r="D155" s="1" t="s">
@@ -3346,11 +3587,11 @@
         <v>207</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="156">
-      <c r="A156" s="2" t="n">
+    <row r="156" spans="1:5" hidden="1">
+      <c r="A156" s="2">
         <v>43317</v>
       </c>
-      <c r="B156" s="1" t="n">
+      <c r="B156" s="1">
         <v>280</v>
       </c>
       <c r="D156" s="1" t="s">
@@ -3360,11 +3601,11 @@
         <v>209</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="157">
-      <c r="A157" s="2" t="n">
+    <row r="157" spans="1:5" hidden="1">
+      <c r="A157" s="2">
         <v>43321</v>
       </c>
-      <c r="C157" s="1" t="n">
+      <c r="C157" s="1">
         <v>710</v>
       </c>
       <c r="D157" s="1" t="s">
@@ -3374,11 +3615,11 @@
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="158">
-      <c r="A158" s="2" t="n">
+    <row r="158" spans="1:5">
+      <c r="A158" s="2">
         <v>43321</v>
       </c>
-      <c r="C158" s="1" t="n">
+      <c r="C158" s="1">
         <v>100</v>
       </c>
       <c r="D158" s="1" t="s">
@@ -3388,11 +3629,11 @@
         <v>212</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="159">
-      <c r="A159" s="2" t="n">
+    <row r="159" spans="1:5">
+      <c r="A159" s="2">
         <v>43319</v>
       </c>
-      <c r="B159" s="1" t="n">
+      <c r="B159" s="1">
         <v>78</v>
       </c>
       <c r="D159" s="1" t="s">
@@ -3402,22 +3643,22 @@
         <v>213</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="160">
-      <c r="A160" s="2" t="n">
+    <row r="160" spans="1:5">
+      <c r="A160" s="2">
         <v>43321</v>
       </c>
-      <c r="B160" s="1" t="n">
+      <c r="B160" s="1">
         <v>1840</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="161">
-      <c r="A161" s="2" t="n">
+    <row r="161" spans="1:5">
+      <c r="A161" s="2">
         <v>43322</v>
       </c>
-      <c r="B161" s="1" t="n">
+      <c r="B161" s="1">
         <v>280</v>
       </c>
       <c r="D161" s="1" t="s">
@@ -3427,11 +3668,11 @@
         <v>216</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="162">
-      <c r="A162" s="7" t="n">
+    <row r="162" spans="1:5">
+      <c r="A162" s="7">
         <v>43324</v>
       </c>
-      <c r="C162" s="1" t="n">
+      <c r="C162" s="1">
         <v>230</v>
       </c>
       <c r="D162" s="1" t="s">
@@ -3441,11 +3682,11 @@
         <v>217</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="163">
-      <c r="A163" s="7" t="n">
+    <row r="163" spans="1:5">
+      <c r="A163" s="7">
         <v>43326</v>
       </c>
-      <c r="C163" s="1" t="n">
+      <c r="C163" s="1">
         <v>450</v>
       </c>
       <c r="D163" s="1" t="s">
@@ -3455,11 +3696,11 @@
         <v>219</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="164">
-      <c r="A164" s="7" t="n">
+    <row r="164" spans="1:5">
+      <c r="A164" s="7">
         <v>43314</v>
       </c>
-      <c r="B164" s="1" t="n">
+      <c r="B164" s="1">
         <v>45</v>
       </c>
       <c r="D164" s="1" t="s">
@@ -3469,1039 +3710,1073 @@
         <v>221</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="165">
-      <c r="A165" s="10" t="n">
+    <row r="165" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A165" s="10">
         <v>43327</v>
       </c>
-      <c r="C165" s="0" t="n">
+      <c r="C165">
         <v>486</v>
       </c>
-      <c r="D165" s="0" t="s">
+      <c r="D165" t="s">
         <v>218</v>
       </c>
-      <c r="E165" s="0" t="s">
+      <c r="E165" t="s">
         <v>222</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="166">
-      <c r="A166" s="10" t="n">
+    <row r="166" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A166" s="10">
         <v>43329</v>
       </c>
-      <c r="C166" s="0" t="n">
+      <c r="C166">
         <v>92</v>
       </c>
-      <c r="D166" s="0" t="s">
+      <c r="D166" t="s">
         <v>223</v>
       </c>
-      <c r="E166" s="0" t="s">
+      <c r="E166" t="s">
         <v>224</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="167">
-      <c r="A167" s="10" t="n">
+    <row r="167" spans="1:5">
+      <c r="A167" s="10">
         <v>43331</v>
       </c>
-      <c r="C167" s="0" t="n">
+      <c r="C167">
         <v>310</v>
       </c>
-      <c r="D167" s="0" t="s">
+      <c r="D167" t="s">
         <v>166</v>
       </c>
-      <c r="E167" s="0" t="s">
+      <c r="E167" t="s">
         <v>225</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="168">
-      <c r="A168" s="10" t="n">
+    <row r="168" spans="1:5">
+      <c r="A168" s="10">
         <v>43334</v>
       </c>
-      <c r="C168" s="0" t="n">
+      <c r="C168">
         <v>464</v>
       </c>
-      <c r="D168" s="0" t="s">
+      <c r="D168" t="s">
         <v>218</v>
       </c>
       <c r="E168" s="11" t="s">
         <v>226</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="169">
-      <c r="A169" s="10" t="n">
+    <row r="169" spans="1:5">
+      <c r="A169" s="10">
         <v>43335</v>
       </c>
-      <c r="C169" s="0" t="n">
+      <c r="C169">
         <v>726</v>
       </c>
-      <c r="D169" s="0" t="s">
+      <c r="D169" t="s">
         <v>227</v>
       </c>
-      <c r="E169" s="0" t="s">
+      <c r="E169" t="s">
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="170">
-      <c r="A170" s="10" t="n">
+    <row r="170" spans="1:5">
+      <c r="A170" s="10">
         <v>43337</v>
       </c>
-      <c r="C170" s="0" t="n">
+      <c r="C170">
         <v>544</v>
       </c>
-      <c r="D170" s="0" t="s">
+      <c r="D170" t="s">
         <v>218</v>
       </c>
-      <c r="E170" s="0" t="s">
+      <c r="E170" t="s">
         <v>228</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="171">
-      <c r="A171" s="10" t="n">
+    <row r="171" spans="1:5">
+      <c r="A171" s="10">
         <v>43337</v>
       </c>
-      <c r="B171" s="0" t="n">
+      <c r="B171">
         <v>100</v>
       </c>
-      <c r="D171" s="0" t="s">
+      <c r="D171" t="s">
         <v>142</v>
       </c>
-      <c r="E171" s="0" t="s">
+      <c r="E171" t="s">
         <v>229</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="172">
-      <c r="A172" s="10" t="n">
+    <row r="172" spans="1:5">
+      <c r="A172" s="10">
         <v>43341</v>
       </c>
-      <c r="C172" s="0" t="n">
+      <c r="C172">
         <v>830</v>
       </c>
-      <c r="D172" s="0" t="s">
+      <c r="D172" t="s">
         <v>230</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="173">
-      <c r="A173" s="10" t="n">
+    <row r="173" spans="1:5">
+      <c r="A173" s="10">
         <v>43335</v>
       </c>
-      <c r="C173" s="0" t="n">
+      <c r="C173">
         <v>22</v>
       </c>
-      <c r="D173" s="0" t="s">
+      <c r="D173" t="s">
         <v>231</v>
       </c>
-      <c r="E173" s="0" t="s">
+      <c r="E173" t="s">
         <v>232</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="174">
-      <c r="A174" s="10" t="n">
+    <row r="174" spans="1:5">
+      <c r="A174" s="10">
         <v>43335</v>
       </c>
-      <c r="B174" s="0" t="n">
+      <c r="B174">
         <v>100</v>
       </c>
-      <c r="D174" s="0" t="s">
+      <c r="D174" t="s">
         <v>233</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="175">
-      <c r="A175" s="10" t="n">
+    <row r="175" spans="1:5">
+      <c r="A175" s="10">
         <v>43344</v>
       </c>
-      <c r="B175" s="0" t="n">
+      <c r="B175">
         <v>500</v>
       </c>
-      <c r="D175" s="0" t="s">
+      <c r="D175" t="s">
         <v>234</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="176">
-      <c r="A176" s="10" t="n">
+    <row r="176" spans="1:5">
+      <c r="A176" s="10">
         <v>43344</v>
       </c>
-      <c r="B176" s="0" t="n">
+      <c r="B176">
         <v>50</v>
       </c>
-      <c r="D176" s="0" t="s">
+      <c r="D176" t="s">
         <v>223</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="177">
-      <c r="A177" s="10" t="n">
+    <row r="177" spans="1:5">
+      <c r="A177" s="10">
         <v>43345</v>
       </c>
-      <c r="C177" s="0" t="n">
+      <c r="C177">
         <v>607</v>
       </c>
-      <c r="D177" s="0" t="s">
+      <c r="D177" t="s">
         <v>235</v>
       </c>
-      <c r="E177" s="0" t="s">
+      <c r="E177" t="s">
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="178">
-      <c r="A178" s="10" t="n">
+    <row r="178" spans="1:5">
+      <c r="A178" s="10">
         <v>43345</v>
       </c>
-      <c r="C178" s="0" t="n">
+      <c r="C178">
         <v>444</v>
       </c>
-      <c r="D178" s="0" t="s">
+      <c r="D178" t="s">
         <v>218</v>
       </c>
-      <c r="E178" s="0" t="s">
+      <c r="E178" t="s">
         <v>204</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="179">
-      <c r="A179" s="10" t="n">
+    <row r="179" spans="1:5">
+      <c r="A179" s="10">
         <v>43345</v>
       </c>
-      <c r="C179" s="0" t="n">
+      <c r="C179">
         <v>312</v>
       </c>
-      <c r="D179" s="0" t="s">
+      <c r="D179" t="s">
         <v>166</v>
       </c>
-      <c r="E179" s="0" t="s">
+      <c r="E179" t="s">
         <v>236</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="180">
-      <c r="A180" s="10" t="n">
+    <row r="180" spans="1:5">
+      <c r="A180" s="10">
         <v>43345</v>
       </c>
-      <c r="C180" s="0" t="n">
+      <c r="C180">
         <v>501</v>
       </c>
-      <c r="D180" s="0" t="s">
+      <c r="D180" t="s">
         <v>218</v>
       </c>
-      <c r="E180" s="0" t="s">
+      <c r="E180" t="s">
         <v>237</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="181">
-      <c r="A181" s="10" t="n">
+    <row r="181" spans="1:5">
+      <c r="A181" s="10">
         <v>43349</v>
       </c>
-      <c r="C181" s="0" t="n">
+      <c r="C181">
         <v>711</v>
       </c>
-      <c r="D181" s="0" t="s">
+      <c r="D181" t="s">
         <v>238</v>
       </c>
-      <c r="E181" s="0" t="s">
+      <c r="E181" t="s">
         <v>239</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="182">
-      <c r="A182" s="10" t="n">
+    <row r="182" spans="1:5">
+      <c r="A182" s="10">
         <v>43354</v>
       </c>
-      <c r="B182" s="0" t="n">
+      <c r="B182">
         <v>126</v>
       </c>
-      <c r="D182" s="0" t="s">
+      <c r="D182" t="s">
         <v>101</v>
       </c>
-      <c r="E182" s="0" t="s">
+      <c r="E182" t="s">
         <v>240</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="183">
-      <c r="A183" s="10" t="n">
+    <row r="183" spans="1:5">
+      <c r="A183" s="10">
         <v>43354</v>
       </c>
-      <c r="C183" s="0" t="n">
+      <c r="C183">
         <v>450</v>
       </c>
-      <c r="D183" s="0" t="s">
+      <c r="D183" t="s">
         <v>241</v>
       </c>
-      <c r="E183" s="0" t="s">
+      <c r="E183" t="s">
         <v>242</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="184">
-      <c r="A184" s="10" t="n">
+    <row r="184" spans="1:5">
+      <c r="A184" s="10">
         <v>43361</v>
       </c>
-      <c r="C184" s="0" t="n">
+      <c r="C184">
         <v>660</v>
       </c>
-      <c r="D184" s="0" t="s">
+      <c r="D184" t="s">
         <v>243</v>
       </c>
-      <c r="E184" s="0" t="s">
+      <c r="E184" t="s">
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="185">
-      <c r="A185" s="10" t="n">
+    <row r="185" spans="1:5">
+      <c r="A185" s="10">
         <v>43363</v>
       </c>
-      <c r="C185" s="0" t="n">
+      <c r="C185">
         <v>230</v>
       </c>
-      <c r="D185" s="0" t="s">
+      <c r="D185" t="s">
         <v>241</v>
       </c>
-      <c r="E185" s="0" t="s">
+      <c r="E185" t="s">
         <v>244</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="186">
-      <c r="A186" s="10" t="n">
+    <row r="186" spans="1:5">
+      <c r="A186" s="10">
         <v>43365</v>
       </c>
-      <c r="B186" s="0" t="n">
+      <c r="B186">
         <v>4859</v>
       </c>
-      <c r="D186" s="0" t="s">
+      <c r="D186" t="s">
         <v>245</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="187">
-      <c r="A187" s="10" t="n">
+    <row r="187" spans="1:5">
+      <c r="A187" s="10">
         <v>43365</v>
       </c>
-      <c r="B187" s="0" t="n">
+      <c r="B187">
         <v>295</v>
       </c>
-      <c r="D187" s="0" t="s">
+      <c r="D187" t="s">
         <v>246</v>
       </c>
-      <c r="E187" s="0" t="s">
+      <c r="E187" t="s">
         <v>247</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="188">
-      <c r="A188" s="10" t="n">
+    <row r="188" spans="1:5">
+      <c r="A188" s="10">
         <v>43365</v>
       </c>
-      <c r="B188" s="0" t="n">
+      <c r="B188">
         <v>50</v>
       </c>
-      <c r="D188" s="0" t="s">
+      <c r="D188" t="s">
         <v>248</v>
       </c>
-      <c r="E188" s="0" t="s">
+      <c r="E188" t="s">
         <v>247</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="189">
-      <c r="A189" s="10" t="n">
+    <row r="189" spans="1:5">
+      <c r="A189" s="10">
         <v>43365</v>
       </c>
-      <c r="B189" s="0" t="n">
+      <c r="B189">
         <v>300</v>
       </c>
-      <c r="D189" s="0" t="s">
+      <c r="D189" t="s">
         <v>249</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="190">
-      <c r="A190" s="10" t="n">
+    <row r="190" spans="1:5">
+      <c r="A190" s="10">
         <v>43378</v>
       </c>
-      <c r="B190" s="0" t="n">
+      <c r="B190">
         <v>506</v>
       </c>
-      <c r="D190" s="0" t="s">
+      <c r="D190" t="s">
         <v>47</v>
       </c>
-      <c r="E190" s="0" t="s">
+      <c r="E190" t="s">
         <v>250</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="191">
-      <c r="A191" s="10" t="n">
+    <row r="191" spans="1:5">
+      <c r="A191" s="10">
         <v>43379</v>
       </c>
-      <c r="B191" s="0" t="n">
+      <c r="B191">
         <v>350</v>
       </c>
-      <c r="D191" s="0" t="s">
+      <c r="D191" t="s">
         <v>251</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="20" outlineLevel="0" r="192">
-      <c r="A192" s="10" t="n">
+    <row r="192" spans="1:5" ht="20.05" customHeight="1">
+      <c r="A192" s="10">
         <v>43383</v>
       </c>
-      <c r="B192" s="0" t="n">
+      <c r="B192">
         <v>189</v>
       </c>
-      <c r="D192" s="0" t="s">
+      <c r="D192" t="s">
         <v>252</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="193">
-      <c r="A193" s="10" t="n">
+    <row r="193" spans="1:5">
+      <c r="A193" s="10">
         <v>43387</v>
       </c>
-      <c r="B193" s="0" t="n">
+      <c r="B193">
         <v>150</v>
       </c>
-      <c r="D193" s="0" t="s">
+      <c r="D193" t="s">
         <v>253</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="194">
-      <c r="A194" s="10" t="n">
+    <row r="194" spans="1:5">
+      <c r="A194" s="10">
         <v>43387</v>
       </c>
-      <c r="B194" s="0" t="n">
+      <c r="B194">
         <v>307</v>
       </c>
-      <c r="D194" s="0" t="s">
+      <c r="D194" t="s">
         <v>254</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="195">
-      <c r="C195" s="0" t="n">
+    <row r="195" spans="1:5">
+      <c r="C195">
         <v>3705</v>
       </c>
-      <c r="E195" s="0" t="s">
+      <c r="E195" t="s">
         <v>255</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="196">
-      <c r="A196" s="10" t="n">
+    <row r="196" spans="1:5">
+      <c r="A196" s="10">
         <v>43385</v>
       </c>
-      <c r="C196" s="0" t="n">
+      <c r="C196">
         <v>608</v>
       </c>
-      <c r="D196" s="0" t="s">
+      <c r="D196" t="s">
         <v>210</v>
       </c>
-      <c r="E196" s="0" t="s">
+      <c r="E196" t="s">
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="197">
-      <c r="A197" s="10" t="n">
+    <row r="197" spans="1:5">
+      <c r="A197" s="10">
         <v>43391</v>
       </c>
-      <c r="B197" s="0" t="n">
+      <c r="B197">
         <v>120</v>
       </c>
-      <c r="D197" s="0" t="s">
+      <c r="D197" t="s">
         <v>223</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="198">
-      <c r="A198" s="10" t="n">
+    <row r="198" spans="1:5">
+      <c r="A198" s="10">
         <v>43392</v>
       </c>
-      <c r="B198" s="0" t="n">
+      <c r="B198">
         <v>130</v>
       </c>
-      <c r="D198" s="0" t="s">
+      <c r="D198" t="s">
         <v>123</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="199">
-      <c r="A199" s="10" t="n">
+    <row r="199" spans="1:5">
+      <c r="A199" s="10">
         <v>43393</v>
       </c>
-      <c r="B199" s="0" t="n">
+      <c r="B199">
         <v>177</v>
       </c>
-      <c r="D199" s="0" t="s">
+      <c r="D199" t="s">
         <v>111</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="200">
-      <c r="A200" s="10" t="n">
+    <row r="200" spans="1:5">
+      <c r="A200" s="10">
         <v>43393</v>
       </c>
-      <c r="C200" s="0" t="n">
+      <c r="C200">
         <v>125</v>
       </c>
-      <c r="D200" s="0" t="s">
+      <c r="D200" t="s">
         <v>256</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="201">
-      <c r="A201" s="10" t="n">
+    <row r="201" spans="1:5">
+      <c r="A201" s="10">
         <v>43395</v>
       </c>
-      <c r="B201" s="0" t="n">
+      <c r="B201">
         <v>2800</v>
       </c>
       <c r="D201" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="E201" s="0" t="s">
+      <c r="E201" t="s">
         <v>258</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="202">
-      <c r="A202" s="10" t="n">
+    <row r="202" spans="1:5">
+      <c r="A202" s="10">
         <v>43395</v>
       </c>
-      <c r="C202" s="0" t="n">
+      <c r="C202">
         <v>71</v>
       </c>
-      <c r="D202" s="0" t="s">
+      <c r="D202" t="s">
         <v>259</v>
       </c>
-      <c r="E202" s="0" t="s">
+      <c r="E202" t="s">
         <v>260</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="203">
-      <c r="A203" s="10" t="n">
+    <row r="203" spans="1:5">
+      <c r="A203" s="10">
         <v>43396</v>
       </c>
-      <c r="C203" s="0" t="n">
+      <c r="C203">
         <v>692</v>
       </c>
-      <c r="D203" s="0" t="s">
+      <c r="D203" t="s">
         <v>210</v>
       </c>
-      <c r="E203" s="0" t="s">
+      <c r="E203" t="s">
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="204">
-      <c r="A204" s="10" t="n">
+    <row r="204" spans="1:5">
+      <c r="A204" s="10">
         <v>43397</v>
       </c>
-      <c r="C204" s="0" t="n">
+      <c r="C204">
         <v>4935</v>
       </c>
-      <c r="D204" s="0" t="s">
+      <c r="D204" t="s">
         <v>261</v>
       </c>
-      <c r="E204" s="0" t="s">
+      <c r="E204" t="s">
         <v>262</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10" outlineLevel="0" r="205">
-      <c r="A205" s="10" t="n">
+    <row r="205" spans="1:5" ht="10" customHeight="1">
+      <c r="A205" s="10">
         <v>43398</v>
       </c>
-      <c r="B205" s="0" t="n">
+      <c r="B205">
         <v>130</v>
       </c>
-      <c r="D205" s="0" t="s">
+      <c r="D205" t="s">
         <v>263</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="206">
-      <c r="A206" s="10" t="n">
+    <row r="206" spans="1:5">
+      <c r="A206" s="10">
         <v>43398</v>
       </c>
-      <c r="B206" s="0" t="n">
+      <c r="B206">
         <v>370</v>
       </c>
-      <c r="D206" s="0" t="s">
+      <c r="D206" t="s">
         <v>161</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="207">
-      <c r="A207" s="10" t="n">
+    <row r="207" spans="1:5">
+      <c r="A207" s="10">
         <v>43398</v>
       </c>
-      <c r="B207" s="0" t="n">
+      <c r="B207">
         <v>4966</v>
       </c>
-      <c r="D207" s="0" t="s">
+      <c r="D207" t="s">
         <v>264</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="208">
-      <c r="A208" s="10" t="n">
+    <row r="208" spans="1:5">
+      <c r="A208" s="10">
         <v>43397</v>
       </c>
-      <c r="C208" s="0" t="n">
+      <c r="C208">
         <v>70</v>
       </c>
-      <c r="D208" s="0" t="s">
+      <c r="D208" t="s">
         <v>265</v>
       </c>
-      <c r="E208" s="0" t="s">
+      <c r="E208" t="s">
         <v>266</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="209">
-      <c r="A209" s="10" t="n">
+    <row r="209" spans="1:5">
+      <c r="A209" s="10">
         <v>43399</v>
       </c>
-      <c r="B209" s="0" t="n">
+      <c r="B209">
         <v>182</v>
       </c>
-      <c r="D209" s="0" t="s">
+      <c r="D209" t="s">
         <v>142</v>
       </c>
-      <c r="E209" s="0" t="s">
+      <c r="E209" t="s">
         <v>267</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="210">
-      <c r="A210" s="10" t="n">
+    <row r="210" spans="1:5">
+      <c r="A210" s="10">
         <v>43401</v>
       </c>
-      <c r="B210" s="0" t="n">
+      <c r="B210">
         <v>700</v>
       </c>
-      <c r="D210" s="0" t="s">
+      <c r="D210" t="s">
         <v>161</v>
       </c>
-      <c r="E210" s="0" t="s">
+      <c r="E210" t="s">
         <v>244</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="211">
-      <c r="A211" s="10" t="n">
+    <row r="211" spans="1:5">
+      <c r="A211" s="10">
         <v>43405</v>
       </c>
-      <c r="B211" s="0" t="n">
+      <c r="B211">
         <v>274</v>
       </c>
-      <c r="D211" s="0" t="s">
+      <c r="D211" t="s">
         <v>268</v>
       </c>
-      <c r="E211" s="0" t="s">
+      <c r="E211" t="s">
         <v>269</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="212">
-      <c r="A212" s="10" t="n">
+    <row r="212" spans="1:5">
+      <c r="A212" s="10">
         <v>43405</v>
       </c>
-      <c r="C212" s="0" t="n">
+      <c r="C212">
         <v>590</v>
       </c>
-      <c r="D212" s="0" t="s">
+      <c r="D212" t="s">
         <v>123</v>
       </c>
-      <c r="E212" s="0" t="s">
+      <c r="E212" t="s">
         <v>250</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="213">
-      <c r="A213" s="10" t="n">
+    <row r="213" spans="1:5" ht="14.15">
+      <c r="A213" s="10">
         <v>43407</v>
       </c>
-      <c r="C213" s="0" t="n">
+      <c r="C213">
         <v>1275</v>
       </c>
       <c r="D213" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="E213" s="0" t="s">
+      <c r="E213" t="s">
         <v>271</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="214">
-      <c r="A214" s="10" t="n">
+    <row r="214" spans="1:5" ht="14.15">
+      <c r="A214" s="10">
         <v>43407</v>
       </c>
-      <c r="C214" s="0" t="n">
+      <c r="C214">
         <v>4781</v>
       </c>
       <c r="D214" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="E214" s="0" t="s">
+      <c r="E214" t="s">
         <v>271</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="215">
-      <c r="A215" s="10" t="n">
+    <row r="215" spans="1:5" ht="14.15">
+      <c r="A215" s="10">
         <v>43407</v>
       </c>
-      <c r="C215" s="0" t="n">
+      <c r="C215">
         <v>4781</v>
       </c>
       <c r="D215" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="E215" s="0" t="s">
+      <c r="E215" t="s">
         <v>271</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="216">
-      <c r="A216" s="10" t="n">
+    <row r="216" spans="1:5">
+      <c r="A216" s="10">
         <v>43406</v>
       </c>
-      <c r="C216" s="0" t="n">
+      <c r="C216">
         <v>50</v>
       </c>
-      <c r="D216" s="0" t="s">
+      <c r="D216" t="s">
         <v>272</v>
       </c>
-      <c r="E216" s="0" t="s">
+      <c r="E216" t="s">
         <v>273</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="217">
-      <c r="A217" s="10" t="n">
+    <row r="217" spans="1:5">
+      <c r="A217" s="10">
         <v>43409</v>
       </c>
-      <c r="C217" s="0" t="n">
+      <c r="C217">
         <v>677</v>
       </c>
-      <c r="D217" s="0" t="s">
+      <c r="D217" t="s">
         <v>210</v>
       </c>
-      <c r="E217" s="0" t="s">
+      <c r="E217" t="s">
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="218">
-      <c r="A218" s="10" t="n">
+    <row r="218" spans="1:5" ht="14.15">
+      <c r="A218" s="10">
         <v>43410</v>
       </c>
-      <c r="B218" s="0" t="n">
+      <c r="B218">
         <v>285</v>
       </c>
       <c r="D218" s="13" t="s">
         <v>274</v>
       </c>
-      <c r="E218" s="0" t="s">
+      <c r="E218" t="s">
         <v>275</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="219">
-      <c r="A219" s="10" t="n">
+    <row r="219" spans="1:5" ht="14.15">
+      <c r="A219" s="10">
         <v>43410</v>
       </c>
-      <c r="B219" s="0" t="n">
+      <c r="B219">
         <v>125</v>
       </c>
       <c r="D219" s="13" t="s">
         <v>276</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="220">
-      <c r="A220" s="10" t="n">
+    <row r="220" spans="1:5" ht="14.15">
+      <c r="A220" s="10">
         <v>43409</v>
       </c>
-      <c r="B220" s="0" t="n">
+      <c r="B220">
         <v>85</v>
       </c>
       <c r="D220" s="13" t="s">
         <v>277</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="221">
-      <c r="A221" s="10" t="n">
+    <row r="221" spans="1:5" ht="14.15">
+      <c r="A221" s="10">
         <v>43410</v>
       </c>
-      <c r="B221" s="0" t="n">
+      <c r="B221">
         <v>44</v>
       </c>
       <c r="D221" s="13" t="s">
         <v>278</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="222">
-      <c r="A222" s="10" t="n">
+    <row r="222" spans="1:5">
+      <c r="A222" s="10">
         <v>43412</v>
       </c>
-      <c r="C222" s="0" t="n">
+      <c r="C222">
         <v>190</v>
       </c>
-      <c r="D222" s="0" t="s">
+      <c r="D222" t="s">
         <v>111</v>
       </c>
-      <c r="E222" s="0" t="s">
+      <c r="E222" t="s">
         <v>279</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="223">
-      <c r="A223" s="10" t="n">
+    <row r="223" spans="1:5" ht="14.15">
+      <c r="A223" s="10">
         <v>43415</v>
       </c>
-      <c r="B223" s="0" t="n">
+      <c r="B223">
         <v>189</v>
       </c>
       <c r="D223" s="13" t="s">
         <v>280</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="224">
-      <c r="A224" s="10" t="n">
+    <row r="224" spans="1:5" ht="14.15">
+      <c r="A224" s="10">
         <v>43415</v>
       </c>
-      <c r="B224" s="0" t="n">
+      <c r="B224">
         <v>336</v>
       </c>
       <c r="D224" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="E224" s="0" t="s">
+      <c r="E224" t="s">
         <v>281</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="225">
-      <c r="A225" s="10" t="n">
+    <row r="225" spans="1:5" ht="14.15">
+      <c r="A225" s="10">
         <v>43419</v>
       </c>
-      <c r="B225" s="0" t="n">
+      <c r="B225">
         <v>158</v>
       </c>
       <c r="D225" s="13" t="s">
         <v>282</v>
       </c>
-      <c r="E225" s="0" t="s">
+      <c r="E225" t="s">
         <v>283</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="226">
-      <c r="A226" s="10" t="n">
+    <row r="226" spans="1:5">
+      <c r="A226" s="10">
         <v>43418</v>
       </c>
-      <c r="C226" s="0" t="n">
+      <c r="C226">
         <v>642</v>
       </c>
-      <c r="D226" s="0" t="s">
+      <c r="D226" t="s">
         <v>210</v>
       </c>
-      <c r="E226" s="0" t="s">
+      <c r="E226" t="s">
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="227">
-      <c r="A227" s="10" t="n">
+    <row r="227" spans="1:5">
+      <c r="A227" s="10">
         <v>43419</v>
       </c>
-      <c r="C227" s="0" t="n">
+      <c r="C227">
         <v>370</v>
       </c>
-      <c r="D227" s="0" t="s">
+      <c r="D227" t="s">
         <v>284</v>
       </c>
-      <c r="E227" s="0" t="s">
+      <c r="E227" t="s">
         <v>285</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="228">
-      <c r="A228" s="10" t="n">
+    <row r="228" spans="1:5">
+      <c r="A228" s="10">
         <v>43419</v>
       </c>
-      <c r="C228" s="0" t="n">
+      <c r="C228">
         <v>222</v>
       </c>
-      <c r="D228" s="0" t="s">
+      <c r="D228" t="s">
         <v>286</v>
       </c>
-      <c r="E228" s="0" t="s">
+      <c r="E228" t="s">
         <v>287</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="229">
-      <c r="A229" s="10" t="n">
+    <row r="229" spans="1:5">
+      <c r="A229" s="10">
         <v>43421</v>
       </c>
-      <c r="B229" s="0" t="n">
+      <c r="B229">
         <v>300</v>
       </c>
-      <c r="D229" s="0" t="s">
+      <c r="D229" t="s">
         <v>288</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="230">
-      <c r="A230" s="10" t="n">
+    <row r="230" spans="1:5">
+      <c r="A230" s="10">
         <v>43422</v>
       </c>
-      <c r="B230" s="0" t="n">
+      <c r="B230">
         <v>158</v>
       </c>
-      <c r="D230" s="0" t="s">
+      <c r="D230" t="s">
         <v>56</v>
       </c>
-      <c r="E230" s="0" t="s">
+      <c r="E230" t="s">
         <v>112</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="231">
-      <c r="A231" s="10" t="n">
+    <row r="231" spans="1:5">
+      <c r="A231" s="10">
         <v>43422</v>
       </c>
-      <c r="B231" s="0" t="n">
+      <c r="B231">
         <v>159</v>
       </c>
-      <c r="D231" s="0" t="s">
+      <c r="D231" t="s">
         <v>164</v>
       </c>
-      <c r="E231" s="0" t="s">
+      <c r="E231" t="s">
         <v>112</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="232">
-      <c r="A232" s="10" t="n">
+    <row r="232" spans="1:5">
+      <c r="A232" s="10">
         <v>43421</v>
       </c>
-      <c r="C232" s="0" t="n">
+      <c r="C232">
         <v>80</v>
       </c>
-      <c r="D232" s="0" t="s">
+      <c r="D232" t="s">
         <v>111</v>
       </c>
-      <c r="E232" s="0" t="s">
+      <c r="E232" t="s">
         <v>289</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="233">
-      <c r="A233" s="10" t="n">
+    <row r="233" spans="1:5">
+      <c r="A233" s="10">
         <v>43422</v>
       </c>
-      <c r="B233" s="0" t="n">
+      <c r="B233">
         <v>11649</v>
       </c>
-      <c r="D233" s="0" t="s">
+      <c r="D233" t="s">
         <v>290</v>
       </c>
-      <c r="E233" s="0" t="s">
+      <c r="E233" t="s">
         <v>291</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="234">
-      <c r="A234" s="10" t="n">
+    <row r="234" spans="1:5">
+      <c r="A234" s="10">
         <v>43426</v>
       </c>
-      <c r="C234" s="0" t="n">
+      <c r="C234">
         <v>308</v>
       </c>
-      <c r="D234" s="0" t="s">
+      <c r="D234" t="s">
         <v>159</v>
       </c>
-      <c r="E234" s="0" t="s">
+      <c r="E234" t="s">
         <v>292</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="235">
-      <c r="A235" s="10" t="n">
+    <row r="235" spans="1:5">
+      <c r="A235" s="10">
         <v>43428</v>
       </c>
-      <c r="B235" s="0" t="n">
+      <c r="B235">
         <v>112</v>
       </c>
-      <c r="D235" s="0" t="s">
+      <c r="D235" t="s">
         <v>164</v>
       </c>
-      <c r="E235" s="0" t="s">
+      <c r="E235" t="s">
         <v>93</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="236">
-      <c r="A236" s="10" t="n">
+    <row r="236" spans="1:5">
+      <c r="A236" s="10">
         <v>43428</v>
       </c>
-      <c r="B236" s="0" t="n">
+      <c r="B236">
         <v>79</v>
       </c>
-      <c r="D236" s="0" t="s">
+      <c r="D236" t="s">
         <v>113</v>
       </c>
-      <c r="E236" s="0" t="s">
+      <c r="E236" t="s">
         <v>293</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="237">
-      <c r="A237" s="10" t="n">
+    <row r="237" spans="1:5">
+      <c r="A237" s="10">
         <v>43425</v>
       </c>
-      <c r="C237" s="0" t="n">
+      <c r="C237">
         <v>93</v>
       </c>
-      <c r="D237" s="0" t="s">
+      <c r="D237" t="s">
         <v>272</v>
       </c>
-      <c r="E237" s="0" t="s">
+      <c r="E237" t="s">
         <v>294</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="238">
-      <c r="A238" s="10" t="n">
+    <row r="238" spans="1:5">
+      <c r="A238" s="10">
         <v>43426</v>
       </c>
-      <c r="C238" s="0" t="n">
+      <c r="C238">
         <v>308</v>
       </c>
-      <c r="D238" s="0" t="s">
+      <c r="D238" t="s">
         <v>295</v>
       </c>
-      <c r="E238" s="0" t="s">
+      <c r="E238" t="s">
         <v>296</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="239">
-      <c r="A239" s="10" t="n">
+    <row r="239" spans="1:5">
+      <c r="A239" s="10">
         <v>43430</v>
       </c>
-      <c r="C239" s="0" t="n">
+      <c r="C239">
         <v>616</v>
       </c>
-      <c r="D239" s="0" t="s">
+      <c r="D239" t="s">
         <v>210</v>
       </c>
-      <c r="E239" s="0" t="s">
+      <c r="E239" t="s">
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="240">
-      <c r="A240" s="10" t="n">
+    <row r="240" spans="1:5">
+      <c r="A240" s="10">
         <v>43430</v>
       </c>
-      <c r="C240" s="0" t="n">
+      <c r="C240">
         <v>243</v>
       </c>
-      <c r="D240" s="0" t="s">
+      <c r="D240" t="s">
         <v>297</v>
       </c>
-      <c r="E240" s="0" t="s">
+      <c r="E240" t="s">
         <v>298</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="241">
-      <c r="A241" s="10" t="n">
+    <row r="241" spans="1:5">
+      <c r="A241" s="10">
         <v>43432</v>
       </c>
-      <c r="C241" s="0" t="n">
+      <c r="C241">
         <v>850</v>
       </c>
-      <c r="D241" s="0" t="s">
+      <c r="D241" t="s">
         <v>299</v>
       </c>
-      <c r="E241" s="0" t="s">
+      <c r="E241" t="s">
         <v>300</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="260">
-      <c r="B260" s="0" t="n">
-        <f aca="false">SUM(B2:B259)</f>
-        <v>69591</v>
-      </c>
-      <c r="C260" s="0" t="n">
-        <f aca="false">SUM(C2:C259)</f>
-        <v>68577</v>
+    <row r="242" spans="1:5">
+      <c r="A242" s="10">
+        <v>43433</v>
+      </c>
+      <c r="B242">
+        <v>75</v>
+      </c>
+      <c r="D242" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5">
+      <c r="A243" s="10">
+        <v>43433</v>
+      </c>
+      <c r="C243">
+        <v>212</v>
+      </c>
+      <c r="D243" t="s">
+        <v>30</v>
+      </c>
+      <c r="E243" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5">
+      <c r="A244" s="10">
+        <v>43433</v>
+      </c>
+      <c r="C244">
+        <v>200</v>
+      </c>
+      <c r="D244" t="s">
+        <v>303</v>
+      </c>
+      <c r="E244" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="260" spans="2:3">
+      <c r="B260">
+        <f>SUM(B2:B259)</f>
+        <v>69666</v>
+      </c>
+      <c r="C260">
+        <f>SUM(C2:C259)</f>
+        <v>68989</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A30:Z32">
-    <cfRule aboveAverage="0" bottom="0" dxfId="0" operator="expression" percent="0" priority="2" rank="0" text="" type="expression">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>LEN(TRIM(A30))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink display="netonnet.se" ref="D33" r:id="rId1"/>
-    <hyperlink display="www.vidaxl.se" ref="D40" r:id="rId2"/>
-    <hyperlink display="https://www.vardia.se/" ref="D201" r:id="rId3"/>
+    <hyperlink ref="D33" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D40" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D201" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
cost update jenny dec3
</commit_message>
<xml_diff>
--- a/Cost.xlsx
+++ b/Cost.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chengkaiyan/github/cost/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7B22DD-E053-E044-94ED-5F216DA076F5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="18900" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="308">
   <si>
     <t>日期</t>
   </si>
@@ -931,7 +926,7 @@
     <t>沙琪玛；tofu，etc</t>
   </si>
   <si>
-    <t xml:space="preserve">ICA taby </t>
+    <t>ICA taby </t>
   </si>
   <si>
     <t>mjork；chips；etc</t>
@@ -941,61 +936,80 @@
   </si>
   <si>
     <t>牛奶酸奶姜葱鸡</t>
+  </si>
+  <si>
+    <t>dishwash gel,brod,semper rice powder</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="yyyy/m/d"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt formatCode="YYYY/M/D" numFmtId="165"/>
+    <numFmt formatCode="M/D/YYYY" numFmtId="166"/>
+    <numFmt formatCode="YYYY\-MM\-DD" numFmtId="167"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="10">
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <family val="0"/>
       <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
       <name val="Arial"/>
       <family val="2"/>
+      <sz val="10"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF666666"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF666666"/>
+      <sz val="11"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0563C1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF0563C1"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0563C1"/>
       <name val="FreeSans"/>
       <family val="2"/>
+      <color rgb="FF0563C1"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF444444"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF444444"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1025,7 +1039,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
@@ -1033,31 +1047,100 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+  <cellStyleXfs count="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="167" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="20">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="7">
+    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle builtinId="8" customBuiltin="false" name="*unknown*" xfId="20"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1068,7 +1151,6 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1127,339 +1209,31 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF444444"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:Z260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A234" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E245" sqref="E245"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A234" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E246" activeCellId="0" pane="topLeft" sqref="E246"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="3" width="14.5"/>
-    <col min="4" max="4" width="26"/>
-    <col min="5" max="5" width="37.83203125"/>
-    <col min="6" max="1025" width="14.5"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="14.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1476,11 +1250,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1">
-      <c r="A2" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="2">
+      <c r="A2" s="2" t="n">
         <v>43121</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="1" t="n">
         <v>250</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1490,11 +1264,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1">
-      <c r="A3" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="3">
+      <c r="A3" s="2" t="n">
         <v>43122</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="1" t="n">
         <v>305</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1504,11 +1278,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1">
-      <c r="A4" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="4">
+      <c r="A4" s="2" t="n">
         <v>43122</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1518,11 +1292,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1">
-      <c r="A5" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="5">
+      <c r="A5" s="2" t="n">
         <v>43125</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="1" t="n">
         <v>98</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1532,11 +1306,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1">
-      <c r="A6" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="6">
+      <c r="A6" s="2" t="n">
         <v>43126</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1546,11 +1320,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1">
-      <c r="A7" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="7">
+      <c r="A7" s="2" t="n">
         <v>43127</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1560,11 +1334,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1">
-      <c r="A8" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="8">
+      <c r="A8" s="2" t="n">
         <v>43128</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="1" t="n">
         <v>656</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1574,11 +1348,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1">
-      <c r="A9" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="9">
+      <c r="A9" s="2" t="n">
         <v>43131</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="1" t="n">
         <v>486</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1588,11 +1362,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1">
-      <c r="A10" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="10">
+      <c r="A10" s="2" t="n">
         <v>43132</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="1" t="n">
         <v>76</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1602,11 +1376,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1">
-      <c r="A11" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="11">
+      <c r="A11" s="2" t="n">
         <v>43133</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="1" t="n">
         <v>399</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1616,11 +1390,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1">
-      <c r="A12" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="12">
+      <c r="A12" s="2" t="n">
         <v>43135</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="1" t="n">
         <v>419</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1630,11 +1404,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1">
-      <c r="A13" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="13">
+      <c r="A13" s="2" t="n">
         <v>43136</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="1" t="n">
         <v>521</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1644,11 +1418,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1">
-      <c r="A14" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="14">
+      <c r="A14" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="1" t="n">
         <v>399</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1658,11 +1432,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1">
-      <c r="A15" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="15">
+      <c r="A15" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="1" t="n">
         <v>138</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1672,11 +1446,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1">
-      <c r="A16" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="16">
+      <c r="A16" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="1" t="n">
         <v>310</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1686,12 +1460,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1">
-      <c r="A17" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="17">
+      <c r="A17" s="2" t="n">
         <v>43138</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="1">
+      <c r="C17" s="1" t="n">
         <v>700</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1701,12 +1475,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1">
-      <c r="A18" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="18">
+      <c r="A18" s="2" t="n">
         <v>43141</v>
       </c>
-      <c r="C18" s="1">
-        <f>F18*G18</f>
+      <c r="C18" s="1" t="n">
+        <f aca="false">F18*G18</f>
         <v>1312</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -1715,18 +1489,18 @@
       <c r="E18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="1" t="n">
         <v>164</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="1" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1">
-      <c r="A19" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="19">
+      <c r="A19" s="2" t="n">
         <v>43141</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="1" t="n">
         <v>1190</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1736,11 +1510,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1">
-      <c r="A20" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="20">
+      <c r="A20" s="2" t="n">
         <v>43154</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="1" t="n">
         <v>438</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1750,11 +1524,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1">
-      <c r="A21" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="21">
+      <c r="A21" s="2" t="n">
         <v>43154</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="1" t="n">
         <v>248</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -1764,22 +1538,22 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1">
-      <c r="A22" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="22">
+      <c r="A22" s="2" t="n">
         <v>43166</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="1" t="n">
         <v>234</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1">
-      <c r="A23" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="23">
+      <c r="A23" s="2" t="n">
         <v>43171</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="1" t="n">
         <v>118</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1789,22 +1563,22 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1">
-      <c r="A24" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="24">
+      <c r="A24" s="2" t="n">
         <v>43173</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="1" t="n">
         <v>82</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1">
-      <c r="A25" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="25">
+      <c r="A25" s="2" t="n">
         <v>43174</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1814,22 +1588,22 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1">
-      <c r="A26" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="26">
+      <c r="A26" s="2" t="n">
         <v>43175</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="1" t="n">
         <v>370</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:7" hidden="1">
-      <c r="A27" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="27">
+      <c r="A27" s="2" t="n">
         <v>43175</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -1839,11 +1613,11 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1">
-      <c r="A28" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="28">
+      <c r="A28" s="2" t="n">
         <v>43176</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="1" t="n">
         <v>624</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -1853,11 +1627,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1">
-      <c r="A29" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="29">
+      <c r="A29" s="2" t="n">
         <v>43177</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="1" t="n">
         <v>170</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1867,22 +1641,22 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1">
-      <c r="A30" s="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="30">
+      <c r="A30" s="4" t="n">
         <v>43179</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1">
-      <c r="A31" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="31">
+      <c r="A31" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="1" t="n">
         <v>90</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -1892,11 +1666,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1">
-      <c r="A32" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="32">
+      <c r="A32" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="1" t="n">
         <v>72</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -1906,11 +1680,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:26" hidden="1">
-      <c r="A33" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="33">
+      <c r="A33" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="1" t="n">
         <v>908</v>
       </c>
       <c r="D33" s="6" t="s">
@@ -1920,11 +1694,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:26" hidden="1">
-      <c r="A34" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="34">
+      <c r="A34" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -1934,11 +1708,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:26" hidden="1">
-      <c r="A35" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="35">
+      <c r="A35" s="2" t="n">
         <v>43181</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -1948,11 +1722,11 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:26" hidden="1">
-      <c r="A36" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="36">
+      <c r="A36" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="1" t="n">
         <v>135</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -1962,11 +1736,11 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:26" hidden="1">
-      <c r="A37" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="37">
+      <c r="A37" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="1" t="n">
         <v>110</v>
       </c>
       <c r="C37" s="1"/>
@@ -1998,11 +1772,11 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38" spans="1:26" hidden="1">
-      <c r="A38" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="38">
+      <c r="A38" s="2" t="n">
         <v>43185</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="1" t="n">
         <v>122</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -2012,22 +1786,22 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:26" hidden="1">
-      <c r="A39" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="39">
+      <c r="A39" s="2" t="n">
         <v>43187</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="1" t="n">
         <v>750</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:26" hidden="1">
-      <c r="A40" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="40">
+      <c r="A40" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="1" t="n">
         <v>379</v>
       </c>
       <c r="D40" s="6" t="s">
@@ -2037,22 +1811,22 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:26" hidden="1">
-      <c r="A41" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="41">
+      <c r="A41" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="1" t="n">
         <v>240</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:26" hidden="1">
-      <c r="A42" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="42">
+      <c r="A42" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="1" t="n">
         <v>540</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -2062,11 +1836,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:26" hidden="1">
-      <c r="A43" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="43">
+      <c r="A43" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -2076,11 +1850,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:26" hidden="1">
-      <c r="A44" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="44">
+      <c r="A44" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -2090,11 +1864,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:26" hidden="1">
-      <c r="A45" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="45">
+      <c r="A45" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="1" t="n">
         <v>462</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -2104,11 +1878,11 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:26" hidden="1">
-      <c r="A46" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="46">
+      <c r="A46" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46" s="1" t="n">
         <v>70</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -2118,11 +1892,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:26" hidden="1">
-      <c r="A47" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="47">
+      <c r="A47" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -2132,11 +1906,11 @@
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="1:26" hidden="1">
-      <c r="A48" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="48">
+      <c r="A48" s="2" t="n">
         <v>43190</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="1" t="n">
         <v>30</v>
       </c>
       <c r="C48" s="1"/>
@@ -2147,11 +1921,11 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1">
-      <c r="A49" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="49">
+      <c r="A49" s="2" t="n">
         <v>43191</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="1" t="n">
         <v>40</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -2161,11 +1935,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1">
-      <c r="A50" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="50">
+      <c r="A50" s="7" t="n">
         <v>43193</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50" s="1" t="n">
         <v>150</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -2175,11 +1949,11 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1">
-      <c r="A51" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="51">
+      <c r="A51" s="2" t="n">
         <v>43194</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51" s="1" t="n">
         <v>1360</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -2189,11 +1963,11 @@
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1">
-      <c r="A52" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="52">
+      <c r="A52" s="2" t="n">
         <v>43195</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" s="1" t="n">
         <v>94</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -2203,11 +1977,11 @@
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1">
-      <c r="A53" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="53">
+      <c r="A53" s="2" t="n">
         <v>43196</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C53" s="1" t="n">
         <v>48</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -2217,11 +1991,11 @@
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1">
-      <c r="A54" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="54">
+      <c r="A54" s="2" t="n">
         <v>43196</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C54" s="1" t="n">
         <v>205</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -2231,11 +2005,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1">
-      <c r="A55" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="55">
+      <c r="A55" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -2245,11 +2019,11 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1">
-      <c r="A56" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="56">
+      <c r="A56" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56" s="1" t="n">
         <v>421</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -2259,11 +2033,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1">
-      <c r="A57" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="57">
+      <c r="A57" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="1" t="n">
         <v>191</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -2273,11 +2047,11 @@
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1">
-      <c r="A58" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="58">
+      <c r="A58" s="2" t="n">
         <v>43198</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58" s="1" t="n">
         <v>226</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -2287,22 +2061,22 @@
         <v>96</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1">
-      <c r="A59" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="59">
+      <c r="A59" s="2" t="n">
         <v>43200</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59" s="1" t="n">
         <v>250</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1">
-      <c r="A60" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="60">
+      <c r="A60" s="2" t="n">
         <v>43200</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60" s="1" t="n">
         <v>1115</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -2312,11 +2086,11 @@
         <v>99</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1">
-      <c r="A61" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="61">
+      <c r="A61" s="2" t="n">
         <v>43201</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -2326,11 +2100,11 @@
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1">
-      <c r="A62" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="62">
+      <c r="A62" s="2" t="n">
         <v>43201</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62" s="1" t="n">
         <v>88</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -2340,11 +2114,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1">
-      <c r="A63" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="63">
+      <c r="A63" s="2" t="n">
         <v>43203</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -2354,11 +2128,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1">
-      <c r="A64" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="64">
+      <c r="A64" s="2" t="n">
         <v>43203</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C64" s="1" t="n">
         <v>364</v>
       </c>
       <c r="D64" s="1" t="s">
@@ -2368,11 +2142,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1">
-      <c r="A65" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="65">
+      <c r="A65" s="2" t="n">
         <v>43204</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65" s="1" t="n">
         <v>65</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -2382,11 +2156,11 @@
         <v>105</v>
       </c>
     </row>
-    <row r="66" spans="1:5" hidden="1">
-      <c r="A66" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="66">
+      <c r="A66" s="2" t="n">
         <v>43208</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -2396,11 +2170,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1">
-      <c r="A67" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="67">
+      <c r="A67" s="2" t="n">
         <v>43208</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C67" s="1" t="n">
         <v>470</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -2410,11 +2184,11 @@
         <v>107</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1">
-      <c r="A68" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="68">
+      <c r="A68" s="2" t="n">
         <v>43209</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68" s="1" t="n">
         <v>180</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -2424,11 +2198,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1">
-      <c r="A69" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="69">
+      <c r="A69" s="2" t="n">
         <v>43210</v>
       </c>
-      <c r="C69" s="1">
+      <c r="C69" s="1" t="n">
         <v>420</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -2438,11 +2212,11 @@
         <v>109</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1">
-      <c r="A70" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="70">
+      <c r="A70" s="2" t="n">
         <v>43212</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70" s="1" t="n">
         <v>50</v>
       </c>
       <c r="D70" s="1" t="s">
@@ -2452,11 +2226,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1">
-      <c r="A71" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="71">
+      <c r="A71" s="2" t="n">
         <v>43212</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71" s="1" t="n">
         <v>164</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -2466,11 +2240,11 @@
         <v>112</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1">
-      <c r="A72" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="72">
+      <c r="A72" s="2" t="n">
         <v>43215</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B72" s="1" t="n">
         <v>300</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -2480,11 +2254,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1">
-      <c r="A73" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="73">
+      <c r="A73" s="2" t="n">
         <v>43217</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73" s="1" t="n">
         <v>364</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -2494,11 +2268,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1">
-      <c r="A74" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="74">
+      <c r="A74" s="2" t="n">
         <v>43218</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74" s="1" t="n">
         <v>185</v>
       </c>
       <c r="D74" s="1" t="s">
@@ -2508,11 +2282,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1">
-      <c r="A75" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="75">
+      <c r="A75" s="2" t="n">
         <v>43218</v>
       </c>
-      <c r="C75" s="1">
+      <c r="C75" s="1" t="n">
         <v>404</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -2522,11 +2296,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="76" spans="1:5" hidden="1">
-      <c r="A76" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="76">
+      <c r="A76" s="2" t="n">
         <v>43220</v>
       </c>
-      <c r="C76" s="1">
+      <c r="C76" s="1" t="n">
         <v>57</v>
       </c>
       <c r="D76" s="1" t="s">
@@ -2536,11 +2310,11 @@
         <v>114</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1">
-      <c r="A77" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="77">
+      <c r="A77" s="2" t="n">
         <v>43221</v>
       </c>
-      <c r="C77" s="1">
+      <c r="C77" s="1" t="n">
         <v>282</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -2550,11 +2324,11 @@
         <v>116</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1">
-      <c r="A78" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="78">
+      <c r="A78" s="2" t="n">
         <v>43220</v>
       </c>
-      <c r="C78" s="1">
+      <c r="C78" s="1" t="n">
         <v>87</v>
       </c>
       <c r="D78" s="1" t="s">
@@ -2564,11 +2338,11 @@
         <v>117</v>
       </c>
     </row>
-    <row r="79" spans="1:5" hidden="1">
-      <c r="A79" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="79">
+      <c r="A79" s="2" t="n">
         <v>43223</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B79" s="1" t="n">
         <v>1878</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -2578,11 +2352,11 @@
         <v>119</v>
       </c>
     </row>
-    <row r="80" spans="1:5" hidden="1">
-      <c r="A80" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="80">
+      <c r="A80" s="2" t="n">
         <v>43224</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B80" s="1" t="n">
         <v>98</v>
       </c>
       <c r="D80" s="1" t="s">
@@ -2592,11 +2366,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="81" spans="1:5" hidden="1">
-      <c r="A81" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="81">
+      <c r="A81" s="2" t="n">
         <v>43225</v>
       </c>
-      <c r="C81" s="1">
+      <c r="C81" s="1" t="n">
         <v>198</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -2606,11 +2380,11 @@
         <v>122</v>
       </c>
     </row>
-    <row r="82" spans="1:5" hidden="1">
-      <c r="A82" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="82">
+      <c r="A82" s="2" t="n">
         <v>43225</v>
       </c>
-      <c r="C82" s="1">
+      <c r="C82" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -2620,11 +2394,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="83" spans="1:5" hidden="1">
-      <c r="A83" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="83">
+      <c r="A83" s="2" t="n">
         <v>43228</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83" s="1" t="n">
         <v>168</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -2634,11 +2408,11 @@
         <v>124</v>
       </c>
     </row>
-    <row r="84" spans="1:5" hidden="1">
-      <c r="A84" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="84">
+      <c r="A84" s="2" t="n">
         <v>43229</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B84" s="1" t="n">
         <v>240</v>
       </c>
       <c r="D84" s="1" t="s">
@@ -2648,12 +2422,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:5" hidden="1">
-      <c r="A85" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="85">
+      <c r="A85" s="2" t="n">
         <v>43230</v>
       </c>
       <c r="B85" s="1"/>
-      <c r="C85" s="1">
+      <c r="C85" s="1" t="n">
         <v>420</v>
       </c>
       <c r="D85" s="1" t="s">
@@ -2663,11 +2437,11 @@
         <v>126</v>
       </c>
     </row>
-    <row r="86" spans="1:5" hidden="1">
-      <c r="A86" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="86">
+      <c r="A86" s="2" t="n">
         <v>43230</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B86" s="1" t="n">
         <v>200</v>
       </c>
       <c r="C86" s="1"/>
@@ -2678,11 +2452,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="87" spans="1:5" hidden="1">
-      <c r="A87" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="87">
+      <c r="A87" s="2" t="n">
         <v>43230</v>
       </c>
-      <c r="C87" s="1">
+      <c r="C87" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D87" s="1" t="s">
@@ -2692,11 +2466,11 @@
         <v>128</v>
       </c>
     </row>
-    <row r="88" spans="1:5" hidden="1">
-      <c r="A88" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="88">
+      <c r="A88" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B88" s="1" t="n">
         <v>462</v>
       </c>
       <c r="D88" s="1" t="s">
@@ -2706,11 +2480,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="89" spans="1:5" hidden="1">
-      <c r="A89" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="89">
+      <c r="A89" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B89" s="1" t="n">
         <v>499</v>
       </c>
       <c r="D89" s="1" t="s">
@@ -2720,11 +2494,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="90" spans="1:5" hidden="1">
-      <c r="A90" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="90">
+      <c r="A90" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B90" s="1">
+      <c r="B90" s="1" t="n">
         <v>398</v>
       </c>
       <c r="D90" s="1" t="s">
@@ -2734,11 +2508,11 @@
         <v>133</v>
       </c>
     </row>
-    <row r="91" spans="1:5" hidden="1">
-      <c r="A91" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="91">
+      <c r="A91" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B91" s="1">
+      <c r="B91" s="1" t="n">
         <v>226</v>
       </c>
       <c r="D91" s="1" t="s">
@@ -2748,11 +2522,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="92" spans="1:5" hidden="1">
-      <c r="A92" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="92">
+      <c r="A92" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B92" s="1">
+      <c r="B92" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D92" s="1" t="s">
@@ -2762,11 +2536,11 @@
         <v>137</v>
       </c>
     </row>
-    <row r="93" spans="1:5" hidden="1">
-      <c r="A93" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="93">
+      <c r="A93" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="B93" s="1">
+      <c r="B93" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D93" s="1" t="s">
@@ -2776,11 +2550,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="94" spans="1:5" hidden="1">
-      <c r="A94" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="94">
+      <c r="A94" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="C94" s="1">
+      <c r="C94" s="1" t="n">
         <v>340</v>
       </c>
       <c r="D94" s="1" t="s">
@@ -2790,11 +2564,11 @@
         <v>139</v>
       </c>
     </row>
-    <row r="95" spans="1:5" hidden="1">
-      <c r="A95" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="95">
+      <c r="A95" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="B95" s="1">
+      <c r="B95" s="1" t="n">
         <v>510</v>
       </c>
       <c r="D95" s="1" t="s">
@@ -2804,11 +2578,11 @@
         <v>141</v>
       </c>
     </row>
-    <row r="96" spans="1:5" hidden="1">
-      <c r="A96" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="96">
+      <c r="A96" s="2" t="n">
         <v>43233</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B96" s="1" t="n">
         <v>170</v>
       </c>
       <c r="D96" s="1" t="s">
@@ -2818,11 +2592,11 @@
         <v>143</v>
       </c>
     </row>
-    <row r="97" spans="1:5" hidden="1">
-      <c r="A97" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="97">
+      <c r="A97" s="2" t="n">
         <v>43233</v>
       </c>
-      <c r="C97" s="1">
+      <c r="C97" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D97" s="1" t="s">
@@ -2832,11 +2606,11 @@
         <v>144</v>
       </c>
     </row>
-    <row r="98" spans="1:5" hidden="1">
-      <c r="A98" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="98">
+      <c r="A98" s="2" t="n">
         <v>43234</v>
       </c>
-      <c r="C98" s="1">
+      <c r="C98" s="1" t="n">
         <v>299</v>
       </c>
       <c r="D98" s="1" t="s">
@@ -2846,11 +2620,11 @@
         <v>145</v>
       </c>
     </row>
-    <row r="99" spans="1:5" hidden="1">
-      <c r="A99" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="99">
+      <c r="A99" s="2" t="n">
         <v>43236</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99" s="1" t="n">
         <v>3659</v>
       </c>
       <c r="D99" s="1" t="s">
@@ -2860,11 +2634,11 @@
         <v>146</v>
       </c>
     </row>
-    <row r="100" spans="1:5" hidden="1">
-      <c r="A100" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="100">
+      <c r="A100" s="2" t="n">
         <v>43237</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B100" s="1" t="n">
         <v>79</v>
       </c>
       <c r="D100" s="1" t="s">
@@ -2874,11 +2648,11 @@
         <v>147</v>
       </c>
     </row>
-    <row r="101" spans="1:5" hidden="1">
-      <c r="A101" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="101">
+      <c r="A101" s="2" t="n">
         <v>43236</v>
       </c>
-      <c r="C101" s="1">
+      <c r="C101" s="1" t="n">
         <v>173</v>
       </c>
       <c r="D101" s="1" t="s">
@@ -2888,11 +2662,11 @@
         <v>148</v>
       </c>
     </row>
-    <row r="102" spans="1:5" hidden="1">
-      <c r="A102" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="102">
+      <c r="A102" s="2" t="n">
         <v>43240</v>
       </c>
-      <c r="B102" s="1">
+      <c r="B102" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D102" s="1" t="s">
@@ -2902,22 +2676,22 @@
         <v>149</v>
       </c>
     </row>
-    <row r="103" spans="1:5" hidden="1">
-      <c r="A103" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="103">
+      <c r="A103" s="2" t="n">
         <v>43240</v>
       </c>
-      <c r="B103" s="1">
+      <c r="B103" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="104" spans="1:5" hidden="1">
-      <c r="A104" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="104">
+      <c r="A104" s="2" t="n">
         <v>43241</v>
       </c>
-      <c r="B104" s="1">
+      <c r="B104" s="1" t="n">
         <v>4070</v>
       </c>
       <c r="D104" s="1" t="s">
@@ -2927,11 +2701,11 @@
         <v>150</v>
       </c>
     </row>
-    <row r="105" spans="1:5" hidden="1">
-      <c r="A105" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="105">
+      <c r="A105" s="2" t="n">
         <v>43241</v>
       </c>
-      <c r="C105" s="1">
+      <c r="C105" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D105" s="1" t="s">
@@ -2941,11 +2715,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="106" spans="1:5" hidden="1">
-      <c r="A106" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="106">
+      <c r="A106" s="2" t="n">
         <v>43242</v>
       </c>
-      <c r="B106" s="1">
+      <c r="B106" s="1" t="n">
         <v>79</v>
       </c>
       <c r="D106" s="1" t="s">
@@ -2955,11 +2729,11 @@
         <v>152</v>
       </c>
     </row>
-    <row r="107" spans="1:5" hidden="1">
-      <c r="A107" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="107">
+      <c r="A107" s="2" t="n">
         <v>43246</v>
       </c>
-      <c r="B107" s="1">
+      <c r="B107" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D107" s="1" t="s">
@@ -2969,11 +2743,11 @@
         <v>154</v>
       </c>
     </row>
-    <row r="108" spans="1:5" hidden="1">
-      <c r="A108" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="108">
+      <c r="A108" s="2" t="n">
         <v>43247</v>
       </c>
-      <c r="B108" s="1">
+      <c r="B108" s="1" t="n">
         <v>70</v>
       </c>
       <c r="D108" s="1" t="s">
@@ -2983,44 +2757,44 @@
         <v>156</v>
       </c>
     </row>
-    <row r="109" spans="1:5" hidden="1">
-      <c r="A109" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="109">
+      <c r="A109" s="2" t="n">
         <v>43253</v>
       </c>
-      <c r="B109" s="1">
+      <c r="B109" s="1" t="n">
         <v>142</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="110" spans="1:5" hidden="1">
-      <c r="A110" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="110">
+      <c r="A110" s="2" t="n">
         <v>43254</v>
       </c>
-      <c r="B110" s="1">
+      <c r="B110" s="1" t="n">
         <v>90</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="111" spans="1:5" hidden="1">
-      <c r="A111" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="111">
+      <c r="A111" s="2" t="n">
         <v>43260</v>
       </c>
-      <c r="C111" s="1">
+      <c r="C111" s="1" t="n">
         <v>1400</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="112" spans="1:5" hidden="1">
-      <c r="A112" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="112">
+      <c r="A112" s="2" t="n">
         <v>43260</v>
       </c>
-      <c r="C112" s="1">
+      <c r="C112" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D112" s="1" t="s">
@@ -3030,33 +2804,33 @@
         <v>91</v>
       </c>
     </row>
-    <row r="113" spans="1:5" hidden="1">
-      <c r="A113" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="113">
+      <c r="A113" s="2" t="n">
         <v>43264</v>
       </c>
-      <c r="B113" s="1">
+      <c r="B113" s="1" t="n">
         <v>546</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="114" spans="1:5" hidden="1">
-      <c r="A114" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="114">
+      <c r="A114" s="2" t="n">
         <v>43264</v>
       </c>
-      <c r="B114" s="1">
+      <c r="B114" s="1" t="n">
         <v>95</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="115" spans="1:5" hidden="1">
-      <c r="A115" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="115">
+      <c r="A115" s="2" t="n">
         <v>43266</v>
       </c>
-      <c r="B115" s="1">
+      <c r="B115" s="1" t="n">
         <v>394</v>
       </c>
       <c r="D115" s="1" t="s">
@@ -3066,11 +2840,11 @@
         <v>163</v>
       </c>
     </row>
-    <row r="116" spans="1:5" hidden="1">
-      <c r="A116" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="116">
+      <c r="A116" s="2" t="n">
         <v>43266</v>
       </c>
-      <c r="B116" s="1">
+      <c r="B116" s="1" t="n">
         <v>1055</v>
       </c>
       <c r="D116" s="1" t="s">
@@ -3080,11 +2854,11 @@
         <v>165</v>
       </c>
     </row>
-    <row r="117" spans="1:5" hidden="1">
-      <c r="A117" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="117">
+      <c r="A117" s="2" t="n">
         <v>43284</v>
       </c>
-      <c r="C117" s="1">
+      <c r="C117" s="1" t="n">
         <v>274</v>
       </c>
       <c r="D117" s="1" t="s">
@@ -3094,11 +2868,11 @@
         <v>167</v>
       </c>
     </row>
-    <row r="118" spans="1:5" hidden="1">
-      <c r="A118" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="118">
+      <c r="A118" s="2" t="n">
         <v>43283</v>
       </c>
-      <c r="C118" s="1">
+      <c r="C118" s="1" t="n">
         <v>105</v>
       </c>
       <c r="D118" s="1" t="s">
@@ -3108,11 +2882,11 @@
         <v>169</v>
       </c>
     </row>
-    <row r="119" spans="1:5" hidden="1">
-      <c r="A119" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="119">
+      <c r="A119" s="2" t="n">
         <v>43289</v>
       </c>
-      <c r="C119" s="1">
+      <c r="C119" s="1" t="n">
         <v>128</v>
       </c>
       <c r="D119" s="1" t="s">
@@ -3122,11 +2896,11 @@
         <v>171</v>
       </c>
     </row>
-    <row r="120" spans="1:5" hidden="1">
-      <c r="A120" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="120">
+      <c r="A120" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C120" s="1">
+      <c r="C120" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D120" s="1" t="s">
@@ -3136,11 +2910,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="121" spans="1:5" hidden="1">
-      <c r="A121" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="121">
+      <c r="A121" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C121" s="1">
+      <c r="C121" s="1" t="n">
         <v>210</v>
       </c>
       <c r="D121" s="1" t="s">
@@ -3150,44 +2924,44 @@
         <v>173</v>
       </c>
     </row>
-    <row r="122" spans="1:5" hidden="1">
-      <c r="A122" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="122">
+      <c r="A122" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B122" s="1">
+      <c r="B122" s="1" t="n">
         <v>980</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="123" spans="1:5" hidden="1">
-      <c r="A123" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="123">
+      <c r="A123" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B123" s="1">
+      <c r="B123" s="1" t="n">
         <v>1260</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="124" spans="1:5" hidden="1">
-      <c r="A124" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="124">
+      <c r="A124" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B124" s="1">
+      <c r="B124" s="1" t="n">
         <v>3687</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="125" spans="1:5" hidden="1">
-      <c r="A125" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="125">
+      <c r="A125" s="2" t="n">
         <v>43298</v>
       </c>
-      <c r="C125" s="1">
+      <c r="C125" s="1" t="n">
         <v>60</v>
       </c>
       <c r="D125" s="1" t="s">
@@ -3197,55 +2971,55 @@
         <v>178</v>
       </c>
     </row>
-    <row r="126" spans="1:5" hidden="1">
-      <c r="A126" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="126">
+      <c r="A126" s="2" t="n">
         <v>43291</v>
       </c>
-      <c r="C126" s="1">
+      <c r="C126" s="1" t="n">
         <v>404</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="127" spans="1:5" hidden="1">
-      <c r="A127" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="127">
+      <c r="A127" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C127" s="1">
+      <c r="C127" s="1" t="n">
         <v>451</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="128" spans="1:5" hidden="1">
-      <c r="A128" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="128">
+      <c r="A128" s="2" t="n">
         <v>43298</v>
       </c>
-      <c r="C128" s="1">
+      <c r="C128" s="1" t="n">
         <v>708</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="129" spans="1:5" hidden="1">
-      <c r="A129" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="129">
+      <c r="A129" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C129" s="1">
+      <c r="C129" s="1" t="n">
         <v>160</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="130" spans="1:5" hidden="1">
-      <c r="A130" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="130">
+      <c r="A130" s="2" t="n">
         <v>43288</v>
       </c>
-      <c r="C130" s="1">
+      <c r="C130" s="1" t="n">
         <v>72</v>
       </c>
       <c r="D130" s="1" t="s">
@@ -3255,11 +3029,11 @@
         <v>181</v>
       </c>
     </row>
-    <row r="131" spans="1:5" hidden="1">
-      <c r="A131" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="131">
+      <c r="A131" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C131" s="1">
+      <c r="C131" s="1" t="n">
         <v>300</v>
       </c>
       <c r="D131" s="1" t="s">
@@ -3269,11 +3043,11 @@
         <v>183</v>
       </c>
     </row>
-    <row r="132" spans="1:5" hidden="1">
-      <c r="A132" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="132">
+      <c r="A132" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C132" s="1">
+      <c r="C132" s="1" t="n">
         <v>230</v>
       </c>
       <c r="D132" s="1" t="s">
@@ -3283,22 +3057,22 @@
         <v>185</v>
       </c>
     </row>
-    <row r="133" spans="1:5" hidden="1">
-      <c r="A133" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="133">
+      <c r="A133" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C133" s="1">
+      <c r="C133" s="1" t="n">
         <v>454</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="134" spans="1:5" hidden="1">
-      <c r="A134" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="134">
+      <c r="A134" s="2" t="n">
         <v>43299</v>
       </c>
-      <c r="C134" s="1">
+      <c r="C134" s="1" t="n">
         <v>686</v>
       </c>
       <c r="D134" s="1" t="s">
@@ -3308,11 +3082,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="135" spans="1:5" hidden="1">
-      <c r="A135" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="135">
+      <c r="A135" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C135" s="1">
+      <c r="C135" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D135" s="1" t="s">
@@ -3322,11 +3096,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="136" spans="1:5" hidden="1">
-      <c r="A136" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="136">
+      <c r="A136" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C136" s="1">
+      <c r="C136" s="1" t="n">
         <v>2067</v>
       </c>
       <c r="D136" s="1" t="s">
@@ -3336,11 +3110,11 @@
         <v>186</v>
       </c>
     </row>
-    <row r="137" spans="1:5" hidden="1">
-      <c r="A137" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="137">
+      <c r="A137" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B137" s="1">
+      <c r="B137" s="1" t="n">
         <v>109</v>
       </c>
       <c r="D137" s="1" t="s">
@@ -3350,11 +3124,11 @@
         <v>187</v>
       </c>
     </row>
-    <row r="138" spans="1:5" hidden="1">
-      <c r="A138" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="138">
+      <c r="A138" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B138" s="1">
+      <c r="B138" s="1" t="n">
         <v>97</v>
       </c>
       <c r="D138" s="1" t="s">
@@ -3364,11 +3138,11 @@
         <v>188</v>
       </c>
     </row>
-    <row r="139" spans="1:5" hidden="1">
-      <c r="A139" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="139">
+      <c r="A139" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B139" s="1">
+      <c r="B139" s="1" t="n">
         <v>1437</v>
       </c>
       <c r="D139" s="1" t="s">
@@ -3378,11 +3152,11 @@
         <v>189</v>
       </c>
     </row>
-    <row r="140" spans="1:5" hidden="1">
-      <c r="A140" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="140">
+      <c r="A140" s="2" t="n">
         <v>43306</v>
       </c>
-      <c r="C140" s="1">
+      <c r="C140" s="1" t="n">
         <v>650</v>
       </c>
       <c r="D140" s="1" t="s">
@@ -3392,11 +3166,11 @@
         <v>190</v>
       </c>
     </row>
-    <row r="141" spans="1:5" hidden="1">
-      <c r="A141" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="141">
+      <c r="A141" s="2" t="n">
         <v>43305</v>
       </c>
-      <c r="C141" s="1">
+      <c r="C141" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D141" s="1" t="s">
@@ -3406,11 +3180,11 @@
         <v>191</v>
       </c>
     </row>
-    <row r="142" spans="1:5" hidden="1">
-      <c r="A142" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="142">
+      <c r="A142" s="2" t="n">
         <v>43309</v>
       </c>
-      <c r="C142" s="1">
+      <c r="C142" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D142" s="1" t="s">
@@ -3420,11 +3194,11 @@
         <v>192</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="14" hidden="1">
-      <c r="A143" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="0" r="143">
+      <c r="A143" s="2" t="n">
         <v>43306</v>
       </c>
-      <c r="B143" s="1">
+      <c r="B143" s="1" t="n">
         <v>167</v>
       </c>
       <c r="D143" s="1" t="s">
@@ -3434,11 +3208,11 @@
         <v>193</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="14" hidden="1">
-      <c r="A144" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="0" r="144">
+      <c r="A144" s="2" t="n">
         <v>43304</v>
       </c>
-      <c r="C144" s="1">
+      <c r="C144" s="1" t="n">
         <v>93</v>
       </c>
       <c r="D144" s="1" t="s">
@@ -3448,11 +3222,11 @@
         <v>194</v>
       </c>
     </row>
-    <row r="145" spans="1:5" hidden="1">
-      <c r="A145" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="145">
+      <c r="A145" s="2" t="n">
         <v>43305</v>
       </c>
-      <c r="C145" s="1">
+      <c r="C145" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D145" s="1" t="s">
@@ -3462,11 +3236,11 @@
         <v>195</v>
       </c>
     </row>
-    <row r="146" spans="1:5" hidden="1">
-      <c r="A146" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="146">
+      <c r="A146" s="2" t="n">
         <v>43303</v>
       </c>
-      <c r="C146" s="1">
+      <c r="C146" s="1" t="n">
         <v>244</v>
       </c>
       <c r="D146" s="1" t="s">
@@ -3476,11 +3250,11 @@
         <v>196</v>
       </c>
     </row>
-    <row r="147" spans="1:5" hidden="1">
-      <c r="A147" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="147">
+      <c r="A147" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C147" s="1">
+      <c r="C147" s="1" t="n">
         <v>482</v>
       </c>
       <c r="D147" s="1" t="s">
@@ -3490,11 +3264,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="148" spans="1:5" hidden="1">
-      <c r="A148" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="148">
+      <c r="A148" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C148" s="1">
+      <c r="C148" s="1" t="n">
         <v>172</v>
       </c>
       <c r="D148" s="1" t="s">
@@ -3504,44 +3278,44 @@
         <v>199</v>
       </c>
     </row>
-    <row r="149" spans="1:5" hidden="1">
-      <c r="A149" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="149">
+      <c r="A149" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="B149" s="1">
+      <c r="B149" s="1" t="n">
         <v>89</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="150" spans="1:5" hidden="1">
-      <c r="A150" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="150">
+      <c r="A150" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="C150" s="1">
+      <c r="C150" s="1" t="n">
         <v>107</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="151" spans="1:5" hidden="1">
-      <c r="A151" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="151">
+      <c r="A151" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="C151" s="1">
+      <c r="C151" s="1" t="n">
         <v>124</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="152" spans="1:5" hidden="1">
-      <c r="A152" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="152">
+      <c r="A152" s="7" t="n">
         <v>43316</v>
       </c>
-      <c r="C152" s="1">
+      <c r="C152" s="1" t="n">
         <v>4500</v>
       </c>
       <c r="D152" s="1" t="s">
@@ -3551,11 +3325,11 @@
         <v>202</v>
       </c>
     </row>
-    <row r="153" spans="1:5" hidden="1">
-      <c r="A153" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="153">
+      <c r="A153" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C153" s="1">
+      <c r="C153" s="1" t="n">
         <v>247</v>
       </c>
       <c r="D153" s="1" t="s">
@@ -3565,11 +3339,11 @@
         <v>204</v>
       </c>
     </row>
-    <row r="154" spans="1:5" hidden="1">
-      <c r="A154" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="154">
+      <c r="A154" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C154" s="1">
+      <c r="C154" s="1" t="n">
         <v>1150</v>
       </c>
       <c r="D154" s="1" t="s">
@@ -3579,11 +3353,11 @@
         <v>205</v>
       </c>
     </row>
-    <row r="155" spans="1:5" hidden="1">
-      <c r="A155" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="155">
+      <c r="A155" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C155" s="1">
+      <c r="C155" s="1" t="n">
         <v>313</v>
       </c>
       <c r="D155" s="1" t="s">
@@ -3593,11 +3367,11 @@
         <v>207</v>
       </c>
     </row>
-    <row r="156" spans="1:5" hidden="1">
-      <c r="A156" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="156">
+      <c r="A156" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="B156" s="1">
+      <c r="B156" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D156" s="1" t="s">
@@ -3607,11 +3381,11 @@
         <v>209</v>
       </c>
     </row>
-    <row r="157" spans="1:5" hidden="1">
-      <c r="A157" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="157">
+      <c r="A157" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="C157" s="1">
+      <c r="C157" s="1" t="n">
         <v>710</v>
       </c>
       <c r="D157" s="1" t="s">
@@ -3621,11 +3395,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="158" spans="1:5">
-      <c r="A158" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="158">
+      <c r="A158" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="C158" s="1">
+      <c r="C158" s="1" t="n">
         <v>100</v>
       </c>
       <c r="D158" s="1" t="s">
@@ -3635,11 +3409,11 @@
         <v>212</v>
       </c>
     </row>
-    <row r="159" spans="1:5">
-      <c r="A159" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="159">
+      <c r="A159" s="2" t="n">
         <v>43319</v>
       </c>
-      <c r="B159" s="1">
+      <c r="B159" s="1" t="n">
         <v>78</v>
       </c>
       <c r="D159" s="1" t="s">
@@ -3649,22 +3423,22 @@
         <v>213</v>
       </c>
     </row>
-    <row r="160" spans="1:5">
-      <c r="A160" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="160">
+      <c r="A160" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="B160" s="1">
+      <c r="B160" s="1" t="n">
         <v>1840</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="161" spans="1:5">
-      <c r="A161" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="161">
+      <c r="A161" s="2" t="n">
         <v>43322</v>
       </c>
-      <c r="B161" s="1">
+      <c r="B161" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D161" s="1" t="s">
@@ -3674,11 +3448,11 @@
         <v>216</v>
       </c>
     </row>
-    <row r="162" spans="1:5">
-      <c r="A162" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="162">
+      <c r="A162" s="7" t="n">
         <v>43324</v>
       </c>
-      <c r="C162" s="1">
+      <c r="C162" s="1" t="n">
         <v>230</v>
       </c>
       <c r="D162" s="1" t="s">
@@ -3688,11 +3462,11 @@
         <v>217</v>
       </c>
     </row>
-    <row r="163" spans="1:5">
-      <c r="A163" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="163">
+      <c r="A163" s="7" t="n">
         <v>43326</v>
       </c>
-      <c r="C163" s="1">
+      <c r="C163" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D163" s="1" t="s">
@@ -3702,11 +3476,11 @@
         <v>219</v>
       </c>
     </row>
-    <row r="164" spans="1:5">
-      <c r="A164" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="164">
+      <c r="A164" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="B164" s="1">
+      <c r="B164" s="1" t="n">
         <v>45</v>
       </c>
       <c r="D164" s="1" t="s">
@@ -3716,1087 +3490,1106 @@
         <v>221</v>
       </c>
     </row>
-    <row r="165" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A165" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="165">
+      <c r="A165" s="10" t="n">
         <v>43327</v>
       </c>
-      <c r="C165">
+      <c r="C165" s="0" t="n">
         <v>486</v>
       </c>
-      <c r="D165" t="s">
+      <c r="D165" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E165" t="s">
+      <c r="E165" s="0" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="166" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A166" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="166">
+      <c r="A166" s="10" t="n">
         <v>43329</v>
       </c>
-      <c r="C166">
+      <c r="C166" s="0" t="n">
         <v>92</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D166" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="E166" t="s">
+      <c r="E166" s="0" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="167" spans="1:5">
-      <c r="A167" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="167">
+      <c r="A167" s="10" t="n">
         <v>43331</v>
       </c>
-      <c r="C167">
+      <c r="C167" s="0" t="n">
         <v>310</v>
       </c>
-      <c r="D167" t="s">
+      <c r="D167" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="E167" t="s">
+      <c r="E167" s="0" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="168" spans="1:5">
-      <c r="A168" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="168">
+      <c r="A168" s="10" t="n">
         <v>43334</v>
       </c>
-      <c r="C168">
+      <c r="C168" s="0" t="n">
         <v>464</v>
       </c>
-      <c r="D168" t="s">
+      <c r="D168" s="0" t="s">
         <v>218</v>
       </c>
       <c r="E168" s="11" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="169" spans="1:5">
-      <c r="A169" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="169">
+      <c r="A169" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="C169">
+      <c r="C169" s="0" t="n">
         <v>726</v>
       </c>
-      <c r="D169" t="s">
+      <c r="D169" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="E169" t="s">
+      <c r="E169" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="170" spans="1:5">
-      <c r="A170" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="170">
+      <c r="A170" s="10" t="n">
         <v>43337</v>
       </c>
-      <c r="C170">
+      <c r="C170" s="0" t="n">
         <v>544</v>
       </c>
-      <c r="D170" t="s">
+      <c r="D170" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E170" t="s">
+      <c r="E170" s="0" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="171" spans="1:5">
-      <c r="A171" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="171">
+      <c r="A171" s="10" t="n">
         <v>43337</v>
       </c>
-      <c r="B171">
+      <c r="B171" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D171" t="s">
+      <c r="D171" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="E171" t="s">
+      <c r="E171" s="0" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="172" spans="1:5">
-      <c r="A172" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="172">
+      <c r="A172" s="10" t="n">
         <v>43341</v>
       </c>
-      <c r="C172">
+      <c r="C172" s="0" t="n">
         <v>830</v>
       </c>
-      <c r="D172" t="s">
+      <c r="D172" s="0" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="173" spans="1:5">
-      <c r="A173" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="173">
+      <c r="A173" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="C173">
+      <c r="C173" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="D173" t="s">
+      <c r="D173" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="E173" t="s">
+      <c r="E173" s="0" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="174" spans="1:5">
-      <c r="A174" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="174">
+      <c r="A174" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="B174">
+      <c r="B174" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D174" t="s">
+      <c r="D174" s="0" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="175" spans="1:5">
-      <c r="A175" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="175">
+      <c r="A175" s="10" t="n">
         <v>43344</v>
       </c>
-      <c r="B175">
+      <c r="B175" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="D175" t="s">
+      <c r="D175" s="0" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="176" spans="1:5">
-      <c r="A176" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="176">
+      <c r="A176" s="10" t="n">
         <v>43344</v>
       </c>
-      <c r="B176">
+      <c r="B176" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D176" t="s">
+      <c r="D176" s="0" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="177" spans="1:5">
-      <c r="A177" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="177">
+      <c r="A177" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C177">
+      <c r="C177" s="0" t="n">
         <v>607</v>
       </c>
-      <c r="D177" t="s">
+      <c r="D177" s="0" t="s">
         <v>235</v>
       </c>
-      <c r="E177" t="s">
+      <c r="E177" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="178" spans="1:5">
-      <c r="A178" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="178">
+      <c r="A178" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C178">
+      <c r="C178" s="0" t="n">
         <v>444</v>
       </c>
-      <c r="D178" t="s">
+      <c r="D178" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E178" t="s">
+      <c r="E178" s="0" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="179" spans="1:5">
-      <c r="A179" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="179">
+      <c r="A179" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C179">
+      <c r="C179" s="0" t="n">
         <v>312</v>
       </c>
-      <c r="D179" t="s">
+      <c r="D179" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="E179" t="s">
+      <c r="E179" s="0" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="180" spans="1:5">
-      <c r="A180" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="180">
+      <c r="A180" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C180">
+      <c r="C180" s="0" t="n">
         <v>501</v>
       </c>
-      <c r="D180" t="s">
+      <c r="D180" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E180" t="s">
+      <c r="E180" s="0" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="181" spans="1:5">
-      <c r="A181" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="181">
+      <c r="A181" s="10" t="n">
         <v>43349</v>
       </c>
-      <c r="C181">
+      <c r="C181" s="0" t="n">
         <v>711</v>
       </c>
-      <c r="D181" t="s">
+      <c r="D181" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="E181" t="s">
+      <c r="E181" s="0" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="182" spans="1:5">
-      <c r="A182" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="182">
+      <c r="A182" s="10" t="n">
         <v>43354</v>
       </c>
-      <c r="B182">
+      <c r="B182" s="0" t="n">
         <v>126</v>
       </c>
-      <c r="D182" t="s">
+      <c r="D182" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="E182" t="s">
+      <c r="E182" s="0" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="183" spans="1:5">
-      <c r="A183" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="183">
+      <c r="A183" s="10" t="n">
         <v>43354</v>
       </c>
-      <c r="C183">
+      <c r="C183" s="0" t="n">
         <v>450</v>
       </c>
-      <c r="D183" t="s">
+      <c r="D183" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="E183" t="s">
+      <c r="E183" s="0" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="184" spans="1:5">
-      <c r="A184" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="184">
+      <c r="A184" s="10" t="n">
         <v>43361</v>
       </c>
-      <c r="C184">
+      <c r="C184" s="0" t="n">
         <v>660</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D184" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="E184" t="s">
+      <c r="E184" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="185" spans="1:5">
-      <c r="A185" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="185">
+      <c r="A185" s="10" t="n">
         <v>43363</v>
       </c>
-      <c r="C185">
+      <c r="C185" s="0" t="n">
         <v>230</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D185" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="E185" t="s">
+      <c r="E185" s="0" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="186" spans="1:5">
-      <c r="A186" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="186">
+      <c r="A186" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B186">
+      <c r="B186" s="0" t="n">
         <v>4859</v>
       </c>
-      <c r="D186" t="s">
+      <c r="D186" s="0" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="187" spans="1:5">
-      <c r="A187" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="187">
+      <c r="A187" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B187">
+      <c r="B187" s="0" t="n">
         <v>295</v>
       </c>
-      <c r="D187" t="s">
+      <c r="D187" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="E187" t="s">
+      <c r="E187" s="0" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="188" spans="1:5">
-      <c r="A188" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="188">
+      <c r="A188" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B188">
+      <c r="B188" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D188" t="s">
+      <c r="D188" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="E188" t="s">
+      <c r="E188" s="0" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="189" spans="1:5">
-      <c r="A189" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="189">
+      <c r="A189" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B189">
+      <c r="B189" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="D189" t="s">
+      <c r="D189" s="0" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="190" spans="1:5">
-      <c r="A190" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="190">
+      <c r="A190" s="10" t="n">
         <v>43378</v>
       </c>
-      <c r="B190">
+      <c r="B190" s="0" t="n">
         <v>506</v>
       </c>
-      <c r="D190" t="s">
+      <c r="D190" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="E190" t="s">
+      <c r="E190" s="0" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="191" spans="1:5">
-      <c r="A191" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="191">
+      <c r="A191" s="10" t="n">
         <v>43379</v>
       </c>
-      <c r="B191">
+      <c r="B191" s="0" t="n">
         <v>350</v>
       </c>
-      <c r="D191" t="s">
+      <c r="D191" s="0" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="192" spans="1:5" ht="20" customHeight="1">
-      <c r="A192" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="20" outlineLevel="0" r="192">
+      <c r="A192" s="10" t="n">
         <v>43383</v>
       </c>
-      <c r="B192">
+      <c r="B192" s="0" t="n">
         <v>189</v>
       </c>
-      <c r="D192" t="s">
+      <c r="D192" s="0" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="193" spans="1:5">
-      <c r="A193" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="193">
+      <c r="A193" s="10" t="n">
         <v>43387</v>
       </c>
-      <c r="B193">
+      <c r="B193" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="D193" t="s">
+      <c r="D193" s="0" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="194" spans="1:5">
-      <c r="A194" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="194">
+      <c r="A194" s="10" t="n">
         <v>43387</v>
       </c>
-      <c r="B194">
+      <c r="B194" s="0" t="n">
         <v>307</v>
       </c>
-      <c r="D194" t="s">
+      <c r="D194" s="0" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="195" spans="1:5">
-      <c r="C195">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="195">
+      <c r="C195" s="0" t="n">
         <v>3705</v>
       </c>
-      <c r="E195" t="s">
+      <c r="E195" s="0" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="196" spans="1:5">
-      <c r="A196" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="196">
+      <c r="A196" s="10" t="n">
         <v>43385</v>
       </c>
-      <c r="C196">
+      <c r="C196" s="0" t="n">
         <v>608</v>
       </c>
-      <c r="D196" t="s">
+      <c r="D196" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E196" t="s">
+      <c r="E196" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="197" spans="1:5">
-      <c r="A197" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="197">
+      <c r="A197" s="10" t="n">
         <v>43391</v>
       </c>
-      <c r="B197">
+      <c r="B197" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="D197" t="s">
+      <c r="D197" s="0" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="198" spans="1:5">
-      <c r="A198" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="198">
+      <c r="A198" s="10" t="n">
         <v>43392</v>
       </c>
-      <c r="B198">
+      <c r="B198" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="D198" t="s">
+      <c r="D198" s="0" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="199" spans="1:5">
-      <c r="A199" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="199">
+      <c r="A199" s="10" t="n">
         <v>43393</v>
       </c>
-      <c r="B199">
+      <c r="B199" s="0" t="n">
         <v>177</v>
       </c>
-      <c r="D199" t="s">
+      <c r="D199" s="0" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="200" spans="1:5">
-      <c r="A200" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="200">
+      <c r="A200" s="10" t="n">
         <v>43393</v>
       </c>
-      <c r="C200">
+      <c r="C200" s="0" t="n">
         <v>125</v>
       </c>
-      <c r="D200" t="s">
+      <c r="D200" s="0" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="201" spans="1:5">
-      <c r="A201" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="201">
+      <c r="A201" s="10" t="n">
         <v>43395</v>
       </c>
-      <c r="B201">
+      <c r="B201" s="0" t="n">
         <v>2800</v>
       </c>
       <c r="D201" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="E201" t="s">
+      <c r="E201" s="0" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="202" spans="1:5">
-      <c r="A202" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="202">
+      <c r="A202" s="10" t="n">
         <v>43395</v>
       </c>
-      <c r="C202">
+      <c r="C202" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="D202" t="s">
+      <c r="D202" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="E202" t="s">
+      <c r="E202" s="0" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="203" spans="1:5">
-      <c r="A203" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="203">
+      <c r="A203" s="10" t="n">
         <v>43396</v>
       </c>
-      <c r="C203">
+      <c r="C203" s="0" t="n">
         <v>692</v>
       </c>
-      <c r="D203" t="s">
+      <c r="D203" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E203" t="s">
+      <c r="E203" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="204" spans="1:5">
-      <c r="A204" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="204">
+      <c r="A204" s="10" t="n">
         <v>43397</v>
       </c>
-      <c r="C204">
+      <c r="C204" s="0" t="n">
         <v>4935</v>
       </c>
-      <c r="D204" t="s">
+      <c r="D204" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="E204" t="s">
+      <c r="E204" s="0" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="205" spans="1:5" ht="10" customHeight="1">
-      <c r="A205" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10" outlineLevel="0" r="205">
+      <c r="A205" s="10" t="n">
         <v>43398</v>
       </c>
-      <c r="B205">
+      <c r="B205" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="D205" t="s">
+      <c r="D205" s="0" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="206" spans="1:5">
-      <c r="A206" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="206">
+      <c r="A206" s="10" t="n">
         <v>43398</v>
       </c>
-      <c r="B206">
+      <c r="B206" s="0" t="n">
         <v>370</v>
       </c>
-      <c r="D206" t="s">
+      <c r="D206" s="0" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="207" spans="1:5">
-      <c r="A207" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="207">
+      <c r="A207" s="10" t="n">
         <v>43398</v>
       </c>
-      <c r="B207">
+      <c r="B207" s="0" t="n">
         <v>4966</v>
       </c>
-      <c r="D207" t="s">
+      <c r="D207" s="0" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="208" spans="1:5">
-      <c r="A208" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="208">
+      <c r="A208" s="10" t="n">
         <v>43397</v>
       </c>
-      <c r="C208">
+      <c r="C208" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="D208" t="s">
+      <c r="D208" s="0" t="s">
         <v>265</v>
       </c>
-      <c r="E208" t="s">
+      <c r="E208" s="0" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="209" spans="1:5">
-      <c r="A209" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="209">
+      <c r="A209" s="10" t="n">
         <v>43399</v>
       </c>
-      <c r="B209">
+      <c r="B209" s="0" t="n">
         <v>182</v>
       </c>
-      <c r="D209" t="s">
+      <c r="D209" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="E209" t="s">
+      <c r="E209" s="0" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="210" spans="1:5">
-      <c r="A210" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="210">
+      <c r="A210" s="10" t="n">
         <v>43401</v>
       </c>
-      <c r="B210">
+      <c r="B210" s="0" t="n">
         <v>700</v>
       </c>
-      <c r="D210" t="s">
+      <c r="D210" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="E210" t="s">
+      <c r="E210" s="0" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="211" spans="1:5">
-      <c r="A211" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="211">
+      <c r="A211" s="10" t="n">
         <v>43405</v>
       </c>
-      <c r="B211">
+      <c r="B211" s="0" t="n">
         <v>274</v>
       </c>
-      <c r="D211" t="s">
+      <c r="D211" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="E211" t="s">
+      <c r="E211" s="0" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="212" spans="1:5">
-      <c r="A212" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="212">
+      <c r="A212" s="10" t="n">
         <v>43405</v>
       </c>
-      <c r="C212">
+      <c r="C212" s="0" t="n">
         <v>590</v>
       </c>
-      <c r="D212" t="s">
+      <c r="D212" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="E212" t="s">
+      <c r="E212" s="0" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="213" spans="1:5" ht="14">
-      <c r="A213" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="213">
+      <c r="A213" s="10" t="n">
         <v>43407</v>
       </c>
-      <c r="C213">
+      <c r="C213" s="0" t="n">
         <v>1275</v>
       </c>
       <c r="D213" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="E213" t="s">
+      <c r="E213" s="0" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="214" spans="1:5" ht="14">
-      <c r="A214" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="214">
+      <c r="A214" s="10" t="n">
         <v>43407</v>
       </c>
-      <c r="C214">
+      <c r="C214" s="0" t="n">
         <v>4781</v>
       </c>
       <c r="D214" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="E214" t="s">
+      <c r="E214" s="0" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="215" spans="1:5" ht="14">
-      <c r="A215" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="215">
+      <c r="A215" s="10" t="n">
         <v>43407</v>
       </c>
-      <c r="C215">
+      <c r="C215" s="0" t="n">
         <v>4781</v>
       </c>
       <c r="D215" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="E215" t="s">
+      <c r="E215" s="0" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="216" spans="1:5">
-      <c r="A216" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="216">
+      <c r="A216" s="10" t="n">
         <v>43406</v>
       </c>
-      <c r="C216">
+      <c r="C216" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D216" t="s">
+      <c r="D216" s="0" t="s">
         <v>272</v>
       </c>
-      <c r="E216" t="s">
+      <c r="E216" s="0" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="217" spans="1:5">
-      <c r="A217" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="217">
+      <c r="A217" s="10" t="n">
         <v>43409</v>
       </c>
-      <c r="C217">
+      <c r="C217" s="0" t="n">
         <v>677</v>
       </c>
-      <c r="D217" t="s">
+      <c r="D217" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E217" t="s">
+      <c r="E217" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="218" spans="1:5" ht="14">
-      <c r="A218" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="218">
+      <c r="A218" s="10" t="n">
         <v>43410</v>
       </c>
-      <c r="B218">
+      <c r="B218" s="0" t="n">
         <v>285</v>
       </c>
       <c r="D218" s="13" t="s">
         <v>274</v>
       </c>
-      <c r="E218" t="s">
+      <c r="E218" s="0" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="219" spans="1:5" ht="14">
-      <c r="A219" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="219">
+      <c r="A219" s="10" t="n">
         <v>43410</v>
       </c>
-      <c r="B219">
+      <c r="B219" s="0" t="n">
         <v>125</v>
       </c>
       <c r="D219" s="13" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="220" spans="1:5" ht="14">
-      <c r="A220" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="220">
+      <c r="A220" s="10" t="n">
         <v>43409</v>
       </c>
-      <c r="B220">
+      <c r="B220" s="0" t="n">
         <v>85</v>
       </c>
       <c r="D220" s="13" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="221" spans="1:5" ht="14">
-      <c r="A221" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="221">
+      <c r="A221" s="10" t="n">
         <v>43410</v>
       </c>
-      <c r="B221">
+      <c r="B221" s="0" t="n">
         <v>44</v>
       </c>
       <c r="D221" s="13" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="222" spans="1:5">
-      <c r="A222" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="222">
+      <c r="A222" s="10" t="n">
         <v>43412</v>
       </c>
-      <c r="C222">
+      <c r="C222" s="0" t="n">
         <v>190</v>
       </c>
-      <c r="D222" t="s">
+      <c r="D222" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="E222" t="s">
+      <c r="E222" s="0" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="223" spans="1:5" ht="14">
-      <c r="A223" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="223">
+      <c r="A223" s="10" t="n">
         <v>43415</v>
       </c>
-      <c r="B223">
+      <c r="B223" s="0" t="n">
         <v>189</v>
       </c>
       <c r="D223" s="13" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="224" spans="1:5" ht="14">
-      <c r="A224" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="224">
+      <c r="A224" s="10" t="n">
         <v>43415</v>
       </c>
-      <c r="B224">
+      <c r="B224" s="0" t="n">
         <v>336</v>
       </c>
       <c r="D224" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="E224" t="s">
+      <c r="E224" s="0" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="225" spans="1:5" ht="14">
-      <c r="A225" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="225">
+      <c r="A225" s="10" t="n">
         <v>43419</v>
       </c>
-      <c r="B225">
+      <c r="B225" s="0" t="n">
         <v>158</v>
       </c>
       <c r="D225" s="13" t="s">
         <v>282</v>
       </c>
-      <c r="E225" t="s">
+      <c r="E225" s="0" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="226" spans="1:5">
-      <c r="A226" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="226">
+      <c r="A226" s="10" t="n">
         <v>43418</v>
       </c>
-      <c r="C226">
+      <c r="C226" s="0" t="n">
         <v>642</v>
       </c>
-      <c r="D226" t="s">
+      <c r="D226" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E226" t="s">
+      <c r="E226" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="227" spans="1:5">
-      <c r="A227" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="227">
+      <c r="A227" s="10" t="n">
         <v>43419</v>
       </c>
-      <c r="C227">
+      <c r="C227" s="0" t="n">
         <v>370</v>
       </c>
-      <c r="D227" t="s">
+      <c r="D227" s="0" t="s">
         <v>284</v>
       </c>
-      <c r="E227" t="s">
+      <c r="E227" s="0" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="228" spans="1:5">
-      <c r="A228" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="228">
+      <c r="A228" s="10" t="n">
         <v>43419</v>
       </c>
-      <c r="C228">
+      <c r="C228" s="0" t="n">
         <v>222</v>
       </c>
-      <c r="D228" t="s">
+      <c r="D228" s="0" t="s">
         <v>286</v>
       </c>
-      <c r="E228" t="s">
+      <c r="E228" s="0" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="229" spans="1:5">
-      <c r="A229" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="229">
+      <c r="A229" s="10" t="n">
         <v>43421</v>
       </c>
-      <c r="B229">
+      <c r="B229" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="D229" t="s">
+      <c r="D229" s="0" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="230" spans="1:5">
-      <c r="A230" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="230">
+      <c r="A230" s="10" t="n">
         <v>43422</v>
       </c>
-      <c r="B230">
+      <c r="B230" s="0" t="n">
         <v>158</v>
       </c>
-      <c r="D230" t="s">
+      <c r="D230" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="E230" t="s">
+      <c r="E230" s="0" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="231" spans="1:5">
-      <c r="A231" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="231">
+      <c r="A231" s="10" t="n">
         <v>43422</v>
       </c>
-      <c r="B231">
+      <c r="B231" s="0" t="n">
         <v>159</v>
       </c>
-      <c r="D231" t="s">
+      <c r="D231" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="E231" t="s">
+      <c r="E231" s="0" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="232" spans="1:5">
-      <c r="A232" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="232">
+      <c r="A232" s="10" t="n">
         <v>43421</v>
       </c>
-      <c r="C232">
+      <c r="C232" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="D232" t="s">
+      <c r="D232" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="E232" t="s">
+      <c r="E232" s="0" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="233" spans="1:5">
-      <c r="A233" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="233">
+      <c r="A233" s="10" t="n">
         <v>43422</v>
       </c>
-      <c r="B233">
+      <c r="B233" s="0" t="n">
         <v>11649</v>
       </c>
-      <c r="D233" t="s">
+      <c r="D233" s="0" t="s">
         <v>290</v>
       </c>
-      <c r="E233" t="s">
+      <c r="E233" s="0" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="234" spans="1:5">
-      <c r="A234" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="234">
+      <c r="A234" s="10" t="n">
         <v>43426</v>
       </c>
-      <c r="C234">
+      <c r="C234" s="0" t="n">
         <v>308</v>
       </c>
-      <c r="D234" t="s">
+      <c r="D234" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="E234" t="s">
+      <c r="E234" s="0" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="235" spans="1:5">
-      <c r="A235" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="235">
+      <c r="A235" s="10" t="n">
         <v>43428</v>
       </c>
-      <c r="B235">
+      <c r="B235" s="0" t="n">
         <v>112</v>
       </c>
-      <c r="D235" t="s">
+      <c r="D235" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="E235" t="s">
+      <c r="E235" s="0" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="236" spans="1:5">
-      <c r="A236" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="236">
+      <c r="A236" s="10" t="n">
         <v>43428</v>
       </c>
-      <c r="B236">
+      <c r="B236" s="0" t="n">
         <v>79</v>
       </c>
-      <c r="D236" t="s">
+      <c r="D236" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="E236" t="s">
+      <c r="E236" s="0" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="237" spans="1:5">
-      <c r="A237" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="237">
+      <c r="A237" s="10" t="n">
         <v>43425</v>
       </c>
-      <c r="C237">
+      <c r="C237" s="0" t="n">
         <v>93</v>
       </c>
-      <c r="D237" t="s">
+      <c r="D237" s="0" t="s">
         <v>272</v>
       </c>
-      <c r="E237" t="s">
+      <c r="E237" s="0" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="238" spans="1:5">
-      <c r="A238" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="238">
+      <c r="A238" s="10" t="n">
         <v>43426</v>
       </c>
-      <c r="C238">
+      <c r="C238" s="0" t="n">
         <v>308</v>
       </c>
-      <c r="D238" t="s">
+      <c r="D238" s="0" t="s">
         <v>295</v>
       </c>
-      <c r="E238" t="s">
+      <c r="E238" s="0" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="239" spans="1:5">
-      <c r="A239" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="239">
+      <c r="A239" s="10" t="n">
         <v>43430</v>
       </c>
-      <c r="C239">
+      <c r="C239" s="0" t="n">
         <v>616</v>
       </c>
-      <c r="D239" t="s">
+      <c r="D239" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E239" t="s">
+      <c r="E239" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="240" spans="1:5">
-      <c r="A240" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="240">
+      <c r="A240" s="10" t="n">
         <v>43430</v>
       </c>
-      <c r="C240">
+      <c r="C240" s="0" t="n">
         <v>243</v>
       </c>
-      <c r="D240" t="s">
+      <c r="D240" s="0" t="s">
         <v>297</v>
       </c>
-      <c r="E240" t="s">
+      <c r="E240" s="0" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="241" spans="1:5">
-      <c r="A241" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="241">
+      <c r="A241" s="10" t="n">
         <v>43432</v>
       </c>
-      <c r="C241">
+      <c r="C241" s="0" t="n">
         <v>850</v>
       </c>
-      <c r="D241" t="s">
+      <c r="D241" s="0" t="s">
         <v>299</v>
       </c>
-      <c r="E241" t="s">
+      <c r="E241" s="0" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="242" spans="1:5">
-      <c r="A242" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="242">
+      <c r="A242" s="10" t="n">
         <v>43433</v>
       </c>
-      <c r="B242">
+      <c r="B242" s="0" t="n">
         <v>75</v>
       </c>
-      <c r="D242" t="s">
+      <c r="D242" s="0" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="243" spans="1:5">
-      <c r="A243" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="243">
+      <c r="A243" s="10" t="n">
         <v>43433</v>
       </c>
-      <c r="C243">
+      <c r="C243" s="0" t="n">
         <v>212</v>
       </c>
-      <c r="D243" t="s">
+      <c r="D243" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E243" t="s">
+      <c r="E243" s="0" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="244" spans="1:5">
-      <c r="A244" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="244">
+      <c r="A244" s="10" t="n">
         <v>43433</v>
       </c>
-      <c r="C244">
+      <c r="C244" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="D244" t="s">
+      <c r="D244" s="0" t="s">
         <v>303</v>
       </c>
-      <c r="E244" t="s">
+      <c r="E244" s="0" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="245" spans="1:5">
-      <c r="A245" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="245">
+      <c r="A245" s="10" t="n">
         <v>43436</v>
       </c>
-      <c r="B245">
+      <c r="B245" s="0" t="n">
         <v>142</v>
       </c>
-      <c r="D245" t="s">
+      <c r="D245" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="E245" t="s">
+      <c r="E245" s="0" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="260" spans="2:3">
-      <c r="B260">
-        <f>SUM(B2:B259)</f>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="246">
+      <c r="A246" s="10" t="n">
+        <v>43436</v>
+      </c>
+      <c r="C246" s="0" t="n">
+        <v>318</v>
+      </c>
+      <c r="D246" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="E246" s="0" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="260">
+      <c r="B260" s="0" t="n">
+        <f aca="false">SUM(B2:B259)</f>
         <v>69808</v>
       </c>
-      <c r="C260">
-        <f>SUM(C2:C259)</f>
-        <v>68989</v>
+      <c r="C260" s="0" t="n">
+        <f aca="false">SUM(C2:C259)</f>
+        <v>69307</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A30:Z32">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule aboveAverage="0" bottom="0" dxfId="0" operator="expression" percent="0" priority="2" rank="0" text="" type="expression">
       <formula>LEN(TRIM(A30))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D33" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D40" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D201" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink display="netonnet.se" ref="D33" r:id="rId1"/>
+    <hyperlink display="www.vidaxl.se" ref="D40" r:id="rId2"/>
+    <hyperlink display="https://www.vardia.se/" ref="D201" r:id="rId3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cost update Jenny 1210
</commit_message>
<xml_diff>
--- a/Cost.xlsx
+++ b/Cost.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chengkaiyan/github/cost/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076B18F6-148D-2D4A-B28E-022CEC998959}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="18300" windowHeight="11260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="317">
   <si>
     <t>日期</t>
   </si>
@@ -962,61 +957,86 @@
   </si>
   <si>
     <t>upplands november 电费</t>
+  </si>
+  <si>
+    <t>banan,honung, tomat plommon</t>
+  </si>
+  <si>
+    <t>green vegetables:qingcai, xiangcai</t>
+  </si>
+  <si>
+    <t>milk,ägg,lax sauce,etc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="yyyy/m/d"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt formatCode="YYYY/M/D" numFmtId="165"/>
+    <numFmt formatCode="M/D/YYYY" numFmtId="166"/>
+    <numFmt formatCode="YYYY\-MM\-DD" numFmtId="167"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="10">
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <family val="0"/>
       <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
       <name val="Arial"/>
       <family val="2"/>
+      <sz val="10"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF666666"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF666666"/>
+      <sz val="11"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0563C1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF0563C1"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0563C1"/>
       <name val="FreeSans"/>
       <family val="2"/>
+      <color rgb="FF0563C1"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF444444"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF444444"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1046,7 +1066,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
@@ -1054,31 +1074,100 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+  <cellStyleXfs count="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="4" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="167" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="20">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="7">
+    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle builtinId="8" customBuiltin="false" name="*unknown*" xfId="20"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1089,7 +1178,6 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1148,339 +1236,31 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF444444"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:Z260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A237" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D252" sqref="D252"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A249" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D261" activeCellId="0" pane="topLeft" sqref="D261"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="3" width="14.5"/>
-    <col min="4" max="4" width="26"/>
-    <col min="5" max="5" width="37.83203125"/>
-    <col min="6" max="1025" width="14.5"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="14.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1497,11 +1277,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1">
-      <c r="A2" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="2">
+      <c r="A2" s="2" t="n">
         <v>43121</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="1" t="n">
         <v>250</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1511,11 +1291,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1">
-      <c r="A3" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="3">
+      <c r="A3" s="2" t="n">
         <v>43122</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="1" t="n">
         <v>305</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1525,11 +1305,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1">
-      <c r="A4" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="4">
+      <c r="A4" s="2" t="n">
         <v>43122</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1539,11 +1319,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1">
-      <c r="A5" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="5">
+      <c r="A5" s="2" t="n">
         <v>43125</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="1" t="n">
         <v>98</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1553,11 +1333,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1">
-      <c r="A6" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="6">
+      <c r="A6" s="2" t="n">
         <v>43126</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1567,11 +1347,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1">
-      <c r="A7" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="7">
+      <c r="A7" s="2" t="n">
         <v>43127</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1581,11 +1361,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1">
-      <c r="A8" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="8">
+      <c r="A8" s="2" t="n">
         <v>43128</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="1" t="n">
         <v>656</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1595,11 +1375,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1">
-      <c r="A9" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="9">
+      <c r="A9" s="2" t="n">
         <v>43131</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="1" t="n">
         <v>486</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1609,11 +1389,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1">
-      <c r="A10" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="10">
+      <c r="A10" s="2" t="n">
         <v>43132</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="1" t="n">
         <v>76</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1623,11 +1403,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1">
-      <c r="A11" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="11">
+      <c r="A11" s="2" t="n">
         <v>43133</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="1" t="n">
         <v>399</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1637,11 +1417,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1">
-      <c r="A12" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="12">
+      <c r="A12" s="2" t="n">
         <v>43135</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="1" t="n">
         <v>419</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1651,11 +1431,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1">
-      <c r="A13" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="13">
+      <c r="A13" s="2" t="n">
         <v>43136</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="1" t="n">
         <v>521</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1665,11 +1445,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1">
-      <c r="A14" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="14">
+      <c r="A14" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="1" t="n">
         <v>399</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1679,11 +1459,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1">
-      <c r="A15" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="15">
+      <c r="A15" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="1" t="n">
         <v>138</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1693,11 +1473,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1">
-      <c r="A16" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="16">
+      <c r="A16" s="2" t="n">
         <v>43137</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="1" t="n">
         <v>310</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1707,12 +1487,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1">
-      <c r="A17" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="17">
+      <c r="A17" s="2" t="n">
         <v>43138</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="1">
+      <c r="C17" s="1" t="n">
         <v>700</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1722,12 +1502,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1">
-      <c r="A18" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="18">
+      <c r="A18" s="2" t="n">
         <v>43141</v>
       </c>
-      <c r="C18" s="1">
-        <f>F18*G18</f>
+      <c r="C18" s="1" t="n">
+        <f aca="false">F18*G18</f>
         <v>1312</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -1736,18 +1516,18 @@
       <c r="E18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="1" t="n">
         <v>164</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="1" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1">
-      <c r="A19" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="19">
+      <c r="A19" s="2" t="n">
         <v>43141</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="1" t="n">
         <v>1190</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1757,11 +1537,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1">
-      <c r="A20" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="20">
+      <c r="A20" s="2" t="n">
         <v>43154</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="1" t="n">
         <v>438</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1771,11 +1551,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1">
-      <c r="A21" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="21">
+      <c r="A21" s="2" t="n">
         <v>43154</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="1" t="n">
         <v>248</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -1785,22 +1565,22 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1">
-      <c r="A22" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="22">
+      <c r="A22" s="2" t="n">
         <v>43166</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="1" t="n">
         <v>234</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1">
-      <c r="A23" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="23">
+      <c r="A23" s="2" t="n">
         <v>43171</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="1" t="n">
         <v>118</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1810,22 +1590,22 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1">
-      <c r="A24" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="24">
+      <c r="A24" s="2" t="n">
         <v>43173</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="1" t="n">
         <v>82</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1">
-      <c r="A25" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="25">
+      <c r="A25" s="2" t="n">
         <v>43174</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1835,22 +1615,22 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1">
-      <c r="A26" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="26">
+      <c r="A26" s="2" t="n">
         <v>43175</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="1" t="n">
         <v>370</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:7" hidden="1">
-      <c r="A27" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="27">
+      <c r="A27" s="2" t="n">
         <v>43175</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -1860,11 +1640,11 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1">
-      <c r="A28" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="28">
+      <c r="A28" s="2" t="n">
         <v>43176</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="1" t="n">
         <v>624</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -1874,11 +1654,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1">
-      <c r="A29" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="29">
+      <c r="A29" s="2" t="n">
         <v>43177</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="1" t="n">
         <v>170</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1888,22 +1668,22 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1">
-      <c r="A30" s="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="30">
+      <c r="A30" s="4" t="n">
         <v>43179</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1">
-      <c r="A31" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="31">
+      <c r="A31" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="1" t="n">
         <v>90</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -1913,11 +1693,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1">
-      <c r="A32" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="32">
+      <c r="A32" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="1" t="n">
         <v>72</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -1927,11 +1707,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:26" hidden="1">
-      <c r="A33" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="33">
+      <c r="A33" s="2" t="n">
         <v>43179</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="1" t="n">
         <v>908</v>
       </c>
       <c r="D33" s="6" t="s">
@@ -1941,11 +1721,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:26" hidden="1">
-      <c r="A34" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="34">
+      <c r="A34" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -1955,11 +1735,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:26" hidden="1">
-      <c r="A35" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="35">
+      <c r="A35" s="2" t="n">
         <v>43181</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -1969,11 +1749,11 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:26" hidden="1">
-      <c r="A36" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="36">
+      <c r="A36" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="1" t="n">
         <v>135</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -1983,11 +1763,11 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:26" hidden="1">
-      <c r="A37" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="37">
+      <c r="A37" s="2" t="n">
         <v>43184</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="1" t="n">
         <v>110</v>
       </c>
       <c r="C37" s="1"/>
@@ -2019,11 +1799,11 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38" spans="1:26" hidden="1">
-      <c r="A38" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="38">
+      <c r="A38" s="2" t="n">
         <v>43185</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="1" t="n">
         <v>122</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -2033,22 +1813,22 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:26" hidden="1">
-      <c r="A39" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="39">
+      <c r="A39" s="2" t="n">
         <v>43187</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="1" t="n">
         <v>750</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:26" hidden="1">
-      <c r="A40" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="40">
+      <c r="A40" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="1" t="n">
         <v>379</v>
       </c>
       <c r="D40" s="6" t="s">
@@ -2058,22 +1838,22 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:26" hidden="1">
-      <c r="A41" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="41">
+      <c r="A41" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="1" t="n">
         <v>240</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:26" hidden="1">
-      <c r="A42" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="42">
+      <c r="A42" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="1" t="n">
         <v>540</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -2083,11 +1863,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:26" hidden="1">
-      <c r="A43" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="43">
+      <c r="A43" s="2" t="n">
         <v>43188</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -2097,11 +1877,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:26" hidden="1">
-      <c r="A44" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="44">
+      <c r="A44" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -2111,11 +1891,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:26" hidden="1">
-      <c r="A45" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="45">
+      <c r="A45" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="1" t="n">
         <v>462</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -2125,11 +1905,11 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:26" hidden="1">
-      <c r="A46" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="46">
+      <c r="A46" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46" s="1" t="n">
         <v>70</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -2139,11 +1919,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:26" hidden="1">
-      <c r="A47" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="47">
+      <c r="A47" s="2" t="n">
         <v>43189</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -2153,11 +1933,11 @@
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="1:26" hidden="1">
-      <c r="A48" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="48">
+      <c r="A48" s="2" t="n">
         <v>43190</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="1" t="n">
         <v>30</v>
       </c>
       <c r="C48" s="1"/>
@@ -2168,11 +1948,11 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1">
-      <c r="A49" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="49">
+      <c r="A49" s="2" t="n">
         <v>43191</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="1" t="n">
         <v>40</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -2182,11 +1962,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1">
-      <c r="A50" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="50">
+      <c r="A50" s="7" t="n">
         <v>43193</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50" s="1" t="n">
         <v>150</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -2196,11 +1976,11 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1">
-      <c r="A51" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="51">
+      <c r="A51" s="2" t="n">
         <v>43194</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51" s="1" t="n">
         <v>1360</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -2210,11 +1990,11 @@
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1">
-      <c r="A52" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="52">
+      <c r="A52" s="2" t="n">
         <v>43195</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" s="1" t="n">
         <v>94</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -2224,11 +2004,11 @@
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1">
-      <c r="A53" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="53">
+      <c r="A53" s="2" t="n">
         <v>43196</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C53" s="1" t="n">
         <v>48</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -2238,11 +2018,11 @@
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1">
-      <c r="A54" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="54">
+      <c r="A54" s="2" t="n">
         <v>43196</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C54" s="1" t="n">
         <v>205</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -2252,11 +2032,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1">
-      <c r="A55" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="55">
+      <c r="A55" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -2266,11 +2046,11 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1">
-      <c r="A56" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="56">
+      <c r="A56" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56" s="1" t="n">
         <v>421</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -2280,11 +2060,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1">
-      <c r="A57" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="57">
+      <c r="A57" s="2" t="n">
         <v>43197</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="1" t="n">
         <v>191</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -2294,11 +2074,11 @@
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1">
-      <c r="A58" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="58">
+      <c r="A58" s="2" t="n">
         <v>43198</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58" s="1" t="n">
         <v>226</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -2308,22 +2088,22 @@
         <v>96</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1">
-      <c r="A59" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="59">
+      <c r="A59" s="2" t="n">
         <v>43200</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59" s="1" t="n">
         <v>250</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1">
-      <c r="A60" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="60">
+      <c r="A60" s="2" t="n">
         <v>43200</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60" s="1" t="n">
         <v>1115</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -2333,11 +2113,11 @@
         <v>99</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1">
-      <c r="A61" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="61">
+      <c r="A61" s="2" t="n">
         <v>43201</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -2347,11 +2127,11 @@
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1">
-      <c r="A62" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="62">
+      <c r="A62" s="2" t="n">
         <v>43201</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62" s="1" t="n">
         <v>88</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -2361,11 +2141,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1">
-      <c r="A63" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="63">
+      <c r="A63" s="2" t="n">
         <v>43203</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -2375,11 +2155,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1">
-      <c r="A64" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="64">
+      <c r="A64" s="2" t="n">
         <v>43203</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C64" s="1" t="n">
         <v>364</v>
       </c>
       <c r="D64" s="1" t="s">
@@ -2389,11 +2169,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1">
-      <c r="A65" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="65">
+      <c r="A65" s="2" t="n">
         <v>43204</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65" s="1" t="n">
         <v>65</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -2403,11 +2183,11 @@
         <v>105</v>
       </c>
     </row>
-    <row r="66" spans="1:5" hidden="1">
-      <c r="A66" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="66">
+      <c r="A66" s="2" t="n">
         <v>43208</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -2417,11 +2197,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1">
-      <c r="A67" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="67">
+      <c r="A67" s="2" t="n">
         <v>43208</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C67" s="1" t="n">
         <v>470</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -2431,11 +2211,11 @@
         <v>107</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1">
-      <c r="A68" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="68">
+      <c r="A68" s="2" t="n">
         <v>43209</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68" s="1" t="n">
         <v>180</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -2445,11 +2225,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1">
-      <c r="A69" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="69">
+      <c r="A69" s="2" t="n">
         <v>43210</v>
       </c>
-      <c r="C69" s="1">
+      <c r="C69" s="1" t="n">
         <v>420</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -2459,11 +2239,11 @@
         <v>109</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1">
-      <c r="A70" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="70">
+      <c r="A70" s="2" t="n">
         <v>43212</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70" s="1" t="n">
         <v>50</v>
       </c>
       <c r="D70" s="1" t="s">
@@ -2473,11 +2253,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1">
-      <c r="A71" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="71">
+      <c r="A71" s="2" t="n">
         <v>43212</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71" s="1" t="n">
         <v>164</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -2487,11 +2267,11 @@
         <v>112</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1">
-      <c r="A72" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="72">
+      <c r="A72" s="2" t="n">
         <v>43215</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B72" s="1" t="n">
         <v>300</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -2501,11 +2281,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1">
-      <c r="A73" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="73">
+      <c r="A73" s="2" t="n">
         <v>43217</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73" s="1" t="n">
         <v>364</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -2515,11 +2295,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1">
-      <c r="A74" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="74">
+      <c r="A74" s="2" t="n">
         <v>43218</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74" s="1" t="n">
         <v>185</v>
       </c>
       <c r="D74" s="1" t="s">
@@ -2529,11 +2309,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1">
-      <c r="A75" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="75">
+      <c r="A75" s="2" t="n">
         <v>43218</v>
       </c>
-      <c r="C75" s="1">
+      <c r="C75" s="1" t="n">
         <v>404</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -2543,11 +2323,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="76" spans="1:5" hidden="1">
-      <c r="A76" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="76">
+      <c r="A76" s="2" t="n">
         <v>43220</v>
       </c>
-      <c r="C76" s="1">
+      <c r="C76" s="1" t="n">
         <v>57</v>
       </c>
       <c r="D76" s="1" t="s">
@@ -2557,11 +2337,11 @@
         <v>114</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1">
-      <c r="A77" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="77">
+      <c r="A77" s="2" t="n">
         <v>43221</v>
       </c>
-      <c r="C77" s="1">
+      <c r="C77" s="1" t="n">
         <v>282</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -2571,11 +2351,11 @@
         <v>116</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1">
-      <c r="A78" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="78">
+      <c r="A78" s="2" t="n">
         <v>43220</v>
       </c>
-      <c r="C78" s="1">
+      <c r="C78" s="1" t="n">
         <v>87</v>
       </c>
       <c r="D78" s="1" t="s">
@@ -2585,11 +2365,11 @@
         <v>117</v>
       </c>
     </row>
-    <row r="79" spans="1:5" hidden="1">
-      <c r="A79" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="79">
+      <c r="A79" s="2" t="n">
         <v>43223</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B79" s="1" t="n">
         <v>1878</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -2599,11 +2379,11 @@
         <v>119</v>
       </c>
     </row>
-    <row r="80" spans="1:5" hidden="1">
-      <c r="A80" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="80">
+      <c r="A80" s="2" t="n">
         <v>43224</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B80" s="1" t="n">
         <v>98</v>
       </c>
       <c r="D80" s="1" t="s">
@@ -2613,11 +2393,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="81" spans="1:5" hidden="1">
-      <c r="A81" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="81">
+      <c r="A81" s="2" t="n">
         <v>43225</v>
       </c>
-      <c r="C81" s="1">
+      <c r="C81" s="1" t="n">
         <v>198</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -2627,11 +2407,11 @@
         <v>122</v>
       </c>
     </row>
-    <row r="82" spans="1:5" hidden="1">
-      <c r="A82" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="82">
+      <c r="A82" s="2" t="n">
         <v>43225</v>
       </c>
-      <c r="C82" s="1">
+      <c r="C82" s="1" t="n">
         <v>406</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -2641,11 +2421,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="83" spans="1:5" hidden="1">
-      <c r="A83" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="83">
+      <c r="A83" s="2" t="n">
         <v>43228</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83" s="1" t="n">
         <v>168</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -2655,11 +2435,11 @@
         <v>124</v>
       </c>
     </row>
-    <row r="84" spans="1:5" hidden="1">
-      <c r="A84" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="84">
+      <c r="A84" s="2" t="n">
         <v>43229</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B84" s="1" t="n">
         <v>240</v>
       </c>
       <c r="D84" s="1" t="s">
@@ -2669,12 +2449,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:5" hidden="1">
-      <c r="A85" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="85">
+      <c r="A85" s="2" t="n">
         <v>43230</v>
       </c>
       <c r="B85" s="1"/>
-      <c r="C85" s="1">
+      <c r="C85" s="1" t="n">
         <v>420</v>
       </c>
       <c r="D85" s="1" t="s">
@@ -2684,11 +2464,11 @@
         <v>126</v>
       </c>
     </row>
-    <row r="86" spans="1:5" hidden="1">
-      <c r="A86" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="86">
+      <c r="A86" s="2" t="n">
         <v>43230</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B86" s="1" t="n">
         <v>200</v>
       </c>
       <c r="C86" s="1"/>
@@ -2699,11 +2479,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="87" spans="1:5" hidden="1">
-      <c r="A87" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="87">
+      <c r="A87" s="2" t="n">
         <v>43230</v>
       </c>
-      <c r="C87" s="1">
+      <c r="C87" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D87" s="1" t="s">
@@ -2713,11 +2493,11 @@
         <v>128</v>
       </c>
     </row>
-    <row r="88" spans="1:5" hidden="1">
-      <c r="A88" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="88">
+      <c r="A88" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B88" s="1" t="n">
         <v>462</v>
       </c>
       <c r="D88" s="1" t="s">
@@ -2727,11 +2507,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="89" spans="1:5" hidden="1">
-      <c r="A89" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="89">
+      <c r="A89" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B89" s="1" t="n">
         <v>499</v>
       </c>
       <c r="D89" s="1" t="s">
@@ -2741,11 +2521,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="90" spans="1:5" hidden="1">
-      <c r="A90" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="90">
+      <c r="A90" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B90" s="1">
+      <c r="B90" s="1" t="n">
         <v>398</v>
       </c>
       <c r="D90" s="1" t="s">
@@ -2755,11 +2535,11 @@
         <v>133</v>
       </c>
     </row>
-    <row r="91" spans="1:5" hidden="1">
-      <c r="A91" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="91">
+      <c r="A91" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B91" s="1">
+      <c r="B91" s="1" t="n">
         <v>226</v>
       </c>
       <c r="D91" s="1" t="s">
@@ -2769,11 +2549,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="92" spans="1:5" hidden="1">
-      <c r="A92" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="92">
+      <c r="A92" s="2" t="n">
         <v>43231</v>
       </c>
-      <c r="B92" s="1">
+      <c r="B92" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D92" s="1" t="s">
@@ -2783,11 +2563,11 @@
         <v>137</v>
       </c>
     </row>
-    <row r="93" spans="1:5" hidden="1">
-      <c r="A93" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="93">
+      <c r="A93" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="B93" s="1">
+      <c r="B93" s="1" t="n">
         <v>80</v>
       </c>
       <c r="D93" s="1" t="s">
@@ -2797,11 +2577,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="94" spans="1:5" hidden="1">
-      <c r="A94" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="94">
+      <c r="A94" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="C94" s="1">
+      <c r="C94" s="1" t="n">
         <v>340</v>
       </c>
       <c r="D94" s="1" t="s">
@@ -2811,11 +2591,11 @@
         <v>139</v>
       </c>
     </row>
-    <row r="95" spans="1:5" hidden="1">
-      <c r="A95" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="95">
+      <c r="A95" s="2" t="n">
         <v>43232</v>
       </c>
-      <c r="B95" s="1">
+      <c r="B95" s="1" t="n">
         <v>510</v>
       </c>
       <c r="D95" s="1" t="s">
@@ -2825,11 +2605,11 @@
         <v>141</v>
       </c>
     </row>
-    <row r="96" spans="1:5" hidden="1">
-      <c r="A96" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="96">
+      <c r="A96" s="2" t="n">
         <v>43233</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B96" s="1" t="n">
         <v>170</v>
       </c>
       <c r="D96" s="1" t="s">
@@ -2839,11 +2619,11 @@
         <v>143</v>
       </c>
     </row>
-    <row r="97" spans="1:5" hidden="1">
-      <c r="A97" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="97">
+      <c r="A97" s="2" t="n">
         <v>43233</v>
       </c>
-      <c r="C97" s="1">
+      <c r="C97" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D97" s="1" t="s">
@@ -2853,11 +2633,11 @@
         <v>144</v>
       </c>
     </row>
-    <row r="98" spans="1:5" hidden="1">
-      <c r="A98" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="98">
+      <c r="A98" s="2" t="n">
         <v>43234</v>
       </c>
-      <c r="C98" s="1">
+      <c r="C98" s="1" t="n">
         <v>299</v>
       </c>
       <c r="D98" s="1" t="s">
@@ -2867,11 +2647,11 @@
         <v>145</v>
       </c>
     </row>
-    <row r="99" spans="1:5" hidden="1">
-      <c r="A99" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="99">
+      <c r="A99" s="2" t="n">
         <v>43236</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99" s="1" t="n">
         <v>3659</v>
       </c>
       <c r="D99" s="1" t="s">
@@ -2881,11 +2661,11 @@
         <v>146</v>
       </c>
     </row>
-    <row r="100" spans="1:5" hidden="1">
-      <c r="A100" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="100">
+      <c r="A100" s="2" t="n">
         <v>43237</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B100" s="1" t="n">
         <v>79</v>
       </c>
       <c r="D100" s="1" t="s">
@@ -2895,11 +2675,11 @@
         <v>147</v>
       </c>
     </row>
-    <row r="101" spans="1:5" hidden="1">
-      <c r="A101" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="101">
+      <c r="A101" s="2" t="n">
         <v>43236</v>
       </c>
-      <c r="C101" s="1">
+      <c r="C101" s="1" t="n">
         <v>173</v>
       </c>
       <c r="D101" s="1" t="s">
@@ -2909,11 +2689,11 @@
         <v>148</v>
       </c>
     </row>
-    <row r="102" spans="1:5" hidden="1">
-      <c r="A102" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="102">
+      <c r="A102" s="2" t="n">
         <v>43240</v>
       </c>
-      <c r="B102" s="1">
+      <c r="B102" s="1" t="n">
         <v>130</v>
       </c>
       <c r="D102" s="1" t="s">
@@ -2923,22 +2703,22 @@
         <v>149</v>
       </c>
     </row>
-    <row r="103" spans="1:5" hidden="1">
-      <c r="A103" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="103">
+      <c r="A103" s="2" t="n">
         <v>43240</v>
       </c>
-      <c r="B103" s="1">
+      <c r="B103" s="1" t="n">
         <v>190</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="104" spans="1:5" hidden="1">
-      <c r="A104" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="104">
+      <c r="A104" s="2" t="n">
         <v>43241</v>
       </c>
-      <c r="B104" s="1">
+      <c r="B104" s="1" t="n">
         <v>4070</v>
       </c>
       <c r="D104" s="1" t="s">
@@ -2948,11 +2728,11 @@
         <v>150</v>
       </c>
     </row>
-    <row r="105" spans="1:5" hidden="1">
-      <c r="A105" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="105">
+      <c r="A105" s="2" t="n">
         <v>43241</v>
       </c>
-      <c r="C105" s="1">
+      <c r="C105" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D105" s="1" t="s">
@@ -2962,11 +2742,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="106" spans="1:5" hidden="1">
-      <c r="A106" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="106">
+      <c r="A106" s="2" t="n">
         <v>43242</v>
       </c>
-      <c r="B106" s="1">
+      <c r="B106" s="1" t="n">
         <v>79</v>
       </c>
       <c r="D106" s="1" t="s">
@@ -2976,11 +2756,11 @@
         <v>152</v>
       </c>
     </row>
-    <row r="107" spans="1:5" hidden="1">
-      <c r="A107" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="107">
+      <c r="A107" s="2" t="n">
         <v>43246</v>
       </c>
-      <c r="B107" s="1">
+      <c r="B107" s="1" t="n">
         <v>220</v>
       </c>
       <c r="D107" s="1" t="s">
@@ -2990,11 +2770,11 @@
         <v>154</v>
       </c>
     </row>
-    <row r="108" spans="1:5" hidden="1">
-      <c r="A108" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="108">
+      <c r="A108" s="2" t="n">
         <v>43247</v>
       </c>
-      <c r="B108" s="1">
+      <c r="B108" s="1" t="n">
         <v>70</v>
       </c>
       <c r="D108" s="1" t="s">
@@ -3004,44 +2784,44 @@
         <v>156</v>
       </c>
     </row>
-    <row r="109" spans="1:5" hidden="1">
-      <c r="A109" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="109">
+      <c r="A109" s="2" t="n">
         <v>43253</v>
       </c>
-      <c r="B109" s="1">
+      <c r="B109" s="1" t="n">
         <v>142</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="110" spans="1:5" hidden="1">
-      <c r="A110" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="110">
+      <c r="A110" s="2" t="n">
         <v>43254</v>
       </c>
-      <c r="B110" s="1">
+      <c r="B110" s="1" t="n">
         <v>90</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="111" spans="1:5" hidden="1">
-      <c r="A111" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="111">
+      <c r="A111" s="2" t="n">
         <v>43260</v>
       </c>
-      <c r="C111" s="1">
+      <c r="C111" s="1" t="n">
         <v>1400</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="112" spans="1:5" hidden="1">
-      <c r="A112" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="112">
+      <c r="A112" s="2" t="n">
         <v>43260</v>
       </c>
-      <c r="C112" s="1">
+      <c r="C112" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D112" s="1" t="s">
@@ -3051,33 +2831,33 @@
         <v>91</v>
       </c>
     </row>
-    <row r="113" spans="1:5" hidden="1">
-      <c r="A113" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="113">
+      <c r="A113" s="2" t="n">
         <v>43264</v>
       </c>
-      <c r="B113" s="1">
+      <c r="B113" s="1" t="n">
         <v>546</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="114" spans="1:5" hidden="1">
-      <c r="A114" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="114">
+      <c r="A114" s="2" t="n">
         <v>43264</v>
       </c>
-      <c r="B114" s="1">
+      <c r="B114" s="1" t="n">
         <v>95</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="115" spans="1:5" hidden="1">
-      <c r="A115" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="115">
+      <c r="A115" s="2" t="n">
         <v>43266</v>
       </c>
-      <c r="B115" s="1">
+      <c r="B115" s="1" t="n">
         <v>394</v>
       </c>
       <c r="D115" s="1" t="s">
@@ -3087,11 +2867,11 @@
         <v>163</v>
       </c>
     </row>
-    <row r="116" spans="1:5" hidden="1">
-      <c r="A116" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="116">
+      <c r="A116" s="2" t="n">
         <v>43266</v>
       </c>
-      <c r="B116" s="1">
+      <c r="B116" s="1" t="n">
         <v>1055</v>
       </c>
       <c r="D116" s="1" t="s">
@@ -3101,11 +2881,11 @@
         <v>165</v>
       </c>
     </row>
-    <row r="117" spans="1:5" hidden="1">
-      <c r="A117" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="117">
+      <c r="A117" s="2" t="n">
         <v>43284</v>
       </c>
-      <c r="C117" s="1">
+      <c r="C117" s="1" t="n">
         <v>274</v>
       </c>
       <c r="D117" s="1" t="s">
@@ -3115,11 +2895,11 @@
         <v>167</v>
       </c>
     </row>
-    <row r="118" spans="1:5" hidden="1">
-      <c r="A118" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="118">
+      <c r="A118" s="2" t="n">
         <v>43283</v>
       </c>
-      <c r="C118" s="1">
+      <c r="C118" s="1" t="n">
         <v>105</v>
       </c>
       <c r="D118" s="1" t="s">
@@ -3129,11 +2909,11 @@
         <v>169</v>
       </c>
     </row>
-    <row r="119" spans="1:5" hidden="1">
-      <c r="A119" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="119">
+      <c r="A119" s="2" t="n">
         <v>43289</v>
       </c>
-      <c r="C119" s="1">
+      <c r="C119" s="1" t="n">
         <v>128</v>
       </c>
       <c r="D119" s="1" t="s">
@@ -3143,11 +2923,11 @@
         <v>171</v>
       </c>
     </row>
-    <row r="120" spans="1:5" hidden="1">
-      <c r="A120" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="120">
+      <c r="A120" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C120" s="1">
+      <c r="C120" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D120" s="1" t="s">
@@ -3157,11 +2937,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="121" spans="1:5" hidden="1">
-      <c r="A121" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="121">
+      <c r="A121" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C121" s="1">
+      <c r="C121" s="1" t="n">
         <v>210</v>
       </c>
       <c r="D121" s="1" t="s">
@@ -3171,44 +2951,44 @@
         <v>173</v>
       </c>
     </row>
-    <row r="122" spans="1:5" hidden="1">
-      <c r="A122" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="122">
+      <c r="A122" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B122" s="1">
+      <c r="B122" s="1" t="n">
         <v>980</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="123" spans="1:5" hidden="1">
-      <c r="A123" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="123">
+      <c r="A123" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B123" s="1">
+      <c r="B123" s="1" t="n">
         <v>1260</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="124" spans="1:5" hidden="1">
-      <c r="A124" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="124">
+      <c r="A124" s="2" t="n">
         <v>43297</v>
       </c>
-      <c r="B124" s="1">
+      <c r="B124" s="1" t="n">
         <v>3687</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="125" spans="1:5" hidden="1">
-      <c r="A125" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="125">
+      <c r="A125" s="2" t="n">
         <v>43298</v>
       </c>
-      <c r="C125" s="1">
+      <c r="C125" s="1" t="n">
         <v>60</v>
       </c>
       <c r="D125" s="1" t="s">
@@ -3218,55 +2998,55 @@
         <v>178</v>
       </c>
     </row>
-    <row r="126" spans="1:5" hidden="1">
-      <c r="A126" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="126">
+      <c r="A126" s="2" t="n">
         <v>43291</v>
       </c>
-      <c r="C126" s="1">
+      <c r="C126" s="1" t="n">
         <v>404</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="127" spans="1:5" hidden="1">
-      <c r="A127" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="127">
+      <c r="A127" s="2" t="n">
         <v>43290</v>
       </c>
-      <c r="C127" s="1">
+      <c r="C127" s="1" t="n">
         <v>451</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="128" spans="1:5" hidden="1">
-      <c r="A128" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="128">
+      <c r="A128" s="2" t="n">
         <v>43298</v>
       </c>
-      <c r="C128" s="1">
+      <c r="C128" s="1" t="n">
         <v>708</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="129" spans="1:5" hidden="1">
-      <c r="A129" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="129">
+      <c r="A129" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C129" s="1">
+      <c r="C129" s="1" t="n">
         <v>160</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="130" spans="1:5" hidden="1">
-      <c r="A130" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="130">
+      <c r="A130" s="2" t="n">
         <v>43288</v>
       </c>
-      <c r="C130" s="1">
+      <c r="C130" s="1" t="n">
         <v>72</v>
       </c>
       <c r="D130" s="1" t="s">
@@ -3276,11 +3056,11 @@
         <v>181</v>
       </c>
     </row>
-    <row r="131" spans="1:5" hidden="1">
-      <c r="A131" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="131">
+      <c r="A131" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C131" s="1">
+      <c r="C131" s="1" t="n">
         <v>300</v>
       </c>
       <c r="D131" s="1" t="s">
@@ -3290,11 +3070,11 @@
         <v>183</v>
       </c>
     </row>
-    <row r="132" spans="1:5" hidden="1">
-      <c r="A132" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="132">
+      <c r="A132" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C132" s="1">
+      <c r="C132" s="1" t="n">
         <v>230</v>
       </c>
       <c r="D132" s="1" t="s">
@@ -3304,22 +3084,22 @@
         <v>185</v>
       </c>
     </row>
-    <row r="133" spans="1:5" hidden="1">
-      <c r="A133" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="133">
+      <c r="A133" s="2" t="n">
         <v>43293</v>
       </c>
-      <c r="C133" s="1">
+      <c r="C133" s="1" t="n">
         <v>454</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="134" spans="1:5" hidden="1">
-      <c r="A134" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="134">
+      <c r="A134" s="2" t="n">
         <v>43299</v>
       </c>
-      <c r="C134" s="1">
+      <c r="C134" s="1" t="n">
         <v>686</v>
       </c>
       <c r="D134" s="1" t="s">
@@ -3329,11 +3109,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="135" spans="1:5" hidden="1">
-      <c r="A135" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="135">
+      <c r="A135" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C135" s="1">
+      <c r="C135" s="1" t="n">
         <v>400</v>
       </c>
       <c r="D135" s="1" t="s">
@@ -3343,11 +3123,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="136" spans="1:5" hidden="1">
-      <c r="A136" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="136">
+      <c r="A136" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C136" s="1">
+      <c r="C136" s="1" t="n">
         <v>2067</v>
       </c>
       <c r="D136" s="1" t="s">
@@ -3357,11 +3137,11 @@
         <v>186</v>
       </c>
     </row>
-    <row r="137" spans="1:5" hidden="1">
-      <c r="A137" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="137">
+      <c r="A137" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B137" s="1">
+      <c r="B137" s="1" t="n">
         <v>109</v>
       </c>
       <c r="D137" s="1" t="s">
@@ -3371,11 +3151,11 @@
         <v>187</v>
       </c>
     </row>
-    <row r="138" spans="1:5" hidden="1">
-      <c r="A138" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="138">
+      <c r="A138" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B138" s="1">
+      <c r="B138" s="1" t="n">
         <v>97</v>
       </c>
       <c r="D138" s="1" t="s">
@@ -3385,11 +3165,11 @@
         <v>188</v>
       </c>
     </row>
-    <row r="139" spans="1:5" hidden="1">
-      <c r="A139" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="139">
+      <c r="A139" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="B139" s="1">
+      <c r="B139" s="1" t="n">
         <v>1437</v>
       </c>
       <c r="D139" s="1" t="s">
@@ -3399,11 +3179,11 @@
         <v>189</v>
       </c>
     </row>
-    <row r="140" spans="1:5" hidden="1">
-      <c r="A140" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="140">
+      <c r="A140" s="2" t="n">
         <v>43306</v>
       </c>
-      <c r="C140" s="1">
+      <c r="C140" s="1" t="n">
         <v>650</v>
       </c>
       <c r="D140" s="1" t="s">
@@ -3413,11 +3193,11 @@
         <v>190</v>
       </c>
     </row>
-    <row r="141" spans="1:5" hidden="1">
-      <c r="A141" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="141">
+      <c r="A141" s="2" t="n">
         <v>43305</v>
       </c>
-      <c r="C141" s="1">
+      <c r="C141" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D141" s="1" t="s">
@@ -3427,11 +3207,11 @@
         <v>191</v>
       </c>
     </row>
-    <row r="142" spans="1:5" hidden="1">
-      <c r="A142" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="142">
+      <c r="A142" s="2" t="n">
         <v>43309</v>
       </c>
-      <c r="C142" s="1">
+      <c r="C142" s="1" t="n">
         <v>120</v>
       </c>
       <c r="D142" s="1" t="s">
@@ -3441,11 +3221,11 @@
         <v>192</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="14" hidden="1">
-      <c r="A143" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="0" r="143">
+      <c r="A143" s="2" t="n">
         <v>43306</v>
       </c>
-      <c r="B143" s="1">
+      <c r="B143" s="1" t="n">
         <v>167</v>
       </c>
       <c r="D143" s="1" t="s">
@@ -3455,11 +3235,11 @@
         <v>193</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="14" hidden="1">
-      <c r="A144" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="0" r="144">
+      <c r="A144" s="2" t="n">
         <v>43304</v>
       </c>
-      <c r="C144" s="1">
+      <c r="C144" s="1" t="n">
         <v>93</v>
       </c>
       <c r="D144" s="1" t="s">
@@ -3469,11 +3249,11 @@
         <v>194</v>
       </c>
     </row>
-    <row r="145" spans="1:5" hidden="1">
-      <c r="A145" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="145">
+      <c r="A145" s="2" t="n">
         <v>43305</v>
       </c>
-      <c r="C145" s="1">
+      <c r="C145" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D145" s="1" t="s">
@@ -3483,11 +3263,11 @@
         <v>195</v>
       </c>
     </row>
-    <row r="146" spans="1:5" hidden="1">
-      <c r="A146" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="146">
+      <c r="A146" s="2" t="n">
         <v>43303</v>
       </c>
-      <c r="C146" s="1">
+      <c r="C146" s="1" t="n">
         <v>244</v>
       </c>
       <c r="D146" s="1" t="s">
@@ -3497,11 +3277,11 @@
         <v>196</v>
       </c>
     </row>
-    <row r="147" spans="1:5" hidden="1">
-      <c r="A147" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="147">
+      <c r="A147" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C147" s="1">
+      <c r="C147" s="1" t="n">
         <v>482</v>
       </c>
       <c r="D147" s="1" t="s">
@@ -3511,11 +3291,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="148" spans="1:5" hidden="1">
-      <c r="A148" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="148">
+      <c r="A148" s="2" t="n">
         <v>43310</v>
       </c>
-      <c r="C148" s="1">
+      <c r="C148" s="1" t="n">
         <v>172</v>
       </c>
       <c r="D148" s="1" t="s">
@@ -3525,44 +3305,44 @@
         <v>199</v>
       </c>
     </row>
-    <row r="149" spans="1:5" hidden="1">
-      <c r="A149" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="149">
+      <c r="A149" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="B149" s="1">
+      <c r="B149" s="1" t="n">
         <v>89</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="150" spans="1:5" hidden="1">
-      <c r="A150" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="150">
+      <c r="A150" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="C150" s="1">
+      <c r="C150" s="1" t="n">
         <v>107</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="151" spans="1:5" hidden="1">
-      <c r="A151" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="151">
+      <c r="A151" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="C151" s="1">
+      <c r="C151" s="1" t="n">
         <v>124</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="152" spans="1:5" hidden="1">
-      <c r="A152" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="152">
+      <c r="A152" s="7" t="n">
         <v>43316</v>
       </c>
-      <c r="C152" s="1">
+      <c r="C152" s="1" t="n">
         <v>4500</v>
       </c>
       <c r="D152" s="1" t="s">
@@ -3572,11 +3352,11 @@
         <v>202</v>
       </c>
     </row>
-    <row r="153" spans="1:5" hidden="1">
-      <c r="A153" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="153">
+      <c r="A153" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C153" s="1">
+      <c r="C153" s="1" t="n">
         <v>247</v>
       </c>
       <c r="D153" s="1" t="s">
@@ -3586,11 +3366,11 @@
         <v>204</v>
       </c>
     </row>
-    <row r="154" spans="1:5" hidden="1">
-      <c r="A154" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="154">
+      <c r="A154" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C154" s="1">
+      <c r="C154" s="1" t="n">
         <v>1150</v>
       </c>
       <c r="D154" s="1" t="s">
@@ -3600,11 +3380,11 @@
         <v>205</v>
       </c>
     </row>
-    <row r="155" spans="1:5" hidden="1">
-      <c r="A155" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="155">
+      <c r="A155" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="C155" s="1">
+      <c r="C155" s="1" t="n">
         <v>313</v>
       </c>
       <c r="D155" s="1" t="s">
@@ -3614,11 +3394,11 @@
         <v>207</v>
       </c>
     </row>
-    <row r="156" spans="1:5" hidden="1">
-      <c r="A156" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="156">
+      <c r="A156" s="2" t="n">
         <v>43317</v>
       </c>
-      <c r="B156" s="1">
+      <c r="B156" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D156" s="1" t="s">
@@ -3628,11 +3408,11 @@
         <v>209</v>
       </c>
     </row>
-    <row r="157" spans="1:5" hidden="1">
-      <c r="A157" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13" outlineLevel="0" r="157">
+      <c r="A157" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="C157" s="1">
+      <c r="C157" s="1" t="n">
         <v>710</v>
       </c>
       <c r="D157" s="1" t="s">
@@ -3642,11 +3422,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="158" spans="1:5">
-      <c r="A158" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="158">
+      <c r="A158" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="C158" s="1">
+      <c r="C158" s="1" t="n">
         <v>100</v>
       </c>
       <c r="D158" s="1" t="s">
@@ -3656,11 +3436,11 @@
         <v>212</v>
       </c>
     </row>
-    <row r="159" spans="1:5">
-      <c r="A159" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="159">
+      <c r="A159" s="2" t="n">
         <v>43319</v>
       </c>
-      <c r="B159" s="1">
+      <c r="B159" s="1" t="n">
         <v>78</v>
       </c>
       <c r="D159" s="1" t="s">
@@ -3670,22 +3450,22 @@
         <v>213</v>
       </c>
     </row>
-    <row r="160" spans="1:5">
-      <c r="A160" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="160">
+      <c r="A160" s="2" t="n">
         <v>43321</v>
       </c>
-      <c r="B160" s="1">
+      <c r="B160" s="1" t="n">
         <v>1840</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="161" spans="1:5">
-      <c r="A161" s="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="161">
+      <c r="A161" s="2" t="n">
         <v>43322</v>
       </c>
-      <c r="B161" s="1">
+      <c r="B161" s="1" t="n">
         <v>280</v>
       </c>
       <c r="D161" s="1" t="s">
@@ -3695,11 +3475,11 @@
         <v>216</v>
       </c>
     </row>
-    <row r="162" spans="1:5">
-      <c r="A162" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="162">
+      <c r="A162" s="7" t="n">
         <v>43324</v>
       </c>
-      <c r="C162" s="1">
+      <c r="C162" s="1" t="n">
         <v>230</v>
       </c>
       <c r="D162" s="1" t="s">
@@ -3709,11 +3489,11 @@
         <v>217</v>
       </c>
     </row>
-    <row r="163" spans="1:5">
-      <c r="A163" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="163">
+      <c r="A163" s="7" t="n">
         <v>43326</v>
       </c>
-      <c r="C163" s="1">
+      <c r="C163" s="1" t="n">
         <v>450</v>
       </c>
       <c r="D163" s="1" t="s">
@@ -3723,11 +3503,11 @@
         <v>219</v>
       </c>
     </row>
-    <row r="164" spans="1:5">
-      <c r="A164" s="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="164">
+      <c r="A164" s="7" t="n">
         <v>43314</v>
       </c>
-      <c r="B164" s="1">
+      <c r="B164" s="1" t="n">
         <v>45</v>
       </c>
       <c r="D164" s="1" t="s">
@@ -3737,1179 +3517,1240 @@
         <v>221</v>
       </c>
     </row>
-    <row r="165" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A165" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="165">
+      <c r="A165" s="10" t="n">
         <v>43327</v>
       </c>
-      <c r="C165">
+      <c r="C165" s="0" t="n">
         <v>486</v>
       </c>
-      <c r="D165" t="s">
+      <c r="D165" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E165" t="s">
+      <c r="E165" s="0" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="166" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A166" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="166">
+      <c r="A166" s="10" t="n">
         <v>43329</v>
       </c>
-      <c r="C166">
+      <c r="C166" s="0" t="n">
         <v>92</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D166" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="E166" t="s">
+      <c r="E166" s="0" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="167" spans="1:5">
-      <c r="A167" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="167">
+      <c r="A167" s="10" t="n">
         <v>43331</v>
       </c>
-      <c r="C167">
+      <c r="C167" s="0" t="n">
         <v>310</v>
       </c>
-      <c r="D167" t="s">
+      <c r="D167" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="E167" t="s">
+      <c r="E167" s="0" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="168" spans="1:5">
-      <c r="A168" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="168">
+      <c r="A168" s="10" t="n">
         <v>43334</v>
       </c>
-      <c r="C168">
+      <c r="C168" s="0" t="n">
         <v>464</v>
       </c>
-      <c r="D168" t="s">
+      <c r="D168" s="0" t="s">
         <v>218</v>
       </c>
       <c r="E168" s="11" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="169" spans="1:5">
-      <c r="A169" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="169">
+      <c r="A169" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="C169">
+      <c r="C169" s="0" t="n">
         <v>726</v>
       </c>
-      <c r="D169" t="s">
+      <c r="D169" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="E169" t="s">
+      <c r="E169" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="170" spans="1:5">
-      <c r="A170" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="170">
+      <c r="A170" s="10" t="n">
         <v>43337</v>
       </c>
-      <c r="C170">
+      <c r="C170" s="0" t="n">
         <v>544</v>
       </c>
-      <c r="D170" t="s">
+      <c r="D170" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E170" t="s">
+      <c r="E170" s="0" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="171" spans="1:5">
-      <c r="A171" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="171">
+      <c r="A171" s="10" t="n">
         <v>43337</v>
       </c>
-      <c r="B171">
+      <c r="B171" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D171" t="s">
+      <c r="D171" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="E171" t="s">
+      <c r="E171" s="0" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="172" spans="1:5">
-      <c r="A172" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="172">
+      <c r="A172" s="10" t="n">
         <v>43341</v>
       </c>
-      <c r="C172">
+      <c r="C172" s="0" t="n">
         <v>830</v>
       </c>
-      <c r="D172" t="s">
+      <c r="D172" s="0" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="173" spans="1:5">
-      <c r="A173" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="173">
+      <c r="A173" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="C173">
+      <c r="C173" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="D173" t="s">
+      <c r="D173" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="E173" t="s">
+      <c r="E173" s="0" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="174" spans="1:5">
-      <c r="A174" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="174">
+      <c r="A174" s="10" t="n">
         <v>43335</v>
       </c>
-      <c r="B174">
+      <c r="B174" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D174" t="s">
+      <c r="D174" s="0" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="175" spans="1:5">
-      <c r="A175" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="175">
+      <c r="A175" s="10" t="n">
         <v>43344</v>
       </c>
-      <c r="B175">
+      <c r="B175" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="D175" t="s">
+      <c r="D175" s="0" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="176" spans="1:5">
-      <c r="A176" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="176">
+      <c r="A176" s="10" t="n">
         <v>43344</v>
       </c>
-      <c r="B176">
+      <c r="B176" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D176" t="s">
+      <c r="D176" s="0" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="177" spans="1:5">
-      <c r="A177" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="177">
+      <c r="A177" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C177">
+      <c r="C177" s="0" t="n">
         <v>607</v>
       </c>
-      <c r="D177" t="s">
+      <c r="D177" s="0" t="s">
         <v>235</v>
       </c>
-      <c r="E177" t="s">
+      <c r="E177" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="178" spans="1:5">
-      <c r="A178" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="178">
+      <c r="A178" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C178">
+      <c r="C178" s="0" t="n">
         <v>444</v>
       </c>
-      <c r="D178" t="s">
+      <c r="D178" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E178" t="s">
+      <c r="E178" s="0" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="179" spans="1:5">
-      <c r="A179" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="179">
+      <c r="A179" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C179">
+      <c r="C179" s="0" t="n">
         <v>312</v>
       </c>
-      <c r="D179" t="s">
+      <c r="D179" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="E179" t="s">
+      <c r="E179" s="0" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="180" spans="1:5">
-      <c r="A180" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="180">
+      <c r="A180" s="10" t="n">
         <v>43345</v>
       </c>
-      <c r="C180">
+      <c r="C180" s="0" t="n">
         <v>501</v>
       </c>
-      <c r="D180" t="s">
+      <c r="D180" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="E180" t="s">
+      <c r="E180" s="0" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="181" spans="1:5">
-      <c r="A181" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="181">
+      <c r="A181" s="10" t="n">
         <v>43349</v>
       </c>
-      <c r="C181">
+      <c r="C181" s="0" t="n">
         <v>711</v>
       </c>
-      <c r="D181" t="s">
+      <c r="D181" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="E181" t="s">
+      <c r="E181" s="0" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="182" spans="1:5">
-      <c r="A182" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="182">
+      <c r="A182" s="10" t="n">
         <v>43354</v>
       </c>
-      <c r="B182">
+      <c r="B182" s="0" t="n">
         <v>126</v>
       </c>
-      <c r="D182" t="s">
+      <c r="D182" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="E182" t="s">
+      <c r="E182" s="0" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="183" spans="1:5">
-      <c r="A183" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="183">
+      <c r="A183" s="10" t="n">
         <v>43354</v>
       </c>
-      <c r="C183">
+      <c r="C183" s="0" t="n">
         <v>450</v>
       </c>
-      <c r="D183" t="s">
+      <c r="D183" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="E183" t="s">
+      <c r="E183" s="0" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="184" spans="1:5">
-      <c r="A184" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="184">
+      <c r="A184" s="10" t="n">
         <v>43361</v>
       </c>
-      <c r="C184">
+      <c r="C184" s="0" t="n">
         <v>660</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D184" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="E184" t="s">
+      <c r="E184" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="185" spans="1:5">
-      <c r="A185" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="185">
+      <c r="A185" s="10" t="n">
         <v>43363</v>
       </c>
-      <c r="C185">
+      <c r="C185" s="0" t="n">
         <v>230</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D185" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="E185" t="s">
+      <c r="E185" s="0" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="186" spans="1:5">
-      <c r="A186" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="186">
+      <c r="A186" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B186">
+      <c r="B186" s="0" t="n">
         <v>4859</v>
       </c>
-      <c r="D186" t="s">
+      <c r="D186" s="0" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="187" spans="1:5">
-      <c r="A187" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="187">
+      <c r="A187" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B187">
+      <c r="B187" s="0" t="n">
         <v>295</v>
       </c>
-      <c r="D187" t="s">
+      <c r="D187" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="E187" t="s">
+      <c r="E187" s="0" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="188" spans="1:5">
-      <c r="A188" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="188">
+      <c r="A188" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B188">
+      <c r="B188" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D188" t="s">
+      <c r="D188" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="E188" t="s">
+      <c r="E188" s="0" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="189" spans="1:5">
-      <c r="A189" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="189">
+      <c r="A189" s="10" t="n">
         <v>43365</v>
       </c>
-      <c r="B189">
+      <c r="B189" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="D189" t="s">
+      <c r="D189" s="0" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="190" spans="1:5">
-      <c r="A190" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="190">
+      <c r="A190" s="10" t="n">
         <v>43378</v>
       </c>
-      <c r="B190">
+      <c r="B190" s="0" t="n">
         <v>506</v>
       </c>
-      <c r="D190" t="s">
+      <c r="D190" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="E190" t="s">
+      <c r="E190" s="0" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="191" spans="1:5">
-      <c r="A191" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="191">
+      <c r="A191" s="10" t="n">
         <v>43379</v>
       </c>
-      <c r="B191">
+      <c r="B191" s="0" t="n">
         <v>350</v>
       </c>
-      <c r="D191" t="s">
+      <c r="D191" s="0" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="192" spans="1:5" ht="20" customHeight="1">
-      <c r="A192" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="20" outlineLevel="0" r="192">
+      <c r="A192" s="10" t="n">
         <v>43383</v>
       </c>
-      <c r="B192">
+      <c r="B192" s="0" t="n">
         <v>189</v>
       </c>
-      <c r="D192" t="s">
+      <c r="D192" s="0" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="193" spans="1:5">
-      <c r="A193" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="193">
+      <c r="A193" s="10" t="n">
         <v>43387</v>
       </c>
-      <c r="B193">
+      <c r="B193" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="D193" t="s">
+      <c r="D193" s="0" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="194" spans="1:5">
-      <c r="A194" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="194">
+      <c r="A194" s="10" t="n">
         <v>43387</v>
       </c>
-      <c r="B194">
+      <c r="B194" s="0" t="n">
         <v>307</v>
       </c>
-      <c r="D194" t="s">
+      <c r="D194" s="0" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="195" spans="1:5">
-      <c r="C195">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="195">
+      <c r="C195" s="0" t="n">
         <v>3705</v>
       </c>
-      <c r="E195" t="s">
+      <c r="E195" s="0" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="196" spans="1:5">
-      <c r="A196" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="196">
+      <c r="A196" s="10" t="n">
         <v>43385</v>
       </c>
-      <c r="C196">
+      <c r="C196" s="0" t="n">
         <v>608</v>
       </c>
-      <c r="D196" t="s">
+      <c r="D196" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E196" t="s">
+      <c r="E196" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="197" spans="1:5">
-      <c r="A197" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="197">
+      <c r="A197" s="10" t="n">
         <v>43391</v>
       </c>
-      <c r="B197">
+      <c r="B197" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="D197" t="s">
+      <c r="D197" s="0" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="198" spans="1:5">
-      <c r="A198" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="198">
+      <c r="A198" s="10" t="n">
         <v>43392</v>
       </c>
-      <c r="B198">
+      <c r="B198" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="D198" t="s">
+      <c r="D198" s="0" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="199" spans="1:5">
-      <c r="A199" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="199">
+      <c r="A199" s="10" t="n">
         <v>43393</v>
       </c>
-      <c r="B199">
+      <c r="B199" s="0" t="n">
         <v>177</v>
       </c>
-      <c r="D199" t="s">
+      <c r="D199" s="0" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="200" spans="1:5">
-      <c r="A200" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="200">
+      <c r="A200" s="10" t="n">
         <v>43393</v>
       </c>
-      <c r="C200">
+      <c r="C200" s="0" t="n">
         <v>125</v>
       </c>
-      <c r="D200" t="s">
+      <c r="D200" s="0" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="201" spans="1:5">
-      <c r="A201" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="201">
+      <c r="A201" s="10" t="n">
         <v>43395</v>
       </c>
-      <c r="B201">
+      <c r="B201" s="0" t="n">
         <v>2800</v>
       </c>
       <c r="D201" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="E201" t="s">
+      <c r="E201" s="0" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="202" spans="1:5">
-      <c r="A202" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="202">
+      <c r="A202" s="10" t="n">
         <v>43395</v>
       </c>
-      <c r="C202">
+      <c r="C202" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="D202" t="s">
+      <c r="D202" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="E202" t="s">
+      <c r="E202" s="0" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="203" spans="1:5">
-      <c r="A203" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="203">
+      <c r="A203" s="10" t="n">
         <v>43396</v>
       </c>
-      <c r="C203">
+      <c r="C203" s="0" t="n">
         <v>692</v>
       </c>
-      <c r="D203" t="s">
+      <c r="D203" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E203" t="s">
+      <c r="E203" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="204" spans="1:5">
-      <c r="A204" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="204">
+      <c r="A204" s="10" t="n">
         <v>43397</v>
       </c>
-      <c r="C204">
+      <c r="C204" s="0" t="n">
         <v>4935</v>
       </c>
-      <c r="D204" t="s">
+      <c r="D204" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="E204" t="s">
+      <c r="E204" s="0" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="205" spans="1:5" ht="10" customHeight="1">
-      <c r="A205" s="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10" outlineLevel="0" r="205">
+      <c r="A205" s="10" t="n">
         <v>43398</v>
       </c>
-      <c r="B205">
+      <c r="B205" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="D205" t="s">
+      <c r="D205" s="0" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="206" spans="1:5">
-      <c r="A206" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="206">
+      <c r="A206" s="10" t="n">
         <v>43398</v>
       </c>
-      <c r="B206">
+      <c r="B206" s="0" t="n">
         <v>370</v>
       </c>
-      <c r="D206" t="s">
+      <c r="D206" s="0" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="207" spans="1:5">
-      <c r="A207" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="207">
+      <c r="A207" s="10" t="n">
         <v>43398</v>
       </c>
-      <c r="B207">
+      <c r="B207" s="0" t="n">
         <v>4966</v>
       </c>
-      <c r="D207" t="s">
+      <c r="D207" s="0" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="208" spans="1:5">
-      <c r="A208" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="208">
+      <c r="A208" s="10" t="n">
         <v>43397</v>
       </c>
-      <c r="C208">
+      <c r="C208" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="D208" t="s">
+      <c r="D208" s="0" t="s">
         <v>265</v>
       </c>
-      <c r="E208" t="s">
+      <c r="E208" s="0" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="209" spans="1:5">
-      <c r="A209" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="209">
+      <c r="A209" s="10" t="n">
         <v>43399</v>
       </c>
-      <c r="B209">
+      <c r="B209" s="0" t="n">
         <v>182</v>
       </c>
-      <c r="D209" t="s">
+      <c r="D209" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="E209" t="s">
+      <c r="E209" s="0" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="210" spans="1:5">
-      <c r="A210" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="210">
+      <c r="A210" s="10" t="n">
         <v>43401</v>
       </c>
-      <c r="B210">
+      <c r="B210" s="0" t="n">
         <v>700</v>
       </c>
-      <c r="D210" t="s">
+      <c r="D210" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="E210" t="s">
+      <c r="E210" s="0" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="211" spans="1:5">
-      <c r="A211" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="211">
+      <c r="A211" s="10" t="n">
         <v>43405</v>
       </c>
-      <c r="B211">
+      <c r="B211" s="0" t="n">
         <v>274</v>
       </c>
-      <c r="D211" t="s">
+      <c r="D211" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="E211" t="s">
+      <c r="E211" s="0" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="212" spans="1:5">
-      <c r="A212" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="212">
+      <c r="A212" s="10" t="n">
         <v>43405</v>
       </c>
-      <c r="C212">
+      <c r="C212" s="0" t="n">
         <v>590</v>
       </c>
-      <c r="D212" t="s">
+      <c r="D212" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="E212" t="s">
+      <c r="E212" s="0" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="213" spans="1:5" ht="14">
-      <c r="A213" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="213">
+      <c r="A213" s="10" t="n">
         <v>43407</v>
       </c>
-      <c r="C213">
+      <c r="C213" s="0" t="n">
         <v>1275</v>
       </c>
       <c r="D213" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="E213" t="s">
+      <c r="E213" s="0" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="214" spans="1:5" ht="14">
-      <c r="A214" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="214">
+      <c r="A214" s="10" t="n">
         <v>43407</v>
       </c>
-      <c r="C214">
+      <c r="C214" s="0" t="n">
         <v>4781</v>
       </c>
       <c r="D214" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="E214" t="s">
+      <c r="E214" s="0" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="215" spans="1:5" ht="14">
-      <c r="A215" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="215">
+      <c r="A215" s="10" t="n">
         <v>43407</v>
       </c>
-      <c r="C215">
+      <c r="C215" s="0" t="n">
         <v>4781</v>
       </c>
       <c r="D215" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="E215" t="s">
+      <c r="E215" s="0" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="216" spans="1:5">
-      <c r="A216" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="216">
+      <c r="A216" s="10" t="n">
         <v>43406</v>
       </c>
-      <c r="C216">
+      <c r="C216" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D216" t="s">
+      <c r="D216" s="0" t="s">
         <v>272</v>
       </c>
-      <c r="E216" t="s">
+      <c r="E216" s="0" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="217" spans="1:5">
-      <c r="A217" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="217">
+      <c r="A217" s="10" t="n">
         <v>43409</v>
       </c>
-      <c r="C217">
+      <c r="C217" s="0" t="n">
         <v>677</v>
       </c>
-      <c r="D217" t="s">
+      <c r="D217" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E217" t="s">
+      <c r="E217" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="218" spans="1:5" ht="14">
-      <c r="A218" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="218">
+      <c r="A218" s="10" t="n">
         <v>43410</v>
       </c>
-      <c r="B218">
+      <c r="B218" s="0" t="n">
         <v>285</v>
       </c>
       <c r="D218" s="13" t="s">
         <v>274</v>
       </c>
-      <c r="E218" t="s">
+      <c r="E218" s="0" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="219" spans="1:5" ht="14">
-      <c r="A219" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="219">
+      <c r="A219" s="10" t="n">
         <v>43410</v>
       </c>
-      <c r="B219">
+      <c r="B219" s="0" t="n">
         <v>125</v>
       </c>
       <c r="D219" s="13" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="220" spans="1:5" ht="14">
-      <c r="A220" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="220">
+      <c r="A220" s="10" t="n">
         <v>43409</v>
       </c>
-      <c r="B220">
+      <c r="B220" s="0" t="n">
         <v>85</v>
       </c>
       <c r="D220" s="13" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="221" spans="1:5" ht="14">
-      <c r="A221" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="221">
+      <c r="A221" s="10" t="n">
         <v>43410</v>
       </c>
-      <c r="B221">
+      <c r="B221" s="0" t="n">
         <v>44</v>
       </c>
       <c r="D221" s="13" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="222" spans="1:5">
-      <c r="A222" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="222">
+      <c r="A222" s="10" t="n">
         <v>43412</v>
       </c>
-      <c r="C222">
+      <c r="C222" s="0" t="n">
         <v>190</v>
       </c>
-      <c r="D222" t="s">
+      <c r="D222" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="E222" t="s">
+      <c r="E222" s="0" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="223" spans="1:5" ht="14">
-      <c r="A223" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="223">
+      <c r="A223" s="10" t="n">
         <v>43415</v>
       </c>
-      <c r="B223">
+      <c r="B223" s="0" t="n">
         <v>189</v>
       </c>
       <c r="D223" s="13" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="224" spans="1:5" ht="14">
-      <c r="A224" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="224">
+      <c r="A224" s="10" t="n">
         <v>43415</v>
       </c>
-      <c r="B224">
+      <c r="B224" s="0" t="n">
         <v>336</v>
       </c>
       <c r="D224" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="E224" t="s">
+      <c r="E224" s="0" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="225" spans="1:5" ht="14">
-      <c r="A225" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="225">
+      <c r="A225" s="10" t="n">
         <v>43419</v>
       </c>
-      <c r="B225">
+      <c r="B225" s="0" t="n">
         <v>158</v>
       </c>
       <c r="D225" s="13" t="s">
         <v>282</v>
       </c>
-      <c r="E225" t="s">
+      <c r="E225" s="0" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="226" spans="1:5">
-      <c r="A226" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="226">
+      <c r="A226" s="10" t="n">
         <v>43418</v>
       </c>
-      <c r="C226">
+      <c r="C226" s="0" t="n">
         <v>642</v>
       </c>
-      <c r="D226" t="s">
+      <c r="D226" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E226" t="s">
+      <c r="E226" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="227" spans="1:5">
-      <c r="A227" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="227">
+      <c r="A227" s="10" t="n">
         <v>43419</v>
       </c>
-      <c r="C227">
+      <c r="C227" s="0" t="n">
         <v>370</v>
       </c>
-      <c r="D227" t="s">
+      <c r="D227" s="0" t="s">
         <v>284</v>
       </c>
-      <c r="E227" t="s">
+      <c r="E227" s="0" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="228" spans="1:5">
-      <c r="A228" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="228">
+      <c r="A228" s="10" t="n">
         <v>43419</v>
       </c>
-      <c r="C228">
+      <c r="C228" s="0" t="n">
         <v>222</v>
       </c>
-      <c r="D228" t="s">
+      <c r="D228" s="0" t="s">
         <v>286</v>
       </c>
-      <c r="E228" t="s">
+      <c r="E228" s="0" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="229" spans="1:5">
-      <c r="A229" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="229">
+      <c r="A229" s="10" t="n">
         <v>43421</v>
       </c>
-      <c r="B229">
+      <c r="B229" s="0" t="n">
         <v>300</v>
       </c>
-      <c r="D229" t="s">
+      <c r="D229" s="0" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="230" spans="1:5">
-      <c r="A230" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="230">
+      <c r="A230" s="10" t="n">
         <v>43422</v>
       </c>
-      <c r="B230">
+      <c r="B230" s="0" t="n">
         <v>158</v>
       </c>
-      <c r="D230" t="s">
+      <c r="D230" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="E230" t="s">
+      <c r="E230" s="0" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="231" spans="1:5">
-      <c r="A231" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="231">
+      <c r="A231" s="10" t="n">
         <v>43422</v>
       </c>
-      <c r="B231">
+      <c r="B231" s="0" t="n">
         <v>159</v>
       </c>
-      <c r="D231" t="s">
+      <c r="D231" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="E231" t="s">
+      <c r="E231" s="0" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="232" spans="1:5">
-      <c r="A232" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="232">
+      <c r="A232" s="10" t="n">
         <v>43421</v>
       </c>
-      <c r="C232">
+      <c r="C232" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="D232" t="s">
+      <c r="D232" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="E232" t="s">
+      <c r="E232" s="0" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="233" spans="1:5">
-      <c r="A233" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="233">
+      <c r="A233" s="10" t="n">
         <v>43422</v>
       </c>
-      <c r="B233">
+      <c r="B233" s="0" t="n">
         <v>11649</v>
       </c>
-      <c r="D233" t="s">
+      <c r="D233" s="0" t="s">
         <v>290</v>
       </c>
-      <c r="E233" t="s">
+      <c r="E233" s="0" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="234" spans="1:5">
-      <c r="A234" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="234">
+      <c r="A234" s="10" t="n">
         <v>43426</v>
       </c>
-      <c r="C234">
+      <c r="C234" s="0" t="n">
         <v>308</v>
       </c>
-      <c r="D234" t="s">
+      <c r="D234" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="E234" t="s">
+      <c r="E234" s="0" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="235" spans="1:5">
-      <c r="A235" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="235">
+      <c r="A235" s="10" t="n">
         <v>43428</v>
       </c>
-      <c r="B235">
+      <c r="B235" s="0" t="n">
         <v>112</v>
       </c>
-      <c r="D235" t="s">
+      <c r="D235" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="E235" t="s">
+      <c r="E235" s="0" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="236" spans="1:5">
-      <c r="A236" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="236">
+      <c r="A236" s="10" t="n">
         <v>43428</v>
       </c>
-      <c r="B236">
+      <c r="B236" s="0" t="n">
         <v>79</v>
       </c>
-      <c r="D236" t="s">
+      <c r="D236" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="E236" t="s">
+      <c r="E236" s="0" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="237" spans="1:5">
-      <c r="A237" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="237">
+      <c r="A237" s="10" t="n">
         <v>43425</v>
       </c>
-      <c r="C237">
+      <c r="C237" s="0" t="n">
         <v>93</v>
       </c>
-      <c r="D237" t="s">
+      <c r="D237" s="0" t="s">
         <v>272</v>
       </c>
-      <c r="E237" t="s">
+      <c r="E237" s="0" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="238" spans="1:5">
-      <c r="A238" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="238">
+      <c r="A238" s="10" t="n">
         <v>43426</v>
       </c>
-      <c r="C238">
+      <c r="C238" s="0" t="n">
         <v>308</v>
       </c>
-      <c r="D238" t="s">
+      <c r="D238" s="0" t="s">
         <v>295</v>
       </c>
-      <c r="E238" t="s">
+      <c r="E238" s="0" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="239" spans="1:5">
-      <c r="A239" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="239">
+      <c r="A239" s="10" t="n">
         <v>43430</v>
       </c>
-      <c r="C239">
+      <c r="C239" s="0" t="n">
         <v>616</v>
       </c>
-      <c r="D239" t="s">
+      <c r="D239" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="E239" t="s">
+      <c r="E239" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="240" spans="1:5">
-      <c r="A240" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="240">
+      <c r="A240" s="10" t="n">
         <v>43430</v>
       </c>
-      <c r="C240">
+      <c r="C240" s="0" t="n">
         <v>243</v>
       </c>
-      <c r="D240" t="s">
+      <c r="D240" s="0" t="s">
         <v>297</v>
       </c>
-      <c r="E240" t="s">
+      <c r="E240" s="0" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="241" spans="1:5">
-      <c r="A241" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="241">
+      <c r="A241" s="10" t="n">
         <v>43432</v>
       </c>
-      <c r="C241">
+      <c r="C241" s="0" t="n">
         <v>850</v>
       </c>
-      <c r="D241" t="s">
+      <c r="D241" s="0" t="s">
         <v>299</v>
       </c>
-      <c r="E241" t="s">
+      <c r="E241" s="0" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="242" spans="1:5">
-      <c r="A242" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="242">
+      <c r="A242" s="10" t="n">
         <v>43433</v>
       </c>
-      <c r="B242">
+      <c r="B242" s="0" t="n">
         <v>75</v>
       </c>
-      <c r="D242" t="s">
+      <c r="D242" s="0" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="243" spans="1:5">
-      <c r="A243" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="243">
+      <c r="A243" s="10" t="n">
         <v>43433</v>
       </c>
-      <c r="C243">
+      <c r="C243" s="0" t="n">
         <v>212</v>
       </c>
-      <c r="D243" t="s">
+      <c r="D243" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E243" t="s">
+      <c r="E243" s="0" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="244" spans="1:5">
-      <c r="A244" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="244">
+      <c r="A244" s="10" t="n">
         <v>43433</v>
       </c>
-      <c r="C244">
+      <c r="C244" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="D244" t="s">
+      <c r="D244" s="0" t="s">
         <v>303</v>
       </c>
-      <c r="E244" t="s">
+      <c r="E244" s="0" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="245" spans="1:5">
-      <c r="A245" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="245">
+      <c r="A245" s="10" t="n">
         <v>43436</v>
       </c>
-      <c r="B245">
+      <c r="B245" s="0" t="n">
         <v>142</v>
       </c>
-      <c r="D245" t="s">
+      <c r="D245" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="E245" t="s">
+      <c r="E245" s="0" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="246" spans="1:5">
-      <c r="A246" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="246">
+      <c r="A246" s="10" t="n">
         <v>43436</v>
       </c>
-      <c r="C246">
+      <c r="C246" s="0" t="n">
         <v>318</v>
       </c>
-      <c r="D246" t="s">
+      <c r="D246" s="0" t="s">
         <v>286</v>
       </c>
-      <c r="E246" t="s">
+      <c r="E246" s="0" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="247" spans="1:5">
-      <c r="A247" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="247">
+      <c r="A247" s="10" t="n">
         <v>43439</v>
       </c>
-      <c r="B247">
+      <c r="B247" s="0" t="n">
         <v>761</v>
       </c>
-      <c r="D247" t="s">
+      <c r="D247" s="0" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="248" spans="1:5">
-      <c r="A248" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="248">
+      <c r="A248" s="10" t="n">
         <v>43440</v>
       </c>
-      <c r="B248">
+      <c r="B248" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="D248" t="s">
+      <c r="D248" s="0" t="s">
         <v>309</v>
       </c>
-      <c r="E248" t="s">
+      <c r="E248" s="0" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="249" spans="1:5">
-      <c r="A249" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="249">
+      <c r="A249" s="10" t="n">
         <v>43440</v>
       </c>
-      <c r="B249">
+      <c r="B249" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="D249" t="s">
+      <c r="D249" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="E249" t="s">
+      <c r="E249" s="0" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="250" spans="1:5">
-      <c r="A250" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="250">
+      <c r="A250" s="10" t="n">
         <v>43440</v>
       </c>
-      <c r="B250">
+      <c r="B250" s="0" t="n">
         <v>140</v>
       </c>
-      <c r="D250" t="s">
+      <c r="D250" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="E250" t="s">
+      <c r="E250" s="0" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="251" spans="1:5">
-      <c r="A251" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="251">
+      <c r="A251" s="10" t="n">
         <v>43440</v>
       </c>
-      <c r="B251">
+      <c r="B251" s="0" t="n">
         <v>66</v>
       </c>
-      <c r="D251" t="s">
+      <c r="D251" s="0" t="s">
         <v>297</v>
       </c>
-      <c r="E251" t="s">
+      <c r="E251" s="0" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="252" spans="1:5">
-      <c r="A252" s="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="252">
+      <c r="A252" s="10" t="n">
         <v>43441</v>
       </c>
-      <c r="B252">
+      <c r="B252" s="0" t="n">
         <v>1287</v>
       </c>
-      <c r="D252" t="s">
+      <c r="D252" s="0" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="260" spans="2:3">
-      <c r="B260">
-        <f>SUM(B2:B259)</f>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="253">
+      <c r="A253" s="10" t="n">
+        <v>43437</v>
+      </c>
+      <c r="C253" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="D253" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="E253" s="0" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="254">
+      <c r="A254" s="10" t="n">
+        <v>43440</v>
+      </c>
+      <c r="C254" s="0" t="n">
+        <v>580</v>
+      </c>
+      <c r="D254" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E254" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="255">
+      <c r="A255" s="10" t="n">
+        <v>43441</v>
+      </c>
+      <c r="C255" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="D255" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="E255" s="0" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="256">
+      <c r="A256" s="10" t="n">
+        <v>43443</v>
+      </c>
+      <c r="C256" s="0" t="n">
+        <v>424</v>
+      </c>
+      <c r="D256" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="E256" s="0" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="260">
+      <c r="B260" s="0" t="n">
+        <f aca="false">SUM(B2:B259)</f>
         <v>72222</v>
       </c>
-      <c r="C260">
-        <f>SUM(C2:C259)</f>
-        <v>69307</v>
+      <c r="C260" s="0" t="n">
+        <f aca="false">SUM(C2:C259)</f>
+        <v>70469</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A30:Z32">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule aboveAverage="0" bottom="0" dxfId="0" operator="expression" percent="0" priority="2" rank="0" text="" type="expression">
       <formula>LEN(TRIM(A30))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D33" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D40" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D201" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink display="netonnet.se" ref="D33" r:id="rId1"/>
+    <hyperlink display="www.vidaxl.se" ref="D40" r:id="rId2"/>
+    <hyperlink display="https://www.vardia.se/" ref="D201" r:id="rId3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" 